<commit_message>
Update dashboards - 2025-10-15
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -2953,7 +2953,7 @@
       </c>
       <c r="N29" s="6" t="inlineStr">
         <is>
-          <t>2025-10-10</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="O29" s="10" t="inlineStr">
@@ -2967,7 +2967,7 @@
         </is>
       </c>
       <c r="Q29" s="6" t="n">
-        <v>2.25</v>
+        <v>2.27</v>
       </c>
       <c r="R29" s="6" t="n">
         <v>2.3</v>
@@ -3036,7 +3036,7 @@
       </c>
       <c r="N30" s="6" t="inlineStr">
         <is>
-          <t>2025-10-10</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="O30" s="10" t="inlineStr">
@@ -3053,16 +3053,16 @@
         <v>2.3</v>
       </c>
       <c r="R30" s="6" t="n">
+        <v/>
+      </c>
+      <c r="S30" s="6" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="T30" s="6" t="n">
         <v>2.34</v>
       </c>
-      <c r="S30" s="6" t="n">
+      <c r="U30" s="11" t="n">
         <v>2.35</v>
-      </c>
-      <c r="T30" s="6" t="n">
-        <v>2.35</v>
-      </c>
-      <c r="U30" s="11" t="n">
-        <v>2.34</v>
       </c>
     </row>
     <row r="31">

</xml_diff>

<commit_message>
Update dashboards - 2025-10-17
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -2957,7 +2957,7 @@
       </c>
       <c r="N29" s="12" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="O29" s="8" t="inlineStr">
@@ -2971,7 +2971,7 @@
         </is>
       </c>
       <c r="Q29" s="8" t="n">
-        <v>2.25</v>
+        <v>2.27</v>
       </c>
       <c r="R29" s="8" t="n">
         <v>2.3</v>
@@ -3040,7 +3040,7 @@
       </c>
       <c r="N30" s="12" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="O30" s="8" t="inlineStr">
@@ -3054,19 +3054,19 @@
         </is>
       </c>
       <c r="Q30" s="8" t="n">
+        <v>2.28</v>
+      </c>
+      <c r="R30" s="8" t="n">
         <v>2.29</v>
       </c>
-      <c r="R30" s="8" t="n">
+      <c r="S30" s="8" t="n">
         <v>2.3</v>
       </c>
-      <c r="S30" s="8" t="n">
+      <c r="T30" s="8" t="n">
         <v/>
       </c>
-      <c r="T30" s="8" t="n">
+      <c r="U30" s="30" t="n">
         <v>2.3</v>
-      </c>
-      <c r="U30" s="30" t="n">
-        <v>2.34</v>
       </c>
     </row>
     <row r="31">
@@ -4438,7 +4438,7 @@
       </c>
       <c r="N48" s="12" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="O48" s="8" t="inlineStr">
@@ -4452,19 +4452,19 @@
         </is>
       </c>
       <c r="Q48" s="8" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="R48" s="8" t="n">
         <v>3.48</v>
       </c>
-      <c r="R48" s="8" t="n">
+      <c r="S48" s="8" t="n">
         <v/>
       </c>
-      <c r="S48" s="8" t="n">
+      <c r="T48" s="8" t="n">
         <v>3.52</v>
       </c>
-      <c r="T48" s="8" t="n">
+      <c r="U48" s="30" t="n">
         <v>3.6</v>
-      </c>
-      <c r="U48" s="30" t="n">
-        <v>3.58</v>
       </c>
     </row>
     <row r="49">
@@ -4517,7 +4517,7 @@
       </c>
       <c r="N49" s="12" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="O49" s="8" t="inlineStr">
@@ -4531,19 +4531,19 @@
         </is>
       </c>
       <c r="Q49" s="8" t="n">
+        <v>3.63</v>
+      </c>
+      <c r="R49" s="8" t="n">
         <v>3.6</v>
       </c>
-      <c r="R49" s="8" t="n">
+      <c r="S49" s="8" t="n">
         <v/>
       </c>
-      <c r="S49" s="8" t="n">
+      <c r="T49" s="8" t="n">
         <v>3.65</v>
       </c>
-      <c r="T49" s="8" t="n">
+      <c r="U49" s="30" t="n">
         <v>3.74</v>
-      </c>
-      <c r="U49" s="30" t="n">
-        <v>3.72</v>
       </c>
     </row>
     <row r="50">
@@ -4600,7 +4600,7 @@
       </c>
       <c r="N50" s="12" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="O50" s="8" t="inlineStr">
@@ -4614,19 +4614,19 @@
         </is>
       </c>
       <c r="Q50" s="8" t="n">
+        <v>4.05</v>
+      </c>
+      <c r="R50" s="8" t="n">
         <v>4.03</v>
       </c>
-      <c r="R50" s="8" t="n">
+      <c r="S50" s="8" t="n">
         <v/>
       </c>
-      <c r="S50" s="8" t="n">
+      <c r="T50" s="8" t="n">
         <v>4.05</v>
       </c>
-      <c r="T50" s="8" t="n">
+      <c r="U50" s="30" t="n">
         <v>4.14</v>
-      </c>
-      <c r="U50" s="30" t="n">
-        <v>4.13</v>
       </c>
     </row>
     <row r="51" ht="31.5" customHeight="1">
@@ -4679,7 +4679,7 @@
       </c>
       <c r="N51" s="12" t="inlineStr">
         <is>
-          <t>2025-10-09</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="O51" s="8" t="inlineStr">
@@ -4693,19 +4693,19 @@
         </is>
       </c>
       <c r="Q51" s="8" t="n">
+        <v>6.27</v>
+      </c>
+      <c r="R51" s="8" t="n">
         <v>6.3</v>
       </c>
-      <c r="R51" s="8" t="n">
+      <c r="S51" s="8" t="n">
         <v>6.34</v>
       </c>
-      <c r="S51" s="8" t="n">
+      <c r="T51" s="8" t="n">
         <v>6.3</v>
       </c>
-      <c r="T51" s="8" t="n">
+      <c r="U51" s="30" t="n">
         <v>6.26</v>
-      </c>
-      <c r="U51" s="30" t="n">
-        <v>6.35</v>
       </c>
     </row>
     <row r="52" ht="16.15" customHeight="1" thickBot="1">
@@ -4732,7 +4732,7 @@
       </c>
       <c r="N52" s="29" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="O52" s="15" t="inlineStr">
@@ -4746,19 +4746,19 @@
         </is>
       </c>
       <c r="Q52" s="15" t="n">
+        <v>5.73</v>
+      </c>
+      <c r="R52" s="15" t="n">
         <v>5.74</v>
       </c>
-      <c r="R52" s="15" t="n">
+      <c r="S52" s="15" t="n">
         <v/>
       </c>
-      <c r="S52" s="15" t="n">
+      <c r="T52" s="15" t="n">
         <v>5.77</v>
       </c>
-      <c r="T52" s="15" t="n">
+      <c r="U52" s="31" t="n">
         <v>5.83</v>
-      </c>
-      <c r="U52" s="31" t="n">
-        <v>5.81</v>
       </c>
     </row>
     <row r="53">

</xml_diff>

<commit_message>
Update dashboards - 2025-10-18
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -2957,7 +2957,7 @@
       </c>
       <c r="N29" s="12" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="O29" s="8" t="inlineStr">
@@ -2971,7 +2971,7 @@
         </is>
       </c>
       <c r="Q29" s="8" t="n">
-        <v>2.27</v>
+        <v>2.25</v>
       </c>
       <c r="R29" s="8" t="n">
         <v>2.3</v>
@@ -3040,7 +3040,7 @@
       </c>
       <c r="N30" s="12" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="O30" s="8" t="inlineStr">
@@ -3054,19 +3054,19 @@
         </is>
       </c>
       <c r="Q30" s="8" t="n">
+        <v>2.27</v>
+      </c>
+      <c r="R30" s="8" t="n">
         <v>2.28</v>
       </c>
-      <c r="R30" s="8" t="n">
+      <c r="S30" s="8" t="n">
         <v>2.29</v>
       </c>
-      <c r="S30" s="8" t="n">
+      <c r="T30" s="8" t="n">
         <v>2.3</v>
       </c>
-      <c r="T30" s="8" t="n">
+      <c r="U30" s="30" t="n">
         <v/>
-      </c>
-      <c r="U30" s="30" t="n">
-        <v>2.3</v>
       </c>
     </row>
     <row r="31">
@@ -4438,7 +4438,7 @@
       </c>
       <c r="N48" s="12" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="O48" s="8" t="inlineStr">
@@ -4452,19 +4452,19 @@
         </is>
       </c>
       <c r="Q48" s="8" t="n">
+        <v>3.41</v>
+      </c>
+      <c r="R48" s="8" t="n">
         <v>3.5</v>
       </c>
-      <c r="R48" s="8" t="n">
+      <c r="S48" s="8" t="n">
         <v>3.48</v>
       </c>
-      <c r="S48" s="8" t="n">
+      <c r="T48" s="8" t="n">
         <v/>
       </c>
-      <c r="T48" s="8" t="n">
+      <c r="U48" s="30" t="n">
         <v>3.52</v>
-      </c>
-      <c r="U48" s="30" t="n">
-        <v>3.6</v>
       </c>
     </row>
     <row r="49">
@@ -4517,7 +4517,7 @@
       </c>
       <c r="N49" s="12" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="O49" s="8" t="inlineStr">
@@ -4531,19 +4531,19 @@
         </is>
       </c>
       <c r="Q49" s="8" t="n">
+        <v>3.55</v>
+      </c>
+      <c r="R49" s="8" t="n">
         <v>3.63</v>
       </c>
-      <c r="R49" s="8" t="n">
+      <c r="S49" s="8" t="n">
         <v>3.6</v>
       </c>
-      <c r="S49" s="8" t="n">
+      <c r="T49" s="8" t="n">
         <v/>
       </c>
-      <c r="T49" s="8" t="n">
+      <c r="U49" s="30" t="n">
         <v>3.65</v>
-      </c>
-      <c r="U49" s="30" t="n">
-        <v>3.74</v>
       </c>
     </row>
     <row r="50">
@@ -4600,7 +4600,7 @@
       </c>
       <c r="N50" s="12" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="O50" s="8" t="inlineStr">
@@ -4614,19 +4614,19 @@
         </is>
       </c>
       <c r="Q50" s="8" t="n">
+        <v>3.99</v>
+      </c>
+      <c r="R50" s="8" t="n">
         <v>4.05</v>
       </c>
-      <c r="R50" s="8" t="n">
+      <c r="S50" s="8" t="n">
         <v>4.03</v>
       </c>
-      <c r="S50" s="8" t="n">
+      <c r="T50" s="8" t="n">
         <v/>
       </c>
-      <c r="T50" s="8" t="n">
+      <c r="U50" s="30" t="n">
         <v>4.05</v>
-      </c>
-      <c r="U50" s="30" t="n">
-        <v>4.14</v>
       </c>
     </row>
     <row r="51" ht="31.5" customHeight="1">
@@ -4732,7 +4732,7 @@
       </c>
       <c r="N52" s="29" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="O52" s="15" t="inlineStr">
@@ -4746,19 +4746,19 @@
         </is>
       </c>
       <c r="Q52" s="15" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="R52" s="15" t="n">
         <v>5.73</v>
       </c>
-      <c r="R52" s="15" t="n">
+      <c r="S52" s="15" t="n">
         <v>5.74</v>
       </c>
-      <c r="S52" s="15" t="n">
+      <c r="T52" s="15" t="n">
         <v/>
       </c>
-      <c r="T52" s="15" t="n">
+      <c r="U52" s="31" t="n">
         <v>5.77</v>
-      </c>
-      <c r="U52" s="31" t="n">
-        <v>5.83</v>
       </c>
     </row>
     <row r="53">

</xml_diff>

<commit_message>
Update dashboards - 2025-10-21
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -2957,7 +2957,7 @@
       </c>
       <c r="N29" s="12" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-20</t>
         </is>
       </c>
       <c r="O29" s="8" t="inlineStr">
@@ -2971,7 +2971,7 @@
         </is>
       </c>
       <c r="Q29" s="8" t="n">
-        <v>2.25</v>
+        <v>2.24</v>
       </c>
       <c r="R29" s="8" t="n">
         <v>2.3</v>
@@ -3040,7 +3040,7 @@
       </c>
       <c r="N30" s="12" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-20</t>
         </is>
       </c>
       <c r="O30" s="8" t="inlineStr">
@@ -3054,19 +3054,19 @@
         </is>
       </c>
       <c r="Q30" s="8" t="n">
+        <v>2.26</v>
+      </c>
+      <c r="R30" s="8" t="n">
         <v>2.27</v>
       </c>
-      <c r="R30" s="8" t="n">
+      <c r="S30" s="8" t="n">
         <v>2.28</v>
       </c>
-      <c r="S30" s="8" t="n">
+      <c r="T30" s="8" t="n">
         <v>2.29</v>
       </c>
-      <c r="T30" s="8" t="n">
+      <c r="U30" s="30" t="n">
         <v>2.3</v>
-      </c>
-      <c r="U30" s="30" t="n">
-        <v/>
       </c>
     </row>
     <row r="31">
@@ -3739,7 +3739,7 @@
       </c>
       <c r="N39" s="12" t="inlineStr">
         <is>
-          <t>2025-10-10</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="O39" s="8" t="inlineStr">
@@ -3753,19 +3753,19 @@
         </is>
       </c>
       <c r="Q39" s="8" t="n">
-        <v>121.5217</v>
+        <v>121.1218</v>
       </c>
       <c r="R39" s="8" t="n">
-        <v>121.4965</v>
+        <v>121.0834</v>
       </c>
       <c r="S39" s="8" t="n">
-        <v>121.1884</v>
+        <v>121.2669</v>
       </c>
       <c r="T39" s="8" t="n">
-        <v>120.9097</v>
+        <v>121.5815</v>
       </c>
       <c r="U39" s="30" t="n">
-        <v>120.7028</v>
+        <v/>
       </c>
     </row>
     <row r="40">
@@ -3818,7 +3818,7 @@
       </c>
       <c r="N40" s="12" t="inlineStr">
         <is>
-          <t>2025-10-10</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="O40" s="8" t="inlineStr">
@@ -3832,7 +3832,7 @@
         </is>
       </c>
       <c r="Q40" s="8" t="n">
-        <v>-2.801846355160221</v>
+        <v>-3.121703151457274</v>
       </c>
       <c r="R40" s="8" t="n">
         <v>-0.7960187542479276</v>
@@ -4438,7 +4438,7 @@
       </c>
       <c r="N48" s="12" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="O48" s="8" t="inlineStr">
@@ -4452,19 +4452,19 @@
         </is>
       </c>
       <c r="Q48" s="8" t="n">
+        <v>3.46</v>
+      </c>
+      <c r="R48" s="8" t="n">
         <v>3.41</v>
       </c>
-      <c r="R48" s="8" t="n">
+      <c r="S48" s="8" t="n">
         <v>3.5</v>
       </c>
-      <c r="S48" s="8" t="n">
+      <c r="T48" s="8" t="n">
         <v>3.48</v>
       </c>
-      <c r="T48" s="8" t="n">
+      <c r="U48" s="30" t="n">
         <v/>
-      </c>
-      <c r="U48" s="30" t="n">
-        <v>3.52</v>
       </c>
     </row>
     <row r="49">
@@ -4517,7 +4517,7 @@
       </c>
       <c r="N49" s="12" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="O49" s="8" t="inlineStr">
@@ -4531,19 +4531,19 @@
         </is>
       </c>
       <c r="Q49" s="8" t="n">
+        <v>3.59</v>
+      </c>
+      <c r="R49" s="8" t="n">
         <v>3.55</v>
       </c>
-      <c r="R49" s="8" t="n">
+      <c r="S49" s="8" t="n">
         <v>3.63</v>
       </c>
-      <c r="S49" s="8" t="n">
+      <c r="T49" s="8" t="n">
         <v>3.6</v>
       </c>
-      <c r="T49" s="8" t="n">
+      <c r="U49" s="30" t="n">
         <v/>
-      </c>
-      <c r="U49" s="30" t="n">
-        <v>3.65</v>
       </c>
     </row>
     <row r="50">
@@ -4600,7 +4600,7 @@
       </c>
       <c r="N50" s="12" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="O50" s="8" t="inlineStr">
@@ -4614,19 +4614,19 @@
         </is>
       </c>
       <c r="Q50" s="8" t="n">
+        <v>4.02</v>
+      </c>
+      <c r="R50" s="8" t="n">
         <v>3.99</v>
       </c>
-      <c r="R50" s="8" t="n">
+      <c r="S50" s="8" t="n">
         <v>4.05</v>
       </c>
-      <c r="S50" s="8" t="n">
+      <c r="T50" s="8" t="n">
         <v>4.03</v>
       </c>
-      <c r="T50" s="8" t="n">
+      <c r="U50" s="30" t="n">
         <v/>
-      </c>
-      <c r="U50" s="30" t="n">
-        <v>4.05</v>
       </c>
     </row>
     <row r="51" ht="31.5" customHeight="1">
@@ -4732,7 +4732,7 @@
       </c>
       <c r="N52" s="29" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="O52" s="15" t="inlineStr">
@@ -4746,19 +4746,19 @@
         </is>
       </c>
       <c r="Q52" s="15" t="n">
+        <v>5.72</v>
+      </c>
+      <c r="R52" s="15" t="n">
         <v>5.7</v>
       </c>
-      <c r="R52" s="15" t="n">
+      <c r="S52" s="15" t="n">
         <v>5.73</v>
       </c>
-      <c r="S52" s="15" t="n">
+      <c r="T52" s="15" t="n">
         <v>5.74</v>
       </c>
-      <c r="T52" s="15" t="n">
+      <c r="U52" s="31" t="n">
         <v/>
-      </c>
-      <c r="U52" s="31" t="n">
-        <v>5.77</v>
       </c>
     </row>
     <row r="53">

</xml_diff>

<commit_message>
Update dashboards - 2025-10-22
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -2993,7 +2993,7 @@
       </c>
       <c r="N29" s="7" t="inlineStr">
         <is>
-          <t>2025-10-20</t>
+          <t>2025-10-21</t>
         </is>
       </c>
       <c r="O29" s="6" t="inlineStr">
@@ -3007,7 +3007,7 @@
         </is>
       </c>
       <c r="Q29" s="6" t="n">
-        <v>2.24</v>
+        <v>2.26</v>
       </c>
       <c r="R29" s="6" t="n">
         <v>2.3</v>
@@ -3076,7 +3076,7 @@
       </c>
       <c r="N30" s="7" t="inlineStr">
         <is>
-          <t>2025-10-20</t>
+          <t>2025-10-21</t>
         </is>
       </c>
       <c r="O30" s="6" t="inlineStr">
@@ -3090,19 +3090,19 @@
         </is>
       </c>
       <c r="Q30" s="6" t="n">
+        <v>2.28</v>
+      </c>
+      <c r="R30" s="6" t="n">
         <v>2.26</v>
       </c>
-      <c r="R30" s="6" t="n">
+      <c r="S30" s="6" t="n">
         <v>2.27</v>
       </c>
-      <c r="S30" s="6" t="n">
+      <c r="T30" s="6" t="n">
         <v>2.28</v>
       </c>
-      <c r="T30" s="6" t="n">
+      <c r="U30" s="21" t="n">
         <v>2.29</v>
-      </c>
-      <c r="U30" s="21" t="n">
-        <v>2.3</v>
       </c>
     </row>
     <row r="31">
@@ -4490,7 +4490,7 @@
       </c>
       <c r="N48" s="7" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-20</t>
         </is>
       </c>
       <c r="O48" s="6" t="inlineStr">
@@ -4507,16 +4507,16 @@
         <v>3.46</v>
       </c>
       <c r="R48" s="6" t="n">
+        <v>3.46</v>
+      </c>
+      <c r="S48" s="6" t="n">
         <v>3.41</v>
       </c>
-      <c r="S48" s="6" t="n">
+      <c r="T48" s="6" t="n">
         <v>3.5</v>
       </c>
-      <c r="T48" s="6" t="n">
+      <c r="U48" s="21" t="n">
         <v>3.48</v>
-      </c>
-      <c r="U48" s="21" t="n">
-        <v/>
       </c>
     </row>
     <row r="49">
@@ -4569,7 +4569,7 @@
       </c>
       <c r="N49" s="7" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-20</t>
         </is>
       </c>
       <c r="O49" s="6" t="inlineStr">
@@ -4583,19 +4583,19 @@
         </is>
       </c>
       <c r="Q49" s="6" t="n">
+        <v>3.58</v>
+      </c>
+      <c r="R49" s="6" t="n">
         <v>3.59</v>
       </c>
-      <c r="R49" s="6" t="n">
+      <c r="S49" s="6" t="n">
         <v>3.55</v>
       </c>
-      <c r="S49" s="6" t="n">
+      <c r="T49" s="6" t="n">
         <v>3.63</v>
       </c>
-      <c r="T49" s="6" t="n">
+      <c r="U49" s="21" t="n">
         <v>3.6</v>
-      </c>
-      <c r="U49" s="21" t="n">
-        <v/>
       </c>
     </row>
     <row r="50">
@@ -4652,7 +4652,7 @@
       </c>
       <c r="N50" s="7" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-20</t>
         </is>
       </c>
       <c r="O50" s="6" t="inlineStr">
@@ -4666,19 +4666,19 @@
         </is>
       </c>
       <c r="Q50" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="R50" s="6" t="n">
         <v>4.02</v>
       </c>
-      <c r="R50" s="6" t="n">
+      <c r="S50" s="6" t="n">
         <v>3.99</v>
       </c>
-      <c r="S50" s="6" t="n">
+      <c r="T50" s="6" t="n">
         <v>4.05</v>
       </c>
-      <c r="T50" s="6" t="n">
+      <c r="U50" s="21" t="n">
         <v>4.03</v>
-      </c>
-      <c r="U50" s="21" t="n">
-        <v/>
       </c>
     </row>
     <row r="51" ht="31.5" customHeight="1">

</xml_diff>

<commit_message>
Update dashboards - 2025-10-23
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -2993,7 +2993,7 @@
       </c>
       <c r="N29" s="7" t="inlineStr">
         <is>
-          <t>2025-10-21</t>
+          <t>2025-10-22</t>
         </is>
       </c>
       <c r="O29" s="6" t="inlineStr">
@@ -3076,7 +3076,7 @@
       </c>
       <c r="N30" s="7" t="inlineStr">
         <is>
-          <t>2025-10-21</t>
+          <t>2025-10-22</t>
         </is>
       </c>
       <c r="O30" s="6" t="inlineStr">
@@ -3090,19 +3090,19 @@
         </is>
       </c>
       <c r="Q30" s="6" t="n">
+        <v>2.29</v>
+      </c>
+      <c r="R30" s="6" t="n">
         <v>2.28</v>
       </c>
-      <c r="R30" s="6" t="n">
+      <c r="S30" s="6" t="n">
         <v>2.26</v>
       </c>
-      <c r="S30" s="6" t="n">
+      <c r="T30" s="6" t="n">
         <v>2.27</v>
       </c>
-      <c r="T30" s="6" t="n">
+      <c r="U30" s="21" t="n">
         <v>2.28</v>
-      </c>
-      <c r="U30" s="21" t="n">
-        <v>2.29</v>
       </c>
     </row>
     <row r="31">
@@ -3991,7 +3991,7 @@
       </c>
       <c r="C42" s="7" t="inlineStr">
         <is>
-          <t>2025-08-01</t>
+          <t>2025-09-01</t>
         </is>
       </c>
       <c r="D42" s="6" t="inlineStr">
@@ -4005,19 +4005,19 @@
         </is>
       </c>
       <c r="F42" s="39" t="n">
+        <v>4060000</v>
+      </c>
+      <c r="G42" s="39" t="n">
         <v>4000000</v>
       </c>
-      <c r="G42" s="39" t="n">
+      <c r="H42" s="39" t="n">
         <v>4010000</v>
       </c>
-      <c r="H42" s="39" t="n">
+      <c r="I42" s="39" t="n">
         <v>3930000</v>
       </c>
-      <c r="I42" s="39" t="n">
+      <c r="J42" s="39" t="n">
         <v>4040000</v>
-      </c>
-      <c r="J42" s="39" t="n">
-        <v>4000000</v>
       </c>
       <c r="K42" s="7" t="n"/>
       <c r="L42" s="43" t="n"/>
@@ -4066,7 +4066,7 @@
       </c>
       <c r="C43" s="7" t="inlineStr">
         <is>
-          <t>2025-08-01</t>
+          <t>2025-09-01</t>
         </is>
       </c>
       <c r="D43" s="6" t="inlineStr">
@@ -4080,7 +4080,7 @@
         </is>
       </c>
       <c r="F43" s="38" t="n">
-        <v>0.0178117048346056</v>
+        <v>0.04102564102564103</v>
       </c>
       <c r="G43" s="38" t="n">
         <v/>
@@ -4490,7 +4490,7 @@
       </c>
       <c r="N48" s="7" t="inlineStr">
         <is>
-          <t>2025-10-20</t>
+          <t>2025-10-21</t>
         </is>
       </c>
       <c r="O48" s="6" t="inlineStr">
@@ -4504,19 +4504,19 @@
         </is>
       </c>
       <c r="Q48" s="6" t="n">
-        <v>3.46</v>
+        <v>3.45</v>
       </c>
       <c r="R48" s="6" t="n">
         <v>3.46</v>
       </c>
       <c r="S48" s="6" t="n">
+        <v>3.46</v>
+      </c>
+      <c r="T48" s="6" t="n">
         <v>3.41</v>
       </c>
-      <c r="T48" s="6" t="n">
+      <c r="U48" s="21" t="n">
         <v>3.5</v>
-      </c>
-      <c r="U48" s="21" t="n">
-        <v>3.48</v>
       </c>
     </row>
     <row r="49">
@@ -4569,7 +4569,7 @@
       </c>
       <c r="N49" s="7" t="inlineStr">
         <is>
-          <t>2025-10-20</t>
+          <t>2025-10-21</t>
         </is>
       </c>
       <c r="O49" s="6" t="inlineStr">
@@ -4583,19 +4583,19 @@
         </is>
       </c>
       <c r="Q49" s="6" t="n">
+        <v>3.56</v>
+      </c>
+      <c r="R49" s="6" t="n">
         <v>3.58</v>
       </c>
-      <c r="R49" s="6" t="n">
+      <c r="S49" s="6" t="n">
         <v>3.59</v>
       </c>
-      <c r="S49" s="6" t="n">
+      <c r="T49" s="6" t="n">
         <v>3.55</v>
       </c>
-      <c r="T49" s="6" t="n">
+      <c r="U49" s="21" t="n">
         <v>3.63</v>
-      </c>
-      <c r="U49" s="21" t="n">
-        <v>3.6</v>
       </c>
     </row>
     <row r="50">
@@ -4652,7 +4652,7 @@
       </c>
       <c r="N50" s="7" t="inlineStr">
         <is>
-          <t>2025-10-20</t>
+          <t>2025-10-21</t>
         </is>
       </c>
       <c r="O50" s="6" t="inlineStr">
@@ -4666,19 +4666,19 @@
         </is>
       </c>
       <c r="Q50" s="6" t="n">
+        <v>3.98</v>
+      </c>
+      <c r="R50" s="6" t="n">
         <v>4</v>
       </c>
-      <c r="R50" s="6" t="n">
+      <c r="S50" s="6" t="n">
         <v>4.02</v>
       </c>
-      <c r="S50" s="6" t="n">
+      <c r="T50" s="6" t="n">
         <v>3.99</v>
       </c>
-      <c r="T50" s="6" t="n">
+      <c r="U50" s="21" t="n">
         <v>4.05</v>
-      </c>
-      <c r="U50" s="21" t="n">
-        <v>4.03</v>
       </c>
     </row>
     <row r="51" ht="31.5" customHeight="1">

</xml_diff>

<commit_message>
Update dashboards - 2025-10-24
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -2110,7 +2110,7 @@
       </c>
       <c r="N18" s="7" t="inlineStr">
         <is>
-          <t>2025-08-01</t>
+          <t>2025-09-01</t>
         </is>
       </c>
       <c r="O18" s="6" t="inlineStr">
@@ -2124,19 +2124,19 @@
         </is>
       </c>
       <c r="Q18" s="38" t="n">
+        <v>0.00310486015759337</v>
+      </c>
+      <c r="R18" s="38" t="n">
         <v>0.003824519141221616</v>
       </c>
-      <c r="R18" s="38" t="n">
+      <c r="S18" s="38" t="n">
         <v>0.00196578538102643</v>
       </c>
-      <c r="S18" s="38" t="n">
+      <c r="T18" s="38" t="n">
         <v>0.002869798490236386</v>
       </c>
-      <c r="T18" s="38" t="n">
+      <c r="U18" s="23" t="n">
         <v>0.0008085639093282637</v>
-      </c>
-      <c r="U18" s="23" t="n">
-        <v>0.002208907591946696</v>
       </c>
     </row>
     <row r="19" ht="31.5" customHeight="1">
@@ -2189,7 +2189,7 @@
       </c>
       <c r="N19" s="7" t="inlineStr">
         <is>
-          <t>2025-08-01</t>
+          <t>2025-09-01</t>
         </is>
       </c>
       <c r="O19" s="6" t="inlineStr">
@@ -2203,19 +2203,19 @@
         </is>
       </c>
       <c r="Q19" s="38" t="n">
+        <v>0.03022699626172379</v>
+      </c>
+      <c r="R19" s="38" t="n">
         <v>0.02939219624933549</v>
       </c>
-      <c r="R19" s="38" t="n">
+      <c r="S19" s="38" t="n">
         <v>0.02731801279475463</v>
       </c>
-      <c r="S19" s="38" t="n">
+      <c r="T19" s="38" t="n">
         <v>0.02672683317844617</v>
       </c>
-      <c r="T19" s="38" t="n">
+      <c r="U19" s="23" t="n">
         <v>0.02375934086989844</v>
-      </c>
-      <c r="U19" s="23" t="n">
-        <v>0.02333746517749893</v>
       </c>
     </row>
     <row r="20">
@@ -2268,7 +2268,7 @@
       </c>
       <c r="N20" s="7" t="inlineStr">
         <is>
-          <t>2025-08-01</t>
+          <t>2025-09-01</t>
         </is>
       </c>
       <c r="O20" s="6" t="inlineStr">
@@ -2282,19 +2282,19 @@
         </is>
       </c>
       <c r="Q20" s="38" t="n">
+        <v>0.002271121582325675</v>
+      </c>
+      <c r="R20" s="38" t="n">
         <v>0.003459544325982167</v>
       </c>
-      <c r="R20" s="38" t="n">
+      <c r="S20" s="38" t="n">
         <v>0.003223443223443256</v>
       </c>
-      <c r="S20" s="38" t="n">
+      <c r="T20" s="38" t="n">
         <v>0.002282364603156228</v>
       </c>
-      <c r="T20" s="38" t="n">
+      <c r="U20" s="23" t="n">
         <v>0.001298900223631438</v>
-      </c>
-      <c r="U20" s="23" t="n">
-        <v>0.002367507116339596</v>
       </c>
     </row>
     <row r="21">
@@ -2347,7 +2347,7 @@
       </c>
       <c r="N21" s="7" t="inlineStr">
         <is>
-          <t>2025-08-01</t>
+          <t>2025-09-01</t>
         </is>
       </c>
       <c r="O21" s="6" t="inlineStr">
@@ -2361,19 +2361,19 @@
         </is>
       </c>
       <c r="Q21" s="38" t="n">
+        <v>0.03025542724453378</v>
+      </c>
+      <c r="R21" s="38" t="n">
         <v>0.03112190821006822</v>
       </c>
-      <c r="R21" s="38" t="n">
+      <c r="S21" s="38" t="n">
         <v>0.03048602684576389</v>
       </c>
-      <c r="S21" s="38" t="n">
+      <c r="T21" s="38" t="n">
         <v>0.02907869813377396</v>
       </c>
-      <c r="T21" s="38" t="n">
+      <c r="U21" s="23" t="n">
         <v>0.02767148871414509</v>
-      </c>
-      <c r="U21" s="23" t="n">
-        <v>0.02781521177848589</v>
       </c>
     </row>
     <row r="22">
@@ -2990,7 +2990,7 @@
       </c>
       <c r="N29" s="7" t="inlineStr">
         <is>
-          <t>2025-10-22</t>
+          <t>2025-10-23</t>
         </is>
       </c>
       <c r="O29" s="6" t="inlineStr">
@@ -3004,7 +3004,7 @@
         </is>
       </c>
       <c r="Q29" s="6" t="n">
-        <v>2.26</v>
+        <v>2.18</v>
       </c>
       <c r="R29" s="6" t="n">
         <v>2.3</v>
@@ -3073,7 +3073,7 @@
       </c>
       <c r="N30" s="7" t="inlineStr">
         <is>
-          <t>2025-10-22</t>
+          <t>2025-10-23</t>
         </is>
       </c>
       <c r="O30" s="6" t="inlineStr">
@@ -3087,19 +3087,19 @@
         </is>
       </c>
       <c r="Q30" s="6" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="R30" s="6" t="n">
         <v>2.29</v>
       </c>
-      <c r="R30" s="6" t="n">
+      <c r="S30" s="6" t="n">
         <v>2.28</v>
       </c>
-      <c r="S30" s="6" t="n">
+      <c r="T30" s="6" t="n">
         <v>2.26</v>
       </c>
-      <c r="T30" s="6" t="n">
+      <c r="U30" s="21" t="n">
         <v>2.27</v>
-      </c>
-      <c r="U30" s="21" t="n">
-        <v>2.28</v>
       </c>
     </row>
     <row r="31">
@@ -4487,7 +4487,7 @@
       </c>
       <c r="N48" s="7" t="inlineStr">
         <is>
-          <t>2025-10-21</t>
+          <t>2025-10-22</t>
         </is>
       </c>
       <c r="O48" s="6" t="inlineStr">
@@ -4504,16 +4504,16 @@
         <v>3.45</v>
       </c>
       <c r="R48" s="6" t="n">
-        <v>3.46</v>
+        <v>3.45</v>
       </c>
       <c r="S48" s="6" t="n">
         <v>3.46</v>
       </c>
       <c r="T48" s="6" t="n">
+        <v>3.46</v>
+      </c>
+      <c r="U48" s="21" t="n">
         <v>3.41</v>
-      </c>
-      <c r="U48" s="21" t="n">
-        <v>3.5</v>
       </c>
     </row>
     <row r="49">
@@ -4566,7 +4566,7 @@
       </c>
       <c r="N49" s="7" t="inlineStr">
         <is>
-          <t>2025-10-21</t>
+          <t>2025-10-22</t>
         </is>
       </c>
       <c r="O49" s="6" t="inlineStr">
@@ -4583,16 +4583,16 @@
         <v>3.56</v>
       </c>
       <c r="R49" s="6" t="n">
+        <v>3.56</v>
+      </c>
+      <c r="S49" s="6" t="n">
         <v>3.58</v>
       </c>
-      <c r="S49" s="6" t="n">
+      <c r="T49" s="6" t="n">
         <v>3.59</v>
       </c>
-      <c r="T49" s="6" t="n">
+      <c r="U49" s="21" t="n">
         <v>3.55</v>
-      </c>
-      <c r="U49" s="21" t="n">
-        <v>3.63</v>
       </c>
     </row>
     <row r="50">
@@ -4649,7 +4649,7 @@
       </c>
       <c r="N50" s="7" t="inlineStr">
         <is>
-          <t>2025-10-21</t>
+          <t>2025-10-22</t>
         </is>
       </c>
       <c r="O50" s="6" t="inlineStr">
@@ -4663,19 +4663,19 @@
         </is>
       </c>
       <c r="Q50" s="6" t="n">
+        <v>3.97</v>
+      </c>
+      <c r="R50" s="6" t="n">
         <v>3.98</v>
       </c>
-      <c r="R50" s="6" t="n">
+      <c r="S50" s="6" t="n">
         <v>4</v>
       </c>
-      <c r="S50" s="6" t="n">
+      <c r="T50" s="6" t="n">
         <v>4.02</v>
       </c>
-      <c r="T50" s="6" t="n">
+      <c r="U50" s="21" t="n">
         <v>3.99</v>
-      </c>
-      <c r="U50" s="21" t="n">
-        <v>4.05</v>
       </c>
     </row>
     <row r="51" ht="31.5" customHeight="1">
@@ -4728,7 +4728,7 @@
       </c>
       <c r="N51" s="7" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-23</t>
         </is>
       </c>
       <c r="O51" s="6" t="inlineStr">
@@ -4742,19 +4742,19 @@
         </is>
       </c>
       <c r="Q51" s="6" t="n">
+        <v>6.19</v>
+      </c>
+      <c r="R51" s="6" t="n">
         <v>6.27</v>
       </c>
-      <c r="R51" s="6" t="n">
+      <c r="S51" s="6" t="n">
         <v>6.3</v>
       </c>
-      <c r="S51" s="6" t="n">
+      <c r="T51" s="6" t="n">
         <v>6.34</v>
       </c>
-      <c r="T51" s="6" t="n">
+      <c r="U51" s="21" t="n">
         <v>6.3</v>
-      </c>
-      <c r="U51" s="21" t="n">
-        <v>6.26</v>
       </c>
     </row>
     <row r="52" ht="16.15" customHeight="1" thickBot="1">
@@ -4781,7 +4781,7 @@
       </c>
       <c r="N52" s="20" t="inlineStr">
         <is>
-          <t>2025-10-20</t>
+          <t>2025-10-22</t>
         </is>
       </c>
       <c r="O52" s="9" t="inlineStr">
@@ -4795,19 +4795,19 @@
         </is>
       </c>
       <c r="Q52" s="9" t="n">
+        <v>5.66</v>
+      </c>
+      <c r="R52" s="9" t="n">
+        <v>5.65</v>
+      </c>
+      <c r="S52" s="9" t="n">
         <v>5.68</v>
       </c>
-      <c r="R52" s="9" t="n">
+      <c r="T52" s="9" t="n">
         <v>5.72</v>
       </c>
-      <c r="S52" s="9" t="n">
+      <c r="U52" s="22" t="n">
         <v>5.7</v>
-      </c>
-      <c r="T52" s="9" t="n">
-        <v>5.73</v>
-      </c>
-      <c r="U52" s="22" t="n">
-        <v>5.74</v>
       </c>
     </row>
     <row r="53" ht="21" customHeight="1">

</xml_diff>

<commit_message>
Update dashboards - 2025-10-25
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -2911,7 +2911,7 @@
       </c>
       <c r="N28" s="7" t="inlineStr">
         <is>
-          <t>2025-08-01</t>
+          <t>2025-09-01</t>
         </is>
       </c>
       <c r="O28" s="6" t="inlineStr">
@@ -2925,16 +2925,16 @@
         </is>
       </c>
       <c r="Q28" s="6" t="n">
+        <v>55.1</v>
+      </c>
+      <c r="R28" s="6" t="n">
         <v>58.2</v>
       </c>
-      <c r="R28" s="6" t="n">
+      <c r="S28" s="6" t="n">
         <v>61.7</v>
       </c>
-      <c r="S28" s="6" t="n">
+      <c r="T28" s="6" t="n">
         <v>60.7</v>
-      </c>
-      <c r="T28" s="6" t="n">
-        <v>52.2</v>
       </c>
       <c r="U28" s="21" t="n">
         <v>52.2</v>
@@ -2990,7 +2990,7 @@
       </c>
       <c r="N29" s="7" t="inlineStr">
         <is>
-          <t>2025-10-23</t>
+          <t>2025-10-24</t>
         </is>
       </c>
       <c r="O29" s="6" t="inlineStr">
@@ -3073,7 +3073,7 @@
       </c>
       <c r="N30" s="7" t="inlineStr">
         <is>
-          <t>2025-10-23</t>
+          <t>2025-10-24</t>
         </is>
       </c>
       <c r="O30" s="6" t="inlineStr">
@@ -3087,19 +3087,19 @@
         </is>
       </c>
       <c r="Q30" s="6" t="n">
+        <v>2.29</v>
+      </c>
+      <c r="R30" s="6" t="n">
         <v>2.3</v>
       </c>
-      <c r="R30" s="6" t="n">
+      <c r="S30" s="6" t="n">
         <v>2.29</v>
       </c>
-      <c r="S30" s="6" t="n">
+      <c r="T30" s="6" t="n">
         <v>2.28</v>
       </c>
-      <c r="T30" s="6" t="n">
+      <c r="U30" s="21" t="n">
         <v>2.26</v>
-      </c>
-      <c r="U30" s="21" t="n">
-        <v>2.27</v>
       </c>
     </row>
     <row r="31">
@@ -4487,7 +4487,7 @@
       </c>
       <c r="N48" s="7" t="inlineStr">
         <is>
-          <t>2025-10-22</t>
+          <t>2025-10-23</t>
         </is>
       </c>
       <c r="O48" s="6" t="inlineStr">
@@ -4501,19 +4501,19 @@
         </is>
       </c>
       <c r="Q48" s="6" t="n">
-        <v>3.45</v>
+        <v>3.48</v>
       </c>
       <c r="R48" s="6" t="n">
         <v>3.45</v>
       </c>
       <c r="S48" s="6" t="n">
-        <v>3.46</v>
+        <v>3.45</v>
       </c>
       <c r="T48" s="6" t="n">
         <v>3.46</v>
       </c>
       <c r="U48" s="21" t="n">
-        <v>3.41</v>
+        <v>3.46</v>
       </c>
     </row>
     <row r="49">
@@ -4566,7 +4566,7 @@
       </c>
       <c r="N49" s="7" t="inlineStr">
         <is>
-          <t>2025-10-22</t>
+          <t>2025-10-23</t>
         </is>
       </c>
       <c r="O49" s="6" t="inlineStr">
@@ -4580,19 +4580,19 @@
         </is>
       </c>
       <c r="Q49" s="6" t="n">
-        <v>3.56</v>
+        <v>3.61</v>
       </c>
       <c r="R49" s="6" t="n">
         <v>3.56</v>
       </c>
       <c r="S49" s="6" t="n">
+        <v>3.56</v>
+      </c>
+      <c r="T49" s="6" t="n">
         <v>3.58</v>
       </c>
-      <c r="T49" s="6" t="n">
+      <c r="U49" s="21" t="n">
         <v>3.59</v>
-      </c>
-      <c r="U49" s="21" t="n">
-        <v>3.55</v>
       </c>
     </row>
     <row r="50">
@@ -4649,7 +4649,7 @@
       </c>
       <c r="N50" s="7" t="inlineStr">
         <is>
-          <t>2025-10-22</t>
+          <t>2025-10-23</t>
         </is>
       </c>
       <c r="O50" s="6" t="inlineStr">
@@ -4663,19 +4663,19 @@
         </is>
       </c>
       <c r="Q50" s="6" t="n">
+        <v>4.01</v>
+      </c>
+      <c r="R50" s="6" t="n">
         <v>3.97</v>
       </c>
-      <c r="R50" s="6" t="n">
+      <c r="S50" s="6" t="n">
         <v>3.98</v>
       </c>
-      <c r="S50" s="6" t="n">
+      <c r="T50" s="6" t="n">
         <v>4</v>
       </c>
-      <c r="T50" s="6" t="n">
+      <c r="U50" s="21" t="n">
         <v>4.02</v>
-      </c>
-      <c r="U50" s="21" t="n">
-        <v>3.99</v>
       </c>
     </row>
     <row r="51" ht="31.5" customHeight="1">
@@ -4781,7 +4781,7 @@
       </c>
       <c r="N52" s="20" t="inlineStr">
         <is>
-          <t>2025-10-22</t>
+          <t>2025-10-23</t>
         </is>
       </c>
       <c r="O52" s="9" t="inlineStr">
@@ -4795,19 +4795,19 @@
         </is>
       </c>
       <c r="Q52" s="9" t="n">
+        <v>5.67</v>
+      </c>
+      <c r="R52" s="9" t="n">
         <v>5.66</v>
       </c>
-      <c r="R52" s="9" t="n">
+      <c r="S52" s="9" t="n">
         <v>5.65</v>
       </c>
-      <c r="S52" s="9" t="n">
+      <c r="T52" s="9" t="n">
         <v>5.68</v>
       </c>
-      <c r="T52" s="9" t="n">
+      <c r="U52" s="22" t="n">
         <v>5.72</v>
-      </c>
-      <c r="U52" s="22" t="n">
-        <v>5.7</v>
       </c>
     </row>
     <row r="53" ht="21" customHeight="1">

</xml_diff>

<commit_message>
Update dashboards - 2025-10-27
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -1210,7 +1210,7 @@
         </is>
       </c>
       <c r="F7" s="25" t="n">
-        <v>0.2975878704341832</v>
+        <v>0.352997932460372</v>
       </c>
       <c r="G7" s="25" t="n">
         <v>-2.062303243282817</v>
@@ -2884,10 +2884,10 @@
         </is>
       </c>
       <c r="F28" s="25" t="n">
-        <v>0.02933036907051223</v>
+        <v>0.0292251268148207</v>
       </c>
       <c r="G28" s="25" t="n">
-        <v>-0.02756598804853716</v>
+        <v>-0.02746655290430811</v>
       </c>
       <c r="H28" s="25" t="n">
         <v>-0.09389977010425232</v>
@@ -2966,7 +2966,7 @@
         <v>0.07634016956050854</v>
       </c>
       <c r="G29" s="25" t="n">
-        <v>0.03387397095834726</v>
+        <v>0.03397968857635882</v>
       </c>
       <c r="H29" s="25" t="n">
         <v>0.1089645997552716</v>
@@ -3046,10 +3046,10 @@
         </is>
       </c>
       <c r="F30" s="25" t="n">
-        <v>0.02037556476894942</v>
+        <v>0.01923414103867871</v>
       </c>
       <c r="G30" s="25" t="n">
-        <v>-0.02457975064120344</v>
+        <v>-0.02348739337531547</v>
       </c>
       <c r="H30" s="25" t="n">
         <v>-0.09442194506291901</v>
@@ -3128,7 +3128,7 @@
         <v>0.06748567650947554</v>
       </c>
       <c r="G31" s="25" t="n">
-        <v>0.03236433616868596</v>
+        <v>0.03352046419083723</v>
       </c>
       <c r="H31" s="25" t="n">
         <v>0.1029410098461701</v>

</xml_diff>

<commit_message>
Update dashboards - 2025-10-28
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -2990,7 +2990,7 @@
       </c>
       <c r="N29" s="7" t="inlineStr">
         <is>
-          <t>2025-10-24</t>
+          <t>2025-10-27</t>
         </is>
       </c>
       <c r="O29" s="6" t="inlineStr">
@@ -3004,7 +3004,7 @@
         </is>
       </c>
       <c r="Q29" s="6" t="n">
-        <v>2.18</v>
+        <v>2.19</v>
       </c>
       <c r="R29" s="6" t="n">
         <v>2.3</v>
@@ -3073,7 +3073,7 @@
       </c>
       <c r="N30" s="7" t="inlineStr">
         <is>
-          <t>2025-10-24</t>
+          <t>2025-10-27</t>
         </is>
       </c>
       <c r="O30" s="6" t="inlineStr">
@@ -3087,19 +3087,19 @@
         </is>
       </c>
       <c r="Q30" s="6" t="n">
+        <v>2.28</v>
+      </c>
+      <c r="R30" s="6" t="n">
         <v>2.29</v>
       </c>
-      <c r="R30" s="6" t="n">
+      <c r="S30" s="6" t="n">
         <v>2.3</v>
       </c>
-      <c r="S30" s="6" t="n">
+      <c r="T30" s="6" t="n">
         <v>2.29</v>
       </c>
-      <c r="T30" s="6" t="n">
+      <c r="U30" s="21" t="n">
         <v>2.28</v>
-      </c>
-      <c r="U30" s="21" t="n">
-        <v>2.26</v>
       </c>
     </row>
     <row r="31">
@@ -3788,7 +3788,7 @@
       </c>
       <c r="N39" s="7" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-24</t>
         </is>
       </c>
       <c r="O39" s="6" t="inlineStr">
@@ -3802,19 +3802,19 @@
         </is>
       </c>
       <c r="Q39" s="6" t="n">
-        <v>121.1218</v>
+        <v>121.342</v>
       </c>
       <c r="R39" s="6" t="n">
-        <v>121.0834</v>
+        <v>121.3633</v>
       </c>
       <c r="S39" s="6" t="n">
-        <v>121.2669</v>
+        <v>121.3075</v>
       </c>
       <c r="T39" s="6" t="n">
-        <v>121.5815</v>
+        <v>121.302</v>
       </c>
       <c r="U39" s="21" t="n">
-        <v/>
+        <v>121.0394</v>
       </c>
     </row>
     <row r="40">
@@ -3867,7 +3867,7 @@
       </c>
       <c r="N40" s="7" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-24</t>
         </is>
       </c>
       <c r="O40" s="6" t="inlineStr">
@@ -3881,7 +3881,7 @@
         </is>
       </c>
       <c r="Q40" s="38" t="n">
-        <v>-0.03121703151457274</v>
+        <v>-0.02945577953796328</v>
       </c>
       <c r="R40" s="38" t="n">
         <v>-0.007960187542479276</v>
@@ -4487,7 +4487,7 @@
       </c>
       <c r="N48" s="7" t="inlineStr">
         <is>
-          <t>2025-10-23</t>
+          <t>2025-10-24</t>
         </is>
       </c>
       <c r="O48" s="6" t="inlineStr">
@@ -4504,13 +4504,13 @@
         <v>3.48</v>
       </c>
       <c r="R48" s="6" t="n">
-        <v>3.45</v>
+        <v>3.48</v>
       </c>
       <c r="S48" s="6" t="n">
         <v>3.45</v>
       </c>
       <c r="T48" s="6" t="n">
-        <v>3.46</v>
+        <v>3.45</v>
       </c>
       <c r="U48" s="21" t="n">
         <v>3.46</v>
@@ -4566,7 +4566,7 @@
       </c>
       <c r="N49" s="7" t="inlineStr">
         <is>
-          <t>2025-10-23</t>
+          <t>2025-10-24</t>
         </is>
       </c>
       <c r="O49" s="6" t="inlineStr">
@@ -4583,16 +4583,16 @@
         <v>3.61</v>
       </c>
       <c r="R49" s="6" t="n">
-        <v>3.56</v>
+        <v>3.61</v>
       </c>
       <c r="S49" s="6" t="n">
         <v>3.56</v>
       </c>
       <c r="T49" s="6" t="n">
+        <v>3.56</v>
+      </c>
+      <c r="U49" s="21" t="n">
         <v>3.58</v>
-      </c>
-      <c r="U49" s="21" t="n">
-        <v>3.59</v>
       </c>
     </row>
     <row r="50">
@@ -4649,7 +4649,7 @@
       </c>
       <c r="N50" s="7" t="inlineStr">
         <is>
-          <t>2025-10-23</t>
+          <t>2025-10-24</t>
         </is>
       </c>
       <c r="O50" s="6" t="inlineStr">
@@ -4663,19 +4663,19 @@
         </is>
       </c>
       <c r="Q50" s="6" t="n">
+        <v>4.02</v>
+      </c>
+      <c r="R50" s="6" t="n">
         <v>4.01</v>
       </c>
-      <c r="R50" s="6" t="n">
+      <c r="S50" s="6" t="n">
         <v>3.97</v>
       </c>
-      <c r="S50" s="6" t="n">
+      <c r="T50" s="6" t="n">
         <v>3.98</v>
       </c>
-      <c r="T50" s="6" t="n">
+      <c r="U50" s="21" t="n">
         <v>4</v>
-      </c>
-      <c r="U50" s="21" t="n">
-        <v>4.02</v>
       </c>
     </row>
     <row r="51" ht="31.5" customHeight="1">
@@ -4781,7 +4781,7 @@
       </c>
       <c r="N52" s="20" t="inlineStr">
         <is>
-          <t>2025-10-23</t>
+          <t>2025-10-24</t>
         </is>
       </c>
       <c r="O52" s="9" t="inlineStr">
@@ -4798,16 +4798,16 @@
         <v>5.67</v>
       </c>
       <c r="R52" s="9" t="n">
+        <v>5.67</v>
+      </c>
+      <c r="S52" s="9" t="n">
         <v>5.66</v>
       </c>
-      <c r="S52" s="9" t="n">
+      <c r="T52" s="9" t="n">
         <v>5.65</v>
       </c>
-      <c r="T52" s="9" t="n">
+      <c r="U52" s="22" t="n">
         <v>5.68</v>
-      </c>
-      <c r="U52" s="22" t="n">
-        <v>5.72</v>
       </c>
     </row>
     <row r="53" ht="21" customHeight="1">

</xml_diff>

<commit_message>
Update dashboards - 2025-10-29
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -2990,7 +2990,7 @@
       </c>
       <c r="N29" s="7" t="inlineStr">
         <is>
-          <t>2025-10-27</t>
+          <t>2025-10-28</t>
         </is>
       </c>
       <c r="O29" s="6" t="inlineStr">
@@ -3004,7 +3004,7 @@
         </is>
       </c>
       <c r="Q29" s="6" t="n">
-        <v>2.19</v>
+        <v>2.2</v>
       </c>
       <c r="R29" s="6" t="n">
         <v>2.3</v>
@@ -3073,7 +3073,7 @@
       </c>
       <c r="N30" s="7" t="inlineStr">
         <is>
-          <t>2025-10-27</t>
+          <t>2025-10-28</t>
         </is>
       </c>
       <c r="O30" s="6" t="inlineStr">
@@ -3090,16 +3090,16 @@
         <v>2.28</v>
       </c>
       <c r="R30" s="6" t="n">
+        <v>2.28</v>
+      </c>
+      <c r="S30" s="6" t="n">
         <v>2.29</v>
       </c>
-      <c r="S30" s="6" t="n">
+      <c r="T30" s="6" t="n">
         <v>2.3</v>
       </c>
-      <c r="T30" s="6" t="n">
+      <c r="U30" s="21" t="n">
         <v>2.29</v>
-      </c>
-      <c r="U30" s="21" t="n">
-        <v>2.28</v>
       </c>
     </row>
     <row r="31">
@@ -3630,7 +3630,7 @@
       </c>
       <c r="N37" s="7" t="inlineStr">
         <is>
-          <t>2025-07-01</t>
+          <t>2025-08-01</t>
         </is>
       </c>
       <c r="O37" s="6" t="inlineStr">
@@ -3644,19 +3644,19 @@
         </is>
       </c>
       <c r="Q37" s="38" t="n">
-        <v>-0.001640179575543299</v>
+        <v>-0.002963719362060191</v>
       </c>
       <c r="R37" s="38" t="n">
-        <v>0.000678843612534008</v>
+        <v>-0.002056167749521443</v>
       </c>
       <c r="S37" s="38" t="n">
-        <v>0.004652769989482053</v>
+        <v>0.0006848529828815675</v>
       </c>
       <c r="T37" s="38" t="n">
-        <v>0.006608796472867606</v>
+        <v>0.004670871764716811</v>
       </c>
       <c r="U37" s="23" t="n">
-        <v>0.008002632687771349</v>
+        <v>0.006620960680036703</v>
       </c>
     </row>
     <row r="38">
@@ -3709,7 +3709,7 @@
       </c>
       <c r="N38" s="7" t="inlineStr">
         <is>
-          <t>2025-07-01</t>
+          <t>2025-08-01</t>
         </is>
       </c>
       <c r="O38" s="6" t="inlineStr">
@@ -3723,19 +3723,19 @@
         </is>
       </c>
       <c r="Q38" s="38" t="n">
-        <v>0.01677495823916664</v>
+        <v>0.01509936545139687</v>
       </c>
       <c r="R38" s="38" t="n">
-        <v>0.01945337521746349</v>
+        <v>0.01637547210366313</v>
       </c>
       <c r="S38" s="38" t="n">
-        <v>0.02364811652032663</v>
+        <v>0.019477605517784</v>
       </c>
       <c r="T38" s="38" t="n">
-        <v>0.02825022518521296</v>
+        <v>0.02366620855788388</v>
       </c>
       <c r="U38" s="23" t="n">
-        <v>0.03416667455516736</v>
+        <v>0.02826572083977447</v>
       </c>
     </row>
     <row r="39" ht="31.5" customHeight="1">
@@ -4487,7 +4487,7 @@
       </c>
       <c r="N48" s="7" t="inlineStr">
         <is>
-          <t>2025-10-24</t>
+          <t>2025-10-27</t>
         </is>
       </c>
       <c r="O48" s="6" t="inlineStr">
@@ -4507,13 +4507,13 @@
         <v>3.48</v>
       </c>
       <c r="S48" s="6" t="n">
-        <v>3.45</v>
+        <v>3.48</v>
       </c>
       <c r="T48" s="6" t="n">
         <v>3.45</v>
       </c>
       <c r="U48" s="21" t="n">
-        <v>3.46</v>
+        <v>3.45</v>
       </c>
     </row>
     <row r="49">
@@ -4566,7 +4566,7 @@
       </c>
       <c r="N49" s="7" t="inlineStr">
         <is>
-          <t>2025-10-24</t>
+          <t>2025-10-27</t>
         </is>
       </c>
       <c r="O49" s="6" t="inlineStr">
@@ -4586,13 +4586,13 @@
         <v>3.61</v>
       </c>
       <c r="S49" s="6" t="n">
-        <v>3.56</v>
+        <v>3.61</v>
       </c>
       <c r="T49" s="6" t="n">
         <v>3.56</v>
       </c>
       <c r="U49" s="21" t="n">
-        <v>3.58</v>
+        <v>3.56</v>
       </c>
     </row>
     <row r="50">
@@ -4649,7 +4649,7 @@
       </c>
       <c r="N50" s="7" t="inlineStr">
         <is>
-          <t>2025-10-24</t>
+          <t>2025-10-27</t>
         </is>
       </c>
       <c r="O50" s="6" t="inlineStr">
@@ -4663,19 +4663,19 @@
         </is>
       </c>
       <c r="Q50" s="6" t="n">
+        <v>4.01</v>
+      </c>
+      <c r="R50" s="6" t="n">
         <v>4.02</v>
       </c>
-      <c r="R50" s="6" t="n">
+      <c r="S50" s="6" t="n">
         <v>4.01</v>
       </c>
-      <c r="S50" s="6" t="n">
+      <c r="T50" s="6" t="n">
         <v>3.97</v>
       </c>
-      <c r="T50" s="6" t="n">
+      <c r="U50" s="21" t="n">
         <v>3.98</v>
-      </c>
-      <c r="U50" s="21" t="n">
-        <v>4</v>
       </c>
     </row>
     <row r="51" ht="31.5" customHeight="1">
@@ -4781,7 +4781,7 @@
       </c>
       <c r="N52" s="20" t="inlineStr">
         <is>
-          <t>2025-10-24</t>
+          <t>2025-10-27</t>
         </is>
       </c>
       <c r="O52" s="9" t="inlineStr">
@@ -4795,19 +4795,19 @@
         </is>
       </c>
       <c r="Q52" s="9" t="n">
-        <v>5.67</v>
+        <v>5.64</v>
       </c>
       <c r="R52" s="9" t="n">
         <v>5.67</v>
       </c>
       <c r="S52" s="9" t="n">
+        <v>5.67</v>
+      </c>
+      <c r="T52" s="9" t="n">
         <v>5.66</v>
       </c>
-      <c r="T52" s="9" t="n">
+      <c r="U52" s="22" t="n">
         <v>5.65</v>
-      </c>
-      <c r="U52" s="22" t="n">
-        <v>5.68</v>
       </c>
     </row>
     <row r="53" ht="21" customHeight="1">

</xml_diff>

<commit_message>
Update dashboards - 2025-10-30
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -2990,7 +2990,7 @@
       </c>
       <c r="N29" s="7" t="inlineStr">
         <is>
-          <t>2025-10-28</t>
+          <t>2025-10-29</t>
         </is>
       </c>
       <c r="O29" s="6" t="inlineStr">
@@ -3004,7 +3004,7 @@
         </is>
       </c>
       <c r="Q29" s="6" t="n">
-        <v>2.2</v>
+        <v>2.23</v>
       </c>
       <c r="R29" s="6" t="n">
         <v>2.3</v>
@@ -3073,7 +3073,7 @@
       </c>
       <c r="N30" s="7" t="inlineStr">
         <is>
-          <t>2025-10-28</t>
+          <t>2025-10-29</t>
         </is>
       </c>
       <c r="O30" s="6" t="inlineStr">
@@ -3087,19 +3087,19 @@
         </is>
       </c>
       <c r="Q30" s="6" t="n">
-        <v>2.28</v>
+        <v>2.3</v>
       </c>
       <c r="R30" s="6" t="n">
         <v>2.28</v>
       </c>
       <c r="S30" s="6" t="n">
+        <v>2.28</v>
+      </c>
+      <c r="T30" s="6" t="n">
         <v>2.29</v>
       </c>
-      <c r="T30" s="6" t="n">
+      <c r="U30" s="21" t="n">
         <v>2.3</v>
-      </c>
-      <c r="U30" s="21" t="n">
-        <v>2.29</v>
       </c>
     </row>
     <row r="31">
@@ -4487,7 +4487,7 @@
       </c>
       <c r="N48" s="7" t="inlineStr">
         <is>
-          <t>2025-10-27</t>
+          <t>2025-10-28</t>
         </is>
       </c>
       <c r="O48" s="6" t="inlineStr">
@@ -4501,7 +4501,7 @@
         </is>
       </c>
       <c r="Q48" s="6" t="n">
-        <v>3.48</v>
+        <v>3.47</v>
       </c>
       <c r="R48" s="6" t="n">
         <v>3.48</v>
@@ -4510,7 +4510,7 @@
         <v>3.48</v>
       </c>
       <c r="T48" s="6" t="n">
-        <v>3.45</v>
+        <v>3.48</v>
       </c>
       <c r="U48" s="21" t="n">
         <v>3.45</v>
@@ -4566,7 +4566,7 @@
       </c>
       <c r="N49" s="7" t="inlineStr">
         <is>
-          <t>2025-10-27</t>
+          <t>2025-10-28</t>
         </is>
       </c>
       <c r="O49" s="6" t="inlineStr">
@@ -4580,7 +4580,7 @@
         </is>
       </c>
       <c r="Q49" s="6" t="n">
-        <v>3.61</v>
+        <v>3.6</v>
       </c>
       <c r="R49" s="6" t="n">
         <v>3.61</v>
@@ -4589,7 +4589,7 @@
         <v>3.61</v>
       </c>
       <c r="T49" s="6" t="n">
-        <v>3.56</v>
+        <v>3.61</v>
       </c>
       <c r="U49" s="21" t="n">
         <v>3.56</v>
@@ -4649,7 +4649,7 @@
       </c>
       <c r="N50" s="7" t="inlineStr">
         <is>
-          <t>2025-10-27</t>
+          <t>2025-10-28</t>
         </is>
       </c>
       <c r="O50" s="6" t="inlineStr">
@@ -4663,19 +4663,19 @@
         </is>
       </c>
       <c r="Q50" s="6" t="n">
+        <v>3.99</v>
+      </c>
+      <c r="R50" s="6" t="n">
         <v>4.01</v>
       </c>
-      <c r="R50" s="6" t="n">
+      <c r="S50" s="6" t="n">
         <v>4.02</v>
       </c>
-      <c r="S50" s="6" t="n">
+      <c r="T50" s="6" t="n">
         <v>4.01</v>
       </c>
-      <c r="T50" s="6" t="n">
+      <c r="U50" s="21" t="n">
         <v>3.97</v>
-      </c>
-      <c r="U50" s="21" t="n">
-        <v>3.98</v>
       </c>
     </row>
     <row r="51" ht="31.5" customHeight="1">
@@ -4781,7 +4781,7 @@
       </c>
       <c r="N52" s="20" t="inlineStr">
         <is>
-          <t>2025-10-27</t>
+          <t>2025-10-28</t>
         </is>
       </c>
       <c r="O52" s="9" t="inlineStr">
@@ -4798,16 +4798,16 @@
         <v>5.64</v>
       </c>
       <c r="R52" s="9" t="n">
-        <v>5.67</v>
+        <v>5.64</v>
       </c>
       <c r="S52" s="9" t="n">
         <v>5.67</v>
       </c>
       <c r="T52" s="9" t="n">
+        <v>5.67</v>
+      </c>
+      <c r="U52" s="22" t="n">
         <v>5.66</v>
-      </c>
-      <c r="U52" s="22" t="n">
-        <v>5.65</v>
       </c>
     </row>
     <row r="53" ht="21" customHeight="1">

</xml_diff>

<commit_message>
Update dashboards - 2025-10-31
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -2990,7 +2990,7 @@
       </c>
       <c r="N29" s="7" t="inlineStr">
         <is>
-          <t>2025-10-29</t>
+          <t>2025-10-30</t>
         </is>
       </c>
       <c r="O29" s="6" t="inlineStr">
@@ -3004,7 +3004,7 @@
         </is>
       </c>
       <c r="Q29" s="6" t="n">
-        <v>2.23</v>
+        <v>2.2</v>
       </c>
       <c r="R29" s="6" t="n">
         <v>2.3</v>
@@ -3073,7 +3073,7 @@
       </c>
       <c r="N30" s="7" t="inlineStr">
         <is>
-          <t>2025-10-29</t>
+          <t>2025-10-30</t>
         </is>
       </c>
       <c r="O30" s="6" t="inlineStr">
@@ -3087,19 +3087,19 @@
         </is>
       </c>
       <c r="Q30" s="6" t="n">
+        <v>2.29</v>
+      </c>
+      <c r="R30" s="6" t="n">
         <v>2.3</v>
-      </c>
-      <c r="R30" s="6" t="n">
-        <v>2.28</v>
       </c>
       <c r="S30" s="6" t="n">
         <v>2.28</v>
       </c>
       <c r="T30" s="6" t="n">
+        <v>2.28</v>
+      </c>
+      <c r="U30" s="21" t="n">
         <v>2.29</v>
-      </c>
-      <c r="U30" s="21" t="n">
-        <v>2.3</v>
       </c>
     </row>
     <row r="31">
@@ -4487,7 +4487,7 @@
       </c>
       <c r="N48" s="7" t="inlineStr">
         <is>
-          <t>2025-10-28</t>
+          <t>2025-10-29</t>
         </is>
       </c>
       <c r="O48" s="6" t="inlineStr">
@@ -4501,10 +4501,10 @@
         </is>
       </c>
       <c r="Q48" s="6" t="n">
+        <v>3.59</v>
+      </c>
+      <c r="R48" s="6" t="n">
         <v>3.47</v>
-      </c>
-      <c r="R48" s="6" t="n">
-        <v>3.48</v>
       </c>
       <c r="S48" s="6" t="n">
         <v>3.48</v>
@@ -4513,7 +4513,7 @@
         <v>3.48</v>
       </c>
       <c r="U48" s="21" t="n">
-        <v>3.45</v>
+        <v>3.48</v>
       </c>
     </row>
     <row r="49">
@@ -4566,7 +4566,7 @@
       </c>
       <c r="N49" s="7" t="inlineStr">
         <is>
-          <t>2025-10-28</t>
+          <t>2025-10-29</t>
         </is>
       </c>
       <c r="O49" s="6" t="inlineStr">
@@ -4580,10 +4580,10 @@
         </is>
       </c>
       <c r="Q49" s="6" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="R49" s="6" t="n">
         <v>3.6</v>
-      </c>
-      <c r="R49" s="6" t="n">
-        <v>3.61</v>
       </c>
       <c r="S49" s="6" t="n">
         <v>3.61</v>
@@ -4592,7 +4592,7 @@
         <v>3.61</v>
       </c>
       <c r="U49" s="21" t="n">
-        <v>3.56</v>
+        <v>3.61</v>
       </c>
     </row>
     <row r="50">
@@ -4649,7 +4649,7 @@
       </c>
       <c r="N50" s="7" t="inlineStr">
         <is>
-          <t>2025-10-28</t>
+          <t>2025-10-29</t>
         </is>
       </c>
       <c r="O50" s="6" t="inlineStr">
@@ -4663,19 +4663,19 @@
         </is>
       </c>
       <c r="Q50" s="6" t="n">
+        <v>4.08</v>
+      </c>
+      <c r="R50" s="6" t="n">
         <v>3.99</v>
       </c>
-      <c r="R50" s="6" t="n">
+      <c r="S50" s="6" t="n">
         <v>4.01</v>
       </c>
-      <c r="S50" s="6" t="n">
+      <c r="T50" s="6" t="n">
         <v>4.02</v>
       </c>
-      <c r="T50" s="6" t="n">
+      <c r="U50" s="21" t="n">
         <v>4.01</v>
-      </c>
-      <c r="U50" s="21" t="n">
-        <v>3.97</v>
       </c>
     </row>
     <row r="51" ht="31.5" customHeight="1">
@@ -4728,7 +4728,7 @@
       </c>
       <c r="N51" s="7" t="inlineStr">
         <is>
-          <t>2025-10-23</t>
+          <t>2025-10-30</t>
         </is>
       </c>
       <c r="O51" s="6" t="inlineStr">
@@ -4742,19 +4742,19 @@
         </is>
       </c>
       <c r="Q51" s="6" t="n">
+        <v>6.17</v>
+      </c>
+      <c r="R51" s="6" t="n">
         <v>6.19</v>
       </c>
-      <c r="R51" s="6" t="n">
+      <c r="S51" s="6" t="n">
         <v>6.27</v>
       </c>
-      <c r="S51" s="6" t="n">
+      <c r="T51" s="6" t="n">
         <v>6.3</v>
       </c>
-      <c r="T51" s="6" t="n">
+      <c r="U51" s="21" t="n">
         <v>6.34</v>
-      </c>
-      <c r="U51" s="21" t="n">
-        <v>6.3</v>
       </c>
     </row>
     <row r="52" ht="16.15" customHeight="1" thickBot="1">
@@ -4781,7 +4781,7 @@
       </c>
       <c r="N52" s="20" t="inlineStr">
         <is>
-          <t>2025-10-28</t>
+          <t>2025-10-29</t>
         </is>
       </c>
       <c r="O52" s="9" t="inlineStr">
@@ -4795,19 +4795,19 @@
         </is>
       </c>
       <c r="Q52" s="9" t="n">
-        <v>5.64</v>
+        <v>5.69</v>
       </c>
       <c r="R52" s="9" t="n">
         <v>5.64</v>
       </c>
       <c r="S52" s="9" t="n">
-        <v>5.67</v>
+        <v>5.64</v>
       </c>
       <c r="T52" s="9" t="n">
         <v>5.67</v>
       </c>
       <c r="U52" s="22" t="n">
-        <v>5.66</v>
+        <v>5.67</v>
       </c>
     </row>
     <row r="53" ht="21" customHeight="1">

</xml_diff>

<commit_message>
Update dashboards - 2025-11-01
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -2990,7 +2990,7 @@
       </c>
       <c r="N29" s="7" t="inlineStr">
         <is>
-          <t>2025-10-30</t>
+          <t>2025-10-31</t>
         </is>
       </c>
       <c r="O29" s="6" t="inlineStr">
@@ -3073,7 +3073,7 @@
       </c>
       <c r="N30" s="7" t="inlineStr">
         <is>
-          <t>2025-10-30</t>
+          <t>2025-10-31</t>
         </is>
       </c>
       <c r="O30" s="6" t="inlineStr">
@@ -3087,19 +3087,19 @@
         </is>
       </c>
       <c r="Q30" s="6" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="R30" s="6" t="n">
         <v>2.29</v>
       </c>
-      <c r="R30" s="6" t="n">
+      <c r="S30" s="6" t="n">
         <v>2.3</v>
-      </c>
-      <c r="S30" s="6" t="n">
-        <v>2.28</v>
       </c>
       <c r="T30" s="6" t="n">
         <v>2.28</v>
       </c>
       <c r="U30" s="21" t="n">
-        <v>2.29</v>
+        <v>2.28</v>
       </c>
     </row>
     <row r="31">
@@ -4487,7 +4487,7 @@
       </c>
       <c r="N48" s="7" t="inlineStr">
         <is>
-          <t>2025-10-29</t>
+          <t>2025-10-30</t>
         </is>
       </c>
       <c r="O48" s="6" t="inlineStr">
@@ -4501,13 +4501,13 @@
         </is>
       </c>
       <c r="Q48" s="6" t="n">
+        <v>3.61</v>
+      </c>
+      <c r="R48" s="6" t="n">
         <v>3.59</v>
       </c>
-      <c r="R48" s="6" t="n">
+      <c r="S48" s="6" t="n">
         <v>3.47</v>
-      </c>
-      <c r="S48" s="6" t="n">
-        <v>3.48</v>
       </c>
       <c r="T48" s="6" t="n">
         <v>3.48</v>
@@ -4566,7 +4566,7 @@
       </c>
       <c r="N49" s="7" t="inlineStr">
         <is>
-          <t>2025-10-29</t>
+          <t>2025-10-30</t>
         </is>
       </c>
       <c r="O49" s="6" t="inlineStr">
@@ -4580,13 +4580,13 @@
         </is>
       </c>
       <c r="Q49" s="6" t="n">
+        <v>3.72</v>
+      </c>
+      <c r="R49" s="6" t="n">
         <v>3.7</v>
       </c>
-      <c r="R49" s="6" t="n">
+      <c r="S49" s="6" t="n">
         <v>3.6</v>
-      </c>
-      <c r="S49" s="6" t="n">
-        <v>3.61</v>
       </c>
       <c r="T49" s="6" t="n">
         <v>3.61</v>
@@ -4649,7 +4649,7 @@
       </c>
       <c r="N50" s="7" t="inlineStr">
         <is>
-          <t>2025-10-29</t>
+          <t>2025-10-30</t>
         </is>
       </c>
       <c r="O50" s="6" t="inlineStr">
@@ -4663,19 +4663,19 @@
         </is>
       </c>
       <c r="Q50" s="6" t="n">
+        <v>4.11</v>
+      </c>
+      <c r="R50" s="6" t="n">
         <v>4.08</v>
       </c>
-      <c r="R50" s="6" t="n">
+      <c r="S50" s="6" t="n">
         <v>3.99</v>
       </c>
-      <c r="S50" s="6" t="n">
+      <c r="T50" s="6" t="n">
         <v>4.01</v>
       </c>
-      <c r="T50" s="6" t="n">
+      <c r="U50" s="21" t="n">
         <v>4.02</v>
-      </c>
-      <c r="U50" s="21" t="n">
-        <v>4.01</v>
       </c>
     </row>
     <row r="51" ht="31.5" customHeight="1">
@@ -4781,7 +4781,7 @@
       </c>
       <c r="N52" s="20" t="inlineStr">
         <is>
-          <t>2025-10-29</t>
+          <t>2025-10-30</t>
         </is>
       </c>
       <c r="O52" s="9" t="inlineStr">
@@ -4795,16 +4795,16 @@
         </is>
       </c>
       <c r="Q52" s="9" t="n">
+        <v>5.75</v>
+      </c>
+      <c r="R52" s="9" t="n">
         <v>5.69</v>
-      </c>
-      <c r="R52" s="9" t="n">
-        <v>5.64</v>
       </c>
       <c r="S52" s="9" t="n">
         <v>5.64</v>
       </c>
       <c r="T52" s="9" t="n">
-        <v>5.67</v>
+        <v>5.64</v>
       </c>
       <c r="U52" s="22" t="n">
         <v>5.67</v>

</xml_diff>

<commit_message>
Change FedFund to DFF
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -706,10 +706,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:U93"/>
+  <dimension ref="A1:U80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="51" workbookViewId="0">
-      <selection activeCell="M26" sqref="M26"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="104" zoomScaleNormal="51" workbookViewId="0">
+      <selection activeCell="O43" sqref="O43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9.1328125" defaultRowHeight="15.75"/>
@@ -2990,7 +2990,7 @@
       </c>
       <c r="N29" s="7" t="inlineStr">
         <is>
-          <t>2025-10-31</t>
+          <t>2025-11-03</t>
         </is>
       </c>
       <c r="O29" s="6" t="inlineStr">
@@ -3004,19 +3004,19 @@
         </is>
       </c>
       <c r="Q29" s="6" t="n">
+        <v>2.21</v>
+      </c>
+      <c r="R29" s="6" t="n">
         <v>2.2</v>
       </c>
-      <c r="R29" s="6" t="n">
+      <c r="S29" s="6" t="n">
         <v>2.3</v>
       </c>
-      <c r="S29" s="6" t="n">
+      <c r="T29" s="6" t="n">
         <v>2.35</v>
       </c>
-      <c r="T29" s="6" t="n">
+      <c r="U29" s="21" t="n">
         <v>2.32</v>
-      </c>
-      <c r="U29" s="21" t="n">
-        <v>2.27</v>
       </c>
     </row>
     <row r="30">
@@ -3073,7 +3073,7 @@
       </c>
       <c r="N30" s="7" t="inlineStr">
         <is>
-          <t>2025-10-31</t>
+          <t>2025-11-03</t>
         </is>
       </c>
       <c r="O30" s="6" t="inlineStr">
@@ -3087,16 +3087,16 @@
         </is>
       </c>
       <c r="Q30" s="6" t="n">
+        <v>2.31</v>
+      </c>
+      <c r="R30" s="6" t="n">
         <v>2.3</v>
       </c>
-      <c r="R30" s="6" t="n">
+      <c r="S30" s="6" t="n">
         <v>2.29</v>
       </c>
-      <c r="S30" s="6" t="n">
+      <c r="T30" s="6" t="n">
         <v>2.3</v>
-      </c>
-      <c r="T30" s="6" t="n">
-        <v>2.28</v>
       </c>
       <c r="U30" s="21" t="n">
         <v>2.28</v>
@@ -3788,7 +3788,7 @@
       </c>
       <c r="N39" s="7" t="inlineStr">
         <is>
-          <t>2025-10-24</t>
+          <t>2025-10-31</t>
         </is>
       </c>
       <c r="O39" s="6" t="inlineStr">
@@ -3802,19 +3802,19 @@
         </is>
       </c>
       <c r="Q39" s="6" t="n">
-        <v>121.342</v>
+        <v>121.7715</v>
       </c>
       <c r="R39" s="6" t="n">
-        <v>121.3633</v>
+        <v>121.665</v>
       </c>
       <c r="S39" s="6" t="n">
-        <v>121.3075</v>
+        <v>120.929</v>
       </c>
       <c r="T39" s="6" t="n">
-        <v>121.302</v>
+        <v>121.0349</v>
       </c>
       <c r="U39" s="21" t="n">
-        <v>121.0394</v>
+        <v>121.2002</v>
       </c>
     </row>
     <row r="40">
@@ -3867,7 +3867,7 @@
       </c>
       <c r="N40" s="7" t="inlineStr">
         <is>
-          <t>2025-10-24</t>
+          <t>2025-10-31</t>
         </is>
       </c>
       <c r="O40" s="6" t="inlineStr">
@@ -3881,7 +3881,7 @@
         </is>
       </c>
       <c r="Q40" s="38" t="n">
-        <v>-0.02945577953796328</v>
+        <v>-0.02602045835742851</v>
       </c>
       <c r="R40" s="38" t="n">
         <v>-0.007960187542479276</v>
@@ -4399,12 +4399,12 @@
       </c>
       <c r="M47" s="15" t="inlineStr">
         <is>
-          <t>FEDFUNDS</t>
+          <t>DFF</t>
         </is>
       </c>
       <c r="N47" s="7" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-10-31</t>
         </is>
       </c>
       <c r="O47" s="6" t="inlineStr">
@@ -4414,23 +4414,23 @@
       </c>
       <c r="P47" s="6" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>D</t>
         </is>
       </c>
       <c r="Q47" s="6" t="n">
-        <v>4.22</v>
+        <v>3.86</v>
       </c>
       <c r="R47" s="6" t="n">
-        <v>4.33</v>
+        <v>3.87</v>
       </c>
       <c r="S47" s="6" t="n">
-        <v>4.33</v>
+        <v>4.12</v>
       </c>
       <c r="T47" s="6" t="n">
-        <v>4.33</v>
+        <v>4.12</v>
       </c>
       <c r="U47" s="21" t="n">
-        <v>4.33</v>
+        <v>4.12</v>
       </c>
     </row>
     <row r="48">
@@ -4487,7 +4487,7 @@
       </c>
       <c r="N48" s="7" t="inlineStr">
         <is>
-          <t>2025-10-30</t>
+          <t>2025-10-31</t>
         </is>
       </c>
       <c r="O48" s="6" t="inlineStr">
@@ -4501,16 +4501,16 @@
         </is>
       </c>
       <c r="Q48" s="6" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="R48" s="6" t="n">
         <v>3.61</v>
       </c>
-      <c r="R48" s="6" t="n">
+      <c r="S48" s="6" t="n">
         <v>3.59</v>
       </c>
-      <c r="S48" s="6" t="n">
+      <c r="T48" s="6" t="n">
         <v>3.47</v>
-      </c>
-      <c r="T48" s="6" t="n">
-        <v>3.48</v>
       </c>
       <c r="U48" s="21" t="n">
         <v>3.48</v>
@@ -4566,7 +4566,7 @@
       </c>
       <c r="N49" s="7" t="inlineStr">
         <is>
-          <t>2025-10-30</t>
+          <t>2025-10-31</t>
         </is>
       </c>
       <c r="O49" s="6" t="inlineStr">
@@ -4580,16 +4580,16 @@
         </is>
       </c>
       <c r="Q49" s="6" t="n">
+        <v>3.71</v>
+      </c>
+      <c r="R49" s="6" t="n">
         <v>3.72</v>
       </c>
-      <c r="R49" s="6" t="n">
+      <c r="S49" s="6" t="n">
         <v>3.7</v>
       </c>
-      <c r="S49" s="6" t="n">
+      <c r="T49" s="6" t="n">
         <v>3.6</v>
-      </c>
-      <c r="T49" s="6" t="n">
-        <v>3.61</v>
       </c>
       <c r="U49" s="21" t="n">
         <v>3.61</v>
@@ -4649,7 +4649,7 @@
       </c>
       <c r="N50" s="7" t="inlineStr">
         <is>
-          <t>2025-10-30</t>
+          <t>2025-10-31</t>
         </is>
       </c>
       <c r="O50" s="6" t="inlineStr">
@@ -4666,16 +4666,16 @@
         <v>4.11</v>
       </c>
       <c r="R50" s="6" t="n">
+        <v>4.11</v>
+      </c>
+      <c r="S50" s="6" t="n">
         <v>4.08</v>
       </c>
-      <c r="S50" s="6" t="n">
+      <c r="T50" s="6" t="n">
         <v>3.99</v>
       </c>
-      <c r="T50" s="6" t="n">
+      <c r="U50" s="21" t="n">
         <v>4.01</v>
-      </c>
-      <c r="U50" s="21" t="n">
-        <v>4.02</v>
       </c>
     </row>
     <row r="51" ht="31.5" customHeight="1">
@@ -4781,7 +4781,7 @@
       </c>
       <c r="N52" s="20" t="inlineStr">
         <is>
-          <t>2025-10-30</t>
+          <t>2025-10-31</t>
         </is>
       </c>
       <c r="O52" s="9" t="inlineStr">
@@ -4795,19 +4795,19 @@
         </is>
       </c>
       <c r="Q52" s="9" t="n">
+        <v>5.8</v>
+      </c>
+      <c r="R52" s="9" t="n">
         <v>5.75</v>
       </c>
-      <c r="R52" s="9" t="n">
+      <c r="S52" s="9" t="n">
         <v>5.69</v>
-      </c>
-      <c r="S52" s="9" t="n">
-        <v>5.64</v>
       </c>
       <c r="T52" s="9" t="n">
         <v>5.64</v>
       </c>
       <c r="U52" s="22" t="n">
-        <v>5.67</v>
+        <v>5.64</v>
       </c>
     </row>
     <row r="53" ht="21" customHeight="1">
@@ -4922,36 +4922,6 @@
     <row r="80">
       <c r="A80" s="4" t="n"/>
     </row>
-    <row r="81"/>
-    <row r="82"/>
-    <row r="83"/>
-    <row r="84"/>
-    <row r="85"/>
-    <row r="86"/>
-    <row r="87"/>
-    <row r="88"/>
-    <row r="89">
-      <c r="A89" s="30" t="inlineStr">
-        <is>
-          <t>GDP</t>
-        </is>
-      </c>
-      <c r="F89" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Inflation </t>
-        </is>
-      </c>
-    </row>
-    <row r="90"/>
-    <row r="91"/>
-    <row r="92"/>
-    <row r="93">
-      <c r="A93" s="30" t="inlineStr">
-        <is>
-          <t>Philly Fed</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:U1"/>

</xml_diff>

<commit_message>
Update dashboards - 2025-11-04
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -2884,10 +2884,10 @@
         </is>
       </c>
       <c r="F28" s="25" t="n">
-        <v>0.0292251268148207</v>
+        <v>0.02933036907051223</v>
       </c>
       <c r="G28" s="25" t="n">
-        <v>-0.02746655290430811</v>
+        <v>-0.02756598804853716</v>
       </c>
       <c r="H28" s="25" t="n">
         <v>-0.09389977010425232</v>
@@ -2966,7 +2966,7 @@
         <v>0.07634016956050854</v>
       </c>
       <c r="G29" s="25" t="n">
-        <v>0.03397968857635882</v>
+        <v>0.03387397095834726</v>
       </c>
       <c r="H29" s="25" t="n">
         <v>0.1089645997552716</v>
@@ -3046,10 +3046,10 @@
         </is>
       </c>
       <c r="F30" s="25" t="n">
-        <v>0.01923414103867871</v>
+        <v>0.02037556476894942</v>
       </c>
       <c r="G30" s="25" t="n">
-        <v>-0.02348739337531547</v>
+        <v>-0.02457975064120344</v>
       </c>
       <c r="H30" s="25" t="n">
         <v>-0.09442194506291901</v>
@@ -3128,7 +3128,7 @@
         <v>0.06748567650947554</v>
       </c>
       <c r="G31" s="25" t="n">
-        <v>0.03352046419083723</v>
+        <v>0.03236433616868596</v>
       </c>
       <c r="H31" s="25" t="n">
         <v>0.1029410098461701</v>

</xml_diff>

<commit_message>
Update dashboards - 2025-11-05
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -1210,7 +1210,7 @@
         </is>
       </c>
       <c r="F7" s="25" t="n">
-        <v>0.352997932460372</v>
+        <v>0.3747070985527221</v>
       </c>
       <c r="G7" s="25" t="n">
         <v>-2.062303243282817</v>
@@ -2990,7 +2990,7 @@
       </c>
       <c r="N29" s="7" t="inlineStr">
         <is>
-          <t>2025-11-03</t>
+          <t>2025-11-04</t>
         </is>
       </c>
       <c r="O29" s="6" t="inlineStr">
@@ -3004,7 +3004,7 @@
         </is>
       </c>
       <c r="Q29" s="6" t="n">
-        <v>2.21</v>
+        <v>2.2</v>
       </c>
       <c r="R29" s="6" t="n">
         <v>2.2</v>
@@ -3073,7 +3073,7 @@
       </c>
       <c r="N30" s="7" t="inlineStr">
         <is>
-          <t>2025-11-03</t>
+          <t>2025-11-04</t>
         </is>
       </c>
       <c r="O30" s="6" t="inlineStr">
@@ -3087,19 +3087,19 @@
         </is>
       </c>
       <c r="Q30" s="6" t="n">
+        <v>2.29</v>
+      </c>
+      <c r="R30" s="6" t="n">
         <v>2.31</v>
       </c>
-      <c r="R30" s="6" t="n">
+      <c r="S30" s="6" t="n">
+        <v/>
+      </c>
+      <c r="T30" s="6" t="n">
+        <v/>
+      </c>
+      <c r="U30" s="21" t="n">
         <v>2.3</v>
-      </c>
-      <c r="S30" s="6" t="n">
-        <v>2.29</v>
-      </c>
-      <c r="T30" s="6" t="n">
-        <v>2.3</v>
-      </c>
-      <c r="U30" s="21" t="n">
-        <v>2.28</v>
       </c>
     </row>
     <row r="31">
@@ -4404,7 +4404,7 @@
       </c>
       <c r="N47" s="7" t="inlineStr">
         <is>
-          <t>2025-10-31</t>
+          <t>2025-11-03</t>
         </is>
       </c>
       <c r="O47" s="6" t="inlineStr">
@@ -4418,19 +4418,19 @@
         </is>
       </c>
       <c r="Q47" s="6" t="n">
+        <v>3.87</v>
+      </c>
+      <c r="R47" s="6" t="n">
         <v>3.86</v>
       </c>
-      <c r="R47" s="6" t="n">
+      <c r="S47" s="6" t="n">
+        <v>3.86</v>
+      </c>
+      <c r="T47" s="6" t="n">
+        <v>3.86</v>
+      </c>
+      <c r="U47" s="21" t="n">
         <v>3.87</v>
-      </c>
-      <c r="S47" s="6" t="n">
-        <v>4.12</v>
-      </c>
-      <c r="T47" s="6" t="n">
-        <v>4.12</v>
-      </c>
-      <c r="U47" s="21" t="n">
-        <v>4.12</v>
       </c>
     </row>
     <row r="48">
@@ -4487,7 +4487,7 @@
       </c>
       <c r="N48" s="7" t="inlineStr">
         <is>
-          <t>2025-10-31</t>
+          <t>2025-11-03</t>
         </is>
       </c>
       <c r="O48" s="6" t="inlineStr">
@@ -4504,16 +4504,16 @@
         <v>3.6</v>
       </c>
       <c r="R48" s="6" t="n">
+        <v/>
+      </c>
+      <c r="S48" s="6" t="n">
+        <v/>
+      </c>
+      <c r="T48" s="6" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="U48" s="21" t="n">
         <v>3.61</v>
-      </c>
-      <c r="S48" s="6" t="n">
-        <v>3.59</v>
-      </c>
-      <c r="T48" s="6" t="n">
-        <v>3.47</v>
-      </c>
-      <c r="U48" s="21" t="n">
-        <v>3.48</v>
       </c>
     </row>
     <row r="49">
@@ -4566,7 +4566,7 @@
       </c>
       <c r="N49" s="7" t="inlineStr">
         <is>
-          <t>2025-10-31</t>
+          <t>2025-11-03</t>
         </is>
       </c>
       <c r="O49" s="6" t="inlineStr">
@@ -4580,19 +4580,19 @@
         </is>
       </c>
       <c r="Q49" s="6" t="n">
+        <v>3.72</v>
+      </c>
+      <c r="R49" s="6" t="n">
+        <v/>
+      </c>
+      <c r="S49" s="6" t="n">
+        <v/>
+      </c>
+      <c r="T49" s="6" t="n">
         <v>3.71</v>
       </c>
-      <c r="R49" s="6" t="n">
+      <c r="U49" s="21" t="n">
         <v>3.72</v>
-      </c>
-      <c r="S49" s="6" t="n">
-        <v>3.7</v>
-      </c>
-      <c r="T49" s="6" t="n">
-        <v>3.6</v>
-      </c>
-      <c r="U49" s="21" t="n">
-        <v>3.61</v>
       </c>
     </row>
     <row r="50">
@@ -4649,7 +4649,7 @@
       </c>
       <c r="N50" s="7" t="inlineStr">
         <is>
-          <t>2025-10-31</t>
+          <t>2025-11-03</t>
         </is>
       </c>
       <c r="O50" s="6" t="inlineStr">
@@ -4663,19 +4663,19 @@
         </is>
       </c>
       <c r="Q50" s="6" t="n">
+        <v>4.13</v>
+      </c>
+      <c r="R50" s="6" t="n">
+        <v/>
+      </c>
+      <c r="S50" s="6" t="n">
+        <v/>
+      </c>
+      <c r="T50" s="6" t="n">
         <v>4.11</v>
       </c>
-      <c r="R50" s="6" t="n">
+      <c r="U50" s="21" t="n">
         <v>4.11</v>
-      </c>
-      <c r="S50" s="6" t="n">
-        <v>4.08</v>
-      </c>
-      <c r="T50" s="6" t="n">
-        <v>3.99</v>
-      </c>
-      <c r="U50" s="21" t="n">
-        <v>4.01</v>
       </c>
     </row>
     <row r="51" ht="31.5" customHeight="1">
@@ -4781,7 +4781,7 @@
       </c>
       <c r="N52" s="20" t="inlineStr">
         <is>
-          <t>2025-10-31</t>
+          <t>2025-11-03</t>
         </is>
       </c>
       <c r="O52" s="9" t="inlineStr">
@@ -4795,19 +4795,19 @@
         </is>
       </c>
       <c r="Q52" s="9" t="n">
+        <v>5.84</v>
+      </c>
+      <c r="R52" s="9" t="n">
+        <v/>
+      </c>
+      <c r="S52" s="9" t="n">
+        <v/>
+      </c>
+      <c r="T52" s="9" t="n">
         <v>5.8</v>
       </c>
-      <c r="R52" s="9" t="n">
+      <c r="U52" s="22" t="n">
         <v>5.75</v>
-      </c>
-      <c r="S52" s="9" t="n">
-        <v>5.69</v>
-      </c>
-      <c r="T52" s="9" t="n">
-        <v>5.64</v>
-      </c>
-      <c r="U52" s="22" t="n">
-        <v>5.64</v>
       </c>
     </row>
     <row r="53" ht="21" customHeight="1">

</xml_diff>

<commit_message>
Update dashboards - 2025-11-06
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -1075,7 +1075,7 @@
       </c>
       <c r="N5" s="7" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="O5" s="6" t="inlineStr">
@@ -1089,19 +1089,19 @@
         </is>
       </c>
       <c r="Q5" s="24" t="n">
-        <v>-32000</v>
+        <v>42000</v>
       </c>
       <c r="R5" s="24" t="n">
+        <v>-29000</v>
+      </c>
+      <c r="S5" s="24" t="n">
         <v>-3000</v>
       </c>
-      <c r="S5" s="24" t="n">
+      <c r="T5" s="24" t="n">
         <v>104000</v>
       </c>
-      <c r="T5" s="24" t="n">
+      <c r="U5" s="26" t="n">
         <v>-23000</v>
-      </c>
-      <c r="U5" s="26" t="n">
-        <v>29000</v>
       </c>
     </row>
     <row r="6">
@@ -2990,7 +2990,7 @@
       </c>
       <c r="N29" s="7" t="inlineStr">
         <is>
-          <t>2025-11-04</t>
+          <t>2025-11-05</t>
         </is>
       </c>
       <c r="O29" s="6" t="inlineStr">
@@ -3004,7 +3004,7 @@
         </is>
       </c>
       <c r="Q29" s="6" t="n">
-        <v>2.2</v>
+        <v>2.21</v>
       </c>
       <c r="R29" s="6" t="n">
         <v>2.2</v>
@@ -3046,10 +3046,10 @@
         </is>
       </c>
       <c r="F30" s="25" t="n">
-        <v>0.02037556476894942</v>
+        <v>0.01923414103867871</v>
       </c>
       <c r="G30" s="25" t="n">
-        <v>-0.02457975064120344</v>
+        <v>-0.02348739337531547</v>
       </c>
       <c r="H30" s="25" t="n">
         <v>-0.09442194506291901</v>
@@ -3073,7 +3073,7 @@
       </c>
       <c r="N30" s="7" t="inlineStr">
         <is>
-          <t>2025-11-04</t>
+          <t>2025-11-05</t>
         </is>
       </c>
       <c r="O30" s="6" t="inlineStr">
@@ -3087,19 +3087,19 @@
         </is>
       </c>
       <c r="Q30" s="6" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="R30" s="6" t="n">
         <v>2.29</v>
       </c>
-      <c r="R30" s="6" t="n">
+      <c r="S30" s="6" t="n">
         <v>2.31</v>
-      </c>
-      <c r="S30" s="6" t="n">
-        <v/>
       </c>
       <c r="T30" s="6" t="n">
         <v/>
       </c>
       <c r="U30" s="21" t="n">
-        <v>2.3</v>
+        <v/>
       </c>
     </row>
     <row r="31">
@@ -3128,7 +3128,7 @@
         <v>0.06748567650947554</v>
       </c>
       <c r="G31" s="25" t="n">
-        <v>0.03236433616868596</v>
+        <v>0.03352046419083723</v>
       </c>
       <c r="H31" s="25" t="n">
         <v>0.1029410098461701</v>
@@ -4404,7 +4404,7 @@
       </c>
       <c r="N47" s="7" t="inlineStr">
         <is>
-          <t>2025-11-03</t>
+          <t>2025-11-04</t>
         </is>
       </c>
       <c r="O47" s="6" t="inlineStr">
@@ -4421,7 +4421,7 @@
         <v>3.87</v>
       </c>
       <c r="R47" s="6" t="n">
-        <v>3.86</v>
+        <v>3.87</v>
       </c>
       <c r="S47" s="6" t="n">
         <v>3.86</v>
@@ -4430,7 +4430,7 @@
         <v>3.86</v>
       </c>
       <c r="U47" s="21" t="n">
-        <v>3.87</v>
+        <v>3.86</v>
       </c>
     </row>
     <row r="48">
@@ -4487,7 +4487,7 @@
       </c>
       <c r="N48" s="7" t="inlineStr">
         <is>
-          <t>2025-11-03</t>
+          <t>2025-11-04</t>
         </is>
       </c>
       <c r="O48" s="6" t="inlineStr">
@@ -4501,19 +4501,19 @@
         </is>
       </c>
       <c r="Q48" s="6" t="n">
+        <v>3.58</v>
+      </c>
+      <c r="R48" s="6" t="n">
         <v>3.6</v>
-      </c>
-      <c r="R48" s="6" t="n">
-        <v/>
       </c>
       <c r="S48" s="6" t="n">
         <v/>
       </c>
       <c r="T48" s="6" t="n">
+        <v/>
+      </c>
+      <c r="U48" s="21" t="n">
         <v>3.6</v>
-      </c>
-      <c r="U48" s="21" t="n">
-        <v>3.61</v>
       </c>
     </row>
     <row r="49">
@@ -4566,7 +4566,7 @@
       </c>
       <c r="N49" s="7" t="inlineStr">
         <is>
-          <t>2025-11-03</t>
+          <t>2025-11-04</t>
         </is>
       </c>
       <c r="O49" s="6" t="inlineStr">
@@ -4580,19 +4580,19 @@
         </is>
       </c>
       <c r="Q49" s="6" t="n">
+        <v>3.69</v>
+      </c>
+      <c r="R49" s="6" t="n">
         <v>3.72</v>
-      </c>
-      <c r="R49" s="6" t="n">
-        <v/>
       </c>
       <c r="S49" s="6" t="n">
         <v/>
       </c>
       <c r="T49" s="6" t="n">
+        <v/>
+      </c>
+      <c r="U49" s="21" t="n">
         <v>3.71</v>
-      </c>
-      <c r="U49" s="21" t="n">
-        <v>3.72</v>
       </c>
     </row>
     <row r="50">
@@ -4649,7 +4649,7 @@
       </c>
       <c r="N50" s="7" t="inlineStr">
         <is>
-          <t>2025-11-03</t>
+          <t>2025-11-04</t>
         </is>
       </c>
       <c r="O50" s="6" t="inlineStr">
@@ -4663,16 +4663,16 @@
         </is>
       </c>
       <c r="Q50" s="6" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="R50" s="6" t="n">
         <v>4.13</v>
-      </c>
-      <c r="R50" s="6" t="n">
-        <v/>
       </c>
       <c r="S50" s="6" t="n">
         <v/>
       </c>
       <c r="T50" s="6" t="n">
-        <v>4.11</v>
+        <v/>
       </c>
       <c r="U50" s="21" t="n">
         <v>4.11</v>
@@ -4781,7 +4781,7 @@
       </c>
       <c r="N52" s="20" t="inlineStr">
         <is>
-          <t>2025-11-03</t>
+          <t>2025-11-04</t>
         </is>
       </c>
       <c r="O52" s="9" t="inlineStr">
@@ -4795,19 +4795,19 @@
         </is>
       </c>
       <c r="Q52" s="9" t="n">
+        <v>5.82</v>
+      </c>
+      <c r="R52" s="9" t="n">
         <v>5.84</v>
-      </c>
-      <c r="R52" s="9" t="n">
-        <v/>
       </c>
       <c r="S52" s="9" t="n">
         <v/>
       </c>
       <c r="T52" s="9" t="n">
+        <v/>
+      </c>
+      <c r="U52" s="22" t="n">
         <v>5.8</v>
-      </c>
-      <c r="U52" s="22" t="n">
-        <v>5.75</v>
       </c>
     </row>
     <row r="53" ht="21" customHeight="1">

</xml_diff>

<commit_message>
Update dashboards - 2025-11-08
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -2480,8 +2480,8 @@
           <t>REVOLSL</t>
         </is>
       </c>
-      <c r="C24" s="47" t="n">
-        <v>45870</v>
+      <c r="C24" s="48" t="n">
+        <v>45901</v>
       </c>
       <c r="D24" s="6" t="inlineStr">
         <is>
@@ -2494,19 +2494,19 @@
         </is>
       </c>
       <c r="F24" s="38" t="n">
-        <v>-0.004542917878486374</v>
+        <v>0.001263881152865798</v>
       </c>
       <c r="G24" s="38" t="n">
-        <v>0.008590832174939722</v>
+        <v>-0.004631607864557297</v>
       </c>
       <c r="H24" s="38" t="n">
+        <v>0.008466932005238847</v>
+      </c>
+      <c r="I24" s="38" t="n">
         <v>7.468713370495372e-05</v>
       </c>
-      <c r="I24" s="38" t="n">
+      <c r="J24" s="38" t="n">
         <v>-0.0009803765564608824</v>
-      </c>
-      <c r="J24" s="38" t="n">
-        <v>0.005427299254220141</v>
       </c>
       <c r="K24" s="5" t="n"/>
       <c r="L24" s="28" t="inlineStr">
@@ -2559,8 +2559,8 @@
           <t>NONREVSL</t>
         </is>
       </c>
-      <c r="C25" s="47" t="n">
-        <v>45870</v>
+      <c r="C25" s="48" t="n">
+        <v>45901</v>
       </c>
       <c r="D25" s="6" t="inlineStr">
         <is>
@@ -2573,19 +2573,19 @@
         </is>
       </c>
       <c r="F25" s="38" t="n">
-        <v>0.001685970567310902</v>
+        <v>0.003044704234780982</v>
       </c>
       <c r="G25" s="38" t="n">
-        <v>0.001838981658635941</v>
+        <v>0.002454000808095547</v>
       </c>
       <c r="H25" s="38" t="n">
-        <v>-0.001267905126547064</v>
+        <v>0.001792092542795443</v>
       </c>
       <c r="I25" s="38" t="n">
-        <v>0.002438560801034662</v>
+        <v>-0.001282602659991805</v>
       </c>
       <c r="J25" s="38" t="n">
-        <v>0.002617969891309135</v>
+        <v>0.002439153249045978</v>
       </c>
       <c r="K25" s="5" t="n"/>
       <c r="L25" s="28" t="n"/>
@@ -2903,7 +2903,7 @@
         </is>
       </c>
       <c r="N29" s="48" t="n">
-        <v>45967</v>
+        <v>45968</v>
       </c>
       <c r="O29" s="6" t="inlineStr">
         <is>
@@ -2916,19 +2916,19 @@
         </is>
       </c>
       <c r="Q29" s="6" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="R29" s="6" t="n">
         <v>2.19</v>
       </c>
-      <c r="R29" s="6" t="n">
+      <c r="S29" s="6" t="n">
         <v>2.21</v>
       </c>
-      <c r="S29" s="6" t="n">
+      <c r="T29" s="6" t="n">
         <v>2.2</v>
       </c>
-      <c r="T29" s="6" t="n">
+      <c r="U29" s="21" t="n">
         <v>2.21</v>
-      </c>
-      <c r="U29" s="21" t="n">
-        <v/>
       </c>
     </row>
     <row r="30">
@@ -2982,7 +2982,7 @@
         </is>
       </c>
       <c r="N30" s="48" t="n">
-        <v>45967</v>
+        <v>45968</v>
       </c>
       <c r="O30" s="6" t="inlineStr">
         <is>
@@ -2998,16 +2998,16 @@
         <v>2.28</v>
       </c>
       <c r="R30" s="6" t="n">
+        <v>2.28</v>
+      </c>
+      <c r="S30" s="6" t="n">
         <v>2.3</v>
       </c>
-      <c r="S30" s="6" t="n">
+      <c r="T30" s="6" t="n">
         <v>2.29</v>
       </c>
-      <c r="T30" s="6" t="n">
+      <c r="U30" s="21" t="n">
         <v>2.31</v>
-      </c>
-      <c r="U30" s="21" t="n">
-        <v/>
       </c>
     </row>
     <row r="31">
@@ -4251,7 +4251,7 @@
         </is>
       </c>
       <c r="N47" s="48" t="n">
-        <v>45966</v>
+        <v>45967</v>
       </c>
       <c r="O47" s="6" t="inlineStr">
         <is>
@@ -4273,7 +4273,7 @@
         <v>3.87</v>
       </c>
       <c r="T47" s="6" t="n">
-        <v>3.86</v>
+        <v>3.87</v>
       </c>
       <c r="U47" s="21" t="n">
         <v>3.86</v>
@@ -4330,7 +4330,7 @@
         </is>
       </c>
       <c r="N48" s="48" t="n">
-        <v>45966</v>
+        <v>45967</v>
       </c>
       <c r="O48" s="6" t="inlineStr">
         <is>
@@ -4343,16 +4343,16 @@
         </is>
       </c>
       <c r="Q48" s="6" t="n">
+        <v>3.57</v>
+      </c>
+      <c r="R48" s="6" t="n">
         <v>3.63</v>
       </c>
-      <c r="R48" s="6" t="n">
+      <c r="S48" s="6" t="n">
         <v>3.58</v>
       </c>
-      <c r="S48" s="6" t="n">
+      <c r="T48" s="6" t="n">
         <v>3.6</v>
-      </c>
-      <c r="T48" s="6" t="n">
-        <v/>
       </c>
       <c r="U48" s="21" t="n">
         <v/>
@@ -4405,7 +4405,7 @@
         </is>
       </c>
       <c r="N49" s="48" t="n">
-        <v>45966</v>
+        <v>45967</v>
       </c>
       <c r="O49" s="6" t="inlineStr">
         <is>
@@ -4418,16 +4418,16 @@
         </is>
       </c>
       <c r="Q49" s="6" t="n">
+        <v>3.69</v>
+      </c>
+      <c r="R49" s="6" t="n">
         <v>3.76</v>
       </c>
-      <c r="R49" s="6" t="n">
+      <c r="S49" s="6" t="n">
         <v>3.69</v>
       </c>
-      <c r="S49" s="6" t="n">
+      <c r="T49" s="6" t="n">
         <v>3.72</v>
-      </c>
-      <c r="T49" s="6" t="n">
-        <v/>
       </c>
       <c r="U49" s="21" t="n">
         <v/>
@@ -4484,7 +4484,7 @@
         </is>
       </c>
       <c r="N50" s="48" t="n">
-        <v>45966</v>
+        <v>45967</v>
       </c>
       <c r="O50" s="6" t="inlineStr">
         <is>
@@ -4497,16 +4497,16 @@
         </is>
       </c>
       <c r="Q50" s="6" t="n">
+        <v>4.11</v>
+      </c>
+      <c r="R50" s="6" t="n">
         <v>4.17</v>
       </c>
-      <c r="R50" s="6" t="n">
+      <c r="S50" s="6" t="n">
         <v>4.1</v>
       </c>
-      <c r="S50" s="6" t="n">
+      <c r="T50" s="6" t="n">
         <v>4.13</v>
-      </c>
-      <c r="T50" s="6" t="n">
-        <v/>
       </c>
       <c r="U50" s="21" t="n">
         <v/>
@@ -4610,7 +4610,7 @@
         </is>
       </c>
       <c r="N52" s="49" t="n">
-        <v>45966</v>
+        <v>45967</v>
       </c>
       <c r="O52" s="9" t="inlineStr">
         <is>
@@ -4623,16 +4623,16 @@
         </is>
       </c>
       <c r="Q52" s="9" t="n">
+        <v>5.83</v>
+      </c>
+      <c r="R52" s="9" t="n">
         <v>5.87</v>
       </c>
-      <c r="R52" s="9" t="n">
+      <c r="S52" s="9" t="n">
         <v>5.82</v>
       </c>
-      <c r="S52" s="9" t="n">
+      <c r="T52" s="9" t="n">
         <v>5.84</v>
-      </c>
-      <c r="T52" s="9" t="n">
-        <v/>
       </c>
       <c r="U52" s="22" t="n">
         <v/>

</xml_diff>

<commit_message>
Update dashboards - 2025-11-10
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -2802,10 +2802,10 @@
         </is>
       </c>
       <c r="F28" s="25" t="n">
-        <v>0.0292251268148207</v>
+        <v>0.02933036907051223</v>
       </c>
       <c r="G28" s="25" t="n">
-        <v>-0.02746655290430811</v>
+        <v>-0.02756598804853716</v>
       </c>
       <c r="H28" s="25" t="n">
         <v>-0.09389977010425232</v>
@@ -2880,7 +2880,7 @@
         <v>0.07634016956050854</v>
       </c>
       <c r="G29" s="25" t="n">
-        <v>0.03397968857635882</v>
+        <v>0.03387397095834726</v>
       </c>
       <c r="H29" s="25" t="n">
         <v>0.1089645997552716</v>

</xml_diff>

<commit_message>
Update dashboards - 2025-11-11
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -2802,10 +2802,10 @@
         </is>
       </c>
       <c r="F28" s="25" t="n">
-        <v>0.02933036907051223</v>
+        <v>0.0292251268148207</v>
       </c>
       <c r="G28" s="25" t="n">
-        <v>-0.02756598804853716</v>
+        <v>-0.02746655290430811</v>
       </c>
       <c r="H28" s="25" t="n">
         <v>-0.09389977010425232</v>
@@ -2880,7 +2880,7 @@
         <v>0.07634016956050854</v>
       </c>
       <c r="G29" s="25" t="n">
-        <v>0.03387397095834726</v>
+        <v>0.03397968857635882</v>
       </c>
       <c r="H29" s="25" t="n">
         <v>0.1089645997552716</v>
@@ -2903,7 +2903,7 @@
         </is>
       </c>
       <c r="N29" s="48" t="n">
-        <v>45968</v>
+        <v>45971</v>
       </c>
       <c r="O29" s="6" t="inlineStr">
         <is>
@@ -2919,16 +2919,16 @@
         <v>2.2</v>
       </c>
       <c r="R29" s="6" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="S29" s="6" t="n">
         <v>2.19</v>
       </c>
-      <c r="S29" s="6" t="n">
+      <c r="T29" s="6" t="n">
         <v>2.21</v>
       </c>
-      <c r="T29" s="6" t="n">
+      <c r="U29" s="21" t="n">
         <v>2.2</v>
-      </c>
-      <c r="U29" s="21" t="n">
-        <v>2.21</v>
       </c>
     </row>
     <row r="30">
@@ -2982,7 +2982,7 @@
         </is>
       </c>
       <c r="N30" s="48" t="n">
-        <v>45968</v>
+        <v>45971</v>
       </c>
       <c r="O30" s="6" t="inlineStr">
         <is>
@@ -2995,19 +2995,19 @@
         </is>
       </c>
       <c r="Q30" s="6" t="n">
-        <v>2.28</v>
+        <v>2.29</v>
       </c>
       <c r="R30" s="6" t="n">
         <v>2.28</v>
       </c>
       <c r="S30" s="6" t="n">
+        <v>2.28</v>
+      </c>
+      <c r="T30" s="6" t="n">
         <v>2.3</v>
       </c>
-      <c r="T30" s="6" t="n">
+      <c r="U30" s="21" t="n">
         <v>2.29</v>
-      </c>
-      <c r="U30" s="21" t="n">
-        <v>2.31</v>
       </c>
     </row>
     <row r="31">
@@ -3660,8 +3660,8 @@
           <t>DTWEXBGS</t>
         </is>
       </c>
-      <c r="N39" s="47" t="n">
-        <v>45961</v>
+      <c r="N39" s="48" t="n">
+        <v>45968</v>
       </c>
       <c r="O39" s="6" t="inlineStr">
         <is>
@@ -3674,19 +3674,19 @@
         </is>
       </c>
       <c r="Q39" s="6" t="n">
-        <v>121.7715</v>
+        <v>121.7835</v>
       </c>
       <c r="R39" s="6" t="n">
-        <v>121.665</v>
+        <v>122.0788</v>
       </c>
       <c r="S39" s="6" t="n">
-        <v>120.929</v>
+        <v>122.2295</v>
       </c>
       <c r="T39" s="6" t="n">
-        <v>121.0349</v>
+        <v>122.2066</v>
       </c>
       <c r="U39" s="21" t="n">
-        <v>121.2002</v>
+        <v>121.8422</v>
       </c>
     </row>
     <row r="40">
@@ -4251,7 +4251,7 @@
         </is>
       </c>
       <c r="N47" s="48" t="n">
-        <v>45967</v>
+        <v>45968</v>
       </c>
       <c r="O47" s="6" t="inlineStr">
         <is>
@@ -4276,7 +4276,7 @@
         <v>3.87</v>
       </c>
       <c r="U47" s="21" t="n">
-        <v>3.86</v>
+        <v>3.87</v>
       </c>
     </row>
     <row r="48">
@@ -4330,7 +4330,7 @@
         </is>
       </c>
       <c r="N48" s="48" t="n">
-        <v>45967</v>
+        <v>45968</v>
       </c>
       <c r="O48" s="6" t="inlineStr">
         <is>
@@ -4343,19 +4343,19 @@
         </is>
       </c>
       <c r="Q48" s="6" t="n">
+        <v>3.55</v>
+      </c>
+      <c r="R48" s="6" t="n">
         <v>3.57</v>
       </c>
-      <c r="R48" s="6" t="n">
+      <c r="S48" s="6" t="n">
         <v>3.63</v>
       </c>
-      <c r="S48" s="6" t="n">
+      <c r="T48" s="6" t="n">
         <v>3.58</v>
       </c>
-      <c r="T48" s="6" t="n">
+      <c r="U48" s="21" t="n">
         <v>3.6</v>
-      </c>
-      <c r="U48" s="21" t="n">
-        <v/>
       </c>
     </row>
     <row r="49">
@@ -4405,7 +4405,7 @@
         </is>
       </c>
       <c r="N49" s="48" t="n">
-        <v>45967</v>
+        <v>45968</v>
       </c>
       <c r="O49" s="6" t="inlineStr">
         <is>
@@ -4418,19 +4418,19 @@
         </is>
       </c>
       <c r="Q49" s="6" t="n">
+        <v>3.67</v>
+      </c>
+      <c r="R49" s="6" t="n">
         <v>3.69</v>
       </c>
-      <c r="R49" s="6" t="n">
+      <c r="S49" s="6" t="n">
         <v>3.76</v>
       </c>
-      <c r="S49" s="6" t="n">
+      <c r="T49" s="6" t="n">
         <v>3.69</v>
       </c>
-      <c r="T49" s="6" t="n">
+      <c r="U49" s="21" t="n">
         <v>3.72</v>
-      </c>
-      <c r="U49" s="21" t="n">
-        <v/>
       </c>
     </row>
     <row r="50">
@@ -4484,7 +4484,7 @@
         </is>
       </c>
       <c r="N50" s="48" t="n">
-        <v>45967</v>
+        <v>45968</v>
       </c>
       <c r="O50" s="6" t="inlineStr">
         <is>
@@ -4500,16 +4500,16 @@
         <v>4.11</v>
       </c>
       <c r="R50" s="6" t="n">
+        <v>4.11</v>
+      </c>
+      <c r="S50" s="6" t="n">
         <v>4.17</v>
       </c>
-      <c r="S50" s="6" t="n">
+      <c r="T50" s="6" t="n">
         <v>4.1</v>
       </c>
-      <c r="T50" s="6" t="n">
+      <c r="U50" s="21" t="n">
         <v>4.13</v>
-      </c>
-      <c r="U50" s="21" t="n">
-        <v/>
       </c>
     </row>
     <row r="51" ht="31.5" customHeight="1">
@@ -4610,7 +4610,7 @@
         </is>
       </c>
       <c r="N52" s="49" t="n">
-        <v>45967</v>
+        <v>45968</v>
       </c>
       <c r="O52" s="9" t="inlineStr">
         <is>
@@ -4623,19 +4623,19 @@
         </is>
       </c>
       <c r="Q52" s="9" t="n">
+        <v>5.86</v>
+      </c>
+      <c r="R52" s="9" t="n">
         <v>5.83</v>
       </c>
-      <c r="R52" s="9" t="n">
+      <c r="S52" s="9" t="n">
         <v>5.87</v>
       </c>
-      <c r="S52" s="9" t="n">
+      <c r="T52" s="9" t="n">
         <v>5.82</v>
       </c>
-      <c r="T52" s="9" t="n">
+      <c r="U52" s="22" t="n">
         <v>5.84</v>
-      </c>
-      <c r="U52" s="22" t="n">
-        <v/>
       </c>
     </row>
     <row r="53" ht="21" customHeight="1">

</xml_diff>

<commit_message>
Update dashboards - 2025-11-12
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -1079,7 +1079,7 @@
           <t>ADPMNUSNERSA</t>
         </is>
       </c>
-      <c r="N5" s="48" t="n">
+      <c r="N5" s="47" t="n">
         <v>45931</v>
       </c>
       <c r="O5" s="6" t="inlineStr">
@@ -2802,10 +2802,10 @@
         </is>
       </c>
       <c r="F28" s="25" t="n">
-        <v>0.0292251268148207</v>
+        <v>0.02933036907051223</v>
       </c>
       <c r="G28" s="25" t="n">
-        <v>-0.02746655290430811</v>
+        <v>-0.02756598804853716</v>
       </c>
       <c r="H28" s="25" t="n">
         <v>-0.09389977010425232</v>
@@ -2880,7 +2880,7 @@
         <v>0.07634016956050854</v>
       </c>
       <c r="G29" s="25" t="n">
-        <v>0.03397968857635882</v>
+        <v>0.03387397095834726</v>
       </c>
       <c r="H29" s="25" t="n">
         <v>0.1089645997552716</v>

</xml_diff>

<commit_message>
Update dashboards - 2025-11-13
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -1194,7 +1194,7 @@
           <t>GDPNOW</t>
         </is>
       </c>
-      <c r="C7" s="48" t="n">
+      <c r="C7" s="47" t="n">
         <v>45839</v>
       </c>
       <c r="D7" s="6" t="inlineStr">
@@ -2802,10 +2802,10 @@
         </is>
       </c>
       <c r="F28" s="25" t="n">
-        <v>0.02933036907051223</v>
+        <v>0.0292251268148207</v>
       </c>
       <c r="G28" s="25" t="n">
-        <v>-0.02756598804853716</v>
+        <v>-0.02746655290430811</v>
       </c>
       <c r="H28" s="25" t="n">
         <v>-0.09389977010425232</v>
@@ -2880,7 +2880,7 @@
         <v>0.07634016956050854</v>
       </c>
       <c r="G29" s="25" t="n">
-        <v>0.03387397095834726</v>
+        <v>0.03397968857635882</v>
       </c>
       <c r="H29" s="25" t="n">
         <v>0.1089645997552716</v>
@@ -2903,7 +2903,7 @@
         </is>
       </c>
       <c r="N29" s="48" t="n">
-        <v>45971</v>
+        <v>45973</v>
       </c>
       <c r="O29" s="6" t="inlineStr">
         <is>
@@ -2916,19 +2916,19 @@
         </is>
       </c>
       <c r="Q29" s="6" t="n">
+        <v>2.17</v>
+      </c>
+      <c r="R29" s="6" t="n">
+        <v/>
+      </c>
+      <c r="S29" s="6" t="n">
         <v>2.2</v>
       </c>
-      <c r="R29" s="6" t="n">
-        <v>2.2</v>
-      </c>
-      <c r="S29" s="6" t="n">
-        <v>2.19</v>
-      </c>
       <c r="T29" s="6" t="n">
-        <v>2.21</v>
+        <v/>
       </c>
       <c r="U29" s="21" t="n">
-        <v>2.2</v>
+        <v/>
       </c>
     </row>
     <row r="30">
@@ -2982,7 +2982,7 @@
         </is>
       </c>
       <c r="N30" s="48" t="n">
-        <v>45971</v>
+        <v>45973</v>
       </c>
       <c r="O30" s="6" t="inlineStr">
         <is>
@@ -2995,19 +2995,19 @@
         </is>
       </c>
       <c r="Q30" s="6" t="n">
+        <v>2.27</v>
+      </c>
+      <c r="R30" s="6" t="n">
+        <v/>
+      </c>
+      <c r="S30" s="6" t="n">
         <v>2.29</v>
       </c>
-      <c r="R30" s="6" t="n">
-        <v>2.28</v>
-      </c>
-      <c r="S30" s="6" t="n">
-        <v>2.28</v>
-      </c>
       <c r="T30" s="6" t="n">
-        <v>2.3</v>
+        <v/>
       </c>
       <c r="U30" s="21" t="n">
-        <v>2.29</v>
+        <v/>
       </c>
     </row>
     <row r="31">
@@ -4251,7 +4251,7 @@
         </is>
       </c>
       <c r="N47" s="48" t="n">
-        <v>45968</v>
+        <v>45972</v>
       </c>
       <c r="O47" s="6" t="inlineStr">
         <is>
@@ -4330,7 +4330,7 @@
         </is>
       </c>
       <c r="N48" s="48" t="n">
-        <v>45968</v>
+        <v>45971</v>
       </c>
       <c r="O48" s="6" t="inlineStr">
         <is>
@@ -4343,19 +4343,19 @@
         </is>
       </c>
       <c r="Q48" s="6" t="n">
+        <v>3.58</v>
+      </c>
+      <c r="R48" s="6" t="n">
+        <v/>
+      </c>
+      <c r="S48" s="6" t="n">
+        <v/>
+      </c>
+      <c r="T48" s="6" t="n">
         <v>3.55</v>
       </c>
-      <c r="R48" s="6" t="n">
+      <c r="U48" s="21" t="n">
         <v>3.57</v>
-      </c>
-      <c r="S48" s="6" t="n">
-        <v>3.63</v>
-      </c>
-      <c r="T48" s="6" t="n">
-        <v>3.58</v>
-      </c>
-      <c r="U48" s="21" t="n">
-        <v>3.6</v>
       </c>
     </row>
     <row r="49">
@@ -4405,7 +4405,7 @@
         </is>
       </c>
       <c r="N49" s="48" t="n">
-        <v>45968</v>
+        <v>45971</v>
       </c>
       <c r="O49" s="6" t="inlineStr">
         <is>
@@ -4418,19 +4418,19 @@
         </is>
       </c>
       <c r="Q49" s="6" t="n">
+        <v>3.72</v>
+      </c>
+      <c r="R49" s="6" t="n">
+        <v/>
+      </c>
+      <c r="S49" s="6" t="n">
+        <v/>
+      </c>
+      <c r="T49" s="6" t="n">
         <v>3.67</v>
       </c>
-      <c r="R49" s="6" t="n">
+      <c r="U49" s="21" t="n">
         <v>3.69</v>
-      </c>
-      <c r="S49" s="6" t="n">
-        <v>3.76</v>
-      </c>
-      <c r="T49" s="6" t="n">
-        <v>3.69</v>
-      </c>
-      <c r="U49" s="21" t="n">
-        <v>3.72</v>
       </c>
     </row>
     <row r="50">
@@ -4484,7 +4484,7 @@
         </is>
       </c>
       <c r="N50" s="48" t="n">
-        <v>45968</v>
+        <v>45971</v>
       </c>
       <c r="O50" s="6" t="inlineStr">
         <is>
@@ -4497,19 +4497,19 @@
         </is>
       </c>
       <c r="Q50" s="6" t="n">
+        <v>4.13</v>
+      </c>
+      <c r="R50" s="6" t="n">
+        <v/>
+      </c>
+      <c r="S50" s="6" t="n">
+        <v/>
+      </c>
+      <c r="T50" s="6" t="n">
         <v>4.11</v>
       </c>
-      <c r="R50" s="6" t="n">
+      <c r="U50" s="21" t="n">
         <v>4.11</v>
-      </c>
-      <c r="S50" s="6" t="n">
-        <v>4.17</v>
-      </c>
-      <c r="T50" s="6" t="n">
-        <v>4.1</v>
-      </c>
-      <c r="U50" s="21" t="n">
-        <v>4.13</v>
       </c>
     </row>
     <row r="51" ht="31.5" customHeight="1">
@@ -4558,7 +4558,7 @@
           <t>MORTGAGE30US</t>
         </is>
       </c>
-      <c r="N51" s="48" t="n">
+      <c r="N51" s="47" t="n">
         <v>45964</v>
       </c>
       <c r="O51" s="6" t="inlineStr">
@@ -4610,7 +4610,7 @@
         </is>
       </c>
       <c r="N52" s="49" t="n">
-        <v>45968</v>
+        <v>45971</v>
       </c>
       <c r="O52" s="9" t="inlineStr">
         <is>
@@ -4626,16 +4626,16 @@
         <v>5.86</v>
       </c>
       <c r="R52" s="9" t="n">
+        <v/>
+      </c>
+      <c r="S52" s="9" t="n">
+        <v/>
+      </c>
+      <c r="T52" s="9" t="n">
+        <v>5.86</v>
+      </c>
+      <c r="U52" s="22" t="n">
         <v>5.83</v>
-      </c>
-      <c r="S52" s="9" t="n">
-        <v>5.87</v>
-      </c>
-      <c r="T52" s="9" t="n">
-        <v>5.82</v>
-      </c>
-      <c r="U52" s="22" t="n">
-        <v>5.84</v>
       </c>
     </row>
     <row r="53" ht="21" customHeight="1">

</xml_diff>

<commit_message>
Update dashboards - 2025-11-14
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -2480,7 +2480,7 @@
           <t>REVOLSL</t>
         </is>
       </c>
-      <c r="C24" s="48" t="n">
+      <c r="C24" s="47" t="n">
         <v>45901</v>
       </c>
       <c r="D24" s="6" t="inlineStr">
@@ -2559,7 +2559,7 @@
           <t>NONREVSL</t>
         </is>
       </c>
-      <c r="C25" s="48" t="n">
+      <c r="C25" s="47" t="n">
         <v>45901</v>
       </c>
       <c r="D25" s="6" t="inlineStr">
@@ -2802,10 +2802,10 @@
         </is>
       </c>
       <c r="F28" s="25" t="n">
-        <v>0.0292251268148207</v>
+        <v>0.02933036907051223</v>
       </c>
       <c r="G28" s="25" t="n">
-        <v>-0.02746655290430811</v>
+        <v>-0.02756598804853716</v>
       </c>
       <c r="H28" s="25" t="n">
         <v>-0.09389977010425232</v>
@@ -2880,7 +2880,7 @@
         <v>0.07634016956050854</v>
       </c>
       <c r="G29" s="25" t="n">
-        <v>0.03397968857635882</v>
+        <v>0.03387397095834726</v>
       </c>
       <c r="H29" s="25" t="n">
         <v>0.1089645997552716</v>
@@ -2903,7 +2903,7 @@
         </is>
       </c>
       <c r="N29" s="48" t="n">
-        <v>45973</v>
+        <v>45974</v>
       </c>
       <c r="O29" s="6" t="inlineStr">
         <is>
@@ -2916,16 +2916,16 @@
         </is>
       </c>
       <c r="Q29" s="6" t="n">
+        <v>2.19</v>
+      </c>
+      <c r="R29" s="6" t="n">
         <v>2.17</v>
       </c>
-      <c r="R29" s="6" t="n">
+      <c r="S29" s="6" t="n">
         <v/>
       </c>
-      <c r="S29" s="6" t="n">
+      <c r="T29" s="6" t="n">
         <v>2.2</v>
-      </c>
-      <c r="T29" s="6" t="n">
-        <v/>
       </c>
       <c r="U29" s="21" t="n">
         <v/>
@@ -2982,7 +2982,7 @@
         </is>
       </c>
       <c r="N30" s="48" t="n">
-        <v>45973</v>
+        <v>45974</v>
       </c>
       <c r="O30" s="6" t="inlineStr">
         <is>
@@ -2995,16 +2995,16 @@
         </is>
       </c>
       <c r="Q30" s="6" t="n">
+        <v>2.28</v>
+      </c>
+      <c r="R30" s="6" t="n">
         <v>2.27</v>
       </c>
-      <c r="R30" s="6" t="n">
+      <c r="S30" s="6" t="n">
         <v/>
       </c>
-      <c r="S30" s="6" t="n">
+      <c r="T30" s="6" t="n">
         <v>2.29</v>
-      </c>
-      <c r="T30" s="6" t="n">
-        <v/>
       </c>
       <c r="U30" s="21" t="n">
         <v/>
@@ -3660,7 +3660,7 @@
           <t>DTWEXBGS</t>
         </is>
       </c>
-      <c r="N39" s="48" t="n">
+      <c r="N39" s="47" t="n">
         <v>45968</v>
       </c>
       <c r="O39" s="6" t="inlineStr">
@@ -4251,7 +4251,7 @@
         </is>
       </c>
       <c r="N47" s="48" t="n">
-        <v>45972</v>
+        <v>45973</v>
       </c>
       <c r="O47" s="6" t="inlineStr">
         <is>
@@ -4330,7 +4330,7 @@
         </is>
       </c>
       <c r="N48" s="48" t="n">
-        <v>45971</v>
+        <v>45973</v>
       </c>
       <c r="O48" s="6" t="inlineStr">
         <is>
@@ -4343,19 +4343,19 @@
         </is>
       </c>
       <c r="Q48" s="6" t="n">
-        <v>3.58</v>
+        <v>3.56</v>
       </c>
       <c r="R48" s="6" t="n">
         <v/>
       </c>
       <c r="S48" s="6" t="n">
+        <v>3.58</v>
+      </c>
+      <c r="T48" s="6" t="n">
         <v/>
       </c>
-      <c r="T48" s="6" t="n">
-        <v>3.55</v>
-      </c>
       <c r="U48" s="21" t="n">
-        <v>3.57</v>
+        <v/>
       </c>
     </row>
     <row r="49">
@@ -4405,7 +4405,7 @@
         </is>
       </c>
       <c r="N49" s="48" t="n">
-        <v>45971</v>
+        <v>45973</v>
       </c>
       <c r="O49" s="6" t="inlineStr">
         <is>
@@ -4418,19 +4418,19 @@
         </is>
       </c>
       <c r="Q49" s="6" t="n">
-        <v>3.72</v>
+        <v>3.68</v>
       </c>
       <c r="R49" s="6" t="n">
         <v/>
       </c>
       <c r="S49" s="6" t="n">
+        <v>3.72</v>
+      </c>
+      <c r="T49" s="6" t="n">
         <v/>
       </c>
-      <c r="T49" s="6" t="n">
-        <v>3.67</v>
-      </c>
       <c r="U49" s="21" t="n">
-        <v>3.69</v>
+        <v/>
       </c>
     </row>
     <row r="50">
@@ -4484,7 +4484,7 @@
         </is>
       </c>
       <c r="N50" s="48" t="n">
-        <v>45971</v>
+        <v>45973</v>
       </c>
       <c r="O50" s="6" t="inlineStr">
         <is>
@@ -4497,19 +4497,19 @@
         </is>
       </c>
       <c r="Q50" s="6" t="n">
-        <v>4.13</v>
+        <v>4.08</v>
       </c>
       <c r="R50" s="6" t="n">
         <v/>
       </c>
       <c r="S50" s="6" t="n">
+        <v>4.13</v>
+      </c>
+      <c r="T50" s="6" t="n">
         <v/>
       </c>
-      <c r="T50" s="6" t="n">
-        <v>4.11</v>
-      </c>
       <c r="U50" s="21" t="n">
-        <v>4.11</v>
+        <v/>
       </c>
     </row>
     <row r="51" ht="31.5" customHeight="1">
@@ -4558,8 +4558,8 @@
           <t>MORTGAGE30US</t>
         </is>
       </c>
-      <c r="N51" s="47" t="n">
-        <v>45964</v>
+      <c r="N51" s="48" t="n">
+        <v>45971</v>
       </c>
       <c r="O51" s="6" t="inlineStr">
         <is>
@@ -4572,19 +4572,19 @@
         </is>
       </c>
       <c r="Q51" s="6" t="n">
+        <v>6.24</v>
+      </c>
+      <c r="R51" s="6" t="n">
         <v>6.22</v>
       </c>
-      <c r="R51" s="6" t="n">
+      <c r="S51" s="6" t="n">
         <v>6.17</v>
       </c>
-      <c r="S51" s="6" t="n">
+      <c r="T51" s="6" t="n">
         <v>6.19</v>
       </c>
-      <c r="T51" s="6" t="n">
+      <c r="U51" s="21" t="n">
         <v>6.27</v>
-      </c>
-      <c r="U51" s="21" t="n">
-        <v>6.3</v>
       </c>
     </row>
     <row r="52" ht="16.15" customHeight="1" thickBot="1">
@@ -4610,7 +4610,7 @@
         </is>
       </c>
       <c r="N52" s="49" t="n">
-        <v>45971</v>
+        <v>45973</v>
       </c>
       <c r="O52" s="9" t="inlineStr">
         <is>
@@ -4623,19 +4623,19 @@
         </is>
       </c>
       <c r="Q52" s="9" t="n">
-        <v>5.86</v>
+        <v>5.83</v>
       </c>
       <c r="R52" s="9" t="n">
         <v/>
       </c>
       <c r="S52" s="9" t="n">
+        <v>5.86</v>
+      </c>
+      <c r="T52" s="9" t="n">
         <v/>
       </c>
-      <c r="T52" s="9" t="n">
-        <v>5.86</v>
-      </c>
       <c r="U52" s="22" t="n">
-        <v>5.83</v>
+        <v/>
       </c>
     </row>
     <row r="53" ht="21" customHeight="1">

</xml_diff>

<commit_message>
Update dashboards - 2025-11-15
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -2802,10 +2802,10 @@
         </is>
       </c>
       <c r="F28" s="25" t="n">
-        <v>0.02933036907051223</v>
+        <v>0.0292251268148207</v>
       </c>
       <c r="G28" s="25" t="n">
-        <v>-0.02756598804853716</v>
+        <v>-0.02746655290430811</v>
       </c>
       <c r="H28" s="25" t="n">
         <v>-0.09389977010425232</v>
@@ -2880,7 +2880,7 @@
         <v>0.07634016956050854</v>
       </c>
       <c r="G29" s="25" t="n">
-        <v>0.03387397095834726</v>
+        <v>0.03397968857635882</v>
       </c>
       <c r="H29" s="25" t="n">
         <v>0.1089645997552716</v>
@@ -2903,7 +2903,7 @@
         </is>
       </c>
       <c r="N29" s="48" t="n">
-        <v>45974</v>
+        <v>45975</v>
       </c>
       <c r="O29" s="6" t="inlineStr">
         <is>
@@ -2916,19 +2916,19 @@
         </is>
       </c>
       <c r="Q29" s="6" t="n">
+        <v>2.18</v>
+      </c>
+      <c r="R29" s="6" t="n">
         <v>2.19</v>
       </c>
-      <c r="R29" s="6" t="n">
+      <c r="S29" s="6" t="n">
         <v>2.17</v>
       </c>
-      <c r="S29" s="6" t="n">
+      <c r="T29" s="6" t="n">
         <v/>
       </c>
-      <c r="T29" s="6" t="n">
+      <c r="U29" s="21" t="n">
         <v>2.2</v>
-      </c>
-      <c r="U29" s="21" t="n">
-        <v/>
       </c>
     </row>
     <row r="30">
@@ -2982,7 +2982,7 @@
         </is>
       </c>
       <c r="N30" s="48" t="n">
-        <v>45974</v>
+        <v>45975</v>
       </c>
       <c r="O30" s="6" t="inlineStr">
         <is>
@@ -2998,16 +2998,16 @@
         <v>2.28</v>
       </c>
       <c r="R30" s="6" t="n">
+        <v>2.28</v>
+      </c>
+      <c r="S30" s="6" t="n">
         <v>2.27</v>
       </c>
-      <c r="S30" s="6" t="n">
+      <c r="T30" s="6" t="n">
         <v/>
       </c>
-      <c r="T30" s="6" t="n">
+      <c r="U30" s="21" t="n">
         <v>2.29</v>
-      </c>
-      <c r="U30" s="21" t="n">
-        <v/>
       </c>
     </row>
     <row r="31">
@@ -4251,7 +4251,7 @@
         </is>
       </c>
       <c r="N47" s="48" t="n">
-        <v>45973</v>
+        <v>45974</v>
       </c>
       <c r="O47" s="6" t="inlineStr">
         <is>
@@ -4264,7 +4264,7 @@
         </is>
       </c>
       <c r="Q47" s="6" t="n">
-        <v>3.87</v>
+        <v>3.88</v>
       </c>
       <c r="R47" s="6" t="n">
         <v>3.87</v>
@@ -4330,7 +4330,7 @@
         </is>
       </c>
       <c r="N48" s="48" t="n">
-        <v>45973</v>
+        <v>45974</v>
       </c>
       <c r="O48" s="6" t="inlineStr">
         <is>
@@ -4343,16 +4343,16 @@
         </is>
       </c>
       <c r="Q48" s="6" t="n">
+        <v>3.58</v>
+      </c>
+      <c r="R48" s="6" t="n">
         <v>3.56</v>
       </c>
-      <c r="R48" s="6" t="n">
+      <c r="S48" s="6" t="n">
         <v/>
       </c>
-      <c r="S48" s="6" t="n">
+      <c r="T48" s="6" t="n">
         <v>3.58</v>
-      </c>
-      <c r="T48" s="6" t="n">
-        <v/>
       </c>
       <c r="U48" s="21" t="n">
         <v/>
@@ -4405,7 +4405,7 @@
         </is>
       </c>
       <c r="N49" s="48" t="n">
-        <v>45973</v>
+        <v>45974</v>
       </c>
       <c r="O49" s="6" t="inlineStr">
         <is>
@@ -4418,16 +4418,16 @@
         </is>
       </c>
       <c r="Q49" s="6" t="n">
+        <v>3.71</v>
+      </c>
+      <c r="R49" s="6" t="n">
         <v>3.68</v>
       </c>
-      <c r="R49" s="6" t="n">
+      <c r="S49" s="6" t="n">
         <v/>
       </c>
-      <c r="S49" s="6" t="n">
+      <c r="T49" s="6" t="n">
         <v>3.72</v>
-      </c>
-      <c r="T49" s="6" t="n">
-        <v/>
       </c>
       <c r="U49" s="21" t="n">
         <v/>
@@ -4484,7 +4484,7 @@
         </is>
       </c>
       <c r="N50" s="48" t="n">
-        <v>45973</v>
+        <v>45974</v>
       </c>
       <c r="O50" s="6" t="inlineStr">
         <is>
@@ -4497,16 +4497,16 @@
         </is>
       </c>
       <c r="Q50" s="6" t="n">
+        <v>4.11</v>
+      </c>
+      <c r="R50" s="6" t="n">
         <v>4.08</v>
       </c>
-      <c r="R50" s="6" t="n">
+      <c r="S50" s="6" t="n">
         <v/>
       </c>
-      <c r="S50" s="6" t="n">
+      <c r="T50" s="6" t="n">
         <v>4.13</v>
-      </c>
-      <c r="T50" s="6" t="n">
-        <v/>
       </c>
       <c r="U50" s="21" t="n">
         <v/>
@@ -4610,7 +4610,7 @@
         </is>
       </c>
       <c r="N52" s="49" t="n">
-        <v>45973</v>
+        <v>45974</v>
       </c>
       <c r="O52" s="9" t="inlineStr">
         <is>
@@ -4623,16 +4623,16 @@
         </is>
       </c>
       <c r="Q52" s="9" t="n">
+        <v>5.88</v>
+      </c>
+      <c r="R52" s="9" t="n">
         <v>5.83</v>
       </c>
-      <c r="R52" s="9" t="n">
+      <c r="S52" s="9" t="n">
         <v/>
       </c>
-      <c r="S52" s="9" t="n">
+      <c r="T52" s="9" t="n">
         <v>5.86</v>
-      </c>
-      <c r="T52" s="9" t="n">
-        <v/>
       </c>
       <c r="U52" s="22" t="n">
         <v/>

</xml_diff>

<commit_message>
Update dashboards - 2025-11-16
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -2802,10 +2802,10 @@
         </is>
       </c>
       <c r="F28" s="25" t="n">
-        <v>0.0292251268148207</v>
+        <v>0.02933036907051223</v>
       </c>
       <c r="G28" s="25" t="n">
-        <v>-0.02746655290430811</v>
+        <v>-0.02756598804853716</v>
       </c>
       <c r="H28" s="25" t="n">
         <v>-0.09389977010425232</v>
@@ -2880,7 +2880,7 @@
         <v>0.07634016956050854</v>
       </c>
       <c r="G29" s="25" t="n">
-        <v>0.03397968857635882</v>
+        <v>0.03387397095834726</v>
       </c>
       <c r="H29" s="25" t="n">
         <v>0.1089645997552716</v>

</xml_diff>

<commit_message>
Update dashboards - 2025-11-17
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -2802,10 +2802,10 @@
         </is>
       </c>
       <c r="F28" s="25" t="n">
-        <v>0.02933036907051223</v>
+        <v>0.0292251268148207</v>
       </c>
       <c r="G28" s="25" t="n">
-        <v>-0.02756598804853716</v>
+        <v>-0.02746655290430811</v>
       </c>
       <c r="H28" s="25" t="n">
         <v>-0.09389977010425232</v>
@@ -2880,7 +2880,7 @@
         <v>0.07634016956050854</v>
       </c>
       <c r="G29" s="25" t="n">
-        <v>0.03387397095834726</v>
+        <v>0.03397968857635882</v>
       </c>
       <c r="H29" s="25" t="n">
         <v>0.1089645997552716</v>

</xml_diff>

<commit_message>
Update dashboards - 2025-11-18
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -2903,7 +2903,7 @@
         </is>
       </c>
       <c r="N29" s="48" t="n">
-        <v>45975</v>
+        <v>45978</v>
       </c>
       <c r="O29" s="6" t="inlineStr">
         <is>
@@ -2916,19 +2916,19 @@
         </is>
       </c>
       <c r="Q29" s="6" t="n">
+        <v>2.19</v>
+      </c>
+      <c r="R29" s="6" t="n">
         <v>2.18</v>
       </c>
-      <c r="R29" s="6" t="n">
+      <c r="S29" s="6" t="n">
         <v>2.19</v>
       </c>
-      <c r="S29" s="6" t="n">
+      <c r="T29" s="6" t="n">
         <v>2.17</v>
       </c>
-      <c r="T29" s="6" t="n">
+      <c r="U29" s="21" t="n">
         <v/>
-      </c>
-      <c r="U29" s="21" t="n">
-        <v>2.2</v>
       </c>
     </row>
     <row r="30">
@@ -2982,7 +2982,7 @@
         </is>
       </c>
       <c r="N30" s="48" t="n">
-        <v>45975</v>
+        <v>45978</v>
       </c>
       <c r="O30" s="6" t="inlineStr">
         <is>
@@ -3001,13 +3001,13 @@
         <v>2.28</v>
       </c>
       <c r="S30" s="6" t="n">
+        <v>2.28</v>
+      </c>
+      <c r="T30" s="6" t="n">
         <v>2.27</v>
       </c>
-      <c r="T30" s="6" t="n">
+      <c r="U30" s="21" t="n">
         <v/>
-      </c>
-      <c r="U30" s="21" t="n">
-        <v>2.29</v>
       </c>
     </row>
     <row r="31">
@@ -3660,8 +3660,8 @@
           <t>DTWEXBGS</t>
         </is>
       </c>
-      <c r="N39" s="47" t="n">
-        <v>45968</v>
+      <c r="N39" s="48" t="n">
+        <v>45975</v>
       </c>
       <c r="O39" s="6" t="inlineStr">
         <is>
@@ -3674,19 +3674,19 @@
         </is>
       </c>
       <c r="Q39" s="6" t="n">
-        <v>121.7835</v>
+        <v>121.363</v>
       </c>
       <c r="R39" s="6" t="n">
-        <v>122.0788</v>
+        <v>121.1756</v>
       </c>
       <c r="S39" s="6" t="n">
-        <v>122.2295</v>
+        <v>121.4459</v>
       </c>
       <c r="T39" s="6" t="n">
-        <v>122.2066</v>
+        <v/>
       </c>
       <c r="U39" s="21" t="n">
-        <v>121.8422</v>
+        <v>121.6932</v>
       </c>
     </row>
     <row r="40">
@@ -4251,7 +4251,7 @@
         </is>
       </c>
       <c r="N47" s="48" t="n">
-        <v>45974</v>
+        <v>45975</v>
       </c>
       <c r="O47" s="6" t="inlineStr">
         <is>
@@ -4267,7 +4267,7 @@
         <v>3.88</v>
       </c>
       <c r="R47" s="6" t="n">
-        <v>3.87</v>
+        <v>3.88</v>
       </c>
       <c r="S47" s="6" t="n">
         <v>3.87</v>
@@ -4330,7 +4330,7 @@
         </is>
       </c>
       <c r="N48" s="48" t="n">
-        <v>45974</v>
+        <v>45975</v>
       </c>
       <c r="O48" s="6" t="inlineStr">
         <is>
@@ -4343,19 +4343,19 @@
         </is>
       </c>
       <c r="Q48" s="6" t="n">
+        <v>3.62</v>
+      </c>
+      <c r="R48" s="6" t="n">
         <v>3.58</v>
       </c>
-      <c r="R48" s="6" t="n">
+      <c r="S48" s="6" t="n">
         <v>3.56</v>
       </c>
-      <c r="S48" s="6" t="n">
+      <c r="T48" s="6" t="n">
         <v/>
       </c>
-      <c r="T48" s="6" t="n">
+      <c r="U48" s="21" t="n">
         <v>3.58</v>
-      </c>
-      <c r="U48" s="21" t="n">
-        <v/>
       </c>
     </row>
     <row r="49">
@@ -4405,7 +4405,7 @@
         </is>
       </c>
       <c r="N49" s="48" t="n">
-        <v>45974</v>
+        <v>45975</v>
       </c>
       <c r="O49" s="6" t="inlineStr">
         <is>
@@ -4418,19 +4418,19 @@
         </is>
       </c>
       <c r="Q49" s="6" t="n">
+        <v>3.74</v>
+      </c>
+      <c r="R49" s="6" t="n">
         <v>3.71</v>
       </c>
-      <c r="R49" s="6" t="n">
+      <c r="S49" s="6" t="n">
         <v>3.68</v>
       </c>
-      <c r="S49" s="6" t="n">
+      <c r="T49" s="6" t="n">
         <v/>
       </c>
-      <c r="T49" s="6" t="n">
+      <c r="U49" s="21" t="n">
         <v>3.72</v>
-      </c>
-      <c r="U49" s="21" t="n">
-        <v/>
       </c>
     </row>
     <row r="50">
@@ -4484,7 +4484,7 @@
         </is>
       </c>
       <c r="N50" s="48" t="n">
-        <v>45974</v>
+        <v>45975</v>
       </c>
       <c r="O50" s="6" t="inlineStr">
         <is>
@@ -4497,19 +4497,19 @@
         </is>
       </c>
       <c r="Q50" s="6" t="n">
+        <v>4.14</v>
+      </c>
+      <c r="R50" s="6" t="n">
         <v>4.11</v>
       </c>
-      <c r="R50" s="6" t="n">
+      <c r="S50" s="6" t="n">
         <v>4.08</v>
       </c>
-      <c r="S50" s="6" t="n">
+      <c r="T50" s="6" t="n">
         <v/>
       </c>
-      <c r="T50" s="6" t="n">
+      <c r="U50" s="21" t="n">
         <v>4.13</v>
-      </c>
-      <c r="U50" s="21" t="n">
-        <v/>
       </c>
     </row>
     <row r="51" ht="31.5" customHeight="1">
@@ -4610,7 +4610,7 @@
         </is>
       </c>
       <c r="N52" s="49" t="n">
-        <v>45974</v>
+        <v>45975</v>
       </c>
       <c r="O52" s="9" t="inlineStr">
         <is>
@@ -4623,19 +4623,19 @@
         </is>
       </c>
       <c r="Q52" s="9" t="n">
+        <v>5.91</v>
+      </c>
+      <c r="R52" s="9" t="n">
         <v>5.88</v>
       </c>
-      <c r="R52" s="9" t="n">
+      <c r="S52" s="9" t="n">
         <v>5.83</v>
       </c>
-      <c r="S52" s="9" t="n">
+      <c r="T52" s="9" t="n">
         <v/>
       </c>
-      <c r="T52" s="9" t="n">
+      <c r="U52" s="22" t="n">
         <v>5.86</v>
-      </c>
-      <c r="U52" s="22" t="n">
-        <v/>
       </c>
     </row>
     <row r="53" ht="21" customHeight="1">

</xml_diff>

<commit_message>
Update dashboards - 2025-11-19
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -2788,7 +2788,7 @@
           <t>DGORDER</t>
         </is>
       </c>
-      <c r="C28" s="47" t="n">
+      <c r="C28" s="48" t="n">
         <v>45870</v>
       </c>
       <c r="D28" s="6" t="inlineStr">
@@ -2802,10 +2802,10 @@
         </is>
       </c>
       <c r="F28" s="25" t="n">
-        <v>0.0292251268148207</v>
+        <v>0.02880223870746335</v>
       </c>
       <c r="G28" s="25" t="n">
-        <v>-0.02746655290430811</v>
+        <v>-0.02799901206372835</v>
       </c>
       <c r="H28" s="25" t="n">
         <v>-0.09389977010425232</v>
@@ -2863,7 +2863,7 @@
           <t>DGORDER</t>
         </is>
       </c>
-      <c r="C29" s="47" t="n">
+      <c r="C29" s="48" t="n">
         <v>45870</v>
       </c>
       <c r="D29" s="6" t="inlineStr">
@@ -2877,10 +2877,10 @@
         </is>
       </c>
       <c r="F29" s="25" t="n">
-        <v>0.07634016956050854</v>
+        <v>0.07530887191904141</v>
       </c>
       <c r="G29" s="25" t="n">
-        <v>0.03397968857635882</v>
+        <v>0.03341358778313566</v>
       </c>
       <c r="H29" s="25" t="n">
         <v>0.1089645997552716</v>
@@ -2903,7 +2903,7 @@
         </is>
       </c>
       <c r="N29" s="48" t="n">
-        <v>45978</v>
+        <v>45979</v>
       </c>
       <c r="O29" s="6" t="inlineStr">
         <is>
@@ -2916,19 +2916,19 @@
         </is>
       </c>
       <c r="Q29" s="6" t="n">
+        <v>2.18</v>
+      </c>
+      <c r="R29" s="6" t="n">
         <v>2.19</v>
       </c>
-      <c r="R29" s="6" t="n">
+      <c r="S29" s="6" t="n">
+        <v/>
+      </c>
+      <c r="T29" s="6" t="n">
+        <v/>
+      </c>
+      <c r="U29" s="21" t="n">
         <v>2.18</v>
-      </c>
-      <c r="S29" s="6" t="n">
-        <v>2.19</v>
-      </c>
-      <c r="T29" s="6" t="n">
-        <v>2.17</v>
-      </c>
-      <c r="U29" s="21" t="n">
-        <v/>
       </c>
     </row>
     <row r="30">
@@ -2942,7 +2942,7 @@
           <t>ADXDNO</t>
         </is>
       </c>
-      <c r="C30" s="47" t="n">
+      <c r="C30" s="48" t="n">
         <v>45870</v>
       </c>
       <c r="D30" s="6" t="inlineStr">
@@ -2956,10 +2956,10 @@
         </is>
       </c>
       <c r="F30" s="25" t="n">
-        <v>0.01923414103867871</v>
+        <v>0.01912935471760346</v>
       </c>
       <c r="G30" s="25" t="n">
-        <v>-0.02348739337531547</v>
+        <v>-0.02404555711932721</v>
       </c>
       <c r="H30" s="25" t="n">
         <v>-0.09442194506291901</v>
@@ -2982,7 +2982,7 @@
         </is>
       </c>
       <c r="N30" s="48" t="n">
-        <v>45978</v>
+        <v>45979</v>
       </c>
       <c r="O30" s="6" t="inlineStr">
         <is>
@@ -2995,19 +2995,19 @@
         </is>
       </c>
       <c r="Q30" s="6" t="n">
-        <v>2.28</v>
+        <v>2.27</v>
       </c>
       <c r="R30" s="6" t="n">
         <v>2.28</v>
       </c>
       <c r="S30" s="6" t="n">
+        <v/>
+      </c>
+      <c r="T30" s="6" t="n">
+        <v/>
+      </c>
+      <c r="U30" s="21" t="n">
         <v>2.28</v>
-      </c>
-      <c r="T30" s="6" t="n">
-        <v>2.27</v>
-      </c>
-      <c r="U30" s="21" t="n">
-        <v/>
       </c>
     </row>
     <row r="31">
@@ -3017,7 +3017,7 @@
           <t>ADXDNO</t>
         </is>
       </c>
-      <c r="C31" s="47" t="n">
+      <c r="C31" s="48" t="n">
         <v>45870</v>
       </c>
       <c r="D31" s="6" t="inlineStr">
@@ -3031,10 +3031,10 @@
         </is>
       </c>
       <c r="F31" s="25" t="n">
-        <v>0.06748567650947554</v>
+        <v>0.06676582929337446</v>
       </c>
       <c r="G31" s="25" t="n">
-        <v>0.03352046419083723</v>
+        <v>0.0329297153895499</v>
       </c>
       <c r="H31" s="25" t="n">
         <v>0.1029410098461701</v>
@@ -4251,7 +4251,7 @@
         </is>
       </c>
       <c r="N47" s="48" t="n">
-        <v>45975</v>
+        <v>45978</v>
       </c>
       <c r="O47" s="6" t="inlineStr">
         <is>
@@ -4270,13 +4270,13 @@
         <v>3.88</v>
       </c>
       <c r="S47" s="6" t="n">
-        <v>3.87</v>
+        <v>3.88</v>
       </c>
       <c r="T47" s="6" t="n">
-        <v>3.87</v>
+        <v>3.88</v>
       </c>
       <c r="U47" s="21" t="n">
-        <v>3.87</v>
+        <v>3.88</v>
       </c>
     </row>
     <row r="48">
@@ -4330,7 +4330,7 @@
         </is>
       </c>
       <c r="N48" s="48" t="n">
-        <v>45975</v>
+        <v>45978</v>
       </c>
       <c r="O48" s="6" t="inlineStr">
         <is>
@@ -4343,16 +4343,16 @@
         </is>
       </c>
       <c r="Q48" s="6" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="R48" s="6" t="n">
+        <v/>
+      </c>
+      <c r="S48" s="6" t="n">
+        <v/>
+      </c>
+      <c r="T48" s="6" t="n">
         <v>3.62</v>
-      </c>
-      <c r="R48" s="6" t="n">
-        <v>3.58</v>
-      </c>
-      <c r="S48" s="6" t="n">
-        <v>3.56</v>
-      </c>
-      <c r="T48" s="6" t="n">
-        <v/>
       </c>
       <c r="U48" s="21" t="n">
         <v>3.58</v>
@@ -4405,7 +4405,7 @@
         </is>
       </c>
       <c r="N49" s="48" t="n">
-        <v>45975</v>
+        <v>45978</v>
       </c>
       <c r="O49" s="6" t="inlineStr">
         <is>
@@ -4418,19 +4418,19 @@
         </is>
       </c>
       <c r="Q49" s="6" t="n">
+        <v>3.72</v>
+      </c>
+      <c r="R49" s="6" t="n">
+        <v/>
+      </c>
+      <c r="S49" s="6" t="n">
+        <v/>
+      </c>
+      <c r="T49" s="6" t="n">
         <v>3.74</v>
       </c>
-      <c r="R49" s="6" t="n">
+      <c r="U49" s="21" t="n">
         <v>3.71</v>
-      </c>
-      <c r="S49" s="6" t="n">
-        <v>3.68</v>
-      </c>
-      <c r="T49" s="6" t="n">
-        <v/>
-      </c>
-      <c r="U49" s="21" t="n">
-        <v>3.72</v>
       </c>
     </row>
     <row r="50">
@@ -4484,7 +4484,7 @@
         </is>
       </c>
       <c r="N50" s="48" t="n">
-        <v>45975</v>
+        <v>45978</v>
       </c>
       <c r="O50" s="6" t="inlineStr">
         <is>
@@ -4497,19 +4497,19 @@
         </is>
       </c>
       <c r="Q50" s="6" t="n">
+        <v>4.13</v>
+      </c>
+      <c r="R50" s="6" t="n">
+        <v/>
+      </c>
+      <c r="S50" s="6" t="n">
+        <v/>
+      </c>
+      <c r="T50" s="6" t="n">
         <v>4.14</v>
       </c>
-      <c r="R50" s="6" t="n">
+      <c r="U50" s="21" t="n">
         <v>4.11</v>
-      </c>
-      <c r="S50" s="6" t="n">
-        <v>4.08</v>
-      </c>
-      <c r="T50" s="6" t="n">
-        <v/>
-      </c>
-      <c r="U50" s="21" t="n">
-        <v>4.13</v>
       </c>
     </row>
     <row r="51" ht="31.5" customHeight="1">
@@ -4610,7 +4610,7 @@
         </is>
       </c>
       <c r="N52" s="49" t="n">
-        <v>45975</v>
+        <v>45978</v>
       </c>
       <c r="O52" s="9" t="inlineStr">
         <is>
@@ -4623,19 +4623,19 @@
         </is>
       </c>
       <c r="Q52" s="9" t="n">
+        <v>5.9</v>
+      </c>
+      <c r="R52" s="9" t="n">
+        <v/>
+      </c>
+      <c r="S52" s="9" t="n">
+        <v/>
+      </c>
+      <c r="T52" s="9" t="n">
         <v>5.91</v>
       </c>
-      <c r="R52" s="9" t="n">
+      <c r="U52" s="22" t="n">
         <v>5.88</v>
-      </c>
-      <c r="S52" s="9" t="n">
-        <v>5.83</v>
-      </c>
-      <c r="T52" s="9" t="n">
-        <v/>
-      </c>
-      <c r="U52" s="22" t="n">
-        <v>5.86</v>
       </c>
     </row>
     <row r="53" ht="21" customHeight="1">

</xml_diff>

<commit_message>
Update dashboards - 2025-11-20
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -929,8 +929,8 @@
           <t>PAYEMS</t>
         </is>
       </c>
-      <c r="N3" s="47" t="n">
-        <v>45870</v>
+      <c r="N3" s="48" t="n">
+        <v>45901</v>
       </c>
       <c r="O3" s="6" t="inlineStr">
         <is>
@@ -943,19 +943,19 @@
         </is>
       </c>
       <c r="Q3" s="24" t="n">
-        <v>22</v>
+        <v>119</v>
       </c>
       <c r="R3" s="24" t="n">
-        <v>79</v>
+        <v>-4</v>
       </c>
       <c r="S3" s="24" t="n">
+        <v>72</v>
+      </c>
+      <c r="T3" s="24" t="n">
         <v>-13</v>
       </c>
-      <c r="T3" s="24" t="n">
+      <c r="U3" s="26" t="n">
         <v>19</v>
-      </c>
-      <c r="U3" s="26" t="n">
-        <v>158</v>
       </c>
     </row>
     <row r="4">
@@ -1000,8 +1000,8 @@
           <t>PAYEMS</t>
         </is>
       </c>
-      <c r="N4" s="47" t="n">
-        <v>45870</v>
+      <c r="N4" s="48" t="n">
+        <v>45901</v>
       </c>
       <c r="O4" s="6" t="inlineStr">
         <is>
@@ -1014,19 +1014,19 @@
         </is>
       </c>
       <c r="Q4" s="38" t="n">
-        <v>0.009274137429305261</v>
+        <v>0.008287327715805298</v>
       </c>
       <c r="R4" s="38" t="n">
-        <v>0.009588425536223995</v>
+        <v>0.009065374444880247</v>
       </c>
       <c r="S4" s="38" t="n">
+        <v>0.009544122579951013</v>
+      </c>
+      <c r="T4" s="38" t="n">
         <v>0.009650761485609347</v>
       </c>
-      <c r="T4" s="38" t="n">
+      <c r="U4" s="23" t="n">
         <v>0.01028968243911093</v>
-      </c>
-      <c r="U4" s="23" t="n">
-        <v>0.01140609636184857</v>
       </c>
     </row>
     <row r="5" ht="31.5" customHeight="1">
@@ -1154,8 +1154,8 @@
           <t>UNRATE</t>
         </is>
       </c>
-      <c r="N6" s="47" t="n">
-        <v>45870</v>
+      <c r="N6" s="48" t="n">
+        <v>45901</v>
       </c>
       <c r="O6" s="6" t="inlineStr">
         <is>
@@ -1168,16 +1168,16 @@
         </is>
       </c>
       <c r="Q6" s="6" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="R6" s="6" t="n">
         <v>4.3</v>
       </c>
-      <c r="R6" s="6" t="n">
+      <c r="S6" s="6" t="n">
         <v>4.2</v>
       </c>
-      <c r="S6" s="6" t="n">
+      <c r="T6" s="6" t="n">
         <v>4.1</v>
-      </c>
-      <c r="T6" s="6" t="n">
-        <v>4.2</v>
       </c>
       <c r="U6" s="21" t="n">
         <v>4.2</v>
@@ -1194,7 +1194,7 @@
           <t>GDPNOW</t>
         </is>
       </c>
-      <c r="C7" s="47" t="n">
+      <c r="C7" s="48" t="n">
         <v>45839</v>
       </c>
       <c r="D7" s="6" t="inlineStr">
@@ -1208,7 +1208,7 @@
         </is>
       </c>
       <c r="F7" s="25" t="n">
-        <v>0.370537560303239</v>
+        <v>0.4573742246726396</v>
       </c>
       <c r="G7" s="25" t="n">
         <v>-2.062303243282817</v>
@@ -1233,8 +1233,8 @@
           <t>U6RATE</t>
         </is>
       </c>
-      <c r="N7" s="47" t="n">
-        <v>45870</v>
+      <c r="N7" s="48" t="n">
+        <v>45901</v>
       </c>
       <c r="O7" s="6" t="inlineStr">
         <is>
@@ -1247,16 +1247,16 @@
         </is>
       </c>
       <c r="Q7" s="6" t="n">
+        <v>8</v>
+      </c>
+      <c r="R7" s="6" t="n">
         <v>8.1</v>
       </c>
-      <c r="R7" s="6" t="n">
+      <c r="S7" s="6" t="n">
         <v>7.9</v>
       </c>
-      <c r="S7" s="6" t="n">
+      <c r="T7" s="6" t="n">
         <v>7.7</v>
-      </c>
-      <c r="T7" s="6" t="n">
-        <v>7.8</v>
       </c>
       <c r="U7" s="21" t="n">
         <v>7.8</v>
@@ -1312,8 +1312,8 @@
           <t>CIVPART</t>
         </is>
       </c>
-      <c r="N8" s="47" t="n">
-        <v>45870</v>
+      <c r="N8" s="48" t="n">
+        <v>45901</v>
       </c>
       <c r="O8" s="6" t="inlineStr">
         <is>
@@ -1326,19 +1326,19 @@
         </is>
       </c>
       <c r="Q8" s="6" t="n">
+        <v>62.4</v>
+      </c>
+      <c r="R8" s="6" t="n">
         <v>62.3</v>
       </c>
-      <c r="R8" s="6" t="n">
+      <c r="S8" s="6" t="n">
         <v>62.2</v>
       </c>
-      <c r="S8" s="6" t="n">
+      <c r="T8" s="6" t="n">
         <v>62.3</v>
       </c>
-      <c r="T8" s="6" t="n">
+      <c r="U8" s="21" t="n">
         <v>62.4</v>
-      </c>
-      <c r="U8" s="21" t="n">
-        <v>62.6</v>
       </c>
     </row>
     <row r="9">
@@ -1391,8 +1391,8 @@
           <t>EMRATIO</t>
         </is>
       </c>
-      <c r="N9" s="47" t="n">
-        <v>45870</v>
+      <c r="N9" s="48" t="n">
+        <v>45901</v>
       </c>
       <c r="O9" s="6" t="inlineStr">
         <is>
@@ -1405,19 +1405,19 @@
         </is>
       </c>
       <c r="Q9" s="6" t="n">
-        <v>59.6</v>
+        <v>59.7</v>
       </c>
       <c r="R9" s="6" t="n">
         <v>59.6</v>
       </c>
       <c r="S9" s="6" t="n">
-        <v>59.7</v>
+        <v>59.6</v>
       </c>
       <c r="T9" s="6" t="n">
         <v>59.7</v>
       </c>
       <c r="U9" s="21" t="n">
-        <v>60</v>
+        <v>59.7</v>
       </c>
     </row>
     <row r="10">
@@ -1699,8 +1699,8 @@
           <t>ICSA</t>
         </is>
       </c>
-      <c r="N13" s="47" t="n">
-        <v>45915</v>
+      <c r="N13" s="48" t="n">
+        <v>45971</v>
       </c>
       <c r="O13" s="6" t="inlineStr">
         <is>
@@ -1713,19 +1713,19 @@
         </is>
       </c>
       <c r="Q13" s="24" t="n">
-        <v>218000</v>
+        <v>220000</v>
       </c>
       <c r="R13" s="24" t="n">
-        <v>232000</v>
+        <v>228000</v>
       </c>
       <c r="S13" s="24" t="n">
-        <v>264000</v>
+        <v>229000</v>
       </c>
       <c r="T13" s="24" t="n">
-        <v>236000</v>
+        <v/>
       </c>
       <c r="U13" s="26" t="n">
-        <v>229000</v>
+        <v/>
       </c>
     </row>
     <row r="14">
@@ -1774,8 +1774,8 @@
           <t>CCSA</t>
         </is>
       </c>
-      <c r="N14" s="47" t="n">
-        <v>45908</v>
+      <c r="N14" s="48" t="n">
+        <v>45964</v>
       </c>
       <c r="O14" s="6" t="inlineStr">
         <is>
@@ -1788,19 +1788,19 @@
         </is>
       </c>
       <c r="Q14" s="24" t="n">
-        <v>1926000</v>
+        <v>1974000</v>
       </c>
       <c r="R14" s="24" t="n">
-        <v>1928000</v>
+        <v>1946000</v>
       </c>
       <c r="S14" s="24" t="n">
-        <v>1927000</v>
+        <v>1964000</v>
       </c>
       <c r="T14" s="24" t="n">
-        <v>1939000</v>
+        <v/>
       </c>
       <c r="U14" s="26" t="n">
-        <v>1944000</v>
+        <v/>
       </c>
     </row>
     <row r="15">
@@ -1853,8 +1853,8 @@
           <t>AWHAETP</t>
         </is>
       </c>
-      <c r="N15" s="47" t="n">
-        <v>45870</v>
+      <c r="N15" s="48" t="n">
+        <v>45901</v>
       </c>
       <c r="O15" s="6" t="inlineStr">
         <is>
@@ -1873,10 +1873,10 @@
         <v>34.2</v>
       </c>
       <c r="S15" s="24" t="n">
+        <v>34.3</v>
+      </c>
+      <c r="T15" s="24" t="n">
         <v>34.2</v>
-      </c>
-      <c r="T15" s="24" t="n">
-        <v>34.3</v>
       </c>
       <c r="U15" s="26" t="n">
         <v>34.3</v>
@@ -2903,7 +2903,7 @@
         </is>
       </c>
       <c r="N29" s="48" t="n">
-        <v>45979</v>
+        <v>45980</v>
       </c>
       <c r="O29" s="6" t="inlineStr">
         <is>
@@ -2919,16 +2919,16 @@
         <v>2.18</v>
       </c>
       <c r="R29" s="6" t="n">
+        <v>2.18</v>
+      </c>
+      <c r="S29" s="6" t="n">
         <v>2.19</v>
-      </c>
-      <c r="S29" s="6" t="n">
-        <v/>
       </c>
       <c r="T29" s="6" t="n">
         <v/>
       </c>
       <c r="U29" s="21" t="n">
-        <v>2.18</v>
+        <v/>
       </c>
     </row>
     <row r="30">
@@ -2982,7 +2982,7 @@
         </is>
       </c>
       <c r="N30" s="48" t="n">
-        <v>45979</v>
+        <v>45980</v>
       </c>
       <c r="O30" s="6" t="inlineStr">
         <is>
@@ -2998,16 +2998,16 @@
         <v>2.27</v>
       </c>
       <c r="R30" s="6" t="n">
+        <v>2.27</v>
+      </c>
+      <c r="S30" s="6" t="n">
         <v>2.28</v>
-      </c>
-      <c r="S30" s="6" t="n">
-        <v/>
       </c>
       <c r="T30" s="6" t="n">
         <v/>
       </c>
       <c r="U30" s="21" t="n">
-        <v>2.28</v>
+        <v/>
       </c>
     </row>
     <row r="31">
@@ -3206,8 +3206,8 @@
           <t>CES0500000003</t>
         </is>
       </c>
-      <c r="N33" s="47" t="n">
-        <v>45870</v>
+      <c r="N33" s="48" t="n">
+        <v>45901</v>
       </c>
       <c r="O33" s="6" t="inlineStr">
         <is>
@@ -3220,19 +3220,19 @@
         </is>
       </c>
       <c r="Q33" s="38" t="n">
-        <v>0.002744990392533619</v>
+        <v>0.002460360852925225</v>
       </c>
       <c r="R33" s="38" t="n">
+        <v>0.004117485588800429</v>
+      </c>
+      <c r="S33" s="38" t="n">
         <v>0.003304874690167825</v>
       </c>
-      <c r="S33" s="38" t="n">
+      <c r="T33" s="38" t="n">
         <v>0.002208114821970808</v>
       </c>
-      <c r="T33" s="38" t="n">
+      <c r="U33" s="23" t="n">
         <v>0.004157427937915736</v>
-      </c>
-      <c r="U33" s="23" t="n">
-        <v>0.001665741254858188</v>
       </c>
     </row>
     <row r="34" ht="31.5" customHeight="1">
@@ -3281,8 +3281,8 @@
           <t>CES0500000003</t>
         </is>
       </c>
-      <c r="N34" s="47" t="n">
-        <v>45870</v>
+      <c r="N34" s="48" t="n">
+        <v>45901</v>
       </c>
       <c r="O34" s="6" t="inlineStr">
         <is>
@@ -3295,19 +3295,19 @@
         </is>
       </c>
       <c r="Q34" s="38" t="n">
-        <v>0.03690036900369016</v>
+        <v>0.03792810642513454</v>
       </c>
       <c r="R34" s="38" t="n">
+        <v>0.03831961396537047</v>
+      </c>
+      <c r="S34" s="38" t="n">
         <v>0.03877958368976332</v>
       </c>
-      <c r="S34" s="38" t="n">
+      <c r="T34" s="38" t="n">
         <v>0.03742857142857149</v>
       </c>
-      <c r="T34" s="38" t="n">
+      <c r="U34" s="23" t="n">
         <v>0.03840642017770124</v>
-      </c>
-      <c r="U34" s="23" t="n">
-        <v>0.03827338129496398</v>
       </c>
     </row>
     <row r="35" ht="31.5" customHeight="1">
@@ -3360,7 +3360,7 @@
           <t>RCES0500000003*</t>
         </is>
       </c>
-      <c r="N35" s="47" t="n">
+      <c r="N35" s="48" t="n">
         <v>45870</v>
       </c>
       <c r="O35" s="6" t="inlineStr">
@@ -3374,7 +3374,7 @@
         </is>
       </c>
       <c r="Q35" s="38" t="n">
-        <v>9.799886350903009e-05</v>
+        <v>0.001466871021821747</v>
       </c>
       <c r="R35" s="38" t="n">
         <v>0.001676812994635402</v>
@@ -3431,7 +3431,7 @@
           <t>RCES0500000003*</t>
         </is>
       </c>
-      <c r="N36" s="47" t="n">
+      <c r="N36" s="48" t="n">
         <v>45870</v>
       </c>
       <c r="O36" s="6" t="inlineStr">
@@ -3445,7 +3445,7 @@
         </is>
       </c>
       <c r="Q36" s="38" t="n">
-        <v>0.009235572263017468</v>
+        <v>0.01061695136548506</v>
       </c>
       <c r="R36" s="38" t="n">
         <v>0.01248872041084645</v>
@@ -4124,8 +4124,8 @@
           <t>BOPTEXP</t>
         </is>
       </c>
-      <c r="C46" s="47" t="n">
-        <v>45839</v>
+      <c r="C46" s="48" t="n">
+        <v>45870</v>
       </c>
       <c r="D46" s="6" t="inlineStr">
         <is>
@@ -4138,19 +4138,19 @@
         </is>
       </c>
       <c r="F46" s="24" t="n">
-        <v>280464</v>
+        <v>280832</v>
       </c>
       <c r="G46" s="24" t="n">
+        <v>280602</v>
+      </c>
+      <c r="H46" s="24" t="n">
         <v>279650</v>
       </c>
-      <c r="H46" s="24" t="n">
+      <c r="I46" s="24" t="n">
         <v>280391</v>
       </c>
-      <c r="I46" s="24" t="n">
+      <c r="J46" s="24" t="n">
         <v>291785</v>
-      </c>
-      <c r="J46" s="24" t="n">
-        <v>283593</v>
       </c>
       <c r="K46" s="5" t="n"/>
       <c r="L46" s="29" t="inlineStr">
@@ -4211,8 +4211,8 @@
           <t>BOPTEXP</t>
         </is>
       </c>
-      <c r="C47" s="47" t="n">
-        <v>45839</v>
+      <c r="C47" s="48" t="n">
+        <v>45870</v>
       </c>
       <c r="D47" s="6" t="inlineStr">
         <is>
@@ -4225,19 +4225,19 @@
         </is>
       </c>
       <c r="F47" s="38" t="n">
-        <v>0.002910781333810064</v>
+        <v>0.0008196662889075057</v>
       </c>
       <c r="G47" s="38" t="n">
+        <v>0.003404255319148897</v>
+      </c>
+      <c r="H47" s="38" t="n">
         <v>-0.002642738176332315</v>
       </c>
-      <c r="H47" s="38" t="n">
+      <c r="I47" s="38" t="n">
         <v>-0.03904929999828644</v>
       </c>
-      <c r="I47" s="38" t="n">
+      <c r="J47" s="38" t="n">
         <v>0.02888646757853675</v>
-      </c>
-      <c r="J47" s="38" t="n">
-        <v>0.009558289546755416</v>
       </c>
       <c r="K47" s="5" t="n"/>
       <c r="L47" s="28" t="inlineStr">
@@ -4251,7 +4251,7 @@
         </is>
       </c>
       <c r="N47" s="48" t="n">
-        <v>45978</v>
+        <v>45979</v>
       </c>
       <c r="O47" s="6" t="inlineStr">
         <is>
@@ -4290,8 +4290,8 @@
           <t>BOPTIMP</t>
         </is>
       </c>
-      <c r="C48" s="47" t="n">
-        <v>45839</v>
+      <c r="C48" s="48" t="n">
+        <v>45870</v>
       </c>
       <c r="D48" s="6" t="inlineStr">
         <is>
@@ -4304,19 +4304,19 @@
         </is>
       </c>
       <c r="F48" s="24" t="n">
-        <v>358775</v>
+        <v>340382</v>
       </c>
       <c r="G48" s="24" t="n">
+        <v>358756</v>
+      </c>
+      <c r="H48" s="24" t="n">
         <v>338736</v>
       </c>
-      <c r="H48" s="24" t="n">
+      <c r="I48" s="24" t="n">
         <v>351506</v>
       </c>
-      <c r="I48" s="24" t="n">
+      <c r="J48" s="24" t="n">
         <v>351977</v>
-      </c>
-      <c r="J48" s="24" t="n">
-        <v>420013</v>
       </c>
       <c r="K48" s="5" t="n"/>
       <c r="L48" s="28" t="inlineStr">
@@ -4330,7 +4330,7 @@
         </is>
       </c>
       <c r="N48" s="48" t="n">
-        <v>45978</v>
+        <v>45979</v>
       </c>
       <c r="O48" s="6" t="inlineStr">
         <is>
@@ -4343,19 +4343,19 @@
         </is>
       </c>
       <c r="Q48" s="6" t="n">
+        <v>3.58</v>
+      </c>
+      <c r="R48" s="6" t="n">
         <v>3.6</v>
-      </c>
-      <c r="R48" s="6" t="n">
-        <v/>
       </c>
       <c r="S48" s="6" t="n">
         <v/>
       </c>
       <c r="T48" s="6" t="n">
+        <v/>
+      </c>
+      <c r="U48" s="21" t="n">
         <v>3.62</v>
-      </c>
-      <c r="U48" s="21" t="n">
-        <v>3.58</v>
       </c>
     </row>
     <row r="49">
@@ -4365,8 +4365,8 @@
           <t>BOPTIMP</t>
         </is>
       </c>
-      <c r="C49" s="47" t="n">
-        <v>45839</v>
+      <c r="C49" s="48" t="n">
+        <v>45870</v>
       </c>
       <c r="D49" s="6" t="inlineStr">
         <is>
@@ -4379,19 +4379,19 @@
         </is>
       </c>
       <c r="F49" s="38" t="n">
-        <v>0.05915816447026589</v>
+        <v>-0.05121586816666479</v>
       </c>
       <c r="G49" s="38" t="n">
+        <v>0.05910207359123332</v>
+      </c>
+      <c r="H49" s="38" t="n">
         <v>-0.03632939409284619</v>
       </c>
-      <c r="H49" s="38" t="n">
+      <c r="I49" s="38" t="n">
         <v>-0.001338155618122783</v>
       </c>
-      <c r="I49" s="38" t="n">
+      <c r="J49" s="38" t="n">
         <v>-0.1619854623547367</v>
-      </c>
-      <c r="J49" s="38" t="n">
-        <v>0.04692835742024903</v>
       </c>
       <c r="K49" s="5" t="n"/>
       <c r="L49" s="28" t="inlineStr">
@@ -4405,7 +4405,7 @@
         </is>
       </c>
       <c r="N49" s="48" t="n">
-        <v>45978</v>
+        <v>45979</v>
       </c>
       <c r="O49" s="6" t="inlineStr">
         <is>
@@ -4418,19 +4418,19 @@
         </is>
       </c>
       <c r="Q49" s="6" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="R49" s="6" t="n">
         <v>3.72</v>
-      </c>
-      <c r="R49" s="6" t="n">
-        <v/>
       </c>
       <c r="S49" s="6" t="n">
         <v/>
       </c>
       <c r="T49" s="6" t="n">
+        <v/>
+      </c>
+      <c r="U49" s="21" t="n">
         <v>3.74</v>
-      </c>
-      <c r="U49" s="21" t="n">
-        <v>3.71</v>
       </c>
     </row>
     <row r="50">
@@ -4444,8 +4444,8 @@
           <t>BOPSTB</t>
         </is>
       </c>
-      <c r="C50" s="47" t="n">
-        <v>45839</v>
+      <c r="C50" s="48" t="n">
+        <v>45870</v>
       </c>
       <c r="D50" s="6" t="inlineStr">
         <is>
@@ -4458,19 +4458,19 @@
         </is>
       </c>
       <c r="F50" s="24" t="n">
-        <v>25565</v>
+        <v>26058</v>
       </c>
       <c r="G50" s="24" t="n">
+        <v>25569</v>
+      </c>
+      <c r="H50" s="24" t="n">
         <v>26631</v>
       </c>
-      <c r="H50" s="24" t="n">
+      <c r="I50" s="24" t="n">
         <v>26236</v>
       </c>
-      <c r="I50" s="24" t="n">
+      <c r="J50" s="24" t="n">
         <v>26721</v>
-      </c>
-      <c r="J50" s="24" t="n">
-        <v>26097</v>
       </c>
       <c r="K50" s="5" t="n"/>
       <c r="L50" s="28" t="inlineStr">
@@ -4484,7 +4484,7 @@
         </is>
       </c>
       <c r="N50" s="48" t="n">
-        <v>45978</v>
+        <v>45979</v>
       </c>
       <c r="O50" s="6" t="inlineStr">
         <is>
@@ -4497,19 +4497,19 @@
         </is>
       </c>
       <c r="Q50" s="6" t="n">
+        <v>4.12</v>
+      </c>
+      <c r="R50" s="6" t="n">
         <v>4.13</v>
-      </c>
-      <c r="R50" s="6" t="n">
-        <v/>
       </c>
       <c r="S50" s="6" t="n">
         <v/>
       </c>
       <c r="T50" s="6" t="n">
+        <v/>
+      </c>
+      <c r="U50" s="21" t="n">
         <v>4.14</v>
-      </c>
-      <c r="U50" s="21" t="n">
-        <v>4.11</v>
       </c>
     </row>
     <row r="51" ht="31.5" customHeight="1">
@@ -4519,8 +4519,8 @@
           <t>BOPSTB</t>
         </is>
       </c>
-      <c r="C51" s="47" t="n">
-        <v>45839</v>
+      <c r="C51" s="48" t="n">
+        <v>45870</v>
       </c>
       <c r="D51" s="6" t="inlineStr">
         <is>
@@ -4533,19 +4533,19 @@
         </is>
       </c>
       <c r="F51" s="38" t="n">
-        <v>-0.04002853816980212</v>
+        <v>0.01912472134225029</v>
       </c>
       <c r="G51" s="38" t="n">
+        <v>-0.03987833727610679</v>
+      </c>
+      <c r="H51" s="38" t="n">
         <v>0.01505564872693999</v>
       </c>
-      <c r="H51" s="38" t="n">
+      <c r="I51" s="38" t="n">
         <v>-0.01815051831892522</v>
       </c>
-      <c r="I51" s="38" t="n">
+      <c r="J51" s="38" t="n">
         <v>0.02391079434417742</v>
-      </c>
-      <c r="J51" s="38" t="n">
-        <v>-0.03028388822829964</v>
       </c>
       <c r="K51" s="5" t="n"/>
       <c r="L51" s="28" t="inlineStr">
@@ -4558,7 +4558,7 @@
           <t>MORTGAGE30US</t>
         </is>
       </c>
-      <c r="N51" s="48" t="n">
+      <c r="N51" s="47" t="n">
         <v>45971</v>
       </c>
       <c r="O51" s="6" t="inlineStr">
@@ -4610,7 +4610,7 @@
         </is>
       </c>
       <c r="N52" s="49" t="n">
-        <v>45978</v>
+        <v>45979</v>
       </c>
       <c r="O52" s="9" t="inlineStr">
         <is>
@@ -4623,19 +4623,19 @@
         </is>
       </c>
       <c r="Q52" s="9" t="n">
+        <v>5.91</v>
+      </c>
+      <c r="R52" s="9" t="n">
         <v>5.9</v>
-      </c>
-      <c r="R52" s="9" t="n">
-        <v/>
       </c>
       <c r="S52" s="9" t="n">
         <v/>
       </c>
       <c r="T52" s="9" t="n">
+        <v/>
+      </c>
+      <c r="U52" s="22" t="n">
         <v>5.91</v>
-      </c>
-      <c r="U52" s="22" t="n">
-        <v>5.88</v>
       </c>
     </row>
     <row r="53" ht="21" customHeight="1">

</xml_diff>

<commit_message>
Update dashboards - 2025-11-21
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -1722,10 +1722,10 @@
         <v>229000</v>
       </c>
       <c r="T13" s="24" t="n">
-        <v/>
+        <v>220000</v>
       </c>
       <c r="U13" s="26" t="n">
-        <v/>
+        <v>232000</v>
       </c>
     </row>
     <row r="14">
@@ -1797,10 +1797,10 @@
         <v>1964000</v>
       </c>
       <c r="T14" s="24" t="n">
-        <v/>
+        <v>1957000</v>
       </c>
       <c r="U14" s="26" t="n">
-        <v/>
+        <v>1947000</v>
       </c>
     </row>
     <row r="15">
@@ -2903,7 +2903,7 @@
         </is>
       </c>
       <c r="N29" s="48" t="n">
-        <v>45980</v>
+        <v>45981</v>
       </c>
       <c r="O29" s="6" t="inlineStr">
         <is>
@@ -2916,16 +2916,16 @@
         </is>
       </c>
       <c r="Q29" s="6" t="n">
-        <v>2.18</v>
+        <v>2.14</v>
       </c>
       <c r="R29" s="6" t="n">
         <v>2.18</v>
       </c>
       <c r="S29" s="6" t="n">
+        <v>2.18</v>
+      </c>
+      <c r="T29" s="6" t="n">
         <v>2.19</v>
-      </c>
-      <c r="T29" s="6" t="n">
-        <v/>
       </c>
       <c r="U29" s="21" t="n">
         <v/>
@@ -2982,7 +2982,7 @@
         </is>
       </c>
       <c r="N30" s="48" t="n">
-        <v>45980</v>
+        <v>45981</v>
       </c>
       <c r="O30" s="6" t="inlineStr">
         <is>
@@ -2995,16 +2995,16 @@
         </is>
       </c>
       <c r="Q30" s="6" t="n">
-        <v>2.27</v>
+        <v>2.24</v>
       </c>
       <c r="R30" s="6" t="n">
         <v>2.27</v>
       </c>
       <c r="S30" s="6" t="n">
+        <v>2.27</v>
+      </c>
+      <c r="T30" s="6" t="n">
         <v>2.28</v>
-      </c>
-      <c r="T30" s="6" t="n">
-        <v/>
       </c>
       <c r="U30" s="21" t="n">
         <v/>
@@ -3660,7 +3660,7 @@
           <t>DTWEXBGS</t>
         </is>
       </c>
-      <c r="N39" s="48" t="n">
+      <c r="N39" s="47" t="n">
         <v>45975</v>
       </c>
       <c r="O39" s="6" t="inlineStr">
@@ -3853,7 +3853,7 @@
         </is>
       </c>
       <c r="C42" s="47" t="n">
-        <v>45901</v>
+        <v>45931</v>
       </c>
       <c r="D42" s="6" t="inlineStr">
         <is>
@@ -3866,19 +3866,19 @@
         </is>
       </c>
       <c r="F42" s="39" t="n">
-        <v>4060000</v>
+        <v>4100000</v>
       </c>
       <c r="G42" s="39" t="n">
+        <v>4050000</v>
+      </c>
+      <c r="H42" s="39" t="n">
         <v>4000000</v>
       </c>
-      <c r="H42" s="39" t="n">
+      <c r="I42" s="39" t="n">
         <v>4010000</v>
       </c>
-      <c r="I42" s="39" t="n">
+      <c r="J42" s="39" t="n">
         <v>3930000</v>
-      </c>
-      <c r="J42" s="39" t="n">
-        <v>4040000</v>
       </c>
       <c r="K42" s="7" t="n"/>
       <c r="L42" s="28" t="n"/>
@@ -3924,7 +3924,7 @@
         </is>
       </c>
       <c r="C43" s="47" t="n">
-        <v>45901</v>
+        <v>45931</v>
       </c>
       <c r="D43" s="6" t="inlineStr">
         <is>
@@ -3937,7 +3937,7 @@
         </is>
       </c>
       <c r="F43" s="38" t="n">
-        <v>0.04102564102564103</v>
+        <v>0.0173697270471464</v>
       </c>
       <c r="G43" s="38" t="n">
         <v/>
@@ -4251,7 +4251,7 @@
         </is>
       </c>
       <c r="N47" s="48" t="n">
-        <v>45979</v>
+        <v>45980</v>
       </c>
       <c r="O47" s="6" t="inlineStr">
         <is>
@@ -4330,7 +4330,7 @@
         </is>
       </c>
       <c r="N48" s="48" t="n">
-        <v>45979</v>
+        <v>45980</v>
       </c>
       <c r="O48" s="6" t="inlineStr">
         <is>
@@ -4346,16 +4346,16 @@
         <v>3.58</v>
       </c>
       <c r="R48" s="6" t="n">
+        <v>3.58</v>
+      </c>
+      <c r="S48" s="6" t="n">
         <v>3.6</v>
-      </c>
-      <c r="S48" s="6" t="n">
-        <v/>
       </c>
       <c r="T48" s="6" t="n">
         <v/>
       </c>
       <c r="U48" s="21" t="n">
-        <v>3.62</v>
+        <v/>
       </c>
     </row>
     <row r="49">
@@ -4405,7 +4405,7 @@
         </is>
       </c>
       <c r="N49" s="48" t="n">
-        <v>45979</v>
+        <v>45980</v>
       </c>
       <c r="O49" s="6" t="inlineStr">
         <is>
@@ -4418,19 +4418,19 @@
         </is>
       </c>
       <c r="Q49" s="6" t="n">
+        <v>3.71</v>
+      </c>
+      <c r="R49" s="6" t="n">
         <v>3.7</v>
       </c>
-      <c r="R49" s="6" t="n">
+      <c r="S49" s="6" t="n">
         <v>3.72</v>
-      </c>
-      <c r="S49" s="6" t="n">
-        <v/>
       </c>
       <c r="T49" s="6" t="n">
         <v/>
       </c>
       <c r="U49" s="21" t="n">
-        <v>3.74</v>
+        <v/>
       </c>
     </row>
     <row r="50">
@@ -4484,7 +4484,7 @@
         </is>
       </c>
       <c r="N50" s="48" t="n">
-        <v>45979</v>
+        <v>45980</v>
       </c>
       <c r="O50" s="6" t="inlineStr">
         <is>
@@ -4497,19 +4497,19 @@
         </is>
       </c>
       <c r="Q50" s="6" t="n">
+        <v>4.13</v>
+      </c>
+      <c r="R50" s="6" t="n">
         <v>4.12</v>
       </c>
-      <c r="R50" s="6" t="n">
+      <c r="S50" s="6" t="n">
         <v>4.13</v>
-      </c>
-      <c r="S50" s="6" t="n">
-        <v/>
       </c>
       <c r="T50" s="6" t="n">
         <v/>
       </c>
       <c r="U50" s="21" t="n">
-        <v>4.14</v>
+        <v/>
       </c>
     </row>
     <row r="51" ht="31.5" customHeight="1">
@@ -4558,8 +4558,8 @@
           <t>MORTGAGE30US</t>
         </is>
       </c>
-      <c r="N51" s="47" t="n">
-        <v>45971</v>
+      <c r="N51" s="48" t="n">
+        <v>45978</v>
       </c>
       <c r="O51" s="6" t="inlineStr">
         <is>
@@ -4572,19 +4572,19 @@
         </is>
       </c>
       <c r="Q51" s="6" t="n">
+        <v>6.26</v>
+      </c>
+      <c r="R51" s="6" t="n">
         <v>6.24</v>
       </c>
-      <c r="R51" s="6" t="n">
+      <c r="S51" s="6" t="n">
         <v>6.22</v>
       </c>
-      <c r="S51" s="6" t="n">
+      <c r="T51" s="6" t="n">
         <v>6.17</v>
       </c>
-      <c r="T51" s="6" t="n">
+      <c r="U51" s="21" t="n">
         <v>6.19</v>
-      </c>
-      <c r="U51" s="21" t="n">
-        <v>6.27</v>
       </c>
     </row>
     <row r="52" ht="16.15" customHeight="1" thickBot="1">
@@ -4610,7 +4610,7 @@
         </is>
       </c>
       <c r="N52" s="49" t="n">
-        <v>45979</v>
+        <v>45980</v>
       </c>
       <c r="O52" s="9" t="inlineStr">
         <is>
@@ -4623,19 +4623,19 @@
         </is>
       </c>
       <c r="Q52" s="9" t="n">
+        <v>5.92</v>
+      </c>
+      <c r="R52" s="9" t="n">
         <v>5.91</v>
       </c>
-      <c r="R52" s="9" t="n">
+      <c r="S52" s="9" t="n">
         <v>5.9</v>
-      </c>
-      <c r="S52" s="9" t="n">
-        <v/>
       </c>
       <c r="T52" s="9" t="n">
         <v/>
       </c>
       <c r="U52" s="22" t="n">
-        <v>5.91</v>
+        <v/>
       </c>
     </row>
     <row r="53" ht="21" customHeight="1">

</xml_diff>

<commit_message>
Update dashboards - 2025-11-22
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -2827,8 +2827,8 @@
           <t>UMCSENT</t>
         </is>
       </c>
-      <c r="N28" s="47" t="n">
-        <v>45901</v>
+      <c r="N28" s="48" t="n">
+        <v>45931</v>
       </c>
       <c r="O28" s="6" t="inlineStr">
         <is>
@@ -2841,19 +2841,19 @@
         </is>
       </c>
       <c r="Q28" s="6" t="n">
+        <v>53.6</v>
+      </c>
+      <c r="R28" s="6" t="n">
         <v>55.1</v>
       </c>
-      <c r="R28" s="6" t="n">
+      <c r="S28" s="6" t="n">
         <v>58.2</v>
       </c>
-      <c r="S28" s="6" t="n">
+      <c r="T28" s="6" t="n">
         <v>61.7</v>
       </c>
-      <c r="T28" s="6" t="n">
+      <c r="U28" s="21" t="n">
         <v>60.7</v>
-      </c>
-      <c r="U28" s="21" t="n">
-        <v>52.2</v>
       </c>
     </row>
     <row r="29">
@@ -2903,7 +2903,7 @@
         </is>
       </c>
       <c r="N29" s="48" t="n">
-        <v>45981</v>
+        <v>45982</v>
       </c>
       <c r="O29" s="6" t="inlineStr">
         <is>
@@ -2916,19 +2916,19 @@
         </is>
       </c>
       <c r="Q29" s="6" t="n">
+        <v>2.16</v>
+      </c>
+      <c r="R29" s="6" t="n">
         <v>2.14</v>
-      </c>
-      <c r="R29" s="6" t="n">
-        <v>2.18</v>
       </c>
       <c r="S29" s="6" t="n">
         <v>2.18</v>
       </c>
       <c r="T29" s="6" t="n">
+        <v>2.18</v>
+      </c>
+      <c r="U29" s="21" t="n">
         <v>2.19</v>
-      </c>
-      <c r="U29" s="21" t="n">
-        <v/>
       </c>
     </row>
     <row r="30">
@@ -2982,7 +2982,7 @@
         </is>
       </c>
       <c r="N30" s="48" t="n">
-        <v>45981</v>
+        <v>45982</v>
       </c>
       <c r="O30" s="6" t="inlineStr">
         <is>
@@ -2998,16 +2998,16 @@
         <v>2.24</v>
       </c>
       <c r="R30" s="6" t="n">
-        <v>2.27</v>
+        <v>2.24</v>
       </c>
       <c r="S30" s="6" t="n">
         <v>2.27</v>
       </c>
       <c r="T30" s="6" t="n">
+        <v>2.27</v>
+      </c>
+      <c r="U30" s="21" t="n">
         <v>2.28</v>
-      </c>
-      <c r="U30" s="21" t="n">
-        <v/>
       </c>
     </row>
     <row r="31">
@@ -4251,7 +4251,7 @@
         </is>
       </c>
       <c r="N47" s="48" t="n">
-        <v>45980</v>
+        <v>45981</v>
       </c>
       <c r="O47" s="6" t="inlineStr">
         <is>
@@ -4330,7 +4330,7 @@
         </is>
       </c>
       <c r="N48" s="48" t="n">
-        <v>45980</v>
+        <v>45981</v>
       </c>
       <c r="O48" s="6" t="inlineStr">
         <is>
@@ -4343,16 +4343,16 @@
         </is>
       </c>
       <c r="Q48" s="6" t="n">
-        <v>3.58</v>
+        <v>3.55</v>
       </c>
       <c r="R48" s="6" t="n">
         <v>3.58</v>
       </c>
       <c r="S48" s="6" t="n">
+        <v>3.58</v>
+      </c>
+      <c r="T48" s="6" t="n">
         <v>3.6</v>
-      </c>
-      <c r="T48" s="6" t="n">
-        <v/>
       </c>
       <c r="U48" s="21" t="n">
         <v/>
@@ -4405,7 +4405,7 @@
         </is>
       </c>
       <c r="N49" s="48" t="n">
-        <v>45980</v>
+        <v>45981</v>
       </c>
       <c r="O49" s="6" t="inlineStr">
         <is>
@@ -4418,16 +4418,16 @@
         </is>
       </c>
       <c r="Q49" s="6" t="n">
+        <v>3.68</v>
+      </c>
+      <c r="R49" s="6" t="n">
         <v>3.71</v>
       </c>
-      <c r="R49" s="6" t="n">
+      <c r="S49" s="6" t="n">
         <v>3.7</v>
       </c>
-      <c r="S49" s="6" t="n">
+      <c r="T49" s="6" t="n">
         <v>3.72</v>
-      </c>
-      <c r="T49" s="6" t="n">
-        <v/>
       </c>
       <c r="U49" s="21" t="n">
         <v/>
@@ -4484,7 +4484,7 @@
         </is>
       </c>
       <c r="N50" s="48" t="n">
-        <v>45980</v>
+        <v>45981</v>
       </c>
       <c r="O50" s="6" t="inlineStr">
         <is>
@@ -4497,16 +4497,16 @@
         </is>
       </c>
       <c r="Q50" s="6" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="R50" s="6" t="n">
         <v>4.13</v>
       </c>
-      <c r="R50" s="6" t="n">
+      <c r="S50" s="6" t="n">
         <v>4.12</v>
       </c>
-      <c r="S50" s="6" t="n">
+      <c r="T50" s="6" t="n">
         <v>4.13</v>
-      </c>
-      <c r="T50" s="6" t="n">
-        <v/>
       </c>
       <c r="U50" s="21" t="n">
         <v/>
@@ -4610,7 +4610,7 @@
         </is>
       </c>
       <c r="N52" s="49" t="n">
-        <v>45980</v>
+        <v>45981</v>
       </c>
       <c r="O52" s="9" t="inlineStr">
         <is>
@@ -4623,16 +4623,16 @@
         </is>
       </c>
       <c r="Q52" s="9" t="n">
+        <v>5.9</v>
+      </c>
+      <c r="R52" s="9" t="n">
         <v>5.92</v>
       </c>
-      <c r="R52" s="9" t="n">
+      <c r="S52" s="9" t="n">
         <v>5.91</v>
       </c>
-      <c r="S52" s="9" t="n">
+      <c r="T52" s="9" t="n">
         <v>5.9</v>
-      </c>
-      <c r="T52" s="9" t="n">
-        <v/>
       </c>
       <c r="U52" s="22" t="n">
         <v/>

</xml_diff>

<commit_message>
Update dashboards - 2025-11-25
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -1940,8 +1940,8 @@
           <t>RSAFS</t>
         </is>
       </c>
-      <c r="C17" s="47" t="n">
-        <v>45870</v>
+      <c r="C17" s="48" t="n">
+        <v>45901</v>
       </c>
       <c r="D17" s="6" t="inlineStr">
         <is>
@@ -1954,19 +1954,19 @@
         </is>
       </c>
       <c r="F17" s="25" t="n">
-        <v>0.006318272675532866</v>
+        <v>0.001637846129888487</v>
       </c>
       <c r="G17" s="25" t="n">
-        <v>0.006059197851273623</v>
+        <v>0.005952781743703284</v>
       </c>
       <c r="H17" s="25" t="n">
+        <v>0.006492096487988874</v>
+      </c>
+      <c r="I17" s="25" t="n">
         <v>0.009680198742914703</v>
       </c>
-      <c r="I17" s="25" t="n">
+      <c r="J17" s="25" t="n">
         <v>-0.007880419346928291</v>
-      </c>
-      <c r="J17" s="25" t="n">
-        <v>-0.001083629036276013</v>
       </c>
       <c r="K17" s="5" t="n"/>
       <c r="L17" s="29" t="inlineStr">
@@ -2027,8 +2027,8 @@
           <t>RSAFS</t>
         </is>
       </c>
-      <c r="C18" s="47" t="n">
-        <v>45870</v>
+      <c r="C18" s="48" t="n">
+        <v>45901</v>
       </c>
       <c r="D18" s="6" t="inlineStr">
         <is>
@@ -2041,19 +2041,19 @@
         </is>
       </c>
       <c r="F18" s="25" t="n">
-        <v>0.04999304317391922</v>
+        <v>0.04261856857461769</v>
       </c>
       <c r="G18" s="25" t="n">
-        <v>0.04089520416121116</v>
+        <v>0.05024109124453582</v>
       </c>
       <c r="H18" s="25" t="n">
+        <v>0.04134309243240536</v>
+      </c>
+      <c r="I18" s="25" t="n">
         <v>0.0441678737351054</v>
       </c>
-      <c r="I18" s="25" t="n">
+      <c r="J18" s="25" t="n">
         <v>0.03367187567662758</v>
-      </c>
-      <c r="J18" s="25" t="n">
-        <v>0.04971916893784486</v>
       </c>
       <c r="K18" s="5" t="n"/>
       <c r="L18" s="28" t="inlineStr">
@@ -2788,7 +2788,7 @@
           <t>DGORDER</t>
         </is>
       </c>
-      <c r="C28" s="48" t="n">
+      <c r="C28" s="47" t="n">
         <v>45870</v>
       </c>
       <c r="D28" s="6" t="inlineStr">
@@ -2863,7 +2863,7 @@
           <t>DGORDER</t>
         </is>
       </c>
-      <c r="C29" s="48" t="n">
+      <c r="C29" s="47" t="n">
         <v>45870</v>
       </c>
       <c r="D29" s="6" t="inlineStr">
@@ -2903,7 +2903,7 @@
         </is>
       </c>
       <c r="N29" s="48" t="n">
-        <v>45982</v>
+        <v>45985</v>
       </c>
       <c r="O29" s="6" t="inlineStr">
         <is>
@@ -2919,16 +2919,16 @@
         <v>2.16</v>
       </c>
       <c r="R29" s="6" t="n">
+        <v>2.16</v>
+      </c>
+      <c r="S29" s="6" t="n">
         <v>2.14</v>
-      </c>
-      <c r="S29" s="6" t="n">
-        <v>2.18</v>
       </c>
       <c r="T29" s="6" t="n">
         <v>2.18</v>
       </c>
       <c r="U29" s="21" t="n">
-        <v>2.19</v>
+        <v>2.18</v>
       </c>
     </row>
     <row r="30">
@@ -2942,7 +2942,7 @@
           <t>ADXDNO</t>
         </is>
       </c>
-      <c r="C30" s="48" t="n">
+      <c r="C30" s="47" t="n">
         <v>45870</v>
       </c>
       <c r="D30" s="6" t="inlineStr">
@@ -2982,7 +2982,7 @@
         </is>
       </c>
       <c r="N30" s="48" t="n">
-        <v>45982</v>
+        <v>45985</v>
       </c>
       <c r="O30" s="6" t="inlineStr">
         <is>
@@ -2995,19 +2995,19 @@
         </is>
       </c>
       <c r="Q30" s="6" t="n">
-        <v>2.24</v>
+        <v>2.23</v>
       </c>
       <c r="R30" s="6" t="n">
         <v>2.24</v>
       </c>
       <c r="S30" s="6" t="n">
-        <v>2.27</v>
+        <v>2.24</v>
       </c>
       <c r="T30" s="6" t="n">
         <v>2.27</v>
       </c>
       <c r="U30" s="21" t="n">
-        <v>2.28</v>
+        <v>2.27</v>
       </c>
     </row>
     <row r="31">
@@ -3017,7 +3017,7 @@
           <t>ADXDNO</t>
         </is>
       </c>
-      <c r="C31" s="48" t="n">
+      <c r="C31" s="47" t="n">
         <v>45870</v>
       </c>
       <c r="D31" s="6" t="inlineStr">
@@ -3096,7 +3096,7 @@
           <t>INDPRO</t>
         </is>
       </c>
-      <c r="C32" s="47" t="n">
+      <c r="C32" s="48" t="n">
         <v>45870</v>
       </c>
       <c r="D32" s="6" t="inlineStr">
@@ -3110,19 +3110,19 @@
         </is>
       </c>
       <c r="F32" s="25" t="n">
-        <v>0.0009718800147178186</v>
+        <v>-0.0007577910391209919</v>
       </c>
       <c r="G32" s="25" t="n">
-        <v>-0.003762540602524678</v>
+        <v>-0.002144439521488684</v>
       </c>
       <c r="H32" s="25" t="n">
-        <v>0.005349373414241132</v>
+        <v>0.00424479189840965</v>
       </c>
       <c r="I32" s="25" t="n">
-        <v>0.0003339046383792343</v>
+        <v>-0.001038119019209582</v>
       </c>
       <c r="J32" s="25" t="n">
-        <v>0.000788095127717714</v>
+        <v>0.001983365069813559</v>
       </c>
       <c r="K32" s="5" t="n"/>
       <c r="L32" s="28" t="n"/>
@@ -3167,7 +3167,7 @@
           <t>INDPRO</t>
         </is>
       </c>
-      <c r="C33" s="47" t="n">
+      <c r="C33" s="48" t="n">
         <v>45870</v>
       </c>
       <c r="D33" s="6" t="inlineStr">
@@ -3181,19 +3181,19 @@
         </is>
       </c>
       <c r="F33" s="25" t="n">
-        <v>0.008742996478340049</v>
+        <v>0.008358981150223696</v>
       </c>
       <c r="G33" s="25" t="n">
-        <v>0.01268250239955056</v>
+        <v>0.01371833355505385</v>
       </c>
       <c r="H33" s="25" t="n">
-        <v>0.009279113327018787</v>
+        <v>0.006650544135429186</v>
       </c>
       <c r="I33" s="25" t="n">
-        <v>0.006577024403838839</v>
+        <v>0.00270366735076292</v>
       </c>
       <c r="J33" s="25" t="n">
-        <v>0.01236459131195966</v>
+        <v>0.009949782230052044</v>
       </c>
       <c r="K33" s="5" t="n"/>
       <c r="L33" s="28" t="inlineStr">
@@ -3246,7 +3246,7 @@
           <t>TCU</t>
         </is>
       </c>
-      <c r="C34" s="47" t="n">
+      <c r="C34" s="48" t="n">
         <v>45870</v>
       </c>
       <c r="D34" s="6" t="inlineStr">
@@ -3260,19 +3260,19 @@
         </is>
       </c>
       <c r="F34" s="24" t="n">
-        <v>77.376</v>
+        <v>75.84010000000001</v>
       </c>
       <c r="G34" s="24" t="n">
-        <v>77.3974</v>
+        <v>75.9897</v>
       </c>
       <c r="H34" s="24" t="n">
-        <v>77.78830000000001</v>
+        <v>76.246</v>
       </c>
       <c r="I34" s="24" t="n">
-        <v>77.4743</v>
+        <v>76.01730000000001</v>
       </c>
       <c r="J34" s="24" t="n">
-        <v>77.5487</v>
+        <v>76.18980000000001</v>
       </c>
       <c r="K34" s="5" t="n"/>
       <c r="L34" s="28" t="n"/>
@@ -3510,8 +3510,8 @@
           <t>CSUSHPINSA</t>
         </is>
       </c>
-      <c r="N37" s="47" t="n">
-        <v>45870</v>
+      <c r="N37" s="48" t="n">
+        <v>45901</v>
       </c>
       <c r="O37" s="6" t="inlineStr">
         <is>
@@ -3524,19 +3524,19 @@
         </is>
       </c>
       <c r="Q37" s="38" t="n">
-        <v>-0.002963719362060191</v>
+        <v>-0.002680233580537372</v>
       </c>
       <c r="R37" s="38" t="n">
-        <v>-0.002056167749521443</v>
+        <v>-0.003492679271734134</v>
       </c>
       <c r="S37" s="38" t="n">
-        <v>0.0006848529828815675</v>
+        <v>-0.002089419937226888</v>
       </c>
       <c r="T37" s="38" t="n">
-        <v>0.004670871764716811</v>
+        <v>0.0006667672348770193</v>
       </c>
       <c r="U37" s="23" t="n">
-        <v>0.006620960680036703</v>
+        <v>0.004670985029205044</v>
       </c>
     </row>
     <row r="38">
@@ -3585,8 +3585,8 @@
           <t>CSUSHPINSA</t>
         </is>
       </c>
-      <c r="N38" s="47" t="n">
-        <v>45870</v>
+      <c r="N38" s="48" t="n">
+        <v>45901</v>
       </c>
       <c r="O38" s="6" t="inlineStr">
         <is>
@@ -3599,19 +3599,19 @@
         </is>
       </c>
       <c r="Q38" s="38" t="n">
-        <v>0.01509936545139687</v>
+        <v>0.01291790739138332</v>
       </c>
       <c r="R38" s="38" t="n">
-        <v>0.01637547210366313</v>
+        <v>0.01449043557431158</v>
       </c>
       <c r="S38" s="38" t="n">
-        <v>0.019477605517784</v>
+        <v>0.01630494859795866</v>
       </c>
       <c r="T38" s="38" t="n">
-        <v>0.02366620855788388</v>
+        <v>0.01943770804710052</v>
       </c>
       <c r="U38" s="23" t="n">
-        <v>0.02826572083977447</v>
+        <v>0.02364466296472451</v>
       </c>
     </row>
     <row r="39" ht="31.5" customHeight="1">
@@ -3660,8 +3660,8 @@
           <t>DTWEXBGS</t>
         </is>
       </c>
-      <c r="N39" s="47" t="n">
-        <v>45975</v>
+      <c r="N39" s="48" t="n">
+        <v>45982</v>
       </c>
       <c r="O39" s="6" t="inlineStr">
         <is>
@@ -3674,19 +3674,19 @@
         </is>
       </c>
       <c r="Q39" s="6" t="n">
-        <v>121.363</v>
+        <v>122.235</v>
       </c>
       <c r="R39" s="6" t="n">
-        <v>121.1756</v>
+        <v>122.0735</v>
       </c>
       <c r="S39" s="6" t="n">
-        <v>121.4459</v>
+        <v>121.8845</v>
       </c>
       <c r="T39" s="6" t="n">
-        <v/>
+        <v>121.6042</v>
       </c>
       <c r="U39" s="21" t="n">
-        <v>121.6932</v>
+        <v>121.5131</v>
       </c>
     </row>
     <row r="40">
@@ -4251,7 +4251,7 @@
         </is>
       </c>
       <c r="N47" s="48" t="n">
-        <v>45981</v>
+        <v>45982</v>
       </c>
       <c r="O47" s="6" t="inlineStr">
         <is>
@@ -4330,7 +4330,7 @@
         </is>
       </c>
       <c r="N48" s="48" t="n">
-        <v>45981</v>
+        <v>45982</v>
       </c>
       <c r="O48" s="6" t="inlineStr">
         <is>
@@ -4343,19 +4343,19 @@
         </is>
       </c>
       <c r="Q48" s="6" t="n">
+        <v>3.51</v>
+      </c>
+      <c r="R48" s="6" t="n">
         <v>3.55</v>
-      </c>
-      <c r="R48" s="6" t="n">
-        <v>3.58</v>
       </c>
       <c r="S48" s="6" t="n">
         <v>3.58</v>
       </c>
       <c r="T48" s="6" t="n">
+        <v>3.58</v>
+      </c>
+      <c r="U48" s="21" t="n">
         <v>3.6</v>
-      </c>
-      <c r="U48" s="21" t="n">
-        <v/>
       </c>
     </row>
     <row r="49">
@@ -4405,7 +4405,7 @@
         </is>
       </c>
       <c r="N49" s="48" t="n">
-        <v>45981</v>
+        <v>45982</v>
       </c>
       <c r="O49" s="6" t="inlineStr">
         <is>
@@ -4418,19 +4418,19 @@
         </is>
       </c>
       <c r="Q49" s="6" t="n">
+        <v>3.62</v>
+      </c>
+      <c r="R49" s="6" t="n">
         <v>3.68</v>
       </c>
-      <c r="R49" s="6" t="n">
+      <c r="S49" s="6" t="n">
         <v>3.71</v>
       </c>
-      <c r="S49" s="6" t="n">
+      <c r="T49" s="6" t="n">
         <v>3.7</v>
       </c>
-      <c r="T49" s="6" t="n">
+      <c r="U49" s="21" t="n">
         <v>3.72</v>
-      </c>
-      <c r="U49" s="21" t="n">
-        <v/>
       </c>
     </row>
     <row r="50">
@@ -4484,7 +4484,7 @@
         </is>
       </c>
       <c r="N50" s="48" t="n">
-        <v>45981</v>
+        <v>45982</v>
       </c>
       <c r="O50" s="6" t="inlineStr">
         <is>
@@ -4497,19 +4497,19 @@
         </is>
       </c>
       <c r="Q50" s="6" t="n">
+        <v>4.06</v>
+      </c>
+      <c r="R50" s="6" t="n">
         <v>4.1</v>
       </c>
-      <c r="R50" s="6" t="n">
+      <c r="S50" s="6" t="n">
         <v>4.13</v>
       </c>
-      <c r="S50" s="6" t="n">
+      <c r="T50" s="6" t="n">
         <v>4.12</v>
       </c>
-      <c r="T50" s="6" t="n">
+      <c r="U50" s="21" t="n">
         <v>4.13</v>
-      </c>
-      <c r="U50" s="21" t="n">
-        <v/>
       </c>
     </row>
     <row r="51" ht="31.5" customHeight="1">
@@ -4610,7 +4610,7 @@
         </is>
       </c>
       <c r="N52" s="49" t="n">
-        <v>45981</v>
+        <v>45982</v>
       </c>
       <c r="O52" s="9" t="inlineStr">
         <is>
@@ -4623,19 +4623,19 @@
         </is>
       </c>
       <c r="Q52" s="9" t="n">
+        <v>5.88</v>
+      </c>
+      <c r="R52" s="9" t="n">
         <v>5.9</v>
       </c>
-      <c r="R52" s="9" t="n">
+      <c r="S52" s="9" t="n">
         <v>5.92</v>
       </c>
-      <c r="S52" s="9" t="n">
+      <c r="T52" s="9" t="n">
         <v>5.91</v>
       </c>
-      <c r="T52" s="9" t="n">
+      <c r="U52" s="22" t="n">
         <v>5.9</v>
-      </c>
-      <c r="U52" s="22" t="n">
-        <v/>
       </c>
     </row>
     <row r="53" ht="21" customHeight="1">

</xml_diff>

<commit_message>
Update dashboards - 2025-11-26
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -1194,7 +1194,7 @@
           <t>GDPNOW</t>
         </is>
       </c>
-      <c r="C7" s="48" t="n">
+      <c r="C7" s="47" t="n">
         <v>45839</v>
       </c>
       <c r="D7" s="6" t="inlineStr">
@@ -1700,7 +1700,7 @@
         </is>
       </c>
       <c r="N13" s="48" t="n">
-        <v>45971</v>
+        <v>45978</v>
       </c>
       <c r="O13" s="6" t="inlineStr">
         <is>
@@ -1713,19 +1713,19 @@
         </is>
       </c>
       <c r="Q13" s="24" t="n">
+        <v>216000</v>
+      </c>
+      <c r="R13" s="24" t="n">
+        <v>222000</v>
+      </c>
+      <c r="S13" s="24" t="n">
+        <v>228000</v>
+      </c>
+      <c r="T13" s="24" t="n">
+        <v>229000</v>
+      </c>
+      <c r="U13" s="26" t="n">
         <v>220000</v>
-      </c>
-      <c r="R13" s="24" t="n">
-        <v>228000</v>
-      </c>
-      <c r="S13" s="24" t="n">
-        <v>229000</v>
-      </c>
-      <c r="T13" s="24" t="n">
-        <v>220000</v>
-      </c>
-      <c r="U13" s="26" t="n">
-        <v>232000</v>
       </c>
     </row>
     <row r="14">
@@ -1775,7 +1775,7 @@
         </is>
       </c>
       <c r="N14" s="48" t="n">
-        <v>45964</v>
+        <v>45971</v>
       </c>
       <c r="O14" s="6" t="inlineStr">
         <is>
@@ -1788,19 +1788,19 @@
         </is>
       </c>
       <c r="Q14" s="24" t="n">
-        <v>1974000</v>
+        <v>1960000</v>
       </c>
       <c r="R14" s="24" t="n">
+        <v>1953000</v>
+      </c>
+      <c r="S14" s="24" t="n">
         <v>1946000</v>
       </c>
-      <c r="S14" s="24" t="n">
+      <c r="T14" s="24" t="n">
         <v>1964000</v>
       </c>
-      <c r="T14" s="24" t="n">
+      <c r="U14" s="26" t="n">
         <v>1957000</v>
-      </c>
-      <c r="U14" s="26" t="n">
-        <v>1947000</v>
       </c>
     </row>
     <row r="15">
@@ -2370,8 +2370,8 @@
           <t>PPIFIS</t>
         </is>
       </c>
-      <c r="N22" s="47" t="n">
-        <v>45870</v>
+      <c r="N22" s="48" t="n">
+        <v>45901</v>
       </c>
       <c r="O22" s="6" t="inlineStr">
         <is>
@@ -2384,19 +2384,19 @@
         </is>
       </c>
       <c r="Q22" s="38" t="n">
-        <v>-0.00121199134865857</v>
+        <v>0.003100806343593332</v>
       </c>
       <c r="R22" s="38" t="n">
-        <v>0.006999184102816525</v>
+        <v>-0.001357686982925266</v>
       </c>
       <c r="S22" s="38" t="n">
-        <v>0.0005127271010003653</v>
+        <v>0.0081178572632572</v>
       </c>
       <c r="T22" s="38" t="n">
-        <v>0.00366317728152965</v>
+        <v>0.0007422151749265637</v>
       </c>
       <c r="U22" s="23" t="n">
-        <v>-0.002532739884236856</v>
+        <v>0.003514212586162468</v>
       </c>
     </row>
     <row r="23">
@@ -2440,8 +2440,8 @@
           <t>PPIFIS</t>
         </is>
       </c>
-      <c r="N23" s="47" t="n">
-        <v>45870</v>
+      <c r="N23" s="48" t="n">
+        <v>45901</v>
       </c>
       <c r="O23" s="6" t="inlineStr">
         <is>
@@ -2454,19 +2454,19 @@
         </is>
       </c>
       <c r="Q23" s="38" t="n">
-        <v>0.02614199229499162</v>
+        <v>0.02734717954345914</v>
       </c>
       <c r="R23" s="38" t="n">
-        <v>0.03086926809738459</v>
+        <v>0.02721518987341764</v>
       </c>
       <c r="S23" s="38" t="n">
-        <v>0.02398690869922453</v>
+        <v>0.0320979643678082</v>
       </c>
       <c r="T23" s="38" t="n">
-        <v>0.02753457419153588</v>
+        <v>0.02406976503324603</v>
       </c>
       <c r="U23" s="23" t="n">
-        <v>0.02411794075224681</v>
+        <v>0.02738206647949823</v>
       </c>
     </row>
     <row r="24">
@@ -2903,7 +2903,7 @@
         </is>
       </c>
       <c r="N29" s="48" t="n">
-        <v>45985</v>
+        <v>45986</v>
       </c>
       <c r="O29" s="6" t="inlineStr">
         <is>
@@ -2916,19 +2916,19 @@
         </is>
       </c>
       <c r="Q29" s="6" t="n">
-        <v>2.16</v>
+        <v>2.17</v>
       </c>
       <c r="R29" s="6" t="n">
         <v>2.16</v>
       </c>
       <c r="S29" s="6" t="n">
-        <v>2.14</v>
+        <v/>
       </c>
       <c r="T29" s="6" t="n">
-        <v>2.18</v>
+        <v/>
       </c>
       <c r="U29" s="21" t="n">
-        <v>2.18</v>
+        <v>2.16</v>
       </c>
     </row>
     <row r="30">
@@ -2982,7 +2982,7 @@
         </is>
       </c>
       <c r="N30" s="48" t="n">
-        <v>45985</v>
+        <v>45986</v>
       </c>
       <c r="O30" s="6" t="inlineStr">
         <is>
@@ -2995,19 +2995,19 @@
         </is>
       </c>
       <c r="Q30" s="6" t="n">
+        <v>2.22</v>
+      </c>
+      <c r="R30" s="6" t="n">
         <v>2.23</v>
       </c>
-      <c r="R30" s="6" t="n">
+      <c r="S30" s="6" t="n">
+        <v/>
+      </c>
+      <c r="T30" s="6" t="n">
+        <v/>
+      </c>
+      <c r="U30" s="21" t="n">
         <v>2.24</v>
-      </c>
-      <c r="S30" s="6" t="n">
-        <v>2.24</v>
-      </c>
-      <c r="T30" s="6" t="n">
-        <v>2.27</v>
-      </c>
-      <c r="U30" s="21" t="n">
-        <v>2.27</v>
       </c>
     </row>
     <row r="31">
@@ -4124,7 +4124,7 @@
           <t>BOPTEXP</t>
         </is>
       </c>
-      <c r="C46" s="48" t="n">
+      <c r="C46" s="47" t="n">
         <v>45870</v>
       </c>
       <c r="D46" s="6" t="inlineStr">
@@ -4211,7 +4211,7 @@
           <t>BOPTEXP</t>
         </is>
       </c>
-      <c r="C47" s="48" t="n">
+      <c r="C47" s="47" t="n">
         <v>45870</v>
       </c>
       <c r="D47" s="6" t="inlineStr">
@@ -4251,7 +4251,7 @@
         </is>
       </c>
       <c r="N47" s="48" t="n">
-        <v>45982</v>
+        <v>45985</v>
       </c>
       <c r="O47" s="6" t="inlineStr">
         <is>
@@ -4290,7 +4290,7 @@
           <t>BOPTIMP</t>
         </is>
       </c>
-      <c r="C48" s="48" t="n">
+      <c r="C48" s="47" t="n">
         <v>45870</v>
       </c>
       <c r="D48" s="6" t="inlineStr">
@@ -4330,7 +4330,7 @@
         </is>
       </c>
       <c r="N48" s="48" t="n">
-        <v>45982</v>
+        <v>45985</v>
       </c>
       <c r="O48" s="6" t="inlineStr">
         <is>
@@ -4343,19 +4343,19 @@
         </is>
       </c>
       <c r="Q48" s="6" t="n">
+        <v>3.46</v>
+      </c>
+      <c r="R48" s="6" t="n">
+        <v/>
+      </c>
+      <c r="S48" s="6" t="n">
+        <v/>
+      </c>
+      <c r="T48" s="6" t="n">
         <v>3.51</v>
       </c>
-      <c r="R48" s="6" t="n">
+      <c r="U48" s="21" t="n">
         <v>3.55</v>
-      </c>
-      <c r="S48" s="6" t="n">
-        <v>3.58</v>
-      </c>
-      <c r="T48" s="6" t="n">
-        <v>3.58</v>
-      </c>
-      <c r="U48" s="21" t="n">
-        <v>3.6</v>
       </c>
     </row>
     <row r="49">
@@ -4365,7 +4365,7 @@
           <t>BOPTIMP</t>
         </is>
       </c>
-      <c r="C49" s="48" t="n">
+      <c r="C49" s="47" t="n">
         <v>45870</v>
       </c>
       <c r="D49" s="6" t="inlineStr">
@@ -4405,7 +4405,7 @@
         </is>
       </c>
       <c r="N49" s="48" t="n">
-        <v>45982</v>
+        <v>45985</v>
       </c>
       <c r="O49" s="6" t="inlineStr">
         <is>
@@ -4418,19 +4418,19 @@
         </is>
       </c>
       <c r="Q49" s="6" t="n">
+        <v>3.61</v>
+      </c>
+      <c r="R49" s="6" t="n">
+        <v/>
+      </c>
+      <c r="S49" s="6" t="n">
+        <v/>
+      </c>
+      <c r="T49" s="6" t="n">
         <v>3.62</v>
       </c>
-      <c r="R49" s="6" t="n">
+      <c r="U49" s="21" t="n">
         <v>3.68</v>
-      </c>
-      <c r="S49" s="6" t="n">
-        <v>3.71</v>
-      </c>
-      <c r="T49" s="6" t="n">
-        <v>3.7</v>
-      </c>
-      <c r="U49" s="21" t="n">
-        <v>3.72</v>
       </c>
     </row>
     <row r="50">
@@ -4444,7 +4444,7 @@
           <t>BOPSTB</t>
         </is>
       </c>
-      <c r="C50" s="48" t="n">
+      <c r="C50" s="47" t="n">
         <v>45870</v>
       </c>
       <c r="D50" s="6" t="inlineStr">
@@ -4484,7 +4484,7 @@
         </is>
       </c>
       <c r="N50" s="48" t="n">
-        <v>45982</v>
+        <v>45985</v>
       </c>
       <c r="O50" s="6" t="inlineStr">
         <is>
@@ -4497,19 +4497,19 @@
         </is>
       </c>
       <c r="Q50" s="6" t="n">
+        <v>4.04</v>
+      </c>
+      <c r="R50" s="6" t="n">
+        <v/>
+      </c>
+      <c r="S50" s="6" t="n">
+        <v/>
+      </c>
+      <c r="T50" s="6" t="n">
         <v>4.06</v>
       </c>
-      <c r="R50" s="6" t="n">
+      <c r="U50" s="21" t="n">
         <v>4.1</v>
-      </c>
-      <c r="S50" s="6" t="n">
-        <v>4.13</v>
-      </c>
-      <c r="T50" s="6" t="n">
-        <v>4.12</v>
-      </c>
-      <c r="U50" s="21" t="n">
-        <v>4.13</v>
       </c>
     </row>
     <row r="51" ht="31.5" customHeight="1">
@@ -4519,7 +4519,7 @@
           <t>BOPSTB</t>
         </is>
       </c>
-      <c r="C51" s="48" t="n">
+      <c r="C51" s="47" t="n">
         <v>45870</v>
       </c>
       <c r="D51" s="6" t="inlineStr">
@@ -4610,7 +4610,7 @@
         </is>
       </c>
       <c r="N52" s="49" t="n">
-        <v>45982</v>
+        <v>45985</v>
       </c>
       <c r="O52" s="9" t="inlineStr">
         <is>
@@ -4623,16 +4623,16 @@
         </is>
       </c>
       <c r="Q52" s="9" t="n">
+        <v>5.84</v>
+      </c>
+      <c r="R52" s="9" t="n">
+        <v/>
+      </c>
+      <c r="S52" s="9" t="n">
+        <v/>
+      </c>
+      <c r="T52" s="9" t="n">
         <v>5.88</v>
-      </c>
-      <c r="R52" s="9" t="n">
-        <v>5.9</v>
-      </c>
-      <c r="S52" s="9" t="n">
-        <v>5.92</v>
-      </c>
-      <c r="T52" s="9" t="n">
-        <v>5.91</v>
       </c>
       <c r="U52" s="22" t="n">
         <v>5.9</v>

</xml_diff>

<commit_message>
Update dashboards - 2025-11-27
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -929,7 +929,7 @@
           <t>PAYEMS</t>
         </is>
       </c>
-      <c r="N3" s="48" t="n">
+      <c r="N3" s="47" t="n">
         <v>45901</v>
       </c>
       <c r="O3" s="6" t="inlineStr">
@@ -1000,7 +1000,7 @@
           <t>PAYEMS</t>
         </is>
       </c>
-      <c r="N4" s="48" t="n">
+      <c r="N4" s="47" t="n">
         <v>45901</v>
       </c>
       <c r="O4" s="6" t="inlineStr">
@@ -1154,7 +1154,7 @@
           <t>UNRATE</t>
         </is>
       </c>
-      <c r="N6" s="48" t="n">
+      <c r="N6" s="47" t="n">
         <v>45901</v>
       </c>
       <c r="O6" s="6" t="inlineStr">
@@ -1194,7 +1194,7 @@
           <t>GDPNOW</t>
         </is>
       </c>
-      <c r="C7" s="47" t="n">
+      <c r="C7" s="48" t="n">
         <v>45839</v>
       </c>
       <c r="D7" s="6" t="inlineStr">
@@ -1208,7 +1208,7 @@
         </is>
       </c>
       <c r="F7" s="25" t="n">
-        <v>0.4573742246726396</v>
+        <v>0.3862508614748448</v>
       </c>
       <c r="G7" s="25" t="n">
         <v>-2.062303243282817</v>
@@ -1233,7 +1233,7 @@
           <t>U6RATE</t>
         </is>
       </c>
-      <c r="N7" s="48" t="n">
+      <c r="N7" s="47" t="n">
         <v>45901</v>
       </c>
       <c r="O7" s="6" t="inlineStr">
@@ -1312,7 +1312,7 @@
           <t>CIVPART</t>
         </is>
       </c>
-      <c r="N8" s="48" t="n">
+      <c r="N8" s="47" t="n">
         <v>45901</v>
       </c>
       <c r="O8" s="6" t="inlineStr">
@@ -1391,7 +1391,7 @@
           <t>EMRATIO</t>
         </is>
       </c>
-      <c r="N9" s="48" t="n">
+      <c r="N9" s="47" t="n">
         <v>45901</v>
       </c>
       <c r="O9" s="6" t="inlineStr">
@@ -1853,7 +1853,7 @@
           <t>AWHAETP</t>
         </is>
       </c>
-      <c r="N15" s="48" t="n">
+      <c r="N15" s="47" t="n">
         <v>45901</v>
       </c>
       <c r="O15" s="6" t="inlineStr">
@@ -2788,8 +2788,8 @@
           <t>DGORDER</t>
         </is>
       </c>
-      <c r="C28" s="47" t="n">
-        <v>45870</v>
+      <c r="C28" s="48" t="n">
+        <v>45901</v>
       </c>
       <c r="D28" s="6" t="inlineStr">
         <is>
@@ -2802,19 +2802,19 @@
         </is>
       </c>
       <c r="F28" s="25" t="n">
-        <v>0.02880223870746335</v>
+        <v>0.004840745558111426</v>
       </c>
       <c r="G28" s="25" t="n">
+        <v>0.03006283164814283</v>
+      </c>
+      <c r="H28" s="25" t="n">
         <v>-0.02799901206372835</v>
       </c>
-      <c r="H28" s="25" t="n">
+      <c r="I28" s="25" t="n">
         <v>-0.09389977010425232</v>
       </c>
-      <c r="I28" s="25" t="n">
+      <c r="J28" s="25" t="n">
         <v>0.165430902790715</v>
-      </c>
-      <c r="J28" s="25" t="n">
-        <v>-0.06636623816074505</v>
       </c>
       <c r="K28" s="5" t="n"/>
       <c r="L28" s="28" t="inlineStr">
@@ -2863,8 +2863,8 @@
           <t>DGORDER</t>
         </is>
       </c>
-      <c r="C29" s="47" t="n">
-        <v>45870</v>
+      <c r="C29" s="48" t="n">
+        <v>45901</v>
       </c>
       <c r="D29" s="6" t="inlineStr">
         <is>
@@ -2877,19 +2877,19 @@
         </is>
       </c>
       <c r="F29" s="25" t="n">
-        <v>0.07530887191904141</v>
+        <v>0.07243160813624692</v>
       </c>
       <c r="G29" s="25" t="n">
+        <v>0.07662644950780544</v>
+      </c>
+      <c r="H29" s="25" t="n">
         <v>0.03341358778313566</v>
       </c>
-      <c r="H29" s="25" t="n">
+      <c r="I29" s="25" t="n">
         <v>0.1089645997552716</v>
       </c>
-      <c r="I29" s="25" t="n">
+      <c r="J29" s="25" t="n">
         <v>0.1995614111543812</v>
-      </c>
-      <c r="J29" s="25" t="n">
-        <v>0.02877284194973726</v>
       </c>
       <c r="K29" s="5" t="n"/>
       <c r="L29" s="28" t="inlineStr">
@@ -2903,7 +2903,7 @@
         </is>
       </c>
       <c r="N29" s="48" t="n">
-        <v>45986</v>
+        <v>45987</v>
       </c>
       <c r="O29" s="6" t="inlineStr">
         <is>
@@ -2919,16 +2919,16 @@
         <v>2.17</v>
       </c>
       <c r="R29" s="6" t="n">
+        <v>2.17</v>
+      </c>
+      <c r="S29" s="6" t="n">
         <v>2.16</v>
-      </c>
-      <c r="S29" s="6" t="n">
-        <v/>
       </c>
       <c r="T29" s="6" t="n">
         <v/>
       </c>
       <c r="U29" s="21" t="n">
-        <v>2.16</v>
+        <v/>
       </c>
     </row>
     <row r="30">
@@ -2942,8 +2942,8 @@
           <t>ADXDNO</t>
         </is>
       </c>
-      <c r="C30" s="47" t="n">
-        <v>45870</v>
+      <c r="C30" s="48" t="n">
+        <v>45901</v>
       </c>
       <c r="D30" s="6" t="inlineStr">
         <is>
@@ -2956,19 +2956,19 @@
         </is>
       </c>
       <c r="F30" s="25" t="n">
-        <v>0.01912935471760346</v>
+        <v>0.0006782625461356773</v>
       </c>
       <c r="G30" s="25" t="n">
+        <v>0.01909075917433611</v>
+      </c>
+      <c r="H30" s="25" t="n">
         <v>-0.02404555711932721</v>
       </c>
-      <c r="H30" s="25" t="n">
+      <c r="I30" s="25" t="n">
         <v>-0.09442194506291901</v>
       </c>
-      <c r="I30" s="25" t="n">
+      <c r="J30" s="25" t="n">
         <v>0.1570751450479186</v>
-      </c>
-      <c r="J30" s="25" t="n">
-        <v>-0.07662005055876375</v>
       </c>
       <c r="K30" s="5" t="n"/>
       <c r="L30" s="28" t="inlineStr">
@@ -2982,7 +2982,7 @@
         </is>
       </c>
       <c r="N30" s="48" t="n">
-        <v>45986</v>
+        <v>45987</v>
       </c>
       <c r="O30" s="6" t="inlineStr">
         <is>
@@ -2995,19 +2995,19 @@
         </is>
       </c>
       <c r="Q30" s="6" t="n">
+        <v>2.23</v>
+      </c>
+      <c r="R30" s="6" t="n">
         <v>2.22</v>
       </c>
-      <c r="R30" s="6" t="n">
+      <c r="S30" s="6" t="n">
         <v>2.23</v>
-      </c>
-      <c r="S30" s="6" t="n">
-        <v/>
       </c>
       <c r="T30" s="6" t="n">
         <v/>
       </c>
       <c r="U30" s="21" t="n">
-        <v>2.24</v>
+        <v/>
       </c>
     </row>
     <row r="31">
@@ -3017,8 +3017,8 @@
           <t>ADXDNO</t>
         </is>
       </c>
-      <c r="C31" s="47" t="n">
-        <v>45870</v>
+      <c r="C31" s="48" t="n">
+        <v>45901</v>
       </c>
       <c r="D31" s="6" t="inlineStr">
         <is>
@@ -3031,19 +3031,19 @@
         </is>
       </c>
       <c r="F31" s="25" t="n">
-        <v>0.06676582929337446</v>
+        <v>0.06450892203111723</v>
       </c>
       <c r="G31" s="25" t="n">
+        <v>0.06672542970471573</v>
+      </c>
+      <c r="H31" s="25" t="n">
         <v>0.0329297153895499</v>
       </c>
-      <c r="H31" s="25" t="n">
+      <c r="I31" s="25" t="n">
         <v>0.1029410098461701</v>
       </c>
-      <c r="I31" s="25" t="n">
+      <c r="J31" s="25" t="n">
         <v>0.1925388202490265</v>
-      </c>
-      <c r="J31" s="25" t="n">
-        <v>0.02590709813261283</v>
       </c>
       <c r="K31" s="5" t="n"/>
       <c r="L31" s="28" t="inlineStr">
@@ -3206,7 +3206,7 @@
           <t>CES0500000003</t>
         </is>
       </c>
-      <c r="N33" s="48" t="n">
+      <c r="N33" s="47" t="n">
         <v>45901</v>
       </c>
       <c r="O33" s="6" t="inlineStr">
@@ -3281,7 +3281,7 @@
           <t>CES0500000003</t>
         </is>
       </c>
-      <c r="N34" s="48" t="n">
+      <c r="N34" s="47" t="n">
         <v>45901</v>
       </c>
       <c r="O34" s="6" t="inlineStr">
@@ -3360,7 +3360,7 @@
           <t>RCES0500000003*</t>
         </is>
       </c>
-      <c r="N35" s="48" t="n">
+      <c r="N35" s="47" t="n">
         <v>45870</v>
       </c>
       <c r="O35" s="6" t="inlineStr">
@@ -3431,7 +3431,7 @@
           <t>RCES0500000003*</t>
         </is>
       </c>
-      <c r="N36" s="48" t="n">
+      <c r="N36" s="47" t="n">
         <v>45870</v>
       </c>
       <c r="O36" s="6" t="inlineStr">
@@ -4251,7 +4251,7 @@
         </is>
       </c>
       <c r="N47" s="48" t="n">
-        <v>45985</v>
+        <v>45986</v>
       </c>
       <c r="O47" s="6" t="inlineStr">
         <is>
@@ -4330,7 +4330,7 @@
         </is>
       </c>
       <c r="N48" s="48" t="n">
-        <v>45985</v>
+        <v>45986</v>
       </c>
       <c r="O48" s="6" t="inlineStr">
         <is>
@@ -4343,19 +4343,19 @@
         </is>
       </c>
       <c r="Q48" s="6" t="n">
+        <v>3.43</v>
+      </c>
+      <c r="R48" s="6" t="n">
         <v>3.46</v>
-      </c>
-      <c r="R48" s="6" t="n">
-        <v/>
       </c>
       <c r="S48" s="6" t="n">
         <v/>
       </c>
       <c r="T48" s="6" t="n">
+        <v/>
+      </c>
+      <c r="U48" s="21" t="n">
         <v>3.51</v>
-      </c>
-      <c r="U48" s="21" t="n">
-        <v>3.55</v>
       </c>
     </row>
     <row r="49">
@@ -4405,7 +4405,7 @@
         </is>
       </c>
       <c r="N49" s="48" t="n">
-        <v>45985</v>
+        <v>45986</v>
       </c>
       <c r="O49" s="6" t="inlineStr">
         <is>
@@ -4418,19 +4418,19 @@
         </is>
       </c>
       <c r="Q49" s="6" t="n">
+        <v>3.55</v>
+      </c>
+      <c r="R49" s="6" t="n">
         <v>3.61</v>
-      </c>
-      <c r="R49" s="6" t="n">
-        <v/>
       </c>
       <c r="S49" s="6" t="n">
         <v/>
       </c>
       <c r="T49" s="6" t="n">
+        <v/>
+      </c>
+      <c r="U49" s="21" t="n">
         <v>3.62</v>
-      </c>
-      <c r="U49" s="21" t="n">
-        <v>3.68</v>
       </c>
     </row>
     <row r="50">
@@ -4484,7 +4484,7 @@
         </is>
       </c>
       <c r="N50" s="48" t="n">
-        <v>45985</v>
+        <v>45986</v>
       </c>
       <c r="O50" s="6" t="inlineStr">
         <is>
@@ -4497,19 +4497,19 @@
         </is>
       </c>
       <c r="Q50" s="6" t="n">
+        <v>4.01</v>
+      </c>
+      <c r="R50" s="6" t="n">
         <v>4.04</v>
-      </c>
-      <c r="R50" s="6" t="n">
-        <v/>
       </c>
       <c r="S50" s="6" t="n">
         <v/>
       </c>
       <c r="T50" s="6" t="n">
+        <v/>
+      </c>
+      <c r="U50" s="21" t="n">
         <v>4.06</v>
-      </c>
-      <c r="U50" s="21" t="n">
-        <v>4.1</v>
       </c>
     </row>
     <row r="51" ht="31.5" customHeight="1">
@@ -4559,7 +4559,7 @@
         </is>
       </c>
       <c r="N51" s="48" t="n">
-        <v>45978</v>
+        <v>45985</v>
       </c>
       <c r="O51" s="6" t="inlineStr">
         <is>
@@ -4572,19 +4572,19 @@
         </is>
       </c>
       <c r="Q51" s="6" t="n">
+        <v>6.23</v>
+      </c>
+      <c r="R51" s="6" t="n">
         <v>6.26</v>
       </c>
-      <c r="R51" s="6" t="n">
+      <c r="S51" s="6" t="n">
         <v>6.24</v>
       </c>
-      <c r="S51" s="6" t="n">
+      <c r="T51" s="6" t="n">
         <v>6.22</v>
       </c>
-      <c r="T51" s="6" t="n">
+      <c r="U51" s="21" t="n">
         <v>6.17</v>
-      </c>
-      <c r="U51" s="21" t="n">
-        <v>6.19</v>
       </c>
     </row>
     <row r="52" ht="16.15" customHeight="1" thickBot="1">
@@ -4610,7 +4610,7 @@
         </is>
       </c>
       <c r="N52" s="49" t="n">
-        <v>45985</v>
+        <v>45986</v>
       </c>
       <c r="O52" s="9" t="inlineStr">
         <is>
@@ -4623,19 +4623,19 @@
         </is>
       </c>
       <c r="Q52" s="9" t="n">
+        <v>5.8</v>
+      </c>
+      <c r="R52" s="9" t="n">
         <v>5.84</v>
-      </c>
-      <c r="R52" s="9" t="n">
-        <v/>
       </c>
       <c r="S52" s="9" t="n">
         <v/>
       </c>
       <c r="T52" s="9" t="n">
+        <v/>
+      </c>
+      <c r="U52" s="22" t="n">
         <v>5.88</v>
-      </c>
-      <c r="U52" s="22" t="n">
-        <v>5.9</v>
       </c>
     </row>
     <row r="53" ht="21" customHeight="1">

</xml_diff>

<commit_message>
Update dashboards - 2025-11-28
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -2827,7 +2827,7 @@
           <t>UMCSENT</t>
         </is>
       </c>
-      <c r="N28" s="48" t="n">
+      <c r="N28" s="47" t="n">
         <v>45931</v>
       </c>
       <c r="O28" s="6" t="inlineStr">
@@ -3660,7 +3660,7 @@
           <t>DTWEXBGS</t>
         </is>
       </c>
-      <c r="N39" s="48" t="n">
+      <c r="N39" s="47" t="n">
         <v>45982</v>
       </c>
       <c r="O39" s="6" t="inlineStr">

</xml_diff>

<commit_message>
Update dashboards - 2025-11-29
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -2903,7 +2903,7 @@
         </is>
       </c>
       <c r="N29" s="48" t="n">
-        <v>45987</v>
+        <v>45989</v>
       </c>
       <c r="O29" s="6" t="inlineStr">
         <is>
@@ -2919,16 +2919,16 @@
         <v>2.17</v>
       </c>
       <c r="R29" s="6" t="n">
+        <v/>
+      </c>
+      <c r="S29" s="6" t="n">
         <v>2.17</v>
       </c>
-      <c r="S29" s="6" t="n">
+      <c r="T29" s="6" t="n">
+        <v>2.17</v>
+      </c>
+      <c r="U29" s="21" t="n">
         <v>2.16</v>
-      </c>
-      <c r="T29" s="6" t="n">
-        <v/>
-      </c>
-      <c r="U29" s="21" t="n">
-        <v/>
       </c>
     </row>
     <row r="30">
@@ -2982,7 +2982,7 @@
         </is>
       </c>
       <c r="N30" s="48" t="n">
-        <v>45987</v>
+        <v>45989</v>
       </c>
       <c r="O30" s="6" t="inlineStr">
         <is>
@@ -2998,16 +2998,16 @@
         <v>2.23</v>
       </c>
       <c r="R30" s="6" t="n">
-        <v>2.22</v>
+        <v/>
       </c>
       <c r="S30" s="6" t="n">
         <v>2.23</v>
       </c>
       <c r="T30" s="6" t="n">
-        <v/>
+        <v>2.22</v>
       </c>
       <c r="U30" s="21" t="n">
-        <v/>
+        <v>2.23</v>
       </c>
     </row>
     <row r="31">
@@ -4251,7 +4251,7 @@
         </is>
       </c>
       <c r="N47" s="48" t="n">
-        <v>45986</v>
+        <v>45988</v>
       </c>
       <c r="O47" s="6" t="inlineStr">
         <is>
@@ -4330,7 +4330,7 @@
         </is>
       </c>
       <c r="N48" s="48" t="n">
-        <v>45986</v>
+        <v>45987</v>
       </c>
       <c r="O48" s="6" t="inlineStr">
         <is>
@@ -4343,19 +4343,19 @@
         </is>
       </c>
       <c r="Q48" s="6" t="n">
+        <v>3.45</v>
+      </c>
+      <c r="R48" s="6" t="n">
         <v>3.43</v>
       </c>
-      <c r="R48" s="6" t="n">
+      <c r="S48" s="6" t="n">
         <v>3.46</v>
-      </c>
-      <c r="S48" s="6" t="n">
-        <v/>
       </c>
       <c r="T48" s="6" t="n">
         <v/>
       </c>
       <c r="U48" s="21" t="n">
-        <v>3.51</v>
+        <v/>
       </c>
     </row>
     <row r="49">
@@ -4405,7 +4405,7 @@
         </is>
       </c>
       <c r="N49" s="48" t="n">
-        <v>45986</v>
+        <v>45987</v>
       </c>
       <c r="O49" s="6" t="inlineStr">
         <is>
@@ -4418,19 +4418,19 @@
         </is>
       </c>
       <c r="Q49" s="6" t="n">
+        <v>3.56</v>
+      </c>
+      <c r="R49" s="6" t="n">
         <v>3.55</v>
       </c>
-      <c r="R49" s="6" t="n">
+      <c r="S49" s="6" t="n">
         <v>3.61</v>
-      </c>
-      <c r="S49" s="6" t="n">
-        <v/>
       </c>
       <c r="T49" s="6" t="n">
         <v/>
       </c>
       <c r="U49" s="21" t="n">
-        <v>3.62</v>
+        <v/>
       </c>
     </row>
     <row r="50">
@@ -4484,7 +4484,7 @@
         </is>
       </c>
       <c r="N50" s="48" t="n">
-        <v>45986</v>
+        <v>45987</v>
       </c>
       <c r="O50" s="6" t="inlineStr">
         <is>
@@ -4497,19 +4497,19 @@
         </is>
       </c>
       <c r="Q50" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="R50" s="6" t="n">
         <v>4.01</v>
       </c>
-      <c r="R50" s="6" t="n">
+      <c r="S50" s="6" t="n">
         <v>4.04</v>
-      </c>
-      <c r="S50" s="6" t="n">
-        <v/>
       </c>
       <c r="T50" s="6" t="n">
         <v/>
       </c>
       <c r="U50" s="21" t="n">
-        <v>4.06</v>
+        <v/>
       </c>
     </row>
     <row r="51" ht="31.5" customHeight="1">
@@ -4610,7 +4610,7 @@
         </is>
       </c>
       <c r="N52" s="49" t="n">
-        <v>45986</v>
+        <v>45987</v>
       </c>
       <c r="O52" s="9" t="inlineStr">
         <is>
@@ -4623,19 +4623,19 @@
         </is>
       </c>
       <c r="Q52" s="9" t="n">
+        <v>5.78</v>
+      </c>
+      <c r="R52" s="9" t="n">
         <v>5.8</v>
       </c>
-      <c r="R52" s="9" t="n">
+      <c r="S52" s="9" t="n">
         <v>5.84</v>
-      </c>
-      <c r="S52" s="9" t="n">
-        <v/>
       </c>
       <c r="T52" s="9" t="n">
         <v/>
       </c>
       <c r="U52" s="22" t="n">
-        <v>5.88</v>
+        <v/>
       </c>
     </row>
     <row r="53" ht="21" customHeight="1">

</xml_diff>

<commit_message>
Update dashboards - 2025-12-01
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -3096,7 +3096,7 @@
           <t>INDPRO</t>
         </is>
       </c>
-      <c r="C32" s="48" t="n">
+      <c r="C32" s="47" t="n">
         <v>45870</v>
       </c>
       <c r="D32" s="6" t="inlineStr">
@@ -3167,7 +3167,7 @@
           <t>INDPRO</t>
         </is>
       </c>
-      <c r="C33" s="48" t="n">
+      <c r="C33" s="47" t="n">
         <v>45870</v>
       </c>
       <c r="D33" s="6" t="inlineStr">
@@ -3246,7 +3246,7 @@
           <t>TCU</t>
         </is>
       </c>
-      <c r="C34" s="48" t="n">
+      <c r="C34" s="47" t="n">
         <v>45870</v>
       </c>
       <c r="D34" s="6" t="inlineStr">

</xml_diff>

<commit_message>
Update dashboards - 2025-12-02
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -1208,7 +1208,7 @@
         </is>
       </c>
       <c r="F7" s="25" t="n">
-        <v>0.3862508614748448</v>
+        <v>0.3276016540317022</v>
       </c>
       <c r="G7" s="25" t="n">
         <v>-2.062303243282817</v>
@@ -1940,7 +1940,7 @@
           <t>RSAFS</t>
         </is>
       </c>
-      <c r="C17" s="48" t="n">
+      <c r="C17" s="47" t="n">
         <v>45901</v>
       </c>
       <c r="D17" s="6" t="inlineStr">
@@ -2027,7 +2027,7 @@
           <t>RSAFS</t>
         </is>
       </c>
-      <c r="C18" s="48" t="n">
+      <c r="C18" s="47" t="n">
         <v>45901</v>
       </c>
       <c r="D18" s="6" t="inlineStr">
@@ -2370,7 +2370,7 @@
           <t>PPIFIS</t>
         </is>
       </c>
-      <c r="N22" s="48" t="n">
+      <c r="N22" s="47" t="n">
         <v>45901</v>
       </c>
       <c r="O22" s="6" t="inlineStr">
@@ -2440,7 +2440,7 @@
           <t>PPIFIS</t>
         </is>
       </c>
-      <c r="N23" s="48" t="n">
+      <c r="N23" s="47" t="n">
         <v>45901</v>
       </c>
       <c r="O23" s="6" t="inlineStr">
@@ -3510,7 +3510,7 @@
           <t>CSUSHPINSA</t>
         </is>
       </c>
-      <c r="N37" s="48" t="n">
+      <c r="N37" s="47" t="n">
         <v>45901</v>
       </c>
       <c r="O37" s="6" t="inlineStr">
@@ -3585,7 +3585,7 @@
           <t>CSUSHPINSA</t>
         </is>
       </c>
-      <c r="N38" s="48" t="n">
+      <c r="N38" s="47" t="n">
         <v>45901</v>
       </c>
       <c r="O38" s="6" t="inlineStr">
@@ -3660,8 +3660,8 @@
           <t>DTWEXBGS</t>
         </is>
       </c>
-      <c r="N39" s="47" t="n">
-        <v>45982</v>
+      <c r="N39" s="48" t="n">
+        <v>45989</v>
       </c>
       <c r="O39" s="6" t="inlineStr">
         <is>
@@ -3674,19 +3674,19 @@
         </is>
       </c>
       <c r="Q39" s="6" t="n">
-        <v>122.235</v>
+        <v>121.4288</v>
       </c>
       <c r="R39" s="6" t="n">
-        <v>122.0735</v>
+        <v/>
       </c>
       <c r="S39" s="6" t="n">
-        <v>121.8845</v>
+        <v>121.6225</v>
       </c>
       <c r="T39" s="6" t="n">
-        <v>121.6042</v>
+        <v>122.0044</v>
       </c>
       <c r="U39" s="21" t="n">
-        <v>121.5131</v>
+        <v>122.2833</v>
       </c>
     </row>
     <row r="40">
@@ -4251,7 +4251,7 @@
         </is>
       </c>
       <c r="N47" s="48" t="n">
-        <v>45988</v>
+        <v>45989</v>
       </c>
       <c r="O47" s="6" t="inlineStr">
         <is>
@@ -4264,7 +4264,7 @@
         </is>
       </c>
       <c r="Q47" s="6" t="n">
-        <v>3.88</v>
+        <v>3.89</v>
       </c>
       <c r="R47" s="6" t="n">
         <v>3.88</v>
@@ -4330,7 +4330,7 @@
         </is>
       </c>
       <c r="N48" s="48" t="n">
-        <v>45987</v>
+        <v>45989</v>
       </c>
       <c r="O48" s="6" t="inlineStr">
         <is>
@@ -4343,19 +4343,19 @@
         </is>
       </c>
       <c r="Q48" s="6" t="n">
+        <v>3.47</v>
+      </c>
+      <c r="R48" s="6" t="n">
+        <v/>
+      </c>
+      <c r="S48" s="6" t="n">
         <v>3.45</v>
       </c>
-      <c r="R48" s="6" t="n">
+      <c r="T48" s="6" t="n">
         <v>3.43</v>
       </c>
-      <c r="S48" s="6" t="n">
+      <c r="U48" s="21" t="n">
         <v>3.46</v>
-      </c>
-      <c r="T48" s="6" t="n">
-        <v/>
-      </c>
-      <c r="U48" s="21" t="n">
-        <v/>
       </c>
     </row>
     <row r="49">
@@ -4405,7 +4405,7 @@
         </is>
       </c>
       <c r="N49" s="48" t="n">
-        <v>45987</v>
+        <v>45989</v>
       </c>
       <c r="O49" s="6" t="inlineStr">
         <is>
@@ -4418,19 +4418,19 @@
         </is>
       </c>
       <c r="Q49" s="6" t="n">
+        <v>3.59</v>
+      </c>
+      <c r="R49" s="6" t="n">
+        <v/>
+      </c>
+      <c r="S49" s="6" t="n">
         <v>3.56</v>
       </c>
-      <c r="R49" s="6" t="n">
+      <c r="T49" s="6" t="n">
         <v>3.55</v>
       </c>
-      <c r="S49" s="6" t="n">
+      <c r="U49" s="21" t="n">
         <v>3.61</v>
-      </c>
-      <c r="T49" s="6" t="n">
-        <v/>
-      </c>
-      <c r="U49" s="21" t="n">
-        <v/>
       </c>
     </row>
     <row r="50">
@@ -4484,7 +4484,7 @@
         </is>
       </c>
       <c r="N50" s="48" t="n">
-        <v>45987</v>
+        <v>45989</v>
       </c>
       <c r="O50" s="6" t="inlineStr">
         <is>
@@ -4497,19 +4497,19 @@
         </is>
       </c>
       <c r="Q50" s="6" t="n">
+        <v>4.02</v>
+      </c>
+      <c r="R50" s="6" t="n">
+        <v/>
+      </c>
+      <c r="S50" s="6" t="n">
         <v>4</v>
       </c>
-      <c r="R50" s="6" t="n">
+      <c r="T50" s="6" t="n">
         <v>4.01</v>
       </c>
-      <c r="S50" s="6" t="n">
+      <c r="U50" s="21" t="n">
         <v>4.04</v>
-      </c>
-      <c r="T50" s="6" t="n">
-        <v/>
-      </c>
-      <c r="U50" s="21" t="n">
-        <v/>
       </c>
     </row>
     <row r="51" ht="31.5" customHeight="1">
@@ -4610,7 +4610,7 @@
         </is>
       </c>
       <c r="N52" s="49" t="n">
-        <v>45987</v>
+        <v>45989</v>
       </c>
       <c r="O52" s="9" t="inlineStr">
         <is>
@@ -4623,19 +4623,19 @@
         </is>
       </c>
       <c r="Q52" s="9" t="n">
+        <v>5.8</v>
+      </c>
+      <c r="R52" s="9" t="n">
+        <v/>
+      </c>
+      <c r="S52" s="9" t="n">
         <v>5.78</v>
       </c>
-      <c r="R52" s="9" t="n">
+      <c r="T52" s="9" t="n">
         <v>5.8</v>
       </c>
-      <c r="S52" s="9" t="n">
+      <c r="U52" s="22" t="n">
         <v>5.84</v>
-      </c>
-      <c r="T52" s="9" t="n">
-        <v/>
-      </c>
-      <c r="U52" s="22" t="n">
-        <v/>
       </c>
     </row>
     <row r="53" ht="21" customHeight="1">

</xml_diff>

<commit_message>
Update dashboards - 2025-12-03
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -1079,8 +1079,8 @@
           <t>ADPMNUSNERSA</t>
         </is>
       </c>
-      <c r="N5" s="47" t="n">
-        <v>45931</v>
+      <c r="N5" s="48" t="n">
+        <v>45962</v>
       </c>
       <c r="O5" s="6" t="inlineStr">
         <is>
@@ -1093,19 +1093,19 @@
         </is>
       </c>
       <c r="Q5" s="24" t="n">
-        <v>42000</v>
+        <v>-31000</v>
       </c>
       <c r="R5" s="24" t="n">
+        <v>47000</v>
+      </c>
+      <c r="S5" s="24" t="n">
         <v>-29000</v>
       </c>
-      <c r="S5" s="24" t="n">
+      <c r="T5" s="24" t="n">
         <v>-3000</v>
       </c>
-      <c r="T5" s="24" t="n">
+      <c r="U5" s="26" t="n">
         <v>104000</v>
-      </c>
-      <c r="U5" s="26" t="n">
-        <v>-23000</v>
       </c>
     </row>
     <row r="6">
@@ -1699,7 +1699,7 @@
           <t>ICSA</t>
         </is>
       </c>
-      <c r="N13" s="48" t="n">
+      <c r="N13" s="47" t="n">
         <v>45978</v>
       </c>
       <c r="O13" s="6" t="inlineStr">
@@ -1774,7 +1774,7 @@
           <t>CCSA</t>
         </is>
       </c>
-      <c r="N14" s="48" t="n">
+      <c r="N14" s="47" t="n">
         <v>45971</v>
       </c>
       <c r="O14" s="6" t="inlineStr">
@@ -2788,7 +2788,7 @@
           <t>DGORDER</t>
         </is>
       </c>
-      <c r="C28" s="48" t="n">
+      <c r="C28" s="47" t="n">
         <v>45901</v>
       </c>
       <c r="D28" s="6" t="inlineStr">
@@ -2863,7 +2863,7 @@
           <t>DGORDER</t>
         </is>
       </c>
-      <c r="C29" s="48" t="n">
+      <c r="C29" s="47" t="n">
         <v>45901</v>
       </c>
       <c r="D29" s="6" t="inlineStr">
@@ -2903,7 +2903,7 @@
         </is>
       </c>
       <c r="N29" s="48" t="n">
-        <v>45989</v>
+        <v>45993</v>
       </c>
       <c r="O29" s="6" t="inlineStr">
         <is>
@@ -2916,19 +2916,19 @@
         </is>
       </c>
       <c r="Q29" s="6" t="n">
+        <v>2.18</v>
+      </c>
+      <c r="R29" s="6" t="n">
         <v>2.17</v>
       </c>
-      <c r="R29" s="6" t="n">
+      <c r="S29" s="6" t="n">
         <v/>
       </c>
-      <c r="S29" s="6" t="n">
+      <c r="T29" s="6" t="n">
+        <v/>
+      </c>
+      <c r="U29" s="21" t="n">
         <v>2.17</v>
-      </c>
-      <c r="T29" s="6" t="n">
-        <v>2.17</v>
-      </c>
-      <c r="U29" s="21" t="n">
-        <v>2.16</v>
       </c>
     </row>
     <row r="30">
@@ -2942,7 +2942,7 @@
           <t>ADXDNO</t>
         </is>
       </c>
-      <c r="C30" s="48" t="n">
+      <c r="C30" s="47" t="n">
         <v>45901</v>
       </c>
       <c r="D30" s="6" t="inlineStr">
@@ -2982,7 +2982,7 @@
         </is>
       </c>
       <c r="N30" s="48" t="n">
-        <v>45989</v>
+        <v>45993</v>
       </c>
       <c r="O30" s="6" t="inlineStr">
         <is>
@@ -2995,16 +2995,16 @@
         </is>
       </c>
       <c r="Q30" s="6" t="n">
-        <v>2.23</v>
+        <v>2.24</v>
       </c>
       <c r="R30" s="6" t="n">
+        <v>2.24</v>
+      </c>
+      <c r="S30" s="6" t="n">
         <v/>
       </c>
-      <c r="S30" s="6" t="n">
-        <v>2.23</v>
-      </c>
       <c r="T30" s="6" t="n">
-        <v>2.22</v>
+        <v/>
       </c>
       <c r="U30" s="21" t="n">
         <v>2.23</v>
@@ -3017,7 +3017,7 @@
           <t>ADXDNO</t>
         </is>
       </c>
-      <c r="C31" s="48" t="n">
+      <c r="C31" s="47" t="n">
         <v>45901</v>
       </c>
       <c r="D31" s="6" t="inlineStr">
@@ -3096,8 +3096,8 @@
           <t>INDPRO</t>
         </is>
       </c>
-      <c r="C32" s="47" t="n">
-        <v>45870</v>
+      <c r="C32" s="48" t="n">
+        <v>45901</v>
       </c>
       <c r="D32" s="6" t="inlineStr">
         <is>
@@ -3110,19 +3110,19 @@
         </is>
       </c>
       <c r="F32" s="25" t="n">
-        <v>-0.0007577910391209919</v>
+        <v>0.0009661502023092794</v>
       </c>
       <c r="G32" s="25" t="n">
-        <v>-0.002144439521488684</v>
+        <v>-0.002569125217784962</v>
       </c>
       <c r="H32" s="25" t="n">
-        <v>0.00424479189840965</v>
+        <v>0.001607051307331187</v>
       </c>
       <c r="I32" s="25" t="n">
-        <v>-0.001038119019209582</v>
+        <v>0.004463379393190303</v>
       </c>
       <c r="J32" s="25" t="n">
-        <v>0.001983365069813559</v>
+        <v>-0.001489203276247131</v>
       </c>
       <c r="K32" s="5" t="n"/>
       <c r="L32" s="28" t="n"/>
@@ -3167,8 +3167,8 @@
           <t>INDPRO</t>
         </is>
       </c>
-      <c r="C33" s="47" t="n">
-        <v>45870</v>
+      <c r="C33" s="48" t="n">
+        <v>45901</v>
       </c>
       <c r="D33" s="6" t="inlineStr">
         <is>
@@ -3181,19 +3181,19 @@
         </is>
       </c>
       <c r="F33" s="25" t="n">
-        <v>0.008358981150223696</v>
+        <v>0.01622608918688194</v>
       </c>
       <c r="G33" s="25" t="n">
-        <v>0.01371833355505385</v>
+        <v>0.008952424004962659</v>
       </c>
       <c r="H33" s="25" t="n">
-        <v>0.006650544135429186</v>
+        <v>0.01615692613305024</v>
       </c>
       <c r="I33" s="25" t="n">
-        <v>0.00270366735076292</v>
+        <v>0.005292683410311731</v>
       </c>
       <c r="J33" s="25" t="n">
-        <v>0.009949782230052044</v>
+        <v>0.001133220308735612</v>
       </c>
       <c r="K33" s="5" t="n"/>
       <c r="L33" s="28" t="inlineStr">
@@ -3246,8 +3246,8 @@
           <t>TCU</t>
         </is>
       </c>
-      <c r="C34" s="47" t="n">
-        <v>45870</v>
+      <c r="C34" s="48" t="n">
+        <v>45901</v>
       </c>
       <c r="D34" s="6" t="inlineStr">
         <is>
@@ -3260,19 +3260,19 @@
         </is>
       </c>
       <c r="F34" s="24" t="n">
-        <v>75.84010000000001</v>
+        <v>75.8665</v>
       </c>
       <c r="G34" s="24" t="n">
-        <v>75.9897</v>
+        <v>75.8847</v>
       </c>
       <c r="H34" s="24" t="n">
-        <v>76.246</v>
+        <v>76.1724</v>
       </c>
       <c r="I34" s="24" t="n">
-        <v>76.01730000000001</v>
+        <v>76.1431</v>
       </c>
       <c r="J34" s="24" t="n">
-        <v>76.18980000000001</v>
+        <v>75.8982</v>
       </c>
       <c r="K34" s="5" t="n"/>
       <c r="L34" s="28" t="n"/>
@@ -3812,8 +3812,8 @@
           <t>IQ</t>
         </is>
       </c>
-      <c r="N41" s="47" t="n">
-        <v>45870</v>
+      <c r="N41" s="48" t="n">
+        <v>45901</v>
       </c>
       <c r="O41" s="6" t="inlineStr">
         <is>
@@ -3826,19 +3826,19 @@
         </is>
       </c>
       <c r="Q41" s="38" t="n">
-        <v>0.002617801047120283</v>
+        <v>0</v>
       </c>
       <c r="R41" s="38" t="n">
-        <v>0.002624671916010568</v>
+        <v>0.0006544502617800152</v>
       </c>
       <c r="S41" s="38" t="n">
-        <v>0.005277044854881341</v>
+        <v>0.003282994090610725</v>
       </c>
       <c r="T41" s="38" t="n">
+        <v>0.004617414248021312</v>
+      </c>
+      <c r="U41" s="23" t="n">
         <v>-0.006553079947575369</v>
-      </c>
-      <c r="U41" s="23" t="n">
-        <v>0.0006557377049178914</v>
       </c>
     </row>
     <row r="42">
@@ -3887,8 +3887,8 @@
           <t>IQ</t>
         </is>
       </c>
-      <c r="N42" s="47" t="n">
-        <v>45870</v>
+      <c r="N42" s="48" t="n">
+        <v>45901</v>
       </c>
       <c r="O42" s="6" t="inlineStr">
         <is>
@@ -3901,19 +3901,19 @@
         </is>
       </c>
       <c r="Q42" s="38" t="n">
-        <v>0.03373819163292847</v>
+        <v>0.03801765105227423</v>
       </c>
       <c r="R42" s="38" t="n">
+        <v>0.03171390013495289</v>
+      </c>
+      <c r="S42" s="38" t="n">
         <v>0.0241286863270779</v>
       </c>
-      <c r="S42" s="38" t="n">
-        <v>0.02695417789757412</v>
-      </c>
       <c r="T42" s="38" t="n">
+        <v>0.02628032345013481</v>
+      </c>
+      <c r="U42" s="23" t="n">
         <v>0.01881720430107515</v>
-      </c>
-      <c r="U42" s="23" t="n">
-        <v>0.01869158878504661</v>
       </c>
     </row>
     <row r="43">
@@ -3962,8 +3962,8 @@
           <t>IR</t>
         </is>
       </c>
-      <c r="N43" s="47" t="n">
-        <v>45870</v>
+      <c r="N43" s="48" t="n">
+        <v>45901</v>
       </c>
       <c r="O43" s="6" t="inlineStr">
         <is>
@@ -3976,19 +3976,19 @@
         </is>
       </c>
       <c r="Q43" s="38" t="n">
-        <v>0.002836879432624118</v>
+        <v>0</v>
       </c>
       <c r="R43" s="38" t="n">
-        <v>0.002132196162047073</v>
+        <v>0.0007082152974506872</v>
       </c>
       <c r="S43" s="38" t="n">
-        <v>-0.002127659574468144</v>
+        <v>0.00284090909090895</v>
       </c>
       <c r="T43" s="38" t="n">
+        <v>-0.001418439716311948</v>
+      </c>
+      <c r="U43" s="23" t="n">
         <v>-0.004940014114325986</v>
-      </c>
-      <c r="U43" s="23" t="n">
-        <v>0.0007062146892655718</v>
       </c>
     </row>
     <row r="44">
@@ -4037,8 +4037,8 @@
           <t>IR</t>
         </is>
       </c>
-      <c r="N44" s="47" t="n">
-        <v>45870</v>
+      <c r="N44" s="48" t="n">
+        <v>45901</v>
       </c>
       <c r="O44" s="6" t="inlineStr">
         <is>
@@ -4051,19 +4051,19 @@
         </is>
       </c>
       <c r="Q44" s="38" t="n">
-        <v>0</v>
+        <v>0.00283889283179564</v>
       </c>
       <c r="R44" s="38" t="n">
-        <v>-0.005641748942172153</v>
+        <v>-0.000707213578500667</v>
       </c>
       <c r="S44" s="38" t="n">
-        <v>-0.006355932203389871</v>
+        <v>-0.004231311706629215</v>
       </c>
       <c r="T44" s="38" t="n">
+        <v>-0.005649717514124173</v>
+      </c>
+      <c r="U44" s="23" t="n">
         <v>-0.00353356890459364</v>
-      </c>
-      <c r="U44" s="23" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="45">
@@ -4251,7 +4251,7 @@
         </is>
       </c>
       <c r="N47" s="48" t="n">
-        <v>45989</v>
+        <v>45992</v>
       </c>
       <c r="O47" s="6" t="inlineStr">
         <is>
@@ -4267,13 +4267,13 @@
         <v>3.89</v>
       </c>
       <c r="R47" s="6" t="n">
-        <v>3.88</v>
+        <v>3.89</v>
       </c>
       <c r="S47" s="6" t="n">
-        <v>3.88</v>
+        <v>3.89</v>
       </c>
       <c r="T47" s="6" t="n">
-        <v>3.88</v>
+        <v>3.89</v>
       </c>
       <c r="U47" s="21" t="n">
         <v>3.88</v>
@@ -4330,7 +4330,7 @@
         </is>
       </c>
       <c r="N48" s="48" t="n">
-        <v>45989</v>
+        <v>45992</v>
       </c>
       <c r="O48" s="6" t="inlineStr">
         <is>
@@ -4343,19 +4343,19 @@
         </is>
       </c>
       <c r="Q48" s="6" t="n">
-        <v>3.47</v>
+        <v>3.54</v>
       </c>
       <c r="R48" s="6" t="n">
         <v/>
       </c>
       <c r="S48" s="6" t="n">
-        <v>3.45</v>
+        <v/>
       </c>
       <c r="T48" s="6" t="n">
-        <v>3.43</v>
+        <v>3.47</v>
       </c>
       <c r="U48" s="21" t="n">
-        <v>3.46</v>
+        <v/>
       </c>
     </row>
     <row r="49">
@@ -4405,7 +4405,7 @@
         </is>
       </c>
       <c r="N49" s="48" t="n">
-        <v>45989</v>
+        <v>45992</v>
       </c>
       <c r="O49" s="6" t="inlineStr">
         <is>
@@ -4418,19 +4418,19 @@
         </is>
       </c>
       <c r="Q49" s="6" t="n">
-        <v>3.59</v>
+        <v>3.67</v>
       </c>
       <c r="R49" s="6" t="n">
         <v/>
       </c>
       <c r="S49" s="6" t="n">
-        <v>3.56</v>
+        <v/>
       </c>
       <c r="T49" s="6" t="n">
-        <v>3.55</v>
+        <v>3.59</v>
       </c>
       <c r="U49" s="21" t="n">
-        <v>3.61</v>
+        <v/>
       </c>
     </row>
     <row r="50">
@@ -4484,7 +4484,7 @@
         </is>
       </c>
       <c r="N50" s="48" t="n">
-        <v>45989</v>
+        <v>45992</v>
       </c>
       <c r="O50" s="6" t="inlineStr">
         <is>
@@ -4497,19 +4497,19 @@
         </is>
       </c>
       <c r="Q50" s="6" t="n">
-        <v>4.02</v>
+        <v>4.09</v>
       </c>
       <c r="R50" s="6" t="n">
         <v/>
       </c>
       <c r="S50" s="6" t="n">
-        <v>4</v>
+        <v/>
       </c>
       <c r="T50" s="6" t="n">
-        <v>4.01</v>
+        <v>4.02</v>
       </c>
       <c r="U50" s="21" t="n">
-        <v>4.04</v>
+        <v/>
       </c>
     </row>
     <row r="51" ht="31.5" customHeight="1">
@@ -4558,7 +4558,7 @@
           <t>MORTGAGE30US</t>
         </is>
       </c>
-      <c r="N51" s="48" t="n">
+      <c r="N51" s="47" t="n">
         <v>45985</v>
       </c>
       <c r="O51" s="6" t="inlineStr">
@@ -4610,7 +4610,7 @@
         </is>
       </c>
       <c r="N52" s="49" t="n">
-        <v>45989</v>
+        <v>45992</v>
       </c>
       <c r="O52" s="9" t="inlineStr">
         <is>
@@ -4623,19 +4623,19 @@
         </is>
       </c>
       <c r="Q52" s="9" t="n">
-        <v>5.8</v>
+        <v>5.87</v>
       </c>
       <c r="R52" s="9" t="n">
         <v/>
       </c>
       <c r="S52" s="9" t="n">
-        <v>5.78</v>
+        <v/>
       </c>
       <c r="T52" s="9" t="n">
         <v>5.8</v>
       </c>
       <c r="U52" s="22" t="n">
-        <v>5.84</v>
+        <v/>
       </c>
     </row>
     <row r="53" ht="21" customHeight="1">

</xml_diff>

<commit_message>
Update dashboards - 2025-12-04
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -1699,8 +1699,8 @@
           <t>ICSA</t>
         </is>
       </c>
-      <c r="N13" s="47" t="n">
-        <v>45978</v>
+      <c r="N13" s="48" t="n">
+        <v>45985</v>
       </c>
       <c r="O13" s="6" t="inlineStr">
         <is>
@@ -1713,19 +1713,19 @@
         </is>
       </c>
       <c r="Q13" s="24" t="n">
-        <v>216000</v>
+        <v>191000</v>
       </c>
       <c r="R13" s="24" t="n">
+        <v>218000</v>
+      </c>
+      <c r="S13" s="24" t="n">
         <v>222000</v>
       </c>
-      <c r="S13" s="24" t="n">
+      <c r="T13" s="24" t="n">
         <v>228000</v>
       </c>
-      <c r="T13" s="24" t="n">
+      <c r="U13" s="26" t="n">
         <v>229000</v>
-      </c>
-      <c r="U13" s="26" t="n">
-        <v>220000</v>
       </c>
     </row>
     <row r="14">
@@ -1774,8 +1774,8 @@
           <t>CCSA</t>
         </is>
       </c>
-      <c r="N14" s="47" t="n">
-        <v>45971</v>
+      <c r="N14" s="48" t="n">
+        <v>45978</v>
       </c>
       <c r="O14" s="6" t="inlineStr">
         <is>
@@ -1788,19 +1788,19 @@
         </is>
       </c>
       <c r="Q14" s="24" t="n">
-        <v>1960000</v>
+        <v>1939000</v>
       </c>
       <c r="R14" s="24" t="n">
+        <v>1943000</v>
+      </c>
+      <c r="S14" s="24" t="n">
         <v>1953000</v>
       </c>
-      <c r="S14" s="24" t="n">
+      <c r="T14" s="24" t="n">
         <v>1946000</v>
       </c>
-      <c r="T14" s="24" t="n">
+      <c r="U14" s="26" t="n">
         <v>1964000</v>
-      </c>
-      <c r="U14" s="26" t="n">
-        <v>1957000</v>
       </c>
     </row>
     <row r="15">
@@ -2903,7 +2903,7 @@
         </is>
       </c>
       <c r="N29" s="48" t="n">
-        <v>45993</v>
+        <v>45994</v>
       </c>
       <c r="O29" s="6" t="inlineStr">
         <is>
@@ -2916,19 +2916,19 @@
         </is>
       </c>
       <c r="Q29" s="6" t="n">
+        <v>2.19</v>
+      </c>
+      <c r="R29" s="6" t="n">
         <v>2.18</v>
       </c>
-      <c r="R29" s="6" t="n">
+      <c r="S29" s="6" t="n">
         <v>2.17</v>
-      </c>
-      <c r="S29" s="6" t="n">
-        <v/>
       </c>
       <c r="T29" s="6" t="n">
         <v/>
       </c>
       <c r="U29" s="21" t="n">
-        <v>2.17</v>
+        <v/>
       </c>
     </row>
     <row r="30">
@@ -2982,7 +2982,7 @@
         </is>
       </c>
       <c r="N30" s="48" t="n">
-        <v>45993</v>
+        <v>45994</v>
       </c>
       <c r="O30" s="6" t="inlineStr">
         <is>
@@ -3001,13 +3001,13 @@
         <v>2.24</v>
       </c>
       <c r="S30" s="6" t="n">
-        <v/>
+        <v>2.24</v>
       </c>
       <c r="T30" s="6" t="n">
         <v/>
       </c>
       <c r="U30" s="21" t="n">
-        <v>2.23</v>
+        <v/>
       </c>
     </row>
     <row r="31">
@@ -4251,7 +4251,7 @@
         </is>
       </c>
       <c r="N47" s="48" t="n">
-        <v>45992</v>
+        <v>45993</v>
       </c>
       <c r="O47" s="6" t="inlineStr">
         <is>
@@ -4276,7 +4276,7 @@
         <v>3.89</v>
       </c>
       <c r="U47" s="21" t="n">
-        <v>3.88</v>
+        <v>3.89</v>
       </c>
     </row>
     <row r="48">
@@ -4330,7 +4330,7 @@
         </is>
       </c>
       <c r="N48" s="48" t="n">
-        <v>45992</v>
+        <v>45993</v>
       </c>
       <c r="O48" s="6" t="inlineStr">
         <is>
@@ -4343,19 +4343,19 @@
         </is>
       </c>
       <c r="Q48" s="6" t="n">
+        <v>3.51</v>
+      </c>
+      <c r="R48" s="6" t="n">
         <v>3.54</v>
-      </c>
-      <c r="R48" s="6" t="n">
-        <v/>
       </c>
       <c r="S48" s="6" t="n">
         <v/>
       </c>
       <c r="T48" s="6" t="n">
+        <v/>
+      </c>
+      <c r="U48" s="21" t="n">
         <v>3.47</v>
-      </c>
-      <c r="U48" s="21" t="n">
-        <v/>
       </c>
     </row>
     <row r="49">
@@ -4405,7 +4405,7 @@
         </is>
       </c>
       <c r="N49" s="48" t="n">
-        <v>45992</v>
+        <v>45993</v>
       </c>
       <c r="O49" s="6" t="inlineStr">
         <is>
@@ -4418,19 +4418,19 @@
         </is>
       </c>
       <c r="Q49" s="6" t="n">
+        <v>3.66</v>
+      </c>
+      <c r="R49" s="6" t="n">
         <v>3.67</v>
-      </c>
-      <c r="R49" s="6" t="n">
-        <v/>
       </c>
       <c r="S49" s="6" t="n">
         <v/>
       </c>
       <c r="T49" s="6" t="n">
+        <v/>
+      </c>
+      <c r="U49" s="21" t="n">
         <v>3.59</v>
-      </c>
-      <c r="U49" s="21" t="n">
-        <v/>
       </c>
     </row>
     <row r="50">
@@ -4484,7 +4484,7 @@
         </is>
       </c>
       <c r="N50" s="48" t="n">
-        <v>45992</v>
+        <v>45993</v>
       </c>
       <c r="O50" s="6" t="inlineStr">
         <is>
@@ -4500,16 +4500,16 @@
         <v>4.09</v>
       </c>
       <c r="R50" s="6" t="n">
-        <v/>
+        <v>4.09</v>
       </c>
       <c r="S50" s="6" t="n">
         <v/>
       </c>
       <c r="T50" s="6" t="n">
+        <v/>
+      </c>
+      <c r="U50" s="21" t="n">
         <v>4.02</v>
-      </c>
-      <c r="U50" s="21" t="n">
-        <v/>
       </c>
     </row>
     <row r="51" ht="31.5" customHeight="1">
@@ -4610,7 +4610,7 @@
         </is>
       </c>
       <c r="N52" s="49" t="n">
-        <v>45992</v>
+        <v>45993</v>
       </c>
       <c r="O52" s="9" t="inlineStr">
         <is>
@@ -4623,19 +4623,19 @@
         </is>
       </c>
       <c r="Q52" s="9" t="n">
+        <v>5.85</v>
+      </c>
+      <c r="R52" s="9" t="n">
         <v>5.87</v>
-      </c>
-      <c r="R52" s="9" t="n">
-        <v/>
       </c>
       <c r="S52" s="9" t="n">
         <v/>
       </c>
       <c r="T52" s="9" t="n">
+        <v/>
+      </c>
+      <c r="U52" s="22" t="n">
         <v>5.8</v>
-      </c>
-      <c r="U52" s="22" t="n">
-        <v/>
       </c>
     </row>
     <row r="53" ht="21" customHeight="1">

</xml_diff>

<commit_message>
Update dashboards - 2025-12-05
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -1208,7 +1208,7 @@
         </is>
       </c>
       <c r="F7" s="25" t="n">
-        <v>0.3276016540317022</v>
+        <v>0.3129565816678153</v>
       </c>
       <c r="G7" s="25" t="n">
         <v>-2.062303243282817</v>
@@ -2788,7 +2788,7 @@
           <t>DGORDER</t>
         </is>
       </c>
-      <c r="C28" s="47" t="n">
+      <c r="C28" s="48" t="n">
         <v>45901</v>
       </c>
       <c r="D28" s="6" t="inlineStr">
@@ -2802,10 +2802,10 @@
         </is>
       </c>
       <c r="F28" s="25" t="n">
-        <v>0.004840745558111426</v>
+        <v>0.005052252529329948</v>
       </c>
       <c r="G28" s="25" t="n">
-        <v>0.03006283164814283</v>
+        <v>0.03004963172206243</v>
       </c>
       <c r="H28" s="25" t="n">
         <v>-0.02799901206372835</v>
@@ -2863,7 +2863,7 @@
           <t>DGORDER</t>
         </is>
       </c>
-      <c r="C29" s="47" t="n">
+      <c r="C29" s="48" t="n">
         <v>45901</v>
       </c>
       <c r="D29" s="6" t="inlineStr">
@@ -2877,10 +2877,10 @@
         </is>
       </c>
       <c r="F29" s="25" t="n">
-        <v>0.07243160813624692</v>
+        <v>0.07264359641534658</v>
       </c>
       <c r="G29" s="25" t="n">
-        <v>0.07662644950780544</v>
+        <v>0.07661265288383932</v>
       </c>
       <c r="H29" s="25" t="n">
         <v>0.03341358778313566</v>
@@ -2903,7 +2903,7 @@
         </is>
       </c>
       <c r="N29" s="48" t="n">
-        <v>45994</v>
+        <v>45995</v>
       </c>
       <c r="O29" s="6" t="inlineStr">
         <is>
@@ -2919,13 +2919,13 @@
         <v>2.19</v>
       </c>
       <c r="R29" s="6" t="n">
+        <v>2.19</v>
+      </c>
+      <c r="S29" s="6" t="n">
         <v>2.18</v>
       </c>
-      <c r="S29" s="6" t="n">
+      <c r="T29" s="6" t="n">
         <v>2.17</v>
-      </c>
-      <c r="T29" s="6" t="n">
-        <v/>
       </c>
       <c r="U29" s="21" t="n">
         <v/>
@@ -2942,7 +2942,7 @@
           <t>ADXDNO</t>
         </is>
       </c>
-      <c r="C30" s="47" t="n">
+      <c r="C30" s="48" t="n">
         <v>45901</v>
       </c>
       <c r="D30" s="6" t="inlineStr">
@@ -2956,10 +2956,10 @@
         </is>
       </c>
       <c r="F30" s="25" t="n">
-        <v>0.0006782625461356773</v>
+        <v>0.000905510184407321</v>
       </c>
       <c r="G30" s="25" t="n">
-        <v>0.01909075917433611</v>
+        <v>0.01907672443132968</v>
       </c>
       <c r="H30" s="25" t="n">
         <v>-0.02404555711932721</v>
@@ -2982,7 +2982,7 @@
         </is>
       </c>
       <c r="N30" s="48" t="n">
-        <v>45994</v>
+        <v>45995</v>
       </c>
       <c r="O30" s="6" t="inlineStr">
         <is>
@@ -2995,7 +2995,7 @@
         </is>
       </c>
       <c r="Q30" s="6" t="n">
-        <v>2.24</v>
+        <v>2.26</v>
       </c>
       <c r="R30" s="6" t="n">
         <v>2.24</v>
@@ -3004,7 +3004,7 @@
         <v>2.24</v>
       </c>
       <c r="T30" s="6" t="n">
-        <v/>
+        <v>2.24</v>
       </c>
       <c r="U30" s="21" t="n">
         <v/>
@@ -3017,7 +3017,7 @@
           <t>ADXDNO</t>
         </is>
       </c>
-      <c r="C31" s="47" t="n">
+      <c r="C31" s="48" t="n">
         <v>45901</v>
       </c>
       <c r="D31" s="6" t="inlineStr">
@@ -3031,10 +3031,10 @@
         </is>
       </c>
       <c r="F31" s="25" t="n">
-        <v>0.06450892203111723</v>
+        <v>0.0647360016408333</v>
       </c>
       <c r="G31" s="25" t="n">
-        <v>0.06672542970471573</v>
+        <v>0.06671073894520346</v>
       </c>
       <c r="H31" s="25" t="n">
         <v>0.0329297153895499</v>
@@ -3660,7 +3660,7 @@
           <t>DTWEXBGS</t>
         </is>
       </c>
-      <c r="N39" s="48" t="n">
+      <c r="N39" s="47" t="n">
         <v>45989</v>
       </c>
       <c r="O39" s="6" t="inlineStr">
@@ -4251,7 +4251,7 @@
         </is>
       </c>
       <c r="N47" s="48" t="n">
-        <v>45993</v>
+        <v>45994</v>
       </c>
       <c r="O47" s="6" t="inlineStr">
         <is>
@@ -4330,7 +4330,7 @@
         </is>
       </c>
       <c r="N48" s="48" t="n">
-        <v>45993</v>
+        <v>45994</v>
       </c>
       <c r="O48" s="6" t="inlineStr">
         <is>
@@ -4343,19 +4343,19 @@
         </is>
       </c>
       <c r="Q48" s="6" t="n">
+        <v>3.49</v>
+      </c>
+      <c r="R48" s="6" t="n">
         <v>3.51</v>
       </c>
-      <c r="R48" s="6" t="n">
+      <c r="S48" s="6" t="n">
         <v>3.54</v>
-      </c>
-      <c r="S48" s="6" t="n">
-        <v/>
       </c>
       <c r="T48" s="6" t="n">
         <v/>
       </c>
       <c r="U48" s="21" t="n">
-        <v>3.47</v>
+        <v/>
       </c>
     </row>
     <row r="49">
@@ -4405,7 +4405,7 @@
         </is>
       </c>
       <c r="N49" s="48" t="n">
-        <v>45993</v>
+        <v>45994</v>
       </c>
       <c r="O49" s="6" t="inlineStr">
         <is>
@@ -4418,19 +4418,19 @@
         </is>
       </c>
       <c r="Q49" s="6" t="n">
+        <v>3.62</v>
+      </c>
+      <c r="R49" s="6" t="n">
         <v>3.66</v>
       </c>
-      <c r="R49" s="6" t="n">
+      <c r="S49" s="6" t="n">
         <v>3.67</v>
-      </c>
-      <c r="S49" s="6" t="n">
-        <v/>
       </c>
       <c r="T49" s="6" t="n">
         <v/>
       </c>
       <c r="U49" s="21" t="n">
-        <v>3.59</v>
+        <v/>
       </c>
     </row>
     <row r="50">
@@ -4484,7 +4484,7 @@
         </is>
       </c>
       <c r="N50" s="48" t="n">
-        <v>45993</v>
+        <v>45994</v>
       </c>
       <c r="O50" s="6" t="inlineStr">
         <is>
@@ -4497,19 +4497,19 @@
         </is>
       </c>
       <c r="Q50" s="6" t="n">
-        <v>4.09</v>
+        <v>4.06</v>
       </c>
       <c r="R50" s="6" t="n">
         <v>4.09</v>
       </c>
       <c r="S50" s="6" t="n">
-        <v/>
+        <v>4.09</v>
       </c>
       <c r="T50" s="6" t="n">
         <v/>
       </c>
       <c r="U50" s="21" t="n">
-        <v>4.02</v>
+        <v/>
       </c>
     </row>
     <row r="51" ht="31.5" customHeight="1">
@@ -4558,8 +4558,8 @@
           <t>MORTGAGE30US</t>
         </is>
       </c>
-      <c r="N51" s="47" t="n">
-        <v>45985</v>
+      <c r="N51" s="48" t="n">
+        <v>45992</v>
       </c>
       <c r="O51" s="6" t="inlineStr">
         <is>
@@ -4572,19 +4572,19 @@
         </is>
       </c>
       <c r="Q51" s="6" t="n">
+        <v>6.19</v>
+      </c>
+      <c r="R51" s="6" t="n">
         <v>6.23</v>
       </c>
-      <c r="R51" s="6" t="n">
+      <c r="S51" s="6" t="n">
         <v>6.26</v>
       </c>
-      <c r="S51" s="6" t="n">
+      <c r="T51" s="6" t="n">
         <v>6.24</v>
       </c>
-      <c r="T51" s="6" t="n">
+      <c r="U51" s="21" t="n">
         <v>6.22</v>
-      </c>
-      <c r="U51" s="21" t="n">
-        <v>6.17</v>
       </c>
     </row>
     <row r="52" ht="16.15" customHeight="1" thickBot="1">
@@ -4610,7 +4610,7 @@
         </is>
       </c>
       <c r="N52" s="49" t="n">
-        <v>45993</v>
+        <v>45994</v>
       </c>
       <c r="O52" s="9" t="inlineStr">
         <is>
@@ -4623,19 +4623,19 @@
         </is>
       </c>
       <c r="Q52" s="9" t="n">
+        <v>5.83</v>
+      </c>
+      <c r="R52" s="9" t="n">
         <v>5.85</v>
       </c>
-      <c r="R52" s="9" t="n">
+      <c r="S52" s="9" t="n">
         <v>5.87</v>
-      </c>
-      <c r="S52" s="9" t="n">
-        <v/>
       </c>
       <c r="T52" s="9" t="n">
         <v/>
       </c>
       <c r="U52" s="22" t="n">
-        <v>5.8</v>
+        <v/>
       </c>
     </row>
     <row r="53" ht="21" customHeight="1">

</xml_diff>

<commit_message>
Update dashboards - 2025-12-06
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -1506,8 +1506,8 @@
           <t>PCEDGC96</t>
         </is>
       </c>
-      <c r="C11" s="47" t="n">
-        <v>45870</v>
+      <c r="C11" s="48" t="n">
+        <v>45901</v>
       </c>
       <c r="D11" s="6" t="inlineStr">
         <is>
@@ -1520,19 +1520,19 @@
         </is>
       </c>
       <c r="F11" s="25" t="n">
-        <v>0.008921103986618384</v>
+        <v>-0.00597293513765762</v>
       </c>
       <c r="G11" s="25" t="n">
-        <v>0.01811817020672679</v>
+        <v>0.0007471747454934619</v>
       </c>
       <c r="H11" s="25" t="n">
+        <v>0.01300913004399451</v>
+      </c>
+      <c r="I11" s="25" t="n">
         <v>-0.001794399584454709</v>
       </c>
-      <c r="I11" s="25" t="n">
+      <c r="J11" s="25" t="n">
         <v>-0.02184757505773682</v>
-      </c>
-      <c r="J11" s="25" t="n">
-        <v>-0.006470561240879191</v>
       </c>
       <c r="K11" s="5" t="n"/>
       <c r="L11" s="28" t="inlineStr">
@@ -1581,8 +1581,8 @@
           <t>PCEDGC96</t>
         </is>
       </c>
-      <c r="C12" s="47" t="n">
-        <v>45870</v>
+      <c r="C12" s="48" t="n">
+        <v>45901</v>
       </c>
       <c r="D12" s="6" t="inlineStr">
         <is>
@@ -1595,19 +1595,19 @@
         </is>
       </c>
       <c r="F12" s="25" t="n">
-        <v>0.05203488372093028</v>
+        <v>0.02065066360021078</v>
       </c>
       <c r="G12" s="25" t="n">
-        <v>0.0392582934955815</v>
+        <v>0.03827519379844961</v>
       </c>
       <c r="H12" s="25" t="n">
+        <v>0.03404316963638997</v>
+      </c>
+      <c r="I12" s="25" t="n">
         <v>0.0349571603427173</v>
       </c>
-      <c r="I12" s="25" t="n">
+      <c r="J12" s="25" t="n">
         <v>0.03610744165565816</v>
-      </c>
-      <c r="J12" s="25" t="n">
-        <v>0.07759693395052517</v>
       </c>
       <c r="K12" s="5" t="n"/>
       <c r="L12" s="28" t="inlineStr">
@@ -1660,8 +1660,8 @@
           <t>PCENDC96</t>
         </is>
       </c>
-      <c r="C13" s="47" t="n">
-        <v>45870</v>
+      <c r="C13" s="48" t="n">
+        <v>45901</v>
       </c>
       <c r="D13" s="6" t="inlineStr">
         <is>
@@ -1674,19 +1674,19 @@
         </is>
       </c>
       <c r="F13" s="25" t="n">
-        <v>0.005385334882798132</v>
+        <v>-0.003324786565608084</v>
       </c>
       <c r="G13" s="25" t="n">
-        <v>0.001504485068695383</v>
+        <v>0.004500169817728938</v>
       </c>
       <c r="H13" s="25" t="n">
+        <v>0.002952197115930311</v>
+      </c>
+      <c r="I13" s="25" t="n">
         <v>0.007003401652231123</v>
       </c>
-      <c r="I13" s="25" t="n">
+      <c r="J13" s="25" t="n">
         <v>-0.00119914346895067</v>
-      </c>
-      <c r="J13" s="25" t="n">
-        <v>-0.0001427347987439376</v>
       </c>
       <c r="K13" s="5" t="n"/>
       <c r="L13" s="28" t="inlineStr">
@@ -1735,8 +1735,8 @@
           <t>PCENDC96</t>
         </is>
       </c>
-      <c r="C14" s="47" t="n">
-        <v>45870</v>
+      <c r="C14" s="48" t="n">
+        <v>45901</v>
       </c>
       <c r="D14" s="6" t="inlineStr">
         <is>
@@ -1749,19 +1749,19 @@
         </is>
       </c>
       <c r="F14" s="25" t="n">
-        <v>0.03661815418785427</v>
+        <v>0.02107207805328638</v>
       </c>
       <c r="G14" s="25" t="n">
-        <v>0.02905060522094208</v>
+        <v>0.03720264188438825</v>
       </c>
       <c r="H14" s="25" t="n">
+        <v>0.03053813621117101</v>
+      </c>
+      <c r="I14" s="25" t="n">
         <v>0.03332160037545476</v>
       </c>
-      <c r="I14" s="25" t="n">
+      <c r="J14" s="25" t="n">
         <v>0.02894202770669728</v>
-      </c>
-      <c r="J14" s="25" t="n">
-        <v>0.03474253301426922</v>
       </c>
       <c r="K14" s="5" t="n"/>
       <c r="L14" s="28" t="inlineStr">
@@ -1814,8 +1814,8 @@
           <t>PCESC96</t>
         </is>
       </c>
-      <c r="C15" s="47" t="n">
-        <v>45870</v>
+      <c r="C15" s="48" t="n">
+        <v>45901</v>
       </c>
       <c r="D15" s="6" t="inlineStr">
         <is>
@@ -1828,19 +1828,19 @@
         </is>
       </c>
       <c r="F15" s="25" t="n">
-        <v>0.002084825774691712</v>
+        <v>0.002492303181351518</v>
       </c>
       <c r="G15" s="25" t="n">
-        <v>0.002301347669195097</v>
+        <v>0.002121114733024232</v>
       </c>
       <c r="H15" s="25" t="n">
+        <v>0.002513071654761001</v>
+      </c>
+      <c r="I15" s="25" t="n">
         <v>0.001973841981958824</v>
       </c>
-      <c r="I15" s="25" t="n">
+      <c r="J15" s="25" t="n">
         <v>0.001829606357419911</v>
-      </c>
-      <c r="J15" s="25" t="n">
-        <v>0.003123754437677873</v>
       </c>
       <c r="K15" s="5" t="n"/>
       <c r="L15" s="28" t="inlineStr">
@@ -1889,8 +1889,8 @@
           <t>PCESC96</t>
         </is>
       </c>
-      <c r="C16" s="47" t="n">
-        <v>45870</v>
+      <c r="C16" s="48" t="n">
+        <v>45901</v>
       </c>
       <c r="D16" s="6" t="inlineStr">
         <is>
@@ -1903,19 +1903,19 @@
         </is>
       </c>
       <c r="F16" s="25" t="n">
-        <v>0.02074056056580463</v>
+        <v>0.02155949168526313</v>
       </c>
       <c r="G16" s="25" t="n">
-        <v>0.02177136315009102</v>
+        <v>0.02099315196647079</v>
       </c>
       <c r="H16" s="25" t="n">
+        <v>0.021987199939941</v>
+      </c>
+      <c r="I16" s="25" t="n">
         <v>0.02094865746266567</v>
       </c>
-      <c r="I16" s="25" t="n">
+      <c r="J16" s="25" t="n">
         <v>0.02239657497430288</v>
-      </c>
-      <c r="J16" s="25" t="n">
-        <v>0.02327956277539295</v>
       </c>
       <c r="K16" s="5" t="n"/>
       <c r="L16" s="28" t="n"/>
@@ -2106,8 +2106,8 @@
           <t>DSPIC96</t>
         </is>
       </c>
-      <c r="C19" s="47" t="n">
-        <v>45870</v>
+      <c r="C19" s="48" t="n">
+        <v>45901</v>
       </c>
       <c r="D19" s="6" t="inlineStr">
         <is>
@@ -2120,19 +2120,19 @@
         </is>
       </c>
       <c r="F19" s="25" t="n">
-        <v>0.001100828110392582</v>
+        <v>0.0006075636146720687</v>
       </c>
       <c r="G19" s="25" t="n">
-        <v>0.002278750512857419</v>
+        <v>0.001139097016782165</v>
       </c>
       <c r="H19" s="25" t="n">
+        <v>0.002677947682993009</v>
+      </c>
+      <c r="I19" s="25" t="n">
         <v>-0.000304849321294598</v>
       </c>
-      <c r="I19" s="25" t="n">
+      <c r="J19" s="25" t="n">
         <v>-0.006984577788051838</v>
-      </c>
-      <c r="J19" s="25" t="n">
-        <v>0.007737491056125867</v>
       </c>
       <c r="K19" s="5" t="n"/>
       <c r="L19" s="28" t="n"/>
@@ -2177,8 +2177,8 @@
           <t>DSPIC96</t>
         </is>
       </c>
-      <c r="C20" s="47" t="n">
-        <v>45870</v>
+      <c r="C20" s="48" t="n">
+        <v>45901</v>
       </c>
       <c r="D20" s="6" t="inlineStr">
         <is>
@@ -2191,19 +2191,19 @@
         </is>
       </c>
       <c r="F20" s="25" t="n">
-        <v>0.01939401449903955</v>
+        <v>0.01948238313102477</v>
       </c>
       <c r="G20" s="25" t="n">
-        <v>0.0188297488615356</v>
+        <v>0.01983901221772201</v>
       </c>
       <c r="H20" s="25" t="n">
+        <v>0.01923553812164656</v>
+      </c>
+      <c r="I20" s="25" t="n">
         <v>0.01606097650286474</v>
       </c>
-      <c r="I20" s="25" t="n">
+      <c r="J20" s="25" t="n">
         <v>0.01853974132431571</v>
-      </c>
-      <c r="J20" s="25" t="n">
-        <v>0.03004773621489234</v>
       </c>
       <c r="K20" s="5" t="n"/>
       <c r="L20" s="28" t="inlineStr">
@@ -2256,8 +2256,8 @@
           <t>PSAVERT</t>
         </is>
       </c>
-      <c r="C21" s="47" t="n">
-        <v>45870</v>
+      <c r="C21" s="48" t="n">
+        <v>45901</v>
       </c>
       <c r="D21" s="6" t="inlineStr">
         <is>
@@ -2270,19 +2270,19 @@
         </is>
       </c>
       <c r="F21" s="6" t="n">
-        <v>4.6</v>
+        <v>4.7</v>
       </c>
       <c r="G21" s="6" t="n">
-        <v>4.8</v>
+        <v>4.7</v>
       </c>
       <c r="H21" s="6" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="I21" s="6" t="n">
         <v>5</v>
       </c>
-      <c r="I21" s="6" t="n">
+      <c r="J21" s="6" t="n">
         <v>5.2</v>
-      </c>
-      <c r="J21" s="6" t="n">
-        <v>5.7</v>
       </c>
       <c r="K21" s="5" t="n"/>
       <c r="L21" s="28" t="n"/>
@@ -2331,8 +2331,8 @@
           <t>TOTALSA</t>
         </is>
       </c>
-      <c r="C22" s="47" t="n">
-        <v>45870</v>
+      <c r="C22" s="48" t="n">
+        <v>45962</v>
       </c>
       <c r="D22" s="6" t="inlineStr">
         <is>
@@ -2345,19 +2345,19 @@
         </is>
       </c>
       <c r="F22" s="24" t="n">
-        <v>16.802</v>
+        <v>15.963</v>
       </c>
       <c r="G22" s="24" t="n">
-        <v>16.896</v>
+        <v>15.63</v>
       </c>
       <c r="H22" s="24" t="n">
-        <v>16.042</v>
+        <v>16.663</v>
       </c>
       <c r="I22" s="24" t="n">
-        <v>16.067</v>
+        <v>16.916</v>
       </c>
       <c r="J22" s="24" t="n">
-        <v>17.59</v>
+        <v>16.969</v>
       </c>
       <c r="K22" s="5" t="n"/>
       <c r="L22" s="28" t="inlineStr">
@@ -2406,8 +2406,8 @@
           <t>TOTALSA</t>
         </is>
       </c>
-      <c r="C23" s="47" t="n">
-        <v>45870</v>
+      <c r="C23" s="48" t="n">
+        <v>45962</v>
       </c>
       <c r="D23" s="6" t="inlineStr">
         <is>
@@ -2420,19 +2420,19 @@
         </is>
       </c>
       <c r="F23" s="25" t="n">
-        <v>0.05262498433780227</v>
+        <v>-0.0612760952660982</v>
       </c>
       <c r="G23" s="25" t="n">
-        <v>0.03497702909647789</v>
+        <v>-0.05593138439236531</v>
       </c>
       <c r="H23" s="25" t="n">
-        <v>0.01698998351718033</v>
+        <v>0.02114229685010411</v>
       </c>
       <c r="I23" s="25" t="n">
-        <v>-0.01700825940654627</v>
+        <v>0.05976694649793263</v>
       </c>
       <c r="J23" s="25" t="n">
-        <v>0.06982118963629727</v>
+        <v>0.03944869831546719</v>
       </c>
       <c r="K23" s="5" t="n"/>
       <c r="M23" s="15" t="inlineStr">
@@ -2480,8 +2480,8 @@
           <t>REVOLSL</t>
         </is>
       </c>
-      <c r="C24" s="47" t="n">
-        <v>45901</v>
+      <c r="C24" s="48" t="n">
+        <v>45931</v>
       </c>
       <c r="D24" s="6" t="inlineStr">
         <is>
@@ -2494,19 +2494,19 @@
         </is>
       </c>
       <c r="F24" s="38" t="n">
-        <v>0.001263881152865798</v>
+        <v>0.004122988119927395</v>
       </c>
       <c r="G24" s="38" t="n">
-        <v>-0.004631607864557297</v>
+        <v>0.003293006621412964</v>
       </c>
       <c r="H24" s="38" t="n">
-        <v>0.008466932005238847</v>
+        <v>-0.00328836233676344</v>
       </c>
       <c r="I24" s="38" t="n">
-        <v>7.468713370495372e-05</v>
+        <v>0.008508856867884829</v>
       </c>
       <c r="J24" s="38" t="n">
-        <v>-0.0009803765564608824</v>
+        <v>6.940322356907558e-05</v>
       </c>
       <c r="K24" s="5" t="n"/>
       <c r="L24" s="28" t="inlineStr">
@@ -2519,8 +2519,8 @@
           <t>PCEPI</t>
         </is>
       </c>
-      <c r="N24" s="47" t="n">
-        <v>45870</v>
+      <c r="N24" s="48" t="n">
+        <v>45901</v>
       </c>
       <c r="O24" s="6" t="inlineStr">
         <is>
@@ -2533,19 +2533,19 @@
         </is>
       </c>
       <c r="Q24" s="38" t="n">
-        <v>0.002646732152281617</v>
+        <v>0.002686925983831356</v>
       </c>
       <c r="R24" s="38" t="n">
-        <v>0.001625336310486558</v>
+        <v>0.002583592611555385</v>
       </c>
       <c r="S24" s="38" t="n">
+        <v>0.001672676203025025</v>
+      </c>
+      <c r="T24" s="38" t="n">
         <v>0.002872289919291005</v>
       </c>
-      <c r="T24" s="38" t="n">
+      <c r="U24" s="23" t="n">
         <v>0.001823226317875459</v>
-      </c>
-      <c r="U24" s="23" t="n">
-        <v>0.001659507229575752</v>
       </c>
     </row>
     <row r="25">
@@ -2559,8 +2559,8 @@
           <t>NONREVSL</t>
         </is>
       </c>
-      <c r="C25" s="47" t="n">
-        <v>45901</v>
+      <c r="C25" s="48" t="n">
+        <v>45931</v>
       </c>
       <c r="D25" s="6" t="inlineStr">
         <is>
@@ -2573,19 +2573,19 @@
         </is>
       </c>
       <c r="F25" s="38" t="n">
-        <v>0.003044704234780982</v>
+        <v>0.001002044138157077</v>
       </c>
       <c r="G25" s="38" t="n">
-        <v>0.002454000808095547</v>
+        <v>0.001783907070203483</v>
       </c>
       <c r="H25" s="38" t="n">
-        <v>0.001792092542795443</v>
+        <v>0.002285485926998732</v>
       </c>
       <c r="I25" s="38" t="n">
-        <v>-0.001282602659991805</v>
+        <v>0.001562654273511654</v>
       </c>
       <c r="J25" s="38" t="n">
-        <v>0.002439153249045978</v>
+        <v>-0.001091050242697622</v>
       </c>
       <c r="K25" s="5" t="n"/>
       <c r="L25" s="28" t="n"/>
@@ -2594,8 +2594,8 @@
           <t>PCEPI</t>
         </is>
       </c>
-      <c r="N25" s="47" t="n">
-        <v>45870</v>
+      <c r="N25" s="48" t="n">
+        <v>45901</v>
       </c>
       <c r="O25" s="6" t="inlineStr">
         <is>
@@ -2608,19 +2608,19 @@
         </is>
       </c>
       <c r="Q25" s="38" t="n">
-        <v>0.02741163460839946</v>
+        <v>0.02787442414870654</v>
       </c>
       <c r="R25" s="38" t="n">
-        <v>0.02596657399625003</v>
+        <v>0.02739549112512011</v>
       </c>
       <c r="S25" s="38" t="n">
+        <v>0.02601506433051007</v>
+      </c>
+      <c r="T25" s="38" t="n">
         <v>0.02593512979706808</v>
       </c>
-      <c r="T25" s="38" t="n">
+      <c r="U25" s="23" t="n">
         <v>0.02458086065440864</v>
-      </c>
-      <c r="U25" s="23" t="n">
-        <v>0.02277425997843387</v>
       </c>
     </row>
     <row r="26">
@@ -2673,8 +2673,8 @@
           <t>PCEPILFE</t>
         </is>
       </c>
-      <c r="N26" s="47" t="n">
-        <v>45870</v>
+      <c r="N26" s="48" t="n">
+        <v>45901</v>
       </c>
       <c r="O26" s="6" t="inlineStr">
         <is>
@@ -2687,19 +2687,19 @@
         </is>
       </c>
       <c r="Q26" s="38" t="n">
-        <v>0.002270246325681402</v>
+        <v>0.001981010710085718</v>
       </c>
       <c r="R26" s="38" t="n">
-        <v>0.002354881423395128</v>
+        <v>0.002206859457065002</v>
       </c>
       <c r="S26" s="38" t="n">
+        <v>0.002402454785483954</v>
+      </c>
+      <c r="T26" s="38" t="n">
         <v>0.002631369743222756</v>
       </c>
-      <c r="T26" s="38" t="n">
+      <c r="U26" s="23" t="n">
         <v>0.002294784146866347</v>
-      </c>
-      <c r="U26" s="23" t="n">
-        <v>0.001875992879210031</v>
       </c>
     </row>
     <row r="27">
@@ -2748,8 +2748,8 @@
           <t>PCEPILFE</t>
         </is>
       </c>
-      <c r="N27" s="47" t="n">
-        <v>45870</v>
+      <c r="N27" s="48" t="n">
+        <v>45901</v>
       </c>
       <c r="O27" s="6" t="inlineStr">
         <is>
@@ -2762,19 +2762,19 @@
         </is>
       </c>
       <c r="Q27" s="38" t="n">
-        <v>0.02905106880644531</v>
+        <v>0.02825069249833962</v>
       </c>
       <c r="R27" s="38" t="n">
-        <v>0.02853284083605214</v>
+        <v>0.02903482554739785</v>
       </c>
       <c r="S27" s="38" t="n">
+        <v>0.02858165664586575</v>
+      </c>
+      <c r="T27" s="38" t="n">
         <v>0.02807372205058803</v>
       </c>
-      <c r="T27" s="38" t="n">
+      <c r="U27" s="23" t="n">
         <v>0.02783883382495944</v>
-      </c>
-      <c r="U27" s="23" t="n">
-        <v>0.02614795918367342</v>
       </c>
     </row>
     <row r="28">
@@ -2903,7 +2903,7 @@
         </is>
       </c>
       <c r="N29" s="48" t="n">
-        <v>45995</v>
+        <v>45996</v>
       </c>
       <c r="O29" s="6" t="inlineStr">
         <is>
@@ -2916,19 +2916,19 @@
         </is>
       </c>
       <c r="Q29" s="6" t="n">
-        <v>2.19</v>
+        <v>2.18</v>
       </c>
       <c r="R29" s="6" t="n">
         <v>2.19</v>
       </c>
       <c r="S29" s="6" t="n">
+        <v>2.19</v>
+      </c>
+      <c r="T29" s="6" t="n">
         <v>2.18</v>
       </c>
-      <c r="T29" s="6" t="n">
+      <c r="U29" s="21" t="n">
         <v>2.17</v>
-      </c>
-      <c r="U29" s="21" t="n">
-        <v/>
       </c>
     </row>
     <row r="30">
@@ -2982,7 +2982,7 @@
         </is>
       </c>
       <c r="N30" s="48" t="n">
-        <v>45995</v>
+        <v>45996</v>
       </c>
       <c r="O30" s="6" t="inlineStr">
         <is>
@@ -2998,7 +2998,7 @@
         <v>2.26</v>
       </c>
       <c r="R30" s="6" t="n">
-        <v>2.24</v>
+        <v>2.26</v>
       </c>
       <c r="S30" s="6" t="n">
         <v>2.24</v>
@@ -3007,7 +3007,7 @@
         <v>2.24</v>
       </c>
       <c r="U30" s="21" t="n">
-        <v/>
+        <v>2.24</v>
       </c>
     </row>
     <row r="31">
@@ -3361,7 +3361,7 @@
         </is>
       </c>
       <c r="N35" s="47" t="n">
-        <v>45870</v>
+        <v>45901</v>
       </c>
       <c r="O35" s="6" t="inlineStr">
         <is>
@@ -3374,19 +3374,19 @@
         </is>
       </c>
       <c r="Q35" s="38" t="n">
-        <v>0.001466871021821747</v>
+        <v>-0.0002259579984887905</v>
       </c>
       <c r="R35" s="38" t="n">
-        <v>0.001676812994635402</v>
+        <v>0.001529940234958005</v>
       </c>
       <c r="S35" s="38" t="n">
+        <v>0.001629472906588658</v>
+      </c>
+      <c r="T35" s="38" t="n">
         <v>-0.0006622728576672898</v>
       </c>
-      <c r="T35" s="38" t="n">
+      <c r="U35" s="23" t="n">
         <v>0.002329953587340228</v>
-      </c>
-      <c r="U35" s="23" t="n">
-        <v>6.223697012197604e-06</v>
       </c>
     </row>
     <row r="36" ht="31.5" customHeight="1">
@@ -3432,7 +3432,7 @@
         </is>
       </c>
       <c r="N36" s="47" t="n">
-        <v>45870</v>
+        <v>45901</v>
       </c>
       <c r="O36" s="6" t="inlineStr">
         <is>
@@ -3445,19 +3445,19 @@
         </is>
       </c>
       <c r="Q36" s="38" t="n">
-        <v>0.01061695136548506</v>
+        <v>0.009781041380375289</v>
       </c>
       <c r="R36" s="38" t="n">
-        <v>0.01248872041084645</v>
+        <v>0.01063283120727662</v>
       </c>
       <c r="S36" s="38" t="n">
+        <v>0.0124408693429683</v>
+      </c>
+      <c r="T36" s="38" t="n">
         <v>0.01120289314371833</v>
       </c>
-      <c r="T36" s="38" t="n">
+      <c r="U36" s="23" t="n">
         <v>0.01349386861907807</v>
-      </c>
-      <c r="U36" s="23" t="n">
-        <v>0.01515400017679062</v>
       </c>
     </row>
     <row r="37">
@@ -4251,7 +4251,7 @@
         </is>
       </c>
       <c r="N47" s="48" t="n">
-        <v>45994</v>
+        <v>45995</v>
       </c>
       <c r="O47" s="6" t="inlineStr">
         <is>
@@ -4330,7 +4330,7 @@
         </is>
       </c>
       <c r="N48" s="48" t="n">
-        <v>45994</v>
+        <v>45995</v>
       </c>
       <c r="O48" s="6" t="inlineStr">
         <is>
@@ -4343,16 +4343,16 @@
         </is>
       </c>
       <c r="Q48" s="6" t="n">
+        <v>3.52</v>
+      </c>
+      <c r="R48" s="6" t="n">
         <v>3.49</v>
       </c>
-      <c r="R48" s="6" t="n">
+      <c r="S48" s="6" t="n">
         <v>3.51</v>
       </c>
-      <c r="S48" s="6" t="n">
+      <c r="T48" s="6" t="n">
         <v>3.54</v>
-      </c>
-      <c r="T48" s="6" t="n">
-        <v/>
       </c>
       <c r="U48" s="21" t="n">
         <v/>
@@ -4405,7 +4405,7 @@
         </is>
       </c>
       <c r="N49" s="48" t="n">
-        <v>45994</v>
+        <v>45995</v>
       </c>
       <c r="O49" s="6" t="inlineStr">
         <is>
@@ -4418,16 +4418,16 @@
         </is>
       </c>
       <c r="Q49" s="6" t="n">
+        <v>3.68</v>
+      </c>
+      <c r="R49" s="6" t="n">
         <v>3.62</v>
       </c>
-      <c r="R49" s="6" t="n">
+      <c r="S49" s="6" t="n">
         <v>3.66</v>
       </c>
-      <c r="S49" s="6" t="n">
+      <c r="T49" s="6" t="n">
         <v>3.67</v>
-      </c>
-      <c r="T49" s="6" t="n">
-        <v/>
       </c>
       <c r="U49" s="21" t="n">
         <v/>
@@ -4484,7 +4484,7 @@
         </is>
       </c>
       <c r="N50" s="48" t="n">
-        <v>45994</v>
+        <v>45995</v>
       </c>
       <c r="O50" s="6" t="inlineStr">
         <is>
@@ -4497,16 +4497,16 @@
         </is>
       </c>
       <c r="Q50" s="6" t="n">
+        <v>4.11</v>
+      </c>
+      <c r="R50" s="6" t="n">
         <v>4.06</v>
-      </c>
-      <c r="R50" s="6" t="n">
-        <v>4.09</v>
       </c>
       <c r="S50" s="6" t="n">
         <v>4.09</v>
       </c>
       <c r="T50" s="6" t="n">
-        <v/>
+        <v>4.09</v>
       </c>
       <c r="U50" s="21" t="n">
         <v/>
@@ -4610,7 +4610,7 @@
         </is>
       </c>
       <c r="N52" s="49" t="n">
-        <v>45994</v>
+        <v>45995</v>
       </c>
       <c r="O52" s="9" t="inlineStr">
         <is>
@@ -4623,16 +4623,16 @@
         </is>
       </c>
       <c r="Q52" s="9" t="n">
+        <v>5.87</v>
+      </c>
+      <c r="R52" s="9" t="n">
         <v>5.83</v>
       </c>
-      <c r="R52" s="9" t="n">
+      <c r="S52" s="9" t="n">
         <v>5.85</v>
       </c>
-      <c r="S52" s="9" t="n">
+      <c r="T52" s="9" t="n">
         <v>5.87</v>
-      </c>
-      <c r="T52" s="9" t="n">
-        <v/>
       </c>
       <c r="U52" s="22" t="n">
         <v/>

</xml_diff>

<commit_message>
Update dashboards - 2025-12-09
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -1093,7 +1093,7 @@
         </is>
       </c>
       <c r="Q5" s="24" t="n">
-        <v>-31000</v>
+        <v>-32000</v>
       </c>
       <c r="R5" s="24" t="n">
         <v>47000</v>
@@ -2903,7 +2903,7 @@
         </is>
       </c>
       <c r="N29" s="48" t="n">
-        <v>45996</v>
+        <v>45999</v>
       </c>
       <c r="O29" s="6" t="inlineStr">
         <is>
@@ -2916,19 +2916,19 @@
         </is>
       </c>
       <c r="Q29" s="6" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="R29" s="6" t="n">
         <v>2.18</v>
-      </c>
-      <c r="R29" s="6" t="n">
-        <v>2.19</v>
       </c>
       <c r="S29" s="6" t="n">
         <v>2.19</v>
       </c>
       <c r="T29" s="6" t="n">
+        <v>2.19</v>
+      </c>
+      <c r="U29" s="21" t="n">
         <v>2.18</v>
-      </c>
-      <c r="U29" s="21" t="n">
-        <v>2.17</v>
       </c>
     </row>
     <row r="30">
@@ -2982,7 +2982,7 @@
         </is>
       </c>
       <c r="N30" s="48" t="n">
-        <v>45996</v>
+        <v>45999</v>
       </c>
       <c r="O30" s="6" t="inlineStr">
         <is>
@@ -3001,7 +3001,7 @@
         <v>2.26</v>
       </c>
       <c r="S30" s="6" t="n">
-        <v>2.24</v>
+        <v>2.26</v>
       </c>
       <c r="T30" s="6" t="n">
         <v>2.24</v>
@@ -3660,8 +3660,8 @@
           <t>DTWEXBGS</t>
         </is>
       </c>
-      <c r="N39" s="47" t="n">
-        <v>45989</v>
+      <c r="N39" s="48" t="n">
+        <v>45996</v>
       </c>
       <c r="O39" s="6" t="inlineStr">
         <is>
@@ -3674,19 +3674,19 @@
         </is>
       </c>
       <c r="Q39" s="6" t="n">
-        <v>121.4288</v>
+        <v>121.0615</v>
       </c>
       <c r="R39" s="6" t="n">
-        <v/>
+        <v>121.0614</v>
       </c>
       <c r="S39" s="6" t="n">
-        <v>121.6225</v>
+        <v>121.1131</v>
       </c>
       <c r="T39" s="6" t="n">
-        <v>122.0044</v>
+        <v>121.5149</v>
       </c>
       <c r="U39" s="21" t="n">
-        <v>122.2833</v>
+        <v>121.3615</v>
       </c>
     </row>
     <row r="40">
@@ -4251,7 +4251,7 @@
         </is>
       </c>
       <c r="N47" s="48" t="n">
-        <v>45995</v>
+        <v>45996</v>
       </c>
       <c r="O47" s="6" t="inlineStr">
         <is>
@@ -4330,7 +4330,7 @@
         </is>
       </c>
       <c r="N48" s="48" t="n">
-        <v>45995</v>
+        <v>45996</v>
       </c>
       <c r="O48" s="6" t="inlineStr">
         <is>
@@ -4343,19 +4343,19 @@
         </is>
       </c>
       <c r="Q48" s="6" t="n">
+        <v>3.56</v>
+      </c>
+      <c r="R48" s="6" t="n">
         <v>3.52</v>
       </c>
-      <c r="R48" s="6" t="n">
+      <c r="S48" s="6" t="n">
         <v>3.49</v>
       </c>
-      <c r="S48" s="6" t="n">
+      <c r="T48" s="6" t="n">
         <v>3.51</v>
       </c>
-      <c r="T48" s="6" t="n">
+      <c r="U48" s="21" t="n">
         <v>3.54</v>
-      </c>
-      <c r="U48" s="21" t="n">
-        <v/>
       </c>
     </row>
     <row r="49">
@@ -4405,7 +4405,7 @@
         </is>
       </c>
       <c r="N49" s="48" t="n">
-        <v>45995</v>
+        <v>45996</v>
       </c>
       <c r="O49" s="6" t="inlineStr">
         <is>
@@ -4418,19 +4418,19 @@
         </is>
       </c>
       <c r="Q49" s="6" t="n">
+        <v>3.72</v>
+      </c>
+      <c r="R49" s="6" t="n">
         <v>3.68</v>
       </c>
-      <c r="R49" s="6" t="n">
+      <c r="S49" s="6" t="n">
         <v>3.62</v>
       </c>
-      <c r="S49" s="6" t="n">
+      <c r="T49" s="6" t="n">
         <v>3.66</v>
       </c>
-      <c r="T49" s="6" t="n">
+      <c r="U49" s="21" t="n">
         <v>3.67</v>
-      </c>
-      <c r="U49" s="21" t="n">
-        <v/>
       </c>
     </row>
     <row r="50">
@@ -4484,7 +4484,7 @@
         </is>
       </c>
       <c r="N50" s="48" t="n">
-        <v>45995</v>
+        <v>45996</v>
       </c>
       <c r="O50" s="6" t="inlineStr">
         <is>
@@ -4497,19 +4497,19 @@
         </is>
       </c>
       <c r="Q50" s="6" t="n">
+        <v>4.14</v>
+      </c>
+      <c r="R50" s="6" t="n">
         <v>4.11</v>
       </c>
-      <c r="R50" s="6" t="n">
+      <c r="S50" s="6" t="n">
         <v>4.06</v>
-      </c>
-      <c r="S50" s="6" t="n">
-        <v>4.09</v>
       </c>
       <c r="T50" s="6" t="n">
         <v>4.09</v>
       </c>
       <c r="U50" s="21" t="n">
-        <v/>
+        <v>4.09</v>
       </c>
     </row>
     <row r="51" ht="31.5" customHeight="1">
@@ -4610,7 +4610,7 @@
         </is>
       </c>
       <c r="N52" s="49" t="n">
-        <v>45995</v>
+        <v>45996</v>
       </c>
       <c r="O52" s="9" t="inlineStr">
         <is>
@@ -4623,19 +4623,19 @@
         </is>
       </c>
       <c r="Q52" s="9" t="n">
+        <v>5.88</v>
+      </c>
+      <c r="R52" s="9" t="n">
         <v>5.87</v>
       </c>
-      <c r="R52" s="9" t="n">
+      <c r="S52" s="9" t="n">
         <v>5.83</v>
       </c>
-      <c r="S52" s="9" t="n">
+      <c r="T52" s="9" t="n">
         <v>5.85</v>
       </c>
-      <c r="T52" s="9" t="n">
+      <c r="U52" s="22" t="n">
         <v>5.87</v>
-      </c>
-      <c r="U52" s="22" t="n">
-        <v/>
       </c>
     </row>
     <row r="53" ht="21" customHeight="1">

</xml_diff>

<commit_message>
Update dashboards - 2025-12-10
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -1079,7 +1079,7 @@
           <t>ADPMNUSNERSA</t>
         </is>
       </c>
-      <c r="N5" s="48" t="n">
+      <c r="N5" s="47" t="n">
         <v>45962</v>
       </c>
       <c r="O5" s="6" t="inlineStr">
@@ -1466,8 +1466,8 @@
           <t>JTSJOR</t>
         </is>
       </c>
-      <c r="N10" s="47" t="n">
-        <v>45870</v>
+      <c r="N10" s="48" t="n">
+        <v>45931</v>
       </c>
       <c r="O10" s="6" t="inlineStr">
         <is>
@@ -1480,16 +1480,16 @@
         </is>
       </c>
       <c r="Q10" s="6" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="R10" s="6" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="S10" s="6" t="n">
         <v>4.3</v>
       </c>
-      <c r="R10" s="6" t="n">
+      <c r="T10" s="6" t="n">
         <v>4.3</v>
-      </c>
-      <c r="S10" s="6" t="n">
-        <v>4.4</v>
-      </c>
-      <c r="T10" s="6" t="n">
-        <v>4.6</v>
       </c>
       <c r="U10" s="21" t="n">
         <v>4.4</v>
@@ -1545,8 +1545,8 @@
           <t>JTSHIR</t>
         </is>
       </c>
-      <c r="N11" s="47" t="n">
-        <v>45870</v>
+      <c r="N11" s="48" t="n">
+        <v>45931</v>
       </c>
       <c r="O11" s="6" t="inlineStr">
         <is>
@@ -1562,16 +1562,16 @@
         <v>3.2</v>
       </c>
       <c r="R11" s="6" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="S11" s="6" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="T11" s="6" t="n">
         <v>3.3</v>
       </c>
-      <c r="S11" s="6" t="n">
+      <c r="U11" s="21" t="n">
         <v>3.3</v>
-      </c>
-      <c r="T11" s="6" t="n">
-        <v>3.4</v>
-      </c>
-      <c r="U11" s="21" t="n">
-        <v>3.5</v>
       </c>
     </row>
     <row r="12">
@@ -1620,8 +1620,8 @@
           <t>JTSTSR</t>
         </is>
       </c>
-      <c r="N12" s="47" t="n">
-        <v>45870</v>
+      <c r="N12" s="48" t="n">
+        <v>45931</v>
       </c>
       <c r="O12" s="6" t="inlineStr">
         <is>
@@ -1640,7 +1640,7 @@
         <v>3.3</v>
       </c>
       <c r="S12" s="6" t="n">
-        <v>3.3</v>
+        <v>3.2</v>
       </c>
       <c r="T12" s="6" t="n">
         <v>3.3</v>
@@ -2903,7 +2903,7 @@
         </is>
       </c>
       <c r="N29" s="48" t="n">
-        <v>45999</v>
+        <v>46000</v>
       </c>
       <c r="O29" s="6" t="inlineStr">
         <is>
@@ -2919,13 +2919,13 @@
         <v>2.2</v>
       </c>
       <c r="R29" s="6" t="n">
-        <v>2.18</v>
+        <v>2.2</v>
       </c>
       <c r="S29" s="6" t="n">
-        <v>2.19</v>
+        <v/>
       </c>
       <c r="T29" s="6" t="n">
-        <v>2.19</v>
+        <v/>
       </c>
       <c r="U29" s="21" t="n">
         <v>2.18</v>
@@ -2982,7 +2982,7 @@
         </is>
       </c>
       <c r="N30" s="48" t="n">
-        <v>45999</v>
+        <v>46000</v>
       </c>
       <c r="O30" s="6" t="inlineStr">
         <is>
@@ -3001,13 +3001,13 @@
         <v>2.26</v>
       </c>
       <c r="S30" s="6" t="n">
+        <v/>
+      </c>
+      <c r="T30" s="6" t="n">
+        <v/>
+      </c>
+      <c r="U30" s="21" t="n">
         <v>2.26</v>
-      </c>
-      <c r="T30" s="6" t="n">
-        <v>2.24</v>
-      </c>
-      <c r="U30" s="21" t="n">
-        <v>2.24</v>
       </c>
     </row>
     <row r="31">
@@ -3056,8 +3056,8 @@
           <t>ECIWAG</t>
         </is>
       </c>
-      <c r="N31" s="47" t="n">
-        <v>45748</v>
+      <c r="N31" s="48" t="n">
+        <v>45839</v>
       </c>
       <c r="O31" s="6" t="inlineStr">
         <is>
@@ -3070,19 +3070,19 @@
         </is>
       </c>
       <c r="Q31" s="38" t="n">
+        <v>0.007996957929548465</v>
+      </c>
+      <c r="R31" s="38" t="n">
         <v>0.01027939464493599</v>
       </c>
-      <c r="R31" s="38" t="n">
+      <c r="S31" s="38" t="n">
         <v>0.007624633431085215</v>
       </c>
-      <c r="S31" s="38" t="n">
+      <c r="T31" s="38" t="n">
         <v>0.009473060982829962</v>
       </c>
-      <c r="T31" s="38" t="n">
+      <c r="U31" s="23" t="n">
         <v>0.007756563245823411</v>
-      </c>
-      <c r="U31" s="23" t="n">
-        <v>0.008423586040914532</v>
       </c>
     </row>
     <row r="32">
@@ -3096,7 +3096,7 @@
           <t>INDPRO</t>
         </is>
       </c>
-      <c r="C32" s="48" t="n">
+      <c r="C32" s="47" t="n">
         <v>45901</v>
       </c>
       <c r="D32" s="6" t="inlineStr">
@@ -3131,8 +3131,8 @@
           <t>ECIWAG</t>
         </is>
       </c>
-      <c r="N32" s="47" t="n">
-        <v>45748</v>
+      <c r="N32" s="48" t="n">
+        <v>45839</v>
       </c>
       <c r="O32" s="6" t="inlineStr">
         <is>
@@ -3145,19 +3145,19 @@
         </is>
       </c>
       <c r="Q32" s="38" t="n">
+        <v>0.03584369449378332</v>
+      </c>
+      <c r="R32" s="38" t="n">
         <v>0.03559665871121723</v>
       </c>
-      <c r="R32" s="38" t="n">
+      <c r="S32" s="38" t="n">
         <v>0.03369434416365838</v>
       </c>
-      <c r="S32" s="38" t="n">
+      <c r="T32" s="38" t="n">
         <v>0.03710462287104619</v>
       </c>
-      <c r="T32" s="38" t="n">
+      <c r="U32" s="23" t="n">
         <v>0.03746928746928743</v>
-      </c>
-      <c r="U32" s="23" t="n">
-        <v>0.04034761018001241</v>
       </c>
     </row>
     <row r="33" ht="31.5" customHeight="1">
@@ -3167,7 +3167,7 @@
           <t>INDPRO</t>
         </is>
       </c>
-      <c r="C33" s="48" t="n">
+      <c r="C33" s="47" t="n">
         <v>45901</v>
       </c>
       <c r="D33" s="6" t="inlineStr">
@@ -3246,7 +3246,7 @@
           <t>TCU</t>
         </is>
       </c>
-      <c r="C34" s="48" t="n">
+      <c r="C34" s="47" t="n">
         <v>45901</v>
       </c>
       <c r="D34" s="6" t="inlineStr">
@@ -3812,7 +3812,7 @@
           <t>IQ</t>
         </is>
       </c>
-      <c r="N41" s="48" t="n">
+      <c r="N41" s="47" t="n">
         <v>45901</v>
       </c>
       <c r="O41" s="6" t="inlineStr">
@@ -3887,7 +3887,7 @@
           <t>IQ</t>
         </is>
       </c>
-      <c r="N42" s="48" t="n">
+      <c r="N42" s="47" t="n">
         <v>45901</v>
       </c>
       <c r="O42" s="6" t="inlineStr">
@@ -3962,7 +3962,7 @@
           <t>IR</t>
         </is>
       </c>
-      <c r="N43" s="48" t="n">
+      <c r="N43" s="47" t="n">
         <v>45901</v>
       </c>
       <c r="O43" s="6" t="inlineStr">
@@ -4037,7 +4037,7 @@
           <t>IR</t>
         </is>
       </c>
-      <c r="N44" s="48" t="n">
+      <c r="N44" s="47" t="n">
         <v>45901</v>
       </c>
       <c r="O44" s="6" t="inlineStr">
@@ -4251,7 +4251,7 @@
         </is>
       </c>
       <c r="N47" s="48" t="n">
-        <v>45996</v>
+        <v>45999</v>
       </c>
       <c r="O47" s="6" t="inlineStr">
         <is>
@@ -4330,7 +4330,7 @@
         </is>
       </c>
       <c r="N48" s="48" t="n">
-        <v>45996</v>
+        <v>45999</v>
       </c>
       <c r="O48" s="6" t="inlineStr">
         <is>
@@ -4343,19 +4343,19 @@
         </is>
       </c>
       <c r="Q48" s="6" t="n">
+        <v>3.57</v>
+      </c>
+      <c r="R48" s="6" t="n">
+        <v/>
+      </c>
+      <c r="S48" s="6" t="n">
+        <v/>
+      </c>
+      <c r="T48" s="6" t="n">
         <v>3.56</v>
       </c>
-      <c r="R48" s="6" t="n">
+      <c r="U48" s="21" t="n">
         <v>3.52</v>
-      </c>
-      <c r="S48" s="6" t="n">
-        <v>3.49</v>
-      </c>
-      <c r="T48" s="6" t="n">
-        <v>3.51</v>
-      </c>
-      <c r="U48" s="21" t="n">
-        <v>3.54</v>
       </c>
     </row>
     <row r="49">
@@ -4405,7 +4405,7 @@
         </is>
       </c>
       <c r="N49" s="48" t="n">
-        <v>45996</v>
+        <v>45999</v>
       </c>
       <c r="O49" s="6" t="inlineStr">
         <is>
@@ -4418,19 +4418,19 @@
         </is>
       </c>
       <c r="Q49" s="6" t="n">
+        <v>3.75</v>
+      </c>
+      <c r="R49" s="6" t="n">
+        <v/>
+      </c>
+      <c r="S49" s="6" t="n">
+        <v/>
+      </c>
+      <c r="T49" s="6" t="n">
         <v>3.72</v>
       </c>
-      <c r="R49" s="6" t="n">
+      <c r="U49" s="21" t="n">
         <v>3.68</v>
-      </c>
-      <c r="S49" s="6" t="n">
-        <v>3.62</v>
-      </c>
-      <c r="T49" s="6" t="n">
-        <v>3.66</v>
-      </c>
-      <c r="U49" s="21" t="n">
-        <v>3.67</v>
       </c>
     </row>
     <row r="50">
@@ -4484,7 +4484,7 @@
         </is>
       </c>
       <c r="N50" s="48" t="n">
-        <v>45996</v>
+        <v>45999</v>
       </c>
       <c r="O50" s="6" t="inlineStr">
         <is>
@@ -4497,19 +4497,19 @@
         </is>
       </c>
       <c r="Q50" s="6" t="n">
+        <v>4.17</v>
+      </c>
+      <c r="R50" s="6" t="n">
+        <v/>
+      </c>
+      <c r="S50" s="6" t="n">
+        <v/>
+      </c>
+      <c r="T50" s="6" t="n">
         <v>4.14</v>
       </c>
-      <c r="R50" s="6" t="n">
+      <c r="U50" s="21" t="n">
         <v>4.11</v>
-      </c>
-      <c r="S50" s="6" t="n">
-        <v>4.06</v>
-      </c>
-      <c r="T50" s="6" t="n">
-        <v>4.09</v>
-      </c>
-      <c r="U50" s="21" t="n">
-        <v>4.09</v>
       </c>
     </row>
     <row r="51" ht="31.5" customHeight="1">
@@ -4610,7 +4610,7 @@
         </is>
       </c>
       <c r="N52" s="49" t="n">
-        <v>45996</v>
+        <v>45999</v>
       </c>
       <c r="O52" s="9" t="inlineStr">
         <is>
@@ -4623,16 +4623,16 @@
         </is>
       </c>
       <c r="Q52" s="9" t="n">
+        <v>5.9</v>
+      </c>
+      <c r="R52" s="9" t="n">
+        <v/>
+      </c>
+      <c r="S52" s="9" t="n">
+        <v/>
+      </c>
+      <c r="T52" s="9" t="n">
         <v>5.88</v>
-      </c>
-      <c r="R52" s="9" t="n">
-        <v>5.87</v>
-      </c>
-      <c r="S52" s="9" t="n">
-        <v>5.83</v>
-      </c>
-      <c r="T52" s="9" t="n">
-        <v>5.85</v>
       </c>
       <c r="U52" s="22" t="n">
         <v>5.87</v>

</xml_diff>

<commit_message>
Update dashboards - 2025-12-11
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -1208,7 +1208,7 @@
         </is>
       </c>
       <c r="F7" s="25" t="n">
-        <v>0.3129565816678153</v>
+        <v>0.215816678152998</v>
       </c>
       <c r="G7" s="25" t="n">
         <v>-2.062303243282817</v>
@@ -1700,7 +1700,7 @@
         </is>
       </c>
       <c r="N13" s="48" t="n">
-        <v>45985</v>
+        <v>45992</v>
       </c>
       <c r="O13" s="6" t="inlineStr">
         <is>
@@ -1713,19 +1713,19 @@
         </is>
       </c>
       <c r="Q13" s="24" t="n">
-        <v>191000</v>
+        <v>236000</v>
       </c>
       <c r="R13" s="24" t="n">
-        <v>218000</v>
+        <v>192000</v>
       </c>
       <c r="S13" s="24" t="n">
+        <v>217000</v>
+      </c>
+      <c r="T13" s="24" t="n">
         <v>222000</v>
       </c>
-      <c r="T13" s="24" t="n">
+      <c r="U13" s="26" t="n">
         <v>228000</v>
-      </c>
-      <c r="U13" s="26" t="n">
-        <v>229000</v>
       </c>
     </row>
     <row r="14">
@@ -1775,7 +1775,7 @@
         </is>
       </c>
       <c r="N14" s="48" t="n">
-        <v>45978</v>
+        <v>45985</v>
       </c>
       <c r="O14" s="6" t="inlineStr">
         <is>
@@ -1788,19 +1788,19 @@
         </is>
       </c>
       <c r="Q14" s="24" t="n">
-        <v>1939000</v>
+        <v>1838000</v>
       </c>
       <c r="R14" s="24" t="n">
-        <v>1943000</v>
+        <v>1937000</v>
       </c>
       <c r="S14" s="24" t="n">
+        <v>1944000</v>
+      </c>
+      <c r="T14" s="24" t="n">
         <v>1953000</v>
       </c>
-      <c r="T14" s="24" t="n">
+      <c r="U14" s="26" t="n">
         <v>1946000</v>
-      </c>
-      <c r="U14" s="26" t="n">
-        <v>1964000</v>
       </c>
     </row>
     <row r="15">
@@ -2788,7 +2788,7 @@
           <t>DGORDER</t>
         </is>
       </c>
-      <c r="C28" s="48" t="n">
+      <c r="C28" s="47" t="n">
         <v>45901</v>
       </c>
       <c r="D28" s="6" t="inlineStr">
@@ -2863,7 +2863,7 @@
           <t>DGORDER</t>
         </is>
       </c>
-      <c r="C29" s="48" t="n">
+      <c r="C29" s="47" t="n">
         <v>45901</v>
       </c>
       <c r="D29" s="6" t="inlineStr">
@@ -2903,7 +2903,7 @@
         </is>
       </c>
       <c r="N29" s="48" t="n">
-        <v>46000</v>
+        <v>46001</v>
       </c>
       <c r="O29" s="6" t="inlineStr">
         <is>
@@ -2916,19 +2916,19 @@
         </is>
       </c>
       <c r="Q29" s="6" t="n">
-        <v>2.2</v>
+        <v>2.18</v>
       </c>
       <c r="R29" s="6" t="n">
         <v>2.2</v>
       </c>
       <c r="S29" s="6" t="n">
-        <v/>
+        <v>2.2</v>
       </c>
       <c r="T29" s="6" t="n">
         <v/>
       </c>
       <c r="U29" s="21" t="n">
-        <v>2.18</v>
+        <v/>
       </c>
     </row>
     <row r="30">
@@ -2942,7 +2942,7 @@
           <t>ADXDNO</t>
         </is>
       </c>
-      <c r="C30" s="48" t="n">
+      <c r="C30" s="47" t="n">
         <v>45901</v>
       </c>
       <c r="D30" s="6" t="inlineStr">
@@ -2982,7 +2982,7 @@
         </is>
       </c>
       <c r="N30" s="48" t="n">
-        <v>46000</v>
+        <v>46001</v>
       </c>
       <c r="O30" s="6" t="inlineStr">
         <is>
@@ -2995,19 +2995,19 @@
         </is>
       </c>
       <c r="Q30" s="6" t="n">
-        <v>2.26</v>
+        <v>2.25</v>
       </c>
       <c r="R30" s="6" t="n">
         <v>2.26</v>
       </c>
       <c r="S30" s="6" t="n">
-        <v/>
+        <v>2.26</v>
       </c>
       <c r="T30" s="6" t="n">
         <v/>
       </c>
       <c r="U30" s="21" t="n">
-        <v>2.26</v>
+        <v/>
       </c>
     </row>
     <row r="31">
@@ -3017,7 +3017,7 @@
           <t>ADXDNO</t>
         </is>
       </c>
-      <c r="C31" s="48" t="n">
+      <c r="C31" s="47" t="n">
         <v>45901</v>
       </c>
       <c r="D31" s="6" t="inlineStr">
@@ -4251,7 +4251,7 @@
         </is>
       </c>
       <c r="N47" s="48" t="n">
-        <v>45999</v>
+        <v>46000</v>
       </c>
       <c r="O47" s="6" t="inlineStr">
         <is>
@@ -4330,7 +4330,7 @@
         </is>
       </c>
       <c r="N48" s="48" t="n">
-        <v>45999</v>
+        <v>46000</v>
       </c>
       <c r="O48" s="6" t="inlineStr">
         <is>
@@ -4343,19 +4343,19 @@
         </is>
       </c>
       <c r="Q48" s="6" t="n">
+        <v>3.61</v>
+      </c>
+      <c r="R48" s="6" t="n">
         <v>3.57</v>
-      </c>
-      <c r="R48" s="6" t="n">
-        <v/>
       </c>
       <c r="S48" s="6" t="n">
         <v/>
       </c>
       <c r="T48" s="6" t="n">
+        <v/>
+      </c>
+      <c r="U48" s="21" t="n">
         <v>3.56</v>
-      </c>
-      <c r="U48" s="21" t="n">
-        <v>3.52</v>
       </c>
     </row>
     <row r="49">
@@ -4405,7 +4405,7 @@
         </is>
       </c>
       <c r="N49" s="48" t="n">
-        <v>45999</v>
+        <v>46000</v>
       </c>
       <c r="O49" s="6" t="inlineStr">
         <is>
@@ -4418,19 +4418,19 @@
         </is>
       </c>
       <c r="Q49" s="6" t="n">
+        <v>3.78</v>
+      </c>
+      <c r="R49" s="6" t="n">
         <v>3.75</v>
-      </c>
-      <c r="R49" s="6" t="n">
-        <v/>
       </c>
       <c r="S49" s="6" t="n">
         <v/>
       </c>
       <c r="T49" s="6" t="n">
+        <v/>
+      </c>
+      <c r="U49" s="21" t="n">
         <v>3.72</v>
-      </c>
-      <c r="U49" s="21" t="n">
-        <v>3.68</v>
       </c>
     </row>
     <row r="50">
@@ -4484,7 +4484,7 @@
         </is>
       </c>
       <c r="N50" s="48" t="n">
-        <v>45999</v>
+        <v>46000</v>
       </c>
       <c r="O50" s="6" t="inlineStr">
         <is>
@@ -4497,19 +4497,19 @@
         </is>
       </c>
       <c r="Q50" s="6" t="n">
+        <v>4.18</v>
+      </c>
+      <c r="R50" s="6" t="n">
         <v>4.17</v>
-      </c>
-      <c r="R50" s="6" t="n">
-        <v/>
       </c>
       <c r="S50" s="6" t="n">
         <v/>
       </c>
       <c r="T50" s="6" t="n">
+        <v/>
+      </c>
+      <c r="U50" s="21" t="n">
         <v>4.14</v>
-      </c>
-      <c r="U50" s="21" t="n">
-        <v>4.11</v>
       </c>
     </row>
     <row r="51" ht="31.5" customHeight="1">
@@ -4558,7 +4558,7 @@
           <t>MORTGAGE30US</t>
         </is>
       </c>
-      <c r="N51" s="48" t="n">
+      <c r="N51" s="47" t="n">
         <v>45992</v>
       </c>
       <c r="O51" s="6" t="inlineStr">
@@ -4610,7 +4610,7 @@
         </is>
       </c>
       <c r="N52" s="49" t="n">
-        <v>45999</v>
+        <v>46000</v>
       </c>
       <c r="O52" s="9" t="inlineStr">
         <is>
@@ -4623,19 +4623,19 @@
         </is>
       </c>
       <c r="Q52" s="9" t="n">
+        <v>5.91</v>
+      </c>
+      <c r="R52" s="9" t="n">
         <v>5.9</v>
-      </c>
-      <c r="R52" s="9" t="n">
-        <v/>
       </c>
       <c r="S52" s="9" t="n">
         <v/>
       </c>
       <c r="T52" s="9" t="n">
+        <v/>
+      </c>
+      <c r="U52" s="22" t="n">
         <v>5.88</v>
-      </c>
-      <c r="U52" s="22" t="n">
-        <v>5.87</v>
       </c>
     </row>
     <row r="53" ht="21" customHeight="1">

</xml_diff>

<commit_message>
Update dashboards - 2025-12-12
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -1506,7 +1506,7 @@
           <t>PCEDGC96</t>
         </is>
       </c>
-      <c r="C11" s="48" t="n">
+      <c r="C11" s="47" t="n">
         <v>45901</v>
       </c>
       <c r="D11" s="6" t="inlineStr">
@@ -1581,7 +1581,7 @@
           <t>PCEDGC96</t>
         </is>
       </c>
-      <c r="C12" s="48" t="n">
+      <c r="C12" s="47" t="n">
         <v>45901</v>
       </c>
       <c r="D12" s="6" t="inlineStr">
@@ -1660,7 +1660,7 @@
           <t>PCENDC96</t>
         </is>
       </c>
-      <c r="C13" s="48" t="n">
+      <c r="C13" s="47" t="n">
         <v>45901</v>
       </c>
       <c r="D13" s="6" t="inlineStr">
@@ -1735,7 +1735,7 @@
           <t>PCENDC96</t>
         </is>
       </c>
-      <c r="C14" s="48" t="n">
+      <c r="C14" s="47" t="n">
         <v>45901</v>
       </c>
       <c r="D14" s="6" t="inlineStr">
@@ -1814,7 +1814,7 @@
           <t>PCESC96</t>
         </is>
       </c>
-      <c r="C15" s="48" t="n">
+      <c r="C15" s="47" t="n">
         <v>45901</v>
       </c>
       <c r="D15" s="6" t="inlineStr">
@@ -1889,7 +1889,7 @@
           <t>PCESC96</t>
         </is>
       </c>
-      <c r="C16" s="48" t="n">
+      <c r="C16" s="47" t="n">
         <v>45901</v>
       </c>
       <c r="D16" s="6" t="inlineStr">
@@ -2106,7 +2106,7 @@
           <t>DSPIC96</t>
         </is>
       </c>
-      <c r="C19" s="48" t="n">
+      <c r="C19" s="47" t="n">
         <v>45901</v>
       </c>
       <c r="D19" s="6" t="inlineStr">
@@ -2177,7 +2177,7 @@
           <t>DSPIC96</t>
         </is>
       </c>
-      <c r="C20" s="48" t="n">
+      <c r="C20" s="47" t="n">
         <v>45901</v>
       </c>
       <c r="D20" s="6" t="inlineStr">
@@ -2256,7 +2256,7 @@
           <t>PSAVERT</t>
         </is>
       </c>
-      <c r="C21" s="48" t="n">
+      <c r="C21" s="47" t="n">
         <v>45901</v>
       </c>
       <c r="D21" s="6" t="inlineStr">
@@ -2331,7 +2331,7 @@
           <t>TOTALSA</t>
         </is>
       </c>
-      <c r="C22" s="48" t="n">
+      <c r="C22" s="47" t="n">
         <v>45962</v>
       </c>
       <c r="D22" s="6" t="inlineStr">
@@ -2406,7 +2406,7 @@
           <t>TOTALSA</t>
         </is>
       </c>
-      <c r="C23" s="48" t="n">
+      <c r="C23" s="47" t="n">
         <v>45962</v>
       </c>
       <c r="D23" s="6" t="inlineStr">
@@ -2480,7 +2480,7 @@
           <t>REVOLSL</t>
         </is>
       </c>
-      <c r="C24" s="48" t="n">
+      <c r="C24" s="47" t="n">
         <v>45931</v>
       </c>
       <c r="D24" s="6" t="inlineStr">
@@ -2519,7 +2519,7 @@
           <t>PCEPI</t>
         </is>
       </c>
-      <c r="N24" s="48" t="n">
+      <c r="N24" s="47" t="n">
         <v>45901</v>
       </c>
       <c r="O24" s="6" t="inlineStr">
@@ -2559,7 +2559,7 @@
           <t>NONREVSL</t>
         </is>
       </c>
-      <c r="C25" s="48" t="n">
+      <c r="C25" s="47" t="n">
         <v>45931</v>
       </c>
       <c r="D25" s="6" t="inlineStr">
@@ -2594,7 +2594,7 @@
           <t>PCEPI</t>
         </is>
       </c>
-      <c r="N25" s="48" t="n">
+      <c r="N25" s="47" t="n">
         <v>45901</v>
       </c>
       <c r="O25" s="6" t="inlineStr">
@@ -2673,7 +2673,7 @@
           <t>PCEPILFE</t>
         </is>
       </c>
-      <c r="N26" s="48" t="n">
+      <c r="N26" s="47" t="n">
         <v>45901</v>
       </c>
       <c r="O26" s="6" t="inlineStr">
@@ -2748,7 +2748,7 @@
           <t>PCEPILFE</t>
         </is>
       </c>
-      <c r="N27" s="48" t="n">
+      <c r="N27" s="47" t="n">
         <v>45901</v>
       </c>
       <c r="O27" s="6" t="inlineStr">
@@ -2903,7 +2903,7 @@
         </is>
       </c>
       <c r="N29" s="48" t="n">
-        <v>46001</v>
+        <v>46002</v>
       </c>
       <c r="O29" s="6" t="inlineStr">
         <is>
@@ -2919,13 +2919,13 @@
         <v>2.18</v>
       </c>
       <c r="R29" s="6" t="n">
-        <v>2.2</v>
+        <v>2.18</v>
       </c>
       <c r="S29" s="6" t="n">
         <v>2.2</v>
       </c>
       <c r="T29" s="6" t="n">
-        <v/>
+        <v>2.2</v>
       </c>
       <c r="U29" s="21" t="n">
         <v/>
@@ -2982,7 +2982,7 @@
         </is>
       </c>
       <c r="N30" s="48" t="n">
-        <v>46001</v>
+        <v>46002</v>
       </c>
       <c r="O30" s="6" t="inlineStr">
         <is>
@@ -2998,13 +2998,13 @@
         <v>2.25</v>
       </c>
       <c r="R30" s="6" t="n">
-        <v>2.26</v>
+        <v>2.25</v>
       </c>
       <c r="S30" s="6" t="n">
         <v>2.26</v>
       </c>
       <c r="T30" s="6" t="n">
-        <v/>
+        <v>2.26</v>
       </c>
       <c r="U30" s="21" t="n">
         <v/>
@@ -3660,7 +3660,7 @@
           <t>DTWEXBGS</t>
         </is>
       </c>
-      <c r="N39" s="48" t="n">
+      <c r="N39" s="47" t="n">
         <v>45996</v>
       </c>
       <c r="O39" s="6" t="inlineStr">
@@ -4124,8 +4124,8 @@
           <t>BOPTEXP</t>
         </is>
       </c>
-      <c r="C46" s="47" t="n">
-        <v>45870</v>
+      <c r="C46" s="48" t="n">
+        <v>45901</v>
       </c>
       <c r="D46" s="6" t="inlineStr">
         <is>
@@ -4138,19 +4138,19 @@
         </is>
       </c>
       <c r="F46" s="24" t="n">
-        <v>280832</v>
+        <v>289305</v>
       </c>
       <c r="G46" s="24" t="n">
-        <v>280602</v>
+        <v>280921</v>
       </c>
       <c r="H46" s="24" t="n">
+        <v>281602</v>
+      </c>
+      <c r="I46" s="24" t="n">
         <v>279650</v>
       </c>
-      <c r="I46" s="24" t="n">
+      <c r="J46" s="24" t="n">
         <v>280391</v>
-      </c>
-      <c r="J46" s="24" t="n">
-        <v>291785</v>
       </c>
       <c r="K46" s="5" t="n"/>
       <c r="L46" s="29" t="inlineStr">
@@ -4211,8 +4211,8 @@
           <t>BOPTEXP</t>
         </is>
       </c>
-      <c r="C47" s="47" t="n">
-        <v>45870</v>
+      <c r="C47" s="48" t="n">
+        <v>45901</v>
       </c>
       <c r="D47" s="6" t="inlineStr">
         <is>
@@ -4225,19 +4225,19 @@
         </is>
       </c>
       <c r="F47" s="38" t="n">
-        <v>0.0008196662889075057</v>
+        <v>0.02984468943226037</v>
       </c>
       <c r="G47" s="38" t="n">
-        <v>0.003404255319148897</v>
+        <v>-0.002418306688162675</v>
       </c>
       <c r="H47" s="38" t="n">
+        <v>0.006980153763633146</v>
+      </c>
+      <c r="I47" s="38" t="n">
         <v>-0.002642738176332315</v>
       </c>
-      <c r="I47" s="38" t="n">
+      <c r="J47" s="38" t="n">
         <v>-0.03904929999828644</v>
-      </c>
-      <c r="J47" s="38" t="n">
-        <v>0.02888646757853675</v>
       </c>
       <c r="K47" s="5" t="n"/>
       <c r="L47" s="28" t="inlineStr">
@@ -4251,7 +4251,7 @@
         </is>
       </c>
       <c r="N47" s="48" t="n">
-        <v>46000</v>
+        <v>46001</v>
       </c>
       <c r="O47" s="6" t="inlineStr">
         <is>
@@ -4290,8 +4290,8 @@
           <t>BOPTIMP</t>
         </is>
       </c>
-      <c r="C48" s="47" t="n">
-        <v>45870</v>
+      <c r="C48" s="48" t="n">
+        <v>45901</v>
       </c>
       <c r="D48" s="6" t="inlineStr">
         <is>
@@ -4304,19 +4304,19 @@
         </is>
       </c>
       <c r="F48" s="24" t="n">
-        <v>340382</v>
+        <v>342133</v>
       </c>
       <c r="G48" s="24" t="n">
+        <v>340185</v>
+      </c>
+      <c r="H48" s="24" t="n">
         <v>358756</v>
       </c>
-      <c r="H48" s="24" t="n">
+      <c r="I48" s="24" t="n">
         <v>338736</v>
       </c>
-      <c r="I48" s="24" t="n">
+      <c r="J48" s="24" t="n">
         <v>351506</v>
-      </c>
-      <c r="J48" s="24" t="n">
-        <v>351977</v>
       </c>
       <c r="K48" s="5" t="n"/>
       <c r="L48" s="28" t="inlineStr">
@@ -4330,7 +4330,7 @@
         </is>
       </c>
       <c r="N48" s="48" t="n">
-        <v>46000</v>
+        <v>46001</v>
       </c>
       <c r="O48" s="6" t="inlineStr">
         <is>
@@ -4343,19 +4343,19 @@
         </is>
       </c>
       <c r="Q48" s="6" t="n">
+        <v>3.54</v>
+      </c>
+      <c r="R48" s="6" t="n">
         <v>3.61</v>
       </c>
-      <c r="R48" s="6" t="n">
+      <c r="S48" s="6" t="n">
         <v>3.57</v>
-      </c>
-      <c r="S48" s="6" t="n">
-        <v/>
       </c>
       <c r="T48" s="6" t="n">
         <v/>
       </c>
       <c r="U48" s="21" t="n">
-        <v>3.56</v>
+        <v/>
       </c>
     </row>
     <row r="49">
@@ -4365,8 +4365,8 @@
           <t>BOPTIMP</t>
         </is>
       </c>
-      <c r="C49" s="47" t="n">
-        <v>45870</v>
+      <c r="C49" s="48" t="n">
+        <v>45901</v>
       </c>
       <c r="D49" s="6" t="inlineStr">
         <is>
@@ -4379,19 +4379,19 @@
         </is>
       </c>
       <c r="F49" s="38" t="n">
-        <v>-0.05121586816666479</v>
+        <v>0.005726295986007601</v>
       </c>
       <c r="G49" s="38" t="n">
+        <v>-0.05176498790264139</v>
+      </c>
+      <c r="H49" s="38" t="n">
         <v>0.05910207359123332</v>
       </c>
-      <c r="H49" s="38" t="n">
+      <c r="I49" s="38" t="n">
         <v>-0.03632939409284619</v>
       </c>
-      <c r="I49" s="38" t="n">
+      <c r="J49" s="38" t="n">
         <v>-0.001338155618122783</v>
-      </c>
-      <c r="J49" s="38" t="n">
-        <v>-0.1619854623547367</v>
       </c>
       <c r="K49" s="5" t="n"/>
       <c r="L49" s="28" t="inlineStr">
@@ -4405,7 +4405,7 @@
         </is>
       </c>
       <c r="N49" s="48" t="n">
-        <v>46000</v>
+        <v>46001</v>
       </c>
       <c r="O49" s="6" t="inlineStr">
         <is>
@@ -4418,19 +4418,19 @@
         </is>
       </c>
       <c r="Q49" s="6" t="n">
+        <v>3.72</v>
+      </c>
+      <c r="R49" s="6" t="n">
         <v>3.78</v>
       </c>
-      <c r="R49" s="6" t="n">
+      <c r="S49" s="6" t="n">
         <v>3.75</v>
-      </c>
-      <c r="S49" s="6" t="n">
-        <v/>
       </c>
       <c r="T49" s="6" t="n">
         <v/>
       </c>
       <c r="U49" s="21" t="n">
-        <v>3.72</v>
+        <v/>
       </c>
     </row>
     <row r="50">
@@ -4444,8 +4444,8 @@
           <t>BOPSTB</t>
         </is>
       </c>
-      <c r="C50" s="47" t="n">
-        <v>45870</v>
+      <c r="C50" s="48" t="n">
+        <v>45901</v>
       </c>
       <c r="D50" s="6" t="inlineStr">
         <is>
@@ -4458,19 +4458,19 @@
         </is>
       </c>
       <c r="F50" s="24" t="n">
-        <v>26058</v>
+        <v>26157</v>
       </c>
       <c r="G50" s="24" t="n">
+        <v>26795</v>
+      </c>
+      <c r="H50" s="24" t="n">
         <v>25569</v>
       </c>
-      <c r="H50" s="24" t="n">
+      <c r="I50" s="24" t="n">
         <v>26631</v>
       </c>
-      <c r="I50" s="24" t="n">
+      <c r="J50" s="24" t="n">
         <v>26236</v>
-      </c>
-      <c r="J50" s="24" t="n">
-        <v>26721</v>
       </c>
       <c r="K50" s="5" t="n"/>
       <c r="L50" s="28" t="inlineStr">
@@ -4484,7 +4484,7 @@
         </is>
       </c>
       <c r="N50" s="48" t="n">
-        <v>46000</v>
+        <v>46001</v>
       </c>
       <c r="O50" s="6" t="inlineStr">
         <is>
@@ -4497,19 +4497,19 @@
         </is>
       </c>
       <c r="Q50" s="6" t="n">
+        <v>4.13</v>
+      </c>
+      <c r="R50" s="6" t="n">
         <v>4.18</v>
       </c>
-      <c r="R50" s="6" t="n">
+      <c r="S50" s="6" t="n">
         <v>4.17</v>
-      </c>
-      <c r="S50" s="6" t="n">
-        <v/>
       </c>
       <c r="T50" s="6" t="n">
         <v/>
       </c>
       <c r="U50" s="21" t="n">
-        <v>4.14</v>
+        <v/>
       </c>
     </row>
     <row r="51" ht="31.5" customHeight="1">
@@ -4519,8 +4519,8 @@
           <t>BOPSTB</t>
         </is>
       </c>
-      <c r="C51" s="47" t="n">
-        <v>45870</v>
+      <c r="C51" s="48" t="n">
+        <v>45901</v>
       </c>
       <c r="D51" s="6" t="inlineStr">
         <is>
@@ -4533,19 +4533,19 @@
         </is>
       </c>
       <c r="F51" s="38" t="n">
-        <v>0.01912472134225029</v>
+        <v>-0.02381041239037129</v>
       </c>
       <c r="G51" s="38" t="n">
+        <v>0.04794868786421058</v>
+      </c>
+      <c r="H51" s="38" t="n">
         <v>-0.03987833727610679</v>
       </c>
-      <c r="H51" s="38" t="n">
+      <c r="I51" s="38" t="n">
         <v>0.01505564872693999</v>
       </c>
-      <c r="I51" s="38" t="n">
+      <c r="J51" s="38" t="n">
         <v>-0.01815051831892522</v>
-      </c>
-      <c r="J51" s="38" t="n">
-        <v>0.02391079434417742</v>
       </c>
       <c r="K51" s="5" t="n"/>
       <c r="L51" s="28" t="inlineStr">
@@ -4558,8 +4558,8 @@
           <t>MORTGAGE30US</t>
         </is>
       </c>
-      <c r="N51" s="47" t="n">
-        <v>45992</v>
+      <c r="N51" s="48" t="n">
+        <v>45999</v>
       </c>
       <c r="O51" s="6" t="inlineStr">
         <is>
@@ -4572,19 +4572,19 @@
         </is>
       </c>
       <c r="Q51" s="6" t="n">
+        <v>6.22</v>
+      </c>
+      <c r="R51" s="6" t="n">
         <v>6.19</v>
       </c>
-      <c r="R51" s="6" t="n">
+      <c r="S51" s="6" t="n">
         <v>6.23</v>
       </c>
-      <c r="S51" s="6" t="n">
+      <c r="T51" s="6" t="n">
         <v>6.26</v>
       </c>
-      <c r="T51" s="6" t="n">
+      <c r="U51" s="21" t="n">
         <v>6.24</v>
-      </c>
-      <c r="U51" s="21" t="n">
-        <v>6.22</v>
       </c>
     </row>
     <row r="52" ht="16.15" customHeight="1" thickBot="1">
@@ -4610,7 +4610,7 @@
         </is>
       </c>
       <c r="N52" s="49" t="n">
-        <v>46000</v>
+        <v>46001</v>
       </c>
       <c r="O52" s="9" t="inlineStr">
         <is>
@@ -4623,19 +4623,19 @@
         </is>
       </c>
       <c r="Q52" s="9" t="n">
+        <v>5.89</v>
+      </c>
+      <c r="R52" s="9" t="n">
         <v>5.91</v>
       </c>
-      <c r="R52" s="9" t="n">
+      <c r="S52" s="9" t="n">
         <v>5.9</v>
-      </c>
-      <c r="S52" s="9" t="n">
-        <v/>
       </c>
       <c r="T52" s="9" t="n">
         <v/>
       </c>
       <c r="U52" s="22" t="n">
-        <v>5.88</v>
+        <v/>
       </c>
     </row>
     <row r="53" ht="21" customHeight="1">

</xml_diff>

<commit_message>
Update dashboards - 2025-12-13
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -2903,7 +2903,7 @@
         </is>
       </c>
       <c r="N29" s="48" t="n">
-        <v>46002</v>
+        <v>46003</v>
       </c>
       <c r="O29" s="6" t="inlineStr">
         <is>
@@ -2916,19 +2916,19 @@
         </is>
       </c>
       <c r="Q29" s="6" t="n">
-        <v>2.18</v>
+        <v>2.2</v>
       </c>
       <c r="R29" s="6" t="n">
         <v>2.18</v>
       </c>
       <c r="S29" s="6" t="n">
-        <v>2.2</v>
+        <v>2.18</v>
       </c>
       <c r="T29" s="6" t="n">
         <v>2.2</v>
       </c>
       <c r="U29" s="21" t="n">
-        <v/>
+        <v>2.2</v>
       </c>
     </row>
     <row r="30">
@@ -2982,7 +2982,7 @@
         </is>
       </c>
       <c r="N30" s="48" t="n">
-        <v>46002</v>
+        <v>46003</v>
       </c>
       <c r="O30" s="6" t="inlineStr">
         <is>
@@ -2995,19 +2995,19 @@
         </is>
       </c>
       <c r="Q30" s="6" t="n">
-        <v>2.25</v>
+        <v>2.26</v>
       </c>
       <c r="R30" s="6" t="n">
         <v>2.25</v>
       </c>
       <c r="S30" s="6" t="n">
-        <v>2.26</v>
+        <v>2.25</v>
       </c>
       <c r="T30" s="6" t="n">
         <v>2.26</v>
       </c>
       <c r="U30" s="21" t="n">
-        <v/>
+        <v>2.26</v>
       </c>
     </row>
     <row r="31">
@@ -4251,7 +4251,7 @@
         </is>
       </c>
       <c r="N47" s="48" t="n">
-        <v>46001</v>
+        <v>46002</v>
       </c>
       <c r="O47" s="6" t="inlineStr">
         <is>
@@ -4264,7 +4264,7 @@
         </is>
       </c>
       <c r="Q47" s="6" t="n">
-        <v>3.89</v>
+        <v>3.64</v>
       </c>
       <c r="R47" s="6" t="n">
         <v>3.89</v>
@@ -4330,7 +4330,7 @@
         </is>
       </c>
       <c r="N48" s="48" t="n">
-        <v>46001</v>
+        <v>46002</v>
       </c>
       <c r="O48" s="6" t="inlineStr">
         <is>
@@ -4343,16 +4343,16 @@
         </is>
       </c>
       <c r="Q48" s="6" t="n">
+        <v>3.52</v>
+      </c>
+      <c r="R48" s="6" t="n">
         <v>3.54</v>
       </c>
-      <c r="R48" s="6" t="n">
+      <c r="S48" s="6" t="n">
         <v>3.61</v>
       </c>
-      <c r="S48" s="6" t="n">
+      <c r="T48" s="6" t="n">
         <v>3.57</v>
-      </c>
-      <c r="T48" s="6" t="n">
-        <v/>
       </c>
       <c r="U48" s="21" t="n">
         <v/>
@@ -4405,7 +4405,7 @@
         </is>
       </c>
       <c r="N49" s="48" t="n">
-        <v>46001</v>
+        <v>46002</v>
       </c>
       <c r="O49" s="6" t="inlineStr">
         <is>
@@ -4421,13 +4421,13 @@
         <v>3.72</v>
       </c>
       <c r="R49" s="6" t="n">
+        <v>3.72</v>
+      </c>
+      <c r="S49" s="6" t="n">
         <v>3.78</v>
       </c>
-      <c r="S49" s="6" t="n">
+      <c r="T49" s="6" t="n">
         <v>3.75</v>
-      </c>
-      <c r="T49" s="6" t="n">
-        <v/>
       </c>
       <c r="U49" s="21" t="n">
         <v/>
@@ -4484,7 +4484,7 @@
         </is>
       </c>
       <c r="N50" s="48" t="n">
-        <v>46001</v>
+        <v>46002</v>
       </c>
       <c r="O50" s="6" t="inlineStr">
         <is>
@@ -4497,16 +4497,16 @@
         </is>
       </c>
       <c r="Q50" s="6" t="n">
+        <v>4.14</v>
+      </c>
+      <c r="R50" s="6" t="n">
         <v>4.13</v>
       </c>
-      <c r="R50" s="6" t="n">
+      <c r="S50" s="6" t="n">
         <v>4.18</v>
       </c>
-      <c r="S50" s="6" t="n">
+      <c r="T50" s="6" t="n">
         <v>4.17</v>
-      </c>
-      <c r="T50" s="6" t="n">
-        <v/>
       </c>
       <c r="U50" s="21" t="n">
         <v/>
@@ -4610,7 +4610,7 @@
         </is>
       </c>
       <c r="N52" s="49" t="n">
-        <v>46001</v>
+        <v>46002</v>
       </c>
       <c r="O52" s="9" t="inlineStr">
         <is>
@@ -4623,16 +4623,16 @@
         </is>
       </c>
       <c r="Q52" s="9" t="n">
+        <v>5.87</v>
+      </c>
+      <c r="R52" s="9" t="n">
         <v>5.89</v>
       </c>
-      <c r="R52" s="9" t="n">
+      <c r="S52" s="9" t="n">
         <v>5.91</v>
       </c>
-      <c r="S52" s="9" t="n">
+      <c r="T52" s="9" t="n">
         <v>5.9</v>
-      </c>
-      <c r="T52" s="9" t="n">
-        <v/>
       </c>
       <c r="U52" s="22" t="n">
         <v/>

</xml_diff>

<commit_message>
Update dashboards - 2025-12-16
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -929,8 +929,8 @@
           <t>PAYEMS</t>
         </is>
       </c>
-      <c r="N3" s="47" t="n">
-        <v>45901</v>
+      <c r="N3" s="48" t="n">
+        <v>45962</v>
       </c>
       <c r="O3" s="6" t="inlineStr">
         <is>
@@ -943,19 +943,19 @@
         </is>
       </c>
       <c r="Q3" s="24" t="n">
-        <v>119</v>
+        <v>64</v>
       </c>
       <c r="R3" s="24" t="n">
-        <v>-4</v>
+        <v>-105</v>
       </c>
       <c r="S3" s="24" t="n">
+        <v>108</v>
+      </c>
+      <c r="T3" s="24" t="n">
+        <v>-26</v>
+      </c>
+      <c r="U3" s="26" t="n">
         <v>72</v>
-      </c>
-      <c r="T3" s="24" t="n">
-        <v>-13</v>
-      </c>
-      <c r="U3" s="26" t="n">
-        <v>19</v>
       </c>
     </row>
     <row r="4">
@@ -1000,8 +1000,8 @@
           <t>PAYEMS</t>
         </is>
       </c>
-      <c r="N4" s="47" t="n">
-        <v>45901</v>
+      <c r="N4" s="48" t="n">
+        <v>45962</v>
       </c>
       <c r="O4" s="6" t="inlineStr">
         <is>
@@ -1014,19 +1014,19 @@
         </is>
       </c>
       <c r="Q4" s="38" t="n">
-        <v>0.008287327715805298</v>
+        <v>0.005882019178030375</v>
       </c>
       <c r="R4" s="38" t="n">
-        <v>0.009065374444880247</v>
+        <v>0.007135730433574559</v>
       </c>
       <c r="S4" s="38" t="n">
+        <v>0.008078881210758367</v>
+      </c>
+      <c r="T4" s="38" t="n">
+        <v>0.008926199121930236</v>
+      </c>
+      <c r="U4" s="23" t="n">
         <v>0.009544122579951013</v>
-      </c>
-      <c r="T4" s="38" t="n">
-        <v>0.009650761485609347</v>
-      </c>
-      <c r="U4" s="23" t="n">
-        <v>0.01028968243911093</v>
       </c>
     </row>
     <row r="5" ht="31.5" customHeight="1">
@@ -1154,8 +1154,8 @@
           <t>UNRATE</t>
         </is>
       </c>
-      <c r="N6" s="47" t="n">
-        <v>45901</v>
+      <c r="N6" s="48" t="n">
+        <v>45962</v>
       </c>
       <c r="O6" s="6" t="inlineStr">
         <is>
@@ -1168,16 +1168,16 @@
         </is>
       </c>
       <c r="Q6" s="6" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="R6" s="6" t="n">
+        <v/>
+      </c>
+      <c r="S6" s="6" t="n">
         <v>4.4</v>
       </c>
-      <c r="R6" s="6" t="n">
+      <c r="T6" s="6" t="n">
         <v>4.3</v>
-      </c>
-      <c r="S6" s="6" t="n">
-        <v>4.2</v>
-      </c>
-      <c r="T6" s="6" t="n">
-        <v>4.1</v>
       </c>
       <c r="U6" s="21" t="n">
         <v>4.2</v>
@@ -1233,8 +1233,8 @@
           <t>U6RATE</t>
         </is>
       </c>
-      <c r="N7" s="47" t="n">
-        <v>45901</v>
+      <c r="N7" s="48" t="n">
+        <v>45962</v>
       </c>
       <c r="O7" s="6" t="inlineStr">
         <is>
@@ -1247,19 +1247,19 @@
         </is>
       </c>
       <c r="Q7" s="6" t="n">
+        <v>8.699999999999999</v>
+      </c>
+      <c r="R7" s="6" t="n">
+        <v/>
+      </c>
+      <c r="S7" s="6" t="n">
         <v>8</v>
       </c>
-      <c r="R7" s="6" t="n">
+      <c r="T7" s="6" t="n">
         <v>8.1</v>
       </c>
-      <c r="S7" s="6" t="n">
+      <c r="U7" s="21" t="n">
         <v>7.9</v>
-      </c>
-      <c r="T7" s="6" t="n">
-        <v>7.7</v>
-      </c>
-      <c r="U7" s="21" t="n">
-        <v>7.8</v>
       </c>
     </row>
     <row r="8" ht="31.5" customHeight="1">
@@ -1312,8 +1312,8 @@
           <t>CIVPART</t>
         </is>
       </c>
-      <c r="N8" s="47" t="n">
-        <v>45901</v>
+      <c r="N8" s="48" t="n">
+        <v>45962</v>
       </c>
       <c r="O8" s="6" t="inlineStr">
         <is>
@@ -1326,19 +1326,19 @@
         </is>
       </c>
       <c r="Q8" s="6" t="n">
+        <v>62.5</v>
+      </c>
+      <c r="R8" s="6" t="n">
+        <v/>
+      </c>
+      <c r="S8" s="6" t="n">
         <v>62.4</v>
-      </c>
-      <c r="R8" s="6" t="n">
-        <v>62.3</v>
-      </c>
-      <c r="S8" s="6" t="n">
-        <v>62.2</v>
       </c>
       <c r="T8" s="6" t="n">
         <v>62.3</v>
       </c>
       <c r="U8" s="21" t="n">
-        <v>62.4</v>
+        <v>62.2</v>
       </c>
     </row>
     <row r="9">
@@ -1391,8 +1391,8 @@
           <t>EMRATIO</t>
         </is>
       </c>
-      <c r="N9" s="47" t="n">
-        <v>45901</v>
+      <c r="N9" s="48" t="n">
+        <v>45962</v>
       </c>
       <c r="O9" s="6" t="inlineStr">
         <is>
@@ -1405,19 +1405,19 @@
         </is>
       </c>
       <c r="Q9" s="6" t="n">
+        <v>59.6</v>
+      </c>
+      <c r="R9" s="6" t="n">
+        <v/>
+      </c>
+      <c r="S9" s="6" t="n">
         <v>59.7</v>
       </c>
-      <c r="R9" s="6" t="n">
+      <c r="T9" s="6" t="n">
         <v>59.6</v>
       </c>
-      <c r="S9" s="6" t="n">
+      <c r="U9" s="21" t="n">
         <v>59.6</v>
-      </c>
-      <c r="T9" s="6" t="n">
-        <v>59.7</v>
-      </c>
-      <c r="U9" s="21" t="n">
-        <v>59.7</v>
       </c>
     </row>
     <row r="10">
@@ -1466,7 +1466,7 @@
           <t>JTSJOR</t>
         </is>
       </c>
-      <c r="N10" s="48" t="n">
+      <c r="N10" s="47" t="n">
         <v>45931</v>
       </c>
       <c r="O10" s="6" t="inlineStr">
@@ -1545,7 +1545,7 @@
           <t>JTSHIR</t>
         </is>
       </c>
-      <c r="N11" s="48" t="n">
+      <c r="N11" s="47" t="n">
         <v>45931</v>
       </c>
       <c r="O11" s="6" t="inlineStr">
@@ -1620,7 +1620,7 @@
           <t>JTSTSR</t>
         </is>
       </c>
-      <c r="N12" s="48" t="n">
+      <c r="N12" s="47" t="n">
         <v>45931</v>
       </c>
       <c r="O12" s="6" t="inlineStr">
@@ -1853,8 +1853,8 @@
           <t>AWHAETP</t>
         </is>
       </c>
-      <c r="N15" s="47" t="n">
-        <v>45901</v>
+      <c r="N15" s="48" t="n">
+        <v>45962</v>
       </c>
       <c r="O15" s="6" t="inlineStr">
         <is>
@@ -1867,13 +1867,13 @@
         </is>
       </c>
       <c r="Q15" s="24" t="n">
-        <v>34.2</v>
+        <v>34.3</v>
       </c>
       <c r="R15" s="24" t="n">
         <v>34.2</v>
       </c>
       <c r="S15" s="24" t="n">
-        <v>34.3</v>
+        <v>34.2</v>
       </c>
       <c r="T15" s="24" t="n">
         <v>34.2</v>
@@ -1940,8 +1940,8 @@
           <t>RSAFS</t>
         </is>
       </c>
-      <c r="C17" s="47" t="n">
-        <v>45901</v>
+      <c r="C17" s="48" t="n">
+        <v>45931</v>
       </c>
       <c r="D17" s="6" t="inlineStr">
         <is>
@@ -1954,19 +1954,19 @@
         </is>
       </c>
       <c r="F17" s="25" t="n">
-        <v>0.001637846129888487</v>
+        <v>0.0002580402051215458</v>
       </c>
       <c r="G17" s="25" t="n">
-        <v>0.005952781743703284</v>
+        <v>0.001016810168101623</v>
       </c>
       <c r="H17" s="25" t="n">
+        <v>0.00545946488174831</v>
+      </c>
+      <c r="I17" s="25" t="n">
         <v>0.006492096487988874</v>
       </c>
-      <c r="I17" s="25" t="n">
+      <c r="J17" s="25" t="n">
         <v>0.009680198742914703</v>
-      </c>
-      <c r="J17" s="25" t="n">
-        <v>-0.007880419346928291</v>
       </c>
       <c r="K17" s="5" t="n"/>
       <c r="L17" s="29" t="inlineStr">
@@ -2027,8 +2027,8 @@
           <t>RSAFS</t>
         </is>
       </c>
-      <c r="C18" s="47" t="n">
-        <v>45901</v>
+      <c r="C18" s="48" t="n">
+        <v>45931</v>
       </c>
       <c r="D18" s="6" t="inlineStr">
         <is>
@@ -2041,19 +2041,19 @@
         </is>
       </c>
       <c r="F18" s="25" t="n">
-        <v>0.04261856857461769</v>
+        <v>0.03469007301537984</v>
       </c>
       <c r="G18" s="25" t="n">
-        <v>0.05024109124453582</v>
+        <v>0.0418018504953382</v>
       </c>
       <c r="H18" s="25" t="n">
+        <v>0.04972605550048132</v>
+      </c>
+      <c r="I18" s="25" t="n">
         <v>0.04134309243240536</v>
       </c>
-      <c r="I18" s="25" t="n">
+      <c r="J18" s="25" t="n">
         <v>0.0441678737351054</v>
-      </c>
-      <c r="J18" s="25" t="n">
-        <v>0.03367187567662758</v>
       </c>
       <c r="K18" s="5" t="n"/>
       <c r="L18" s="28" t="inlineStr">
@@ -2903,7 +2903,7 @@
         </is>
       </c>
       <c r="N29" s="48" t="n">
-        <v>46003</v>
+        <v>46006</v>
       </c>
       <c r="O29" s="6" t="inlineStr">
         <is>
@@ -2916,16 +2916,16 @@
         </is>
       </c>
       <c r="Q29" s="6" t="n">
+        <v>2.21</v>
+      </c>
+      <c r="R29" s="6" t="n">
         <v>2.2</v>
-      </c>
-      <c r="R29" s="6" t="n">
-        <v>2.18</v>
       </c>
       <c r="S29" s="6" t="n">
         <v>2.18</v>
       </c>
       <c r="T29" s="6" t="n">
-        <v>2.2</v>
+        <v>2.18</v>
       </c>
       <c r="U29" s="21" t="n">
         <v>2.2</v>
@@ -2982,7 +2982,7 @@
         </is>
       </c>
       <c r="N30" s="48" t="n">
-        <v>46003</v>
+        <v>46006</v>
       </c>
       <c r="O30" s="6" t="inlineStr">
         <is>
@@ -2995,16 +2995,16 @@
         </is>
       </c>
       <c r="Q30" s="6" t="n">
+        <v>2.25</v>
+      </c>
+      <c r="R30" s="6" t="n">
         <v>2.26</v>
-      </c>
-      <c r="R30" s="6" t="n">
-        <v>2.25</v>
       </c>
       <c r="S30" s="6" t="n">
         <v>2.25</v>
       </c>
       <c r="T30" s="6" t="n">
-        <v>2.26</v>
+        <v>2.25</v>
       </c>
       <c r="U30" s="21" t="n">
         <v>2.26</v>
@@ -3206,8 +3206,8 @@
           <t>CES0500000003</t>
         </is>
       </c>
-      <c r="N33" s="47" t="n">
-        <v>45901</v>
+      <c r="N33" s="48" t="n">
+        <v>45962</v>
       </c>
       <c r="O33" s="6" t="inlineStr">
         <is>
@@ -3220,19 +3220,19 @@
         </is>
       </c>
       <c r="Q33" s="38" t="n">
-        <v>0.002460360852925225</v>
+        <v>0.001358326541700539</v>
       </c>
       <c r="R33" s="38" t="n">
+        <v>0.004365620736698661</v>
+      </c>
+      <c r="S33" s="38" t="n">
+        <v>0.001913613996719521</v>
+      </c>
+      <c r="T33" s="38" t="n">
         <v>0.004117485588800429</v>
       </c>
-      <c r="S33" s="38" t="n">
+      <c r="U33" s="23" t="n">
         <v>0.003304874690167825</v>
-      </c>
-      <c r="T33" s="38" t="n">
-        <v>0.002208114821970808</v>
-      </c>
-      <c r="U33" s="23" t="n">
-        <v>0.004157427937915736</v>
       </c>
     </row>
     <row r="34" ht="31.5" customHeight="1">
@@ -3281,8 +3281,8 @@
           <t>CES0500000003</t>
         </is>
       </c>
-      <c r="N34" s="47" t="n">
-        <v>45901</v>
+      <c r="N34" s="48" t="n">
+        <v>45962</v>
       </c>
       <c r="O34" s="6" t="inlineStr">
         <is>
@@ -3295,19 +3295,19 @@
         </is>
       </c>
       <c r="Q34" s="38" t="n">
-        <v>0.03792810642513454</v>
+        <v>0.03510249929795001</v>
       </c>
       <c r="R34" s="38" t="n">
+        <v>0.03748590755355145</v>
+      </c>
+      <c r="S34" s="38" t="n">
+        <v>0.03736201528446081</v>
+      </c>
+      <c r="T34" s="38" t="n">
         <v>0.03831961396537047</v>
       </c>
-      <c r="S34" s="38" t="n">
+      <c r="U34" s="23" t="n">
         <v>0.03877958368976332</v>
-      </c>
-      <c r="T34" s="38" t="n">
-        <v>0.03742857142857149</v>
-      </c>
-      <c r="U34" s="23" t="n">
-        <v>0.03840642017770124</v>
       </c>
     </row>
     <row r="35" ht="31.5" customHeight="1">
@@ -3360,7 +3360,7 @@
           <t>RCES0500000003*</t>
         </is>
       </c>
-      <c r="N35" s="47" t="n">
+      <c r="N35" s="48" t="n">
         <v>45901</v>
       </c>
       <c r="O35" s="6" t="inlineStr">
@@ -3374,7 +3374,7 @@
         </is>
       </c>
       <c r="Q35" s="38" t="n">
-        <v>-0.0002259579984887905</v>
+        <v>-0.0007712397230601464</v>
       </c>
       <c r="R35" s="38" t="n">
         <v>0.001529940234958005</v>
@@ -3431,7 +3431,7 @@
           <t>RCES0500000003*</t>
         </is>
       </c>
-      <c r="N36" s="47" t="n">
+      <c r="N36" s="48" t="n">
         <v>45901</v>
       </c>
       <c r="O36" s="6" t="inlineStr">
@@ -3445,7 +3445,7 @@
         </is>
       </c>
       <c r="Q36" s="38" t="n">
-        <v>0.009781041380375289</v>
+        <v>0.009230301788676142</v>
       </c>
       <c r="R36" s="38" t="n">
         <v>0.01063283120727662</v>
@@ -3660,8 +3660,8 @@
           <t>DTWEXBGS</t>
         </is>
       </c>
-      <c r="N39" s="47" t="n">
-        <v>45996</v>
+      <c r="N39" s="48" t="n">
+        <v>46003</v>
       </c>
       <c r="O39" s="6" t="inlineStr">
         <is>
@@ -3674,19 +3674,19 @@
         </is>
       </c>
       <c r="Q39" s="6" t="n">
-        <v>121.0615</v>
+        <v>120.5383</v>
       </c>
       <c r="R39" s="6" t="n">
-        <v>121.0614</v>
+        <v>120.3821</v>
       </c>
       <c r="S39" s="6" t="n">
-        <v>121.1131</v>
+        <v>121.0557</v>
       </c>
       <c r="T39" s="6" t="n">
-        <v>121.5149</v>
+        <v>121.0601</v>
       </c>
       <c r="U39" s="21" t="n">
-        <v>121.3615</v>
+        <v>121.1478</v>
       </c>
     </row>
     <row r="40">
@@ -4251,7 +4251,7 @@
         </is>
       </c>
       <c r="N47" s="48" t="n">
-        <v>46002</v>
+        <v>46003</v>
       </c>
       <c r="O47" s="6" t="inlineStr">
         <is>
@@ -4267,7 +4267,7 @@
         <v>3.64</v>
       </c>
       <c r="R47" s="6" t="n">
-        <v>3.89</v>
+        <v>3.64</v>
       </c>
       <c r="S47" s="6" t="n">
         <v>3.89</v>
@@ -4330,7 +4330,7 @@
         </is>
       </c>
       <c r="N48" s="48" t="n">
-        <v>46002</v>
+        <v>46003</v>
       </c>
       <c r="O48" s="6" t="inlineStr">
         <is>
@@ -4346,16 +4346,16 @@
         <v>3.52</v>
       </c>
       <c r="R48" s="6" t="n">
+        <v>3.52</v>
+      </c>
+      <c r="S48" s="6" t="n">
         <v>3.54</v>
       </c>
-      <c r="S48" s="6" t="n">
+      <c r="T48" s="6" t="n">
         <v>3.61</v>
       </c>
-      <c r="T48" s="6" t="n">
+      <c r="U48" s="21" t="n">
         <v>3.57</v>
-      </c>
-      <c r="U48" s="21" t="n">
-        <v/>
       </c>
     </row>
     <row r="49">
@@ -4405,7 +4405,7 @@
         </is>
       </c>
       <c r="N49" s="48" t="n">
-        <v>46002</v>
+        <v>46003</v>
       </c>
       <c r="O49" s="6" t="inlineStr">
         <is>
@@ -4418,19 +4418,19 @@
         </is>
       </c>
       <c r="Q49" s="6" t="n">
-        <v>3.72</v>
+        <v>3.75</v>
       </c>
       <c r="R49" s="6" t="n">
         <v>3.72</v>
       </c>
       <c r="S49" s="6" t="n">
+        <v>3.72</v>
+      </c>
+      <c r="T49" s="6" t="n">
         <v>3.78</v>
       </c>
-      <c r="T49" s="6" t="n">
+      <c r="U49" s="21" t="n">
         <v>3.75</v>
-      </c>
-      <c r="U49" s="21" t="n">
-        <v/>
       </c>
     </row>
     <row r="50">
@@ -4484,7 +4484,7 @@
         </is>
       </c>
       <c r="N50" s="48" t="n">
-        <v>46002</v>
+        <v>46003</v>
       </c>
       <c r="O50" s="6" t="inlineStr">
         <is>
@@ -4497,19 +4497,19 @@
         </is>
       </c>
       <c r="Q50" s="6" t="n">
+        <v>4.19</v>
+      </c>
+      <c r="R50" s="6" t="n">
         <v>4.14</v>
       </c>
-      <c r="R50" s="6" t="n">
+      <c r="S50" s="6" t="n">
         <v>4.13</v>
       </c>
-      <c r="S50" s="6" t="n">
+      <c r="T50" s="6" t="n">
         <v>4.18</v>
       </c>
-      <c r="T50" s="6" t="n">
+      <c r="U50" s="21" t="n">
         <v>4.17</v>
-      </c>
-      <c r="U50" s="21" t="n">
-        <v/>
       </c>
     </row>
     <row r="51" ht="31.5" customHeight="1">
@@ -4610,7 +4610,7 @@
         </is>
       </c>
       <c r="N52" s="49" t="n">
-        <v>46002</v>
+        <v>46003</v>
       </c>
       <c r="O52" s="9" t="inlineStr">
         <is>
@@ -4623,19 +4623,19 @@
         </is>
       </c>
       <c r="Q52" s="9" t="n">
+        <v>5.95</v>
+      </c>
+      <c r="R52" s="9" t="n">
         <v>5.87</v>
       </c>
-      <c r="R52" s="9" t="n">
+      <c r="S52" s="9" t="n">
         <v>5.89</v>
       </c>
-      <c r="S52" s="9" t="n">
+      <c r="T52" s="9" t="n">
         <v>5.91</v>
       </c>
-      <c r="T52" s="9" t="n">
+      <c r="U52" s="22" t="n">
         <v>5.9</v>
-      </c>
-      <c r="U52" s="22" t="n">
-        <v/>
       </c>
     </row>
     <row r="53" ht="21" customHeight="1">

</xml_diff>

<commit_message>
Update dashboards - 2025-12-17
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -1208,7 +1208,7 @@
         </is>
       </c>
       <c r="F7" s="25" t="n">
-        <v>0.215816678152998</v>
+        <v>0.2303583735354926</v>
       </c>
       <c r="G7" s="25" t="n">
         <v>-2.062303243282817</v>
@@ -2903,7 +2903,7 @@
         </is>
       </c>
       <c r="N29" s="48" t="n">
-        <v>46006</v>
+        <v>46007</v>
       </c>
       <c r="O29" s="6" t="inlineStr">
         <is>
@@ -2919,13 +2919,13 @@
         <v>2.21</v>
       </c>
       <c r="R29" s="6" t="n">
-        <v>2.2</v>
+        <v>2.21</v>
       </c>
       <c r="S29" s="6" t="n">
-        <v>2.18</v>
+        <v/>
       </c>
       <c r="T29" s="6" t="n">
-        <v>2.18</v>
+        <v/>
       </c>
       <c r="U29" s="21" t="n">
         <v>2.2</v>
@@ -2982,7 +2982,7 @@
         </is>
       </c>
       <c r="N30" s="48" t="n">
-        <v>46006</v>
+        <v>46007</v>
       </c>
       <c r="O30" s="6" t="inlineStr">
         <is>
@@ -2995,16 +2995,16 @@
         </is>
       </c>
       <c r="Q30" s="6" t="n">
+        <v>2.23</v>
+      </c>
+      <c r="R30" s="6" t="n">
         <v>2.25</v>
       </c>
-      <c r="R30" s="6" t="n">
-        <v>2.26</v>
-      </c>
       <c r="S30" s="6" t="n">
-        <v>2.25</v>
+        <v/>
       </c>
       <c r="T30" s="6" t="n">
-        <v>2.25</v>
+        <v/>
       </c>
       <c r="U30" s="21" t="n">
         <v>2.26</v>
@@ -3056,7 +3056,7 @@
           <t>ECIWAG</t>
         </is>
       </c>
-      <c r="N31" s="48" t="n">
+      <c r="N31" s="47" t="n">
         <v>45839</v>
       </c>
       <c r="O31" s="6" t="inlineStr">
@@ -3131,7 +3131,7 @@
           <t>ECIWAG</t>
         </is>
       </c>
-      <c r="N32" s="48" t="n">
+      <c r="N32" s="47" t="n">
         <v>45839</v>
       </c>
       <c r="O32" s="6" t="inlineStr">
@@ -4251,7 +4251,7 @@
         </is>
       </c>
       <c r="N47" s="48" t="n">
-        <v>46003</v>
+        <v>46006</v>
       </c>
       <c r="O47" s="6" t="inlineStr">
         <is>
@@ -4270,13 +4270,13 @@
         <v>3.64</v>
       </c>
       <c r="S47" s="6" t="n">
-        <v>3.89</v>
+        <v>3.64</v>
       </c>
       <c r="T47" s="6" t="n">
-        <v>3.89</v>
+        <v>3.64</v>
       </c>
       <c r="U47" s="21" t="n">
-        <v>3.89</v>
+        <v>3.64</v>
       </c>
     </row>
     <row r="48">
@@ -4330,7 +4330,7 @@
         </is>
       </c>
       <c r="N48" s="48" t="n">
-        <v>46003</v>
+        <v>46006</v>
       </c>
       <c r="O48" s="6" t="inlineStr">
         <is>
@@ -4343,19 +4343,19 @@
         </is>
       </c>
       <c r="Q48" s="6" t="n">
+        <v>3.51</v>
+      </c>
+      <c r="R48" s="6" t="n">
+        <v/>
+      </c>
+      <c r="S48" s="6" t="n">
+        <v/>
+      </c>
+      <c r="T48" s="6" t="n">
         <v>3.52</v>
       </c>
-      <c r="R48" s="6" t="n">
+      <c r="U48" s="21" t="n">
         <v>3.52</v>
-      </c>
-      <c r="S48" s="6" t="n">
-        <v>3.54</v>
-      </c>
-      <c r="T48" s="6" t="n">
-        <v>3.61</v>
-      </c>
-      <c r="U48" s="21" t="n">
-        <v>3.57</v>
       </c>
     </row>
     <row r="49">
@@ -4405,7 +4405,7 @@
         </is>
       </c>
       <c r="N49" s="48" t="n">
-        <v>46003</v>
+        <v>46006</v>
       </c>
       <c r="O49" s="6" t="inlineStr">
         <is>
@@ -4418,19 +4418,19 @@
         </is>
       </c>
       <c r="Q49" s="6" t="n">
+        <v>3.73</v>
+      </c>
+      <c r="R49" s="6" t="n">
+        <v/>
+      </c>
+      <c r="S49" s="6" t="n">
+        <v/>
+      </c>
+      <c r="T49" s="6" t="n">
         <v>3.75</v>
       </c>
-      <c r="R49" s="6" t="n">
+      <c r="U49" s="21" t="n">
         <v>3.72</v>
-      </c>
-      <c r="S49" s="6" t="n">
-        <v>3.72</v>
-      </c>
-      <c r="T49" s="6" t="n">
-        <v>3.78</v>
-      </c>
-      <c r="U49" s="21" t="n">
-        <v>3.75</v>
       </c>
     </row>
     <row r="50">
@@ -4484,7 +4484,7 @@
         </is>
       </c>
       <c r="N50" s="48" t="n">
-        <v>46003</v>
+        <v>46006</v>
       </c>
       <c r="O50" s="6" t="inlineStr">
         <is>
@@ -4497,19 +4497,19 @@
         </is>
       </c>
       <c r="Q50" s="6" t="n">
+        <v>4.18</v>
+      </c>
+      <c r="R50" s="6" t="n">
+        <v/>
+      </c>
+      <c r="S50" s="6" t="n">
+        <v/>
+      </c>
+      <c r="T50" s="6" t="n">
         <v>4.19</v>
       </c>
-      <c r="R50" s="6" t="n">
+      <c r="U50" s="21" t="n">
         <v>4.14</v>
-      </c>
-      <c r="S50" s="6" t="n">
-        <v>4.13</v>
-      </c>
-      <c r="T50" s="6" t="n">
-        <v>4.18</v>
-      </c>
-      <c r="U50" s="21" t="n">
-        <v>4.17</v>
       </c>
     </row>
     <row r="51" ht="31.5" customHeight="1">
@@ -4610,7 +4610,7 @@
         </is>
       </c>
       <c r="N52" s="49" t="n">
-        <v>46003</v>
+        <v>46006</v>
       </c>
       <c r="O52" s="9" t="inlineStr">
         <is>
@@ -4626,16 +4626,16 @@
         <v>5.95</v>
       </c>
       <c r="R52" s="9" t="n">
+        <v/>
+      </c>
+      <c r="S52" s="9" t="n">
+        <v/>
+      </c>
+      <c r="T52" s="9" t="n">
+        <v>5.95</v>
+      </c>
+      <c r="U52" s="22" t="n">
         <v>5.87</v>
-      </c>
-      <c r="S52" s="9" t="n">
-        <v>5.89</v>
-      </c>
-      <c r="T52" s="9" t="n">
-        <v>5.91</v>
-      </c>
-      <c r="U52" s="22" t="n">
-        <v>5.9</v>
       </c>
     </row>
     <row r="53" ht="21" customHeight="1">

</xml_diff>

<commit_message>
Update dashboards - 2025-12-18
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -1208,7 +1208,7 @@
         </is>
       </c>
       <c r="F7" s="25" t="n">
-        <v>0.2303583735354926</v>
+        <v>0.1966919365954514</v>
       </c>
       <c r="G7" s="25" t="n">
         <v>-2.062303243282817</v>
@@ -1700,7 +1700,7 @@
         </is>
       </c>
       <c r="N13" s="48" t="n">
-        <v>45992</v>
+        <v>45999</v>
       </c>
       <c r="O13" s="6" t="inlineStr">
         <is>
@@ -1713,19 +1713,19 @@
         </is>
       </c>
       <c r="Q13" s="24" t="n">
-        <v>236000</v>
+        <v>224000</v>
       </c>
       <c r="R13" s="24" t="n">
+        <v>237000</v>
+      </c>
+      <c r="S13" s="24" t="n">
         <v>192000</v>
       </c>
-      <c r="S13" s="24" t="n">
+      <c r="T13" s="24" t="n">
         <v>217000</v>
       </c>
-      <c r="T13" s="24" t="n">
+      <c r="U13" s="26" t="n">
         <v>222000</v>
-      </c>
-      <c r="U13" s="26" t="n">
-        <v>228000</v>
       </c>
     </row>
     <row r="14">
@@ -1775,7 +1775,7 @@
         </is>
       </c>
       <c r="N14" s="48" t="n">
-        <v>45985</v>
+        <v>45992</v>
       </c>
       <c r="O14" s="6" t="inlineStr">
         <is>
@@ -1788,19 +1788,19 @@
         </is>
       </c>
       <c r="Q14" s="24" t="n">
-        <v>1838000</v>
+        <v>1897000</v>
       </c>
       <c r="R14" s="24" t="n">
+        <v>1830000</v>
+      </c>
+      <c r="S14" s="24" t="n">
         <v>1937000</v>
       </c>
-      <c r="S14" s="24" t="n">
+      <c r="T14" s="24" t="n">
         <v>1944000</v>
       </c>
-      <c r="T14" s="24" t="n">
+      <c r="U14" s="26" t="n">
         <v>1953000</v>
-      </c>
-      <c r="U14" s="26" t="n">
-        <v>1946000</v>
       </c>
     </row>
     <row r="15">
@@ -2066,8 +2066,8 @@
           <t>CPIAUCSL</t>
         </is>
       </c>
-      <c r="N18" s="47" t="n">
-        <v>45901</v>
+      <c r="N18" s="48" t="n">
+        <v>45962</v>
       </c>
       <c r="O18" s="6" t="inlineStr">
         <is>
@@ -2080,19 +2080,19 @@
         </is>
       </c>
       <c r="Q18" s="38" t="n">
+        <v/>
+      </c>
+      <c r="R18" s="38" t="n">
+        <v/>
+      </c>
+      <c r="S18" s="38" t="n">
         <v>0.00310486015759337</v>
       </c>
-      <c r="R18" s="38" t="n">
+      <c r="T18" s="38" t="n">
         <v>0.003824519141221616</v>
       </c>
-      <c r="S18" s="38" t="n">
+      <c r="U18" s="23" t="n">
         <v>0.00196578538102643</v>
-      </c>
-      <c r="T18" s="38" t="n">
-        <v>0.002869798490236386</v>
-      </c>
-      <c r="U18" s="23" t="n">
-        <v>0.0008085639093282637</v>
       </c>
     </row>
     <row r="19" ht="31.5" customHeight="1">
@@ -2141,8 +2141,8 @@
           <t>CPIAUCSL</t>
         </is>
       </c>
-      <c r="N19" s="47" t="n">
-        <v>45901</v>
+      <c r="N19" s="48" t="n">
+        <v>45962</v>
       </c>
       <c r="O19" s="6" t="inlineStr">
         <is>
@@ -2155,19 +2155,19 @@
         </is>
       </c>
       <c r="Q19" s="38" t="n">
+        <v>0.0271196938527219</v>
+      </c>
+      <c r="R19" s="38" t="n">
+        <v/>
+      </c>
+      <c r="S19" s="38" t="n">
         <v>0.03022699626172379</v>
       </c>
-      <c r="R19" s="38" t="n">
+      <c r="T19" s="38" t="n">
         <v>0.02939219624933549</v>
       </c>
-      <c r="S19" s="38" t="n">
+      <c r="U19" s="23" t="n">
         <v>0.02731801279475463</v>
-      </c>
-      <c r="T19" s="38" t="n">
-        <v>0.02672683317844617</v>
-      </c>
-      <c r="U19" s="23" t="n">
-        <v>0.02375934086989844</v>
       </c>
     </row>
     <row r="20">
@@ -2216,8 +2216,8 @@
           <t>CPILFESL</t>
         </is>
       </c>
-      <c r="N20" s="47" t="n">
-        <v>45901</v>
+      <c r="N20" s="48" t="n">
+        <v>45962</v>
       </c>
       <c r="O20" s="6" t="inlineStr">
         <is>
@@ -2230,19 +2230,19 @@
         </is>
       </c>
       <c r="Q20" s="38" t="n">
+        <v/>
+      </c>
+      <c r="R20" s="38" t="n">
+        <v/>
+      </c>
+      <c r="S20" s="38" t="n">
         <v>0.002271121582325675</v>
       </c>
-      <c r="R20" s="38" t="n">
+      <c r="T20" s="38" t="n">
         <v>0.003459544325982167</v>
       </c>
-      <c r="S20" s="38" t="n">
+      <c r="U20" s="23" t="n">
         <v>0.003223443223443256</v>
-      </c>
-      <c r="T20" s="38" t="n">
-        <v>0.002282364603156228</v>
-      </c>
-      <c r="U20" s="23" t="n">
-        <v>0.001298900223631438</v>
       </c>
     </row>
     <row r="21">
@@ -2291,8 +2291,8 @@
           <t>CPILFESL</t>
         </is>
       </c>
-      <c r="N21" s="47" t="n">
-        <v>45901</v>
+      <c r="N21" s="48" t="n">
+        <v>45962</v>
       </c>
       <c r="O21" s="6" t="inlineStr">
         <is>
@@ -2305,19 +2305,19 @@
         </is>
       </c>
       <c r="Q21" s="38" t="n">
+        <v>0.02618878615332623</v>
+      </c>
+      <c r="R21" s="38" t="n">
+        <v/>
+      </c>
+      <c r="S21" s="38" t="n">
         <v>0.03025542724453378</v>
       </c>
-      <c r="R21" s="38" t="n">
+      <c r="T21" s="38" t="n">
         <v>0.03112190821006822</v>
       </c>
-      <c r="S21" s="38" t="n">
+      <c r="U21" s="23" t="n">
         <v>0.03048602684576389</v>
-      </c>
-      <c r="T21" s="38" t="n">
-        <v>0.02907869813377396</v>
-      </c>
-      <c r="U21" s="23" t="n">
-        <v>0.02767148871414509</v>
       </c>
     </row>
     <row r="22">
@@ -2903,7 +2903,7 @@
         </is>
       </c>
       <c r="N29" s="48" t="n">
-        <v>46007</v>
+        <v>46008</v>
       </c>
       <c r="O29" s="6" t="inlineStr">
         <is>
@@ -2916,19 +2916,19 @@
         </is>
       </c>
       <c r="Q29" s="6" t="n">
-        <v>2.21</v>
+        <v>2.22</v>
       </c>
       <c r="R29" s="6" t="n">
         <v>2.21</v>
       </c>
       <c r="S29" s="6" t="n">
-        <v/>
+        <v>2.21</v>
       </c>
       <c r="T29" s="6" t="n">
         <v/>
       </c>
       <c r="U29" s="21" t="n">
-        <v>2.2</v>
+        <v/>
       </c>
     </row>
     <row r="30">
@@ -2982,7 +2982,7 @@
         </is>
       </c>
       <c r="N30" s="48" t="n">
-        <v>46007</v>
+        <v>46008</v>
       </c>
       <c r="O30" s="6" t="inlineStr">
         <is>
@@ -2995,19 +2995,19 @@
         </is>
       </c>
       <c r="Q30" s="6" t="n">
+        <v>2.24</v>
+      </c>
+      <c r="R30" s="6" t="n">
         <v>2.23</v>
       </c>
-      <c r="R30" s="6" t="n">
+      <c r="S30" s="6" t="n">
         <v>2.25</v>
-      </c>
-      <c r="S30" s="6" t="n">
-        <v/>
       </c>
       <c r="T30" s="6" t="n">
         <v/>
       </c>
       <c r="U30" s="21" t="n">
-        <v>2.26</v>
+        <v/>
       </c>
     </row>
     <row r="31">
@@ -4124,7 +4124,7 @@
           <t>BOPTEXP</t>
         </is>
       </c>
-      <c r="C46" s="48" t="n">
+      <c r="C46" s="47" t="n">
         <v>45901</v>
       </c>
       <c r="D46" s="6" t="inlineStr">
@@ -4211,7 +4211,7 @@
           <t>BOPTEXP</t>
         </is>
       </c>
-      <c r="C47" s="48" t="n">
+      <c r="C47" s="47" t="n">
         <v>45901</v>
       </c>
       <c r="D47" s="6" t="inlineStr">
@@ -4251,7 +4251,7 @@
         </is>
       </c>
       <c r="N47" s="48" t="n">
-        <v>46006</v>
+        <v>46007</v>
       </c>
       <c r="O47" s="6" t="inlineStr">
         <is>
@@ -4290,7 +4290,7 @@
           <t>BOPTIMP</t>
         </is>
       </c>
-      <c r="C48" s="48" t="n">
+      <c r="C48" s="47" t="n">
         <v>45901</v>
       </c>
       <c r="D48" s="6" t="inlineStr">
@@ -4330,7 +4330,7 @@
         </is>
       </c>
       <c r="N48" s="48" t="n">
-        <v>46006</v>
+        <v>46007</v>
       </c>
       <c r="O48" s="6" t="inlineStr">
         <is>
@@ -4343,16 +4343,16 @@
         </is>
       </c>
       <c r="Q48" s="6" t="n">
+        <v>3.48</v>
+      </c>
+      <c r="R48" s="6" t="n">
         <v>3.51</v>
-      </c>
-      <c r="R48" s="6" t="n">
-        <v/>
       </c>
       <c r="S48" s="6" t="n">
         <v/>
       </c>
       <c r="T48" s="6" t="n">
-        <v>3.52</v>
+        <v/>
       </c>
       <c r="U48" s="21" t="n">
         <v>3.52</v>
@@ -4365,7 +4365,7 @@
           <t>BOPTIMP</t>
         </is>
       </c>
-      <c r="C49" s="48" t="n">
+      <c r="C49" s="47" t="n">
         <v>45901</v>
       </c>
       <c r="D49" s="6" t="inlineStr">
@@ -4405,7 +4405,7 @@
         </is>
       </c>
       <c r="N49" s="48" t="n">
-        <v>46006</v>
+        <v>46007</v>
       </c>
       <c r="O49" s="6" t="inlineStr">
         <is>
@@ -4418,19 +4418,19 @@
         </is>
       </c>
       <c r="Q49" s="6" t="n">
+        <v>3.69</v>
+      </c>
+      <c r="R49" s="6" t="n">
         <v>3.73</v>
-      </c>
-      <c r="R49" s="6" t="n">
-        <v/>
       </c>
       <c r="S49" s="6" t="n">
         <v/>
       </c>
       <c r="T49" s="6" t="n">
+        <v/>
+      </c>
+      <c r="U49" s="21" t="n">
         <v>3.75</v>
-      </c>
-      <c r="U49" s="21" t="n">
-        <v>3.72</v>
       </c>
     </row>
     <row r="50">
@@ -4444,7 +4444,7 @@
           <t>BOPSTB</t>
         </is>
       </c>
-      <c r="C50" s="48" t="n">
+      <c r="C50" s="47" t="n">
         <v>45901</v>
       </c>
       <c r="D50" s="6" t="inlineStr">
@@ -4484,7 +4484,7 @@
         </is>
       </c>
       <c r="N50" s="48" t="n">
-        <v>46006</v>
+        <v>46007</v>
       </c>
       <c r="O50" s="6" t="inlineStr">
         <is>
@@ -4497,19 +4497,19 @@
         </is>
       </c>
       <c r="Q50" s="6" t="n">
+        <v>4.15</v>
+      </c>
+      <c r="R50" s="6" t="n">
         <v>4.18</v>
-      </c>
-      <c r="R50" s="6" t="n">
-        <v/>
       </c>
       <c r="S50" s="6" t="n">
         <v/>
       </c>
       <c r="T50" s="6" t="n">
+        <v/>
+      </c>
+      <c r="U50" s="21" t="n">
         <v>4.19</v>
-      </c>
-      <c r="U50" s="21" t="n">
-        <v>4.14</v>
       </c>
     </row>
     <row r="51" ht="31.5" customHeight="1">
@@ -4519,7 +4519,7 @@
           <t>BOPSTB</t>
         </is>
       </c>
-      <c r="C51" s="48" t="n">
+      <c r="C51" s="47" t="n">
         <v>45901</v>
       </c>
       <c r="D51" s="6" t="inlineStr">
@@ -4558,7 +4558,7 @@
           <t>MORTGAGE30US</t>
         </is>
       </c>
-      <c r="N51" s="48" t="n">
+      <c r="N51" s="47" t="n">
         <v>45999</v>
       </c>
       <c r="O51" s="6" t="inlineStr">
@@ -4610,7 +4610,7 @@
         </is>
       </c>
       <c r="N52" s="49" t="n">
-        <v>46006</v>
+        <v>46007</v>
       </c>
       <c r="O52" s="9" t="inlineStr">
         <is>
@@ -4623,19 +4623,19 @@
         </is>
       </c>
       <c r="Q52" s="9" t="n">
+        <v>5.93</v>
+      </c>
+      <c r="R52" s="9" t="n">
         <v>5.95</v>
-      </c>
-      <c r="R52" s="9" t="n">
-        <v/>
       </c>
       <c r="S52" s="9" t="n">
         <v/>
       </c>
       <c r="T52" s="9" t="n">
+        <v/>
+      </c>
+      <c r="U52" s="22" t="n">
         <v>5.95</v>
-      </c>
-      <c r="U52" s="22" t="n">
-        <v>5.87</v>
       </c>
     </row>
     <row r="53" ht="21" customHeight="1">

</xml_diff>

<commit_message>
Update dashboards - 2025-12-19
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -2903,7 +2903,7 @@
         </is>
       </c>
       <c r="N29" s="48" t="n">
-        <v>46008</v>
+        <v>46009</v>
       </c>
       <c r="O29" s="6" t="inlineStr">
         <is>
@@ -2919,13 +2919,13 @@
         <v>2.22</v>
       </c>
       <c r="R29" s="6" t="n">
-        <v>2.21</v>
+        <v>2.22</v>
       </c>
       <c r="S29" s="6" t="n">
         <v>2.21</v>
       </c>
       <c r="T29" s="6" t="n">
-        <v/>
+        <v>2.21</v>
       </c>
       <c r="U29" s="21" t="n">
         <v/>
@@ -2982,7 +2982,7 @@
         </is>
       </c>
       <c r="N30" s="48" t="n">
-        <v>46008</v>
+        <v>46009</v>
       </c>
       <c r="O30" s="6" t="inlineStr">
         <is>
@@ -2998,13 +2998,13 @@
         <v>2.24</v>
       </c>
       <c r="R30" s="6" t="n">
+        <v>2.24</v>
+      </c>
+      <c r="S30" s="6" t="n">
         <v>2.23</v>
       </c>
-      <c r="S30" s="6" t="n">
+      <c r="T30" s="6" t="n">
         <v>2.25</v>
-      </c>
-      <c r="T30" s="6" t="n">
-        <v/>
       </c>
       <c r="U30" s="21" t="n">
         <v/>
@@ -3660,7 +3660,7 @@
           <t>DTWEXBGS</t>
         </is>
       </c>
-      <c r="N39" s="48" t="n">
+      <c r="N39" s="47" t="n">
         <v>46003</v>
       </c>
       <c r="O39" s="6" t="inlineStr">
@@ -4251,7 +4251,7 @@
         </is>
       </c>
       <c r="N47" s="48" t="n">
-        <v>46007</v>
+        <v>46008</v>
       </c>
       <c r="O47" s="6" t="inlineStr">
         <is>
@@ -4330,7 +4330,7 @@
         </is>
       </c>
       <c r="N48" s="48" t="n">
-        <v>46007</v>
+        <v>46008</v>
       </c>
       <c r="O48" s="6" t="inlineStr">
         <is>
@@ -4343,19 +4343,19 @@
         </is>
       </c>
       <c r="Q48" s="6" t="n">
+        <v>3.49</v>
+      </c>
+      <c r="R48" s="6" t="n">
         <v>3.48</v>
       </c>
-      <c r="R48" s="6" t="n">
+      <c r="S48" s="6" t="n">
         <v>3.51</v>
-      </c>
-      <c r="S48" s="6" t="n">
-        <v/>
       </c>
       <c r="T48" s="6" t="n">
         <v/>
       </c>
       <c r="U48" s="21" t="n">
-        <v>3.52</v>
+        <v/>
       </c>
     </row>
     <row r="49">
@@ -4405,7 +4405,7 @@
         </is>
       </c>
       <c r="N49" s="48" t="n">
-        <v>46007</v>
+        <v>46008</v>
       </c>
       <c r="O49" s="6" t="inlineStr">
         <is>
@@ -4418,19 +4418,19 @@
         </is>
       </c>
       <c r="Q49" s="6" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="R49" s="6" t="n">
         <v>3.69</v>
       </c>
-      <c r="R49" s="6" t="n">
+      <c r="S49" s="6" t="n">
         <v>3.73</v>
-      </c>
-      <c r="S49" s="6" t="n">
-        <v/>
       </c>
       <c r="T49" s="6" t="n">
         <v/>
       </c>
       <c r="U49" s="21" t="n">
-        <v>3.75</v>
+        <v/>
       </c>
     </row>
     <row r="50">
@@ -4484,7 +4484,7 @@
         </is>
       </c>
       <c r="N50" s="48" t="n">
-        <v>46007</v>
+        <v>46008</v>
       </c>
       <c r="O50" s="6" t="inlineStr">
         <is>
@@ -4497,19 +4497,19 @@
         </is>
       </c>
       <c r="Q50" s="6" t="n">
+        <v>4.16</v>
+      </c>
+      <c r="R50" s="6" t="n">
         <v>4.15</v>
       </c>
-      <c r="R50" s="6" t="n">
+      <c r="S50" s="6" t="n">
         <v>4.18</v>
-      </c>
-      <c r="S50" s="6" t="n">
-        <v/>
       </c>
       <c r="T50" s="6" t="n">
         <v/>
       </c>
       <c r="U50" s="21" t="n">
-        <v>4.19</v>
+        <v/>
       </c>
     </row>
     <row r="51" ht="31.5" customHeight="1">
@@ -4558,8 +4558,8 @@
           <t>MORTGAGE30US</t>
         </is>
       </c>
-      <c r="N51" s="47" t="n">
-        <v>45999</v>
+      <c r="N51" s="48" t="n">
+        <v>46006</v>
       </c>
       <c r="O51" s="6" t="inlineStr">
         <is>
@@ -4572,19 +4572,19 @@
         </is>
       </c>
       <c r="Q51" s="6" t="n">
+        <v>6.21</v>
+      </c>
+      <c r="R51" s="6" t="n">
         <v>6.22</v>
       </c>
-      <c r="R51" s="6" t="n">
+      <c r="S51" s="6" t="n">
         <v>6.19</v>
       </c>
-      <c r="S51" s="6" t="n">
+      <c r="T51" s="6" t="n">
         <v>6.23</v>
       </c>
-      <c r="T51" s="6" t="n">
+      <c r="U51" s="21" t="n">
         <v>6.26</v>
-      </c>
-      <c r="U51" s="21" t="n">
-        <v>6.24</v>
       </c>
     </row>
     <row r="52" ht="16.15" customHeight="1" thickBot="1">
@@ -4610,7 +4610,7 @@
         </is>
       </c>
       <c r="N52" s="49" t="n">
-        <v>46007</v>
+        <v>46008</v>
       </c>
       <c r="O52" s="9" t="inlineStr">
         <is>
@@ -4623,19 +4623,19 @@
         </is>
       </c>
       <c r="Q52" s="9" t="n">
+        <v>5.94</v>
+      </c>
+      <c r="R52" s="9" t="n">
         <v>5.93</v>
       </c>
-      <c r="R52" s="9" t="n">
+      <c r="S52" s="9" t="n">
         <v>5.95</v>
-      </c>
-      <c r="S52" s="9" t="n">
-        <v/>
       </c>
       <c r="T52" s="9" t="n">
         <v/>
       </c>
       <c r="U52" s="22" t="n">
-        <v>5.95</v>
+        <v/>
       </c>
     </row>
     <row r="53" ht="21" customHeight="1">

</xml_diff>

<commit_message>
Update dashboards - 2025-12-20
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -2828,7 +2828,7 @@
         </is>
       </c>
       <c r="N28" s="47" t="n">
-        <v>45931</v>
+        <v>45962</v>
       </c>
       <c r="O28" s="6" t="inlineStr">
         <is>
@@ -2841,19 +2841,19 @@
         </is>
       </c>
       <c r="Q28" s="6" t="n">
+        <v>51</v>
+      </c>
+      <c r="R28" s="6" t="n">
         <v>53.6</v>
       </c>
-      <c r="R28" s="6" t="n">
+      <c r="S28" s="6" t="n">
         <v>55.1</v>
       </c>
-      <c r="S28" s="6" t="n">
+      <c r="T28" s="6" t="n">
         <v>58.2</v>
       </c>
-      <c r="T28" s="6" t="n">
+      <c r="U28" s="21" t="n">
         <v>61.7</v>
-      </c>
-      <c r="U28" s="21" t="n">
-        <v>60.7</v>
       </c>
     </row>
     <row r="29">
@@ -2903,7 +2903,7 @@
         </is>
       </c>
       <c r="N29" s="48" t="n">
-        <v>46009</v>
+        <v>46010</v>
       </c>
       <c r="O29" s="6" t="inlineStr">
         <is>
@@ -2916,19 +2916,19 @@
         </is>
       </c>
       <c r="Q29" s="6" t="n">
-        <v>2.22</v>
+        <v>2.21</v>
       </c>
       <c r="R29" s="6" t="n">
         <v>2.22</v>
       </c>
       <c r="S29" s="6" t="n">
-        <v>2.21</v>
+        <v>2.22</v>
       </c>
       <c r="T29" s="6" t="n">
         <v>2.21</v>
       </c>
       <c r="U29" s="21" t="n">
-        <v/>
+        <v>2.21</v>
       </c>
     </row>
     <row r="30">
@@ -2982,7 +2982,7 @@
         </is>
       </c>
       <c r="N30" s="48" t="n">
-        <v>46009</v>
+        <v>46010</v>
       </c>
       <c r="O30" s="6" t="inlineStr">
         <is>
@@ -3001,13 +3001,13 @@
         <v>2.24</v>
       </c>
       <c r="S30" s="6" t="n">
+        <v>2.24</v>
+      </c>
+      <c r="T30" s="6" t="n">
         <v>2.23</v>
       </c>
-      <c r="T30" s="6" t="n">
+      <c r="U30" s="21" t="n">
         <v>2.25</v>
-      </c>
-      <c r="U30" s="21" t="n">
-        <v/>
       </c>
     </row>
     <row r="31">
@@ -3853,7 +3853,7 @@
         </is>
       </c>
       <c r="C42" s="47" t="n">
-        <v>45931</v>
+        <v>45962</v>
       </c>
       <c r="D42" s="6" t="inlineStr">
         <is>
@@ -3866,19 +3866,19 @@
         </is>
       </c>
       <c r="F42" s="39" t="n">
-        <v>4100000</v>
+        <v>4130000</v>
       </c>
       <c r="G42" s="39" t="n">
+        <v>4110000</v>
+      </c>
+      <c r="H42" s="39" t="n">
         <v>4050000</v>
       </c>
-      <c r="H42" s="39" t="n">
+      <c r="I42" s="39" t="n">
         <v>4000000</v>
       </c>
-      <c r="I42" s="39" t="n">
+      <c r="J42" s="39" t="n">
         <v>4010000</v>
-      </c>
-      <c r="J42" s="39" t="n">
-        <v>3930000</v>
       </c>
       <c r="K42" s="7" t="n"/>
       <c r="L42" s="28" t="n"/>
@@ -3924,7 +3924,7 @@
         </is>
       </c>
       <c r="C43" s="47" t="n">
-        <v>45931</v>
+        <v>45962</v>
       </c>
       <c r="D43" s="6" t="inlineStr">
         <is>
@@ -3937,7 +3937,7 @@
         </is>
       </c>
       <c r="F43" s="38" t="n">
-        <v>0.0173697270471464</v>
+        <v>-0.009592326139088728</v>
       </c>
       <c r="G43" s="38" t="n">
         <v/>
@@ -4251,7 +4251,7 @@
         </is>
       </c>
       <c r="N47" s="48" t="n">
-        <v>46008</v>
+        <v>46009</v>
       </c>
       <c r="O47" s="6" t="inlineStr">
         <is>
@@ -4330,7 +4330,7 @@
         </is>
       </c>
       <c r="N48" s="48" t="n">
-        <v>46008</v>
+        <v>46009</v>
       </c>
       <c r="O48" s="6" t="inlineStr">
         <is>
@@ -4343,16 +4343,16 @@
         </is>
       </c>
       <c r="Q48" s="6" t="n">
+        <v>3.46</v>
+      </c>
+      <c r="R48" s="6" t="n">
         <v>3.49</v>
       </c>
-      <c r="R48" s="6" t="n">
+      <c r="S48" s="6" t="n">
         <v>3.48</v>
       </c>
-      <c r="S48" s="6" t="n">
+      <c r="T48" s="6" t="n">
         <v>3.51</v>
-      </c>
-      <c r="T48" s="6" t="n">
-        <v/>
       </c>
       <c r="U48" s="21" t="n">
         <v/>
@@ -4405,7 +4405,7 @@
         </is>
       </c>
       <c r="N49" s="48" t="n">
-        <v>46008</v>
+        <v>46009</v>
       </c>
       <c r="O49" s="6" t="inlineStr">
         <is>
@@ -4418,16 +4418,16 @@
         </is>
       </c>
       <c r="Q49" s="6" t="n">
+        <v>3.66</v>
+      </c>
+      <c r="R49" s="6" t="n">
         <v>3.7</v>
       </c>
-      <c r="R49" s="6" t="n">
+      <c r="S49" s="6" t="n">
         <v>3.69</v>
       </c>
-      <c r="S49" s="6" t="n">
+      <c r="T49" s="6" t="n">
         <v>3.73</v>
-      </c>
-      <c r="T49" s="6" t="n">
-        <v/>
       </c>
       <c r="U49" s="21" t="n">
         <v/>
@@ -4484,7 +4484,7 @@
         </is>
       </c>
       <c r="N50" s="48" t="n">
-        <v>46008</v>
+        <v>46009</v>
       </c>
       <c r="O50" s="6" t="inlineStr">
         <is>
@@ -4497,16 +4497,16 @@
         </is>
       </c>
       <c r="Q50" s="6" t="n">
+        <v>4.12</v>
+      </c>
+      <c r="R50" s="6" t="n">
         <v>4.16</v>
       </c>
-      <c r="R50" s="6" t="n">
+      <c r="S50" s="6" t="n">
         <v>4.15</v>
       </c>
-      <c r="S50" s="6" t="n">
+      <c r="T50" s="6" t="n">
         <v>4.18</v>
-      </c>
-      <c r="T50" s="6" t="n">
-        <v/>
       </c>
       <c r="U50" s="21" t="n">
         <v/>
@@ -4610,7 +4610,7 @@
         </is>
       </c>
       <c r="N52" s="49" t="n">
-        <v>46008</v>
+        <v>46009</v>
       </c>
       <c r="O52" s="9" t="inlineStr">
         <is>
@@ -4623,16 +4623,16 @@
         </is>
       </c>
       <c r="Q52" s="9" t="n">
+        <v>5.9</v>
+      </c>
+      <c r="R52" s="9" t="n">
         <v>5.94</v>
       </c>
-      <c r="R52" s="9" t="n">
+      <c r="S52" s="9" t="n">
         <v>5.93</v>
       </c>
-      <c r="S52" s="9" t="n">
+      <c r="T52" s="9" t="n">
         <v>5.95</v>
-      </c>
-      <c r="T52" s="9" t="n">
-        <v/>
       </c>
       <c r="U52" s="22" t="n">
         <v/>

</xml_diff>

<commit_message>
Update dashboards - 2025-12-22
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -1040,7 +1040,7 @@
           <t>NGDPSAXDCUSQ</t>
         </is>
       </c>
-      <c r="C5" s="47" t="n">
+      <c r="C5" s="48" t="n">
         <v>45748</v>
       </c>
       <c r="D5" s="6" t="inlineStr">
@@ -1054,19 +1054,19 @@
         </is>
       </c>
       <c r="F5" s="24" t="n">
-        <v>7582779.3</v>
+        <v>7621432.3</v>
       </c>
       <c r="G5" s="24" t="n">
-        <v>7490511.8</v>
+        <v>7510528.3</v>
       </c>
       <c r="H5" s="24" t="n">
-        <v>7430966</v>
+        <v>7456295.5</v>
       </c>
       <c r="I5" s="24" t="n">
-        <v>7343728.5</v>
+        <v>7377916</v>
       </c>
       <c r="J5" s="24" t="n">
-        <v>7254178.5</v>
+        <v>7286761</v>
       </c>
       <c r="K5" s="5" t="n"/>
       <c r="L5" s="28" t="inlineStr">
@@ -1115,7 +1115,7 @@
           <t>NGDPSAXDCUSQ</t>
         </is>
       </c>
-      <c r="C6" s="47" t="n">
+      <c r="C6" s="48" t="n">
         <v>45748</v>
       </c>
       <c r="D6" s="6" t="inlineStr">
@@ -1129,19 +1129,19 @@
         </is>
       </c>
       <c r="F6" s="25" t="n">
-        <v>0.01231791664756465</v>
+        <v>0.0147664712214719</v>
       </c>
       <c r="G6" s="25" t="n">
-        <v>0.008013197745757372</v>
+        <v>0.007273424182290045</v>
       </c>
       <c r="H6" s="25" t="n">
-        <v>0.01187918371437613</v>
+        <v>0.01062352837847436</v>
       </c>
       <c r="I6" s="25" t="n">
-        <v>0.01234460938616277</v>
+        <v>0.01250967336516173</v>
       </c>
       <c r="J6" s="25" t="n">
-        <v>0.01371729495399632</v>
+        <v>0.01528773636675829</v>
       </c>
       <c r="K6" s="5" t="n"/>
       <c r="L6" s="28" t="inlineStr">

</xml_diff>

<commit_message>
Update dashboards - 2025-12-23
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -350,10 +350,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="167" fontId="1" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="167" fontId="1" fillId="3" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -891,7 +891,7 @@
         </is>
       </c>
       <c r="C3" s="47" t="n">
-        <v>45748</v>
+        <v>45839</v>
       </c>
       <c r="D3" s="6" t="inlineStr">
         <is>
@@ -904,19 +904,19 @@
         </is>
       </c>
       <c r="F3" s="24" t="n">
+        <v>24024.957</v>
+      </c>
+      <c r="G3" s="24" t="n">
         <v>23770.976</v>
       </c>
-      <c r="G3" s="24" t="n">
+      <c r="H3" s="24" t="n">
         <v>23548.21</v>
       </c>
-      <c r="H3" s="24" t="n">
+      <c r="I3" s="24" t="n">
         <v>23586.542</v>
       </c>
-      <c r="I3" s="24" t="n">
+      <c r="J3" s="24" t="n">
         <v>23478.57</v>
-      </c>
-      <c r="J3" s="24" t="n">
-        <v>23286.508</v>
       </c>
       <c r="K3" s="5" t="n"/>
       <c r="L3" s="28" t="inlineStr">
@@ -966,7 +966,7 @@
         </is>
       </c>
       <c r="C4" s="47" t="n">
-        <v>45748</v>
+        <v>45839</v>
       </c>
       <c r="D4" s="6" t="inlineStr">
         <is>
@@ -979,19 +979,19 @@
         </is>
       </c>
       <c r="F4" s="25" t="n">
+        <v>0.01068450029144774</v>
+      </c>
+      <c r="G4" s="25" t="n">
         <v>0.009459997171759493</v>
       </c>
-      <c r="G4" s="25" t="n">
+      <c r="H4" s="25" t="n">
         <v>-0.001625164044818495</v>
       </c>
-      <c r="H4" s="25" t="n">
+      <c r="I4" s="25" t="n">
         <v>0.004598746857240599</v>
       </c>
-      <c r="I4" s="25" t="n">
+      <c r="J4" s="25" t="n">
         <v>0.008247780216767531</v>
-      </c>
-      <c r="J4" s="25" t="n">
-        <v>0.008854862935244512</v>
       </c>
       <c r="K4" s="5" t="n"/>
       <c r="L4" s="28" t="n"/>
@@ -1040,7 +1040,7 @@
           <t>NGDPSAXDCUSQ</t>
         </is>
       </c>
-      <c r="C5" s="48" t="n">
+      <c r="C5" s="47" t="n">
         <v>45748</v>
       </c>
       <c r="D5" s="6" t="inlineStr">
@@ -1079,7 +1079,7 @@
           <t>ADPMNUSNERSA</t>
         </is>
       </c>
-      <c r="N5" s="47" t="n">
+      <c r="N5" s="48" t="n">
         <v>45962</v>
       </c>
       <c r="O5" s="6" t="inlineStr">
@@ -1115,7 +1115,7 @@
           <t>NGDPSAXDCUSQ</t>
         </is>
       </c>
-      <c r="C6" s="48" t="n">
+      <c r="C6" s="47" t="n">
         <v>45748</v>
       </c>
       <c r="D6" s="6" t="inlineStr">
@@ -1194,7 +1194,7 @@
           <t>GDPNOW</t>
         </is>
       </c>
-      <c r="C7" s="48" t="n">
+      <c r="C7" s="47" t="n">
         <v>45839</v>
       </c>
       <c r="D7" s="6" t="inlineStr">
@@ -1273,7 +1273,7 @@
           <t>RECPROUSM156N</t>
         </is>
       </c>
-      <c r="C8" s="47" t="n">
+      <c r="C8" s="48" t="n">
         <v>45870</v>
       </c>
       <c r="D8" s="6" t="inlineStr">
@@ -1353,7 +1353,7 @@
         </is>
       </c>
       <c r="C9" s="47" t="n">
-        <v>45748</v>
+        <v>45839</v>
       </c>
       <c r="D9" s="6" t="inlineStr">
         <is>
@@ -1366,19 +1366,19 @@
         </is>
       </c>
       <c r="F9" s="24" t="n">
+        <v>16589.126</v>
+      </c>
+      <c r="G9" s="24" t="n">
         <v>16445.685</v>
       </c>
-      <c r="G9" s="24" t="n">
+      <c r="H9" s="24" t="n">
         <v>16345.793</v>
       </c>
-      <c r="H9" s="24" t="n">
+      <c r="I9" s="24" t="n">
         <v>16320.89</v>
       </c>
-      <c r="I9" s="24" t="n">
+      <c r="J9" s="24" t="n">
         <v>16165.768</v>
-      </c>
-      <c r="J9" s="24" t="n">
-        <v>16009.637</v>
       </c>
       <c r="K9" s="5" t="n"/>
       <c r="L9" s="28" t="inlineStr">
@@ -1428,7 +1428,7 @@
         </is>
       </c>
       <c r="C10" s="47" t="n">
-        <v>45748</v>
+        <v>45839</v>
       </c>
       <c r="D10" s="6" t="inlineStr">
         <is>
@@ -1441,19 +1441,19 @@
         </is>
       </c>
       <c r="F10" s="25" t="n">
+        <v>0.008722105524944679</v>
+      </c>
+      <c r="G10" s="25" t="n">
         <v>0.006111174905983452</v>
       </c>
-      <c r="G10" s="25" t="n">
+      <c r="H10" s="25" t="n">
         <v>0.001525835907232986</v>
       </c>
-      <c r="H10" s="25" t="n">
+      <c r="I10" s="25" t="n">
         <v>0.009595708660423696</v>
       </c>
-      <c r="I10" s="25" t="n">
+      <c r="J10" s="25" t="n">
         <v>0.009752313559639125</v>
-      </c>
-      <c r="J10" s="25" t="n">
-        <v>0.009581021313047611</v>
       </c>
       <c r="K10" s="5" t="n"/>
       <c r="L10" s="28" t="inlineStr">
@@ -1466,7 +1466,7 @@
           <t>JTSJOR</t>
         </is>
       </c>
-      <c r="N10" s="47" t="n">
+      <c r="N10" s="48" t="n">
         <v>45931</v>
       </c>
       <c r="O10" s="6" t="inlineStr">
@@ -1506,7 +1506,7 @@
           <t>PCEDGC96</t>
         </is>
       </c>
-      <c r="C11" s="47" t="n">
+      <c r="C11" s="48" t="n">
         <v>45901</v>
       </c>
       <c r="D11" s="6" t="inlineStr">
@@ -1545,7 +1545,7 @@
           <t>JTSHIR</t>
         </is>
       </c>
-      <c r="N11" s="47" t="n">
+      <c r="N11" s="48" t="n">
         <v>45931</v>
       </c>
       <c r="O11" s="6" t="inlineStr">
@@ -1581,7 +1581,7 @@
           <t>PCEDGC96</t>
         </is>
       </c>
-      <c r="C12" s="47" t="n">
+      <c r="C12" s="48" t="n">
         <v>45901</v>
       </c>
       <c r="D12" s="6" t="inlineStr">
@@ -1620,7 +1620,7 @@
           <t>JTSTSR</t>
         </is>
       </c>
-      <c r="N12" s="47" t="n">
+      <c r="N12" s="48" t="n">
         <v>45931</v>
       </c>
       <c r="O12" s="6" t="inlineStr">
@@ -1660,7 +1660,7 @@
           <t>PCENDC96</t>
         </is>
       </c>
-      <c r="C13" s="47" t="n">
+      <c r="C13" s="48" t="n">
         <v>45901</v>
       </c>
       <c r="D13" s="6" t="inlineStr">
@@ -1699,7 +1699,7 @@
           <t>ICSA</t>
         </is>
       </c>
-      <c r="N13" s="48" t="n">
+      <c r="N13" s="47" t="n">
         <v>45999</v>
       </c>
       <c r="O13" s="6" t="inlineStr">
@@ -1735,7 +1735,7 @@
           <t>PCENDC96</t>
         </is>
       </c>
-      <c r="C14" s="47" t="n">
+      <c r="C14" s="48" t="n">
         <v>45901</v>
       </c>
       <c r="D14" s="6" t="inlineStr">
@@ -1774,7 +1774,7 @@
           <t>CCSA</t>
         </is>
       </c>
-      <c r="N14" s="48" t="n">
+      <c r="N14" s="47" t="n">
         <v>45992</v>
       </c>
       <c r="O14" s="6" t="inlineStr">
@@ -1814,7 +1814,7 @@
           <t>PCESC96</t>
         </is>
       </c>
-      <c r="C15" s="47" t="n">
+      <c r="C15" s="48" t="n">
         <v>45901</v>
       </c>
       <c r="D15" s="6" t="inlineStr">
@@ -1889,7 +1889,7 @@
           <t>PCESC96</t>
         </is>
       </c>
-      <c r="C16" s="47" t="n">
+      <c r="C16" s="48" t="n">
         <v>45901</v>
       </c>
       <c r="D16" s="6" t="inlineStr">
@@ -2066,7 +2066,7 @@
           <t>CPIAUCSL</t>
         </is>
       </c>
-      <c r="N18" s="48" t="n">
+      <c r="N18" s="47" t="n">
         <v>45962</v>
       </c>
       <c r="O18" s="6" t="inlineStr">
@@ -2106,7 +2106,7 @@
           <t>DSPIC96</t>
         </is>
       </c>
-      <c r="C19" s="47" t="n">
+      <c r="C19" s="48" t="n">
         <v>45901</v>
       </c>
       <c r="D19" s="6" t="inlineStr">
@@ -2141,7 +2141,7 @@
           <t>CPIAUCSL</t>
         </is>
       </c>
-      <c r="N19" s="48" t="n">
+      <c r="N19" s="47" t="n">
         <v>45962</v>
       </c>
       <c r="O19" s="6" t="inlineStr">
@@ -2177,7 +2177,7 @@
           <t>DSPIC96</t>
         </is>
       </c>
-      <c r="C20" s="47" t="n">
+      <c r="C20" s="48" t="n">
         <v>45901</v>
       </c>
       <c r="D20" s="6" t="inlineStr">
@@ -2216,7 +2216,7 @@
           <t>CPILFESL</t>
         </is>
       </c>
-      <c r="N20" s="48" t="n">
+      <c r="N20" s="47" t="n">
         <v>45962</v>
       </c>
       <c r="O20" s="6" t="inlineStr">
@@ -2256,7 +2256,7 @@
           <t>PSAVERT</t>
         </is>
       </c>
-      <c r="C21" s="47" t="n">
+      <c r="C21" s="48" t="n">
         <v>45901</v>
       </c>
       <c r="D21" s="6" t="inlineStr">
@@ -2291,7 +2291,7 @@
           <t>CPILFESL</t>
         </is>
       </c>
-      <c r="N21" s="48" t="n">
+      <c r="N21" s="47" t="n">
         <v>45962</v>
       </c>
       <c r="O21" s="6" t="inlineStr">
@@ -2331,7 +2331,7 @@
           <t>TOTALSA</t>
         </is>
       </c>
-      <c r="C22" s="47" t="n">
+      <c r="C22" s="48" t="n">
         <v>45962</v>
       </c>
       <c r="D22" s="6" t="inlineStr">
@@ -2370,7 +2370,7 @@
           <t>PPIFIS</t>
         </is>
       </c>
-      <c r="N22" s="47" t="n">
+      <c r="N22" s="48" t="n">
         <v>45901</v>
       </c>
       <c r="O22" s="6" t="inlineStr">
@@ -2406,7 +2406,7 @@
           <t>TOTALSA</t>
         </is>
       </c>
-      <c r="C23" s="47" t="n">
+      <c r="C23" s="48" t="n">
         <v>45962</v>
       </c>
       <c r="D23" s="6" t="inlineStr">
@@ -2440,7 +2440,7 @@
           <t>PPIFIS</t>
         </is>
       </c>
-      <c r="N23" s="47" t="n">
+      <c r="N23" s="48" t="n">
         <v>45901</v>
       </c>
       <c r="O23" s="6" t="inlineStr">
@@ -2480,7 +2480,7 @@
           <t>REVOLSL</t>
         </is>
       </c>
-      <c r="C24" s="47" t="n">
+      <c r="C24" s="48" t="n">
         <v>45931</v>
       </c>
       <c r="D24" s="6" t="inlineStr">
@@ -2519,7 +2519,7 @@
           <t>PCEPI</t>
         </is>
       </c>
-      <c r="N24" s="47" t="n">
+      <c r="N24" s="48" t="n">
         <v>45901</v>
       </c>
       <c r="O24" s="6" t="inlineStr">
@@ -2559,7 +2559,7 @@
           <t>NONREVSL</t>
         </is>
       </c>
-      <c r="C25" s="47" t="n">
+      <c r="C25" s="48" t="n">
         <v>45931</v>
       </c>
       <c r="D25" s="6" t="inlineStr">
@@ -2594,7 +2594,7 @@
           <t>PCEPI</t>
         </is>
       </c>
-      <c r="N25" s="47" t="n">
+      <c r="N25" s="48" t="n">
         <v>45901</v>
       </c>
       <c r="O25" s="6" t="inlineStr">
@@ -2635,7 +2635,7 @@
         </is>
       </c>
       <c r="C26" s="47" t="n">
-        <v>45748</v>
+        <v>45839</v>
       </c>
       <c r="D26" s="6" t="inlineStr">
         <is>
@@ -2648,19 +2648,19 @@
         </is>
       </c>
       <c r="F26" s="38" t="n">
+        <v>0.00701605762819324</v>
+      </c>
+      <c r="G26" s="38" t="n">
         <v>0.01778138610314484</v>
       </c>
-      <c r="G26" s="38" t="n">
+      <c r="H26" s="38" t="n">
         <v>0.02303791460563676</v>
       </c>
-      <c r="H26" s="38" t="n">
+      <c r="I26" s="38" t="n">
         <v>-0.009359213919614473</v>
       </c>
-      <c r="I26" s="38" t="n">
+      <c r="J26" s="38" t="n">
         <v>0.008576359077288709</v>
-      </c>
-      <c r="J26" s="38" t="n">
-        <v>0.00613124906143403</v>
       </c>
       <c r="K26" s="5" t="n"/>
       <c r="L26" s="28" t="inlineStr">
@@ -2673,7 +2673,7 @@
           <t>PCEPILFE</t>
         </is>
       </c>
-      <c r="N26" s="47" t="n">
+      <c r="N26" s="48" t="n">
         <v>45901</v>
       </c>
       <c r="O26" s="6" t="inlineStr">
@@ -2714,7 +2714,7 @@
         </is>
       </c>
       <c r="C27" s="47" t="n">
-        <v>45748</v>
+        <v>45839</v>
       </c>
       <c r="D27" s="6" t="inlineStr">
         <is>
@@ -2727,19 +2727,19 @@
         </is>
       </c>
       <c r="F27" s="38" t="n">
+        <v>-0.01313886426984179</v>
+      </c>
+      <c r="G27" s="38" t="n">
         <v>-0.01299350008050415</v>
       </c>
-      <c r="G27" s="38" t="n">
+      <c r="H27" s="38" t="n">
         <v>-0.002410568051752549</v>
       </c>
-      <c r="H27" s="38" t="n">
+      <c r="I27" s="38" t="n">
         <v>0.01049622222903812</v>
       </c>
-      <c r="I27" s="38" t="n">
+      <c r="J27" s="38" t="n">
         <v>-0.01224730930325912</v>
-      </c>
-      <c r="J27" s="38" t="n">
-        <v>-0.00502527710616385</v>
       </c>
       <c r="K27" s="5" t="n"/>
       <c r="L27" s="28" t="n"/>
@@ -2748,7 +2748,7 @@
           <t>PCEPILFE</t>
         </is>
       </c>
-      <c r="N27" s="47" t="n">
+      <c r="N27" s="48" t="n">
         <v>45901</v>
       </c>
       <c r="O27" s="6" t="inlineStr">
@@ -2789,7 +2789,7 @@
         </is>
       </c>
       <c r="C28" s="47" t="n">
-        <v>45901</v>
+        <v>45931</v>
       </c>
       <c r="D28" s="6" t="inlineStr">
         <is>
@@ -2802,19 +2802,19 @@
         </is>
       </c>
       <c r="F28" s="25" t="n">
-        <v>0.005052252529329948</v>
+        <v>-0.02165298568032004</v>
       </c>
       <c r="G28" s="25" t="n">
+        <v>0.006551589361115884</v>
+      </c>
+      <c r="H28" s="25" t="n">
         <v>0.03004963172206243</v>
       </c>
-      <c r="H28" s="25" t="n">
+      <c r="I28" s="25" t="n">
         <v>-0.02799901206372835</v>
       </c>
-      <c r="I28" s="25" t="n">
+      <c r="J28" s="25" t="n">
         <v>-0.09389977010425232</v>
-      </c>
-      <c r="J28" s="25" t="n">
-        <v>0.165430902790715</v>
       </c>
       <c r="K28" s="5" t="n"/>
       <c r="L28" s="28" t="inlineStr">
@@ -2827,7 +2827,7 @@
           <t>UMCSENT</t>
         </is>
       </c>
-      <c r="N28" s="47" t="n">
+      <c r="N28" s="48" t="n">
         <v>45962</v>
       </c>
       <c r="O28" s="6" t="inlineStr">
@@ -2864,7 +2864,7 @@
         </is>
       </c>
       <c r="C29" s="47" t="n">
-        <v>45901</v>
+        <v>45931</v>
       </c>
       <c r="D29" s="6" t="inlineStr">
         <is>
@@ -2877,19 +2877,19 @@
         </is>
       </c>
       <c r="F29" s="25" t="n">
-        <v>0.07264359641534658</v>
+        <v>0.04812695641499526</v>
       </c>
       <c r="G29" s="25" t="n">
+        <v>0.07424376600596987</v>
+      </c>
+      <c r="H29" s="25" t="n">
         <v>0.07661265288383932</v>
       </c>
-      <c r="H29" s="25" t="n">
+      <c r="I29" s="25" t="n">
         <v>0.03341358778313566</v>
       </c>
-      <c r="I29" s="25" t="n">
+      <c r="J29" s="25" t="n">
         <v>0.1089645997552716</v>
-      </c>
-      <c r="J29" s="25" t="n">
-        <v>0.1995614111543812</v>
       </c>
       <c r="K29" s="5" t="n"/>
       <c r="L29" s="28" t="inlineStr">
@@ -2902,8 +2902,8 @@
           <t>T5YIFR</t>
         </is>
       </c>
-      <c r="N29" s="48" t="n">
-        <v>46010</v>
+      <c r="N29" s="47" t="n">
+        <v>46013</v>
       </c>
       <c r="O29" s="6" t="inlineStr">
         <is>
@@ -2919,13 +2919,13 @@
         <v>2.21</v>
       </c>
       <c r="R29" s="6" t="n">
-        <v>2.22</v>
+        <v>2.21</v>
       </c>
       <c r="S29" s="6" t="n">
         <v>2.22</v>
       </c>
       <c r="T29" s="6" t="n">
-        <v>2.21</v>
+        <v>2.22</v>
       </c>
       <c r="U29" s="21" t="n">
         <v>2.21</v>
@@ -2943,7 +2943,7 @@
         </is>
       </c>
       <c r="C30" s="47" t="n">
-        <v>45901</v>
+        <v>45931</v>
       </c>
       <c r="D30" s="6" t="inlineStr">
         <is>
@@ -2956,19 +2956,19 @@
         </is>
       </c>
       <c r="F30" s="25" t="n">
-        <v>0.000905510184407321</v>
+        <v>-0.01501954810691108</v>
       </c>
       <c r="G30" s="25" t="n">
+        <v>0.00129801269780061</v>
+      </c>
+      <c r="H30" s="25" t="n">
         <v>0.01907672443132968</v>
       </c>
-      <c r="H30" s="25" t="n">
+      <c r="I30" s="25" t="n">
         <v>-0.02404555711932721</v>
       </c>
-      <c r="I30" s="25" t="n">
+      <c r="J30" s="25" t="n">
         <v>-0.09442194506291901</v>
-      </c>
-      <c r="J30" s="25" t="n">
-        <v>0.1570751450479186</v>
       </c>
       <c r="K30" s="5" t="n"/>
       <c r="L30" s="28" t="inlineStr">
@@ -2981,8 +2981,8 @@
           <t>T10YIE</t>
         </is>
       </c>
-      <c r="N30" s="48" t="n">
-        <v>46010</v>
+      <c r="N30" s="47" t="n">
+        <v>46013</v>
       </c>
       <c r="O30" s="6" t="inlineStr">
         <is>
@@ -2995,7 +2995,7 @@
         </is>
       </c>
       <c r="Q30" s="6" t="n">
-        <v>2.24</v>
+        <v>2.23</v>
       </c>
       <c r="R30" s="6" t="n">
         <v>2.24</v>
@@ -3004,10 +3004,10 @@
         <v>2.24</v>
       </c>
       <c r="T30" s="6" t="n">
+        <v>2.24</v>
+      </c>
+      <c r="U30" s="21" t="n">
         <v>2.23</v>
-      </c>
-      <c r="U30" s="21" t="n">
-        <v>2.25</v>
       </c>
     </row>
     <row r="31">
@@ -3018,7 +3018,7 @@
         </is>
       </c>
       <c r="C31" s="47" t="n">
-        <v>45901</v>
+        <v>45931</v>
       </c>
       <c r="D31" s="6" t="inlineStr">
         <is>
@@ -3031,19 +3031,19 @@
         </is>
       </c>
       <c r="F31" s="25" t="n">
-        <v>0.0647360016408333</v>
+        <v>0.04791954754640503</v>
       </c>
       <c r="G31" s="25" t="n">
+        <v>0.06515353511676288</v>
+      </c>
+      <c r="H31" s="25" t="n">
         <v>0.06671073894520346</v>
       </c>
-      <c r="H31" s="25" t="n">
+      <c r="I31" s="25" t="n">
         <v>0.0329297153895499</v>
       </c>
-      <c r="I31" s="25" t="n">
+      <c r="J31" s="25" t="n">
         <v>0.1029410098461701</v>
-      </c>
-      <c r="J31" s="25" t="n">
-        <v>0.1925388202490265</v>
       </c>
       <c r="K31" s="5" t="n"/>
       <c r="L31" s="28" t="inlineStr">
@@ -3056,7 +3056,7 @@
           <t>ECIWAG</t>
         </is>
       </c>
-      <c r="N31" s="47" t="n">
+      <c r="N31" s="48" t="n">
         <v>45839</v>
       </c>
       <c r="O31" s="6" t="inlineStr">
@@ -3097,7 +3097,7 @@
         </is>
       </c>
       <c r="C32" s="47" t="n">
-        <v>45901</v>
+        <v>45962</v>
       </c>
       <c r="D32" s="6" t="inlineStr">
         <is>
@@ -3110,19 +3110,19 @@
         </is>
       </c>
       <c r="F32" s="25" t="n">
-        <v>0.0009661502023092794</v>
+        <v>0.001746772161864252</v>
       </c>
       <c r="G32" s="25" t="n">
-        <v>-0.002569125217784962</v>
+        <v>-0.0005596378189272055</v>
       </c>
       <c r="H32" s="25" t="n">
-        <v>0.001607051307331187</v>
+        <v>0.0006988058294186139</v>
       </c>
       <c r="I32" s="25" t="n">
-        <v>0.004463379393190303</v>
+        <v>-0.002668988493606861</v>
       </c>
       <c r="J32" s="25" t="n">
-        <v>-0.001489203276247131</v>
+        <v>0.003895406416137392</v>
       </c>
       <c r="K32" s="5" t="n"/>
       <c r="L32" s="28" t="n"/>
@@ -3131,7 +3131,7 @@
           <t>ECIWAG</t>
         </is>
       </c>
-      <c r="N32" s="47" t="n">
+      <c r="N32" s="48" t="n">
         <v>45839</v>
       </c>
       <c r="O32" s="6" t="inlineStr">
@@ -3168,7 +3168,7 @@
         </is>
       </c>
       <c r="C33" s="47" t="n">
-        <v>45901</v>
+        <v>45962</v>
       </c>
       <c r="D33" s="6" t="inlineStr">
         <is>
@@ -3181,19 +3181,19 @@
         </is>
       </c>
       <c r="F33" s="25" t="n">
-        <v>0.01622608918688194</v>
+        <v>0.02518820656142197</v>
       </c>
       <c r="G33" s="25" t="n">
-        <v>0.008952424004962659</v>
+        <v>0.02157947913682087</v>
       </c>
       <c r="H33" s="25" t="n">
-        <v>0.01615692613305024</v>
+        <v>0.01868079239823494</v>
       </c>
       <c r="I33" s="25" t="n">
-        <v>0.005292683410311731</v>
+        <v>0.01165975810233709</v>
       </c>
       <c r="J33" s="25" t="n">
-        <v>0.001133220308735612</v>
+        <v>0.01898561350408149</v>
       </c>
       <c r="K33" s="5" t="n"/>
       <c r="L33" s="28" t="inlineStr">
@@ -3247,7 +3247,7 @@
         </is>
       </c>
       <c r="C34" s="47" t="n">
-        <v>45901</v>
+        <v>45962</v>
       </c>
       <c r="D34" s="6" t="inlineStr">
         <is>
@@ -3260,19 +3260,19 @@
         </is>
       </c>
       <c r="F34" s="24" t="n">
-        <v>75.8665</v>
+        <v>75.95659999999999</v>
       </c>
       <c r="G34" s="24" t="n">
-        <v>75.8847</v>
+        <v>75.9156</v>
       </c>
       <c r="H34" s="24" t="n">
-        <v>76.1724</v>
+        <v>76.0498</v>
       </c>
       <c r="I34" s="24" t="n">
-        <v>76.1431</v>
+        <v>76.08839999999999</v>
       </c>
       <c r="J34" s="24" t="n">
-        <v>75.8982</v>
+        <v>76.3844</v>
       </c>
       <c r="K34" s="5" t="n"/>
       <c r="L34" s="28" t="n"/>
@@ -3321,7 +3321,7 @@
           <t>PRS85006092</t>
         </is>
       </c>
-      <c r="C35" s="47" t="n">
+      <c r="C35" s="48" t="n">
         <v>45748</v>
       </c>
       <c r="D35" s="6" t="inlineStr">
@@ -3396,7 +3396,7 @@
           <t>HOUST</t>
         </is>
       </c>
-      <c r="C36" s="47" t="n">
+      <c r="C36" s="48" t="n">
         <v>45870</v>
       </c>
       <c r="D36" s="6" t="inlineStr">
@@ -3471,7 +3471,7 @@
           <t>HOUST</t>
         </is>
       </c>
-      <c r="C37" s="47" t="n">
+      <c r="C37" s="48" t="n">
         <v>45870</v>
       </c>
       <c r="D37" s="6" t="inlineStr">
@@ -3510,7 +3510,7 @@
           <t>CSUSHPINSA</t>
         </is>
       </c>
-      <c r="N37" s="47" t="n">
+      <c r="N37" s="48" t="n">
         <v>45901</v>
       </c>
       <c r="O37" s="6" t="inlineStr">
@@ -3550,7 +3550,7 @@
           <t>PERMIT</t>
         </is>
       </c>
-      <c r="C38" s="47" t="n">
+      <c r="C38" s="48" t="n">
         <v>45870</v>
       </c>
       <c r="D38" s="6" t="inlineStr">
@@ -3585,7 +3585,7 @@
           <t>CSUSHPINSA</t>
         </is>
       </c>
-      <c r="N38" s="47" t="n">
+      <c r="N38" s="48" t="n">
         <v>45901</v>
       </c>
       <c r="O38" s="6" t="inlineStr">
@@ -3621,7 +3621,7 @@
           <t>PERMIT</t>
         </is>
       </c>
-      <c r="C39" s="47" t="n">
+      <c r="C39" s="48" t="n">
         <v>45870</v>
       </c>
       <c r="D39" s="6" t="inlineStr">
@@ -3661,7 +3661,7 @@
         </is>
       </c>
       <c r="N39" s="47" t="n">
-        <v>46003</v>
+        <v>46010</v>
       </c>
       <c r="O39" s="6" t="inlineStr">
         <is>
@@ -3674,19 +3674,19 @@
         </is>
       </c>
       <c r="Q39" s="6" t="n">
-        <v>120.5383</v>
+        <v>120.5571</v>
       </c>
       <c r="R39" s="6" t="n">
-        <v>120.3821</v>
+        <v>120.4409</v>
       </c>
       <c r="S39" s="6" t="n">
-        <v>121.0557</v>
+        <v>120.5451</v>
       </c>
       <c r="T39" s="6" t="n">
-        <v>121.0601</v>
+        <v>120.283</v>
       </c>
       <c r="U39" s="21" t="n">
-        <v>121.1478</v>
+        <v>120.3501</v>
       </c>
     </row>
     <row r="40">
@@ -3700,7 +3700,7 @@
           <t>HSN1F</t>
         </is>
       </c>
-      <c r="C40" s="47" t="n">
+      <c r="C40" s="48" t="n">
         <v>45870</v>
       </c>
       <c r="D40" s="6" t="inlineStr">
@@ -3773,7 +3773,7 @@
           <t>HSN1F</t>
         </is>
       </c>
-      <c r="C41" s="47" t="n">
+      <c r="C41" s="48" t="n">
         <v>45870</v>
       </c>
       <c r="D41" s="6" t="inlineStr">
@@ -3812,7 +3812,7 @@
           <t>IQ</t>
         </is>
       </c>
-      <c r="N41" s="47" t="n">
+      <c r="N41" s="48" t="n">
         <v>45901</v>
       </c>
       <c r="O41" s="6" t="inlineStr">
@@ -3852,7 +3852,7 @@
           <t>EXHOSLUSM495S</t>
         </is>
       </c>
-      <c r="C42" s="47" t="n">
+      <c r="C42" s="48" t="n">
         <v>45962</v>
       </c>
       <c r="D42" s="6" t="inlineStr">
@@ -3887,7 +3887,7 @@
           <t>IQ</t>
         </is>
       </c>
-      <c r="N42" s="47" t="n">
+      <c r="N42" s="48" t="n">
         <v>45901</v>
       </c>
       <c r="O42" s="6" t="inlineStr">
@@ -3923,7 +3923,7 @@
           <t>EXHOSLUSM495S</t>
         </is>
       </c>
-      <c r="C43" s="47" t="n">
+      <c r="C43" s="48" t="n">
         <v>45962</v>
       </c>
       <c r="D43" s="6" t="inlineStr">
@@ -3962,7 +3962,7 @@
           <t>IR</t>
         </is>
       </c>
-      <c r="N43" s="47" t="n">
+      <c r="N43" s="48" t="n">
         <v>45901</v>
       </c>
       <c r="O43" s="6" t="inlineStr">
@@ -4003,7 +4003,7 @@
         </is>
       </c>
       <c r="C44" s="47" t="n">
-        <v>45748</v>
+        <v>45839</v>
       </c>
       <c r="D44" s="6" t="inlineStr">
         <is>
@@ -4016,19 +4016,19 @@
         </is>
       </c>
       <c r="F44" s="24" t="n">
+        <v>5323.099</v>
+      </c>
+      <c r="G44" s="24" t="n">
         <v>5236.97</v>
       </c>
-      <c r="G44" s="24" t="n">
+      <c r="H44" s="24" t="n">
         <v>5195.517</v>
       </c>
-      <c r="H44" s="24" t="n">
+      <c r="I44" s="24" t="n">
         <v>5150.725</v>
       </c>
-      <c r="I44" s="24" t="n">
+      <c r="J44" s="24" t="n">
         <v>5086.922</v>
-      </c>
-      <c r="J44" s="24" t="n">
-        <v>4995.15</v>
       </c>
       <c r="K44" s="5" t="n"/>
       <c r="L44" s="28" t="n"/>
@@ -4037,7 +4037,7 @@
           <t>IR</t>
         </is>
       </c>
-      <c r="N44" s="47" t="n">
+      <c r="N44" s="48" t="n">
         <v>45901</v>
       </c>
       <c r="O44" s="6" t="inlineStr">
@@ -4074,7 +4074,7 @@
         </is>
       </c>
       <c r="C45" s="47" t="n">
-        <v>45748</v>
+        <v>45839</v>
       </c>
       <c r="D45" s="6" t="inlineStr">
         <is>
@@ -4087,19 +4087,19 @@
         </is>
       </c>
       <c r="F45" s="38" t="n">
+        <v>0.01644634206420892</v>
+      </c>
+      <c r="G45" s="38" t="n">
         <v>0.007978609251013902</v>
       </c>
-      <c r="G45" s="38" t="n">
+      <c r="H45" s="38" t="n">
         <v>0.008696251498575336</v>
       </c>
-      <c r="H45" s="38" t="n">
+      <c r="I45" s="38" t="n">
         <v>0.01254255520332359</v>
       </c>
-      <c r="I45" s="38" t="n">
+      <c r="J45" s="38" t="n">
         <v>0.01837222105442282</v>
-      </c>
-      <c r="J45" s="38" t="n">
-        <v>0.01284993218468711</v>
       </c>
       <c r="K45" s="5" t="n"/>
       <c r="L45" s="28" t="n"/>
@@ -4124,7 +4124,7 @@
           <t>BOPTEXP</t>
         </is>
       </c>
-      <c r="C46" s="47" t="n">
+      <c r="C46" s="48" t="n">
         <v>45901</v>
       </c>
       <c r="D46" s="6" t="inlineStr">
@@ -4211,7 +4211,7 @@
           <t>BOPTEXP</t>
         </is>
       </c>
-      <c r="C47" s="47" t="n">
+      <c r="C47" s="48" t="n">
         <v>45901</v>
       </c>
       <c r="D47" s="6" t="inlineStr">
@@ -4250,8 +4250,8 @@
           <t>DFF</t>
         </is>
       </c>
-      <c r="N47" s="48" t="n">
-        <v>46009</v>
+      <c r="N47" s="47" t="n">
+        <v>46010</v>
       </c>
       <c r="O47" s="6" t="inlineStr">
         <is>
@@ -4290,7 +4290,7 @@
           <t>BOPTIMP</t>
         </is>
       </c>
-      <c r="C48" s="47" t="n">
+      <c r="C48" s="48" t="n">
         <v>45901</v>
       </c>
       <c r="D48" s="6" t="inlineStr">
@@ -4329,8 +4329,8 @@
           <t>DGS2</t>
         </is>
       </c>
-      <c r="N48" s="48" t="n">
-        <v>46009</v>
+      <c r="N48" s="47" t="n">
+        <v>46010</v>
       </c>
       <c r="O48" s="6" t="inlineStr">
         <is>
@@ -4343,19 +4343,19 @@
         </is>
       </c>
       <c r="Q48" s="6" t="n">
+        <v>3.48</v>
+      </c>
+      <c r="R48" s="6" t="n">
         <v>3.46</v>
       </c>
-      <c r="R48" s="6" t="n">
+      <c r="S48" s="6" t="n">
         <v>3.49</v>
       </c>
-      <c r="S48" s="6" t="n">
+      <c r="T48" s="6" t="n">
         <v>3.48</v>
       </c>
-      <c r="T48" s="6" t="n">
+      <c r="U48" s="21" t="n">
         <v>3.51</v>
-      </c>
-      <c r="U48" s="21" t="n">
-        <v/>
       </c>
     </row>
     <row r="49">
@@ -4365,7 +4365,7 @@
           <t>BOPTIMP</t>
         </is>
       </c>
-      <c r="C49" s="47" t="n">
+      <c r="C49" s="48" t="n">
         <v>45901</v>
       </c>
       <c r="D49" s="6" t="inlineStr">
@@ -4404,8 +4404,8 @@
           <t>DGS5</t>
         </is>
       </c>
-      <c r="N49" s="48" t="n">
-        <v>46009</v>
+      <c r="N49" s="47" t="n">
+        <v>46010</v>
       </c>
       <c r="O49" s="6" t="inlineStr">
         <is>
@@ -4418,19 +4418,19 @@
         </is>
       </c>
       <c r="Q49" s="6" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="R49" s="6" t="n">
         <v>3.66</v>
       </c>
-      <c r="R49" s="6" t="n">
+      <c r="S49" s="6" t="n">
         <v>3.7</v>
       </c>
-      <c r="S49" s="6" t="n">
+      <c r="T49" s="6" t="n">
         <v>3.69</v>
       </c>
-      <c r="T49" s="6" t="n">
+      <c r="U49" s="21" t="n">
         <v>3.73</v>
-      </c>
-      <c r="U49" s="21" t="n">
-        <v/>
       </c>
     </row>
     <row r="50">
@@ -4444,7 +4444,7 @@
           <t>BOPSTB</t>
         </is>
       </c>
-      <c r="C50" s="47" t="n">
+      <c r="C50" s="48" t="n">
         <v>45901</v>
       </c>
       <c r="D50" s="6" t="inlineStr">
@@ -4483,8 +4483,8 @@
           <t>DGS10</t>
         </is>
       </c>
-      <c r="N50" s="48" t="n">
-        <v>46009</v>
+      <c r="N50" s="47" t="n">
+        <v>46010</v>
       </c>
       <c r="O50" s="6" t="inlineStr">
         <is>
@@ -4497,19 +4497,19 @@
         </is>
       </c>
       <c r="Q50" s="6" t="n">
+        <v>4.16</v>
+      </c>
+      <c r="R50" s="6" t="n">
         <v>4.12</v>
       </c>
-      <c r="R50" s="6" t="n">
+      <c r="S50" s="6" t="n">
         <v>4.16</v>
       </c>
-      <c r="S50" s="6" t="n">
+      <c r="T50" s="6" t="n">
         <v>4.15</v>
       </c>
-      <c r="T50" s="6" t="n">
+      <c r="U50" s="21" t="n">
         <v>4.18</v>
-      </c>
-      <c r="U50" s="21" t="n">
-        <v/>
       </c>
     </row>
     <row r="51" ht="31.5" customHeight="1">
@@ -4519,7 +4519,7 @@
           <t>BOPSTB</t>
         </is>
       </c>
-      <c r="C51" s="47" t="n">
+      <c r="C51" s="48" t="n">
         <v>45901</v>
       </c>
       <c r="D51" s="6" t="inlineStr">
@@ -4558,7 +4558,7 @@
           <t>MORTGAGE30US</t>
         </is>
       </c>
-      <c r="N51" s="48" t="n">
+      <c r="N51" s="47" t="n">
         <v>46006</v>
       </c>
       <c r="O51" s="6" t="inlineStr">
@@ -4610,7 +4610,7 @@
         </is>
       </c>
       <c r="N52" s="49" t="n">
-        <v>46009</v>
+        <v>46010</v>
       </c>
       <c r="O52" s="9" t="inlineStr">
         <is>
@@ -4623,19 +4623,19 @@
         </is>
       </c>
       <c r="Q52" s="9" t="n">
+        <v>5.92</v>
+      </c>
+      <c r="R52" s="9" t="n">
         <v>5.9</v>
       </c>
-      <c r="R52" s="9" t="n">
+      <c r="S52" s="9" t="n">
         <v>5.94</v>
       </c>
-      <c r="S52" s="9" t="n">
+      <c r="T52" s="9" t="n">
         <v>5.93</v>
       </c>
-      <c r="T52" s="9" t="n">
+      <c r="U52" s="22" t="n">
         <v>5.95</v>
-      </c>
-      <c r="U52" s="22" t="n">
-        <v/>
       </c>
     </row>
     <row r="53" ht="21" customHeight="1">

</xml_diff>

<commit_message>
Update dashboards - 2025-12-24
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -1719,7 +1719,7 @@
         </is>
       </c>
       <c r="N13" s="48" t="n">
-        <v>45999</v>
+        <v>46006</v>
       </c>
       <c r="O13" s="6" t="inlineStr">
         <is>
@@ -1732,19 +1732,19 @@
         </is>
       </c>
       <c r="Q13" s="24" t="n">
+        <v>214000</v>
+      </c>
+      <c r="R13" s="24" t="n">
         <v>224000</v>
       </c>
-      <c r="R13" s="24" t="n">
+      <c r="S13" s="24" t="n">
         <v>237000</v>
       </c>
-      <c r="S13" s="24" t="n">
+      <c r="T13" s="24" t="n">
         <v>192000</v>
       </c>
-      <c r="T13" s="24" t="n">
+      <c r="U13" s="26" t="n">
         <v>217000</v>
-      </c>
-      <c r="U13" s="26" t="n">
-        <v>222000</v>
       </c>
     </row>
     <row r="14">
@@ -1794,7 +1794,7 @@
         </is>
       </c>
       <c r="N14" s="48" t="n">
-        <v>45992</v>
+        <v>45999</v>
       </c>
       <c r="O14" s="6" t="inlineStr">
         <is>
@@ -1807,19 +1807,19 @@
         </is>
       </c>
       <c r="Q14" s="24" t="n">
-        <v>1897000</v>
+        <v>1923000</v>
       </c>
       <c r="R14" s="24" t="n">
+        <v>1885000</v>
+      </c>
+      <c r="S14" s="24" t="n">
         <v>1830000</v>
       </c>
-      <c r="S14" s="24" t="n">
+      <c r="T14" s="24" t="n">
         <v>1937000</v>
       </c>
-      <c r="T14" s="24" t="n">
+      <c r="U14" s="26" t="n">
         <v>1944000</v>
-      </c>
-      <c r="U14" s="26" t="n">
-        <v>1953000</v>
       </c>
     </row>
     <row r="15">

</xml_diff>

<commit_message>
Update dashboards - 2025-12-25
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -1213,8 +1213,8 @@
           <t>GDPNOW</t>
         </is>
       </c>
-      <c r="C7" s="49" t="n">
-        <v>45839</v>
+      <c r="C7" s="48" t="n">
+        <v>45931</v>
       </c>
       <c r="D7" s="6" t="inlineStr">
         <is>
@@ -1227,19 +1227,19 @@
         </is>
       </c>
       <c r="F7" s="44" t="n">
+        <v>2.9721</v>
+      </c>
+      <c r="G7" s="44" t="n">
         <v>3.4728</v>
       </c>
-      <c r="G7" s="44" t="n">
+      <c r="H7" s="44" t="n">
         <v>2.902</v>
       </c>
-      <c r="H7" s="44" t="n">
+      <c r="I7" s="44" t="n">
         <v>-2.7318</v>
       </c>
-      <c r="I7" s="44" t="n">
+      <c r="J7" s="44" t="n">
         <v>2.2711</v>
-      </c>
-      <c r="J7" s="44" t="n">
-        <v>2.789</v>
       </c>
       <c r="K7" s="5" t="n"/>
       <c r="L7" s="28" t="inlineStr">
@@ -2085,7 +2085,7 @@
           <t>CPIAUCSL</t>
         </is>
       </c>
-      <c r="N18" s="48" t="n">
+      <c r="N18" s="49" t="n">
         <v>45962</v>
       </c>
       <c r="O18" s="6" t="inlineStr">
@@ -2160,7 +2160,7 @@
           <t>CPIAUCSL</t>
         </is>
       </c>
-      <c r="N19" s="48" t="n">
+      <c r="N19" s="49" t="n">
         <v>45962</v>
       </c>
       <c r="O19" s="6" t="inlineStr">
@@ -2235,7 +2235,7 @@
           <t>CPILFESL</t>
         </is>
       </c>
-      <c r="N20" s="48" t="n">
+      <c r="N20" s="49" t="n">
         <v>45962</v>
       </c>
       <c r="O20" s="6" t="inlineStr">
@@ -2310,7 +2310,7 @@
           <t>CPILFESL</t>
         </is>
       </c>
-      <c r="N21" s="48" t="n">
+      <c r="N21" s="49" t="n">
         <v>45962</v>
       </c>
       <c r="O21" s="6" t="inlineStr">
@@ -2922,7 +2922,7 @@
         </is>
       </c>
       <c r="N29" s="48" t="n">
-        <v>46014</v>
+        <v>46015</v>
       </c>
       <c r="O29" s="6" t="inlineStr">
         <is>
@@ -2938,13 +2938,13 @@
         <v>2.24</v>
       </c>
       <c r="R29" s="6" t="n">
-        <v>2.21</v>
+        <v>2.24</v>
       </c>
       <c r="S29" s="6" t="n">
         <v>2.21</v>
       </c>
       <c r="T29" s="6" t="n">
-        <v>2.22</v>
+        <v>2.21</v>
       </c>
       <c r="U29" s="21" t="n">
         <v>2.22</v>
@@ -3001,7 +3001,7 @@
         </is>
       </c>
       <c r="N30" s="48" t="n">
-        <v>46014</v>
+        <v>46015</v>
       </c>
       <c r="O30" s="6" t="inlineStr">
         <is>
@@ -3017,10 +3017,10 @@
         <v>2.24</v>
       </c>
       <c r="R30" s="6" t="n">
+        <v>2.24</v>
+      </c>
+      <c r="S30" s="6" t="n">
         <v>2.23</v>
-      </c>
-      <c r="S30" s="6" t="n">
-        <v>2.24</v>
       </c>
       <c r="T30" s="6" t="n">
         <v>2.24</v>
@@ -4576,7 +4576,7 @@
         </is>
       </c>
       <c r="N51" s="48" t="n">
-        <v>46006</v>
+        <v>46013</v>
       </c>
       <c r="O51" s="6" t="inlineStr">
         <is>
@@ -4589,19 +4589,19 @@
         </is>
       </c>
       <c r="Q51" s="6" t="n">
+        <v>6.18</v>
+      </c>
+      <c r="R51" s="6" t="n">
         <v>6.21</v>
       </c>
-      <c r="R51" s="6" t="n">
+      <c r="S51" s="6" t="n">
         <v>6.22</v>
       </c>
-      <c r="S51" s="6" t="n">
+      <c r="T51" s="6" t="n">
         <v>6.19</v>
       </c>
-      <c r="T51" s="6" t="n">
+      <c r="U51" s="21" t="n">
         <v>6.23</v>
-      </c>
-      <c r="U51" s="21" t="n">
-        <v>6.26</v>
       </c>
     </row>
     <row r="52" ht="16.15" customHeight="1" thickBot="1">
@@ -4627,7 +4627,7 @@
         </is>
       </c>
       <c r="N52" s="53" t="n">
-        <v>46013</v>
+        <v>46014</v>
       </c>
       <c r="O52" s="9" t="inlineStr">
         <is>
@@ -4640,19 +4640,19 @@
         </is>
       </c>
       <c r="Q52" s="9" t="n">
+        <v>5.92</v>
+      </c>
+      <c r="R52" s="9" t="n">
         <v>5.93</v>
       </c>
-      <c r="R52" s="9" t="n">
+      <c r="S52" s="9" t="n">
         <v>5.92</v>
       </c>
-      <c r="S52" s="9" t="n">
+      <c r="T52" s="9" t="n">
         <v>5.9</v>
       </c>
-      <c r="T52" s="9" t="n">
+      <c r="U52" s="22" t="n">
         <v>5.94</v>
-      </c>
-      <c r="U52" s="22" t="n">
-        <v>5.93</v>
       </c>
     </row>
     <row r="53" ht="21" customHeight="1">

</xml_diff>

<commit_message>
Update dashboards - 2025-12-27
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -2364,7 +2364,7 @@
         </is>
       </c>
       <c r="F22" s="24" t="n">
-        <v>15.963</v>
+        <v>15.926</v>
       </c>
       <c r="G22" s="24" t="n">
         <v>15.63</v>
@@ -2439,7 +2439,7 @@
         </is>
       </c>
       <c r="F23" s="25" t="n">
-        <v>-0.0612760952660982</v>
+        <v>-0.06345192590414578</v>
       </c>
       <c r="G23" s="25" t="n">
         <v>-0.05593138439236531</v>
@@ -2922,7 +2922,7 @@
         </is>
       </c>
       <c r="N29" s="48" t="n">
-        <v>46015</v>
+        <v>46017</v>
       </c>
       <c r="O29" s="6" t="inlineStr">
         <is>
@@ -2941,13 +2941,13 @@
         <v>2.24</v>
       </c>
       <c r="S29" s="6" t="n">
-        <v>2.21</v>
+        <v>2.24</v>
       </c>
       <c r="T29" s="6" t="n">
         <v>2.21</v>
       </c>
       <c r="U29" s="21" t="n">
-        <v>2.22</v>
+        <v>2.21</v>
       </c>
     </row>
     <row r="30">
@@ -3001,7 +3001,7 @@
         </is>
       </c>
       <c r="N30" s="48" t="n">
-        <v>46015</v>
+        <v>46017</v>
       </c>
       <c r="O30" s="6" t="inlineStr">
         <is>
@@ -3014,16 +3014,16 @@
         </is>
       </c>
       <c r="Q30" s="6" t="n">
-        <v>2.24</v>
+        <v>2.23</v>
       </c>
       <c r="R30" s="6" t="n">
         <v>2.24</v>
       </c>
       <c r="S30" s="6" t="n">
+        <v>2.24</v>
+      </c>
+      <c r="T30" s="6" t="n">
         <v>2.23</v>
-      </c>
-      <c r="T30" s="6" t="n">
-        <v>2.24</v>
       </c>
       <c r="U30" s="21" t="n">
         <v>2.24</v>

</xml_diff>

<commit_message>
Update dashboards - 2025-12-29
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -1059,8 +1059,8 @@
           <t>NGDPSAXDCUSQ</t>
         </is>
       </c>
-      <c r="C5" s="49" t="n">
-        <v>45748</v>
+      <c r="C5" s="48" t="n">
+        <v>45839</v>
       </c>
       <c r="D5" s="6" t="inlineStr">
         <is>
@@ -1073,19 +1073,19 @@
         </is>
       </c>
       <c r="F5" s="24" t="n">
+        <v>7773772.3</v>
+      </c>
+      <c r="G5" s="24" t="n">
         <v>7621432.3</v>
       </c>
-      <c r="G5" s="24" t="n">
+      <c r="H5" s="24" t="n">
         <v>7510528.3</v>
       </c>
-      <c r="H5" s="24" t="n">
+      <c r="I5" s="24" t="n">
         <v>7456295.5</v>
       </c>
-      <c r="I5" s="24" t="n">
+      <c r="J5" s="24" t="n">
         <v>7377916</v>
-      </c>
-      <c r="J5" s="24" t="n">
-        <v>7286761</v>
       </c>
       <c r="K5" s="5" t="n"/>
       <c r="L5" s="28" t="inlineStr">
@@ -1134,8 +1134,8 @@
           <t>NGDPSAXDCUSQ</t>
         </is>
       </c>
-      <c r="C6" s="49" t="n">
-        <v>45748</v>
+      <c r="C6" s="48" t="n">
+        <v>45839</v>
       </c>
       <c r="D6" s="6" t="inlineStr">
         <is>
@@ -1148,19 +1148,19 @@
         </is>
       </c>
       <c r="F6" s="25" t="n">
+        <v>0.01998836885292543</v>
+      </c>
+      <c r="G6" s="25" t="n">
         <v>0.0147664712214719</v>
       </c>
-      <c r="G6" s="25" t="n">
+      <c r="H6" s="25" t="n">
         <v>0.007273424182290045</v>
       </c>
-      <c r="H6" s="25" t="n">
+      <c r="I6" s="25" t="n">
         <v>0.01062352837847436</v>
       </c>
-      <c r="I6" s="25" t="n">
+      <c r="J6" s="25" t="n">
         <v>0.01250967336516173</v>
-      </c>
-      <c r="J6" s="25" t="n">
-        <v>0.01528773636675829</v>
       </c>
       <c r="K6" s="5" t="n"/>
       <c r="L6" s="28" t="inlineStr">
@@ -4267,7 +4267,7 @@
           <t>DFF</t>
         </is>
       </c>
-      <c r="N47" s="48" t="n">
+      <c r="N47" s="49" t="n">
         <v>46013</v>
       </c>
       <c r="O47" s="6" t="inlineStr">
@@ -4346,7 +4346,7 @@
           <t>DGS2</t>
         </is>
       </c>
-      <c r="N48" s="48" t="n">
+      <c r="N48" s="49" t="n">
         <v>46013</v>
       </c>
       <c r="O48" s="6" t="inlineStr">
@@ -4421,7 +4421,7 @@
           <t>DGS5</t>
         </is>
       </c>
-      <c r="N49" s="48" t="n">
+      <c r="N49" s="49" t="n">
         <v>46013</v>
       </c>
       <c r="O49" s="6" t="inlineStr">
@@ -4500,7 +4500,7 @@
           <t>DGS10</t>
         </is>
       </c>
-      <c r="N50" s="48" t="n">
+      <c r="N50" s="49" t="n">
         <v>46013</v>
       </c>
       <c r="O50" s="6" t="inlineStr">

</xml_diff>

<commit_message>
Update dashboards - 2025-12-30
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -360,10 +360,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="168" fontId="1" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="1" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
@@ -948,7 +948,7 @@
           <t>PAYEMS</t>
         </is>
       </c>
-      <c r="N3" s="49" t="n">
+      <c r="N3" s="48" t="n">
         <v>45962</v>
       </c>
       <c r="O3" s="6" t="inlineStr">
@@ -1019,7 +1019,7 @@
           <t>PAYEMS</t>
         </is>
       </c>
-      <c r="N4" s="49" t="n">
+      <c r="N4" s="48" t="n">
         <v>45962</v>
       </c>
       <c r="O4" s="6" t="inlineStr">
@@ -1059,7 +1059,7 @@
           <t>NGDPSAXDCUSQ</t>
         </is>
       </c>
-      <c r="C5" s="48" t="n">
+      <c r="C5" s="49" t="n">
         <v>45839</v>
       </c>
       <c r="D5" s="6" t="inlineStr">
@@ -1098,7 +1098,7 @@
           <t>ADPMNUSNERSA</t>
         </is>
       </c>
-      <c r="N5" s="49" t="n">
+      <c r="N5" s="48" t="n">
         <v>45962</v>
       </c>
       <c r="O5" s="6" t="inlineStr">
@@ -1134,7 +1134,7 @@
           <t>NGDPSAXDCUSQ</t>
         </is>
       </c>
-      <c r="C6" s="48" t="n">
+      <c r="C6" s="49" t="n">
         <v>45839</v>
       </c>
       <c r="D6" s="6" t="inlineStr">
@@ -1173,7 +1173,7 @@
           <t>UNRATE</t>
         </is>
       </c>
-      <c r="N6" s="49" t="n">
+      <c r="N6" s="48" t="n">
         <v>45962</v>
       </c>
       <c r="O6" s="6" t="inlineStr">
@@ -1213,7 +1213,7 @@
           <t>GDPNOW</t>
         </is>
       </c>
-      <c r="C7" s="48" t="n">
+      <c r="C7" s="49" t="n">
         <v>45931</v>
       </c>
       <c r="D7" s="6" t="inlineStr">
@@ -1252,7 +1252,7 @@
           <t>U6RATE</t>
         </is>
       </c>
-      <c r="N7" s="49" t="n">
+      <c r="N7" s="48" t="n">
         <v>45962</v>
       </c>
       <c r="O7" s="6" t="inlineStr">
@@ -1292,7 +1292,7 @@
           <t>RECPROUSM156N</t>
         </is>
       </c>
-      <c r="C8" s="49" t="n">
+      <c r="C8" s="48" t="n">
         <v>45870</v>
       </c>
       <c r="D8" s="6" t="inlineStr">
@@ -1331,7 +1331,7 @@
           <t>CIVPART</t>
         </is>
       </c>
-      <c r="N8" s="49" t="n">
+      <c r="N8" s="48" t="n">
         <v>45962</v>
       </c>
       <c r="O8" s="6" t="inlineStr">
@@ -1410,7 +1410,7 @@
           <t>EMRATIO</t>
         </is>
       </c>
-      <c r="N9" s="49" t="n">
+      <c r="N9" s="48" t="n">
         <v>45962</v>
       </c>
       <c r="O9" s="6" t="inlineStr">
@@ -1485,7 +1485,7 @@
           <t>JTSJOR</t>
         </is>
       </c>
-      <c r="N10" s="49" t="n">
+      <c r="N10" s="48" t="n">
         <v>45931</v>
       </c>
       <c r="O10" s="6" t="inlineStr">
@@ -1525,7 +1525,7 @@
           <t>PCEDGC96</t>
         </is>
       </c>
-      <c r="C11" s="49" t="n">
+      <c r="C11" s="48" t="n">
         <v>45901</v>
       </c>
       <c r="D11" s="6" t="inlineStr">
@@ -1539,13 +1539,13 @@
         </is>
       </c>
       <c r="F11" s="25" t="n">
-        <v>-0.00597293513765762</v>
+        <v>-0.003916814324349538</v>
       </c>
       <c r="G11" s="25" t="n">
-        <v>0.0007471747454934619</v>
+        <v>0.001447583469530667</v>
       </c>
       <c r="H11" s="25" t="n">
-        <v>0.01300913004399451</v>
+        <v>0.01305643597142714</v>
       </c>
       <c r="I11" s="25" t="n">
         <v>-0.001794399584454709</v>
@@ -1564,7 +1564,7 @@
           <t>JTSHIR</t>
         </is>
       </c>
-      <c r="N11" s="49" t="n">
+      <c r="N11" s="48" t="n">
         <v>45931</v>
       </c>
       <c r="O11" s="6" t="inlineStr">
@@ -1600,7 +1600,7 @@
           <t>PCEDGC96</t>
         </is>
       </c>
-      <c r="C12" s="49" t="n">
+      <c r="C12" s="48" t="n">
         <v>45901</v>
       </c>
       <c r="D12" s="6" t="inlineStr">
@@ -1614,13 +1614,13 @@
         </is>
       </c>
       <c r="F12" s="25" t="n">
-        <v>0.02065066360021078</v>
+        <v>0.02352546595754871</v>
       </c>
       <c r="G12" s="25" t="n">
-        <v>0.03827519379844961</v>
+        <v>0.03905038759689918</v>
       </c>
       <c r="H12" s="25" t="n">
-        <v>0.03404316963638997</v>
+        <v>0.03409145782027134</v>
       </c>
       <c r="I12" s="25" t="n">
         <v>0.0349571603427173</v>
@@ -1639,7 +1639,7 @@
           <t>JTSTSR</t>
         </is>
       </c>
-      <c r="N12" s="49" t="n">
+      <c r="N12" s="48" t="n">
         <v>45931</v>
       </c>
       <c r="O12" s="6" t="inlineStr">
@@ -1679,7 +1679,7 @@
           <t>PCENDC96</t>
         </is>
       </c>
-      <c r="C13" s="49" t="n">
+      <c r="C13" s="48" t="n">
         <v>45901</v>
       </c>
       <c r="D13" s="6" t="inlineStr">
@@ -1693,13 +1693,13 @@
         </is>
       </c>
       <c r="F13" s="25" t="n">
-        <v>-0.003324786565608084</v>
+        <v>-0.003153419489258624</v>
       </c>
       <c r="G13" s="25" t="n">
-        <v>0.004500169817728938</v>
+        <v>0.00520759629807821</v>
       </c>
       <c r="H13" s="25" t="n">
-        <v>0.002952197115930311</v>
+        <v>0.002980583626660538</v>
       </c>
       <c r="I13" s="25" t="n">
         <v>0.007003401652231123</v>
@@ -1718,7 +1718,7 @@
           <t>ICSA</t>
         </is>
       </c>
-      <c r="N13" s="48" t="n">
+      <c r="N13" s="49" t="n">
         <v>46006</v>
       </c>
       <c r="O13" s="6" t="inlineStr">
@@ -1754,7 +1754,7 @@
           <t>PCENDC96</t>
         </is>
       </c>
-      <c r="C14" s="49" t="n">
+      <c r="C14" s="48" t="n">
         <v>45901</v>
       </c>
       <c r="D14" s="6" t="inlineStr">
@@ -1768,13 +1768,13 @@
         </is>
       </c>
       <c r="F14" s="25" t="n">
-        <v>0.02107207805328638</v>
+        <v>0.02199578558438929</v>
       </c>
       <c r="G14" s="25" t="n">
-        <v>0.03720264188438825</v>
+        <v>0.03796247588988241</v>
       </c>
       <c r="H14" s="25" t="n">
-        <v>0.03053813621117101</v>
+        <v>0.03056730348548933</v>
       </c>
       <c r="I14" s="25" t="n">
         <v>0.03332160037545476</v>
@@ -1793,7 +1793,7 @@
           <t>CCSA</t>
         </is>
       </c>
-      <c r="N14" s="48" t="n">
+      <c r="N14" s="49" t="n">
         <v>45999</v>
       </c>
       <c r="O14" s="6" t="inlineStr">
@@ -1833,7 +1833,7 @@
           <t>PCESC96</t>
         </is>
       </c>
-      <c r="C15" s="49" t="n">
+      <c r="C15" s="48" t="n">
         <v>45901</v>
       </c>
       <c r="D15" s="6" t="inlineStr">
@@ -1847,13 +1847,13 @@
         </is>
       </c>
       <c r="F15" s="25" t="n">
-        <v>0.002492303181351518</v>
+        <v>0.003107917877840594</v>
       </c>
       <c r="G15" s="25" t="n">
-        <v>0.002121114733024232</v>
+        <v>0.002529279155440545</v>
       </c>
       <c r="H15" s="25" t="n">
-        <v>0.002513071654761001</v>
+        <v>0.004510641431622275</v>
       </c>
       <c r="I15" s="25" t="n">
         <v>0.001973841981958824</v>
@@ -1872,7 +1872,7 @@
           <t>AWHAETP</t>
         </is>
       </c>
-      <c r="N15" s="49" t="n">
+      <c r="N15" s="48" t="n">
         <v>45962</v>
       </c>
       <c r="O15" s="6" t="inlineStr">
@@ -1908,7 +1908,7 @@
           <t>PCESC96</t>
         </is>
       </c>
-      <c r="C16" s="49" t="n">
+      <c r="C16" s="48" t="n">
         <v>45901</v>
       </c>
       <c r="D16" s="6" t="inlineStr">
@@ -1922,13 +1922,13 @@
         </is>
       </c>
       <c r="F16" s="25" t="n">
-        <v>0.02155949168526313</v>
+        <v>0.02464075294820676</v>
       </c>
       <c r="G16" s="25" t="n">
-        <v>0.02099315196647079</v>
+        <v>0.02344422407663796</v>
       </c>
       <c r="H16" s="25" t="n">
-        <v>0.021987199939941</v>
+        <v>0.02402357313113493</v>
       </c>
       <c r="I16" s="25" t="n">
         <v>0.02094865746266567</v>
@@ -1959,7 +1959,7 @@
           <t>RSAFS</t>
         </is>
       </c>
-      <c r="C17" s="49" t="n">
+      <c r="C17" s="48" t="n">
         <v>45931</v>
       </c>
       <c r="D17" s="6" t="inlineStr">
@@ -2046,7 +2046,7 @@
           <t>RSAFS</t>
         </is>
       </c>
-      <c r="C18" s="49" t="n">
+      <c r="C18" s="48" t="n">
         <v>45931</v>
       </c>
       <c r="D18" s="6" t="inlineStr">
@@ -2085,7 +2085,7 @@
           <t>CPIAUCSL</t>
         </is>
       </c>
-      <c r="N18" s="49" t="n">
+      <c r="N18" s="48" t="n">
         <v>45962</v>
       </c>
       <c r="O18" s="6" t="inlineStr">
@@ -2125,7 +2125,7 @@
           <t>DSPIC96</t>
         </is>
       </c>
-      <c r="C19" s="49" t="n">
+      <c r="C19" s="48" t="n">
         <v>45901</v>
       </c>
       <c r="D19" s="6" t="inlineStr">
@@ -2139,19 +2139,19 @@
         </is>
       </c>
       <c r="F19" s="25" t="n">
-        <v>0.0006075636146720687</v>
+        <v>0.0005379773162141888</v>
       </c>
       <c r="G19" s="25" t="n">
-        <v>0.001139097016782165</v>
+        <v>0.001065997457151857</v>
       </c>
       <c r="H19" s="25" t="n">
-        <v>0.002677947682993009</v>
+        <v>0.002739100661949267</v>
       </c>
       <c r="I19" s="25" t="n">
-        <v>-0.000304849321294598</v>
+        <v>-0.001045553893298079</v>
       </c>
       <c r="J19" s="25" t="n">
-        <v>-0.006984577788051838</v>
+        <v>-0.008382553259544845</v>
       </c>
       <c r="K19" s="5" t="n"/>
       <c r="L19" s="28" t="n"/>
@@ -2160,7 +2160,7 @@
           <t>CPIAUCSL</t>
         </is>
       </c>
-      <c r="N19" s="49" t="n">
+      <c r="N19" s="48" t="n">
         <v>45962</v>
       </c>
       <c r="O19" s="6" t="inlineStr">
@@ -2196,7 +2196,7 @@
           <t>DSPIC96</t>
         </is>
       </c>
-      <c r="C20" s="49" t="n">
+      <c r="C20" s="48" t="n">
         <v>45901</v>
       </c>
       <c r="D20" s="6" t="inlineStr">
@@ -2210,19 +2210,19 @@
         </is>
       </c>
       <c r="F20" s="25" t="n">
-        <v>0.01948238313102477</v>
+        <v>0.01521111542552289</v>
       </c>
       <c r="G20" s="25" t="n">
-        <v>0.01983901221772201</v>
+        <v>0.01563688186155493</v>
       </c>
       <c r="H20" s="25" t="n">
-        <v>0.01923553812164656</v>
+        <v>0.01511001397718554</v>
       </c>
       <c r="I20" s="25" t="n">
-        <v>0.01606097650286474</v>
+        <v>0.01188658731008219</v>
       </c>
       <c r="J20" s="25" t="n">
-        <v>0.01853974132431571</v>
+        <v>0.01510729226061785</v>
       </c>
       <c r="K20" s="5" t="n"/>
       <c r="L20" s="28" t="inlineStr">
@@ -2235,7 +2235,7 @@
           <t>CPILFESL</t>
         </is>
       </c>
-      <c r="N20" s="49" t="n">
+      <c r="N20" s="48" t="n">
         <v>45962</v>
       </c>
       <c r="O20" s="6" t="inlineStr">
@@ -2275,7 +2275,7 @@
           <t>PSAVERT</t>
         </is>
       </c>
-      <c r="C21" s="49" t="n">
+      <c r="C21" s="48" t="n">
         <v>45901</v>
       </c>
       <c r="D21" s="6" t="inlineStr">
@@ -2289,19 +2289,19 @@
         </is>
       </c>
       <c r="F21" s="6" t="n">
-        <v>4.7</v>
+        <v>4</v>
       </c>
       <c r="G21" s="6" t="n">
-        <v>4.7</v>
+        <v>4.1</v>
       </c>
       <c r="H21" s="6" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="I21" s="6" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="J21" s="6" t="n">
         <v>4.9</v>
-      </c>
-      <c r="I21" s="6" t="n">
-        <v>5</v>
-      </c>
-      <c r="J21" s="6" t="n">
-        <v>5.2</v>
       </c>
       <c r="K21" s="5" t="n"/>
       <c r="L21" s="28" t="n"/>
@@ -2310,7 +2310,7 @@
           <t>CPILFESL</t>
         </is>
       </c>
-      <c r="N21" s="49" t="n">
+      <c r="N21" s="48" t="n">
         <v>45962</v>
       </c>
       <c r="O21" s="6" t="inlineStr">
@@ -2350,7 +2350,7 @@
           <t>TOTALSA</t>
         </is>
       </c>
-      <c r="C22" s="49" t="n">
+      <c r="C22" s="48" t="n">
         <v>45962</v>
       </c>
       <c r="D22" s="6" t="inlineStr">
@@ -2389,7 +2389,7 @@
           <t>PPIFIS</t>
         </is>
       </c>
-      <c r="N22" s="49" t="n">
+      <c r="N22" s="48" t="n">
         <v>45901</v>
       </c>
       <c r="O22" s="6" t="inlineStr">
@@ -2425,7 +2425,7 @@
           <t>TOTALSA</t>
         </is>
       </c>
-      <c r="C23" s="49" t="n">
+      <c r="C23" s="48" t="n">
         <v>45962</v>
       </c>
       <c r="D23" s="6" t="inlineStr">
@@ -2459,7 +2459,7 @@
           <t>PPIFIS</t>
         </is>
       </c>
-      <c r="N23" s="49" t="n">
+      <c r="N23" s="48" t="n">
         <v>45901</v>
       </c>
       <c r="O23" s="6" t="inlineStr">
@@ -2499,7 +2499,7 @@
           <t>REVOLSL</t>
         </is>
       </c>
-      <c r="C24" s="49" t="n">
+      <c r="C24" s="48" t="n">
         <v>45931</v>
       </c>
       <c r="D24" s="6" t="inlineStr">
@@ -2538,7 +2538,7 @@
           <t>PCEPI</t>
         </is>
       </c>
-      <c r="N24" s="49" t="n">
+      <c r="N24" s="48" t="n">
         <v>45901</v>
       </c>
       <c r="O24" s="6" t="inlineStr">
@@ -2552,13 +2552,13 @@
         </is>
       </c>
       <c r="Q24" s="38" t="n">
-        <v>0.002686925983831356</v>
+        <v>0.002663272761554536</v>
       </c>
       <c r="R24" s="38" t="n">
-        <v>0.002583592611555385</v>
+        <v>0.002599305276589803</v>
       </c>
       <c r="S24" s="38" t="n">
-        <v>0.001672676203025025</v>
+        <v>0.001688456167204588</v>
       </c>
       <c r="T24" s="38" t="n">
         <v>0.002872289919291005</v>
@@ -2578,7 +2578,7 @@
           <t>NONREVSL</t>
         </is>
       </c>
-      <c r="C25" s="49" t="n">
+      <c r="C25" s="48" t="n">
         <v>45931</v>
       </c>
       <c r="D25" s="6" t="inlineStr">
@@ -2613,7 +2613,7 @@
           <t>PCEPI</t>
         </is>
       </c>
-      <c r="N25" s="49" t="n">
+      <c r="N25" s="48" t="n">
         <v>45901</v>
       </c>
       <c r="O25" s="6" t="inlineStr">
@@ -2627,13 +2627,13 @@
         </is>
       </c>
       <c r="Q25" s="38" t="n">
-        <v>0.02787442414870654</v>
+        <v>0.02788247801295064</v>
       </c>
       <c r="R25" s="38" t="n">
-        <v>0.02739549112512011</v>
+        <v>0.02742777809167892</v>
       </c>
       <c r="S25" s="38" t="n">
-        <v>0.02601506433051007</v>
+        <v>0.02603122777526338</v>
       </c>
       <c r="T25" s="38" t="n">
         <v>0.02593512979706808</v>
@@ -2692,7 +2692,7 @@
           <t>PCEPILFE</t>
         </is>
       </c>
-      <c r="N26" s="49" t="n">
+      <c r="N26" s="48" t="n">
         <v>45901</v>
       </c>
       <c r="O26" s="6" t="inlineStr">
@@ -2706,13 +2706,13 @@
         </is>
       </c>
       <c r="Q26" s="38" t="n">
-        <v>0.001981010710085718</v>
+        <v>0.0019572715003906</v>
       </c>
       <c r="R26" s="38" t="n">
-        <v>0.002206859457065002</v>
+        <v>0.002222644076376623</v>
       </c>
       <c r="S26" s="38" t="n">
-        <v>0.002402454785483954</v>
+        <v>0.002418312572846748</v>
       </c>
       <c r="T26" s="38" t="n">
         <v>0.002631369743222756</v>
@@ -2767,7 +2767,7 @@
           <t>PCEPILFE</t>
         </is>
       </c>
-      <c r="N27" s="49" t="n">
+      <c r="N27" s="48" t="n">
         <v>45901</v>
       </c>
       <c r="O27" s="6" t="inlineStr">
@@ -2781,13 +2781,13 @@
         </is>
       </c>
       <c r="Q27" s="38" t="n">
-        <v>0.02825069249833962</v>
+        <v>0.02825879189412473</v>
       </c>
       <c r="R27" s="38" t="n">
-        <v>0.02903482554739785</v>
+        <v>0.02906731206549277</v>
       </c>
       <c r="S27" s="38" t="n">
-        <v>0.02858165664586575</v>
+        <v>0.02859792858247025</v>
       </c>
       <c r="T27" s="38" t="n">
         <v>0.02807372205058803</v>
@@ -2846,7 +2846,7 @@
           <t>MICH</t>
         </is>
       </c>
-      <c r="N28" s="49" t="n">
+      <c r="N28" s="48" t="n">
         <v>45962</v>
       </c>
       <c r="O28" s="6" t="inlineStr">
@@ -2921,8 +2921,8 @@
           <t>T5YIFR</t>
         </is>
       </c>
-      <c r="N29" s="48" t="n">
-        <v>46017</v>
+      <c r="N29" s="49" t="n">
+        <v>46020</v>
       </c>
       <c r="O29" s="6" t="inlineStr">
         <is>
@@ -2935,7 +2935,7 @@
         </is>
       </c>
       <c r="Q29" s="6" t="n">
-        <v>2.24</v>
+        <v>2.21</v>
       </c>
       <c r="R29" s="6" t="n">
         <v>2.24</v>
@@ -2944,7 +2944,7 @@
         <v>2.24</v>
       </c>
       <c r="T29" s="6" t="n">
-        <v>2.21</v>
+        <v>2.24</v>
       </c>
       <c r="U29" s="21" t="n">
         <v>2.21</v>
@@ -3000,8 +3000,8 @@
           <t>T10YIE</t>
         </is>
       </c>
-      <c r="N30" s="48" t="n">
-        <v>46017</v>
+      <c r="N30" s="49" t="n">
+        <v>46020</v>
       </c>
       <c r="O30" s="6" t="inlineStr">
         <is>
@@ -3014,19 +3014,19 @@
         </is>
       </c>
       <c r="Q30" s="6" t="n">
+        <v>2.22</v>
+      </c>
+      <c r="R30" s="6" t="n">
         <v>2.23</v>
-      </c>
-      <c r="R30" s="6" t="n">
-        <v>2.24</v>
       </c>
       <c r="S30" s="6" t="n">
         <v>2.24</v>
       </c>
       <c r="T30" s="6" t="n">
+        <v>2.24</v>
+      </c>
+      <c r="U30" s="21" t="n">
         <v>2.23</v>
-      </c>
-      <c r="U30" s="21" t="n">
-        <v>2.24</v>
       </c>
     </row>
     <row r="31">
@@ -3075,7 +3075,7 @@
           <t>ECIWAG</t>
         </is>
       </c>
-      <c r="N31" s="49" t="n">
+      <c r="N31" s="48" t="n">
         <v>45839</v>
       </c>
       <c r="O31" s="6" t="inlineStr">
@@ -3150,7 +3150,7 @@
           <t>ECIWAG</t>
         </is>
       </c>
-      <c r="N32" s="49" t="n">
+      <c r="N32" s="48" t="n">
         <v>45839</v>
       </c>
       <c r="O32" s="6" t="inlineStr">
@@ -3225,7 +3225,7 @@
           <t>CES0500000003</t>
         </is>
       </c>
-      <c r="N33" s="49" t="n">
+      <c r="N33" s="48" t="n">
         <v>45962</v>
       </c>
       <c r="O33" s="6" t="inlineStr">
@@ -3300,7 +3300,7 @@
           <t>RCES0500000003*</t>
         </is>
       </c>
-      <c r="N34" s="49" t="n">
+      <c r="N34" s="48" t="n">
         <v>45901</v>
       </c>
       <c r="O34" s="6" t="inlineStr">
@@ -3314,13 +3314,13 @@
         </is>
       </c>
       <c r="Q34" s="38" t="n">
-        <v>0.009230301788676142</v>
+        <v>0.00922239407158258</v>
       </c>
       <c r="R34" s="38" t="n">
-        <v>0.01063283120727662</v>
+        <v>0.01060107202271849</v>
       </c>
       <c r="S34" s="38" t="n">
-        <v>0.0124408693429683</v>
+        <v>0.01242491999209615</v>
       </c>
       <c r="T34" s="38" t="n">
         <v>0.01120289314371833</v>
@@ -3340,7 +3340,7 @@
           <t>PRS85006092</t>
         </is>
       </c>
-      <c r="C35" s="49" t="n">
+      <c r="C35" s="48" t="n">
         <v>45748</v>
       </c>
       <c r="D35" s="6" t="inlineStr">
@@ -3379,7 +3379,7 @@
           <t>RCES0500000003*</t>
         </is>
       </c>
-      <c r="N35" s="49" t="n">
+      <c r="N35" s="48" t="n">
         <v>45901</v>
       </c>
       <c r="O35" s="6" t="inlineStr">
@@ -3393,13 +3393,13 @@
         </is>
       </c>
       <c r="Q35" s="38" t="n">
-        <v>-0.0007712397230601464</v>
+        <v>-0.0007476675222880536</v>
       </c>
       <c r="R35" s="38" t="n">
-        <v>0.001529940234958005</v>
+        <v>0.00151424432893621</v>
       </c>
       <c r="S35" s="38" t="n">
-        <v>0.001629472906588658</v>
+        <v>0.001613693871594046</v>
       </c>
       <c r="T35" s="38" t="n">
         <v>-0.0006622728576672898</v>
@@ -3415,7 +3415,7 @@
           <t>HOUST</t>
         </is>
       </c>
-      <c r="C36" s="49" t="n">
+      <c r="C36" s="48" t="n">
         <v>45870</v>
       </c>
       <c r="D36" s="6" t="inlineStr">
@@ -3450,7 +3450,7 @@
           <t>RCES0500000003*</t>
         </is>
       </c>
-      <c r="N36" s="49" t="n">
+      <c r="N36" s="48" t="n">
         <v>45901</v>
       </c>
       <c r="O36" s="6" t="inlineStr">
@@ -3464,13 +3464,13 @@
         </is>
       </c>
       <c r="Q36" s="38" t="n">
-        <v>0.009230301788676142</v>
+        <v>0.00922239407158258</v>
       </c>
       <c r="R36" s="38" t="n">
-        <v>0.01063283120727662</v>
+        <v>0.01060107202271849</v>
       </c>
       <c r="S36" s="38" t="n">
-        <v>0.0124408693429683</v>
+        <v>0.01242491999209615</v>
       </c>
       <c r="T36" s="38" t="n">
         <v>0.01120289314371833</v>
@@ -3490,7 +3490,7 @@
           <t>HOUST</t>
         </is>
       </c>
-      <c r="C37" s="49" t="n">
+      <c r="C37" s="48" t="n">
         <v>45870</v>
       </c>
       <c r="D37" s="6" t="inlineStr">
@@ -3530,7 +3530,7 @@
         </is>
       </c>
       <c r="N37" s="49" t="n">
-        <v>45901</v>
+        <v>45931</v>
       </c>
       <c r="O37" s="6" t="inlineStr">
         <is>
@@ -3543,19 +3543,19 @@
         </is>
       </c>
       <c r="Q37" s="38" t="n">
-        <v>-0.002680233580537372</v>
+        <v>-0.001629288280675323</v>
       </c>
       <c r="R37" s="38" t="n">
-        <v>-0.003492679271734134</v>
+        <v>-0.00274944298770774</v>
       </c>
       <c r="S37" s="38" t="n">
-        <v>-0.002089419937226888</v>
+        <v>-0.003326424682615015</v>
       </c>
       <c r="T37" s="38" t="n">
-        <v>0.0006667672348770193</v>
+        <v>-0.001932894486878389</v>
       </c>
       <c r="U37" s="23" t="n">
-        <v>0.004670985029205044</v>
+        <v>0.0005672235313285423</v>
       </c>
     </row>
     <row r="38">
@@ -3569,7 +3569,7 @@
           <t>PERMIT</t>
         </is>
       </c>
-      <c r="C38" s="49" t="n">
+      <c r="C38" s="48" t="n">
         <v>45870</v>
       </c>
       <c r="D38" s="6" t="inlineStr">
@@ -3605,7 +3605,7 @@
         </is>
       </c>
       <c r="N38" s="49" t="n">
-        <v>45901</v>
+        <v>45931</v>
       </c>
       <c r="O38" s="6" t="inlineStr">
         <is>
@@ -3618,19 +3618,19 @@
         </is>
       </c>
       <c r="Q38" s="38" t="n">
-        <v>0.01291790739138332</v>
+        <v>0.01361915137225375</v>
       </c>
       <c r="R38" s="38" t="n">
-        <v>0.01449043557431158</v>
+        <v>0.01314403621693212</v>
       </c>
       <c r="S38" s="38" t="n">
-        <v>0.01630494859795866</v>
+        <v>0.0147934636823388</v>
       </c>
       <c r="T38" s="38" t="n">
-        <v>0.01943770804710052</v>
+        <v>0.01644499448762562</v>
       </c>
       <c r="U38" s="23" t="n">
-        <v>0.02364466296472451</v>
+        <v>0.01942153460248559</v>
       </c>
     </row>
     <row r="39" ht="31.5" customHeight="1">
@@ -3640,7 +3640,7 @@
           <t>PERMIT</t>
         </is>
       </c>
-      <c r="C39" s="49" t="n">
+      <c r="C39" s="48" t="n">
         <v>45870</v>
       </c>
       <c r="D39" s="6" t="inlineStr">
@@ -3679,7 +3679,7 @@
           <t>TWEXBGSMTH</t>
         </is>
       </c>
-      <c r="N39" s="49" t="n">
+      <c r="N39" s="48" t="n">
         <v>45962</v>
       </c>
       <c r="O39" s="6" t="inlineStr">
@@ -3719,7 +3719,7 @@
           <t>HSN1F</t>
         </is>
       </c>
-      <c r="C40" s="49" t="n">
+      <c r="C40" s="48" t="n">
         <v>45870</v>
       </c>
       <c r="D40" s="6" t="inlineStr">
@@ -3754,7 +3754,7 @@
           <t>TWEXBGSMTH</t>
         </is>
       </c>
-      <c r="N40" s="49" t="n">
+      <c r="N40" s="48" t="n">
         <v>45962</v>
       </c>
       <c r="O40" s="6" t="inlineStr">
@@ -3790,7 +3790,7 @@
           <t>HSN1F</t>
         </is>
       </c>
-      <c r="C41" s="49" t="n">
+      <c r="C41" s="48" t="n">
         <v>45870</v>
       </c>
       <c r="D41" s="6" t="inlineStr">
@@ -3829,7 +3829,7 @@
           <t>IQ</t>
         </is>
       </c>
-      <c r="N41" s="49" t="n">
+      <c r="N41" s="48" t="n">
         <v>45901</v>
       </c>
       <c r="O41" s="6" t="inlineStr">
@@ -3869,7 +3869,7 @@
           <t>EXHOSLUSM495S</t>
         </is>
       </c>
-      <c r="C42" s="49" t="n">
+      <c r="C42" s="48" t="n">
         <v>45962</v>
       </c>
       <c r="D42" s="6" t="inlineStr">
@@ -3904,7 +3904,7 @@
           <t>IQ</t>
         </is>
       </c>
-      <c r="N42" s="49" t="n">
+      <c r="N42" s="48" t="n">
         <v>45901</v>
       </c>
       <c r="O42" s="6" t="inlineStr">
@@ -3940,7 +3940,7 @@
           <t>EXHOSLUSM495S</t>
         </is>
       </c>
-      <c r="C43" s="49" t="n">
+      <c r="C43" s="48" t="n">
         <v>45962</v>
       </c>
       <c r="D43" s="6" t="inlineStr">
@@ -3979,7 +3979,7 @@
           <t>IR</t>
         </is>
       </c>
-      <c r="N43" s="49" t="n">
+      <c r="N43" s="48" t="n">
         <v>45901</v>
       </c>
       <c r="O43" s="6" t="inlineStr">
@@ -4054,7 +4054,7 @@
           <t>IR</t>
         </is>
       </c>
-      <c r="N44" s="49" t="n">
+      <c r="N44" s="48" t="n">
         <v>45901</v>
       </c>
       <c r="O44" s="6" t="inlineStr">
@@ -4141,7 +4141,7 @@
           <t>BOPTEXP</t>
         </is>
       </c>
-      <c r="C46" s="49" t="n">
+      <c r="C46" s="48" t="n">
         <v>45901</v>
       </c>
       <c r="D46" s="6" t="inlineStr">
@@ -4228,7 +4228,7 @@
           <t>BOPTEXP</t>
         </is>
       </c>
-      <c r="C47" s="49" t="n">
+      <c r="C47" s="48" t="n">
         <v>45901</v>
       </c>
       <c r="D47" s="6" t="inlineStr">
@@ -4268,7 +4268,7 @@
         </is>
       </c>
       <c r="N47" s="49" t="n">
-        <v>46013</v>
+        <v>46017</v>
       </c>
       <c r="O47" s="6" t="inlineStr">
         <is>
@@ -4307,7 +4307,7 @@
           <t>BOPTIMP</t>
         </is>
       </c>
-      <c r="C48" s="49" t="n">
+      <c r="C48" s="48" t="n">
         <v>45901</v>
       </c>
       <c r="D48" s="6" t="inlineStr">
@@ -4347,7 +4347,7 @@
         </is>
       </c>
       <c r="N48" s="49" t="n">
-        <v>46013</v>
+        <v>46017</v>
       </c>
       <c r="O48" s="6" t="inlineStr">
         <is>
@@ -4360,16 +4360,16 @@
         </is>
       </c>
       <c r="Q48" s="6" t="n">
+        <v>3.46</v>
+      </c>
+      <c r="R48" s="6" t="n">
+        <v>3.47</v>
+      </c>
+      <c r="S48" s="6" t="n">
+        <v>3.48</v>
+      </c>
+      <c r="T48" s="6" t="n">
         <v>3.44</v>
-      </c>
-      <c r="R48" s="6" t="n">
-        <v>3.48</v>
-      </c>
-      <c r="S48" s="6" t="n">
-        <v>3.46</v>
-      </c>
-      <c r="T48" s="6" t="n">
-        <v>3.49</v>
       </c>
       <c r="U48" s="21" t="n">
         <v>3.48</v>
@@ -4382,7 +4382,7 @@
           <t>BOPTIMP</t>
         </is>
       </c>
-      <c r="C49" s="49" t="n">
+      <c r="C49" s="48" t="n">
         <v>45901</v>
       </c>
       <c r="D49" s="6" t="inlineStr">
@@ -4422,7 +4422,7 @@
         </is>
       </c>
       <c r="N49" s="49" t="n">
-        <v>46013</v>
+        <v>46017</v>
       </c>
       <c r="O49" s="6" t="inlineStr">
         <is>
@@ -4435,19 +4435,19 @@
         </is>
       </c>
       <c r="Q49" s="6" t="n">
-        <v>3.71</v>
+        <v>3.68</v>
       </c>
       <c r="R49" s="6" t="n">
         <v>3.7</v>
       </c>
       <c r="S49" s="6" t="n">
-        <v>3.66</v>
+        <v>3.72</v>
       </c>
       <c r="T49" s="6" t="n">
+        <v>3.71</v>
+      </c>
+      <c r="U49" s="21" t="n">
         <v>3.7</v>
-      </c>
-      <c r="U49" s="21" t="n">
-        <v>3.69</v>
       </c>
     </row>
     <row r="50">
@@ -4461,7 +4461,7 @@
           <t>BOPSTB</t>
         </is>
       </c>
-      <c r="C50" s="49" t="n">
+      <c r="C50" s="48" t="n">
         <v>45901</v>
       </c>
       <c r="D50" s="6" t="inlineStr">
@@ -4501,7 +4501,7 @@
         </is>
       </c>
       <c r="N50" s="49" t="n">
-        <v>46013</v>
+        <v>46017</v>
       </c>
       <c r="O50" s="6" t="inlineStr">
         <is>
@@ -4514,19 +4514,19 @@
         </is>
       </c>
       <c r="Q50" s="6" t="n">
+        <v>4.14</v>
+      </c>
+      <c r="R50" s="6" t="n">
+        <v>4.15</v>
+      </c>
+      <c r="S50" s="6" t="n">
+        <v>4.18</v>
+      </c>
+      <c r="T50" s="6" t="n">
         <v>4.17</v>
       </c>
-      <c r="R50" s="6" t="n">
+      <c r="U50" s="21" t="n">
         <v>4.16</v>
-      </c>
-      <c r="S50" s="6" t="n">
-        <v>4.12</v>
-      </c>
-      <c r="T50" s="6" t="n">
-        <v>4.16</v>
-      </c>
-      <c r="U50" s="21" t="n">
-        <v>4.15</v>
       </c>
     </row>
     <row r="51" ht="31.5" customHeight="1">
@@ -4536,7 +4536,7 @@
           <t>BOPSTB</t>
         </is>
       </c>
-      <c r="C51" s="49" t="n">
+      <c r="C51" s="48" t="n">
         <v>45901</v>
       </c>
       <c r="D51" s="6" t="inlineStr">
@@ -4575,7 +4575,7 @@
           <t>MORTGAGE30US</t>
         </is>
       </c>
-      <c r="N51" s="48" t="n">
+      <c r="N51" s="49" t="n">
         <v>46013</v>
       </c>
       <c r="O51" s="6" t="inlineStr">
@@ -4627,7 +4627,7 @@
         </is>
       </c>
       <c r="N52" s="53" t="n">
-        <v>46014</v>
+        <v>46017</v>
       </c>
       <c r="O52" s="9" t="inlineStr">
         <is>
@@ -4640,19 +4640,19 @@
         </is>
       </c>
       <c r="Q52" s="9" t="n">
-        <v>5.92</v>
+        <v>5.89</v>
       </c>
       <c r="R52" s="9" t="n">
-        <v>5.93</v>
+        <v>5.88</v>
       </c>
       <c r="S52" s="9" t="n">
         <v>5.92</v>
       </c>
       <c r="T52" s="9" t="n">
-        <v>5.9</v>
+        <v>5.93</v>
       </c>
       <c r="U52" s="22" t="n">
-        <v>5.94</v>
+        <v>5.92</v>
       </c>
     </row>
     <row r="53" ht="21" customHeight="1">

</xml_diff>

<commit_message>
Update dashboards - 2025-12-31
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -1213,7 +1213,7 @@
           <t>GDPNOW</t>
         </is>
       </c>
-      <c r="C7" s="49" t="n">
+      <c r="C7" s="48" t="n">
         <v>45931</v>
       </c>
       <c r="D7" s="6" t="inlineStr">
@@ -1292,8 +1292,8 @@
           <t>RECPROUSM156N</t>
         </is>
       </c>
-      <c r="C8" s="48" t="n">
-        <v>45870</v>
+      <c r="C8" s="49" t="n">
+        <v>45962</v>
       </c>
       <c r="D8" s="6" t="inlineStr">
         <is>
@@ -1306,19 +1306,19 @@
         </is>
       </c>
       <c r="F8" s="24" t="n">
-        <v>0.96</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="G8" s="24" t="n">
-        <v>0.64</v>
+        <v>0.9</v>
       </c>
       <c r="H8" s="24" t="n">
-        <v>0.34</v>
+        <v>0.72</v>
       </c>
       <c r="I8" s="24" t="n">
-        <v>0.42</v>
+        <v>0.7</v>
       </c>
       <c r="J8" s="24" t="n">
-        <v>0.24</v>
+        <v>0.32</v>
       </c>
       <c r="K8" s="5" t="n"/>
       <c r="L8" s="28" t="inlineStr">
@@ -1719,7 +1719,7 @@
         </is>
       </c>
       <c r="N13" s="49" t="n">
-        <v>46006</v>
+        <v>46013</v>
       </c>
       <c r="O13" s="6" t="inlineStr">
         <is>
@@ -1732,19 +1732,19 @@
         </is>
       </c>
       <c r="Q13" s="24" t="n">
-        <v>214000</v>
+        <v>199000</v>
       </c>
       <c r="R13" s="24" t="n">
+        <v>215000</v>
+      </c>
+      <c r="S13" s="24" t="n">
         <v>224000</v>
       </c>
-      <c r="S13" s="24" t="n">
+      <c r="T13" s="24" t="n">
         <v>237000</v>
       </c>
-      <c r="T13" s="24" t="n">
+      <c r="U13" s="26" t="n">
         <v>192000</v>
-      </c>
-      <c r="U13" s="26" t="n">
-        <v>217000</v>
       </c>
     </row>
     <row r="14">
@@ -1794,7 +1794,7 @@
         </is>
       </c>
       <c r="N14" s="49" t="n">
-        <v>45999</v>
+        <v>46006</v>
       </c>
       <c r="O14" s="6" t="inlineStr">
         <is>
@@ -1807,19 +1807,19 @@
         </is>
       </c>
       <c r="Q14" s="24" t="n">
-        <v>1923000</v>
+        <v>1866000</v>
       </c>
       <c r="R14" s="24" t="n">
+        <v>1913000</v>
+      </c>
+      <c r="S14" s="24" t="n">
         <v>1885000</v>
       </c>
-      <c r="S14" s="24" t="n">
+      <c r="T14" s="24" t="n">
         <v>1830000</v>
       </c>
-      <c r="T14" s="24" t="n">
+      <c r="U14" s="26" t="n">
         <v>1937000</v>
-      </c>
-      <c r="U14" s="26" t="n">
-        <v>1944000</v>
       </c>
     </row>
     <row r="15">
@@ -2922,7 +2922,7 @@
         </is>
       </c>
       <c r="N29" s="49" t="n">
-        <v>46020</v>
+        <v>46021</v>
       </c>
       <c r="O29" s="6" t="inlineStr">
         <is>
@@ -2935,10 +2935,10 @@
         </is>
       </c>
       <c r="Q29" s="6" t="n">
+        <v>2.23</v>
+      </c>
+      <c r="R29" s="6" t="n">
         <v>2.21</v>
-      </c>
-      <c r="R29" s="6" t="n">
-        <v>2.24</v>
       </c>
       <c r="S29" s="6" t="n">
         <v>2.24</v>
@@ -2947,7 +2947,7 @@
         <v>2.24</v>
       </c>
       <c r="U29" s="21" t="n">
-        <v>2.21</v>
+        <v>2.24</v>
       </c>
     </row>
     <row r="30">
@@ -3001,7 +3001,7 @@
         </is>
       </c>
       <c r="N30" s="49" t="n">
-        <v>46020</v>
+        <v>46021</v>
       </c>
       <c r="O30" s="6" t="inlineStr">
         <is>
@@ -3014,19 +3014,19 @@
         </is>
       </c>
       <c r="Q30" s="6" t="n">
+        <v>2.24</v>
+      </c>
+      <c r="R30" s="6" t="n">
         <v>2.22</v>
       </c>
-      <c r="R30" s="6" t="n">
+      <c r="S30" s="6" t="n">
         <v>2.23</v>
-      </c>
-      <c r="S30" s="6" t="n">
-        <v>2.24</v>
       </c>
       <c r="T30" s="6" t="n">
         <v>2.24</v>
       </c>
       <c r="U30" s="21" t="n">
-        <v>2.23</v>
+        <v>2.24</v>
       </c>
     </row>
     <row r="31">
@@ -4268,7 +4268,7 @@
         </is>
       </c>
       <c r="N47" s="49" t="n">
-        <v>46017</v>
+        <v>46020</v>
       </c>
       <c r="O47" s="6" t="inlineStr">
         <is>
@@ -4347,7 +4347,7 @@
         </is>
       </c>
       <c r="N48" s="49" t="n">
-        <v>46017</v>
+        <v>46020</v>
       </c>
       <c r="O48" s="6" t="inlineStr">
         <is>
@@ -4360,19 +4360,19 @@
         </is>
       </c>
       <c r="Q48" s="6" t="n">
+        <v>3.45</v>
+      </c>
+      <c r="R48" s="6" t="n">
         <v>3.46</v>
       </c>
-      <c r="R48" s="6" t="n">
+      <c r="S48" s="6" t="n">
         <v>3.47</v>
       </c>
-      <c r="S48" s="6" t="n">
+      <c r="T48" s="6" t="n">
         <v>3.48</v>
       </c>
-      <c r="T48" s="6" t="n">
+      <c r="U48" s="21" t="n">
         <v>3.44</v>
-      </c>
-      <c r="U48" s="21" t="n">
-        <v>3.48</v>
       </c>
     </row>
     <row r="49">
@@ -4422,7 +4422,7 @@
         </is>
       </c>
       <c r="N49" s="49" t="n">
-        <v>46017</v>
+        <v>46020</v>
       </c>
       <c r="O49" s="6" t="inlineStr">
         <is>
@@ -4435,19 +4435,19 @@
         </is>
       </c>
       <c r="Q49" s="6" t="n">
+        <v>3.67</v>
+      </c>
+      <c r="R49" s="6" t="n">
         <v>3.68</v>
       </c>
-      <c r="R49" s="6" t="n">
+      <c r="S49" s="6" t="n">
         <v>3.7</v>
       </c>
-      <c r="S49" s="6" t="n">
+      <c r="T49" s="6" t="n">
         <v>3.72</v>
       </c>
-      <c r="T49" s="6" t="n">
+      <c r="U49" s="21" t="n">
         <v>3.71</v>
-      </c>
-      <c r="U49" s="21" t="n">
-        <v>3.7</v>
       </c>
     </row>
     <row r="50">
@@ -4501,7 +4501,7 @@
         </is>
       </c>
       <c r="N50" s="49" t="n">
-        <v>46017</v>
+        <v>46020</v>
       </c>
       <c r="O50" s="6" t="inlineStr">
         <is>
@@ -4514,19 +4514,19 @@
         </is>
       </c>
       <c r="Q50" s="6" t="n">
+        <v>4.12</v>
+      </c>
+      <c r="R50" s="6" t="n">
         <v>4.14</v>
       </c>
-      <c r="R50" s="6" t="n">
+      <c r="S50" s="6" t="n">
         <v>4.15</v>
       </c>
-      <c r="S50" s="6" t="n">
+      <c r="T50" s="6" t="n">
         <v>4.18</v>
       </c>
-      <c r="T50" s="6" t="n">
+      <c r="U50" s="21" t="n">
         <v>4.17</v>
-      </c>
-      <c r="U50" s="21" t="n">
-        <v>4.16</v>
       </c>
     </row>
     <row r="51" ht="31.5" customHeight="1">
@@ -4575,7 +4575,7 @@
           <t>MORTGAGE30US</t>
         </is>
       </c>
-      <c r="N51" s="49" t="n">
+      <c r="N51" s="48" t="n">
         <v>46013</v>
       </c>
       <c r="O51" s="6" t="inlineStr">
@@ -4627,7 +4627,7 @@
         </is>
       </c>
       <c r="N52" s="53" t="n">
-        <v>46017</v>
+        <v>46020</v>
       </c>
       <c r="O52" s="9" t="inlineStr">
         <is>
@@ -4640,19 +4640,19 @@
         </is>
       </c>
       <c r="Q52" s="9" t="n">
+        <v>5.88</v>
+      </c>
+      <c r="R52" s="9" t="n">
         <v>5.89</v>
       </c>
-      <c r="R52" s="9" t="n">
+      <c r="S52" s="9" t="n">
         <v>5.88</v>
       </c>
-      <c r="S52" s="9" t="n">
+      <c r="T52" s="9" t="n">
         <v>5.92</v>
       </c>
-      <c r="T52" s="9" t="n">
+      <c r="U52" s="22" t="n">
         <v>5.93</v>
-      </c>
-      <c r="U52" s="22" t="n">
-        <v>5.92</v>
       </c>
     </row>
     <row r="53" ht="21" customHeight="1">

</xml_diff>

<commit_message>
Update dashboards - 2026-01-01
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -2922,7 +2922,7 @@
         </is>
       </c>
       <c r="N29" s="49" t="n">
-        <v>46021</v>
+        <v>46022</v>
       </c>
       <c r="O29" s="6" t="inlineStr">
         <is>
@@ -2935,13 +2935,13 @@
         </is>
       </c>
       <c r="Q29" s="6" t="n">
+        <v>2.24</v>
+      </c>
+      <c r="R29" s="6" t="n">
         <v>2.23</v>
       </c>
-      <c r="R29" s="6" t="n">
+      <c r="S29" s="6" t="n">
         <v>2.21</v>
-      </c>
-      <c r="S29" s="6" t="n">
-        <v>2.24</v>
       </c>
       <c r="T29" s="6" t="n">
         <v>2.24</v>
@@ -3001,7 +3001,7 @@
         </is>
       </c>
       <c r="N30" s="49" t="n">
-        <v>46021</v>
+        <v>46022</v>
       </c>
       <c r="O30" s="6" t="inlineStr">
         <is>
@@ -3014,16 +3014,16 @@
         </is>
       </c>
       <c r="Q30" s="6" t="n">
+        <v>2.25</v>
+      </c>
+      <c r="R30" s="6" t="n">
         <v>2.24</v>
       </c>
-      <c r="R30" s="6" t="n">
+      <c r="S30" s="6" t="n">
         <v>2.22</v>
       </c>
-      <c r="S30" s="6" t="n">
+      <c r="T30" s="6" t="n">
         <v>2.23</v>
-      </c>
-      <c r="T30" s="6" t="n">
-        <v>2.24</v>
       </c>
       <c r="U30" s="21" t="n">
         <v>2.24</v>
@@ -4268,7 +4268,7 @@
         </is>
       </c>
       <c r="N47" s="49" t="n">
-        <v>46020</v>
+        <v>46021</v>
       </c>
       <c r="O47" s="6" t="inlineStr">
         <is>
@@ -4347,7 +4347,7 @@
         </is>
       </c>
       <c r="N48" s="49" t="n">
-        <v>46020</v>
+        <v>46021</v>
       </c>
       <c r="O48" s="6" t="inlineStr">
         <is>
@@ -4363,16 +4363,16 @@
         <v>3.45</v>
       </c>
       <c r="R48" s="6" t="n">
+        <v>3.45</v>
+      </c>
+      <c r="S48" s="6" t="n">
         <v>3.46</v>
       </c>
-      <c r="S48" s="6" t="n">
+      <c r="T48" s="6" t="n">
         <v>3.47</v>
       </c>
-      <c r="T48" s="6" t="n">
+      <c r="U48" s="21" t="n">
         <v>3.48</v>
-      </c>
-      <c r="U48" s="21" t="n">
-        <v>3.44</v>
       </c>
     </row>
     <row r="49">
@@ -4422,7 +4422,7 @@
         </is>
       </c>
       <c r="N49" s="49" t="n">
-        <v>46020</v>
+        <v>46021</v>
       </c>
       <c r="O49" s="6" t="inlineStr">
         <is>
@@ -4435,19 +4435,19 @@
         </is>
       </c>
       <c r="Q49" s="6" t="n">
+        <v>3.68</v>
+      </c>
+      <c r="R49" s="6" t="n">
         <v>3.67</v>
       </c>
-      <c r="R49" s="6" t="n">
+      <c r="S49" s="6" t="n">
         <v>3.68</v>
       </c>
-      <c r="S49" s="6" t="n">
+      <c r="T49" s="6" t="n">
         <v>3.7</v>
       </c>
-      <c r="T49" s="6" t="n">
+      <c r="U49" s="21" t="n">
         <v>3.72</v>
-      </c>
-      <c r="U49" s="21" t="n">
-        <v>3.71</v>
       </c>
     </row>
     <row r="50">
@@ -4501,7 +4501,7 @@
         </is>
       </c>
       <c r="N50" s="49" t="n">
-        <v>46020</v>
+        <v>46021</v>
       </c>
       <c r="O50" s="6" t="inlineStr">
         <is>
@@ -4514,19 +4514,19 @@
         </is>
       </c>
       <c r="Q50" s="6" t="n">
+        <v>4.14</v>
+      </c>
+      <c r="R50" s="6" t="n">
         <v>4.12</v>
       </c>
-      <c r="R50" s="6" t="n">
+      <c r="S50" s="6" t="n">
         <v>4.14</v>
       </c>
-      <c r="S50" s="6" t="n">
+      <c r="T50" s="6" t="n">
         <v>4.15</v>
       </c>
-      <c r="T50" s="6" t="n">
+      <c r="U50" s="21" t="n">
         <v>4.18</v>
-      </c>
-      <c r="U50" s="21" t="n">
-        <v>4.17</v>
       </c>
     </row>
     <row r="51" ht="31.5" customHeight="1">
@@ -4575,8 +4575,8 @@
           <t>MORTGAGE30US</t>
         </is>
       </c>
-      <c r="N51" s="48" t="n">
-        <v>46013</v>
+      <c r="N51" s="49" t="n">
+        <v>46020</v>
       </c>
       <c r="O51" s="6" t="inlineStr">
         <is>
@@ -4589,19 +4589,19 @@
         </is>
       </c>
       <c r="Q51" s="6" t="n">
+        <v>6.15</v>
+      </c>
+      <c r="R51" s="6" t="n">
         <v>6.18</v>
       </c>
-      <c r="R51" s="6" t="n">
+      <c r="S51" s="6" t="n">
         <v>6.21</v>
       </c>
-      <c r="S51" s="6" t="n">
+      <c r="T51" s="6" t="n">
         <v>6.22</v>
       </c>
-      <c r="T51" s="6" t="n">
+      <c r="U51" s="21" t="n">
         <v>6.19</v>
-      </c>
-      <c r="U51" s="21" t="n">
-        <v>6.23</v>
       </c>
     </row>
     <row r="52" ht="16.15" customHeight="1" thickBot="1">
@@ -4627,7 +4627,7 @@
         </is>
       </c>
       <c r="N52" s="53" t="n">
-        <v>46020</v>
+        <v>46021</v>
       </c>
       <c r="O52" s="9" t="inlineStr">
         <is>
@@ -4640,19 +4640,19 @@
         </is>
       </c>
       <c r="Q52" s="9" t="n">
+        <v>5.89</v>
+      </c>
+      <c r="R52" s="9" t="n">
         <v>5.88</v>
       </c>
-      <c r="R52" s="9" t="n">
+      <c r="S52" s="9" t="n">
         <v>5.89</v>
       </c>
-      <c r="S52" s="9" t="n">
+      <c r="T52" s="9" t="n">
         <v>5.88</v>
       </c>
-      <c r="T52" s="9" t="n">
+      <c r="U52" s="22" t="n">
         <v>5.92</v>
-      </c>
-      <c r="U52" s="22" t="n">
-        <v>5.93</v>
       </c>
     </row>
     <row r="53" ht="21" customHeight="1">

</xml_diff>

<commit_message>
Update dashboards - 2026-01-03
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -2922,7 +2922,7 @@
         </is>
       </c>
       <c r="N29" s="49" t="n">
-        <v>46022</v>
+        <v>46024</v>
       </c>
       <c r="O29" s="6" t="inlineStr">
         <is>
@@ -2935,16 +2935,16 @@
         </is>
       </c>
       <c r="Q29" s="6" t="n">
+        <v>2.22</v>
+      </c>
+      <c r="R29" s="6" t="n">
         <v>2.24</v>
       </c>
-      <c r="R29" s="6" t="n">
+      <c r="S29" s="6" t="n">
         <v>2.23</v>
       </c>
-      <c r="S29" s="6" t="n">
+      <c r="T29" s="6" t="n">
         <v>2.21</v>
-      </c>
-      <c r="T29" s="6" t="n">
-        <v>2.24</v>
       </c>
       <c r="U29" s="21" t="n">
         <v>2.24</v>
@@ -3001,7 +3001,7 @@
         </is>
       </c>
       <c r="N30" s="49" t="n">
-        <v>46022</v>
+        <v>46024</v>
       </c>
       <c r="O30" s="6" t="inlineStr">
         <is>
@@ -3017,16 +3017,16 @@
         <v>2.25</v>
       </c>
       <c r="R30" s="6" t="n">
+        <v>2.25</v>
+      </c>
+      <c r="S30" s="6" t="n">
         <v>2.24</v>
       </c>
-      <c r="S30" s="6" t="n">
+      <c r="T30" s="6" t="n">
         <v>2.22</v>
       </c>
-      <c r="T30" s="6" t="n">
+      <c r="U30" s="21" t="n">
         <v>2.23</v>
-      </c>
-      <c r="U30" s="21" t="n">
-        <v>2.24</v>
       </c>
     </row>
     <row r="31">
@@ -4268,7 +4268,7 @@
         </is>
       </c>
       <c r="N47" s="49" t="n">
-        <v>46021</v>
+        <v>46023</v>
       </c>
       <c r="O47" s="6" t="inlineStr">
         <is>
@@ -4347,7 +4347,7 @@
         </is>
       </c>
       <c r="N48" s="49" t="n">
-        <v>46021</v>
+        <v>46022</v>
       </c>
       <c r="O48" s="6" t="inlineStr">
         <is>
@@ -4360,19 +4360,19 @@
         </is>
       </c>
       <c r="Q48" s="6" t="n">
-        <v>3.45</v>
+        <v>3.47</v>
       </c>
       <c r="R48" s="6" t="n">
         <v>3.45</v>
       </c>
       <c r="S48" s="6" t="n">
+        <v>3.45</v>
+      </c>
+      <c r="T48" s="6" t="n">
         <v>3.46</v>
       </c>
-      <c r="T48" s="6" t="n">
+      <c r="U48" s="21" t="n">
         <v>3.47</v>
-      </c>
-      <c r="U48" s="21" t="n">
-        <v>3.48</v>
       </c>
     </row>
     <row r="49">
@@ -4422,7 +4422,7 @@
         </is>
       </c>
       <c r="N49" s="49" t="n">
-        <v>46021</v>
+        <v>46022</v>
       </c>
       <c r="O49" s="6" t="inlineStr">
         <is>
@@ -4435,19 +4435,19 @@
         </is>
       </c>
       <c r="Q49" s="6" t="n">
+        <v>3.73</v>
+      </c>
+      <c r="R49" s="6" t="n">
         <v>3.68</v>
       </c>
-      <c r="R49" s="6" t="n">
+      <c r="S49" s="6" t="n">
         <v>3.67</v>
       </c>
-      <c r="S49" s="6" t="n">
+      <c r="T49" s="6" t="n">
         <v>3.68</v>
       </c>
-      <c r="T49" s="6" t="n">
+      <c r="U49" s="21" t="n">
         <v>3.7</v>
-      </c>
-      <c r="U49" s="21" t="n">
-        <v>3.72</v>
       </c>
     </row>
     <row r="50">
@@ -4501,7 +4501,7 @@
         </is>
       </c>
       <c r="N50" s="49" t="n">
-        <v>46021</v>
+        <v>46022</v>
       </c>
       <c r="O50" s="6" t="inlineStr">
         <is>
@@ -4514,19 +4514,19 @@
         </is>
       </c>
       <c r="Q50" s="6" t="n">
+        <v>4.18</v>
+      </c>
+      <c r="R50" s="6" t="n">
         <v>4.14</v>
       </c>
-      <c r="R50" s="6" t="n">
+      <c r="S50" s="6" t="n">
         <v>4.12</v>
       </c>
-      <c r="S50" s="6" t="n">
+      <c r="T50" s="6" t="n">
         <v>4.14</v>
       </c>
-      <c r="T50" s="6" t="n">
+      <c r="U50" s="21" t="n">
         <v>4.15</v>
-      </c>
-      <c r="U50" s="21" t="n">
-        <v>4.18</v>
       </c>
     </row>
     <row r="51" ht="31.5" customHeight="1">

</xml_diff>

<commit_message>
Update dashboards - 2026-01-05
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -77,14 +77,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FFFF00"/>
-        <bgColor rgb="00FFFF00"/>
+        <fgColor rgb="00CCFFCC"/>
+        <bgColor rgb="00CCFFCC"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00CCFFCC"/>
-        <bgColor rgb="00CCFFCC"/>
+        <fgColor rgb="00FFFF00"/>
+        <bgColor rgb="00FFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -363,19 +363,19 @@
     <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="1" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="4" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="1" fillId="3" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="168" fontId="1" fillId="4" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1059,7 +1059,7 @@
           <t>NGDPSAXDCUSQ</t>
         </is>
       </c>
-      <c r="C5" s="49" t="n">
+      <c r="C5" s="48" t="n">
         <v>45839</v>
       </c>
       <c r="D5" s="6" t="inlineStr">
@@ -1120,10 +1120,10 @@
       <c r="S5" s="24" t="n">
         <v>-29000</v>
       </c>
-      <c r="T5" s="50" t="n">
+      <c r="T5" s="49" t="n">
         <v>-3000</v>
       </c>
-      <c r="U5" s="51" t="n">
+      <c r="U5" s="50" t="n">
         <v>104000</v>
       </c>
     </row>
@@ -1134,7 +1134,7 @@
           <t>NGDPSAXDCUSQ</t>
         </is>
       </c>
-      <c r="C6" s="49" t="n">
+      <c r="C6" s="48" t="n">
         <v>45839</v>
       </c>
       <c r="D6" s="6" t="inlineStr">
@@ -1198,7 +1198,7 @@
       <c r="T6" s="6" t="n">
         <v>4.3</v>
       </c>
-      <c r="U6" s="52" t="n">
+      <c r="U6" s="51" t="n">
         <v>4.2</v>
       </c>
     </row>
@@ -1277,7 +1277,7 @@
       <c r="T7" s="6" t="n">
         <v>8.1</v>
       </c>
-      <c r="U7" s="52" t="n">
+      <c r="U7" s="51" t="n">
         <v>7.9</v>
       </c>
     </row>
@@ -1292,7 +1292,7 @@
           <t>RECPROUSM156N</t>
         </is>
       </c>
-      <c r="C8" s="49" t="n">
+      <c r="C8" s="48" t="n">
         <v>45962</v>
       </c>
       <c r="D8" s="6" t="inlineStr">
@@ -1356,7 +1356,7 @@
       <c r="T8" s="6" t="n">
         <v>62.3</v>
       </c>
-      <c r="U8" s="52" t="n">
+      <c r="U8" s="51" t="n">
         <v>62.2</v>
       </c>
     </row>
@@ -1435,7 +1435,7 @@
       <c r="T9" s="6" t="n">
         <v>59.6</v>
       </c>
-      <c r="U9" s="52" t="n">
+      <c r="U9" s="51" t="n">
         <v>59.6</v>
       </c>
     </row>
@@ -1718,7 +1718,7 @@
           <t>ICSA</t>
         </is>
       </c>
-      <c r="N13" s="49" t="n">
+      <c r="N13" s="52" t="n">
         <v>46013</v>
       </c>
       <c r="O13" s="6" t="inlineStr">
@@ -1793,7 +1793,7 @@
           <t>CCSA</t>
         </is>
       </c>
-      <c r="N14" s="49" t="n">
+      <c r="N14" s="52" t="n">
         <v>46006</v>
       </c>
       <c r="O14" s="6" t="inlineStr">
@@ -2871,7 +2871,7 @@
       <c r="T28" s="6" t="n">
         <v>4.8</v>
       </c>
-      <c r="U28" s="52" t="n">
+      <c r="U28" s="51" t="n">
         <v>4.5</v>
       </c>
     </row>
@@ -2921,7 +2921,7 @@
           <t>T5YIFR</t>
         </is>
       </c>
-      <c r="N29" s="49" t="n">
+      <c r="N29" s="52" t="n">
         <v>46024</v>
       </c>
       <c r="O29" s="6" t="inlineStr">
@@ -3000,7 +3000,7 @@
           <t>T10YIE</t>
         </is>
       </c>
-      <c r="N30" s="49" t="n">
+      <c r="N30" s="52" t="n">
         <v>46024</v>
       </c>
       <c r="O30" s="6" t="inlineStr">
@@ -3529,7 +3529,7 @@
           <t>CSUSHPINSA</t>
         </is>
       </c>
-      <c r="N37" s="49" t="n">
+      <c r="N37" s="52" t="n">
         <v>45931</v>
       </c>
       <c r="O37" s="6" t="inlineStr">
@@ -3604,7 +3604,7 @@
           <t>CSUSHPINSA</t>
         </is>
       </c>
-      <c r="N38" s="49" t="n">
+      <c r="N38" s="52" t="n">
         <v>45931</v>
       </c>
       <c r="O38" s="6" t="inlineStr">
@@ -4267,7 +4267,7 @@
           <t>DFF</t>
         </is>
       </c>
-      <c r="N47" s="49" t="n">
+      <c r="N47" s="52" t="n">
         <v>46023</v>
       </c>
       <c r="O47" s="6" t="inlineStr">
@@ -4346,7 +4346,7 @@
           <t>DGS2</t>
         </is>
       </c>
-      <c r="N48" s="49" t="n">
+      <c r="N48" s="52" t="n">
         <v>46022</v>
       </c>
       <c r="O48" s="6" t="inlineStr">
@@ -4421,7 +4421,7 @@
           <t>DGS5</t>
         </is>
       </c>
-      <c r="N49" s="49" t="n">
+      <c r="N49" s="52" t="n">
         <v>46022</v>
       </c>
       <c r="O49" s="6" t="inlineStr">
@@ -4500,7 +4500,7 @@
           <t>DGS10</t>
         </is>
       </c>
-      <c r="N50" s="49" t="n">
+      <c r="N50" s="52" t="n">
         <v>46022</v>
       </c>
       <c r="O50" s="6" t="inlineStr">
@@ -4575,7 +4575,7 @@
           <t>MORTGAGE30US</t>
         </is>
       </c>
-      <c r="N51" s="49" t="n">
+      <c r="N51" s="52" t="n">
         <v>46020</v>
       </c>
       <c r="O51" s="6" t="inlineStr">

</xml_diff>

<commit_message>
Update dashboards - 2026-01-06
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -363,17 +363,17 @@
     <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="1" fillId="3" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="168" fontId="1" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="168" fontId="1" fillId="4" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
@@ -1120,10 +1120,10 @@
       <c r="S5" s="24" t="n">
         <v>-29000</v>
       </c>
-      <c r="T5" s="49" t="n">
+      <c r="T5" s="24" t="n">
         <v>-3000</v>
       </c>
-      <c r="U5" s="50" t="n">
+      <c r="U5" s="49" t="n">
         <v>104000</v>
       </c>
     </row>
@@ -1198,7 +1198,7 @@
       <c r="T6" s="6" t="n">
         <v>4.3</v>
       </c>
-      <c r="U6" s="51" t="n">
+      <c r="U6" s="21" t="n">
         <v>4.2</v>
       </c>
     </row>
@@ -1227,7 +1227,7 @@
         </is>
       </c>
       <c r="F7" s="44" t="n">
-        <v>2.9721</v>
+        <v>2.6786</v>
       </c>
       <c r="G7" s="44" t="n">
         <v>3.4728</v>
@@ -1277,7 +1277,7 @@
       <c r="T7" s="6" t="n">
         <v>8.1</v>
       </c>
-      <c r="U7" s="51" t="n">
+      <c r="U7" s="21" t="n">
         <v>7.9</v>
       </c>
     </row>
@@ -1356,7 +1356,7 @@
       <c r="T8" s="6" t="n">
         <v>62.3</v>
       </c>
-      <c r="U8" s="51" t="n">
+      <c r="U8" s="21" t="n">
         <v>62.2</v>
       </c>
     </row>
@@ -1435,7 +1435,7 @@
       <c r="T9" s="6" t="n">
         <v>59.6</v>
       </c>
-      <c r="U9" s="51" t="n">
+      <c r="U9" s="21" t="n">
         <v>59.6</v>
       </c>
     </row>
@@ -1718,7 +1718,7 @@
           <t>ICSA</t>
         </is>
       </c>
-      <c r="N13" s="52" t="n">
+      <c r="N13" s="50" t="n">
         <v>46013</v>
       </c>
       <c r="O13" s="6" t="inlineStr">
@@ -1793,7 +1793,7 @@
           <t>CCSA</t>
         </is>
       </c>
-      <c r="N14" s="52" t="n">
+      <c r="N14" s="50" t="n">
         <v>46006</v>
       </c>
       <c r="O14" s="6" t="inlineStr">
@@ -2871,7 +2871,7 @@
       <c r="T28" s="6" t="n">
         <v>4.8</v>
       </c>
-      <c r="U28" s="51" t="n">
+      <c r="U28" s="21" t="n">
         <v>4.5</v>
       </c>
     </row>
@@ -2921,8 +2921,8 @@
           <t>T5YIFR</t>
         </is>
       </c>
-      <c r="N29" s="52" t="n">
-        <v>46024</v>
+      <c r="N29" s="50" t="n">
+        <v>46027</v>
       </c>
       <c r="O29" s="6" t="inlineStr">
         <is>
@@ -2935,19 +2935,19 @@
         </is>
       </c>
       <c r="Q29" s="6" t="n">
+        <v>2.23</v>
+      </c>
+      <c r="R29" s="6" t="n">
         <v>2.22</v>
       </c>
-      <c r="R29" s="6" t="n">
+      <c r="S29" s="6" t="n">
         <v>2.24</v>
       </c>
-      <c r="S29" s="6" t="n">
+      <c r="T29" s="6" t="n">
         <v>2.23</v>
       </c>
-      <c r="T29" s="6" t="n">
+      <c r="U29" s="21" t="n">
         <v>2.21</v>
-      </c>
-      <c r="U29" s="21" t="n">
-        <v>2.24</v>
       </c>
     </row>
     <row r="30">
@@ -3000,8 +3000,8 @@
           <t>T10YIE</t>
         </is>
       </c>
-      <c r="N30" s="52" t="n">
-        <v>46024</v>
+      <c r="N30" s="50" t="n">
+        <v>46027</v>
       </c>
       <c r="O30" s="6" t="inlineStr">
         <is>
@@ -3014,19 +3014,19 @@
         </is>
       </c>
       <c r="Q30" s="6" t="n">
-        <v>2.25</v>
+        <v>2.26</v>
       </c>
       <c r="R30" s="6" t="n">
         <v>2.25</v>
       </c>
       <c r="S30" s="6" t="n">
+        <v>2.25</v>
+      </c>
+      <c r="T30" s="6" t="n">
         <v>2.24</v>
       </c>
-      <c r="T30" s="6" t="n">
+      <c r="U30" s="21" t="n">
         <v>2.22</v>
-      </c>
-      <c r="U30" s="21" t="n">
-        <v>2.23</v>
       </c>
     </row>
     <row r="31">
@@ -3529,7 +3529,7 @@
           <t>CSUSHPINSA</t>
         </is>
       </c>
-      <c r="N37" s="52" t="n">
+      <c r="N37" s="48" t="n">
         <v>45931</v>
       </c>
       <c r="O37" s="6" t="inlineStr">
@@ -3604,7 +3604,7 @@
           <t>CSUSHPINSA</t>
         </is>
       </c>
-      <c r="N38" s="52" t="n">
+      <c r="N38" s="48" t="n">
         <v>45931</v>
       </c>
       <c r="O38" s="6" t="inlineStr">
@@ -3679,8 +3679,8 @@
           <t>TWEXBGSMTH</t>
         </is>
       </c>
-      <c r="N39" s="48" t="n">
-        <v>45962</v>
+      <c r="N39" s="50" t="n">
+        <v>45992</v>
       </c>
       <c r="O39" s="6" t="inlineStr">
         <is>
@@ -3693,19 +3693,19 @@
         </is>
       </c>
       <c r="Q39" s="6" t="n">
+        <v>120.5723</v>
+      </c>
+      <c r="R39" s="51" t="n">
         <v>121.8038</v>
       </c>
-      <c r="R39" s="6" t="n">
+      <c r="S39" s="6" t="n">
         <v>121.1712</v>
       </c>
-      <c r="S39" s="6" t="n">
+      <c r="T39" s="6" t="n">
         <v>120.4534</v>
       </c>
-      <c r="T39" s="6" t="n">
+      <c r="U39" s="21" t="n">
         <v>120.9844</v>
-      </c>
-      <c r="U39" s="21" t="n">
-        <v>120.5266</v>
       </c>
     </row>
     <row r="40" ht="31.5" customHeight="1">
@@ -3754,8 +3754,8 @@
           <t>TWEXBGSMTH</t>
         </is>
       </c>
-      <c r="N40" s="48" t="n">
-        <v>45962</v>
+      <c r="N40" s="50" t="n">
+        <v>45992</v>
       </c>
       <c r="O40" s="6" t="inlineStr">
         <is>
@@ -3768,19 +3768,19 @@
         </is>
       </c>
       <c r="Q40" s="38" t="n">
+        <v>-0.05665811256982799</v>
+      </c>
+      <c r="R40" s="52" t="n">
         <v>-0.03737446940677091</v>
       </c>
-      <c r="R40" s="38" t="n">
+      <c r="S40" s="38" t="n">
         <v>-0.02147927417205711</v>
       </c>
-      <c r="S40" s="38" t="n">
+      <c r="T40" s="38" t="n">
         <v>-0.0137247645124523</v>
       </c>
-      <c r="T40" s="38" t="n">
+      <c r="U40" s="23" t="n">
         <v>-0.0154280347850997</v>
-      </c>
-      <c r="U40" s="23" t="n">
-        <v>-0.02581780913152837</v>
       </c>
     </row>
     <row r="41">
@@ -4267,8 +4267,8 @@
           <t>DFF</t>
         </is>
       </c>
-      <c r="N47" s="52" t="n">
-        <v>46023</v>
+      <c r="N47" s="50" t="n">
+        <v>46024</v>
       </c>
       <c r="O47" s="6" t="inlineStr">
         <is>
@@ -4346,8 +4346,8 @@
           <t>DGS2</t>
         </is>
       </c>
-      <c r="N48" s="52" t="n">
-        <v>46022</v>
+      <c r="N48" s="50" t="n">
+        <v>46024</v>
       </c>
       <c r="O48" s="6" t="inlineStr">
         <is>
@@ -4363,16 +4363,16 @@
         <v>3.47</v>
       </c>
       <c r="R48" s="6" t="n">
-        <v>3.45</v>
+        <v>3.47</v>
       </c>
       <c r="S48" s="6" t="n">
         <v>3.45</v>
       </c>
       <c r="T48" s="6" t="n">
+        <v>3.45</v>
+      </c>
+      <c r="U48" s="21" t="n">
         <v>3.46</v>
-      </c>
-      <c r="U48" s="21" t="n">
-        <v>3.47</v>
       </c>
     </row>
     <row r="49">
@@ -4421,8 +4421,8 @@
           <t>DGS5</t>
         </is>
       </c>
-      <c r="N49" s="52" t="n">
-        <v>46022</v>
+      <c r="N49" s="50" t="n">
+        <v>46024</v>
       </c>
       <c r="O49" s="6" t="inlineStr">
         <is>
@@ -4435,19 +4435,19 @@
         </is>
       </c>
       <c r="Q49" s="6" t="n">
+        <v>3.74</v>
+      </c>
+      <c r="R49" s="6" t="n">
         <v>3.73</v>
       </c>
-      <c r="R49" s="6" t="n">
+      <c r="S49" s="6" t="n">
         <v>3.68</v>
       </c>
-      <c r="S49" s="6" t="n">
+      <c r="T49" s="6" t="n">
         <v>3.67</v>
       </c>
-      <c r="T49" s="6" t="n">
+      <c r="U49" s="21" t="n">
         <v>3.68</v>
-      </c>
-      <c r="U49" s="21" t="n">
-        <v>3.7</v>
       </c>
     </row>
     <row r="50">
@@ -4500,8 +4500,8 @@
           <t>DGS10</t>
         </is>
       </c>
-      <c r="N50" s="52" t="n">
-        <v>46022</v>
+      <c r="N50" s="50" t="n">
+        <v>46024</v>
       </c>
       <c r="O50" s="6" t="inlineStr">
         <is>
@@ -4514,19 +4514,19 @@
         </is>
       </c>
       <c r="Q50" s="6" t="n">
+        <v>4.19</v>
+      </c>
+      <c r="R50" s="6" t="n">
         <v>4.18</v>
       </c>
-      <c r="R50" s="6" t="n">
+      <c r="S50" s="6" t="n">
         <v>4.14</v>
       </c>
-      <c r="S50" s="6" t="n">
+      <c r="T50" s="6" t="n">
         <v>4.12</v>
       </c>
-      <c r="T50" s="6" t="n">
+      <c r="U50" s="21" t="n">
         <v>4.14</v>
-      </c>
-      <c r="U50" s="21" t="n">
-        <v>4.15</v>
       </c>
     </row>
     <row r="51" ht="31.5" customHeight="1">
@@ -4575,7 +4575,7 @@
           <t>MORTGAGE30US</t>
         </is>
       </c>
-      <c r="N51" s="52" t="n">
+      <c r="N51" s="50" t="n">
         <v>46020</v>
       </c>
       <c r="O51" s="6" t="inlineStr">
@@ -4627,7 +4627,7 @@
         </is>
       </c>
       <c r="N52" s="53" t="n">
-        <v>46021</v>
+        <v>46024</v>
       </c>
       <c r="O52" s="9" t="inlineStr">
         <is>
@@ -4640,10 +4640,10 @@
         </is>
       </c>
       <c r="Q52" s="9" t="n">
-        <v>5.89</v>
+        <v>5.93</v>
       </c>
       <c r="R52" s="9" t="n">
-        <v>5.88</v>
+        <v>5.9</v>
       </c>
       <c r="S52" s="9" t="n">
         <v>5.89</v>
@@ -4652,7 +4652,7 @@
         <v>5.88</v>
       </c>
       <c r="U52" s="22" t="n">
-        <v>5.92</v>
+        <v>5.89</v>
       </c>
     </row>
     <row r="53" ht="21" customHeight="1">

</xml_diff>

<commit_message>
Update dashboards - 2026-01-07
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -77,14 +77,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00CCFFCC"/>
-        <bgColor rgb="00CCFFCC"/>
+        <fgColor rgb="00FFFF00"/>
+        <bgColor rgb="00FFFF00"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FFFF00"/>
-        <bgColor rgb="00FFFF00"/>
+        <fgColor rgb="00CCFFCC"/>
+        <bgColor rgb="00CCFFCC"/>
       </patternFill>
     </fill>
   </fills>
@@ -363,19 +363,19 @@
     <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="3" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+    <xf numFmtId="168" fontId="1" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="4" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="168" fontId="1" fillId="3" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1098,8 +1098,8 @@
           <t>ADPMNUSNERSA</t>
         </is>
       </c>
-      <c r="N5" s="48" t="n">
-        <v>45962</v>
+      <c r="N5" s="49" t="n">
+        <v>45992</v>
       </c>
       <c r="O5" s="6" t="inlineStr">
         <is>
@@ -1112,19 +1112,19 @@
         </is>
       </c>
       <c r="Q5" s="24" t="n">
-        <v>-32000</v>
+        <v>41000</v>
       </c>
       <c r="R5" s="24" t="n">
+        <v>-29000</v>
+      </c>
+      <c r="S5" s="24" t="n">
         <v>47000</v>
       </c>
-      <c r="S5" s="24" t="n">
+      <c r="T5" s="24" t="n">
         <v>-29000</v>
       </c>
-      <c r="T5" s="24" t="n">
+      <c r="U5" s="50" t="n">
         <v>-3000</v>
-      </c>
-      <c r="U5" s="49" t="n">
-        <v>104000</v>
       </c>
     </row>
     <row r="6">
@@ -1718,7 +1718,7 @@
           <t>ICSA</t>
         </is>
       </c>
-      <c r="N13" s="50" t="n">
+      <c r="N13" s="48" t="n">
         <v>46013</v>
       </c>
       <c r="O13" s="6" t="inlineStr">
@@ -1793,7 +1793,7 @@
           <t>CCSA</t>
         </is>
       </c>
-      <c r="N14" s="50" t="n">
+      <c r="N14" s="48" t="n">
         <v>46006</v>
       </c>
       <c r="O14" s="6" t="inlineStr">
@@ -2921,8 +2921,8 @@
           <t>T5YIFR</t>
         </is>
       </c>
-      <c r="N29" s="50" t="n">
-        <v>46027</v>
+      <c r="N29" s="49" t="n">
+        <v>46028</v>
       </c>
       <c r="O29" s="6" t="inlineStr">
         <is>
@@ -2935,19 +2935,19 @@
         </is>
       </c>
       <c r="Q29" s="6" t="n">
+        <v>2.24</v>
+      </c>
+      <c r="R29" s="6" t="n">
         <v>2.23</v>
       </c>
-      <c r="R29" s="6" t="n">
+      <c r="S29" s="6" t="n">
         <v>2.22</v>
       </c>
-      <c r="S29" s="6" t="n">
+      <c r="T29" s="6" t="n">
         <v>2.24</v>
       </c>
-      <c r="T29" s="6" t="n">
+      <c r="U29" s="21" t="n">
         <v>2.23</v>
-      </c>
-      <c r="U29" s="21" t="n">
-        <v>2.21</v>
       </c>
     </row>
     <row r="30">
@@ -3000,8 +3000,8 @@
           <t>T10YIE</t>
         </is>
       </c>
-      <c r="N30" s="50" t="n">
-        <v>46027</v>
+      <c r="N30" s="49" t="n">
+        <v>46028</v>
       </c>
       <c r="O30" s="6" t="inlineStr">
         <is>
@@ -3014,19 +3014,19 @@
         </is>
       </c>
       <c r="Q30" s="6" t="n">
+        <v>2.27</v>
+      </c>
+      <c r="R30" s="6" t="n">
         <v>2.26</v>
-      </c>
-      <c r="R30" s="6" t="n">
-        <v>2.25</v>
       </c>
       <c r="S30" s="6" t="n">
         <v>2.25</v>
       </c>
       <c r="T30" s="6" t="n">
+        <v>2.25</v>
+      </c>
+      <c r="U30" s="21" t="n">
         <v>2.24</v>
-      </c>
-      <c r="U30" s="21" t="n">
-        <v>2.22</v>
       </c>
     </row>
     <row r="31">
@@ -3679,7 +3679,7 @@
           <t>TWEXBGSMTH</t>
         </is>
       </c>
-      <c r="N39" s="50" t="n">
+      <c r="N39" s="49" t="n">
         <v>45992</v>
       </c>
       <c r="O39" s="6" t="inlineStr">
@@ -3754,7 +3754,7 @@
           <t>TWEXBGSMTH</t>
         </is>
       </c>
-      <c r="N40" s="50" t="n">
+      <c r="N40" s="49" t="n">
         <v>45992</v>
       </c>
       <c r="O40" s="6" t="inlineStr">
@@ -4267,8 +4267,8 @@
           <t>DFF</t>
         </is>
       </c>
-      <c r="N47" s="50" t="n">
-        <v>46024</v>
+      <c r="N47" s="49" t="n">
+        <v>46027</v>
       </c>
       <c r="O47" s="6" t="inlineStr">
         <is>
@@ -4346,8 +4346,8 @@
           <t>DGS2</t>
         </is>
       </c>
-      <c r="N48" s="50" t="n">
-        <v>46024</v>
+      <c r="N48" s="49" t="n">
+        <v>46027</v>
       </c>
       <c r="O48" s="6" t="inlineStr">
         <is>
@@ -4360,19 +4360,19 @@
         </is>
       </c>
       <c r="Q48" s="6" t="n">
-        <v>3.47</v>
+        <v>3.46</v>
       </c>
       <c r="R48" s="6" t="n">
         <v>3.47</v>
       </c>
       <c r="S48" s="6" t="n">
-        <v>3.45</v>
+        <v>3.47</v>
       </c>
       <c r="T48" s="6" t="n">
         <v>3.45</v>
       </c>
       <c r="U48" s="21" t="n">
-        <v>3.46</v>
+        <v>3.45</v>
       </c>
     </row>
     <row r="49">
@@ -4421,8 +4421,8 @@
           <t>DGS5</t>
         </is>
       </c>
-      <c r="N49" s="50" t="n">
-        <v>46024</v>
+      <c r="N49" s="49" t="n">
+        <v>46027</v>
       </c>
       <c r="O49" s="6" t="inlineStr">
         <is>
@@ -4435,19 +4435,19 @@
         </is>
       </c>
       <c r="Q49" s="6" t="n">
+        <v>3.71</v>
+      </c>
+      <c r="R49" s="6" t="n">
         <v>3.74</v>
       </c>
-      <c r="R49" s="6" t="n">
+      <c r="S49" s="6" t="n">
         <v>3.73</v>
       </c>
-      <c r="S49" s="6" t="n">
+      <c r="T49" s="6" t="n">
         <v>3.68</v>
       </c>
-      <c r="T49" s="6" t="n">
+      <c r="U49" s="21" t="n">
         <v>3.67</v>
-      </c>
-      <c r="U49" s="21" t="n">
-        <v>3.68</v>
       </c>
     </row>
     <row r="50">
@@ -4500,8 +4500,8 @@
           <t>DGS10</t>
         </is>
       </c>
-      <c r="N50" s="50" t="n">
-        <v>46024</v>
+      <c r="N50" s="49" t="n">
+        <v>46027</v>
       </c>
       <c r="O50" s="6" t="inlineStr">
         <is>
@@ -4514,19 +4514,19 @@
         </is>
       </c>
       <c r="Q50" s="6" t="n">
+        <v>4.17</v>
+      </c>
+      <c r="R50" s="6" t="n">
         <v>4.19</v>
       </c>
-      <c r="R50" s="6" t="n">
+      <c r="S50" s="6" t="n">
         <v>4.18</v>
       </c>
-      <c r="S50" s="6" t="n">
+      <c r="T50" s="6" t="n">
         <v>4.14</v>
       </c>
-      <c r="T50" s="6" t="n">
+      <c r="U50" s="21" t="n">
         <v>4.12</v>
-      </c>
-      <c r="U50" s="21" t="n">
-        <v>4.14</v>
       </c>
     </row>
     <row r="51" ht="31.5" customHeight="1">
@@ -4575,7 +4575,7 @@
           <t>MORTGAGE30US</t>
         </is>
       </c>
-      <c r="N51" s="50" t="n">
+      <c r="N51" s="48" t="n">
         <v>46020</v>
       </c>
       <c r="O51" s="6" t="inlineStr">
@@ -4627,7 +4627,7 @@
         </is>
       </c>
       <c r="N52" s="53" t="n">
-        <v>46024</v>
+        <v>46027</v>
       </c>
       <c r="O52" s="9" t="inlineStr">
         <is>
@@ -4640,19 +4640,19 @@
         </is>
       </c>
       <c r="Q52" s="9" t="n">
+        <v>5.92</v>
+      </c>
+      <c r="R52" s="9" t="n">
         <v>5.93</v>
       </c>
-      <c r="R52" s="9" t="n">
+      <c r="S52" s="9" t="n">
         <v>5.9</v>
       </c>
-      <c r="S52" s="9" t="n">
+      <c r="T52" s="9" t="n">
         <v>5.89</v>
       </c>
-      <c r="T52" s="9" t="n">
+      <c r="U52" s="22" t="n">
         <v>5.88</v>
-      </c>
-      <c r="U52" s="22" t="n">
-        <v>5.89</v>
       </c>
     </row>
     <row r="53" ht="21" customHeight="1">

</xml_diff>

<commit_message>
Update dashboards - 2026-01-08
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -1485,8 +1485,8 @@
           <t>JTSJOR</t>
         </is>
       </c>
-      <c r="N10" s="48" t="n">
-        <v>45931</v>
+      <c r="N10" s="49" t="n">
+        <v>45962</v>
       </c>
       <c r="O10" s="6" t="inlineStr">
         <is>
@@ -1499,19 +1499,19 @@
         </is>
       </c>
       <c r="Q10" s="6" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="R10" s="6" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="S10" s="6" t="n">
         <v>4.6</v>
-      </c>
-      <c r="R10" s="6" t="n">
-        <v>4.6</v>
-      </c>
-      <c r="S10" s="6" t="n">
-        <v>4.3</v>
       </c>
       <c r="T10" s="6" t="n">
         <v>4.3</v>
       </c>
       <c r="U10" s="21" t="n">
-        <v>4.4</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="11">
@@ -1564,8 +1564,8 @@
           <t>JTSHIR</t>
         </is>
       </c>
-      <c r="N11" s="48" t="n">
-        <v>45931</v>
+      <c r="N11" s="49" t="n">
+        <v>45962</v>
       </c>
       <c r="O11" s="6" t="inlineStr">
         <is>
@@ -1584,10 +1584,10 @@
         <v>3.4</v>
       </c>
       <c r="S11" s="6" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="T11" s="6" t="n">
         <v>3.2</v>
-      </c>
-      <c r="T11" s="6" t="n">
-        <v>3.3</v>
       </c>
       <c r="U11" s="21" t="n">
         <v>3.3</v>
@@ -1639,8 +1639,8 @@
           <t>JTSTSR</t>
         </is>
       </c>
-      <c r="N12" s="48" t="n">
-        <v>45931</v>
+      <c r="N12" s="49" t="n">
+        <v>45962</v>
       </c>
       <c r="O12" s="6" t="inlineStr">
         <is>
@@ -1656,13 +1656,13 @@
         <v>3.2</v>
       </c>
       <c r="R12" s="6" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="S12" s="6" t="n">
         <v>3.3</v>
       </c>
-      <c r="S12" s="6" t="n">
+      <c r="T12" s="6" t="n">
         <v>3.2</v>
-      </c>
-      <c r="T12" s="6" t="n">
-        <v>3.3</v>
       </c>
       <c r="U12" s="21" t="n">
         <v>3.3</v>
@@ -1718,8 +1718,8 @@
           <t>ICSA</t>
         </is>
       </c>
-      <c r="N13" s="48" t="n">
-        <v>46013</v>
+      <c r="N13" s="49" t="n">
+        <v>46020</v>
       </c>
       <c r="O13" s="6" t="inlineStr">
         <is>
@@ -1732,19 +1732,19 @@
         </is>
       </c>
       <c r="Q13" s="24" t="n">
-        <v>199000</v>
+        <v>208000</v>
       </c>
       <c r="R13" s="24" t="n">
+        <v>200000</v>
+      </c>
+      <c r="S13" s="24" t="n">
         <v>215000</v>
       </c>
-      <c r="S13" s="24" t="n">
+      <c r="T13" s="24" t="n">
         <v>224000</v>
       </c>
-      <c r="T13" s="24" t="n">
+      <c r="U13" s="26" t="n">
         <v>237000</v>
-      </c>
-      <c r="U13" s="26" t="n">
-        <v>192000</v>
       </c>
     </row>
     <row r="14">
@@ -1793,8 +1793,8 @@
           <t>CCSA</t>
         </is>
       </c>
-      <c r="N14" s="48" t="n">
-        <v>46006</v>
+      <c r="N14" s="49" t="n">
+        <v>46013</v>
       </c>
       <c r="O14" s="6" t="inlineStr">
         <is>
@@ -1807,19 +1807,19 @@
         </is>
       </c>
       <c r="Q14" s="24" t="n">
-        <v>1866000</v>
+        <v>1914000</v>
       </c>
       <c r="R14" s="24" t="n">
-        <v>1913000</v>
+        <v>1858000</v>
       </c>
       <c r="S14" s="24" t="n">
+        <v>1914000</v>
+      </c>
+      <c r="T14" s="24" t="n">
         <v>1885000</v>
       </c>
-      <c r="T14" s="24" t="n">
+      <c r="U14" s="26" t="n">
         <v>1830000</v>
-      </c>
-      <c r="U14" s="26" t="n">
-        <v>1937000</v>
       </c>
     </row>
     <row r="15">
@@ -2821,10 +2821,10 @@
         </is>
       </c>
       <c r="F28" s="25" t="n">
-        <v>-0.02165298568032004</v>
+        <v>-0.02191649132412532</v>
       </c>
       <c r="G28" s="25" t="n">
-        <v>0.006551589361115884</v>
+        <v>0.006436255758670795</v>
       </c>
       <c r="H28" s="25" t="n">
         <v>0.03004963172206243</v>
@@ -2896,10 +2896,10 @@
         </is>
       </c>
       <c r="F29" s="25" t="n">
-        <v>0.04812695641499526</v>
+        <v>0.04772459132664544</v>
       </c>
       <c r="G29" s="25" t="n">
-        <v>0.07424376600596987</v>
+        <v>0.07412067603746038</v>
       </c>
       <c r="H29" s="25" t="n">
         <v>0.07661265288383932</v>
@@ -2922,7 +2922,7 @@
         </is>
       </c>
       <c r="N29" s="49" t="n">
-        <v>46028</v>
+        <v>46029</v>
       </c>
       <c r="O29" s="6" t="inlineStr">
         <is>
@@ -2938,16 +2938,16 @@
         <v>2.24</v>
       </c>
       <c r="R29" s="6" t="n">
+        <v>2.24</v>
+      </c>
+      <c r="S29" s="6" t="n">
         <v>2.23</v>
       </c>
-      <c r="S29" s="6" t="n">
+      <c r="T29" s="6" t="n">
         <v>2.22</v>
       </c>
-      <c r="T29" s="6" t="n">
+      <c r="U29" s="21" t="n">
         <v>2.24</v>
-      </c>
-      <c r="U29" s="21" t="n">
-        <v>2.23</v>
       </c>
     </row>
     <row r="30">
@@ -2975,10 +2975,10 @@
         </is>
       </c>
       <c r="F30" s="25" t="n">
-        <v>-0.01501954810691108</v>
+        <v>-0.01529652492391287</v>
       </c>
       <c r="G30" s="25" t="n">
-        <v>0.00129801269780061</v>
+        <v>0.001174064535676367</v>
       </c>
       <c r="H30" s="25" t="n">
         <v>0.01907672443132968</v>
@@ -3001,7 +3001,7 @@
         </is>
       </c>
       <c r="N30" s="49" t="n">
-        <v>46028</v>
+        <v>46029</v>
       </c>
       <c r="O30" s="6" t="inlineStr">
         <is>
@@ -3017,16 +3017,16 @@
         <v>2.27</v>
       </c>
       <c r="R30" s="6" t="n">
+        <v>2.27</v>
+      </c>
+      <c r="S30" s="6" t="n">
         <v>2.26</v>
-      </c>
-      <c r="S30" s="6" t="n">
-        <v>2.25</v>
       </c>
       <c r="T30" s="6" t="n">
         <v>2.25</v>
       </c>
       <c r="U30" s="21" t="n">
-        <v>2.24</v>
+        <v>2.25</v>
       </c>
     </row>
     <row r="31">
@@ -3050,10 +3050,10 @@
         </is>
       </c>
       <c r="F31" s="25" t="n">
-        <v>0.04791954754640503</v>
+        <v>0.04749518938811943</v>
       </c>
       <c r="G31" s="25" t="n">
-        <v>0.06515353511676288</v>
+        <v>0.06502168244015354</v>
       </c>
       <c r="H31" s="25" t="n">
         <v>0.06671073894520346</v>
@@ -3340,8 +3340,8 @@
           <t>PRS85006092</t>
         </is>
       </c>
-      <c r="C35" s="48" t="n">
-        <v>45748</v>
+      <c r="C35" s="49" t="n">
+        <v>45839</v>
       </c>
       <c r="D35" s="6" t="inlineStr">
         <is>
@@ -3354,19 +3354,19 @@
         </is>
       </c>
       <c r="F35" s="44" t="n">
-        <v>3.3</v>
+        <v>4.9</v>
       </c>
       <c r="G35" s="44" t="n">
-        <v>-1.8</v>
+        <v>4.1</v>
       </c>
       <c r="H35" s="44" t="n">
-        <v>1.7</v>
+        <v>-2.1</v>
       </c>
       <c r="I35" s="44" t="n">
-        <v>2.9</v>
+        <v>0.9</v>
       </c>
       <c r="J35" s="44" t="n">
-        <v>2.1</v>
+        <v>3.1</v>
       </c>
       <c r="K35" s="5" t="n"/>
       <c r="L35" s="28" t="inlineStr">
@@ -4268,7 +4268,7 @@
         </is>
       </c>
       <c r="N47" s="49" t="n">
-        <v>46027</v>
+        <v>46028</v>
       </c>
       <c r="O47" s="6" t="inlineStr">
         <is>
@@ -4347,7 +4347,7 @@
         </is>
       </c>
       <c r="N48" s="49" t="n">
-        <v>46027</v>
+        <v>46028</v>
       </c>
       <c r="O48" s="6" t="inlineStr">
         <is>
@@ -4360,16 +4360,16 @@
         </is>
       </c>
       <c r="Q48" s="6" t="n">
+        <v>3.47</v>
+      </c>
+      <c r="R48" s="6" t="n">
         <v>3.46</v>
-      </c>
-      <c r="R48" s="6" t="n">
-        <v>3.47</v>
       </c>
       <c r="S48" s="6" t="n">
         <v>3.47</v>
       </c>
       <c r="T48" s="6" t="n">
-        <v>3.45</v>
+        <v>3.47</v>
       </c>
       <c r="U48" s="21" t="n">
         <v>3.45</v>
@@ -4422,7 +4422,7 @@
         </is>
       </c>
       <c r="N49" s="49" t="n">
-        <v>46027</v>
+        <v>46028</v>
       </c>
       <c r="O49" s="6" t="inlineStr">
         <is>
@@ -4435,19 +4435,19 @@
         </is>
       </c>
       <c r="Q49" s="6" t="n">
+        <v>3.72</v>
+      </c>
+      <c r="R49" s="6" t="n">
         <v>3.71</v>
       </c>
-      <c r="R49" s="6" t="n">
+      <c r="S49" s="6" t="n">
         <v>3.74</v>
       </c>
-      <c r="S49" s="6" t="n">
+      <c r="T49" s="6" t="n">
         <v>3.73</v>
       </c>
-      <c r="T49" s="6" t="n">
+      <c r="U49" s="21" t="n">
         <v>3.68</v>
-      </c>
-      <c r="U49" s="21" t="n">
-        <v>3.67</v>
       </c>
     </row>
     <row r="50">
@@ -4501,7 +4501,7 @@
         </is>
       </c>
       <c r="N50" s="49" t="n">
-        <v>46027</v>
+        <v>46028</v>
       </c>
       <c r="O50" s="6" t="inlineStr">
         <is>
@@ -4514,19 +4514,19 @@
         </is>
       </c>
       <c r="Q50" s="6" t="n">
+        <v>4.18</v>
+      </c>
+      <c r="R50" s="6" t="n">
         <v>4.17</v>
       </c>
-      <c r="R50" s="6" t="n">
+      <c r="S50" s="6" t="n">
         <v>4.19</v>
       </c>
-      <c r="S50" s="6" t="n">
+      <c r="T50" s="6" t="n">
         <v>4.18</v>
       </c>
-      <c r="T50" s="6" t="n">
+      <c r="U50" s="21" t="n">
         <v>4.14</v>
-      </c>
-      <c r="U50" s="21" t="n">
-        <v>4.12</v>
       </c>
     </row>
     <row r="51" ht="31.5" customHeight="1">
@@ -4627,7 +4627,7 @@
         </is>
       </c>
       <c r="N52" s="53" t="n">
-        <v>46027</v>
+        <v>46028</v>
       </c>
       <c r="O52" s="9" t="inlineStr">
         <is>
@@ -4643,16 +4643,16 @@
         <v>5.92</v>
       </c>
       <c r="R52" s="9" t="n">
+        <v>5.92</v>
+      </c>
+      <c r="S52" s="9" t="n">
         <v>5.93</v>
       </c>
-      <c r="S52" s="9" t="n">
+      <c r="T52" s="9" t="n">
         <v>5.9</v>
       </c>
-      <c r="T52" s="9" t="n">
+      <c r="U52" s="22" t="n">
         <v>5.89</v>
-      </c>
-      <c r="U52" s="22" t="n">
-        <v>5.88</v>
       </c>
     </row>
     <row r="53" ht="21" customHeight="1">

</xml_diff>

<commit_message>
Update dashboards - 2026-01-09
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -948,8 +948,8 @@
           <t>PAYEMS</t>
         </is>
       </c>
-      <c r="N3" s="48" t="n">
-        <v>45962</v>
+      <c r="N3" s="49" t="n">
+        <v>45992</v>
       </c>
       <c r="O3" s="6" t="inlineStr">
         <is>
@@ -962,19 +962,19 @@
         </is>
       </c>
       <c r="Q3" s="24" t="n">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="R3" s="24" t="n">
-        <v>-105</v>
+        <v>56</v>
       </c>
       <c r="S3" s="24" t="n">
+        <v>-173</v>
+      </c>
+      <c r="T3" s="24" t="n">
         <v>108</v>
       </c>
-      <c r="T3" s="24" t="n">
+      <c r="U3" s="26" t="n">
         <v>-26</v>
-      </c>
-      <c r="U3" s="26" t="n">
-        <v>72</v>
       </c>
     </row>
     <row r="4">
@@ -1019,8 +1019,8 @@
           <t>PAYEMS</t>
         </is>
       </c>
-      <c r="N4" s="48" t="n">
-        <v>45962</v>
+      <c r="N4" s="49" t="n">
+        <v>45992</v>
       </c>
       <c r="O4" s="6" t="inlineStr">
         <is>
@@ -1033,19 +1033,19 @@
         </is>
       </c>
       <c r="Q4" s="38" t="n">
-        <v>0.005882019178030375</v>
+        <v>0.003674296284179135</v>
       </c>
       <c r="R4" s="38" t="n">
-        <v>0.007135730433574559</v>
+        <v>0.005402883639412681</v>
       </c>
       <c r="S4" s="38" t="n">
+        <v>0.006706323646421399</v>
+      </c>
+      <c r="T4" s="38" t="n">
         <v>0.008078881210758367</v>
       </c>
-      <c r="T4" s="38" t="n">
+      <c r="U4" s="23" t="n">
         <v>0.008926199121930236</v>
-      </c>
-      <c r="U4" s="23" t="n">
-        <v>0.009544122579951013</v>
       </c>
     </row>
     <row r="5" ht="31.5" customHeight="1">
@@ -1173,8 +1173,8 @@
           <t>UNRATE</t>
         </is>
       </c>
-      <c r="N6" s="48" t="n">
-        <v>45962</v>
+      <c r="N6" s="49" t="n">
+        <v>45992</v>
       </c>
       <c r="O6" s="6" t="inlineStr">
         <is>
@@ -1187,19 +1187,19 @@
         </is>
       </c>
       <c r="Q6" s="6" t="n">
-        <v>4.6</v>
+        <v>4.4</v>
       </c>
       <c r="R6" s="6" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="S6" s="6" t="n">
         <v/>
       </c>
-      <c r="S6" s="6" t="n">
+      <c r="T6" s="6" t="n">
         <v>4.4</v>
       </c>
-      <c r="T6" s="6" t="n">
+      <c r="U6" s="21" t="n">
         <v>4.3</v>
-      </c>
-      <c r="U6" s="21" t="n">
-        <v>4.2</v>
       </c>
     </row>
     <row r="7" ht="16.15" customHeight="1">
@@ -1252,8 +1252,8 @@
           <t>U6RATE</t>
         </is>
       </c>
-      <c r="N7" s="48" t="n">
-        <v>45962</v>
+      <c r="N7" s="49" t="n">
+        <v>45992</v>
       </c>
       <c r="O7" s="6" t="inlineStr">
         <is>
@@ -1266,19 +1266,19 @@
         </is>
       </c>
       <c r="Q7" s="6" t="n">
+        <v>8.4</v>
+      </c>
+      <c r="R7" s="6" t="n">
         <v>8.699999999999999</v>
       </c>
-      <c r="R7" s="6" t="n">
+      <c r="S7" s="6" t="n">
         <v/>
-      </c>
-      <c r="S7" s="6" t="n">
-        <v>8</v>
       </c>
       <c r="T7" s="6" t="n">
         <v>8.1</v>
       </c>
       <c r="U7" s="21" t="n">
-        <v>7.9</v>
+        <v>8.1</v>
       </c>
     </row>
     <row r="8" ht="31.5" customHeight="1">
@@ -1331,8 +1331,8 @@
           <t>CIVPART</t>
         </is>
       </c>
-      <c r="N8" s="48" t="n">
-        <v>45962</v>
+      <c r="N8" s="49" t="n">
+        <v>45992</v>
       </c>
       <c r="O8" s="6" t="inlineStr">
         <is>
@@ -1345,19 +1345,19 @@
         </is>
       </c>
       <c r="Q8" s="6" t="n">
+        <v>62.4</v>
+      </c>
+      <c r="R8" s="6" t="n">
         <v>62.5</v>
       </c>
-      <c r="R8" s="6" t="n">
+      <c r="S8" s="6" t="n">
         <v/>
       </c>
-      <c r="S8" s="6" t="n">
-        <v>62.4</v>
-      </c>
       <c r="T8" s="6" t="n">
+        <v>62.5</v>
+      </c>
+      <c r="U8" s="21" t="n">
         <v>62.3</v>
-      </c>
-      <c r="U8" s="21" t="n">
-        <v>62.2</v>
       </c>
     </row>
     <row r="9">
@@ -1410,8 +1410,8 @@
           <t>EMRATIO</t>
         </is>
       </c>
-      <c r="N9" s="48" t="n">
-        <v>45962</v>
+      <c r="N9" s="49" t="n">
+        <v>45992</v>
       </c>
       <c r="O9" s="6" t="inlineStr">
         <is>
@@ -1424,16 +1424,16 @@
         </is>
       </c>
       <c r="Q9" s="6" t="n">
+        <v>59.7</v>
+      </c>
+      <c r="R9" s="6" t="n">
         <v>59.6</v>
       </c>
-      <c r="R9" s="6" t="n">
+      <c r="S9" s="6" t="n">
         <v/>
       </c>
-      <c r="S9" s="6" t="n">
+      <c r="T9" s="6" t="n">
         <v>59.7</v>
-      </c>
-      <c r="T9" s="6" t="n">
-        <v>59.6</v>
       </c>
       <c r="U9" s="21" t="n">
         <v>59.6</v>
@@ -1872,8 +1872,8 @@
           <t>AWHAETP</t>
         </is>
       </c>
-      <c r="N15" s="48" t="n">
-        <v>45962</v>
+      <c r="N15" s="49" t="n">
+        <v>45992</v>
       </c>
       <c r="O15" s="6" t="inlineStr">
         <is>
@@ -1886,10 +1886,10 @@
         </is>
       </c>
       <c r="Q15" s="24" t="n">
+        <v>34.2</v>
+      </c>
+      <c r="R15" s="24" t="n">
         <v>34.3</v>
-      </c>
-      <c r="R15" s="24" t="n">
-        <v>34.2</v>
       </c>
       <c r="S15" s="24" t="n">
         <v>34.2</v>
@@ -1898,7 +1898,7 @@
         <v>34.2</v>
       </c>
       <c r="U15" s="26" t="n">
-        <v>34.3</v>
+        <v>34.2</v>
       </c>
     </row>
     <row r="16">
@@ -2499,8 +2499,8 @@
           <t>REVOLSL</t>
         </is>
       </c>
-      <c r="C24" s="48" t="n">
-        <v>45931</v>
+      <c r="C24" s="49" t="n">
+        <v>45962</v>
       </c>
       <c r="D24" s="6" t="inlineStr">
         <is>
@@ -2513,19 +2513,19 @@
         </is>
       </c>
       <c r="F24" s="38" t="n">
-        <v>0.004122988119927395</v>
+        <v>-0.001551215487983981</v>
       </c>
       <c r="G24" s="38" t="n">
-        <v>0.003293006621412964</v>
+        <v>0.004120302067736503</v>
       </c>
       <c r="H24" s="38" t="n">
-        <v>-0.00328836233676344</v>
+        <v>0.003065216912115698</v>
       </c>
       <c r="I24" s="38" t="n">
-        <v>0.008508856867884829</v>
+        <v>-0.003484844670176512</v>
       </c>
       <c r="J24" s="38" t="n">
-        <v>6.940322356907558e-05</v>
+        <v>0.008311712980978658</v>
       </c>
       <c r="K24" s="5" t="n"/>
       <c r="L24" s="28" t="inlineStr">
@@ -2578,8 +2578,8 @@
           <t>NONREVSL</t>
         </is>
       </c>
-      <c r="C25" s="48" t="n">
-        <v>45931</v>
+      <c r="C25" s="49" t="n">
+        <v>45962</v>
       </c>
       <c r="D25" s="6" t="inlineStr">
         <is>
@@ -2592,19 +2592,19 @@
         </is>
       </c>
       <c r="F25" s="38" t="n">
-        <v>0.001002044138157077</v>
+        <v>0.001665686369376251</v>
       </c>
       <c r="G25" s="38" t="n">
-        <v>0.001783907070203483</v>
+        <v>0.001019986599621658</v>
       </c>
       <c r="H25" s="38" t="n">
-        <v>0.002285485926998732</v>
+        <v>0.001988823510608029</v>
       </c>
       <c r="I25" s="38" t="n">
-        <v>0.001562654273511654</v>
+        <v>0.001936089671301433</v>
       </c>
       <c r="J25" s="38" t="n">
-        <v>-0.001091050242697622</v>
+        <v>0.0009927073679749654</v>
       </c>
       <c r="K25" s="5" t="n"/>
       <c r="L25" s="28" t="n"/>
@@ -2922,7 +2922,7 @@
         </is>
       </c>
       <c r="N29" s="49" t="n">
-        <v>46029</v>
+        <v>46030</v>
       </c>
       <c r="O29" s="6" t="inlineStr">
         <is>
@@ -2935,19 +2935,19 @@
         </is>
       </c>
       <c r="Q29" s="6" t="n">
-        <v>2.24</v>
+        <v>2.23</v>
       </c>
       <c r="R29" s="6" t="n">
         <v>2.24</v>
       </c>
       <c r="S29" s="6" t="n">
+        <v>2.24</v>
+      </c>
+      <c r="T29" s="6" t="n">
         <v>2.23</v>
       </c>
-      <c r="T29" s="6" t="n">
+      <c r="U29" s="21" t="n">
         <v>2.22</v>
-      </c>
-      <c r="U29" s="21" t="n">
-        <v>2.24</v>
       </c>
     </row>
     <row r="30">
@@ -3001,7 +3001,7 @@
         </is>
       </c>
       <c r="N30" s="49" t="n">
-        <v>46029</v>
+        <v>46030</v>
       </c>
       <c r="O30" s="6" t="inlineStr">
         <is>
@@ -3020,10 +3020,10 @@
         <v>2.27</v>
       </c>
       <c r="S30" s="6" t="n">
+        <v>2.27</v>
+      </c>
+      <c r="T30" s="6" t="n">
         <v>2.26</v>
-      </c>
-      <c r="T30" s="6" t="n">
-        <v>2.25</v>
       </c>
       <c r="U30" s="21" t="n">
         <v>2.25</v>
@@ -3225,8 +3225,8 @@
           <t>CES0500000003</t>
         </is>
       </c>
-      <c r="N33" s="48" t="n">
-        <v>45962</v>
+      <c r="N33" s="49" t="n">
+        <v>45992</v>
       </c>
       <c r="O33" s="6" t="inlineStr">
         <is>
@@ -3239,19 +3239,19 @@
         </is>
       </c>
       <c r="Q33" s="38" t="n">
-        <v>0.001358326541700539</v>
+        <v>0.003252032520325354</v>
       </c>
       <c r="R33" s="38" t="n">
+        <v>0.002444987775060969</v>
+      </c>
+      <c r="S33" s="38" t="n">
         <v>0.004365620736698661</v>
       </c>
-      <c r="S33" s="38" t="n">
+      <c r="T33" s="38" t="n">
         <v>0.001913613996719521</v>
       </c>
-      <c r="T33" s="38" t="n">
+      <c r="U33" s="23" t="n">
         <v>0.004117485588800429</v>
-      </c>
-      <c r="U33" s="23" t="n">
-        <v>0.003304874690167825</v>
       </c>
     </row>
     <row r="34" ht="31.5" customHeight="1">
@@ -3415,8 +3415,8 @@
           <t>HOUST</t>
         </is>
       </c>
-      <c r="C36" s="48" t="n">
-        <v>45870</v>
+      <c r="C36" s="49" t="n">
+        <v>45931</v>
       </c>
       <c r="D36" s="6" t="inlineStr">
         <is>
@@ -3429,19 +3429,19 @@
         </is>
       </c>
       <c r="F36" s="24" t="n">
-        <v>1307</v>
+        <v>1246</v>
       </c>
       <c r="G36" s="24" t="n">
-        <v>1429</v>
+        <v>1306</v>
       </c>
       <c r="H36" s="24" t="n">
+        <v>1291</v>
+      </c>
+      <c r="I36" s="24" t="n">
+        <v>1420</v>
+      </c>
+      <c r="J36" s="24" t="n">
         <v>1382</v>
-      </c>
-      <c r="I36" s="24" t="n">
-        <v>1282</v>
-      </c>
-      <c r="J36" s="24" t="n">
-        <v>1398</v>
       </c>
       <c r="K36" s="5" t="n"/>
       <c r="L36" s="28" t="n"/>
@@ -3490,8 +3490,8 @@
           <t>HOUST</t>
         </is>
       </c>
-      <c r="C37" s="48" t="n">
-        <v>45870</v>
+      <c r="C37" s="49" t="n">
+        <v>45931</v>
       </c>
       <c r="D37" s="6" t="inlineStr">
         <is>
@@ -3504,19 +3504,19 @@
         </is>
       </c>
       <c r="F37" s="25" t="n">
-        <v>-0.0603882099209202</v>
+        <v>-0.07840236686390532</v>
       </c>
       <c r="G37" s="25" t="n">
-        <v>0.1296442687747036</v>
+        <v>-0.03758290346352248</v>
       </c>
       <c r="H37" s="25" t="n">
+        <v>-0.07189072609633357</v>
+      </c>
+      <c r="I37" s="25" t="n">
+        <v>0.1225296442687747</v>
+      </c>
+      <c r="J37" s="25" t="n">
         <v>0.04144687264506405</v>
-      </c>
-      <c r="I37" s="25" t="n">
-        <v>-0.02583586626139818</v>
-      </c>
-      <c r="J37" s="25" t="n">
-        <v>0.009386281588447653</v>
       </c>
       <c r="K37" s="5" t="n"/>
       <c r="L37" s="28" t="inlineStr">
@@ -3569,8 +3569,8 @@
           <t>PERMIT</t>
         </is>
       </c>
-      <c r="C38" s="48" t="n">
-        <v>45870</v>
+      <c r="C38" s="49" t="n">
+        <v>45931</v>
       </c>
       <c r="D38" s="6" t="inlineStr">
         <is>
@@ -3583,19 +3583,19 @@
         </is>
       </c>
       <c r="F38" s="24" t="n">
+        <v>1412</v>
+      </c>
+      <c r="G38" s="24" t="n">
+        <v>1415</v>
+      </c>
+      <c r="H38" s="24" t="n">
         <v>1330</v>
       </c>
-      <c r="G38" s="24" t="n">
+      <c r="I38" s="24" t="n">
         <v>1362</v>
       </c>
-      <c r="H38" s="24" t="n">
+      <c r="J38" s="24" t="n">
         <v>1393</v>
-      </c>
-      <c r="I38" s="24" t="n">
-        <v>1394</v>
-      </c>
-      <c r="J38" s="24" t="n">
-        <v>1422</v>
       </c>
       <c r="K38" s="5" t="n"/>
       <c r="L38" s="28" t="n"/>
@@ -3640,8 +3640,8 @@
           <t>PERMIT</t>
         </is>
       </c>
-      <c r="C39" s="48" t="n">
-        <v>45870</v>
+      <c r="C39" s="49" t="n">
+        <v>45931</v>
       </c>
       <c r="D39" s="6" t="inlineStr">
         <is>
@@ -3654,19 +3654,19 @@
         </is>
       </c>
       <c r="F39" s="38" t="n">
+        <v>-0.01120448179271709</v>
+      </c>
+      <c r="G39" s="38" t="n">
+        <v>-0.01324965132496513</v>
+      </c>
+      <c r="H39" s="38" t="n">
         <v>-0.0989159891598916</v>
       </c>
-      <c r="G39" s="38" t="n">
+      <c r="I39" s="38" t="n">
         <v>-0.05153203342618384</v>
       </c>
-      <c r="H39" s="38" t="n">
+      <c r="J39" s="38" t="n">
         <v>-0.04654346338124572</v>
-      </c>
-      <c r="I39" s="38" t="n">
-        <v>-0.009239516702203269</v>
-      </c>
-      <c r="J39" s="38" t="n">
-        <v>-0.0253598355037697</v>
       </c>
       <c r="K39" s="5" t="n"/>
       <c r="L39" s="28" t="inlineStr">
@@ -4141,8 +4141,8 @@
           <t>BOPTEXP</t>
         </is>
       </c>
-      <c r="C46" s="48" t="n">
-        <v>45901</v>
+      <c r="C46" s="49" t="n">
+        <v>45931</v>
       </c>
       <c r="D46" s="6" t="inlineStr">
         <is>
@@ -4155,19 +4155,19 @@
         </is>
       </c>
       <c r="F46" s="24" t="n">
-        <v>289305</v>
+        <v>302015</v>
       </c>
       <c r="G46" s="24" t="n">
-        <v>280921</v>
+        <v>294225</v>
       </c>
       <c r="H46" s="24" t="n">
-        <v>281602</v>
+        <v>284060</v>
       </c>
       <c r="I46" s="24" t="n">
-        <v>279650</v>
+        <v>283923</v>
       </c>
       <c r="J46" s="24" t="n">
-        <v>280391</v>
+        <v>280519</v>
       </c>
       <c r="K46" s="5" t="n"/>
       <c r="L46" s="29" t="inlineStr">
@@ -4228,8 +4228,8 @@
           <t>BOPTEXP</t>
         </is>
       </c>
-      <c r="C47" s="48" t="n">
-        <v>45901</v>
+      <c r="C47" s="49" t="n">
+        <v>45931</v>
       </c>
       <c r="D47" s="6" t="inlineStr">
         <is>
@@ -4242,19 +4242,19 @@
         </is>
       </c>
       <c r="F47" s="38" t="n">
-        <v>0.02984468943226037</v>
+        <v>0.02647633613730993</v>
       </c>
       <c r="G47" s="38" t="n">
-        <v>-0.002418306688162675</v>
+        <v>0.03578469337463908</v>
       </c>
       <c r="H47" s="38" t="n">
-        <v>0.006980153763633146</v>
+        <v>0.0004825251916893425</v>
       </c>
       <c r="I47" s="38" t="n">
-        <v>-0.002642738176332315</v>
+        <v>0.01213465041583639</v>
       </c>
       <c r="J47" s="38" t="n">
-        <v>-0.03904929999828644</v>
+        <v>0.0004065548046574552</v>
       </c>
       <c r="K47" s="5" t="n"/>
       <c r="L47" s="28" t="inlineStr">
@@ -4268,7 +4268,7 @@
         </is>
       </c>
       <c r="N47" s="49" t="n">
-        <v>46028</v>
+        <v>46029</v>
       </c>
       <c r="O47" s="6" t="inlineStr">
         <is>
@@ -4307,8 +4307,8 @@
           <t>BOPTIMP</t>
         </is>
       </c>
-      <c r="C48" s="48" t="n">
-        <v>45901</v>
+      <c r="C48" s="49" t="n">
+        <v>45931</v>
       </c>
       <c r="D48" s="6" t="inlineStr">
         <is>
@@ -4321,19 +4321,19 @@
         </is>
       </c>
       <c r="F48" s="24" t="n">
-        <v>342133</v>
+        <v>331366</v>
       </c>
       <c r="G48" s="24" t="n">
-        <v>340185</v>
+        <v>342363</v>
       </c>
       <c r="H48" s="24" t="n">
-        <v>358756</v>
+        <v>339690</v>
       </c>
       <c r="I48" s="24" t="n">
-        <v>338736</v>
+        <v>358321</v>
       </c>
       <c r="J48" s="24" t="n">
-        <v>351506</v>
+        <v>338704</v>
       </c>
       <c r="K48" s="5" t="n"/>
       <c r="L48" s="28" t="inlineStr">
@@ -4347,7 +4347,7 @@
         </is>
       </c>
       <c r="N48" s="49" t="n">
-        <v>46028</v>
+        <v>46029</v>
       </c>
       <c r="O48" s="6" t="inlineStr">
         <is>
@@ -4363,16 +4363,16 @@
         <v>3.47</v>
       </c>
       <c r="R48" s="6" t="n">
+        <v>3.47</v>
+      </c>
+      <c r="S48" s="6" t="n">
         <v>3.46</v>
-      </c>
-      <c r="S48" s="6" t="n">
-        <v>3.47</v>
       </c>
       <c r="T48" s="6" t="n">
         <v>3.47</v>
       </c>
       <c r="U48" s="21" t="n">
-        <v>3.45</v>
+        <v>3.47</v>
       </c>
     </row>
     <row r="49">
@@ -4382,8 +4382,8 @@
           <t>BOPTIMP</t>
         </is>
       </c>
-      <c r="C49" s="48" t="n">
-        <v>45901</v>
+      <c r="C49" s="49" t="n">
+        <v>45931</v>
       </c>
       <c r="D49" s="6" t="inlineStr">
         <is>
@@ -4396,19 +4396,19 @@
         </is>
       </c>
       <c r="F49" s="38" t="n">
-        <v>0.005726295986007601</v>
+        <v>-0.03212087754809956</v>
       </c>
       <c r="G49" s="38" t="n">
-        <v>-0.05176498790264139</v>
+        <v>0.007868939327033475</v>
       </c>
       <c r="H49" s="38" t="n">
-        <v>0.05910207359123332</v>
+        <v>-0.05199527797700942</v>
       </c>
       <c r="I49" s="38" t="n">
-        <v>-0.03632939409284619</v>
+        <v>0.05791782795597333</v>
       </c>
       <c r="J49" s="38" t="n">
-        <v>-0.001338155618122783</v>
+        <v>-0.03628608905214581</v>
       </c>
       <c r="K49" s="5" t="n"/>
       <c r="L49" s="28" t="inlineStr">
@@ -4422,7 +4422,7 @@
         </is>
       </c>
       <c r="N49" s="49" t="n">
-        <v>46028</v>
+        <v>46029</v>
       </c>
       <c r="O49" s="6" t="inlineStr">
         <is>
@@ -4435,19 +4435,19 @@
         </is>
       </c>
       <c r="Q49" s="6" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="R49" s="6" t="n">
         <v>3.72</v>
       </c>
-      <c r="R49" s="6" t="n">
+      <c r="S49" s="6" t="n">
         <v>3.71</v>
       </c>
-      <c r="S49" s="6" t="n">
+      <c r="T49" s="6" t="n">
         <v>3.74</v>
       </c>
-      <c r="T49" s="6" t="n">
+      <c r="U49" s="21" t="n">
         <v>3.73</v>
-      </c>
-      <c r="U49" s="21" t="n">
-        <v>3.68</v>
       </c>
     </row>
     <row r="50">
@@ -4461,8 +4461,8 @@
           <t>BOPSTB</t>
         </is>
       </c>
-      <c r="C50" s="48" t="n">
-        <v>45901</v>
+      <c r="C50" s="49" t="n">
+        <v>45931</v>
       </c>
       <c r="D50" s="6" t="inlineStr">
         <is>
@@ -4475,19 +4475,19 @@
         </is>
       </c>
       <c r="F50" s="24" t="n">
-        <v>26157</v>
+        <v>29796</v>
       </c>
       <c r="G50" s="24" t="n">
-        <v>26795</v>
+        <v>30169</v>
       </c>
       <c r="H50" s="24" t="n">
-        <v>25569</v>
+        <v>30416</v>
       </c>
       <c r="I50" s="24" t="n">
-        <v>26631</v>
+        <v>28606</v>
       </c>
       <c r="J50" s="24" t="n">
-        <v>26236</v>
+        <v>27839</v>
       </c>
       <c r="K50" s="5" t="n"/>
       <c r="L50" s="28" t="inlineStr">
@@ -4501,7 +4501,7 @@
         </is>
       </c>
       <c r="N50" s="49" t="n">
-        <v>46028</v>
+        <v>46029</v>
       </c>
       <c r="O50" s="6" t="inlineStr">
         <is>
@@ -4514,19 +4514,19 @@
         </is>
       </c>
       <c r="Q50" s="6" t="n">
+        <v>4.15</v>
+      </c>
+      <c r="R50" s="6" t="n">
         <v>4.18</v>
       </c>
-      <c r="R50" s="6" t="n">
+      <c r="S50" s="6" t="n">
         <v>4.17</v>
       </c>
-      <c r="S50" s="6" t="n">
+      <c r="T50" s="6" t="n">
         <v>4.19</v>
       </c>
-      <c r="T50" s="6" t="n">
+      <c r="U50" s="21" t="n">
         <v>4.18</v>
-      </c>
-      <c r="U50" s="21" t="n">
-        <v>4.14</v>
       </c>
     </row>
     <row r="51" ht="31.5" customHeight="1">
@@ -4536,8 +4536,8 @@
           <t>BOPSTB</t>
         </is>
       </c>
-      <c r="C51" s="48" t="n">
-        <v>45901</v>
+      <c r="C51" s="49" t="n">
+        <v>45931</v>
       </c>
       <c r="D51" s="6" t="inlineStr">
         <is>
@@ -4550,19 +4550,19 @@
         </is>
       </c>
       <c r="F51" s="38" t="n">
-        <v>-0.02381041239037129</v>
+        <v>-0.01236368457688353</v>
       </c>
       <c r="G51" s="38" t="n">
-        <v>0.04794868786421058</v>
+        <v>-0.008120725933719042</v>
       </c>
       <c r="H51" s="38" t="n">
-        <v>-0.03987833727610679</v>
+        <v>0.06327343913864225</v>
       </c>
       <c r="I51" s="38" t="n">
-        <v>0.01505564872693999</v>
+        <v>0.02755127698552395</v>
       </c>
       <c r="J51" s="38" t="n">
-        <v>-0.01815051831892522</v>
+        <v>0.05614780530369123</v>
       </c>
       <c r="K51" s="5" t="n"/>
       <c r="L51" s="28" t="inlineStr">
@@ -4575,8 +4575,8 @@
           <t>MORTGAGE30US</t>
         </is>
       </c>
-      <c r="N51" s="48" t="n">
-        <v>46020</v>
+      <c r="N51" s="49" t="n">
+        <v>46027</v>
       </c>
       <c r="O51" s="6" t="inlineStr">
         <is>
@@ -4589,19 +4589,19 @@
         </is>
       </c>
       <c r="Q51" s="6" t="n">
+        <v>6.16</v>
+      </c>
+      <c r="R51" s="6" t="n">
         <v>6.15</v>
       </c>
-      <c r="R51" s="6" t="n">
+      <c r="S51" s="6" t="n">
         <v>6.18</v>
       </c>
-      <c r="S51" s="6" t="n">
+      <c r="T51" s="6" t="n">
         <v>6.21</v>
       </c>
-      <c r="T51" s="6" t="n">
+      <c r="U51" s="21" t="n">
         <v>6.22</v>
-      </c>
-      <c r="U51" s="21" t="n">
-        <v>6.19</v>
       </c>
     </row>
     <row r="52" ht="16.15" customHeight="1" thickBot="1">
@@ -4627,7 +4627,7 @@
         </is>
       </c>
       <c r="N52" s="53" t="n">
-        <v>46028</v>
+        <v>46029</v>
       </c>
       <c r="O52" s="9" t="inlineStr">
         <is>
@@ -4640,19 +4640,19 @@
         </is>
       </c>
       <c r="Q52" s="9" t="n">
-        <v>5.92</v>
+        <v>5.88</v>
       </c>
       <c r="R52" s="9" t="n">
         <v>5.92</v>
       </c>
       <c r="S52" s="9" t="n">
+        <v>5.92</v>
+      </c>
+      <c r="T52" s="9" t="n">
         <v>5.93</v>
       </c>
-      <c r="T52" s="9" t="n">
+      <c r="U52" s="22" t="n">
         <v>5.9</v>
-      </c>
-      <c r="U52" s="22" t="n">
-        <v>5.89</v>
       </c>
     </row>
     <row r="53" ht="21" customHeight="1">

</xml_diff>

<commit_message>
Update dashboards - 2026-01-10
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -2922,7 +2922,7 @@
         </is>
       </c>
       <c r="N29" s="49" t="n">
-        <v>46030</v>
+        <v>46031</v>
       </c>
       <c r="O29" s="6" t="inlineStr">
         <is>
@@ -2935,19 +2935,19 @@
         </is>
       </c>
       <c r="Q29" s="6" t="n">
+        <v>2.24</v>
+      </c>
+      <c r="R29" s="6" t="n">
         <v>2.23</v>
-      </c>
-      <c r="R29" s="6" t="n">
-        <v>2.24</v>
       </c>
       <c r="S29" s="6" t="n">
         <v>2.24</v>
       </c>
       <c r="T29" s="6" t="n">
+        <v>2.24</v>
+      </c>
+      <c r="U29" s="21" t="n">
         <v>2.23</v>
-      </c>
-      <c r="U29" s="21" t="n">
-        <v>2.22</v>
       </c>
     </row>
     <row r="30">
@@ -3001,7 +3001,7 @@
         </is>
       </c>
       <c r="N30" s="49" t="n">
-        <v>46030</v>
+        <v>46031</v>
       </c>
       <c r="O30" s="6" t="inlineStr">
         <is>
@@ -3014,7 +3014,7 @@
         </is>
       </c>
       <c r="Q30" s="6" t="n">
-        <v>2.27</v>
+        <v>2.28</v>
       </c>
       <c r="R30" s="6" t="n">
         <v>2.27</v>
@@ -3023,10 +3023,10 @@
         <v>2.27</v>
       </c>
       <c r="T30" s="6" t="n">
+        <v>2.27</v>
+      </c>
+      <c r="U30" s="21" t="n">
         <v>2.26</v>
-      </c>
-      <c r="U30" s="21" t="n">
-        <v>2.25</v>
       </c>
     </row>
     <row r="31">
@@ -4268,7 +4268,7 @@
         </is>
       </c>
       <c r="N47" s="49" t="n">
-        <v>46029</v>
+        <v>46030</v>
       </c>
       <c r="O47" s="6" t="inlineStr">
         <is>
@@ -4347,7 +4347,7 @@
         </is>
       </c>
       <c r="N48" s="49" t="n">
-        <v>46029</v>
+        <v>46030</v>
       </c>
       <c r="O48" s="6" t="inlineStr">
         <is>
@@ -4360,16 +4360,16 @@
         </is>
       </c>
       <c r="Q48" s="6" t="n">
-        <v>3.47</v>
+        <v>3.49</v>
       </c>
       <c r="R48" s="6" t="n">
         <v>3.47</v>
       </c>
       <c r="S48" s="6" t="n">
+        <v>3.47</v>
+      </c>
+      <c r="T48" s="6" t="n">
         <v>3.46</v>
-      </c>
-      <c r="T48" s="6" t="n">
-        <v>3.47</v>
       </c>
       <c r="U48" s="21" t="n">
         <v>3.47</v>
@@ -4422,7 +4422,7 @@
         </is>
       </c>
       <c r="N49" s="49" t="n">
-        <v>46029</v>
+        <v>46030</v>
       </c>
       <c r="O49" s="6" t="inlineStr">
         <is>
@@ -4435,19 +4435,19 @@
         </is>
       </c>
       <c r="Q49" s="6" t="n">
+        <v>3.74</v>
+      </c>
+      <c r="R49" s="6" t="n">
         <v>3.7</v>
       </c>
-      <c r="R49" s="6" t="n">
+      <c r="S49" s="6" t="n">
         <v>3.72</v>
       </c>
-      <c r="S49" s="6" t="n">
+      <c r="T49" s="6" t="n">
         <v>3.71</v>
       </c>
-      <c r="T49" s="6" t="n">
+      <c r="U49" s="21" t="n">
         <v>3.74</v>
-      </c>
-      <c r="U49" s="21" t="n">
-        <v>3.73</v>
       </c>
     </row>
     <row r="50">
@@ -4501,7 +4501,7 @@
         </is>
       </c>
       <c r="N50" s="49" t="n">
-        <v>46029</v>
+        <v>46030</v>
       </c>
       <c r="O50" s="6" t="inlineStr">
         <is>
@@ -4514,19 +4514,19 @@
         </is>
       </c>
       <c r="Q50" s="6" t="n">
+        <v>4.19</v>
+      </c>
+      <c r="R50" s="6" t="n">
         <v>4.15</v>
       </c>
-      <c r="R50" s="6" t="n">
+      <c r="S50" s="6" t="n">
         <v>4.18</v>
       </c>
-      <c r="S50" s="6" t="n">
+      <c r="T50" s="6" t="n">
         <v>4.17</v>
       </c>
-      <c r="T50" s="6" t="n">
+      <c r="U50" s="21" t="n">
         <v>4.19</v>
-      </c>
-      <c r="U50" s="21" t="n">
-        <v>4.18</v>
       </c>
     </row>
     <row r="51" ht="31.5" customHeight="1">
@@ -4627,7 +4627,7 @@
         </is>
       </c>
       <c r="N52" s="53" t="n">
-        <v>46029</v>
+        <v>46030</v>
       </c>
       <c r="O52" s="9" t="inlineStr">
         <is>
@@ -4640,19 +4640,19 @@
         </is>
       </c>
       <c r="Q52" s="9" t="n">
+        <v>5.92</v>
+      </c>
+      <c r="R52" s="9" t="n">
         <v>5.88</v>
-      </c>
-      <c r="R52" s="9" t="n">
-        <v>5.92</v>
       </c>
       <c r="S52" s="9" t="n">
         <v>5.92</v>
       </c>
       <c r="T52" s="9" t="n">
+        <v>5.92</v>
+      </c>
+      <c r="U52" s="22" t="n">
         <v>5.93</v>
-      </c>
-      <c r="U52" s="22" t="n">
-        <v>5.9</v>
       </c>
     </row>
     <row r="53" ht="21" customHeight="1">

</xml_diff>

<commit_message>
Update dashboards - 2026-01-12
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -3679,7 +3679,7 @@
           <t>TWEXBGSMTH</t>
         </is>
       </c>
-      <c r="N39" s="49" t="n">
+      <c r="N39" s="48" t="n">
         <v>45992</v>
       </c>
       <c r="O39" s="6" t="inlineStr">
@@ -3754,7 +3754,7 @@
           <t>TWEXBGSMTH</t>
         </is>
       </c>
-      <c r="N40" s="49" t="n">
+      <c r="N40" s="48" t="n">
         <v>45992</v>
       </c>
       <c r="O40" s="6" t="inlineStr">

</xml_diff>

<commit_message>
Update dashboards - 2026-01-13
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -2085,8 +2085,8 @@
           <t>CPIAUCSL</t>
         </is>
       </c>
-      <c r="N18" s="48" t="n">
-        <v>45962</v>
+      <c r="N18" s="49" t="n">
+        <v>45992</v>
       </c>
       <c r="O18" s="6" t="inlineStr">
         <is>
@@ -2099,19 +2099,19 @@
         </is>
       </c>
       <c r="Q18" s="38" t="n">
-        <v/>
+        <v>0.003073552984176775</v>
       </c>
       <c r="R18" s="38" t="n">
         <v/>
       </c>
       <c r="S18" s="38" t="n">
+        <v/>
+      </c>
+      <c r="T18" s="38" t="n">
         <v>0.00310486015759337</v>
       </c>
-      <c r="T18" s="38" t="n">
+      <c r="U18" s="23" t="n">
         <v>0.003824519141221616</v>
-      </c>
-      <c r="U18" s="23" t="n">
-        <v>0.00196578538102643</v>
       </c>
     </row>
     <row r="19" ht="31.5" customHeight="1">
@@ -2160,8 +2160,8 @@
           <t>CPIAUCSL</t>
         </is>
       </c>
-      <c r="N19" s="48" t="n">
-        <v>45962</v>
+      <c r="N19" s="49" t="n">
+        <v>45992</v>
       </c>
       <c r="O19" s="6" t="inlineStr">
         <is>
@@ -2174,19 +2174,19 @@
         </is>
       </c>
       <c r="Q19" s="38" t="n">
+        <v>0.02653312468710926</v>
+      </c>
+      <c r="R19" s="38" t="n">
         <v>0.0271196938527219</v>
       </c>
-      <c r="R19" s="38" t="n">
+      <c r="S19" s="38" t="n">
         <v/>
       </c>
-      <c r="S19" s="38" t="n">
+      <c r="T19" s="38" t="n">
         <v>0.03022699626172379</v>
       </c>
-      <c r="T19" s="38" t="n">
+      <c r="U19" s="23" t="n">
         <v>0.02939219624933549</v>
-      </c>
-      <c r="U19" s="23" t="n">
-        <v>0.02731801279475463</v>
       </c>
     </row>
     <row r="20">
@@ -2235,8 +2235,8 @@
           <t>CPILFESL</t>
         </is>
       </c>
-      <c r="N20" s="48" t="n">
-        <v>45962</v>
+      <c r="N20" s="49" t="n">
+        <v>45992</v>
       </c>
       <c r="O20" s="6" t="inlineStr">
         <is>
@@ -2249,19 +2249,19 @@
         </is>
       </c>
       <c r="Q20" s="38" t="n">
-        <v/>
+        <v>0.00239225778389951</v>
       </c>
       <c r="R20" s="38" t="n">
         <v/>
       </c>
       <c r="S20" s="38" t="n">
+        <v/>
+      </c>
+      <c r="T20" s="38" t="n">
         <v>0.002271121582325675</v>
       </c>
-      <c r="T20" s="38" t="n">
+      <c r="U20" s="23" t="n">
         <v>0.003459544325982167</v>
-      </c>
-      <c r="U20" s="23" t="n">
-        <v>0.003223443223443256</v>
       </c>
     </row>
     <row r="21">
@@ -2310,8 +2310,8 @@
           <t>CPILFESL</t>
         </is>
       </c>
-      <c r="N21" s="48" t="n">
-        <v>45962</v>
+      <c r="N21" s="49" t="n">
+        <v>45992</v>
       </c>
       <c r="O21" s="6" t="inlineStr">
         <is>
@@ -2324,19 +2324,19 @@
         </is>
       </c>
       <c r="Q21" s="38" t="n">
+        <v>0.02648965653766215</v>
+      </c>
+      <c r="R21" s="38" t="n">
         <v>0.02618878615332623</v>
       </c>
-      <c r="R21" s="38" t="n">
+      <c r="S21" s="38" t="n">
         <v/>
       </c>
-      <c r="S21" s="38" t="n">
+      <c r="T21" s="38" t="n">
         <v>0.03025542724453378</v>
       </c>
-      <c r="T21" s="38" t="n">
+      <c r="U21" s="23" t="n">
         <v>0.03112190821006822</v>
-      </c>
-      <c r="U21" s="23" t="n">
-        <v>0.03048602684576389</v>
       </c>
     </row>
     <row r="22">
@@ -2922,7 +2922,7 @@
         </is>
       </c>
       <c r="N29" s="49" t="n">
-        <v>46031</v>
+        <v>46034</v>
       </c>
       <c r="O29" s="6" t="inlineStr">
         <is>
@@ -2935,19 +2935,19 @@
         </is>
       </c>
       <c r="Q29" s="6" t="n">
+        <v>2.22</v>
+      </c>
+      <c r="R29" s="6" t="n">
         <v>2.24</v>
       </c>
-      <c r="R29" s="6" t="n">
+      <c r="S29" s="6" t="n">
         <v>2.23</v>
-      </c>
-      <c r="S29" s="6" t="n">
-        <v>2.24</v>
       </c>
       <c r="T29" s="6" t="n">
         <v>2.24</v>
       </c>
       <c r="U29" s="21" t="n">
-        <v>2.23</v>
+        <v>2.24</v>
       </c>
     </row>
     <row r="30">
@@ -3001,7 +3001,7 @@
         </is>
       </c>
       <c r="N30" s="49" t="n">
-        <v>46031</v>
+        <v>46034</v>
       </c>
       <c r="O30" s="6" t="inlineStr">
         <is>
@@ -3014,10 +3014,10 @@
         </is>
       </c>
       <c r="Q30" s="6" t="n">
+        <v>2.29</v>
+      </c>
+      <c r="R30" s="6" t="n">
         <v>2.28</v>
-      </c>
-      <c r="R30" s="6" t="n">
-        <v>2.27</v>
       </c>
       <c r="S30" s="6" t="n">
         <v>2.27</v>
@@ -3026,7 +3026,7 @@
         <v>2.27</v>
       </c>
       <c r="U30" s="21" t="n">
-        <v>2.26</v>
+        <v>2.27</v>
       </c>
     </row>
     <row r="31">
@@ -4268,7 +4268,7 @@
         </is>
       </c>
       <c r="N47" s="49" t="n">
-        <v>46030</v>
+        <v>46031</v>
       </c>
       <c r="O47" s="6" t="inlineStr">
         <is>
@@ -4347,7 +4347,7 @@
         </is>
       </c>
       <c r="N48" s="49" t="n">
-        <v>46030</v>
+        <v>46031</v>
       </c>
       <c r="O48" s="6" t="inlineStr">
         <is>
@@ -4360,19 +4360,19 @@
         </is>
       </c>
       <c r="Q48" s="6" t="n">
+        <v>3.54</v>
+      </c>
+      <c r="R48" s="6" t="n">
         <v>3.49</v>
-      </c>
-      <c r="R48" s="6" t="n">
-        <v>3.47</v>
       </c>
       <c r="S48" s="6" t="n">
         <v>3.47</v>
       </c>
       <c r="T48" s="6" t="n">
+        <v>3.47</v>
+      </c>
+      <c r="U48" s="21" t="n">
         <v>3.46</v>
-      </c>
-      <c r="U48" s="21" t="n">
-        <v>3.47</v>
       </c>
     </row>
     <row r="49">
@@ -4422,7 +4422,7 @@
         </is>
       </c>
       <c r="N49" s="49" t="n">
-        <v>46030</v>
+        <v>46031</v>
       </c>
       <c r="O49" s="6" t="inlineStr">
         <is>
@@ -4435,19 +4435,19 @@
         </is>
       </c>
       <c r="Q49" s="6" t="n">
+        <v>3.75</v>
+      </c>
+      <c r="R49" s="6" t="n">
         <v>3.74</v>
       </c>
-      <c r="R49" s="6" t="n">
+      <c r="S49" s="6" t="n">
         <v>3.7</v>
       </c>
-      <c r="S49" s="6" t="n">
+      <c r="T49" s="6" t="n">
         <v>3.72</v>
       </c>
-      <c r="T49" s="6" t="n">
+      <c r="U49" s="21" t="n">
         <v>3.71</v>
-      </c>
-      <c r="U49" s="21" t="n">
-        <v>3.74</v>
       </c>
     </row>
     <row r="50">
@@ -4501,7 +4501,7 @@
         </is>
       </c>
       <c r="N50" s="49" t="n">
-        <v>46030</v>
+        <v>46031</v>
       </c>
       <c r="O50" s="6" t="inlineStr">
         <is>
@@ -4514,19 +4514,19 @@
         </is>
       </c>
       <c r="Q50" s="6" t="n">
+        <v>4.18</v>
+      </c>
+      <c r="R50" s="6" t="n">
         <v>4.19</v>
       </c>
-      <c r="R50" s="6" t="n">
+      <c r="S50" s="6" t="n">
         <v>4.15</v>
       </c>
-      <c r="S50" s="6" t="n">
+      <c r="T50" s="6" t="n">
         <v>4.18</v>
       </c>
-      <c r="T50" s="6" t="n">
+      <c r="U50" s="21" t="n">
         <v>4.17</v>
-      </c>
-      <c r="U50" s="21" t="n">
-        <v>4.19</v>
       </c>
     </row>
     <row r="51" ht="31.5" customHeight="1">
@@ -4627,7 +4627,7 @@
         </is>
       </c>
       <c r="N52" s="53" t="n">
-        <v>46030</v>
+        <v>46031</v>
       </c>
       <c r="O52" s="9" t="inlineStr">
         <is>
@@ -4640,19 +4640,19 @@
         </is>
       </c>
       <c r="Q52" s="9" t="n">
+        <v>5.88</v>
+      </c>
+      <c r="R52" s="9" t="n">
         <v>5.92</v>
       </c>
-      <c r="R52" s="9" t="n">
+      <c r="S52" s="9" t="n">
         <v>5.88</v>
-      </c>
-      <c r="S52" s="9" t="n">
-        <v>5.92</v>
       </c>
       <c r="T52" s="9" t="n">
         <v>5.92</v>
       </c>
       <c r="U52" s="22" t="n">
-        <v>5.93</v>
+        <v>5.92</v>
       </c>
     </row>
     <row r="53" ht="21" customHeight="1">

</xml_diff>

<commit_message>
Update dashboards - 2026-01-14
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -1098,7 +1098,7 @@
           <t>ADPMNUSNERSA</t>
         </is>
       </c>
-      <c r="N5" s="49" t="n">
+      <c r="N5" s="48" t="n">
         <v>45992</v>
       </c>
       <c r="O5" s="6" t="inlineStr">
@@ -1485,7 +1485,7 @@
           <t>JTSJOR</t>
         </is>
       </c>
-      <c r="N10" s="49" t="n">
+      <c r="N10" s="48" t="n">
         <v>45962</v>
       </c>
       <c r="O10" s="6" t="inlineStr">
@@ -1564,7 +1564,7 @@
           <t>JTSHIR</t>
         </is>
       </c>
-      <c r="N11" s="49" t="n">
+      <c r="N11" s="48" t="n">
         <v>45962</v>
       </c>
       <c r="O11" s="6" t="inlineStr">
@@ -1639,7 +1639,7 @@
           <t>JTSTSR</t>
         </is>
       </c>
-      <c r="N12" s="49" t="n">
+      <c r="N12" s="48" t="n">
         <v>45962</v>
       </c>
       <c r="O12" s="6" t="inlineStr">
@@ -1959,8 +1959,8 @@
           <t>RSAFS</t>
         </is>
       </c>
-      <c r="C17" s="48" t="n">
-        <v>45931</v>
+      <c r="C17" s="49" t="n">
+        <v>45962</v>
       </c>
       <c r="D17" s="6" t="inlineStr">
         <is>
@@ -1973,19 +1973,19 @@
         </is>
       </c>
       <c r="F17" s="25" t="n">
-        <v>0.0002580402051215458</v>
+        <v>0.006141545394387826</v>
       </c>
       <c r="G17" s="25" t="n">
-        <v>0.001016810168101623</v>
+        <v>-0.001065294349023249</v>
       </c>
       <c r="H17" s="25" t="n">
+        <v>0.0006724067240673204</v>
+      </c>
+      <c r="I17" s="25" t="n">
         <v>0.00545946488174831</v>
       </c>
-      <c r="I17" s="25" t="n">
+      <c r="J17" s="25" t="n">
         <v>0.006492096487988874</v>
-      </c>
-      <c r="J17" s="25" t="n">
-        <v>0.009680198742914703</v>
       </c>
       <c r="K17" s="5" t="n"/>
       <c r="L17" s="29" t="inlineStr">
@@ -2046,8 +2046,8 @@
           <t>RSAFS</t>
         </is>
       </c>
-      <c r="C18" s="48" t="n">
-        <v>45931</v>
+      <c r="C18" s="49" t="n">
+        <v>45962</v>
       </c>
       <c r="D18" s="6" t="inlineStr">
         <is>
@@ -2060,19 +2060,19 @@
         </is>
       </c>
       <c r="F18" s="25" t="n">
-        <v>0.03469007301537984</v>
+        <v>0.03331905781584583</v>
       </c>
       <c r="G18" s="25" t="n">
-        <v>0.0418018504953382</v>
+        <v>0.03264482062432054</v>
       </c>
       <c r="H18" s="25" t="n">
+        <v>0.04144341481107452</v>
+      </c>
+      <c r="I18" s="25" t="n">
         <v>0.04972605550048132</v>
       </c>
-      <c r="I18" s="25" t="n">
+      <c r="J18" s="25" t="n">
         <v>0.04134309243240536</v>
-      </c>
-      <c r="J18" s="25" t="n">
-        <v>0.0441678737351054</v>
       </c>
       <c r="K18" s="5" t="n"/>
       <c r="L18" s="28" t="inlineStr">
@@ -2922,7 +2922,7 @@
         </is>
       </c>
       <c r="N29" s="49" t="n">
-        <v>46034</v>
+        <v>46035</v>
       </c>
       <c r="O29" s="6" t="inlineStr">
         <is>
@@ -2935,16 +2935,16 @@
         </is>
       </c>
       <c r="Q29" s="6" t="n">
+        <v>2.23</v>
+      </c>
+      <c r="R29" s="6" t="n">
         <v>2.22</v>
       </c>
-      <c r="R29" s="6" t="n">
+      <c r="S29" s="6" t="n">
         <v>2.24</v>
       </c>
-      <c r="S29" s="6" t="n">
+      <c r="T29" s="6" t="n">
         <v>2.23</v>
-      </c>
-      <c r="T29" s="6" t="n">
-        <v>2.24</v>
       </c>
       <c r="U29" s="21" t="n">
         <v>2.24</v>
@@ -3001,7 +3001,7 @@
         </is>
       </c>
       <c r="N30" s="49" t="n">
-        <v>46034</v>
+        <v>46035</v>
       </c>
       <c r="O30" s="6" t="inlineStr">
         <is>
@@ -3014,13 +3014,13 @@
         </is>
       </c>
       <c r="Q30" s="6" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="R30" s="6" t="n">
         <v>2.29</v>
       </c>
-      <c r="R30" s="6" t="n">
+      <c r="S30" s="6" t="n">
         <v>2.28</v>
-      </c>
-      <c r="S30" s="6" t="n">
-        <v>2.27</v>
       </c>
       <c r="T30" s="6" t="n">
         <v>2.27</v>
@@ -3719,8 +3719,8 @@
           <t>HSN1F</t>
         </is>
       </c>
-      <c r="C40" s="48" t="n">
-        <v>45870</v>
+      <c r="C40" s="49" t="n">
+        <v>45931</v>
       </c>
       <c r="D40" s="6" t="inlineStr">
         <is>
@@ -3733,19 +3733,19 @@
         </is>
       </c>
       <c r="F40" s="24" t="n">
-        <v>800</v>
+        <v>737</v>
       </c>
       <c r="G40" s="24" t="n">
-        <v>664</v>
+        <v>738</v>
       </c>
       <c r="H40" s="24" t="n">
-        <v>676</v>
+        <v>711</v>
       </c>
       <c r="I40" s="24" t="n">
-        <v>627</v>
+        <v>639</v>
       </c>
       <c r="J40" s="24" t="n">
-        <v>706</v>
+        <v>662</v>
       </c>
       <c r="K40" s="5" t="n"/>
       <c r="L40" s="28" t="n"/>
@@ -3790,8 +3790,8 @@
           <t>HSN1F</t>
         </is>
       </c>
-      <c r="C41" s="48" t="n">
-        <v>45870</v>
+      <c r="C41" s="49" t="n">
+        <v>45931</v>
       </c>
       <c r="D41" s="6" t="inlineStr">
         <is>
@@ -3804,19 +3804,19 @@
         </is>
       </c>
       <c r="F41" s="38" t="n">
-        <v>0.1544011544011544</v>
+        <v>0.1867954911433172</v>
       </c>
       <c r="G41" s="38" t="n">
-        <v>-0.06478873239436619</v>
+        <v>0.02928870292887029</v>
       </c>
       <c r="H41" s="38" t="n">
-        <v>0.007451564828614009</v>
+        <v>0.02597402597402598</v>
       </c>
       <c r="I41" s="38" t="n">
-        <v>-0.05714285714285714</v>
+        <v>-0.1</v>
       </c>
       <c r="J41" s="38" t="n">
-        <v>-0.01808066759388039</v>
+        <v>-0.01341281669150522</v>
       </c>
       <c r="K41" s="5" t="n"/>
       <c r="L41" s="28" t="inlineStr">
@@ -4268,7 +4268,7 @@
         </is>
       </c>
       <c r="N47" s="49" t="n">
-        <v>46031</v>
+        <v>46034</v>
       </c>
       <c r="O47" s="6" t="inlineStr">
         <is>
@@ -4347,7 +4347,7 @@
         </is>
       </c>
       <c r="N48" s="49" t="n">
-        <v>46031</v>
+        <v>46034</v>
       </c>
       <c r="O48" s="6" t="inlineStr">
         <is>
@@ -4363,16 +4363,16 @@
         <v>3.54</v>
       </c>
       <c r="R48" s="6" t="n">
+        <v>3.54</v>
+      </c>
+      <c r="S48" s="6" t="n">
         <v>3.49</v>
-      </c>
-      <c r="S48" s="6" t="n">
-        <v>3.47</v>
       </c>
       <c r="T48" s="6" t="n">
         <v>3.47</v>
       </c>
       <c r="U48" s="21" t="n">
-        <v>3.46</v>
+        <v>3.47</v>
       </c>
     </row>
     <row r="49">
@@ -4422,7 +4422,7 @@
         </is>
       </c>
       <c r="N49" s="49" t="n">
-        <v>46031</v>
+        <v>46034</v>
       </c>
       <c r="O49" s="6" t="inlineStr">
         <is>
@@ -4435,19 +4435,19 @@
         </is>
       </c>
       <c r="Q49" s="6" t="n">
+        <v>3.77</v>
+      </c>
+      <c r="R49" s="6" t="n">
         <v>3.75</v>
       </c>
-      <c r="R49" s="6" t="n">
+      <c r="S49" s="6" t="n">
         <v>3.74</v>
       </c>
-      <c r="S49" s="6" t="n">
+      <c r="T49" s="6" t="n">
         <v>3.7</v>
       </c>
-      <c r="T49" s="6" t="n">
+      <c r="U49" s="21" t="n">
         <v>3.72</v>
-      </c>
-      <c r="U49" s="21" t="n">
-        <v>3.71</v>
       </c>
     </row>
     <row r="50">
@@ -4501,7 +4501,7 @@
         </is>
       </c>
       <c r="N50" s="49" t="n">
-        <v>46031</v>
+        <v>46034</v>
       </c>
       <c r="O50" s="6" t="inlineStr">
         <is>
@@ -4514,19 +4514,19 @@
         </is>
       </c>
       <c r="Q50" s="6" t="n">
+        <v>4.19</v>
+      </c>
+      <c r="R50" s="6" t="n">
         <v>4.18</v>
       </c>
-      <c r="R50" s="6" t="n">
+      <c r="S50" s="6" t="n">
         <v>4.19</v>
       </c>
-      <c r="S50" s="6" t="n">
+      <c r="T50" s="6" t="n">
         <v>4.15</v>
       </c>
-      <c r="T50" s="6" t="n">
+      <c r="U50" s="21" t="n">
         <v>4.18</v>
-      </c>
-      <c r="U50" s="21" t="n">
-        <v>4.17</v>
       </c>
     </row>
     <row r="51" ht="31.5" customHeight="1">
@@ -4627,7 +4627,7 @@
         </is>
       </c>
       <c r="N52" s="53" t="n">
-        <v>46031</v>
+        <v>46034</v>
       </c>
       <c r="O52" s="9" t="inlineStr">
         <is>
@@ -4640,16 +4640,16 @@
         </is>
       </c>
       <c r="Q52" s="9" t="n">
+        <v>5.89</v>
+      </c>
+      <c r="R52" s="9" t="n">
         <v>5.88</v>
       </c>
-      <c r="R52" s="9" t="n">
+      <c r="S52" s="9" t="n">
         <v>5.92</v>
       </c>
-      <c r="S52" s="9" t="n">
+      <c r="T52" s="9" t="n">
         <v>5.88</v>
-      </c>
-      <c r="T52" s="9" t="n">
-        <v>5.92</v>
       </c>
       <c r="U52" s="22" t="n">
         <v>5.92</v>

</xml_diff>

<commit_message>
Update dashboards - 2026-01-15
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -1719,7 +1719,7 @@
         </is>
       </c>
       <c r="N13" s="49" t="n">
-        <v>46020</v>
+        <v>46027</v>
       </c>
       <c r="O13" s="6" t="inlineStr">
         <is>
@@ -1732,19 +1732,19 @@
         </is>
       </c>
       <c r="Q13" s="24" t="n">
-        <v>208000</v>
+        <v>198000</v>
       </c>
       <c r="R13" s="24" t="n">
+        <v>207000</v>
+      </c>
+      <c r="S13" s="24" t="n">
         <v>200000</v>
       </c>
-      <c r="S13" s="24" t="n">
+      <c r="T13" s="24" t="n">
         <v>215000</v>
       </c>
-      <c r="T13" s="24" t="n">
+      <c r="U13" s="26" t="n">
         <v>224000</v>
-      </c>
-      <c r="U13" s="26" t="n">
-        <v>237000</v>
       </c>
     </row>
     <row r="14">
@@ -1794,7 +1794,7 @@
         </is>
       </c>
       <c r="N14" s="49" t="n">
-        <v>46013</v>
+        <v>46020</v>
       </c>
       <c r="O14" s="6" t="inlineStr">
         <is>
@@ -1807,19 +1807,19 @@
         </is>
       </c>
       <c r="Q14" s="24" t="n">
+        <v>1884000</v>
+      </c>
+      <c r="R14" s="24" t="n">
+        <v>1903000</v>
+      </c>
+      <c r="S14" s="24" t="n">
+        <v>1856000</v>
+      </c>
+      <c r="T14" s="24" t="n">
         <v>1914000</v>
       </c>
-      <c r="R14" s="24" t="n">
-        <v>1858000</v>
-      </c>
-      <c r="S14" s="24" t="n">
-        <v>1914000</v>
-      </c>
-      <c r="T14" s="24" t="n">
+      <c r="U14" s="26" t="n">
         <v>1885000</v>
-      </c>
-      <c r="U14" s="26" t="n">
-        <v>1830000</v>
       </c>
     </row>
     <row r="15">
@@ -2389,8 +2389,8 @@
           <t>PPIFIS</t>
         </is>
       </c>
-      <c r="N22" s="48" t="n">
-        <v>45901</v>
+      <c r="N22" s="49" t="n">
+        <v>45962</v>
       </c>
       <c r="O22" s="6" t="inlineStr">
         <is>
@@ -2403,19 +2403,19 @@
         </is>
       </c>
       <c r="Q22" s="38" t="n">
-        <v>0.003100806343593332</v>
+        <v>0.002481174999334979</v>
       </c>
       <c r="R22" s="38" t="n">
-        <v>-0.001357686982925266</v>
+        <v>0.001165446832315453</v>
       </c>
       <c r="S22" s="38" t="n">
-        <v>0.0081178572632572</v>
+        <v>0.005928774318023633</v>
       </c>
       <c r="T22" s="38" t="n">
-        <v>0.0007422151749265637</v>
+        <v>-0.001765461159854542</v>
       </c>
       <c r="U22" s="23" t="n">
-        <v>0.003514212586162468</v>
+        <v>0.007967429257047298</v>
       </c>
     </row>
     <row r="23">
@@ -2459,8 +2459,8 @@
           <t>PPIFIS</t>
         </is>
       </c>
-      <c r="N23" s="48" t="n">
-        <v>45901</v>
+      <c r="N23" s="49" t="n">
+        <v>45962</v>
       </c>
       <c r="O23" s="6" t="inlineStr">
         <is>
@@ -2473,19 +2473,19 @@
         </is>
       </c>
       <c r="Q23" s="38" t="n">
-        <v>0.02734717954345914</v>
+        <v>0.02946902473512731</v>
       </c>
       <c r="R23" s="38" t="n">
-        <v>0.02721518987341764</v>
+        <v>0.02796734180331234</v>
       </c>
       <c r="S23" s="38" t="n">
-        <v>0.0320979643678082</v>
+        <v>0.02993991439859532</v>
       </c>
       <c r="T23" s="38" t="n">
-        <v>0.02406976503324603</v>
+        <v>0.02691249312052819</v>
       </c>
       <c r="U23" s="23" t="n">
-        <v>0.02738206647949823</v>
+        <v>0.03221531176442166</v>
       </c>
     </row>
     <row r="24">
@@ -2499,7 +2499,7 @@
           <t>REVOLSL</t>
         </is>
       </c>
-      <c r="C24" s="49" t="n">
+      <c r="C24" s="48" t="n">
         <v>45962</v>
       </c>
       <c r="D24" s="6" t="inlineStr">
@@ -2578,7 +2578,7 @@
           <t>NONREVSL</t>
         </is>
       </c>
-      <c r="C25" s="49" t="n">
+      <c r="C25" s="48" t="n">
         <v>45962</v>
       </c>
       <c r="D25" s="6" t="inlineStr">
@@ -2922,7 +2922,7 @@
         </is>
       </c>
       <c r="N29" s="49" t="n">
-        <v>46035</v>
+        <v>46036</v>
       </c>
       <c r="O29" s="6" t="inlineStr">
         <is>
@@ -2935,19 +2935,19 @@
         </is>
       </c>
       <c r="Q29" s="6" t="n">
+        <v>2.22</v>
+      </c>
+      <c r="R29" s="6" t="n">
         <v>2.23</v>
       </c>
-      <c r="R29" s="6" t="n">
+      <c r="S29" s="6" t="n">
         <v>2.22</v>
       </c>
-      <c r="S29" s="6" t="n">
+      <c r="T29" s="6" t="n">
         <v>2.24</v>
       </c>
-      <c r="T29" s="6" t="n">
+      <c r="U29" s="21" t="n">
         <v>2.23</v>
-      </c>
-      <c r="U29" s="21" t="n">
-        <v>2.24</v>
       </c>
     </row>
     <row r="30">
@@ -3001,7 +3001,7 @@
         </is>
       </c>
       <c r="N30" s="49" t="n">
-        <v>46035</v>
+        <v>46036</v>
       </c>
       <c r="O30" s="6" t="inlineStr">
         <is>
@@ -3014,16 +3014,16 @@
         </is>
       </c>
       <c r="Q30" s="6" t="n">
+        <v>2.29</v>
+      </c>
+      <c r="R30" s="6" t="n">
         <v>2.3</v>
       </c>
-      <c r="R30" s="6" t="n">
+      <c r="S30" s="6" t="n">
         <v>2.29</v>
       </c>
-      <c r="S30" s="6" t="n">
+      <c r="T30" s="6" t="n">
         <v>2.28</v>
-      </c>
-      <c r="T30" s="6" t="n">
-        <v>2.27</v>
       </c>
       <c r="U30" s="21" t="n">
         <v>2.27</v>
@@ -3340,7 +3340,7 @@
           <t>PRS85006092</t>
         </is>
       </c>
-      <c r="C35" s="49" t="n">
+      <c r="C35" s="48" t="n">
         <v>45839</v>
       </c>
       <c r="D35" s="6" t="inlineStr">
@@ -3829,8 +3829,8 @@
           <t>IQ</t>
         </is>
       </c>
-      <c r="N41" s="48" t="n">
-        <v>45901</v>
+      <c r="N41" s="49" t="n">
+        <v>45962</v>
       </c>
       <c r="O41" s="6" t="inlineStr">
         <is>
@@ -3843,19 +3843,19 @@
         </is>
       </c>
       <c r="Q41" s="38" t="n">
+        <v/>
+      </c>
+      <c r="R41" s="38" t="n">
+        <v/>
+      </c>
+      <c r="S41" s="38" t="n">
         <v>0</v>
       </c>
-      <c r="R41" s="38" t="n">
-        <v>0.0006544502617800152</v>
-      </c>
-      <c r="S41" s="38" t="n">
+      <c r="T41" s="38" t="n">
+        <v>0.00130890052356003</v>
+      </c>
+      <c r="U41" s="23" t="n">
         <v>0.003282994090610725</v>
-      </c>
-      <c r="T41" s="38" t="n">
-        <v>0.004617414248021312</v>
-      </c>
-      <c r="U41" s="23" t="n">
-        <v>-0.006553079947575369</v>
       </c>
     </row>
     <row r="42">
@@ -3870,7 +3870,7 @@
         </is>
       </c>
       <c r="C42" s="48" t="n">
-        <v>45962</v>
+        <v>45992</v>
       </c>
       <c r="D42" s="6" t="inlineStr">
         <is>
@@ -3883,19 +3883,19 @@
         </is>
       </c>
       <c r="F42" s="39" t="n">
-        <v>4130000</v>
+        <v>4350000</v>
       </c>
       <c r="G42" s="39" t="n">
+        <v>4140000</v>
+      </c>
+      <c r="H42" s="39" t="n">
         <v>4110000</v>
       </c>
-      <c r="H42" s="39" t="n">
+      <c r="I42" s="39" t="n">
         <v>4050000</v>
       </c>
-      <c r="I42" s="39" t="n">
+      <c r="J42" s="39" t="n">
         <v>4000000</v>
-      </c>
-      <c r="J42" s="39" t="n">
-        <v>4010000</v>
       </c>
       <c r="K42" s="7" t="n"/>
       <c r="L42" s="28" t="n"/>
@@ -3904,8 +3904,8 @@
           <t>IQ</t>
         </is>
       </c>
-      <c r="N42" s="48" t="n">
-        <v>45901</v>
+      <c r="N42" s="49" t="n">
+        <v>45962</v>
       </c>
       <c r="O42" s="6" t="inlineStr">
         <is>
@@ -3918,19 +3918,19 @@
         </is>
       </c>
       <c r="Q42" s="38" t="n">
-        <v>0.03801765105227423</v>
+        <v>0.03293010752688157</v>
       </c>
       <c r="R42" s="38" t="n">
-        <v>0.03171390013495289</v>
+        <v/>
       </c>
       <c r="S42" s="38" t="n">
+        <v>0.03869653767820766</v>
+      </c>
+      <c r="T42" s="38" t="n">
+        <v>0.03238866396761141</v>
+      </c>
+      <c r="U42" s="23" t="n">
         <v>0.0241286863270779</v>
-      </c>
-      <c r="T42" s="38" t="n">
-        <v>0.02628032345013481</v>
-      </c>
-      <c r="U42" s="23" t="n">
-        <v>0.01881720430107515</v>
       </c>
     </row>
     <row r="43">
@@ -3941,7 +3941,7 @@
         </is>
       </c>
       <c r="C43" s="48" t="n">
-        <v>45962</v>
+        <v>45992</v>
       </c>
       <c r="D43" s="6" t="inlineStr">
         <is>
@@ -3954,7 +3954,7 @@
         </is>
       </c>
       <c r="F43" s="38" t="n">
-        <v>-0.009592326139088728</v>
+        <v>0.01398601398601399</v>
       </c>
       <c r="G43" s="38" t="n">
         <v/>
@@ -3979,8 +3979,8 @@
           <t>IR</t>
         </is>
       </c>
-      <c r="N43" s="48" t="n">
-        <v>45901</v>
+      <c r="N43" s="49" t="n">
+        <v>45962</v>
       </c>
       <c r="O43" s="6" t="inlineStr">
         <is>
@@ -3993,19 +3993,19 @@
         </is>
       </c>
       <c r="Q43" s="38" t="n">
-        <v>0</v>
+        <v/>
       </c>
       <c r="R43" s="38" t="n">
-        <v>0.0007082152974506872</v>
+        <v/>
       </c>
       <c r="S43" s="38" t="n">
+        <v>-0.0007092198581559739</v>
+      </c>
+      <c r="T43" s="38" t="n">
+        <v>-0.001416430594900819</v>
+      </c>
+      <c r="U43" s="23" t="n">
         <v>0.00284090909090895</v>
-      </c>
-      <c r="T43" s="38" t="n">
-        <v>-0.001418439716311948</v>
-      </c>
-      <c r="U43" s="23" t="n">
-        <v>-0.004940014114325986</v>
       </c>
     </row>
     <row r="44">
@@ -4054,8 +4054,8 @@
           <t>IR</t>
         </is>
       </c>
-      <c r="N44" s="48" t="n">
-        <v>45901</v>
+      <c r="N44" s="49" t="n">
+        <v>45962</v>
       </c>
       <c r="O44" s="6" t="inlineStr">
         <is>
@@ -4068,19 +4068,19 @@
         </is>
       </c>
       <c r="Q44" s="38" t="n">
-        <v>0.00283889283179564</v>
+        <v>0.0007077140835102215</v>
       </c>
       <c r="R44" s="38" t="n">
-        <v>-0.000707213578500667</v>
+        <v/>
       </c>
       <c r="S44" s="38" t="n">
+        <v>0</v>
+      </c>
+      <c r="T44" s="38" t="n">
+        <v>-0.002828854314002869</v>
+      </c>
+      <c r="U44" s="23" t="n">
         <v>-0.004231311706629215</v>
-      </c>
-      <c r="T44" s="38" t="n">
-        <v>-0.005649717514124173</v>
-      </c>
-      <c r="U44" s="23" t="n">
-        <v>-0.00353356890459364</v>
       </c>
     </row>
     <row r="45">
@@ -4141,7 +4141,7 @@
           <t>BOPTEXP</t>
         </is>
       </c>
-      <c r="C46" s="49" t="n">
+      <c r="C46" s="48" t="n">
         <v>45931</v>
       </c>
       <c r="D46" s="6" t="inlineStr">
@@ -4228,7 +4228,7 @@
           <t>BOPTEXP</t>
         </is>
       </c>
-      <c r="C47" s="49" t="n">
+      <c r="C47" s="48" t="n">
         <v>45931</v>
       </c>
       <c r="D47" s="6" t="inlineStr">
@@ -4268,7 +4268,7 @@
         </is>
       </c>
       <c r="N47" s="49" t="n">
-        <v>46034</v>
+        <v>46035</v>
       </c>
       <c r="O47" s="6" t="inlineStr">
         <is>
@@ -4307,7 +4307,7 @@
           <t>BOPTIMP</t>
         </is>
       </c>
-      <c r="C48" s="49" t="n">
+      <c r="C48" s="48" t="n">
         <v>45931</v>
       </c>
       <c r="D48" s="6" t="inlineStr">
@@ -4347,7 +4347,7 @@
         </is>
       </c>
       <c r="N48" s="49" t="n">
-        <v>46034</v>
+        <v>46035</v>
       </c>
       <c r="O48" s="6" t="inlineStr">
         <is>
@@ -4360,16 +4360,16 @@
         </is>
       </c>
       <c r="Q48" s="6" t="n">
-        <v>3.54</v>
+        <v>3.53</v>
       </c>
       <c r="R48" s="6" t="n">
         <v>3.54</v>
       </c>
       <c r="S48" s="6" t="n">
+        <v>3.54</v>
+      </c>
+      <c r="T48" s="6" t="n">
         <v>3.49</v>
-      </c>
-      <c r="T48" s="6" t="n">
-        <v>3.47</v>
       </c>
       <c r="U48" s="21" t="n">
         <v>3.47</v>
@@ -4382,7 +4382,7 @@
           <t>BOPTIMP</t>
         </is>
       </c>
-      <c r="C49" s="49" t="n">
+      <c r="C49" s="48" t="n">
         <v>45931</v>
       </c>
       <c r="D49" s="6" t="inlineStr">
@@ -4422,7 +4422,7 @@
         </is>
       </c>
       <c r="N49" s="49" t="n">
-        <v>46034</v>
+        <v>46035</v>
       </c>
       <c r="O49" s="6" t="inlineStr">
         <is>
@@ -4435,19 +4435,19 @@
         </is>
       </c>
       <c r="Q49" s="6" t="n">
+        <v>3.75</v>
+      </c>
+      <c r="R49" s="6" t="n">
         <v>3.77</v>
       </c>
-      <c r="R49" s="6" t="n">
+      <c r="S49" s="6" t="n">
         <v>3.75</v>
       </c>
-      <c r="S49" s="6" t="n">
+      <c r="T49" s="6" t="n">
         <v>3.74</v>
       </c>
-      <c r="T49" s="6" t="n">
+      <c r="U49" s="21" t="n">
         <v>3.7</v>
-      </c>
-      <c r="U49" s="21" t="n">
-        <v>3.72</v>
       </c>
     </row>
     <row r="50">
@@ -4461,7 +4461,7 @@
           <t>BOPSTB</t>
         </is>
       </c>
-      <c r="C50" s="49" t="n">
+      <c r="C50" s="48" t="n">
         <v>45931</v>
       </c>
       <c r="D50" s="6" t="inlineStr">
@@ -4501,7 +4501,7 @@
         </is>
       </c>
       <c r="N50" s="49" t="n">
-        <v>46034</v>
+        <v>46035</v>
       </c>
       <c r="O50" s="6" t="inlineStr">
         <is>
@@ -4514,19 +4514,19 @@
         </is>
       </c>
       <c r="Q50" s="6" t="n">
+        <v>4.18</v>
+      </c>
+      <c r="R50" s="6" t="n">
         <v>4.19</v>
       </c>
-      <c r="R50" s="6" t="n">
+      <c r="S50" s="6" t="n">
         <v>4.18</v>
       </c>
-      <c r="S50" s="6" t="n">
+      <c r="T50" s="6" t="n">
         <v>4.19</v>
       </c>
-      <c r="T50" s="6" t="n">
+      <c r="U50" s="21" t="n">
         <v>4.15</v>
-      </c>
-      <c r="U50" s="21" t="n">
-        <v>4.18</v>
       </c>
     </row>
     <row r="51" ht="31.5" customHeight="1">
@@ -4536,7 +4536,7 @@
           <t>BOPSTB</t>
         </is>
       </c>
-      <c r="C51" s="49" t="n">
+      <c r="C51" s="48" t="n">
         <v>45931</v>
       </c>
       <c r="D51" s="6" t="inlineStr">
@@ -4575,7 +4575,7 @@
           <t>MORTGAGE30US</t>
         </is>
       </c>
-      <c r="N51" s="49" t="n">
+      <c r="N51" s="48" t="n">
         <v>46027</v>
       </c>
       <c r="O51" s="6" t="inlineStr">
@@ -4627,7 +4627,7 @@
         </is>
       </c>
       <c r="N52" s="53" t="n">
-        <v>46034</v>
+        <v>46035</v>
       </c>
       <c r="O52" s="9" t="inlineStr">
         <is>
@@ -4640,19 +4640,19 @@
         </is>
       </c>
       <c r="Q52" s="9" t="n">
+        <v>5.87</v>
+      </c>
+      <c r="R52" s="9" t="n">
         <v>5.89</v>
       </c>
-      <c r="R52" s="9" t="n">
+      <c r="S52" s="9" t="n">
         <v>5.88</v>
       </c>
-      <c r="S52" s="9" t="n">
+      <c r="T52" s="9" t="n">
         <v>5.92</v>
       </c>
-      <c r="T52" s="9" t="n">
+      <c r="U52" s="22" t="n">
         <v>5.88</v>
-      </c>
-      <c r="U52" s="22" t="n">
-        <v>5.92</v>
       </c>
     </row>
     <row r="53" ht="21" customHeight="1">

</xml_diff>

<commit_message>
Update dashboards - 2026-01-16
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -77,14 +77,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FFFF00"/>
-        <bgColor rgb="00FFFF00"/>
+        <fgColor rgb="00CCFFCC"/>
+        <bgColor rgb="00CCFFCC"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00CCFFCC"/>
-        <bgColor rgb="00CCFFCC"/>
+        <fgColor rgb="00FFFF00"/>
+        <bgColor rgb="00FFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -363,19 +363,19 @@
     <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="1" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="4" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="1" fillId="3" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="168" fontId="1" fillId="4" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -948,7 +948,7 @@
           <t>PAYEMS</t>
         </is>
       </c>
-      <c r="N3" s="49" t="n">
+      <c r="N3" s="48" t="n">
         <v>45992</v>
       </c>
       <c r="O3" s="6" t="inlineStr">
@@ -1019,7 +1019,7 @@
           <t>PAYEMS</t>
         </is>
       </c>
-      <c r="N4" s="49" t="n">
+      <c r="N4" s="48" t="n">
         <v>45992</v>
       </c>
       <c r="O4" s="6" t="inlineStr">
@@ -1123,7 +1123,7 @@
       <c r="T5" s="24" t="n">
         <v>-29000</v>
       </c>
-      <c r="U5" s="50" t="n">
+      <c r="U5" s="49" t="n">
         <v>-3000</v>
       </c>
     </row>
@@ -1173,7 +1173,7 @@
           <t>UNRATE</t>
         </is>
       </c>
-      <c r="N6" s="49" t="n">
+      <c r="N6" s="48" t="n">
         <v>45992</v>
       </c>
       <c r="O6" s="6" t="inlineStr">
@@ -1252,7 +1252,7 @@
           <t>U6RATE</t>
         </is>
       </c>
-      <c r="N7" s="49" t="n">
+      <c r="N7" s="48" t="n">
         <v>45992</v>
       </c>
       <c r="O7" s="6" t="inlineStr">
@@ -1331,7 +1331,7 @@
           <t>CIVPART</t>
         </is>
       </c>
-      <c r="N8" s="49" t="n">
+      <c r="N8" s="48" t="n">
         <v>45992</v>
       </c>
       <c r="O8" s="6" t="inlineStr">
@@ -1410,7 +1410,7 @@
           <t>EMRATIO</t>
         </is>
       </c>
-      <c r="N9" s="49" t="n">
+      <c r="N9" s="48" t="n">
         <v>45992</v>
       </c>
       <c r="O9" s="6" t="inlineStr">
@@ -1718,7 +1718,7 @@
           <t>ICSA</t>
         </is>
       </c>
-      <c r="N13" s="49" t="n">
+      <c r="N13" s="50" t="n">
         <v>46027</v>
       </c>
       <c r="O13" s="6" t="inlineStr">
@@ -1793,7 +1793,7 @@
           <t>CCSA</t>
         </is>
       </c>
-      <c r="N14" s="49" t="n">
+      <c r="N14" s="50" t="n">
         <v>46020</v>
       </c>
       <c r="O14" s="6" t="inlineStr">
@@ -1872,7 +1872,7 @@
           <t>AWHAETP</t>
         </is>
       </c>
-      <c r="N15" s="49" t="n">
+      <c r="N15" s="48" t="n">
         <v>45992</v>
       </c>
       <c r="O15" s="6" t="inlineStr">
@@ -1959,7 +1959,7 @@
           <t>RSAFS</t>
         </is>
       </c>
-      <c r="C17" s="49" t="n">
+      <c r="C17" s="50" t="n">
         <v>45962</v>
       </c>
       <c r="D17" s="6" t="inlineStr">
@@ -2046,7 +2046,7 @@
           <t>RSAFS</t>
         </is>
       </c>
-      <c r="C18" s="49" t="n">
+      <c r="C18" s="50" t="n">
         <v>45962</v>
       </c>
       <c r="D18" s="6" t="inlineStr">
@@ -2085,7 +2085,7 @@
           <t>CPIAUCSL</t>
         </is>
       </c>
-      <c r="N18" s="49" t="n">
+      <c r="N18" s="50" t="n">
         <v>45992</v>
       </c>
       <c r="O18" s="6" t="inlineStr">
@@ -2160,7 +2160,7 @@
           <t>CPIAUCSL</t>
         </is>
       </c>
-      <c r="N19" s="49" t="n">
+      <c r="N19" s="50" t="n">
         <v>45992</v>
       </c>
       <c r="O19" s="6" t="inlineStr">
@@ -2235,7 +2235,7 @@
           <t>CPILFESL</t>
         </is>
       </c>
-      <c r="N20" s="49" t="n">
+      <c r="N20" s="50" t="n">
         <v>45992</v>
       </c>
       <c r="O20" s="6" t="inlineStr">
@@ -2310,7 +2310,7 @@
           <t>CPILFESL</t>
         </is>
       </c>
-      <c r="N21" s="49" t="n">
+      <c r="N21" s="50" t="n">
         <v>45992</v>
       </c>
       <c r="O21" s="6" t="inlineStr">
@@ -2389,7 +2389,7 @@
           <t>PPIFIS</t>
         </is>
       </c>
-      <c r="N22" s="49" t="n">
+      <c r="N22" s="50" t="n">
         <v>45962</v>
       </c>
       <c r="O22" s="6" t="inlineStr">
@@ -2459,7 +2459,7 @@
           <t>PPIFIS</t>
         </is>
       </c>
-      <c r="N23" s="49" t="n">
+      <c r="N23" s="50" t="n">
         <v>45962</v>
       </c>
       <c r="O23" s="6" t="inlineStr">
@@ -2921,8 +2921,8 @@
           <t>T5YIFR</t>
         </is>
       </c>
-      <c r="N29" s="49" t="n">
-        <v>46036</v>
+      <c r="N29" s="50" t="n">
+        <v>46037</v>
       </c>
       <c r="O29" s="6" t="inlineStr">
         <is>
@@ -2938,16 +2938,16 @@
         <v>2.22</v>
       </c>
       <c r="R29" s="6" t="n">
+        <v>2.22</v>
+      </c>
+      <c r="S29" s="6" t="n">
         <v>2.23</v>
       </c>
-      <c r="S29" s="6" t="n">
+      <c r="T29" s="6" t="n">
         <v>2.22</v>
       </c>
-      <c r="T29" s="6" t="n">
+      <c r="U29" s="21" t="n">
         <v>2.24</v>
-      </c>
-      <c r="U29" s="21" t="n">
-        <v>2.23</v>
       </c>
     </row>
     <row r="30">
@@ -3000,8 +3000,8 @@
           <t>T10YIE</t>
         </is>
       </c>
-      <c r="N30" s="49" t="n">
-        <v>46036</v>
+      <c r="N30" s="50" t="n">
+        <v>46037</v>
       </c>
       <c r="O30" s="6" t="inlineStr">
         <is>
@@ -3017,16 +3017,16 @@
         <v>2.29</v>
       </c>
       <c r="R30" s="6" t="n">
+        <v>2.29</v>
+      </c>
+      <c r="S30" s="6" t="n">
         <v>2.3</v>
       </c>
-      <c r="S30" s="6" t="n">
+      <c r="T30" s="6" t="n">
         <v>2.29</v>
       </c>
-      <c r="T30" s="6" t="n">
+      <c r="U30" s="21" t="n">
         <v>2.28</v>
-      </c>
-      <c r="U30" s="21" t="n">
-        <v>2.27</v>
       </c>
     </row>
     <row r="31">
@@ -3115,8 +3115,8 @@
           <t>INDPRO</t>
         </is>
       </c>
-      <c r="C32" s="48" t="n">
-        <v>45962</v>
+      <c r="C32" s="50" t="n">
+        <v>45992</v>
       </c>
       <c r="D32" s="6" t="inlineStr">
         <is>
@@ -3129,19 +3129,19 @@
         </is>
       </c>
       <c r="F32" s="25" t="n">
-        <v>0.001746772161864252</v>
+        <v>0.003650708955516668</v>
       </c>
       <c r="G32" s="25" t="n">
-        <v>-0.0005596378189272055</v>
+        <v>0.004299802100746319</v>
       </c>
       <c r="H32" s="25" t="n">
-        <v>0.0006988058294186139</v>
+        <v>-0.002570302590248041</v>
       </c>
       <c r="I32" s="25" t="n">
-        <v>-0.002668988493606861</v>
+        <v>0.001882136145775037</v>
       </c>
       <c r="J32" s="25" t="n">
-        <v>0.003895406416137392</v>
+        <v>-0.003015879247060815</v>
       </c>
       <c r="K32" s="5" t="n"/>
       <c r="L32" s="28" t="n"/>
@@ -3186,8 +3186,8 @@
           <t>INDPRO</t>
         </is>
       </c>
-      <c r="C33" s="48" t="n">
-        <v>45962</v>
+      <c r="C33" s="50" t="n">
+        <v>45992</v>
       </c>
       <c r="D33" s="6" t="inlineStr">
         <is>
@@ -3200,19 +3200,19 @@
         </is>
       </c>
       <c r="F33" s="25" t="n">
-        <v>0.02518820656142197</v>
+        <v>0.01991182858504125</v>
       </c>
       <c r="G33" s="25" t="n">
-        <v>0.02157947913682087</v>
+        <v>0.02679255734320309</v>
       </c>
       <c r="H33" s="25" t="n">
-        <v>0.01868079239823494</v>
+        <v>0.02057716184358024</v>
       </c>
       <c r="I33" s="25" t="n">
-        <v>0.01165975810233709</v>
+        <v>0.01973280806024339</v>
       </c>
       <c r="J33" s="25" t="n">
-        <v>0.01898561350408149</v>
+        <v>0.01150841026018884</v>
       </c>
       <c r="K33" s="5" t="n"/>
       <c r="L33" s="28" t="inlineStr">
@@ -3225,7 +3225,7 @@
           <t>CES0500000003</t>
         </is>
       </c>
-      <c r="N33" s="49" t="n">
+      <c r="N33" s="48" t="n">
         <v>45992</v>
       </c>
       <c r="O33" s="6" t="inlineStr">
@@ -3265,8 +3265,8 @@
           <t>TCU</t>
         </is>
       </c>
-      <c r="C34" s="48" t="n">
-        <v>45962</v>
+      <c r="C34" s="50" t="n">
+        <v>45992</v>
       </c>
       <c r="D34" s="6" t="inlineStr">
         <is>
@@ -3279,19 +3279,19 @@
         </is>
       </c>
       <c r="F34" s="24" t="n">
-        <v>75.95659999999999</v>
+        <v>76.2615</v>
       </c>
       <c r="G34" s="24" t="n">
-        <v>75.9156</v>
+        <v>76.07550000000001</v>
       </c>
       <c r="H34" s="24" t="n">
-        <v>76.0498</v>
+        <v>75.8411</v>
       </c>
       <c r="I34" s="24" t="n">
-        <v>76.08839999999999</v>
+        <v>76.1283</v>
       </c>
       <c r="J34" s="24" t="n">
-        <v>76.3844</v>
+        <v>76.077</v>
       </c>
       <c r="K34" s="5" t="n"/>
       <c r="L34" s="28" t="n"/>
@@ -3415,7 +3415,7 @@
           <t>HOUST</t>
         </is>
       </c>
-      <c r="C36" s="49" t="n">
+      <c r="C36" s="48" t="n">
         <v>45931</v>
       </c>
       <c r="D36" s="6" t="inlineStr">
@@ -3490,7 +3490,7 @@
           <t>HOUST</t>
         </is>
       </c>
-      <c r="C37" s="49" t="n">
+      <c r="C37" s="48" t="n">
         <v>45931</v>
       </c>
       <c r="D37" s="6" t="inlineStr">
@@ -3569,7 +3569,7 @@
           <t>PERMIT</t>
         </is>
       </c>
-      <c r="C38" s="49" t="n">
+      <c r="C38" s="48" t="n">
         <v>45931</v>
       </c>
       <c r="D38" s="6" t="inlineStr">
@@ -3640,7 +3640,7 @@
           <t>PERMIT</t>
         </is>
       </c>
-      <c r="C39" s="49" t="n">
+      <c r="C39" s="48" t="n">
         <v>45931</v>
       </c>
       <c r="D39" s="6" t="inlineStr">
@@ -3719,7 +3719,7 @@
           <t>HSN1F</t>
         </is>
       </c>
-      <c r="C40" s="49" t="n">
+      <c r="C40" s="50" t="n">
         <v>45931</v>
       </c>
       <c r="D40" s="6" t="inlineStr">
@@ -3790,7 +3790,7 @@
           <t>HSN1F</t>
         </is>
       </c>
-      <c r="C41" s="49" t="n">
+      <c r="C41" s="50" t="n">
         <v>45931</v>
       </c>
       <c r="D41" s="6" t="inlineStr">
@@ -3829,7 +3829,7 @@
           <t>IQ</t>
         </is>
       </c>
-      <c r="N41" s="49" t="n">
+      <c r="N41" s="50" t="n">
         <v>45962</v>
       </c>
       <c r="O41" s="6" t="inlineStr">
@@ -3904,7 +3904,7 @@
           <t>IQ</t>
         </is>
       </c>
-      <c r="N42" s="49" t="n">
+      <c r="N42" s="50" t="n">
         <v>45962</v>
       </c>
       <c r="O42" s="6" t="inlineStr">
@@ -3979,7 +3979,7 @@
           <t>IR</t>
         </is>
       </c>
-      <c r="N43" s="49" t="n">
+      <c r="N43" s="50" t="n">
         <v>45962</v>
       </c>
       <c r="O43" s="6" t="inlineStr">
@@ -4054,7 +4054,7 @@
           <t>IR</t>
         </is>
       </c>
-      <c r="N44" s="49" t="n">
+      <c r="N44" s="50" t="n">
         <v>45962</v>
       </c>
       <c r="O44" s="6" t="inlineStr">
@@ -4267,8 +4267,8 @@
           <t>DFF</t>
         </is>
       </c>
-      <c r="N47" s="49" t="n">
-        <v>46035</v>
+      <c r="N47" s="50" t="n">
+        <v>46036</v>
       </c>
       <c r="O47" s="6" t="inlineStr">
         <is>
@@ -4346,8 +4346,8 @@
           <t>DGS2</t>
         </is>
       </c>
-      <c r="N48" s="49" t="n">
-        <v>46035</v>
+      <c r="N48" s="50" t="n">
+        <v>46036</v>
       </c>
       <c r="O48" s="6" t="inlineStr">
         <is>
@@ -4360,19 +4360,19 @@
         </is>
       </c>
       <c r="Q48" s="6" t="n">
+        <v>3.51</v>
+      </c>
+      <c r="R48" s="6" t="n">
         <v>3.53</v>
-      </c>
-      <c r="R48" s="6" t="n">
-        <v>3.54</v>
       </c>
       <c r="S48" s="6" t="n">
         <v>3.54</v>
       </c>
       <c r="T48" s="6" t="n">
+        <v>3.54</v>
+      </c>
+      <c r="U48" s="21" t="n">
         <v>3.49</v>
-      </c>
-      <c r="U48" s="21" t="n">
-        <v>3.47</v>
       </c>
     </row>
     <row r="49">
@@ -4421,8 +4421,8 @@
           <t>DGS5</t>
         </is>
       </c>
-      <c r="N49" s="49" t="n">
-        <v>46035</v>
+      <c r="N49" s="50" t="n">
+        <v>46036</v>
       </c>
       <c r="O49" s="6" t="inlineStr">
         <is>
@@ -4435,19 +4435,19 @@
         </is>
       </c>
       <c r="Q49" s="6" t="n">
+        <v>3.72</v>
+      </c>
+      <c r="R49" s="6" t="n">
         <v>3.75</v>
       </c>
-      <c r="R49" s="6" t="n">
+      <c r="S49" s="6" t="n">
         <v>3.77</v>
       </c>
-      <c r="S49" s="6" t="n">
+      <c r="T49" s="6" t="n">
         <v>3.75</v>
       </c>
-      <c r="T49" s="6" t="n">
+      <c r="U49" s="21" t="n">
         <v>3.74</v>
-      </c>
-      <c r="U49" s="21" t="n">
-        <v>3.7</v>
       </c>
     </row>
     <row r="50">
@@ -4500,8 +4500,8 @@
           <t>DGS10</t>
         </is>
       </c>
-      <c r="N50" s="49" t="n">
-        <v>46035</v>
+      <c r="N50" s="50" t="n">
+        <v>46036</v>
       </c>
       <c r="O50" s="6" t="inlineStr">
         <is>
@@ -4514,19 +4514,19 @@
         </is>
       </c>
       <c r="Q50" s="6" t="n">
+        <v>4.15</v>
+      </c>
+      <c r="R50" s="6" t="n">
         <v>4.18</v>
       </c>
-      <c r="R50" s="6" t="n">
+      <c r="S50" s="6" t="n">
         <v>4.19</v>
       </c>
-      <c r="S50" s="6" t="n">
+      <c r="T50" s="6" t="n">
         <v>4.18</v>
       </c>
-      <c r="T50" s="6" t="n">
+      <c r="U50" s="21" t="n">
         <v>4.19</v>
-      </c>
-      <c r="U50" s="21" t="n">
-        <v>4.15</v>
       </c>
     </row>
     <row r="51" ht="31.5" customHeight="1">
@@ -4575,8 +4575,8 @@
           <t>MORTGAGE30US</t>
         </is>
       </c>
-      <c r="N51" s="48" t="n">
-        <v>46027</v>
+      <c r="N51" s="50" t="n">
+        <v>46034</v>
       </c>
       <c r="O51" s="6" t="inlineStr">
         <is>
@@ -4589,19 +4589,19 @@
         </is>
       </c>
       <c r="Q51" s="6" t="n">
+        <v>6.06</v>
+      </c>
+      <c r="R51" s="6" t="n">
         <v>6.16</v>
       </c>
-      <c r="R51" s="6" t="n">
+      <c r="S51" s="6" t="n">
         <v>6.15</v>
       </c>
-      <c r="S51" s="6" t="n">
+      <c r="T51" s="6" t="n">
         <v>6.18</v>
       </c>
-      <c r="T51" s="6" t="n">
+      <c r="U51" s="21" t="n">
         <v>6.21</v>
-      </c>
-      <c r="U51" s="21" t="n">
-        <v>6.22</v>
       </c>
     </row>
     <row r="52" ht="16.15" customHeight="1" thickBot="1">
@@ -4627,7 +4627,7 @@
         </is>
       </c>
       <c r="N52" s="53" t="n">
-        <v>46035</v>
+        <v>46036</v>
       </c>
       <c r="O52" s="9" t="inlineStr">
         <is>
@@ -4640,19 +4640,19 @@
         </is>
       </c>
       <c r="Q52" s="9" t="n">
+        <v>5.83</v>
+      </c>
+      <c r="R52" s="9" t="n">
         <v>5.87</v>
       </c>
-      <c r="R52" s="9" t="n">
+      <c r="S52" s="9" t="n">
         <v>5.89</v>
       </c>
-      <c r="S52" s="9" t="n">
+      <c r="T52" s="9" t="n">
         <v>5.88</v>
       </c>
-      <c r="T52" s="9" t="n">
+      <c r="U52" s="22" t="n">
         <v>5.92</v>
-      </c>
-      <c r="U52" s="22" t="n">
-        <v>5.88</v>
       </c>
     </row>
     <row r="53" ht="21" customHeight="1">

</xml_diff>

<commit_message>
Update dashboards - 2026-01-17
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -2922,7 +2922,7 @@
         </is>
       </c>
       <c r="N29" s="50" t="n">
-        <v>46037</v>
+        <v>46038</v>
       </c>
       <c r="O29" s="6" t="inlineStr">
         <is>
@@ -2935,19 +2935,19 @@
         </is>
       </c>
       <c r="Q29" s="6" t="n">
-        <v>2.22</v>
+        <v>2.27</v>
       </c>
       <c r="R29" s="6" t="n">
         <v>2.22</v>
       </c>
       <c r="S29" s="6" t="n">
+        <v>2.22</v>
+      </c>
+      <c r="T29" s="6" t="n">
         <v>2.23</v>
       </c>
-      <c r="T29" s="6" t="n">
+      <c r="U29" s="21" t="n">
         <v>2.22</v>
-      </c>
-      <c r="U29" s="21" t="n">
-        <v>2.24</v>
       </c>
     </row>
     <row r="30">
@@ -3001,7 +3001,7 @@
         </is>
       </c>
       <c r="N30" s="50" t="n">
-        <v>46037</v>
+        <v>46038</v>
       </c>
       <c r="O30" s="6" t="inlineStr">
         <is>
@@ -3014,19 +3014,19 @@
         </is>
       </c>
       <c r="Q30" s="6" t="n">
-        <v>2.29</v>
+        <v>2.33</v>
       </c>
       <c r="R30" s="6" t="n">
         <v>2.29</v>
       </c>
       <c r="S30" s="6" t="n">
+        <v>2.29</v>
+      </c>
+      <c r="T30" s="6" t="n">
         <v>2.3</v>
       </c>
-      <c r="T30" s="6" t="n">
+      <c r="U30" s="21" t="n">
         <v>2.29</v>
-      </c>
-      <c r="U30" s="21" t="n">
-        <v>2.28</v>
       </c>
     </row>
     <row r="31">
@@ -4268,7 +4268,7 @@
         </is>
       </c>
       <c r="N47" s="50" t="n">
-        <v>46036</v>
+        <v>46037</v>
       </c>
       <c r="O47" s="6" t="inlineStr">
         <is>
@@ -4347,7 +4347,7 @@
         </is>
       </c>
       <c r="N48" s="50" t="n">
-        <v>46036</v>
+        <v>46037</v>
       </c>
       <c r="O48" s="6" t="inlineStr">
         <is>
@@ -4360,19 +4360,19 @@
         </is>
       </c>
       <c r="Q48" s="6" t="n">
+        <v>3.56</v>
+      </c>
+      <c r="R48" s="6" t="n">
         <v>3.51</v>
       </c>
-      <c r="R48" s="6" t="n">
+      <c r="S48" s="6" t="n">
         <v>3.53</v>
-      </c>
-      <c r="S48" s="6" t="n">
-        <v>3.54</v>
       </c>
       <c r="T48" s="6" t="n">
         <v>3.54</v>
       </c>
       <c r="U48" s="21" t="n">
-        <v>3.49</v>
+        <v>3.54</v>
       </c>
     </row>
     <row r="49">
@@ -4422,7 +4422,7 @@
         </is>
       </c>
       <c r="N49" s="50" t="n">
-        <v>46036</v>
+        <v>46037</v>
       </c>
       <c r="O49" s="6" t="inlineStr">
         <is>
@@ -4435,19 +4435,19 @@
         </is>
       </c>
       <c r="Q49" s="6" t="n">
+        <v>3.77</v>
+      </c>
+      <c r="R49" s="6" t="n">
         <v>3.72</v>
       </c>
-      <c r="R49" s="6" t="n">
+      <c r="S49" s="6" t="n">
         <v>3.75</v>
       </c>
-      <c r="S49" s="6" t="n">
+      <c r="T49" s="6" t="n">
         <v>3.77</v>
       </c>
-      <c r="T49" s="6" t="n">
+      <c r="U49" s="21" t="n">
         <v>3.75</v>
-      </c>
-      <c r="U49" s="21" t="n">
-        <v>3.74</v>
       </c>
     </row>
     <row r="50">
@@ -4501,7 +4501,7 @@
         </is>
       </c>
       <c r="N50" s="50" t="n">
-        <v>46036</v>
+        <v>46037</v>
       </c>
       <c r="O50" s="6" t="inlineStr">
         <is>
@@ -4514,19 +4514,19 @@
         </is>
       </c>
       <c r="Q50" s="6" t="n">
+        <v>4.17</v>
+      </c>
+      <c r="R50" s="6" t="n">
         <v>4.15</v>
       </c>
-      <c r="R50" s="6" t="n">
+      <c r="S50" s="6" t="n">
         <v>4.18</v>
       </c>
-      <c r="S50" s="6" t="n">
+      <c r="T50" s="6" t="n">
         <v>4.19</v>
       </c>
-      <c r="T50" s="6" t="n">
+      <c r="U50" s="21" t="n">
         <v>4.18</v>
-      </c>
-      <c r="U50" s="21" t="n">
-        <v>4.19</v>
       </c>
     </row>
     <row r="51" ht="31.5" customHeight="1">
@@ -4627,7 +4627,7 @@
         </is>
       </c>
       <c r="N52" s="53" t="n">
-        <v>46036</v>
+        <v>46037</v>
       </c>
       <c r="O52" s="9" t="inlineStr">
         <is>
@@ -4640,19 +4640,19 @@
         </is>
       </c>
       <c r="Q52" s="9" t="n">
+        <v>5.82</v>
+      </c>
+      <c r="R52" s="9" t="n">
         <v>5.83</v>
       </c>
-      <c r="R52" s="9" t="n">
+      <c r="S52" s="9" t="n">
         <v>5.87</v>
       </c>
-      <c r="S52" s="9" t="n">
+      <c r="T52" s="9" t="n">
         <v>5.89</v>
       </c>
-      <c r="T52" s="9" t="n">
+      <c r="U52" s="22" t="n">
         <v>5.88</v>
-      </c>
-      <c r="U52" s="22" t="n">
-        <v>5.92</v>
       </c>
     </row>
     <row r="53" ht="21" customHeight="1">

</xml_diff>

<commit_message>
Update dashboards - 2026-01-20
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -2085,7 +2085,7 @@
           <t>CPIAUCSL</t>
         </is>
       </c>
-      <c r="N18" s="50" t="n">
+      <c r="N18" s="48" t="n">
         <v>45992</v>
       </c>
       <c r="O18" s="6" t="inlineStr">
@@ -2160,7 +2160,7 @@
           <t>CPIAUCSL</t>
         </is>
       </c>
-      <c r="N19" s="50" t="n">
+      <c r="N19" s="48" t="n">
         <v>45992</v>
       </c>
       <c r="O19" s="6" t="inlineStr">
@@ -2235,7 +2235,7 @@
           <t>CPILFESL</t>
         </is>
       </c>
-      <c r="N20" s="50" t="n">
+      <c r="N20" s="48" t="n">
         <v>45992</v>
       </c>
       <c r="O20" s="6" t="inlineStr">
@@ -2310,7 +2310,7 @@
           <t>CPILFESL</t>
         </is>
       </c>
-      <c r="N21" s="50" t="n">
+      <c r="N21" s="48" t="n">
         <v>45992</v>
       </c>
       <c r="O21" s="6" t="inlineStr">
@@ -3719,7 +3719,7 @@
           <t>HSN1F</t>
         </is>
       </c>
-      <c r="C40" s="50" t="n">
+      <c r="C40" s="48" t="n">
         <v>45931</v>
       </c>
       <c r="D40" s="6" t="inlineStr">
@@ -3790,7 +3790,7 @@
           <t>HSN1F</t>
         </is>
       </c>
-      <c r="C41" s="50" t="n">
+      <c r="C41" s="48" t="n">
         <v>45931</v>
       </c>
       <c r="D41" s="6" t="inlineStr">

</xml_diff>

<commit_message>
Update dashboards - 2026-01-21
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -1959,7 +1959,7 @@
           <t>RSAFS</t>
         </is>
       </c>
-      <c r="C17" s="50" t="n">
+      <c r="C17" s="48" t="n">
         <v>45962</v>
       </c>
       <c r="D17" s="6" t="inlineStr">
@@ -2046,7 +2046,7 @@
           <t>RSAFS</t>
         </is>
       </c>
-      <c r="C18" s="50" t="n">
+      <c r="C18" s="48" t="n">
         <v>45962</v>
       </c>
       <c r="D18" s="6" t="inlineStr">
@@ -2389,7 +2389,7 @@
           <t>PPIFIS</t>
         </is>
       </c>
-      <c r="N22" s="50" t="n">
+      <c r="N22" s="48" t="n">
         <v>45962</v>
       </c>
       <c r="O22" s="6" t="inlineStr">
@@ -2459,7 +2459,7 @@
           <t>PPIFIS</t>
         </is>
       </c>
-      <c r="N23" s="50" t="n">
+      <c r="N23" s="48" t="n">
         <v>45962</v>
       </c>
       <c r="O23" s="6" t="inlineStr">
@@ -2922,7 +2922,7 @@
         </is>
       </c>
       <c r="N29" s="50" t="n">
-        <v>46038</v>
+        <v>46042</v>
       </c>
       <c r="O29" s="6" t="inlineStr">
         <is>
@@ -2935,19 +2935,19 @@
         </is>
       </c>
       <c r="Q29" s="6" t="n">
+        <v>2.26</v>
+      </c>
+      <c r="R29" s="6" t="n">
         <v>2.27</v>
-      </c>
-      <c r="R29" s="6" t="n">
-        <v>2.22</v>
       </c>
       <c r="S29" s="6" t="n">
         <v>2.22</v>
       </c>
       <c r="T29" s="6" t="n">
+        <v>2.22</v>
+      </c>
+      <c r="U29" s="21" t="n">
         <v>2.23</v>
-      </c>
-      <c r="U29" s="21" t="n">
-        <v>2.22</v>
       </c>
     </row>
     <row r="30">
@@ -3001,7 +3001,7 @@
         </is>
       </c>
       <c r="N30" s="50" t="n">
-        <v>46038</v>
+        <v>46042</v>
       </c>
       <c r="O30" s="6" t="inlineStr">
         <is>
@@ -3017,16 +3017,16 @@
         <v>2.33</v>
       </c>
       <c r="R30" s="6" t="n">
-        <v>2.29</v>
+        <v>2.33</v>
       </c>
       <c r="S30" s="6" t="n">
         <v>2.29</v>
       </c>
       <c r="T30" s="6" t="n">
+        <v>2.29</v>
+      </c>
+      <c r="U30" s="21" t="n">
         <v>2.3</v>
-      </c>
-      <c r="U30" s="21" t="n">
-        <v>2.29</v>
       </c>
     </row>
     <row r="31">
@@ -4268,7 +4268,7 @@
         </is>
       </c>
       <c r="N47" s="50" t="n">
-        <v>46037</v>
+        <v>46041</v>
       </c>
       <c r="O47" s="6" t="inlineStr">
         <is>
@@ -4347,7 +4347,7 @@
         </is>
       </c>
       <c r="N48" s="50" t="n">
-        <v>46037</v>
+        <v>46038</v>
       </c>
       <c r="O48" s="6" t="inlineStr">
         <is>
@@ -4360,16 +4360,16 @@
         </is>
       </c>
       <c r="Q48" s="6" t="n">
+        <v>3.59</v>
+      </c>
+      <c r="R48" s="6" t="n">
         <v>3.56</v>
       </c>
-      <c r="R48" s="6" t="n">
+      <c r="S48" s="6" t="n">
         <v>3.51</v>
       </c>
-      <c r="S48" s="6" t="n">
+      <c r="T48" s="6" t="n">
         <v>3.53</v>
-      </c>
-      <c r="T48" s="6" t="n">
-        <v>3.54</v>
       </c>
       <c r="U48" s="21" t="n">
         <v>3.54</v>
@@ -4422,7 +4422,7 @@
         </is>
       </c>
       <c r="N49" s="50" t="n">
-        <v>46037</v>
+        <v>46038</v>
       </c>
       <c r="O49" s="6" t="inlineStr">
         <is>
@@ -4435,19 +4435,19 @@
         </is>
       </c>
       <c r="Q49" s="6" t="n">
+        <v>3.82</v>
+      </c>
+      <c r="R49" s="6" t="n">
         <v>3.77</v>
       </c>
-      <c r="R49" s="6" t="n">
+      <c r="S49" s="6" t="n">
         <v>3.72</v>
       </c>
-      <c r="S49" s="6" t="n">
+      <c r="T49" s="6" t="n">
         <v>3.75</v>
       </c>
-      <c r="T49" s="6" t="n">
+      <c r="U49" s="21" t="n">
         <v>3.77</v>
-      </c>
-      <c r="U49" s="21" t="n">
-        <v>3.75</v>
       </c>
     </row>
     <row r="50">
@@ -4501,7 +4501,7 @@
         </is>
       </c>
       <c r="N50" s="50" t="n">
-        <v>46037</v>
+        <v>46038</v>
       </c>
       <c r="O50" s="6" t="inlineStr">
         <is>
@@ -4514,19 +4514,19 @@
         </is>
       </c>
       <c r="Q50" s="6" t="n">
+        <v>4.24</v>
+      </c>
+      <c r="R50" s="6" t="n">
         <v>4.17</v>
       </c>
-      <c r="R50" s="6" t="n">
+      <c r="S50" s="6" t="n">
         <v>4.15</v>
       </c>
-      <c r="S50" s="6" t="n">
+      <c r="T50" s="6" t="n">
         <v>4.18</v>
       </c>
-      <c r="T50" s="6" t="n">
+      <c r="U50" s="21" t="n">
         <v>4.19</v>
-      </c>
-      <c r="U50" s="21" t="n">
-        <v>4.18</v>
       </c>
     </row>
     <row r="51" ht="31.5" customHeight="1">
@@ -4627,7 +4627,7 @@
         </is>
       </c>
       <c r="N52" s="53" t="n">
-        <v>46037</v>
+        <v>46038</v>
       </c>
       <c r="O52" s="9" t="inlineStr">
         <is>
@@ -4640,19 +4640,19 @@
         </is>
       </c>
       <c r="Q52" s="9" t="n">
+        <v>5.87</v>
+      </c>
+      <c r="R52" s="9" t="n">
         <v>5.82</v>
       </c>
-      <c r="R52" s="9" t="n">
+      <c r="S52" s="9" t="n">
         <v>5.83</v>
       </c>
-      <c r="S52" s="9" t="n">
+      <c r="T52" s="9" t="n">
         <v>5.87</v>
       </c>
-      <c r="T52" s="9" t="n">
+      <c r="U52" s="22" t="n">
         <v>5.89</v>
-      </c>
-      <c r="U52" s="22" t="n">
-        <v>5.88</v>
       </c>
     </row>
     <row r="53" ht="21" customHeight="1">

</xml_diff>

<commit_message>
Update dashboards - 2026-01-22
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -923,7 +923,7 @@
         </is>
       </c>
       <c r="F3" s="24" t="n">
-        <v>24024.957</v>
+        <v>24026.834</v>
       </c>
       <c r="G3" s="24" t="n">
         <v>23770.976</v>
@@ -998,7 +998,7 @@
         </is>
       </c>
       <c r="F4" s="25" t="n">
-        <v>0.01068450029144774</v>
+        <v>0.0107634621312982</v>
       </c>
       <c r="G4" s="25" t="n">
         <v>0.009459997171759493</v>
@@ -1385,7 +1385,7 @@
         </is>
       </c>
       <c r="F9" s="24" t="n">
-        <v>16589.126</v>
+        <v>16585.878</v>
       </c>
       <c r="G9" s="24" t="n">
         <v>16445.685</v>
@@ -1460,7 +1460,7 @@
         </is>
       </c>
       <c r="F10" s="25" t="n">
-        <v>0.008722105524944679</v>
+        <v>0.008524606910566446</v>
       </c>
       <c r="G10" s="25" t="n">
         <v>0.006111174905983452</v>
@@ -1719,7 +1719,7 @@
         </is>
       </c>
       <c r="N13" s="50" t="n">
-        <v>46027</v>
+        <v>46034</v>
       </c>
       <c r="O13" s="6" t="inlineStr">
         <is>
@@ -1732,19 +1732,19 @@
         </is>
       </c>
       <c r="Q13" s="24" t="n">
-        <v>198000</v>
+        <v>200000</v>
       </c>
       <c r="R13" s="24" t="n">
+        <v>199000</v>
+      </c>
+      <c r="S13" s="24" t="n">
         <v>207000</v>
       </c>
-      <c r="S13" s="24" t="n">
+      <c r="T13" s="24" t="n">
         <v>200000</v>
       </c>
-      <c r="T13" s="24" t="n">
+      <c r="U13" s="26" t="n">
         <v>215000</v>
-      </c>
-      <c r="U13" s="26" t="n">
-        <v>224000</v>
       </c>
     </row>
     <row r="14">
@@ -1794,7 +1794,7 @@
         </is>
       </c>
       <c r="N14" s="50" t="n">
-        <v>46020</v>
+        <v>46027</v>
       </c>
       <c r="O14" s="6" t="inlineStr">
         <is>
@@ -1807,19 +1807,19 @@
         </is>
       </c>
       <c r="Q14" s="24" t="n">
-        <v>1884000</v>
+        <v>1849000</v>
       </c>
       <c r="R14" s="24" t="n">
+        <v>1875000</v>
+      </c>
+      <c r="S14" s="24" t="n">
         <v>1903000</v>
       </c>
-      <c r="S14" s="24" t="n">
+      <c r="T14" s="24" t="n">
         <v>1856000</v>
       </c>
-      <c r="T14" s="24" t="n">
+      <c r="U14" s="26" t="n">
         <v>1914000</v>
-      </c>
-      <c r="U14" s="26" t="n">
-        <v>1885000</v>
       </c>
     </row>
     <row r="15">
@@ -2667,7 +2667,7 @@
         </is>
       </c>
       <c r="F26" s="38" t="n">
-        <v>0.00701605762819324</v>
+        <v>0.007794617579222285</v>
       </c>
       <c r="G26" s="38" t="n">
         <v>0.01778138610314484</v>
@@ -2746,7 +2746,7 @@
         </is>
       </c>
       <c r="F27" s="38" t="n">
-        <v>-0.01313886426984179</v>
+        <v>-0.01832684674964358</v>
       </c>
       <c r="G27" s="38" t="n">
         <v>-0.01299350008050415</v>
@@ -2922,7 +2922,7 @@
         </is>
       </c>
       <c r="N29" s="50" t="n">
-        <v>46042</v>
+        <v>46043</v>
       </c>
       <c r="O29" s="6" t="inlineStr">
         <is>
@@ -2938,16 +2938,16 @@
         <v>2.26</v>
       </c>
       <c r="R29" s="6" t="n">
+        <v>2.26</v>
+      </c>
+      <c r="S29" s="6" t="n">
         <v>2.27</v>
-      </c>
-      <c r="S29" s="6" t="n">
-        <v>2.22</v>
       </c>
       <c r="T29" s="6" t="n">
         <v>2.22</v>
       </c>
       <c r="U29" s="21" t="n">
-        <v>2.23</v>
+        <v>2.22</v>
       </c>
     </row>
     <row r="30">
@@ -3001,7 +3001,7 @@
         </is>
       </c>
       <c r="N30" s="50" t="n">
-        <v>46042</v>
+        <v>46043</v>
       </c>
       <c r="O30" s="6" t="inlineStr">
         <is>
@@ -3014,19 +3014,19 @@
         </is>
       </c>
       <c r="Q30" s="6" t="n">
-        <v>2.33</v>
+        <v>2.34</v>
       </c>
       <c r="R30" s="6" t="n">
         <v>2.33</v>
       </c>
       <c r="S30" s="6" t="n">
-        <v>2.29</v>
+        <v>2.33</v>
       </c>
       <c r="T30" s="6" t="n">
         <v>2.29</v>
       </c>
       <c r="U30" s="21" t="n">
-        <v>2.3</v>
+        <v>2.29</v>
       </c>
     </row>
     <row r="31">
@@ -3829,7 +3829,7 @@
           <t>IQ</t>
         </is>
       </c>
-      <c r="N41" s="50" t="n">
+      <c r="N41" s="48" t="n">
         <v>45962</v>
       </c>
       <c r="O41" s="6" t="inlineStr">
@@ -3904,7 +3904,7 @@
           <t>IQ</t>
         </is>
       </c>
-      <c r="N42" s="50" t="n">
+      <c r="N42" s="48" t="n">
         <v>45962</v>
       </c>
       <c r="O42" s="6" t="inlineStr">
@@ -3979,7 +3979,7 @@
           <t>IR</t>
         </is>
       </c>
-      <c r="N43" s="50" t="n">
+      <c r="N43" s="48" t="n">
         <v>45962</v>
       </c>
       <c r="O43" s="6" t="inlineStr">
@@ -4033,7 +4033,7 @@
         </is>
       </c>
       <c r="F44" s="24" t="n">
-        <v>5323.099</v>
+        <v>5324.402</v>
       </c>
       <c r="G44" s="24" t="n">
         <v>5236.97</v>
@@ -4054,7 +4054,7 @@
           <t>IR</t>
         </is>
       </c>
-      <c r="N44" s="50" t="n">
+      <c r="N44" s="48" t="n">
         <v>45962</v>
       </c>
       <c r="O44" s="6" t="inlineStr">
@@ -4104,7 +4104,7 @@
         </is>
       </c>
       <c r="F45" s="38" t="n">
-        <v>0.01644634206420892</v>
+        <v>0.01669515005814426</v>
       </c>
       <c r="G45" s="38" t="n">
         <v>0.007978609251013902</v>
@@ -4268,7 +4268,7 @@
         </is>
       </c>
       <c r="N47" s="50" t="n">
-        <v>46041</v>
+        <v>46042</v>
       </c>
       <c r="O47" s="6" t="inlineStr">
         <is>
@@ -4347,7 +4347,7 @@
         </is>
       </c>
       <c r="N48" s="50" t="n">
-        <v>46038</v>
+        <v>46042</v>
       </c>
       <c r="O48" s="6" t="inlineStr">
         <is>
@@ -4360,19 +4360,19 @@
         </is>
       </c>
       <c r="Q48" s="6" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="R48" s="6" t="n">
         <v>3.59</v>
       </c>
-      <c r="R48" s="6" t="n">
+      <c r="S48" s="6" t="n">
         <v>3.56</v>
       </c>
-      <c r="S48" s="6" t="n">
+      <c r="T48" s="6" t="n">
         <v>3.51</v>
       </c>
-      <c r="T48" s="6" t="n">
+      <c r="U48" s="21" t="n">
         <v>3.53</v>
-      </c>
-      <c r="U48" s="21" t="n">
-        <v>3.54</v>
       </c>
     </row>
     <row r="49">
@@ -4422,7 +4422,7 @@
         </is>
       </c>
       <c r="N49" s="50" t="n">
-        <v>46038</v>
+        <v>46042</v>
       </c>
       <c r="O49" s="6" t="inlineStr">
         <is>
@@ -4435,19 +4435,19 @@
         </is>
       </c>
       <c r="Q49" s="6" t="n">
+        <v>3.86</v>
+      </c>
+      <c r="R49" s="6" t="n">
         <v>3.82</v>
       </c>
-      <c r="R49" s="6" t="n">
+      <c r="S49" s="6" t="n">
         <v>3.77</v>
       </c>
-      <c r="S49" s="6" t="n">
+      <c r="T49" s="6" t="n">
         <v>3.72</v>
       </c>
-      <c r="T49" s="6" t="n">
+      <c r="U49" s="21" t="n">
         <v>3.75</v>
-      </c>
-      <c r="U49" s="21" t="n">
-        <v>3.77</v>
       </c>
     </row>
     <row r="50">
@@ -4501,7 +4501,7 @@
         </is>
       </c>
       <c r="N50" s="50" t="n">
-        <v>46038</v>
+        <v>46042</v>
       </c>
       <c r="O50" s="6" t="inlineStr">
         <is>
@@ -4514,19 +4514,19 @@
         </is>
       </c>
       <c r="Q50" s="6" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="R50" s="6" t="n">
         <v>4.24</v>
       </c>
-      <c r="R50" s="6" t="n">
+      <c r="S50" s="6" t="n">
         <v>4.17</v>
       </c>
-      <c r="S50" s="6" t="n">
+      <c r="T50" s="6" t="n">
         <v>4.15</v>
       </c>
-      <c r="T50" s="6" t="n">
+      <c r="U50" s="21" t="n">
         <v>4.18</v>
-      </c>
-      <c r="U50" s="21" t="n">
-        <v>4.19</v>
       </c>
     </row>
     <row r="51" ht="31.5" customHeight="1">
@@ -4575,7 +4575,7 @@
           <t>MORTGAGE30US</t>
         </is>
       </c>
-      <c r="N51" s="50" t="n">
+      <c r="N51" s="48" t="n">
         <v>46034</v>
       </c>
       <c r="O51" s="6" t="inlineStr">
@@ -4627,7 +4627,7 @@
         </is>
       </c>
       <c r="N52" s="53" t="n">
-        <v>46038</v>
+        <v>46042</v>
       </c>
       <c r="O52" s="9" t="inlineStr">
         <is>
@@ -4640,19 +4640,19 @@
         </is>
       </c>
       <c r="Q52" s="9" t="n">
+        <v>5.95</v>
+      </c>
+      <c r="R52" s="9" t="n">
         <v>5.87</v>
       </c>
-      <c r="R52" s="9" t="n">
+      <c r="S52" s="9" t="n">
         <v>5.82</v>
       </c>
-      <c r="S52" s="9" t="n">
+      <c r="T52" s="9" t="n">
         <v>5.83</v>
       </c>
-      <c r="T52" s="9" t="n">
+      <c r="U52" s="22" t="n">
         <v>5.87</v>
-      </c>
-      <c r="U52" s="22" t="n">
-        <v>5.89</v>
       </c>
     </row>
     <row r="53" ht="21" customHeight="1">

</xml_diff>

<commit_message>
Update dashboards - 2026-01-23
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -1525,8 +1525,8 @@
           <t>PCEDGC96</t>
         </is>
       </c>
-      <c r="C11" s="48" t="n">
-        <v>45901</v>
+      <c r="C11" s="50" t="n">
+        <v>45962</v>
       </c>
       <c r="D11" s="6" t="inlineStr">
         <is>
@@ -1539,19 +1539,19 @@
         </is>
       </c>
       <c r="F11" s="25" t="n">
-        <v>-0.003916814324349538</v>
+        <v>0.006303109534036899</v>
       </c>
       <c r="G11" s="25" t="n">
-        <v>0.001447583469530667</v>
+        <v>0.003232001498899351</v>
       </c>
       <c r="H11" s="25" t="n">
-        <v>0.01305643597142714</v>
+        <v>-0.00461581499440511</v>
       </c>
       <c r="I11" s="25" t="n">
-        <v>-0.001794399584454709</v>
+        <v>0.001494209936496294</v>
       </c>
       <c r="J11" s="25" t="n">
-        <v>-0.02184757505773682</v>
+        <v>0.01310374189885977</v>
       </c>
       <c r="K11" s="5" t="n"/>
       <c r="L11" s="28" t="inlineStr">
@@ -1600,8 +1600,8 @@
           <t>PCEDGC96</t>
         </is>
       </c>
-      <c r="C12" s="48" t="n">
-        <v>45901</v>
+      <c r="C12" s="50" t="n">
+        <v>45962</v>
       </c>
       <c r="D12" s="6" t="inlineStr">
         <is>
@@ -1614,19 +1614,19 @@
         </is>
       </c>
       <c r="F12" s="25" t="n">
-        <v>0.02352546595754871</v>
+        <v>0.01107097621616567</v>
       </c>
       <c r="G12" s="25" t="n">
-        <v>0.03905038759689918</v>
+        <v>0.02185114503816803</v>
       </c>
       <c r="H12" s="25" t="n">
-        <v>0.03409145782027134</v>
+        <v>0.02290259211345895</v>
       </c>
       <c r="I12" s="25" t="n">
-        <v>0.0349571603427173</v>
+        <v>0.03914728682170551</v>
       </c>
       <c r="J12" s="25" t="n">
-        <v>0.03610744165565816</v>
+        <v>0.0341397460041527</v>
       </c>
       <c r="K12" s="5" t="n"/>
       <c r="L12" s="28" t="inlineStr">
@@ -1679,8 +1679,8 @@
           <t>PCENDC96</t>
         </is>
       </c>
-      <c r="C13" s="48" t="n">
-        <v>45901</v>
+      <c r="C13" s="50" t="n">
+        <v>45962</v>
       </c>
       <c r="D13" s="6" t="inlineStr">
         <is>
@@ -1693,19 +1693,19 @@
         </is>
       </c>
       <c r="F13" s="25" t="n">
-        <v>-0.003153419489258624</v>
+        <v>0.005120414134593743</v>
       </c>
       <c r="G13" s="25" t="n">
-        <v>0.00520759629807821</v>
+        <v>0.004379892056853851</v>
       </c>
       <c r="H13" s="25" t="n">
-        <v>0.002980583626660538</v>
+        <v>-0.00357585313661446</v>
       </c>
       <c r="I13" s="25" t="n">
-        <v>0.007003401652231123</v>
+        <v>0.005207743688441013</v>
       </c>
       <c r="J13" s="25" t="n">
-        <v>-0.00119914346895067</v>
+        <v>0.002952197115930311</v>
       </c>
       <c r="K13" s="5" t="n"/>
       <c r="L13" s="28" t="inlineStr">
@@ -1754,8 +1754,8 @@
           <t>PCENDC96</t>
         </is>
       </c>
-      <c r="C14" s="48" t="n">
-        <v>45901</v>
+      <c r="C14" s="50" t="n">
+        <v>45962</v>
       </c>
       <c r="D14" s="6" t="inlineStr">
         <is>
@@ -1768,19 +1768,19 @@
         </is>
       </c>
       <c r="F14" s="25" t="n">
-        <v>0.02199578558438929</v>
+        <v>0.03287172222382833</v>
       </c>
       <c r="G14" s="25" t="n">
-        <v>0.03796247588988241</v>
+        <v>0.02743170978465099</v>
       </c>
       <c r="H14" s="25" t="n">
-        <v>0.03056730348548933</v>
+        <v>0.02153393181883783</v>
       </c>
       <c r="I14" s="25" t="n">
-        <v>0.03332160037545476</v>
+        <v>0.03793325150505573</v>
       </c>
       <c r="J14" s="25" t="n">
-        <v>0.02894202770669728</v>
+        <v>0.03053813621117101</v>
       </c>
       <c r="K14" s="5" t="n"/>
       <c r="L14" s="28" t="inlineStr">
@@ -1833,8 +1833,8 @@
           <t>PCESC96</t>
         </is>
       </c>
-      <c r="C15" s="48" t="n">
-        <v>45901</v>
+      <c r="C15" s="50" t="n">
+        <v>45962</v>
       </c>
       <c r="D15" s="6" t="inlineStr">
         <is>
@@ -1847,19 +1847,19 @@
         </is>
       </c>
       <c r="F15" s="25" t="n">
-        <v>0.003107917877840594</v>
+        <v>0.001899602810321532</v>
       </c>
       <c r="G15" s="25" t="n">
-        <v>0.002529279155440545</v>
+        <v>0.002642778380250288</v>
       </c>
       <c r="H15" s="25" t="n">
-        <v>0.004510641431622275</v>
+        <v>0.003374053619106698</v>
       </c>
       <c r="I15" s="25" t="n">
-        <v>0.001973841981958824</v>
+        <v>0.002493308400249195</v>
       </c>
       <c r="J15" s="25" t="n">
-        <v>0.001829606357419911</v>
+        <v>0.004234479711318961</v>
       </c>
       <c r="K15" s="5" t="n"/>
       <c r="L15" s="28" t="inlineStr">
@@ -1908,8 +1908,8 @@
           <t>PCESC96</t>
         </is>
       </c>
-      <c r="C16" s="48" t="n">
-        <v>45901</v>
+      <c r="C16" s="50" t="n">
+        <v>45962</v>
       </c>
       <c r="D16" s="6" t="inlineStr">
         <is>
@@ -1922,19 +1922,19 @@
         </is>
       </c>
       <c r="F16" s="25" t="n">
-        <v>0.02464075294820676</v>
+        <v>0.02567156402073092</v>
       </c>
       <c r="G16" s="25" t="n">
-        <v>0.02344422407663796</v>
+        <v>0.02575027269930347</v>
       </c>
       <c r="H16" s="25" t="n">
-        <v>0.02402357313113493</v>
+        <v>0.0245940671714955</v>
       </c>
       <c r="I16" s="25" t="n">
-        <v>0.02094865746266567</v>
+        <v>0.02312614601653996</v>
       </c>
       <c r="J16" s="25" t="n">
-        <v>0.02239657497430288</v>
+        <v>0.02374204688350444</v>
       </c>
       <c r="K16" s="5" t="n"/>
       <c r="L16" s="28" t="n"/>
@@ -2125,8 +2125,8 @@
           <t>DSPIC96</t>
         </is>
       </c>
-      <c r="C19" s="48" t="n">
-        <v>45901</v>
+      <c r="C19" s="50" t="n">
+        <v>45962</v>
       </c>
       <c r="D19" s="6" t="inlineStr">
         <is>
@@ -2139,19 +2139,19 @@
         </is>
       </c>
       <c r="F19" s="25" t="n">
-        <v>0.0005379773162141888</v>
+        <v>0.0006937237425563847</v>
       </c>
       <c r="G19" s="25" t="n">
-        <v>0.001065997457151857</v>
+        <v>-0.001064425459726515</v>
       </c>
       <c r="H19" s="25" t="n">
-        <v>0.002739100661949267</v>
+        <v>0.0005713461581133839</v>
       </c>
       <c r="I19" s="25" t="n">
-        <v>-0.001045553893298079</v>
+        <v>0.001005025125628167</v>
       </c>
       <c r="J19" s="25" t="n">
-        <v>-0.008382553259544845</v>
+        <v>0.00263888966212189</v>
       </c>
       <c r="K19" s="5" t="n"/>
       <c r="L19" s="28" t="n"/>
@@ -2196,8 +2196,8 @@
           <t>DSPIC96</t>
         </is>
       </c>
-      <c r="C20" s="48" t="n">
-        <v>45901</v>
+      <c r="C20" s="50" t="n">
+        <v>45962</v>
       </c>
       <c r="D20" s="6" t="inlineStr">
         <is>
@@ -2210,19 +2210,19 @@
         </is>
       </c>
       <c r="F20" s="25" t="n">
-        <v>0.01521111542552289</v>
+        <v>0.01007203916779632</v>
       </c>
       <c r="G20" s="25" t="n">
-        <v>0.01563688186155493</v>
+        <v>0.01168973358412177</v>
       </c>
       <c r="H20" s="25" t="n">
-        <v>0.01511001397718554</v>
+        <v>0.01508168307081075</v>
       </c>
       <c r="I20" s="25" t="n">
-        <v>0.01188658731008219</v>
+        <v>0.01547352826862074</v>
       </c>
       <c r="J20" s="25" t="n">
-        <v>0.01510729226061785</v>
+        <v>0.01500856666215786</v>
       </c>
       <c r="K20" s="5" t="n"/>
       <c r="L20" s="28" t="inlineStr">
@@ -2275,8 +2275,8 @@
           <t>PSAVERT</t>
         </is>
       </c>
-      <c r="C21" s="48" t="n">
-        <v>45901</v>
+      <c r="C21" s="50" t="n">
+        <v>45962</v>
       </c>
       <c r="D21" s="6" t="inlineStr">
         <is>
@@ -2289,19 +2289,19 @@
         </is>
       </c>
       <c r="F21" s="6" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="G21" s="6" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="H21" s="6" t="n">
         <v>4</v>
       </c>
-      <c r="G21" s="6" t="n">
+      <c r="I21" s="6" t="n">
         <v>4.1</v>
       </c>
-      <c r="H21" s="6" t="n">
+      <c r="J21" s="6" t="n">
         <v>4.3</v>
-      </c>
-      <c r="I21" s="6" t="n">
-        <v>4.6</v>
-      </c>
-      <c r="J21" s="6" t="n">
-        <v>4.9</v>
       </c>
       <c r="K21" s="5" t="n"/>
       <c r="L21" s="28" t="n"/>
@@ -2350,8 +2350,8 @@
           <t>TOTALSA</t>
         </is>
       </c>
-      <c r="C22" s="48" t="n">
-        <v>45962</v>
+      <c r="C22" s="50" t="n">
+        <v>45992</v>
       </c>
       <c r="D22" s="6" t="inlineStr">
         <is>
@@ -2364,19 +2364,19 @@
         </is>
       </c>
       <c r="F22" s="24" t="n">
-        <v>15.926</v>
+        <v>16.481</v>
       </c>
       <c r="G22" s="24" t="n">
-        <v>15.63</v>
+        <v>16.117</v>
       </c>
       <c r="H22" s="24" t="n">
+        <v>15.807</v>
+      </c>
+      <c r="I22" s="24" t="n">
         <v>16.663</v>
       </c>
-      <c r="I22" s="24" t="n">
+      <c r="J22" s="24" t="n">
         <v>16.916</v>
-      </c>
-      <c r="J22" s="24" t="n">
-        <v>16.969</v>
       </c>
       <c r="K22" s="5" t="n"/>
       <c r="L22" s="28" t="inlineStr">
@@ -2425,8 +2425,8 @@
           <t>TOTALSA</t>
         </is>
       </c>
-      <c r="C23" s="48" t="n">
-        <v>45962</v>
+      <c r="C23" s="50" t="n">
+        <v>45992</v>
       </c>
       <c r="D23" s="6" t="inlineStr">
         <is>
@@ -2439,19 +2439,19 @@
         </is>
       </c>
       <c r="F23" s="25" t="n">
-        <v>-0.06345192590414578</v>
+        <v>-0.04761629586824606</v>
       </c>
       <c r="G23" s="25" t="n">
-        <v>-0.05593138439236531</v>
+        <v>-0.05221993531314308</v>
       </c>
       <c r="H23" s="25" t="n">
+        <v>-0.04524039623097369</v>
+      </c>
+      <c r="I23" s="25" t="n">
         <v>0.02114229685010411</v>
       </c>
-      <c r="I23" s="25" t="n">
+      <c r="J23" s="25" t="n">
         <v>0.05976694649793263</v>
-      </c>
-      <c r="J23" s="25" t="n">
-        <v>0.03944869831546719</v>
       </c>
       <c r="K23" s="5" t="n"/>
       <c r="M23" s="15" t="inlineStr">
@@ -2538,8 +2538,8 @@
           <t>PCEPI</t>
         </is>
       </c>
-      <c r="N24" s="48" t="n">
-        <v>45901</v>
+      <c r="N24" s="50" t="n">
+        <v>45962</v>
       </c>
       <c r="O24" s="6" t="inlineStr">
         <is>
@@ -2552,19 +2552,19 @@
         </is>
       </c>
       <c r="Q24" s="38" t="n">
-        <v>0.002663272761554536</v>
+        <v>0.002073098225740644</v>
       </c>
       <c r="R24" s="38" t="n">
-        <v>0.002599305276589803</v>
+        <v>0.001590597453477116</v>
       </c>
       <c r="S24" s="38" t="n">
-        <v>0.001688456167204588</v>
+        <v>0.002608155986582039</v>
       </c>
       <c r="T24" s="38" t="n">
-        <v>0.002872289919291005</v>
+        <v>0.002622873345935917</v>
       </c>
       <c r="U24" s="23" t="n">
-        <v>0.001823226317875459</v>
+        <v>0.001712126113473822</v>
       </c>
     </row>
     <row r="25">
@@ -2613,8 +2613,8 @@
           <t>PCEPI</t>
         </is>
       </c>
-      <c r="N25" s="48" t="n">
-        <v>45901</v>
+      <c r="N25" s="50" t="n">
+        <v>45962</v>
       </c>
       <c r="O25" s="6" t="inlineStr">
         <is>
@@ -2627,19 +2627,19 @@
         </is>
       </c>
       <c r="Q25" s="38" t="n">
-        <v>0.02788247801295064</v>
+        <v>0.02772852363262907</v>
       </c>
       <c r="R25" s="38" t="n">
-        <v>0.02742777809167892</v>
+        <v>0.02678040708789181</v>
       </c>
       <c r="S25" s="38" t="n">
-        <v>0.02603122777526338</v>
+        <v>0.02787442414870654</v>
       </c>
       <c r="T25" s="38" t="n">
-        <v>0.02593512979706808</v>
+        <v>0.02747620854151709</v>
       </c>
       <c r="U25" s="23" t="n">
-        <v>0.02458086065440864</v>
+        <v>0.0260554729423934</v>
       </c>
     </row>
     <row r="26">
@@ -2692,8 +2692,8 @@
           <t>PCEPILFE</t>
         </is>
       </c>
-      <c r="N26" s="48" t="n">
-        <v>45901</v>
+      <c r="N26" s="50" t="n">
+        <v>45962</v>
       </c>
       <c r="O26" s="6" t="inlineStr">
         <is>
@@ -2706,19 +2706,19 @@
         </is>
       </c>
       <c r="Q26" s="38" t="n">
-        <v>0.0019572715003906</v>
+        <v>0.001603546667924283</v>
       </c>
       <c r="R26" s="38" t="n">
-        <v>0.002222644076376623</v>
+        <v>0.002079493359799622</v>
       </c>
       <c r="S26" s="38" t="n">
-        <v>0.002418312572846748</v>
+        <v>0.001894029073346237</v>
       </c>
       <c r="T26" s="38" t="n">
-        <v>0.002631369743222756</v>
+        <v>0.002246302301668779</v>
       </c>
       <c r="U26" s="23" t="n">
-        <v>0.002294784146866347</v>
+        <v>0.002450028147572558</v>
       </c>
     </row>
     <row r="27">
@@ -2767,8 +2767,8 @@
           <t>PCEPILFE</t>
         </is>
       </c>
-      <c r="N27" s="48" t="n">
-        <v>45901</v>
+      <c r="N27" s="50" t="n">
+        <v>45962</v>
       </c>
       <c r="O27" s="6" t="inlineStr">
         <is>
@@ -2781,19 +2781,19 @@
         </is>
       </c>
       <c r="Q27" s="38" t="n">
-        <v>0.02825879189412473</v>
+        <v>0.02791177941627268</v>
       </c>
       <c r="R27" s="38" t="n">
-        <v>0.02906731206549277</v>
+        <v>0.02734349764196662</v>
       </c>
       <c r="S27" s="38" t="n">
-        <v>0.02859792858247025</v>
+        <v>0.02825069249833962</v>
       </c>
       <c r="T27" s="38" t="n">
-        <v>0.02807372205058803</v>
+        <v>0.02912416347215904</v>
       </c>
       <c r="U27" s="23" t="n">
-        <v>0.02783883382495944</v>
+        <v>0.02863047245567936</v>
       </c>
     </row>
     <row r="28">
@@ -2922,7 +2922,7 @@
         </is>
       </c>
       <c r="N29" s="50" t="n">
-        <v>46043</v>
+        <v>46044</v>
       </c>
       <c r="O29" s="6" t="inlineStr">
         <is>
@@ -2935,16 +2935,16 @@
         </is>
       </c>
       <c r="Q29" s="6" t="n">
-        <v>2.26</v>
+        <v>2.2</v>
       </c>
       <c r="R29" s="6" t="n">
         <v>2.26</v>
       </c>
       <c r="S29" s="6" t="n">
+        <v>2.26</v>
+      </c>
+      <c r="T29" s="6" t="n">
         <v>2.27</v>
-      </c>
-      <c r="T29" s="6" t="n">
-        <v>2.22</v>
       </c>
       <c r="U29" s="21" t="n">
         <v>2.22</v>
@@ -3001,7 +3001,7 @@
         </is>
       </c>
       <c r="N30" s="50" t="n">
-        <v>46043</v>
+        <v>46044</v>
       </c>
       <c r="O30" s="6" t="inlineStr">
         <is>
@@ -3014,16 +3014,16 @@
         </is>
       </c>
       <c r="Q30" s="6" t="n">
+        <v>2.31</v>
+      </c>
+      <c r="R30" s="6" t="n">
         <v>2.34</v>
-      </c>
-      <c r="R30" s="6" t="n">
-        <v>2.33</v>
       </c>
       <c r="S30" s="6" t="n">
         <v>2.33</v>
       </c>
       <c r="T30" s="6" t="n">
-        <v>2.29</v>
+        <v>2.33</v>
       </c>
       <c r="U30" s="21" t="n">
         <v>2.29</v>
@@ -3115,7 +3115,7 @@
           <t>INDPRO</t>
         </is>
       </c>
-      <c r="C32" s="50" t="n">
+      <c r="C32" s="48" t="n">
         <v>45992</v>
       </c>
       <c r="D32" s="6" t="inlineStr">
@@ -3186,7 +3186,7 @@
           <t>INDPRO</t>
         </is>
       </c>
-      <c r="C33" s="50" t="n">
+      <c r="C33" s="48" t="n">
         <v>45992</v>
       </c>
       <c r="D33" s="6" t="inlineStr">
@@ -3265,7 +3265,7 @@
           <t>TCU</t>
         </is>
       </c>
-      <c r="C34" s="50" t="n">
+      <c r="C34" s="48" t="n">
         <v>45992</v>
       </c>
       <c r="D34" s="6" t="inlineStr">
@@ -3301,7 +3301,7 @@
         </is>
       </c>
       <c r="N34" s="48" t="n">
-        <v>45901</v>
+        <v>45962</v>
       </c>
       <c r="O34" s="6" t="inlineStr">
         <is>
@@ -3314,19 +3314,19 @@
         </is>
       </c>
       <c r="Q34" s="38" t="n">
-        <v>0.00922239407158258</v>
+        <v>0.008267996311731092</v>
       </c>
       <c r="R34" s="38" t="n">
-        <v>0.01060107202271849</v>
+        <v>0.01042628043129703</v>
       </c>
       <c r="S34" s="38" t="n">
-        <v>0.01242491999209615</v>
+        <v>0.009230301788676142</v>
       </c>
       <c r="T34" s="38" t="n">
-        <v>0.01120289314371833</v>
+        <v>0.01055343698833223</v>
       </c>
       <c r="U34" s="23" t="n">
-        <v>0.01349386861907807</v>
+        <v>0.01240099690797541</v>
       </c>
     </row>
     <row r="35" ht="31.5" customHeight="1">
@@ -3380,7 +3380,7 @@
         </is>
       </c>
       <c r="N35" s="48" t="n">
-        <v>45901</v>
+        <v>45962</v>
       </c>
       <c r="O35" s="6" t="inlineStr">
         <is>
@@ -3393,19 +3393,19 @@
         </is>
       </c>
       <c r="Q35" s="38" t="n">
-        <v>-0.0007476675222880536</v>
+        <v>0.0003711201807323761</v>
       </c>
       <c r="R35" s="38" t="n">
-        <v>0.00151424432893621</v>
+        <v>0.002770616347913979</v>
       </c>
       <c r="S35" s="38" t="n">
-        <v>0.001613693871594046</v>
+        <v>-0.0006927352283296884</v>
       </c>
       <c r="T35" s="38" t="n">
-        <v>-0.0006622728576672898</v>
+        <v>0.001490702319483894</v>
       </c>
       <c r="U35" s="23" t="n">
-        <v>0.002329953587340228</v>
+        <v>0.001590026251228505</v>
       </c>
     </row>
     <row r="36" ht="31.5" customHeight="1">
@@ -3451,7 +3451,7 @@
         </is>
       </c>
       <c r="N36" s="48" t="n">
-        <v>45901</v>
+        <v>45962</v>
       </c>
       <c r="O36" s="6" t="inlineStr">
         <is>
@@ -3464,19 +3464,19 @@
         </is>
       </c>
       <c r="Q36" s="38" t="n">
-        <v>0.00922239407158258</v>
+        <v>0.008267996311731092</v>
       </c>
       <c r="R36" s="38" t="n">
-        <v>0.01060107202271849</v>
+        <v>0.01042628043129703</v>
       </c>
       <c r="S36" s="38" t="n">
-        <v>0.01242491999209615</v>
+        <v>0.009230301788676142</v>
       </c>
       <c r="T36" s="38" t="n">
-        <v>0.01120289314371833</v>
+        <v>0.01055343698833223</v>
       </c>
       <c r="U36" s="23" t="n">
-        <v>0.01349386861907807</v>
+        <v>0.01240099690797541</v>
       </c>
     </row>
     <row r="37">
@@ -4268,7 +4268,7 @@
         </is>
       </c>
       <c r="N47" s="50" t="n">
-        <v>46042</v>
+        <v>46043</v>
       </c>
       <c r="O47" s="6" t="inlineStr">
         <is>
@@ -4347,7 +4347,7 @@
         </is>
       </c>
       <c r="N48" s="50" t="n">
-        <v>46042</v>
+        <v>46043</v>
       </c>
       <c r="O48" s="6" t="inlineStr">
         <is>
@@ -4363,16 +4363,16 @@
         <v>3.6</v>
       </c>
       <c r="R48" s="6" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="S48" s="6" t="n">
         <v>3.59</v>
       </c>
-      <c r="S48" s="6" t="n">
+      <c r="T48" s="6" t="n">
         <v>3.56</v>
       </c>
-      <c r="T48" s="6" t="n">
+      <c r="U48" s="21" t="n">
         <v>3.51</v>
-      </c>
-      <c r="U48" s="21" t="n">
-        <v>3.53</v>
       </c>
     </row>
     <row r="49">
@@ -4422,7 +4422,7 @@
         </is>
       </c>
       <c r="N49" s="50" t="n">
-        <v>46042</v>
+        <v>46043</v>
       </c>
       <c r="O49" s="6" t="inlineStr">
         <is>
@@ -4435,19 +4435,19 @@
         </is>
       </c>
       <c r="Q49" s="6" t="n">
+        <v>3.83</v>
+      </c>
+      <c r="R49" s="6" t="n">
         <v>3.86</v>
       </c>
-      <c r="R49" s="6" t="n">
+      <c r="S49" s="6" t="n">
         <v>3.82</v>
       </c>
-      <c r="S49" s="6" t="n">
+      <c r="T49" s="6" t="n">
         <v>3.77</v>
       </c>
-      <c r="T49" s="6" t="n">
+      <c r="U49" s="21" t="n">
         <v>3.72</v>
-      </c>
-      <c r="U49" s="21" t="n">
-        <v>3.75</v>
       </c>
     </row>
     <row r="50">
@@ -4501,7 +4501,7 @@
         </is>
       </c>
       <c r="N50" s="50" t="n">
-        <v>46042</v>
+        <v>46043</v>
       </c>
       <c r="O50" s="6" t="inlineStr">
         <is>
@@ -4514,19 +4514,19 @@
         </is>
       </c>
       <c r="Q50" s="6" t="n">
+        <v>4.26</v>
+      </c>
+      <c r="R50" s="6" t="n">
         <v>4.3</v>
       </c>
-      <c r="R50" s="6" t="n">
+      <c r="S50" s="6" t="n">
         <v>4.24</v>
       </c>
-      <c r="S50" s="6" t="n">
+      <c r="T50" s="6" t="n">
         <v>4.17</v>
       </c>
-      <c r="T50" s="6" t="n">
+      <c r="U50" s="21" t="n">
         <v>4.15</v>
-      </c>
-      <c r="U50" s="21" t="n">
-        <v>4.18</v>
       </c>
     </row>
     <row r="51" ht="31.5" customHeight="1">
@@ -4575,8 +4575,8 @@
           <t>MORTGAGE30US</t>
         </is>
       </c>
-      <c r="N51" s="48" t="n">
-        <v>46034</v>
+      <c r="N51" s="50" t="n">
+        <v>46041</v>
       </c>
       <c r="O51" s="6" t="inlineStr">
         <is>
@@ -4589,19 +4589,19 @@
         </is>
       </c>
       <c r="Q51" s="6" t="n">
+        <v>6.09</v>
+      </c>
+      <c r="R51" s="6" t="n">
         <v>6.06</v>
       </c>
-      <c r="R51" s="6" t="n">
+      <c r="S51" s="6" t="n">
         <v>6.16</v>
       </c>
-      <c r="S51" s="6" t="n">
+      <c r="T51" s="6" t="n">
         <v>6.15</v>
       </c>
-      <c r="T51" s="6" t="n">
+      <c r="U51" s="21" t="n">
         <v>6.18</v>
-      </c>
-      <c r="U51" s="21" t="n">
-        <v>6.21</v>
       </c>
     </row>
     <row r="52" ht="16.15" customHeight="1" thickBot="1">
@@ -4627,7 +4627,7 @@
         </is>
       </c>
       <c r="N52" s="53" t="n">
-        <v>46042</v>
+        <v>46043</v>
       </c>
       <c r="O52" s="9" t="inlineStr">
         <is>
@@ -4640,19 +4640,19 @@
         </is>
       </c>
       <c r="Q52" s="9" t="n">
+        <v>5.88</v>
+      </c>
+      <c r="R52" s="9" t="n">
         <v>5.95</v>
       </c>
-      <c r="R52" s="9" t="n">
+      <c r="S52" s="9" t="n">
         <v>5.87</v>
       </c>
-      <c r="S52" s="9" t="n">
+      <c r="T52" s="9" t="n">
         <v>5.82</v>
       </c>
-      <c r="T52" s="9" t="n">
+      <c r="U52" s="22" t="n">
         <v>5.83</v>
-      </c>
-      <c r="U52" s="22" t="n">
-        <v>5.87</v>
       </c>
     </row>
     <row r="53" ht="21" customHeight="1">

</xml_diff>

<commit_message>
Update dashboards - 2026-01-24
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -1227,7 +1227,7 @@
         </is>
       </c>
       <c r="F7" s="44" t="n">
-        <v>2.6786</v>
+        <v>5.3721</v>
       </c>
       <c r="G7" s="44" t="n">
         <v>3.4728</v>
@@ -2847,7 +2847,7 @@
         </is>
       </c>
       <c r="N28" s="48" t="n">
-        <v>45962</v>
+        <v>45992</v>
       </c>
       <c r="O28" s="6" t="inlineStr">
         <is>
@@ -2860,19 +2860,19 @@
         </is>
       </c>
       <c r="Q28" s="6" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="R28" s="6" t="n">
         <v>4.5</v>
       </c>
-      <c r="R28" s="6" t="n">
+      <c r="S28" s="6" t="n">
         <v>4.6</v>
       </c>
-      <c r="S28" s="6" t="n">
+      <c r="T28" s="6" t="n">
         <v>4.7</v>
       </c>
-      <c r="T28" s="6" t="n">
+      <c r="U28" s="21" t="n">
         <v>4.8</v>
-      </c>
-      <c r="U28" s="21" t="n">
-        <v>4.5</v>
       </c>
     </row>
     <row r="29">
@@ -2922,7 +2922,7 @@
         </is>
       </c>
       <c r="N29" s="50" t="n">
-        <v>46044</v>
+        <v>46045</v>
       </c>
       <c r="O29" s="6" t="inlineStr">
         <is>
@@ -2935,19 +2935,19 @@
         </is>
       </c>
       <c r="Q29" s="6" t="n">
+        <v>2.18</v>
+      </c>
+      <c r="R29" s="6" t="n">
         <v>2.2</v>
-      </c>
-      <c r="R29" s="6" t="n">
-        <v>2.26</v>
       </c>
       <c r="S29" s="6" t="n">
         <v>2.26</v>
       </c>
       <c r="T29" s="6" t="n">
+        <v>2.26</v>
+      </c>
+      <c r="U29" s="21" t="n">
         <v>2.27</v>
-      </c>
-      <c r="U29" s="21" t="n">
-        <v>2.22</v>
       </c>
     </row>
     <row r="30">
@@ -3001,7 +3001,7 @@
         </is>
       </c>
       <c r="N30" s="50" t="n">
-        <v>46044</v>
+        <v>46045</v>
       </c>
       <c r="O30" s="6" t="inlineStr">
         <is>
@@ -3014,19 +3014,19 @@
         </is>
       </c>
       <c r="Q30" s="6" t="n">
+        <v>2.32</v>
+      </c>
+      <c r="R30" s="6" t="n">
         <v>2.31</v>
       </c>
-      <c r="R30" s="6" t="n">
+      <c r="S30" s="6" t="n">
         <v>2.34</v>
-      </c>
-      <c r="S30" s="6" t="n">
-        <v>2.33</v>
       </c>
       <c r="T30" s="6" t="n">
         <v>2.33</v>
       </c>
       <c r="U30" s="21" t="n">
-        <v>2.29</v>
+        <v>2.33</v>
       </c>
     </row>
     <row r="31">
@@ -4268,7 +4268,7 @@
         </is>
       </c>
       <c r="N47" s="50" t="n">
-        <v>46043</v>
+        <v>46044</v>
       </c>
       <c r="O47" s="6" t="inlineStr">
         <is>
@@ -4347,7 +4347,7 @@
         </is>
       </c>
       <c r="N48" s="50" t="n">
-        <v>46043</v>
+        <v>46044</v>
       </c>
       <c r="O48" s="6" t="inlineStr">
         <is>
@@ -4360,19 +4360,19 @@
         </is>
       </c>
       <c r="Q48" s="6" t="n">
-        <v>3.6</v>
+        <v>3.61</v>
       </c>
       <c r="R48" s="6" t="n">
         <v>3.6</v>
       </c>
       <c r="S48" s="6" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="T48" s="6" t="n">
         <v>3.59</v>
       </c>
-      <c r="T48" s="6" t="n">
+      <c r="U48" s="21" t="n">
         <v>3.56</v>
-      </c>
-      <c r="U48" s="21" t="n">
-        <v>3.51</v>
       </c>
     </row>
     <row r="49">
@@ -4422,7 +4422,7 @@
         </is>
       </c>
       <c r="N49" s="50" t="n">
-        <v>46043</v>
+        <v>46044</v>
       </c>
       <c r="O49" s="6" t="inlineStr">
         <is>
@@ -4435,19 +4435,19 @@
         </is>
       </c>
       <c r="Q49" s="6" t="n">
+        <v>3.85</v>
+      </c>
+      <c r="R49" s="6" t="n">
         <v>3.83</v>
       </c>
-      <c r="R49" s="6" t="n">
+      <c r="S49" s="6" t="n">
         <v>3.86</v>
       </c>
-      <c r="S49" s="6" t="n">
+      <c r="T49" s="6" t="n">
         <v>3.82</v>
       </c>
-      <c r="T49" s="6" t="n">
+      <c r="U49" s="21" t="n">
         <v>3.77</v>
-      </c>
-      <c r="U49" s="21" t="n">
-        <v>3.72</v>
       </c>
     </row>
     <row r="50">
@@ -4501,7 +4501,7 @@
         </is>
       </c>
       <c r="N50" s="50" t="n">
-        <v>46043</v>
+        <v>46044</v>
       </c>
       <c r="O50" s="6" t="inlineStr">
         <is>
@@ -4517,16 +4517,16 @@
         <v>4.26</v>
       </c>
       <c r="R50" s="6" t="n">
+        <v>4.26</v>
+      </c>
+      <c r="S50" s="6" t="n">
         <v>4.3</v>
       </c>
-      <c r="S50" s="6" t="n">
+      <c r="T50" s="6" t="n">
         <v>4.24</v>
       </c>
-      <c r="T50" s="6" t="n">
+      <c r="U50" s="21" t="n">
         <v>4.17</v>
-      </c>
-      <c r="U50" s="21" t="n">
-        <v>4.15</v>
       </c>
     </row>
     <row r="51" ht="31.5" customHeight="1">
@@ -4627,7 +4627,7 @@
         </is>
       </c>
       <c r="N52" s="53" t="n">
-        <v>46043</v>
+        <v>46044</v>
       </c>
       <c r="O52" s="9" t="inlineStr">
         <is>
@@ -4640,19 +4640,19 @@
         </is>
       </c>
       <c r="Q52" s="9" t="n">
+        <v>5.85</v>
+      </c>
+      <c r="R52" s="9" t="n">
         <v>5.88</v>
       </c>
-      <c r="R52" s="9" t="n">
+      <c r="S52" s="9" t="n">
         <v>5.95</v>
       </c>
-      <c r="S52" s="9" t="n">
+      <c r="T52" s="9" t="n">
         <v>5.87</v>
       </c>
-      <c r="T52" s="9" t="n">
+      <c r="U52" s="22" t="n">
         <v>5.82</v>
-      </c>
-      <c r="U52" s="22" t="n">
-        <v>5.83</v>
       </c>
     </row>
     <row r="53" ht="21" customHeight="1">

</xml_diff>

<commit_message>
Update dashboards - 2026-01-26
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -1073,7 +1073,7 @@
         </is>
       </c>
       <c r="F5" s="24" t="n">
-        <v>7773772.3</v>
+        <v>7774506.8</v>
       </c>
       <c r="G5" s="24" t="n">
         <v>7621432.3</v>
@@ -1148,7 +1148,7 @@
         </is>
       </c>
       <c r="F6" s="25" t="n">
-        <v>0.01998836885292543</v>
+        <v>0.02008474181421249</v>
       </c>
       <c r="G6" s="25" t="n">
         <v>0.0147664712214719</v>
@@ -2807,8 +2807,8 @@
           <t>DGORDER</t>
         </is>
       </c>
-      <c r="C28" s="48" t="n">
-        <v>45931</v>
+      <c r="C28" s="50" t="n">
+        <v>45962</v>
       </c>
       <c r="D28" s="6" t="inlineStr">
         <is>
@@ -2821,19 +2821,19 @@
         </is>
       </c>
       <c r="F28" s="25" t="n">
-        <v>-0.02191649132412532</v>
+        <v>0.05330084643761013</v>
       </c>
       <c r="G28" s="25" t="n">
+        <v>-0.02145810719185604</v>
+      </c>
+      <c r="H28" s="25" t="n">
         <v>0.006436255758670795</v>
       </c>
-      <c r="H28" s="25" t="n">
+      <c r="I28" s="25" t="n">
         <v>0.03004963172206243</v>
       </c>
-      <c r="I28" s="25" t="n">
+      <c r="J28" s="25" t="n">
         <v>-0.02799901206372835</v>
-      </c>
-      <c r="J28" s="25" t="n">
-        <v>-0.09389977010425232</v>
       </c>
       <c r="K28" s="5" t="n"/>
       <c r="L28" s="28" t="inlineStr">
@@ -2882,8 +2882,8 @@
           <t>DGORDER</t>
         </is>
       </c>
-      <c r="C29" s="48" t="n">
-        <v>45931</v>
+      <c r="C29" s="50" t="n">
+        <v>45962</v>
       </c>
       <c r="D29" s="6" t="inlineStr">
         <is>
@@ -2896,19 +2896,19 @@
         </is>
       </c>
       <c r="F29" s="25" t="n">
-        <v>0.04772459132664544</v>
+        <v>0.1229486023444545</v>
       </c>
       <c r="G29" s="25" t="n">
+        <v>0.04821561312937742</v>
+      </c>
+      <c r="H29" s="25" t="n">
         <v>0.07412067603746038</v>
       </c>
-      <c r="H29" s="25" t="n">
+      <c r="I29" s="25" t="n">
         <v>0.07661265288383932</v>
       </c>
-      <c r="I29" s="25" t="n">
+      <c r="J29" s="25" t="n">
         <v>0.03341358778313566</v>
-      </c>
-      <c r="J29" s="25" t="n">
-        <v>0.1089645997552716</v>
       </c>
       <c r="K29" s="5" t="n"/>
       <c r="L29" s="28" t="inlineStr">
@@ -2961,8 +2961,8 @@
           <t>ADXDNO</t>
         </is>
       </c>
-      <c r="C30" s="48" t="n">
-        <v>45931</v>
+      <c r="C30" s="50" t="n">
+        <v>45962</v>
       </c>
       <c r="D30" s="6" t="inlineStr">
         <is>
@@ -2975,19 +2975,19 @@
         </is>
       </c>
       <c r="F30" s="25" t="n">
-        <v>-0.01529652492391287</v>
+        <v>0.06566119548130511</v>
       </c>
       <c r="G30" s="25" t="n">
+        <v>-0.01337070344068647</v>
+      </c>
+      <c r="H30" s="25" t="n">
         <v>0.001174064535676367</v>
       </c>
-      <c r="H30" s="25" t="n">
+      <c r="I30" s="25" t="n">
         <v>0.01907672443132968</v>
       </c>
-      <c r="I30" s="25" t="n">
+      <c r="J30" s="25" t="n">
         <v>-0.02404555711932721</v>
-      </c>
-      <c r="J30" s="25" t="n">
-        <v>-0.09442194506291901</v>
       </c>
       <c r="K30" s="5" t="n"/>
       <c r="L30" s="28" t="inlineStr">
@@ -3036,8 +3036,8 @@
           <t>ADXDNO</t>
         </is>
       </c>
-      <c r="C31" s="48" t="n">
-        <v>45931</v>
+      <c r="C31" s="50" t="n">
+        <v>45962</v>
       </c>
       <c r="D31" s="6" t="inlineStr">
         <is>
@@ -3050,19 +3050,19 @@
         </is>
       </c>
       <c r="F31" s="25" t="n">
-        <v>0.04749518938811943</v>
+        <v>0.1256397039873348</v>
       </c>
       <c r="G31" s="25" t="n">
+        <v>0.04954381497984299</v>
+      </c>
+      <c r="H31" s="25" t="n">
         <v>0.06502168244015354</v>
       </c>
-      <c r="H31" s="25" t="n">
+      <c r="I31" s="25" t="n">
         <v>0.06671073894520346</v>
       </c>
-      <c r="I31" s="25" t="n">
+      <c r="J31" s="25" t="n">
         <v>0.0329297153895499</v>
-      </c>
-      <c r="J31" s="25" t="n">
-        <v>0.1029410098461701</v>
       </c>
       <c r="K31" s="5" t="n"/>
       <c r="L31" s="28" t="inlineStr">

</xml_diff>

<commit_message>
Update dashboards - 2026-01-27
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -1227,7 +1227,7 @@
         </is>
       </c>
       <c r="F7" s="44" t="n">
-        <v>5.3721</v>
+        <v>5.3988</v>
       </c>
       <c r="G7" s="44" t="n">
         <v>3.4728</v>
@@ -2922,7 +2922,7 @@
         </is>
       </c>
       <c r="N29" s="50" t="n">
-        <v>46045</v>
+        <v>46048</v>
       </c>
       <c r="O29" s="6" t="inlineStr">
         <is>
@@ -2935,19 +2935,19 @@
         </is>
       </c>
       <c r="Q29" s="6" t="n">
+        <v>2.19</v>
+      </c>
+      <c r="R29" s="6" t="n">
         <v>2.18</v>
       </c>
-      <c r="R29" s="6" t="n">
+      <c r="S29" s="6" t="n">
         <v>2.2</v>
-      </c>
-      <c r="S29" s="6" t="n">
-        <v>2.26</v>
       </c>
       <c r="T29" s="6" t="n">
         <v>2.26</v>
       </c>
       <c r="U29" s="21" t="n">
-        <v>2.27</v>
+        <v>2.26</v>
       </c>
     </row>
     <row r="30">
@@ -3001,7 +3001,7 @@
         </is>
       </c>
       <c r="N30" s="50" t="n">
-        <v>46045</v>
+        <v>46048</v>
       </c>
       <c r="O30" s="6" t="inlineStr">
         <is>
@@ -3017,13 +3017,13 @@
         <v>2.32</v>
       </c>
       <c r="R30" s="6" t="n">
+        <v>2.32</v>
+      </c>
+      <c r="S30" s="6" t="n">
         <v>2.31</v>
       </c>
-      <c r="S30" s="6" t="n">
+      <c r="T30" s="6" t="n">
         <v>2.34</v>
-      </c>
-      <c r="T30" s="6" t="n">
-        <v>2.33</v>
       </c>
       <c r="U30" s="21" t="n">
         <v>2.33</v>
@@ -3529,8 +3529,8 @@
           <t>CSUSHPINSA</t>
         </is>
       </c>
-      <c r="N37" s="48" t="n">
-        <v>45931</v>
+      <c r="N37" s="50" t="n">
+        <v>45962</v>
       </c>
       <c r="O37" s="6" t="inlineStr">
         <is>
@@ -3543,19 +3543,19 @@
         </is>
       </c>
       <c r="Q37" s="38" t="n">
-        <v>-0.001629288280675323</v>
+        <v>-0.001086738141768961</v>
       </c>
       <c r="R37" s="38" t="n">
-        <v>-0.00274944298770774</v>
+        <v>-0.001422604825913387</v>
       </c>
       <c r="S37" s="38" t="n">
-        <v>-0.003326424682615015</v>
+        <v>-0.002737383934011794</v>
       </c>
       <c r="T37" s="38" t="n">
-        <v>-0.001932894486878389</v>
+        <v>-0.003323493777513176</v>
       </c>
       <c r="U37" s="23" t="n">
-        <v>0.0005672235313285423</v>
+        <v>-0.001935956624922186</v>
       </c>
     </row>
     <row r="38">
@@ -3583,7 +3583,7 @@
         </is>
       </c>
       <c r="F38" s="24" t="n">
-        <v>1412</v>
+        <v>1411</v>
       </c>
       <c r="G38" s="24" t="n">
         <v>1415</v>
@@ -3604,8 +3604,8 @@
           <t>CSUSHPINSA</t>
         </is>
       </c>
-      <c r="N38" s="48" t="n">
-        <v>45931</v>
+      <c r="N38" s="50" t="n">
+        <v>45962</v>
       </c>
       <c r="O38" s="6" t="inlineStr">
         <is>
@@ -3618,19 +3618,19 @@
         </is>
       </c>
       <c r="Q38" s="38" t="n">
-        <v>0.01361915137225375</v>
+        <v>0.0136158225247961</v>
       </c>
       <c r="R38" s="38" t="n">
-        <v>0.01314403621693212</v>
+        <v>0.01383543760782397</v>
       </c>
       <c r="S38" s="38" t="n">
-        <v>0.0147934636823388</v>
+        <v>0.01314419813616001</v>
       </c>
       <c r="T38" s="38" t="n">
-        <v>0.01644499448762562</v>
+        <v>0.0147750973624467</v>
       </c>
       <c r="U38" s="23" t="n">
-        <v>0.01942153460248559</v>
+        <v>0.01642359863525655</v>
       </c>
     </row>
     <row r="39" ht="31.5" customHeight="1">
@@ -3654,7 +3654,7 @@
         </is>
       </c>
       <c r="F39" s="38" t="n">
-        <v>-0.01120448179271709</v>
+        <v>-0.0119047619047619</v>
       </c>
       <c r="G39" s="38" t="n">
         <v>-0.01324965132496513</v>
@@ -4268,7 +4268,7 @@
         </is>
       </c>
       <c r="N47" s="50" t="n">
-        <v>46044</v>
+        <v>46045</v>
       </c>
       <c r="O47" s="6" t="inlineStr">
         <is>
@@ -4347,7 +4347,7 @@
         </is>
       </c>
       <c r="N48" s="50" t="n">
-        <v>46044</v>
+        <v>46045</v>
       </c>
       <c r="O48" s="6" t="inlineStr">
         <is>
@@ -4360,19 +4360,19 @@
         </is>
       </c>
       <c r="Q48" s="6" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="R48" s="6" t="n">
         <v>3.61</v>
-      </c>
-      <c r="R48" s="6" t="n">
-        <v>3.6</v>
       </c>
       <c r="S48" s="6" t="n">
         <v>3.6</v>
       </c>
       <c r="T48" s="6" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="U48" s="21" t="n">
         <v>3.59</v>
-      </c>
-      <c r="U48" s="21" t="n">
-        <v>3.56</v>
       </c>
     </row>
     <row r="49">
@@ -4422,7 +4422,7 @@
         </is>
       </c>
       <c r="N49" s="50" t="n">
-        <v>46044</v>
+        <v>46045</v>
       </c>
       <c r="O49" s="6" t="inlineStr">
         <is>
@@ -4435,19 +4435,19 @@
         </is>
       </c>
       <c r="Q49" s="6" t="n">
+        <v>3.84</v>
+      </c>
+      <c r="R49" s="6" t="n">
         <v>3.85</v>
       </c>
-      <c r="R49" s="6" t="n">
+      <c r="S49" s="6" t="n">
         <v>3.83</v>
       </c>
-      <c r="S49" s="6" t="n">
+      <c r="T49" s="6" t="n">
         <v>3.86</v>
       </c>
-      <c r="T49" s="6" t="n">
+      <c r="U49" s="21" t="n">
         <v>3.82</v>
-      </c>
-      <c r="U49" s="21" t="n">
-        <v>3.77</v>
       </c>
     </row>
     <row r="50">
@@ -4501,7 +4501,7 @@
         </is>
       </c>
       <c r="N50" s="50" t="n">
-        <v>46044</v>
+        <v>46045</v>
       </c>
       <c r="O50" s="6" t="inlineStr">
         <is>
@@ -4514,19 +4514,19 @@
         </is>
       </c>
       <c r="Q50" s="6" t="n">
-        <v>4.26</v>
+        <v>4.24</v>
       </c>
       <c r="R50" s="6" t="n">
         <v>4.26</v>
       </c>
       <c r="S50" s="6" t="n">
+        <v>4.26</v>
+      </c>
+      <c r="T50" s="6" t="n">
         <v>4.3</v>
       </c>
-      <c r="T50" s="6" t="n">
+      <c r="U50" s="21" t="n">
         <v>4.24</v>
-      </c>
-      <c r="U50" s="21" t="n">
-        <v>4.17</v>
       </c>
     </row>
     <row r="51" ht="31.5" customHeight="1">
@@ -4627,7 +4627,7 @@
         </is>
       </c>
       <c r="N52" s="53" t="n">
-        <v>46044</v>
+        <v>46045</v>
       </c>
       <c r="O52" s="9" t="inlineStr">
         <is>
@@ -4643,16 +4643,16 @@
         <v>5.85</v>
       </c>
       <c r="R52" s="9" t="n">
+        <v>5.85</v>
+      </c>
+      <c r="S52" s="9" t="n">
         <v>5.88</v>
       </c>
-      <c r="S52" s="9" t="n">
+      <c r="T52" s="9" t="n">
         <v>5.95</v>
       </c>
-      <c r="T52" s="9" t="n">
+      <c r="U52" s="22" t="n">
         <v>5.87</v>
-      </c>
-      <c r="U52" s="22" t="n">
-        <v>5.82</v>
       </c>
     </row>
     <row r="53" ht="21" customHeight="1">

</xml_diff>

<commit_message>
Update dashboards - 2026-01-28
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -2922,7 +2922,7 @@
         </is>
       </c>
       <c r="N29" s="50" t="n">
-        <v>46048</v>
+        <v>46049</v>
       </c>
       <c r="O29" s="6" t="inlineStr">
         <is>
@@ -2935,16 +2935,16 @@
         </is>
       </c>
       <c r="Q29" s="6" t="n">
+        <v>2.21</v>
+      </c>
+      <c r="R29" s="6" t="n">
         <v>2.19</v>
       </c>
-      <c r="R29" s="6" t="n">
+      <c r="S29" s="6" t="n">
         <v>2.18</v>
       </c>
-      <c r="S29" s="6" t="n">
+      <c r="T29" s="6" t="n">
         <v>2.2</v>
-      </c>
-      <c r="T29" s="6" t="n">
-        <v>2.26</v>
       </c>
       <c r="U29" s="21" t="n">
         <v>2.26</v>
@@ -3001,7 +3001,7 @@
         </is>
       </c>
       <c r="N30" s="50" t="n">
-        <v>46048</v>
+        <v>46049</v>
       </c>
       <c r="O30" s="6" t="inlineStr">
         <is>
@@ -3014,19 +3014,19 @@
         </is>
       </c>
       <c r="Q30" s="6" t="n">
-        <v>2.32</v>
+        <v>2.34</v>
       </c>
       <c r="R30" s="6" t="n">
         <v>2.32</v>
       </c>
       <c r="S30" s="6" t="n">
+        <v>2.32</v>
+      </c>
+      <c r="T30" s="6" t="n">
         <v>2.31</v>
       </c>
-      <c r="T30" s="6" t="n">
+      <c r="U30" s="21" t="n">
         <v>2.34</v>
-      </c>
-      <c r="U30" s="21" t="n">
-        <v>2.33</v>
       </c>
     </row>
     <row r="31">
@@ -4268,7 +4268,7 @@
         </is>
       </c>
       <c r="N47" s="50" t="n">
-        <v>46045</v>
+        <v>46048</v>
       </c>
       <c r="O47" s="6" t="inlineStr">
         <is>
@@ -4347,7 +4347,7 @@
         </is>
       </c>
       <c r="N48" s="50" t="n">
-        <v>46045</v>
+        <v>46048</v>
       </c>
       <c r="O48" s="6" t="inlineStr">
         <is>
@@ -4360,19 +4360,19 @@
         </is>
       </c>
       <c r="Q48" s="6" t="n">
+        <v>3.56</v>
+      </c>
+      <c r="R48" s="6" t="n">
         <v>3.6</v>
       </c>
-      <c r="R48" s="6" t="n">
+      <c r="S48" s="6" t="n">
         <v>3.61</v>
-      </c>
-      <c r="S48" s="6" t="n">
-        <v>3.6</v>
       </c>
       <c r="T48" s="6" t="n">
         <v>3.6</v>
       </c>
       <c r="U48" s="21" t="n">
-        <v>3.59</v>
+        <v>3.6</v>
       </c>
     </row>
     <row r="49">
@@ -4422,7 +4422,7 @@
         </is>
       </c>
       <c r="N49" s="50" t="n">
-        <v>46045</v>
+        <v>46048</v>
       </c>
       <c r="O49" s="6" t="inlineStr">
         <is>
@@ -4435,19 +4435,19 @@
         </is>
       </c>
       <c r="Q49" s="6" t="n">
+        <v>3.82</v>
+      </c>
+      <c r="R49" s="6" t="n">
         <v>3.84</v>
       </c>
-      <c r="R49" s="6" t="n">
+      <c r="S49" s="6" t="n">
         <v>3.85</v>
       </c>
-      <c r="S49" s="6" t="n">
+      <c r="T49" s="6" t="n">
         <v>3.83</v>
       </c>
-      <c r="T49" s="6" t="n">
+      <c r="U49" s="21" t="n">
         <v>3.86</v>
-      </c>
-      <c r="U49" s="21" t="n">
-        <v>3.82</v>
       </c>
     </row>
     <row r="50">
@@ -4501,7 +4501,7 @@
         </is>
       </c>
       <c r="N50" s="50" t="n">
-        <v>46045</v>
+        <v>46048</v>
       </c>
       <c r="O50" s="6" t="inlineStr">
         <is>
@@ -4514,19 +4514,19 @@
         </is>
       </c>
       <c r="Q50" s="6" t="n">
+        <v>4.22</v>
+      </c>
+      <c r="R50" s="6" t="n">
         <v>4.24</v>
-      </c>
-      <c r="R50" s="6" t="n">
-        <v>4.26</v>
       </c>
       <c r="S50" s="6" t="n">
         <v>4.26</v>
       </c>
       <c r="T50" s="6" t="n">
+        <v>4.26</v>
+      </c>
+      <c r="U50" s="21" t="n">
         <v>4.3</v>
-      </c>
-      <c r="U50" s="21" t="n">
-        <v>4.24</v>
       </c>
     </row>
     <row r="51" ht="31.5" customHeight="1">
@@ -4627,7 +4627,7 @@
         </is>
       </c>
       <c r="N52" s="53" t="n">
-        <v>46045</v>
+        <v>46048</v>
       </c>
       <c r="O52" s="9" t="inlineStr">
         <is>
@@ -4640,19 +4640,19 @@
         </is>
       </c>
       <c r="Q52" s="9" t="n">
-        <v>5.85</v>
+        <v>5.83</v>
       </c>
       <c r="R52" s="9" t="n">
         <v>5.85</v>
       </c>
       <c r="S52" s="9" t="n">
+        <v>5.85</v>
+      </c>
+      <c r="T52" s="9" t="n">
         <v>5.88</v>
       </c>
-      <c r="T52" s="9" t="n">
+      <c r="U52" s="22" t="n">
         <v>5.95</v>
-      </c>
-      <c r="U52" s="22" t="n">
-        <v>5.87</v>
       </c>
     </row>
     <row r="53" ht="21" customHeight="1">

</xml_diff>

<commit_message>
Update dashboards - 2026-01-29
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -1525,7 +1525,7 @@
           <t>PCEDGC96</t>
         </is>
       </c>
-      <c r="C11" s="50" t="n">
+      <c r="C11" s="48" t="n">
         <v>45962</v>
       </c>
       <c r="D11" s="6" t="inlineStr">
@@ -1600,7 +1600,7 @@
           <t>PCEDGC96</t>
         </is>
       </c>
-      <c r="C12" s="50" t="n">
+      <c r="C12" s="48" t="n">
         <v>45962</v>
       </c>
       <c r="D12" s="6" t="inlineStr">
@@ -1679,7 +1679,7 @@
           <t>PCENDC96</t>
         </is>
       </c>
-      <c r="C13" s="50" t="n">
+      <c r="C13" s="48" t="n">
         <v>45962</v>
       </c>
       <c r="D13" s="6" t="inlineStr">
@@ -1719,7 +1719,7 @@
         </is>
       </c>
       <c r="N13" s="50" t="n">
-        <v>46034</v>
+        <v>46041</v>
       </c>
       <c r="O13" s="6" t="inlineStr">
         <is>
@@ -1732,19 +1732,19 @@
         </is>
       </c>
       <c r="Q13" s="24" t="n">
+        <v>209000</v>
+      </c>
+      <c r="R13" s="24" t="n">
+        <v>210000</v>
+      </c>
+      <c r="S13" s="24" t="n">
+        <v>199000</v>
+      </c>
+      <c r="T13" s="24" t="n">
+        <v>207000</v>
+      </c>
+      <c r="U13" s="26" t="n">
         <v>200000</v>
-      </c>
-      <c r="R13" s="24" t="n">
-        <v>199000</v>
-      </c>
-      <c r="S13" s="24" t="n">
-        <v>207000</v>
-      </c>
-      <c r="T13" s="24" t="n">
-        <v>200000</v>
-      </c>
-      <c r="U13" s="26" t="n">
-        <v>215000</v>
       </c>
     </row>
     <row r="14">
@@ -1754,7 +1754,7 @@
           <t>PCENDC96</t>
         </is>
       </c>
-      <c r="C14" s="50" t="n">
+      <c r="C14" s="48" t="n">
         <v>45962</v>
       </c>
       <c r="D14" s="6" t="inlineStr">
@@ -1794,7 +1794,7 @@
         </is>
       </c>
       <c r="N14" s="50" t="n">
-        <v>46027</v>
+        <v>46034</v>
       </c>
       <c r="O14" s="6" t="inlineStr">
         <is>
@@ -1807,19 +1807,19 @@
         </is>
       </c>
       <c r="Q14" s="24" t="n">
-        <v>1849000</v>
+        <v>1827000</v>
       </c>
       <c r="R14" s="24" t="n">
+        <v>1865000</v>
+      </c>
+      <c r="S14" s="24" t="n">
         <v>1875000</v>
       </c>
-      <c r="S14" s="24" t="n">
+      <c r="T14" s="24" t="n">
         <v>1903000</v>
       </c>
-      <c r="T14" s="24" t="n">
+      <c r="U14" s="26" t="n">
         <v>1856000</v>
-      </c>
-      <c r="U14" s="26" t="n">
-        <v>1914000</v>
       </c>
     </row>
     <row r="15">
@@ -1833,7 +1833,7 @@
           <t>PCESC96</t>
         </is>
       </c>
-      <c r="C15" s="50" t="n">
+      <c r="C15" s="48" t="n">
         <v>45962</v>
       </c>
       <c r="D15" s="6" t="inlineStr">
@@ -1908,7 +1908,7 @@
           <t>PCESC96</t>
         </is>
       </c>
-      <c r="C16" s="50" t="n">
+      <c r="C16" s="48" t="n">
         <v>45962</v>
       </c>
       <c r="D16" s="6" t="inlineStr">
@@ -2125,7 +2125,7 @@
           <t>DSPIC96</t>
         </is>
       </c>
-      <c r="C19" s="50" t="n">
+      <c r="C19" s="48" t="n">
         <v>45962</v>
       </c>
       <c r="D19" s="6" t="inlineStr">
@@ -2196,7 +2196,7 @@
           <t>DSPIC96</t>
         </is>
       </c>
-      <c r="C20" s="50" t="n">
+      <c r="C20" s="48" t="n">
         <v>45962</v>
       </c>
       <c r="D20" s="6" t="inlineStr">
@@ -2275,7 +2275,7 @@
           <t>PSAVERT</t>
         </is>
       </c>
-      <c r="C21" s="50" t="n">
+      <c r="C21" s="48" t="n">
         <v>45962</v>
       </c>
       <c r="D21" s="6" t="inlineStr">
@@ -2350,7 +2350,7 @@
           <t>TOTALSA</t>
         </is>
       </c>
-      <c r="C22" s="50" t="n">
+      <c r="C22" s="48" t="n">
         <v>45992</v>
       </c>
       <c r="D22" s="6" t="inlineStr">
@@ -2425,7 +2425,7 @@
           <t>TOTALSA</t>
         </is>
       </c>
-      <c r="C23" s="50" t="n">
+      <c r="C23" s="48" t="n">
         <v>45992</v>
       </c>
       <c r="D23" s="6" t="inlineStr">
@@ -2538,7 +2538,7 @@
           <t>PCEPI</t>
         </is>
       </c>
-      <c r="N24" s="50" t="n">
+      <c r="N24" s="48" t="n">
         <v>45962</v>
       </c>
       <c r="O24" s="6" t="inlineStr">
@@ -2613,7 +2613,7 @@
           <t>PCEPI</t>
         </is>
       </c>
-      <c r="N25" s="50" t="n">
+      <c r="N25" s="48" t="n">
         <v>45962</v>
       </c>
       <c r="O25" s="6" t="inlineStr">
@@ -2692,7 +2692,7 @@
           <t>PCEPILFE</t>
         </is>
       </c>
-      <c r="N26" s="50" t="n">
+      <c r="N26" s="48" t="n">
         <v>45962</v>
       </c>
       <c r="O26" s="6" t="inlineStr">
@@ -2767,7 +2767,7 @@
           <t>PCEPILFE</t>
         </is>
       </c>
-      <c r="N27" s="50" t="n">
+      <c r="N27" s="48" t="n">
         <v>45962</v>
       </c>
       <c r="O27" s="6" t="inlineStr">
@@ -2922,7 +2922,7 @@
         </is>
       </c>
       <c r="N29" s="50" t="n">
-        <v>46049</v>
+        <v>46050</v>
       </c>
       <c r="O29" s="6" t="inlineStr">
         <is>
@@ -2935,19 +2935,19 @@
         </is>
       </c>
       <c r="Q29" s="6" t="n">
+        <v>2.22</v>
+      </c>
+      <c r="R29" s="6" t="n">
         <v>2.21</v>
       </c>
-      <c r="R29" s="6" t="n">
+      <c r="S29" s="6" t="n">
         <v>2.19</v>
       </c>
-      <c r="S29" s="6" t="n">
+      <c r="T29" s="6" t="n">
         <v>2.18</v>
       </c>
-      <c r="T29" s="6" t="n">
+      <c r="U29" s="21" t="n">
         <v>2.2</v>
-      </c>
-      <c r="U29" s="21" t="n">
-        <v>2.26</v>
       </c>
     </row>
     <row r="30">
@@ -3001,7 +3001,7 @@
         </is>
       </c>
       <c r="N30" s="50" t="n">
-        <v>46049</v>
+        <v>46050</v>
       </c>
       <c r="O30" s="6" t="inlineStr">
         <is>
@@ -3014,19 +3014,19 @@
         </is>
       </c>
       <c r="Q30" s="6" t="n">
+        <v>2.36</v>
+      </c>
+      <c r="R30" s="6" t="n">
         <v>2.34</v>
-      </c>
-      <c r="R30" s="6" t="n">
-        <v>2.32</v>
       </c>
       <c r="S30" s="6" t="n">
         <v>2.32</v>
       </c>
       <c r="T30" s="6" t="n">
+        <v>2.32</v>
+      </c>
+      <c r="U30" s="21" t="n">
         <v>2.31</v>
-      </c>
-      <c r="U30" s="21" t="n">
-        <v>2.34</v>
       </c>
     </row>
     <row r="31">
@@ -4268,7 +4268,7 @@
         </is>
       </c>
       <c r="N47" s="50" t="n">
-        <v>46048</v>
+        <v>46049</v>
       </c>
       <c r="O47" s="6" t="inlineStr">
         <is>
@@ -4347,7 +4347,7 @@
         </is>
       </c>
       <c r="N48" s="50" t="n">
-        <v>46048</v>
+        <v>46049</v>
       </c>
       <c r="O48" s="6" t="inlineStr">
         <is>
@@ -4360,16 +4360,16 @@
         </is>
       </c>
       <c r="Q48" s="6" t="n">
+        <v>3.53</v>
+      </c>
+      <c r="R48" s="6" t="n">
         <v>3.56</v>
       </c>
-      <c r="R48" s="6" t="n">
+      <c r="S48" s="6" t="n">
         <v>3.6</v>
       </c>
-      <c r="S48" s="6" t="n">
+      <c r="T48" s="6" t="n">
         <v>3.61</v>
-      </c>
-      <c r="T48" s="6" t="n">
-        <v>3.6</v>
       </c>
       <c r="U48" s="21" t="n">
         <v>3.6</v>
@@ -4422,7 +4422,7 @@
         </is>
       </c>
       <c r="N49" s="50" t="n">
-        <v>46048</v>
+        <v>46049</v>
       </c>
       <c r="O49" s="6" t="inlineStr">
         <is>
@@ -4435,19 +4435,19 @@
         </is>
       </c>
       <c r="Q49" s="6" t="n">
+        <v>3.81</v>
+      </c>
+      <c r="R49" s="6" t="n">
         <v>3.82</v>
       </c>
-      <c r="R49" s="6" t="n">
+      <c r="S49" s="6" t="n">
         <v>3.84</v>
       </c>
-      <c r="S49" s="6" t="n">
+      <c r="T49" s="6" t="n">
         <v>3.85</v>
       </c>
-      <c r="T49" s="6" t="n">
+      <c r="U49" s="21" t="n">
         <v>3.83</v>
-      </c>
-      <c r="U49" s="21" t="n">
-        <v>3.86</v>
       </c>
     </row>
     <row r="50">
@@ -4501,7 +4501,7 @@
         </is>
       </c>
       <c r="N50" s="50" t="n">
-        <v>46048</v>
+        <v>46049</v>
       </c>
       <c r="O50" s="6" t="inlineStr">
         <is>
@@ -4514,19 +4514,19 @@
         </is>
       </c>
       <c r="Q50" s="6" t="n">
+        <v>4.24</v>
+      </c>
+      <c r="R50" s="6" t="n">
         <v>4.22</v>
       </c>
-      <c r="R50" s="6" t="n">
+      <c r="S50" s="6" t="n">
         <v>4.24</v>
-      </c>
-      <c r="S50" s="6" t="n">
-        <v>4.26</v>
       </c>
       <c r="T50" s="6" t="n">
         <v>4.26</v>
       </c>
       <c r="U50" s="21" t="n">
-        <v>4.3</v>
+        <v>4.26</v>
       </c>
     </row>
     <row r="51" ht="31.5" customHeight="1">
@@ -4575,7 +4575,7 @@
           <t>MORTGAGE30US</t>
         </is>
       </c>
-      <c r="N51" s="50" t="n">
+      <c r="N51" s="48" t="n">
         <v>46041</v>
       </c>
       <c r="O51" s="6" t="inlineStr">
@@ -4627,7 +4627,7 @@
         </is>
       </c>
       <c r="N52" s="53" t="n">
-        <v>46048</v>
+        <v>46049</v>
       </c>
       <c r="O52" s="9" t="inlineStr">
         <is>
@@ -4640,19 +4640,19 @@
         </is>
       </c>
       <c r="Q52" s="9" t="n">
+        <v>5.85</v>
+      </c>
+      <c r="R52" s="9" t="n">
         <v>5.83</v>
-      </c>
-      <c r="R52" s="9" t="n">
-        <v>5.85</v>
       </c>
       <c r="S52" s="9" t="n">
         <v>5.85</v>
       </c>
       <c r="T52" s="9" t="n">
+        <v>5.85</v>
+      </c>
+      <c r="U52" s="22" t="n">
         <v>5.88</v>
-      </c>
-      <c r="U52" s="22" t="n">
-        <v>5.95</v>
       </c>
     </row>
     <row r="53" ht="21" customHeight="1">

</xml_diff>

<commit_message>
Update dashboards - 2026-01-30
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -1227,7 +1227,7 @@
         </is>
       </c>
       <c r="F7" s="44" t="n">
-        <v>5.3988</v>
+        <v>4.2373</v>
       </c>
       <c r="G7" s="44" t="n">
         <v>3.4728</v>
@@ -2807,7 +2807,7 @@
           <t>DGORDER</t>
         </is>
       </c>
-      <c r="C28" s="50" t="n">
+      <c r="C28" s="48" t="n">
         <v>45962</v>
       </c>
       <c r="D28" s="6" t="inlineStr">
@@ -2821,10 +2821,10 @@
         </is>
       </c>
       <c r="F28" s="25" t="n">
-        <v>0.05330084643761013</v>
+        <v>0.0526514289430049</v>
       </c>
       <c r="G28" s="25" t="n">
-        <v>-0.02145810719185604</v>
+        <v>-0.02093605859677161</v>
       </c>
       <c r="H28" s="25" t="n">
         <v>0.006436255758670795</v>
@@ -2882,7 +2882,7 @@
           <t>DGORDER</t>
         </is>
       </c>
-      <c r="C29" s="50" t="n">
+      <c r="C29" s="48" t="n">
         <v>45962</v>
       </c>
       <c r="D29" s="6" t="inlineStr">
@@ -2896,10 +2896,10 @@
         </is>
       </c>
       <c r="F29" s="25" t="n">
-        <v>0.1229486023444545</v>
+        <v>0.1228549628910314</v>
       </c>
       <c r="G29" s="25" t="n">
-        <v>0.04821561312937742</v>
+        <v>0.04877483240471108</v>
       </c>
       <c r="H29" s="25" t="n">
         <v>0.07412067603746038</v>
@@ -2922,7 +2922,7 @@
         </is>
       </c>
       <c r="N29" s="50" t="n">
-        <v>46050</v>
+        <v>46051</v>
       </c>
       <c r="O29" s="6" t="inlineStr">
         <is>
@@ -2935,19 +2935,19 @@
         </is>
       </c>
       <c r="Q29" s="6" t="n">
+        <v>2.18</v>
+      </c>
+      <c r="R29" s="6" t="n">
         <v>2.22</v>
       </c>
-      <c r="R29" s="6" t="n">
+      <c r="S29" s="6" t="n">
         <v>2.21</v>
       </c>
-      <c r="S29" s="6" t="n">
+      <c r="T29" s="6" t="n">
         <v>2.19</v>
       </c>
-      <c r="T29" s="6" t="n">
+      <c r="U29" s="21" t="n">
         <v>2.18</v>
-      </c>
-      <c r="U29" s="21" t="n">
-        <v>2.2</v>
       </c>
     </row>
     <row r="30">
@@ -2961,7 +2961,7 @@
           <t>ADXDNO</t>
         </is>
       </c>
-      <c r="C30" s="50" t="n">
+      <c r="C30" s="48" t="n">
         <v>45962</v>
       </c>
       <c r="D30" s="6" t="inlineStr">
@@ -2975,10 +2975,10 @@
         </is>
       </c>
       <c r="F30" s="25" t="n">
-        <v>0.06566119548130511</v>
+        <v>0.06490461658514834</v>
       </c>
       <c r="G30" s="25" t="n">
-        <v>-0.01337070344068647</v>
+        <v>-0.0128376635658648</v>
       </c>
       <c r="H30" s="25" t="n">
         <v>0.001174064535676367</v>
@@ -3001,7 +3001,7 @@
         </is>
       </c>
       <c r="N30" s="50" t="n">
-        <v>46050</v>
+        <v>46051</v>
       </c>
       <c r="O30" s="6" t="inlineStr">
         <is>
@@ -3014,19 +3014,19 @@
         </is>
       </c>
       <c r="Q30" s="6" t="n">
+        <v>2.35</v>
+      </c>
+      <c r="R30" s="6" t="n">
         <v>2.36</v>
       </c>
-      <c r="R30" s="6" t="n">
+      <c r="S30" s="6" t="n">
         <v>2.34</v>
-      </c>
-      <c r="S30" s="6" t="n">
-        <v>2.32</v>
       </c>
       <c r="T30" s="6" t="n">
         <v>2.32</v>
       </c>
       <c r="U30" s="21" t="n">
-        <v>2.31</v>
+        <v>2.32</v>
       </c>
     </row>
     <row r="31">
@@ -3036,7 +3036,7 @@
           <t>ADXDNO</t>
         </is>
       </c>
-      <c r="C31" s="50" t="n">
+      <c r="C31" s="48" t="n">
         <v>45962</v>
       </c>
       <c r="D31" s="6" t="inlineStr">
@@ -3050,10 +3050,10 @@
         </is>
       </c>
       <c r="F31" s="25" t="n">
-        <v>0.1256397039873348</v>
+        <v>0.1254482530098303</v>
       </c>
       <c r="G31" s="25" t="n">
-        <v>0.04954381497984299</v>
+        <v>0.05011084527755218</v>
       </c>
       <c r="H31" s="25" t="n">
         <v>0.06502168244015354</v>
@@ -4141,8 +4141,8 @@
           <t>BOPTEXP</t>
         </is>
       </c>
-      <c r="C46" s="48" t="n">
-        <v>45931</v>
+      <c r="C46" s="50" t="n">
+        <v>45962</v>
       </c>
       <c r="D46" s="6" t="inlineStr">
         <is>
@@ -4155,19 +4155,19 @@
         </is>
       </c>
       <c r="F46" s="24" t="n">
-        <v>302015</v>
+        <v>292052</v>
       </c>
       <c r="G46" s="24" t="n">
+        <v>302919</v>
+      </c>
+      <c r="H46" s="24" t="n">
         <v>294225</v>
       </c>
-      <c r="H46" s="24" t="n">
+      <c r="I46" s="24" t="n">
         <v>284060</v>
       </c>
-      <c r="I46" s="24" t="n">
+      <c r="J46" s="24" t="n">
         <v>283923</v>
-      </c>
-      <c r="J46" s="24" t="n">
-        <v>280519</v>
       </c>
       <c r="K46" s="5" t="n"/>
       <c r="L46" s="29" t="inlineStr">
@@ -4228,8 +4228,8 @@
           <t>BOPTEXP</t>
         </is>
       </c>
-      <c r="C47" s="48" t="n">
-        <v>45931</v>
+      <c r="C47" s="50" t="n">
+        <v>45962</v>
       </c>
       <c r="D47" s="6" t="inlineStr">
         <is>
@@ -4242,19 +4242,19 @@
         </is>
       </c>
       <c r="F47" s="38" t="n">
-        <v>0.02647633613730993</v>
+        <v>-0.0358742766218032</v>
       </c>
       <c r="G47" s="38" t="n">
+        <v>0.02954881468264081</v>
+      </c>
+      <c r="H47" s="38" t="n">
         <v>0.03578469337463908</v>
       </c>
-      <c r="H47" s="38" t="n">
+      <c r="I47" s="38" t="n">
         <v>0.0004825251916893425</v>
       </c>
-      <c r="I47" s="38" t="n">
+      <c r="J47" s="38" t="n">
         <v>0.01213465041583639</v>
-      </c>
-      <c r="J47" s="38" t="n">
-        <v>0.0004065548046574552</v>
       </c>
       <c r="K47" s="5" t="n"/>
       <c r="L47" s="28" t="inlineStr">
@@ -4268,7 +4268,7 @@
         </is>
       </c>
       <c r="N47" s="50" t="n">
-        <v>46049</v>
+        <v>46050</v>
       </c>
       <c r="O47" s="6" t="inlineStr">
         <is>
@@ -4307,8 +4307,8 @@
           <t>BOPTIMP</t>
         </is>
       </c>
-      <c r="C48" s="48" t="n">
-        <v>45931</v>
+      <c r="C48" s="50" t="n">
+        <v>45962</v>
       </c>
       <c r="D48" s="6" t="inlineStr">
         <is>
@@ -4321,19 +4321,19 @@
         </is>
       </c>
       <c r="F48" s="24" t="n">
-        <v>331366</v>
+        <v>348877</v>
       </c>
       <c r="G48" s="24" t="n">
+        <v>332124</v>
+      </c>
+      <c r="H48" s="24" t="n">
         <v>342363</v>
       </c>
-      <c r="H48" s="24" t="n">
+      <c r="I48" s="24" t="n">
         <v>339690</v>
       </c>
-      <c r="I48" s="24" t="n">
+      <c r="J48" s="24" t="n">
         <v>358321</v>
-      </c>
-      <c r="J48" s="24" t="n">
-        <v>338704</v>
       </c>
       <c r="K48" s="5" t="n"/>
       <c r="L48" s="28" t="inlineStr">
@@ -4347,7 +4347,7 @@
         </is>
       </c>
       <c r="N48" s="50" t="n">
-        <v>46049</v>
+        <v>46050</v>
       </c>
       <c r="O48" s="6" t="inlineStr">
         <is>
@@ -4360,19 +4360,19 @@
         </is>
       </c>
       <c r="Q48" s="6" t="n">
+        <v>3.56</v>
+      </c>
+      <c r="R48" s="6" t="n">
         <v>3.53</v>
       </c>
-      <c r="R48" s="6" t="n">
+      <c r="S48" s="6" t="n">
         <v>3.56</v>
       </c>
-      <c r="S48" s="6" t="n">
+      <c r="T48" s="6" t="n">
         <v>3.6</v>
       </c>
-      <c r="T48" s="6" t="n">
+      <c r="U48" s="21" t="n">
         <v>3.61</v>
-      </c>
-      <c r="U48" s="21" t="n">
-        <v>3.6</v>
       </c>
     </row>
     <row r="49">
@@ -4382,8 +4382,8 @@
           <t>BOPTIMP</t>
         </is>
       </c>
-      <c r="C49" s="48" t="n">
-        <v>45931</v>
+      <c r="C49" s="50" t="n">
+        <v>45962</v>
       </c>
       <c r="D49" s="6" t="inlineStr">
         <is>
@@ -4396,19 +4396,19 @@
         </is>
       </c>
       <c r="F49" s="38" t="n">
-        <v>-0.03212087754809956</v>
+        <v>0.05044200358902096</v>
       </c>
       <c r="G49" s="38" t="n">
+        <v>-0.02990685325224984</v>
+      </c>
+      <c r="H49" s="38" t="n">
         <v>0.007868939327033475</v>
       </c>
-      <c r="H49" s="38" t="n">
+      <c r="I49" s="38" t="n">
         <v>-0.05199527797700942</v>
       </c>
-      <c r="I49" s="38" t="n">
+      <c r="J49" s="38" t="n">
         <v>0.05791782795597333</v>
-      </c>
-      <c r="J49" s="38" t="n">
-        <v>-0.03628608905214581</v>
       </c>
       <c r="K49" s="5" t="n"/>
       <c r="L49" s="28" t="inlineStr">
@@ -4422,7 +4422,7 @@
         </is>
       </c>
       <c r="N49" s="50" t="n">
-        <v>46049</v>
+        <v>46050</v>
       </c>
       <c r="O49" s="6" t="inlineStr">
         <is>
@@ -4435,19 +4435,19 @@
         </is>
       </c>
       <c r="Q49" s="6" t="n">
+        <v>3.83</v>
+      </c>
+      <c r="R49" s="6" t="n">
         <v>3.81</v>
       </c>
-      <c r="R49" s="6" t="n">
+      <c r="S49" s="6" t="n">
         <v>3.82</v>
       </c>
-      <c r="S49" s="6" t="n">
+      <c r="T49" s="6" t="n">
         <v>3.84</v>
       </c>
-      <c r="T49" s="6" t="n">
+      <c r="U49" s="21" t="n">
         <v>3.85</v>
-      </c>
-      <c r="U49" s="21" t="n">
-        <v>3.83</v>
       </c>
     </row>
     <row r="50">
@@ -4461,8 +4461,8 @@
           <t>BOPSTB</t>
         </is>
       </c>
-      <c r="C50" s="48" t="n">
-        <v>45931</v>
+      <c r="C50" s="50" t="n">
+        <v>45962</v>
       </c>
       <c r="D50" s="6" t="inlineStr">
         <is>
@@ -4475,19 +4475,19 @@
         </is>
       </c>
       <c r="F50" s="24" t="n">
-        <v>29796</v>
+        <v>30075</v>
       </c>
       <c r="G50" s="24" t="n">
+        <v>29777</v>
+      </c>
+      <c r="H50" s="24" t="n">
         <v>30169</v>
       </c>
-      <c r="H50" s="24" t="n">
+      <c r="I50" s="24" t="n">
         <v>30416</v>
       </c>
-      <c r="I50" s="24" t="n">
+      <c r="J50" s="24" t="n">
         <v>28606</v>
-      </c>
-      <c r="J50" s="24" t="n">
-        <v>27839</v>
       </c>
       <c r="K50" s="5" t="n"/>
       <c r="L50" s="28" t="inlineStr">
@@ -4501,7 +4501,7 @@
         </is>
       </c>
       <c r="N50" s="50" t="n">
-        <v>46049</v>
+        <v>46050</v>
       </c>
       <c r="O50" s="6" t="inlineStr">
         <is>
@@ -4514,16 +4514,16 @@
         </is>
       </c>
       <c r="Q50" s="6" t="n">
+        <v>4.26</v>
+      </c>
+      <c r="R50" s="6" t="n">
         <v>4.24</v>
       </c>
-      <c r="R50" s="6" t="n">
+      <c r="S50" s="6" t="n">
         <v>4.22</v>
       </c>
-      <c r="S50" s="6" t="n">
+      <c r="T50" s="6" t="n">
         <v>4.24</v>
-      </c>
-      <c r="T50" s="6" t="n">
-        <v>4.26</v>
       </c>
       <c r="U50" s="21" t="n">
         <v>4.26</v>
@@ -4536,8 +4536,8 @@
           <t>BOPSTB</t>
         </is>
       </c>
-      <c r="C51" s="48" t="n">
-        <v>45931</v>
+      <c r="C51" s="50" t="n">
+        <v>45962</v>
       </c>
       <c r="D51" s="6" t="inlineStr">
         <is>
@@ -4550,19 +4550,19 @@
         </is>
       </c>
       <c r="F51" s="38" t="n">
-        <v>-0.01236368457688353</v>
+        <v>0.01000772408234551</v>
       </c>
       <c r="G51" s="38" t="n">
+        <v>-0.01299347011833341</v>
+      </c>
+      <c r="H51" s="38" t="n">
         <v>-0.008120725933719042</v>
       </c>
-      <c r="H51" s="38" t="n">
+      <c r="I51" s="38" t="n">
         <v>0.06327343913864225</v>
       </c>
-      <c r="I51" s="38" t="n">
+      <c r="J51" s="38" t="n">
         <v>0.02755127698552395</v>
-      </c>
-      <c r="J51" s="38" t="n">
-        <v>0.05614780530369123</v>
       </c>
       <c r="K51" s="5" t="n"/>
       <c r="L51" s="28" t="inlineStr">
@@ -4575,8 +4575,8 @@
           <t>MORTGAGE30US</t>
         </is>
       </c>
-      <c r="N51" s="48" t="n">
-        <v>46041</v>
+      <c r="N51" s="50" t="n">
+        <v>46048</v>
       </c>
       <c r="O51" s="6" t="inlineStr">
         <is>
@@ -4589,19 +4589,19 @@
         </is>
       </c>
       <c r="Q51" s="6" t="n">
+        <v>6.1</v>
+      </c>
+      <c r="R51" s="6" t="n">
         <v>6.09</v>
       </c>
-      <c r="R51" s="6" t="n">
+      <c r="S51" s="6" t="n">
         <v>6.06</v>
       </c>
-      <c r="S51" s="6" t="n">
+      <c r="T51" s="6" t="n">
         <v>6.16</v>
       </c>
-      <c r="T51" s="6" t="n">
+      <c r="U51" s="21" t="n">
         <v>6.15</v>
-      </c>
-      <c r="U51" s="21" t="n">
-        <v>6.18</v>
       </c>
     </row>
     <row r="52" ht="16.15" customHeight="1" thickBot="1">
@@ -4627,7 +4627,7 @@
         </is>
       </c>
       <c r="N52" s="53" t="n">
-        <v>46049</v>
+        <v>46050</v>
       </c>
       <c r="O52" s="9" t="inlineStr">
         <is>
@@ -4640,19 +4640,19 @@
         </is>
       </c>
       <c r="Q52" s="9" t="n">
+        <v>5.88</v>
+      </c>
+      <c r="R52" s="9" t="n">
         <v>5.85</v>
       </c>
-      <c r="R52" s="9" t="n">
+      <c r="S52" s="9" t="n">
         <v>5.83</v>
-      </c>
-      <c r="S52" s="9" t="n">
-        <v>5.85</v>
       </c>
       <c r="T52" s="9" t="n">
         <v>5.85</v>
       </c>
       <c r="U52" s="22" t="n">
-        <v>5.88</v>
+        <v>5.85</v>
       </c>
     </row>
     <row r="53" ht="21" customHeight="1">

</xml_diff>

<commit_message>
Update dashboards - 2026-01-31
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -2389,8 +2389,8 @@
           <t>PPIFIS</t>
         </is>
       </c>
-      <c r="N22" s="48" t="n">
-        <v>45962</v>
+      <c r="N22" s="50" t="n">
+        <v>45992</v>
       </c>
       <c r="O22" s="6" t="inlineStr">
         <is>
@@ -2403,19 +2403,19 @@
         </is>
       </c>
       <c r="Q22" s="38" t="n">
-        <v>0.002481174999334979</v>
+        <v>0.004902708763177221</v>
       </c>
       <c r="R22" s="38" t="n">
-        <v>0.001165446832315453</v>
+        <v>0.002380714879468115</v>
       </c>
       <c r="S22" s="38" t="n">
-        <v>0.005928774318023633</v>
+        <v>0.0008919003467759978</v>
       </c>
       <c r="T22" s="38" t="n">
-        <v>-0.001765461159854542</v>
+        <v>0.006579167755378368</v>
       </c>
       <c r="U22" s="23" t="n">
-        <v>0.007967429257047298</v>
+        <v>-0.001852396747271667</v>
       </c>
     </row>
     <row r="23">
@@ -2459,8 +2459,8 @@
           <t>PPIFIS</t>
         </is>
       </c>
-      <c r="N23" s="48" t="n">
-        <v>45962</v>
+      <c r="N23" s="50" t="n">
+        <v>45992</v>
       </c>
       <c r="O23" s="6" t="inlineStr">
         <is>
@@ -2473,19 +2473,19 @@
         </is>
       </c>
       <c r="Q23" s="38" t="n">
-        <v>0.02946902473512731</v>
+        <v>0.02953930644481603</v>
       </c>
       <c r="R23" s="38" t="n">
-        <v>0.02796734180331234</v>
+        <v>0.02966029332404323</v>
       </c>
       <c r="S23" s="38" t="n">
-        <v>0.02993991439859532</v>
+        <v>0.02826137498119562</v>
       </c>
       <c r="T23" s="38" t="n">
-        <v>0.02691249312052819</v>
+        <v>0.03051607769973669</v>
       </c>
       <c r="U23" s="23" t="n">
-        <v>0.03221531176442166</v>
+        <v>0.02682305998899265</v>
       </c>
     </row>
     <row r="24">
@@ -2922,7 +2922,7 @@
         </is>
       </c>
       <c r="N29" s="50" t="n">
-        <v>46051</v>
+        <v>46052</v>
       </c>
       <c r="O29" s="6" t="inlineStr">
         <is>
@@ -2935,19 +2935,19 @@
         </is>
       </c>
       <c r="Q29" s="6" t="n">
+        <v>2.19</v>
+      </c>
+      <c r="R29" s="6" t="n">
         <v>2.18</v>
       </c>
-      <c r="R29" s="6" t="n">
+      <c r="S29" s="6" t="n">
         <v>2.22</v>
       </c>
-      <c r="S29" s="6" t="n">
+      <c r="T29" s="6" t="n">
         <v>2.21</v>
       </c>
-      <c r="T29" s="6" t="n">
+      <c r="U29" s="21" t="n">
         <v>2.19</v>
-      </c>
-      <c r="U29" s="21" t="n">
-        <v>2.18</v>
       </c>
     </row>
     <row r="30">
@@ -3001,7 +3001,7 @@
         </is>
       </c>
       <c r="N30" s="50" t="n">
-        <v>46051</v>
+        <v>46052</v>
       </c>
       <c r="O30" s="6" t="inlineStr">
         <is>
@@ -3014,16 +3014,16 @@
         </is>
       </c>
       <c r="Q30" s="6" t="n">
+        <v>2.36</v>
+      </c>
+      <c r="R30" s="6" t="n">
         <v>2.35</v>
       </c>
-      <c r="R30" s="6" t="n">
+      <c r="S30" s="6" t="n">
         <v>2.36</v>
       </c>
-      <c r="S30" s="6" t="n">
+      <c r="T30" s="6" t="n">
         <v>2.34</v>
-      </c>
-      <c r="T30" s="6" t="n">
-        <v>2.32</v>
       </c>
       <c r="U30" s="21" t="n">
         <v>2.32</v>
@@ -4268,7 +4268,7 @@
         </is>
       </c>
       <c r="N47" s="50" t="n">
-        <v>46050</v>
+        <v>46051</v>
       </c>
       <c r="O47" s="6" t="inlineStr">
         <is>
@@ -4347,7 +4347,7 @@
         </is>
       </c>
       <c r="N48" s="50" t="n">
-        <v>46050</v>
+        <v>46051</v>
       </c>
       <c r="O48" s="6" t="inlineStr">
         <is>
@@ -4360,19 +4360,19 @@
         </is>
       </c>
       <c r="Q48" s="6" t="n">
+        <v>3.53</v>
+      </c>
+      <c r="R48" s="6" t="n">
         <v>3.56</v>
       </c>
-      <c r="R48" s="6" t="n">
+      <c r="S48" s="6" t="n">
         <v>3.53</v>
       </c>
-      <c r="S48" s="6" t="n">
+      <c r="T48" s="6" t="n">
         <v>3.56</v>
       </c>
-      <c r="T48" s="6" t="n">
+      <c r="U48" s="21" t="n">
         <v>3.6</v>
-      </c>
-      <c r="U48" s="21" t="n">
-        <v>3.61</v>
       </c>
     </row>
     <row r="49">
@@ -4422,7 +4422,7 @@
         </is>
       </c>
       <c r="N49" s="50" t="n">
-        <v>46050</v>
+        <v>46051</v>
       </c>
       <c r="O49" s="6" t="inlineStr">
         <is>
@@ -4435,19 +4435,19 @@
         </is>
       </c>
       <c r="Q49" s="6" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="R49" s="6" t="n">
         <v>3.83</v>
       </c>
-      <c r="R49" s="6" t="n">
+      <c r="S49" s="6" t="n">
         <v>3.81</v>
       </c>
-      <c r="S49" s="6" t="n">
+      <c r="T49" s="6" t="n">
         <v>3.82</v>
       </c>
-      <c r="T49" s="6" t="n">
+      <c r="U49" s="21" t="n">
         <v>3.84</v>
-      </c>
-      <c r="U49" s="21" t="n">
-        <v>3.85</v>
       </c>
     </row>
     <row r="50">
@@ -4501,7 +4501,7 @@
         </is>
       </c>
       <c r="N50" s="50" t="n">
-        <v>46050</v>
+        <v>46051</v>
       </c>
       <c r="O50" s="6" t="inlineStr">
         <is>
@@ -4514,19 +4514,19 @@
         </is>
       </c>
       <c r="Q50" s="6" t="n">
+        <v>4.24</v>
+      </c>
+      <c r="R50" s="6" t="n">
         <v>4.26</v>
       </c>
-      <c r="R50" s="6" t="n">
+      <c r="S50" s="6" t="n">
         <v>4.24</v>
       </c>
-      <c r="S50" s="6" t="n">
+      <c r="T50" s="6" t="n">
         <v>4.22</v>
       </c>
-      <c r="T50" s="6" t="n">
+      <c r="U50" s="21" t="n">
         <v>4.24</v>
-      </c>
-      <c r="U50" s="21" t="n">
-        <v>4.26</v>
       </c>
     </row>
     <row r="51" ht="31.5" customHeight="1">
@@ -4627,7 +4627,7 @@
         </is>
       </c>
       <c r="N52" s="53" t="n">
-        <v>46050</v>
+        <v>46051</v>
       </c>
       <c r="O52" s="9" t="inlineStr">
         <is>
@@ -4640,16 +4640,16 @@
         </is>
       </c>
       <c r="Q52" s="9" t="n">
+        <v>5.87</v>
+      </c>
+      <c r="R52" s="9" t="n">
         <v>5.88</v>
       </c>
-      <c r="R52" s="9" t="n">
+      <c r="S52" s="9" t="n">
         <v>5.85</v>
       </c>
-      <c r="S52" s="9" t="n">
+      <c r="T52" s="9" t="n">
         <v>5.83</v>
-      </c>
-      <c r="T52" s="9" t="n">
-        <v>5.85</v>
       </c>
       <c r="U52" s="22" t="n">
         <v>5.85</v>

</xml_diff>

<commit_message>
Update dashboards - 2026-02-02
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -1292,8 +1292,8 @@
           <t>RECPROUSM156N</t>
         </is>
       </c>
-      <c r="C8" s="48" t="n">
-        <v>45962</v>
+      <c r="C8" s="50" t="n">
+        <v>45992</v>
       </c>
       <c r="D8" s="6" t="inlineStr">
         <is>
@@ -1306,19 +1306,19 @@
         </is>
       </c>
       <c r="F8" s="24" t="n">
-        <v>0.9399999999999999</v>
+        <v>0.8</v>
       </c>
       <c r="G8" s="24" t="n">
-        <v>0.9</v>
+        <v>0.62</v>
       </c>
       <c r="H8" s="24" t="n">
-        <v>0.72</v>
+        <v>0.86</v>
       </c>
       <c r="I8" s="24" t="n">
-        <v>0.7</v>
+        <v>0.82</v>
       </c>
       <c r="J8" s="24" t="n">
-        <v>0.32</v>
+        <v>0.88</v>
       </c>
       <c r="K8" s="5" t="n"/>
       <c r="L8" s="28" t="inlineStr">

</xml_diff>

<commit_message>
Update dashboards - 2026-02-03
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -62,7 +62,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill/>
     </fill>
@@ -73,12 +73,6 @@
       <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00CCFFCC"/>
-        <bgColor rgb="00CCFFCC"/>
       </patternFill>
     </fill>
     <fill>
@@ -223,7 +217,7 @@
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -363,19 +357,10 @@
     <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="3" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="1" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="168" fontId="1" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="1" fillId="4" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="168" fontId="1" fillId="3" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1123,7 +1108,7 @@
       <c r="T5" s="24" t="n">
         <v>-29000</v>
       </c>
-      <c r="U5" s="49" t="n">
+      <c r="U5" s="26" t="n">
         <v>-3000</v>
       </c>
     </row>
@@ -1292,7 +1277,7 @@
           <t>RECPROUSM156N</t>
         </is>
       </c>
-      <c r="C8" s="50" t="n">
+      <c r="C8" s="49" t="n">
         <v>45992</v>
       </c>
       <c r="D8" s="6" t="inlineStr">
@@ -1718,7 +1703,7 @@
           <t>ICSA</t>
         </is>
       </c>
-      <c r="N13" s="50" t="n">
+      <c r="N13" s="49" t="n">
         <v>46041</v>
       </c>
       <c r="O13" s="6" t="inlineStr">
@@ -1793,7 +1778,7 @@
           <t>CCSA</t>
         </is>
       </c>
-      <c r="N14" s="50" t="n">
+      <c r="N14" s="49" t="n">
         <v>46034</v>
       </c>
       <c r="O14" s="6" t="inlineStr">
@@ -2389,7 +2374,7 @@
           <t>PPIFIS</t>
         </is>
       </c>
-      <c r="N22" s="50" t="n">
+      <c r="N22" s="49" t="n">
         <v>45992</v>
       </c>
       <c r="O22" s="6" t="inlineStr">
@@ -2459,7 +2444,7 @@
           <t>PPIFIS</t>
         </is>
       </c>
-      <c r="N23" s="50" t="n">
+      <c r="N23" s="49" t="n">
         <v>45992</v>
       </c>
       <c r="O23" s="6" t="inlineStr">
@@ -2921,8 +2906,8 @@
           <t>T5YIFR</t>
         </is>
       </c>
-      <c r="N29" s="50" t="n">
-        <v>46052</v>
+      <c r="N29" s="49" t="n">
+        <v>46055</v>
       </c>
       <c r="O29" s="6" t="inlineStr">
         <is>
@@ -2935,19 +2920,19 @@
         </is>
       </c>
       <c r="Q29" s="6" t="n">
+        <v>2.18</v>
+      </c>
+      <c r="R29" s="6" t="n">
         <v>2.19</v>
       </c>
-      <c r="R29" s="6" t="n">
+      <c r="S29" s="6" t="n">
         <v>2.18</v>
       </c>
-      <c r="S29" s="6" t="n">
+      <c r="T29" s="6" t="n">
         <v>2.22</v>
       </c>
-      <c r="T29" s="6" t="n">
+      <c r="U29" s="21" t="n">
         <v>2.21</v>
-      </c>
-      <c r="U29" s="21" t="n">
-        <v>2.19</v>
       </c>
     </row>
     <row r="30">
@@ -3000,8 +2985,8 @@
           <t>T10YIE</t>
         </is>
       </c>
-      <c r="N30" s="50" t="n">
-        <v>46052</v>
+      <c r="N30" s="49" t="n">
+        <v>46055</v>
       </c>
       <c r="O30" s="6" t="inlineStr">
         <is>
@@ -3014,19 +2999,19 @@
         </is>
       </c>
       <c r="Q30" s="6" t="n">
+        <v>2.35</v>
+      </c>
+      <c r="R30" s="6" t="n">
         <v>2.36</v>
       </c>
-      <c r="R30" s="6" t="n">
+      <c r="S30" s="6" t="n">
         <v>2.35</v>
       </c>
-      <c r="S30" s="6" t="n">
+      <c r="T30" s="6" t="n">
         <v>2.36</v>
       </c>
-      <c r="T30" s="6" t="n">
+      <c r="U30" s="21" t="n">
         <v>2.34</v>
-      </c>
-      <c r="U30" s="21" t="n">
-        <v>2.32</v>
       </c>
     </row>
     <row r="31">
@@ -3529,7 +3514,7 @@
           <t>CSUSHPINSA</t>
         </is>
       </c>
-      <c r="N37" s="50" t="n">
+      <c r="N37" s="48" t="n">
         <v>45962</v>
       </c>
       <c r="O37" s="6" t="inlineStr">
@@ -3604,7 +3589,7 @@
           <t>CSUSHPINSA</t>
         </is>
       </c>
-      <c r="N38" s="50" t="n">
+      <c r="N38" s="48" t="n">
         <v>45962</v>
       </c>
       <c r="O38" s="6" t="inlineStr">
@@ -3679,8 +3664,8 @@
           <t>TWEXBGSMTH</t>
         </is>
       </c>
-      <c r="N39" s="48" t="n">
-        <v>45992</v>
+      <c r="N39" s="49" t="n">
+        <v>46023</v>
       </c>
       <c r="O39" s="6" t="inlineStr">
         <is>
@@ -3693,19 +3678,19 @@
         </is>
       </c>
       <c r="Q39" s="6" t="n">
-        <v>120.5723</v>
-      </c>
-      <c r="R39" s="51" t="n">
-        <v>121.8038</v>
+        <v>119.2298</v>
+      </c>
+      <c r="R39" s="6" t="n">
+        <v>120.1883</v>
       </c>
       <c r="S39" s="6" t="n">
-        <v>121.1712</v>
+        <v>121.4177</v>
       </c>
       <c r="T39" s="6" t="n">
-        <v>120.4534</v>
+        <v>120.7618</v>
       </c>
       <c r="U39" s="21" t="n">
-        <v>120.9844</v>
+        <v>120.0291</v>
       </c>
     </row>
     <row r="40" ht="31.5" customHeight="1">
@@ -3754,8 +3739,8 @@
           <t>TWEXBGSMTH</t>
         </is>
       </c>
-      <c r="N40" s="48" t="n">
-        <v>45992</v>
+      <c r="N40" s="49" t="n">
+        <v>46023</v>
       </c>
       <c r="O40" s="6" t="inlineStr">
         <is>
@@ -3768,19 +3753,19 @@
         </is>
       </c>
       <c r="Q40" s="38" t="n">
-        <v>-0.05665811256982799</v>
-      </c>
-      <c r="R40" s="52" t="n">
-        <v>-0.03737446940677091</v>
+        <v>-0.07456792269916472</v>
+      </c>
+      <c r="R40" s="38" t="n">
+        <v>-0.05790675033979801</v>
       </c>
       <c r="S40" s="38" t="n">
-        <v>-0.02147927417205711</v>
+        <v>-0.03874237696864814</v>
       </c>
       <c r="T40" s="38" t="n">
-        <v>-0.0137247645124523</v>
+        <v>-0.02292562904900106</v>
       </c>
       <c r="U40" s="23" t="n">
-        <v>-0.0154280347850997</v>
+        <v>-0.0152258401163721</v>
       </c>
     </row>
     <row r="41">
@@ -4141,7 +4126,7 @@
           <t>BOPTEXP</t>
         </is>
       </c>
-      <c r="C46" s="50" t="n">
+      <c r="C46" s="49" t="n">
         <v>45962</v>
       </c>
       <c r="D46" s="6" t="inlineStr">
@@ -4228,7 +4213,7 @@
           <t>BOPTEXP</t>
         </is>
       </c>
-      <c r="C47" s="50" t="n">
+      <c r="C47" s="49" t="n">
         <v>45962</v>
       </c>
       <c r="D47" s="6" t="inlineStr">
@@ -4267,8 +4252,8 @@
           <t>DFF</t>
         </is>
       </c>
-      <c r="N47" s="50" t="n">
-        <v>46051</v>
+      <c r="N47" s="49" t="n">
+        <v>46052</v>
       </c>
       <c r="O47" s="6" t="inlineStr">
         <is>
@@ -4307,7 +4292,7 @@
           <t>BOPTIMP</t>
         </is>
       </c>
-      <c r="C48" s="50" t="n">
+      <c r="C48" s="49" t="n">
         <v>45962</v>
       </c>
       <c r="D48" s="6" t="inlineStr">
@@ -4346,8 +4331,8 @@
           <t>DGS2</t>
         </is>
       </c>
-      <c r="N48" s="50" t="n">
-        <v>46051</v>
+      <c r="N48" s="49" t="n">
+        <v>46052</v>
       </c>
       <c r="O48" s="6" t="inlineStr">
         <is>
@@ -4360,19 +4345,19 @@
         </is>
       </c>
       <c r="Q48" s="6" t="n">
+        <v>3.52</v>
+      </c>
+      <c r="R48" s="6" t="n">
         <v>3.53</v>
       </c>
-      <c r="R48" s="6" t="n">
+      <c r="S48" s="6" t="n">
         <v>3.56</v>
       </c>
-      <c r="S48" s="6" t="n">
+      <c r="T48" s="6" t="n">
         <v>3.53</v>
       </c>
-      <c r="T48" s="6" t="n">
+      <c r="U48" s="21" t="n">
         <v>3.56</v>
-      </c>
-      <c r="U48" s="21" t="n">
-        <v>3.6</v>
       </c>
     </row>
     <row r="49">
@@ -4382,7 +4367,7 @@
           <t>BOPTIMP</t>
         </is>
       </c>
-      <c r="C49" s="50" t="n">
+      <c r="C49" s="49" t="n">
         <v>45962</v>
       </c>
       <c r="D49" s="6" t="inlineStr">
@@ -4421,8 +4406,8 @@
           <t>DGS5</t>
         </is>
       </c>
-      <c r="N49" s="50" t="n">
-        <v>46051</v>
+      <c r="N49" s="49" t="n">
+        <v>46052</v>
       </c>
       <c r="O49" s="6" t="inlineStr">
         <is>
@@ -4435,19 +4420,19 @@
         </is>
       </c>
       <c r="Q49" s="6" t="n">
+        <v>3.79</v>
+      </c>
+      <c r="R49" s="6" t="n">
         <v>3.8</v>
       </c>
-      <c r="R49" s="6" t="n">
+      <c r="S49" s="6" t="n">
         <v>3.83</v>
       </c>
-      <c r="S49" s="6" t="n">
+      <c r="T49" s="6" t="n">
         <v>3.81</v>
       </c>
-      <c r="T49" s="6" t="n">
+      <c r="U49" s="21" t="n">
         <v>3.82</v>
-      </c>
-      <c r="U49" s="21" t="n">
-        <v>3.84</v>
       </c>
     </row>
     <row r="50">
@@ -4461,7 +4446,7 @@
           <t>BOPSTB</t>
         </is>
       </c>
-      <c r="C50" s="50" t="n">
+      <c r="C50" s="49" t="n">
         <v>45962</v>
       </c>
       <c r="D50" s="6" t="inlineStr">
@@ -4500,8 +4485,8 @@
           <t>DGS10</t>
         </is>
       </c>
-      <c r="N50" s="50" t="n">
-        <v>46051</v>
+      <c r="N50" s="49" t="n">
+        <v>46052</v>
       </c>
       <c r="O50" s="6" t="inlineStr">
         <is>
@@ -4514,19 +4499,19 @@
         </is>
       </c>
       <c r="Q50" s="6" t="n">
+        <v>4.26</v>
+      </c>
+      <c r="R50" s="6" t="n">
         <v>4.24</v>
       </c>
-      <c r="R50" s="6" t="n">
+      <c r="S50" s="6" t="n">
         <v>4.26</v>
       </c>
-      <c r="S50" s="6" t="n">
+      <c r="T50" s="6" t="n">
         <v>4.24</v>
       </c>
-      <c r="T50" s="6" t="n">
+      <c r="U50" s="21" t="n">
         <v>4.22</v>
-      </c>
-      <c r="U50" s="21" t="n">
-        <v>4.24</v>
       </c>
     </row>
     <row r="51" ht="31.5" customHeight="1">
@@ -4536,7 +4521,7 @@
           <t>BOPSTB</t>
         </is>
       </c>
-      <c r="C51" s="50" t="n">
+      <c r="C51" s="49" t="n">
         <v>45962</v>
       </c>
       <c r="D51" s="6" t="inlineStr">
@@ -4575,7 +4560,7 @@
           <t>MORTGAGE30US</t>
         </is>
       </c>
-      <c r="N51" s="50" t="n">
+      <c r="N51" s="49" t="n">
         <v>46048</v>
       </c>
       <c r="O51" s="6" t="inlineStr">
@@ -4626,8 +4611,8 @@
           <t>DBAA</t>
         </is>
       </c>
-      <c r="N52" s="53" t="n">
-        <v>46051</v>
+      <c r="N52" s="50" t="n">
+        <v>46052</v>
       </c>
       <c r="O52" s="9" t="inlineStr">
         <is>
@@ -4640,19 +4625,19 @@
         </is>
       </c>
       <c r="Q52" s="9" t="n">
+        <v>5.88</v>
+      </c>
+      <c r="R52" s="9" t="n">
         <v>5.87</v>
       </c>
-      <c r="R52" s="9" t="n">
+      <c r="S52" s="9" t="n">
         <v>5.88</v>
       </c>
-      <c r="S52" s="9" t="n">
+      <c r="T52" s="9" t="n">
         <v>5.85</v>
       </c>
-      <c r="T52" s="9" t="n">
+      <c r="U52" s="22" t="n">
         <v>5.83</v>
-      </c>
-      <c r="U52" s="22" t="n">
-        <v>5.85</v>
       </c>
     </row>
     <row r="53" ht="21" customHeight="1">

</xml_diff>

<commit_message>
Update dashboards - 2026-02-04
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -1083,8 +1083,8 @@
           <t>ADPMNUSNERSA</t>
         </is>
       </c>
-      <c r="N5" s="48" t="n">
-        <v>45992</v>
+      <c r="N5" s="49" t="n">
+        <v>46023</v>
       </c>
       <c r="O5" s="6" t="inlineStr">
         <is>
@@ -1097,19 +1097,19 @@
         </is>
       </c>
       <c r="Q5" s="24" t="n">
-        <v>41000</v>
+        <v>22000</v>
       </c>
       <c r="R5" s="24" t="n">
-        <v>-29000</v>
+        <v>37000</v>
       </c>
       <c r="S5" s="24" t="n">
-        <v>47000</v>
+        <v>74000</v>
       </c>
       <c r="T5" s="24" t="n">
-        <v>-29000</v>
+        <v>20000</v>
       </c>
       <c r="U5" s="26" t="n">
-        <v>-3000</v>
+        <v>88000</v>
       </c>
     </row>
     <row r="6">
@@ -2907,7 +2907,7 @@
         </is>
       </c>
       <c r="N29" s="49" t="n">
-        <v>46055</v>
+        <v>46056</v>
       </c>
       <c r="O29" s="6" t="inlineStr">
         <is>
@@ -2920,19 +2920,19 @@
         </is>
       </c>
       <c r="Q29" s="6" t="n">
+        <v>2.19</v>
+      </c>
+      <c r="R29" s="6" t="n">
         <v>2.18</v>
       </c>
-      <c r="R29" s="6" t="n">
+      <c r="S29" s="6" t="n">
         <v>2.19</v>
       </c>
-      <c r="S29" s="6" t="n">
+      <c r="T29" s="6" t="n">
         <v>2.18</v>
       </c>
-      <c r="T29" s="6" t="n">
+      <c r="U29" s="21" t="n">
         <v>2.22</v>
-      </c>
-      <c r="U29" s="21" t="n">
-        <v>2.21</v>
       </c>
     </row>
     <row r="30">
@@ -2986,7 +2986,7 @@
         </is>
       </c>
       <c r="N30" s="49" t="n">
-        <v>46055</v>
+        <v>46056</v>
       </c>
       <c r="O30" s="6" t="inlineStr">
         <is>
@@ -2999,19 +2999,19 @@
         </is>
       </c>
       <c r="Q30" s="6" t="n">
+        <v>2.36</v>
+      </c>
+      <c r="R30" s="6" t="n">
         <v>2.35</v>
       </c>
-      <c r="R30" s="6" t="n">
+      <c r="S30" s="6" t="n">
         <v>2.36</v>
       </c>
-      <c r="S30" s="6" t="n">
+      <c r="T30" s="6" t="n">
         <v>2.35</v>
       </c>
-      <c r="T30" s="6" t="n">
+      <c r="U30" s="21" t="n">
         <v>2.36</v>
-      </c>
-      <c r="U30" s="21" t="n">
-        <v>2.34</v>
       </c>
     </row>
     <row r="31">
@@ -4253,7 +4253,7 @@
         </is>
       </c>
       <c r="N47" s="49" t="n">
-        <v>46052</v>
+        <v>46055</v>
       </c>
       <c r="O47" s="6" t="inlineStr">
         <is>
@@ -4332,7 +4332,7 @@
         </is>
       </c>
       <c r="N48" s="49" t="n">
-        <v>46052</v>
+        <v>46055</v>
       </c>
       <c r="O48" s="6" t="inlineStr">
         <is>
@@ -4345,19 +4345,19 @@
         </is>
       </c>
       <c r="Q48" s="6" t="n">
+        <v>3.57</v>
+      </c>
+      <c r="R48" s="6" t="n">
         <v>3.52</v>
       </c>
-      <c r="R48" s="6" t="n">
+      <c r="S48" s="6" t="n">
         <v>3.53</v>
       </c>
-      <c r="S48" s="6" t="n">
+      <c r="T48" s="6" t="n">
         <v>3.56</v>
       </c>
-      <c r="T48" s="6" t="n">
+      <c r="U48" s="21" t="n">
         <v>3.53</v>
-      </c>
-      <c r="U48" s="21" t="n">
-        <v>3.56</v>
       </c>
     </row>
     <row r="49">
@@ -4407,7 +4407,7 @@
         </is>
       </c>
       <c r="N49" s="49" t="n">
-        <v>46052</v>
+        <v>46055</v>
       </c>
       <c r="O49" s="6" t="inlineStr">
         <is>
@@ -4420,19 +4420,19 @@
         </is>
       </c>
       <c r="Q49" s="6" t="n">
+        <v>3.83</v>
+      </c>
+      <c r="R49" s="6" t="n">
         <v>3.79</v>
       </c>
-      <c r="R49" s="6" t="n">
+      <c r="S49" s="6" t="n">
         <v>3.8</v>
       </c>
-      <c r="S49" s="6" t="n">
+      <c r="T49" s="6" t="n">
         <v>3.83</v>
       </c>
-      <c r="T49" s="6" t="n">
+      <c r="U49" s="21" t="n">
         <v>3.81</v>
-      </c>
-      <c r="U49" s="21" t="n">
-        <v>3.82</v>
       </c>
     </row>
     <row r="50">
@@ -4486,7 +4486,7 @@
         </is>
       </c>
       <c r="N50" s="49" t="n">
-        <v>46052</v>
+        <v>46055</v>
       </c>
       <c r="O50" s="6" t="inlineStr">
         <is>
@@ -4499,19 +4499,19 @@
         </is>
       </c>
       <c r="Q50" s="6" t="n">
+        <v>4.29</v>
+      </c>
+      <c r="R50" s="6" t="n">
         <v>4.26</v>
       </c>
-      <c r="R50" s="6" t="n">
+      <c r="S50" s="6" t="n">
         <v>4.24</v>
       </c>
-      <c r="S50" s="6" t="n">
+      <c r="T50" s="6" t="n">
         <v>4.26</v>
       </c>
-      <c r="T50" s="6" t="n">
+      <c r="U50" s="21" t="n">
         <v>4.24</v>
-      </c>
-      <c r="U50" s="21" t="n">
-        <v>4.22</v>
       </c>
     </row>
     <row r="51" ht="31.5" customHeight="1">
@@ -4612,7 +4612,7 @@
         </is>
       </c>
       <c r="N52" s="50" t="n">
-        <v>46052</v>
+        <v>46055</v>
       </c>
       <c r="O52" s="9" t="inlineStr">
         <is>
@@ -4625,19 +4625,19 @@
         </is>
       </c>
       <c r="Q52" s="9" t="n">
+        <v>5.9</v>
+      </c>
+      <c r="R52" s="9" t="n">
         <v>5.88</v>
       </c>
-      <c r="R52" s="9" t="n">
+      <c r="S52" s="9" t="n">
         <v>5.87</v>
       </c>
-      <c r="S52" s="9" t="n">
+      <c r="T52" s="9" t="n">
         <v>5.88</v>
       </c>
-      <c r="T52" s="9" t="n">
+      <c r="U52" s="22" t="n">
         <v>5.85</v>
-      </c>
-      <c r="U52" s="22" t="n">
-        <v>5.83</v>
       </c>
     </row>
     <row r="53" ht="21" customHeight="1">

</xml_diff>

<commit_message>
Update dashboards - 2026-02-05
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -1704,7 +1704,7 @@
         </is>
       </c>
       <c r="N13" s="49" t="n">
-        <v>46041</v>
+        <v>46048</v>
       </c>
       <c r="O13" s="6" t="inlineStr">
         <is>
@@ -1717,19 +1717,19 @@
         </is>
       </c>
       <c r="Q13" s="24" t="n">
+        <v>231000</v>
+      </c>
+      <c r="R13" s="24" t="n">
         <v>209000</v>
       </c>
-      <c r="R13" s="24" t="n">
+      <c r="S13" s="24" t="n">
         <v>210000</v>
       </c>
-      <c r="S13" s="24" t="n">
+      <c r="T13" s="24" t="n">
         <v>199000</v>
       </c>
-      <c r="T13" s="24" t="n">
+      <c r="U13" s="26" t="n">
         <v>207000</v>
-      </c>
-      <c r="U13" s="26" t="n">
-        <v>200000</v>
       </c>
     </row>
     <row r="14">
@@ -1779,7 +1779,7 @@
         </is>
       </c>
       <c r="N14" s="49" t="n">
-        <v>46034</v>
+        <v>46041</v>
       </c>
       <c r="O14" s="6" t="inlineStr">
         <is>
@@ -1792,19 +1792,19 @@
         </is>
       </c>
       <c r="Q14" s="24" t="n">
-        <v>1827000</v>
+        <v>1844000</v>
       </c>
       <c r="R14" s="24" t="n">
+        <v>1819000</v>
+      </c>
+      <c r="S14" s="24" t="n">
         <v>1865000</v>
       </c>
-      <c r="S14" s="24" t="n">
+      <c r="T14" s="24" t="n">
         <v>1875000</v>
       </c>
-      <c r="T14" s="24" t="n">
+      <c r="U14" s="26" t="n">
         <v>1903000</v>
-      </c>
-      <c r="U14" s="26" t="n">
-        <v>1856000</v>
       </c>
     </row>
     <row r="15">
@@ -2907,7 +2907,7 @@
         </is>
       </c>
       <c r="N29" s="49" t="n">
-        <v>46056</v>
+        <v>46057</v>
       </c>
       <c r="O29" s="6" t="inlineStr">
         <is>
@@ -2923,16 +2923,16 @@
         <v>2.19</v>
       </c>
       <c r="R29" s="6" t="n">
+        <v>2.19</v>
+      </c>
+      <c r="S29" s="6" t="n">
         <v>2.18</v>
       </c>
-      <c r="S29" s="6" t="n">
+      <c r="T29" s="6" t="n">
         <v>2.19</v>
       </c>
-      <c r="T29" s="6" t="n">
+      <c r="U29" s="21" t="n">
         <v>2.18</v>
-      </c>
-      <c r="U29" s="21" t="n">
-        <v>2.22</v>
       </c>
     </row>
     <row r="30">
@@ -2986,7 +2986,7 @@
         </is>
       </c>
       <c r="N30" s="49" t="n">
-        <v>46056</v>
+        <v>46057</v>
       </c>
       <c r="O30" s="6" t="inlineStr">
         <is>
@@ -2999,19 +2999,19 @@
         </is>
       </c>
       <c r="Q30" s="6" t="n">
+        <v>2.35</v>
+      </c>
+      <c r="R30" s="6" t="n">
         <v>2.36</v>
       </c>
-      <c r="R30" s="6" t="n">
+      <c r="S30" s="6" t="n">
         <v>2.35</v>
       </c>
-      <c r="S30" s="6" t="n">
+      <c r="T30" s="6" t="n">
         <v>2.36</v>
       </c>
-      <c r="T30" s="6" t="n">
+      <c r="U30" s="21" t="n">
         <v>2.35</v>
-      </c>
-      <c r="U30" s="21" t="n">
-        <v>2.36</v>
       </c>
     </row>
     <row r="31">
@@ -4126,7 +4126,7 @@
           <t>BOPTEXP</t>
         </is>
       </c>
-      <c r="C46" s="49" t="n">
+      <c r="C46" s="48" t="n">
         <v>45962</v>
       </c>
       <c r="D46" s="6" t="inlineStr">
@@ -4213,7 +4213,7 @@
           <t>BOPTEXP</t>
         </is>
       </c>
-      <c r="C47" s="49" t="n">
+      <c r="C47" s="48" t="n">
         <v>45962</v>
       </c>
       <c r="D47" s="6" t="inlineStr">
@@ -4253,7 +4253,7 @@
         </is>
       </c>
       <c r="N47" s="49" t="n">
-        <v>46055</v>
+        <v>46056</v>
       </c>
       <c r="O47" s="6" t="inlineStr">
         <is>
@@ -4292,7 +4292,7 @@
           <t>BOPTIMP</t>
         </is>
       </c>
-      <c r="C48" s="49" t="n">
+      <c r="C48" s="48" t="n">
         <v>45962</v>
       </c>
       <c r="D48" s="6" t="inlineStr">
@@ -4332,7 +4332,7 @@
         </is>
       </c>
       <c r="N48" s="49" t="n">
-        <v>46055</v>
+        <v>46056</v>
       </c>
       <c r="O48" s="6" t="inlineStr">
         <is>
@@ -4348,16 +4348,16 @@
         <v>3.57</v>
       </c>
       <c r="R48" s="6" t="n">
+        <v>3.57</v>
+      </c>
+      <c r="S48" s="6" t="n">
         <v>3.52</v>
       </c>
-      <c r="S48" s="6" t="n">
+      <c r="T48" s="6" t="n">
         <v>3.53</v>
       </c>
-      <c r="T48" s="6" t="n">
+      <c r="U48" s="21" t="n">
         <v>3.56</v>
-      </c>
-      <c r="U48" s="21" t="n">
-        <v>3.53</v>
       </c>
     </row>
     <row r="49">
@@ -4367,7 +4367,7 @@
           <t>BOPTIMP</t>
         </is>
       </c>
-      <c r="C49" s="49" t="n">
+      <c r="C49" s="48" t="n">
         <v>45962</v>
       </c>
       <c r="D49" s="6" t="inlineStr">
@@ -4407,7 +4407,7 @@
         </is>
       </c>
       <c r="N49" s="49" t="n">
-        <v>46055</v>
+        <v>46056</v>
       </c>
       <c r="O49" s="6" t="inlineStr">
         <is>
@@ -4423,16 +4423,16 @@
         <v>3.83</v>
       </c>
       <c r="R49" s="6" t="n">
+        <v>3.83</v>
+      </c>
+      <c r="S49" s="6" t="n">
         <v>3.79</v>
       </c>
-      <c r="S49" s="6" t="n">
+      <c r="T49" s="6" t="n">
         <v>3.8</v>
       </c>
-      <c r="T49" s="6" t="n">
+      <c r="U49" s="21" t="n">
         <v>3.83</v>
-      </c>
-      <c r="U49" s="21" t="n">
-        <v>3.81</v>
       </c>
     </row>
     <row r="50">
@@ -4446,7 +4446,7 @@
           <t>BOPSTB</t>
         </is>
       </c>
-      <c r="C50" s="49" t="n">
+      <c r="C50" s="48" t="n">
         <v>45962</v>
       </c>
       <c r="D50" s="6" t="inlineStr">
@@ -4486,7 +4486,7 @@
         </is>
       </c>
       <c r="N50" s="49" t="n">
-        <v>46055</v>
+        <v>46056</v>
       </c>
       <c r="O50" s="6" t="inlineStr">
         <is>
@@ -4499,19 +4499,19 @@
         </is>
       </c>
       <c r="Q50" s="6" t="n">
+        <v>4.28</v>
+      </c>
+      <c r="R50" s="6" t="n">
         <v>4.29</v>
       </c>
-      <c r="R50" s="6" t="n">
+      <c r="S50" s="6" t="n">
         <v>4.26</v>
       </c>
-      <c r="S50" s="6" t="n">
+      <c r="T50" s="6" t="n">
         <v>4.24</v>
       </c>
-      <c r="T50" s="6" t="n">
+      <c r="U50" s="21" t="n">
         <v>4.26</v>
-      </c>
-      <c r="U50" s="21" t="n">
-        <v>4.24</v>
       </c>
     </row>
     <row r="51" ht="31.5" customHeight="1">
@@ -4521,7 +4521,7 @@
           <t>BOPSTB</t>
         </is>
       </c>
-      <c r="C51" s="49" t="n">
+      <c r="C51" s="48" t="n">
         <v>45962</v>
       </c>
       <c r="D51" s="6" t="inlineStr">
@@ -4560,7 +4560,7 @@
           <t>MORTGAGE30US</t>
         </is>
       </c>
-      <c r="N51" s="49" t="n">
+      <c r="N51" s="48" t="n">
         <v>46048</v>
       </c>
       <c r="O51" s="6" t="inlineStr">
@@ -4612,7 +4612,7 @@
         </is>
       </c>
       <c r="N52" s="50" t="n">
-        <v>46055</v>
+        <v>46056</v>
       </c>
       <c r="O52" s="9" t="inlineStr">
         <is>
@@ -4625,19 +4625,19 @@
         </is>
       </c>
       <c r="Q52" s="9" t="n">
+        <v>5.91</v>
+      </c>
+      <c r="R52" s="9" t="n">
         <v>5.9</v>
       </c>
-      <c r="R52" s="9" t="n">
+      <c r="S52" s="9" t="n">
         <v>5.88</v>
       </c>
-      <c r="S52" s="9" t="n">
+      <c r="T52" s="9" t="n">
         <v>5.87</v>
       </c>
-      <c r="T52" s="9" t="n">
+      <c r="U52" s="22" t="n">
         <v>5.88</v>
-      </c>
-      <c r="U52" s="22" t="n">
-        <v>5.85</v>
       </c>
     </row>
     <row r="53" ht="21" customHeight="1">

</xml_diff>

<commit_message>
Update dashboards - 2026-02-06
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -1470,8 +1470,8 @@
           <t>JTSJOR</t>
         </is>
       </c>
-      <c r="N10" s="48" t="n">
-        <v>45962</v>
+      <c r="N10" s="49" t="n">
+        <v>45992</v>
       </c>
       <c r="O10" s="6" t="inlineStr">
         <is>
@@ -1484,16 +1484,16 @@
         </is>
       </c>
       <c r="Q10" s="6" t="n">
-        <v>4.3</v>
+        <v>3.9</v>
       </c>
       <c r="R10" s="6" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="S10" s="6" t="n">
         <v>4.5</v>
       </c>
-      <c r="S10" s="6" t="n">
+      <c r="T10" s="6" t="n">
         <v>4.6</v>
-      </c>
-      <c r="T10" s="6" t="n">
-        <v>4.3</v>
       </c>
       <c r="U10" s="21" t="n">
         <v>4.3</v>
@@ -1549,8 +1549,8 @@
           <t>JTSHIR</t>
         </is>
       </c>
-      <c r="N11" s="48" t="n">
-        <v>45962</v>
+      <c r="N11" s="49" t="n">
+        <v>45992</v>
       </c>
       <c r="O11" s="6" t="inlineStr">
         <is>
@@ -1563,19 +1563,19 @@
         </is>
       </c>
       <c r="Q11" s="6" t="n">
+        <v>3.3</v>
+      </c>
+      <c r="R11" s="6" t="n">
         <v>3.2</v>
-      </c>
-      <c r="R11" s="6" t="n">
-        <v>3.4</v>
       </c>
       <c r="S11" s="6" t="n">
         <v>3.4</v>
       </c>
       <c r="T11" s="6" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="U11" s="21" t="n">
         <v>3.2</v>
-      </c>
-      <c r="U11" s="21" t="n">
-        <v>3.3</v>
       </c>
     </row>
     <row r="12">
@@ -1624,8 +1624,8 @@
           <t>JTSTSR</t>
         </is>
       </c>
-      <c r="N12" s="48" t="n">
-        <v>45962</v>
+      <c r="N12" s="49" t="n">
+        <v>45992</v>
       </c>
       <c r="O12" s="6" t="inlineStr">
         <is>
@@ -1638,19 +1638,19 @@
         </is>
       </c>
       <c r="Q12" s="6" t="n">
-        <v>3.2</v>
+        <v>3.3</v>
       </c>
       <c r="R12" s="6" t="n">
         <v>3.2</v>
       </c>
       <c r="S12" s="6" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="T12" s="6" t="n">
         <v>3.3</v>
       </c>
-      <c r="T12" s="6" t="n">
+      <c r="U12" s="21" t="n">
         <v>3.2</v>
-      </c>
-      <c r="U12" s="21" t="n">
-        <v>3.3</v>
       </c>
     </row>
     <row r="13">
@@ -2374,7 +2374,7 @@
           <t>PPIFIS</t>
         </is>
       </c>
-      <c r="N22" s="49" t="n">
+      <c r="N22" s="48" t="n">
         <v>45992</v>
       </c>
       <c r="O22" s="6" t="inlineStr">
@@ -2444,7 +2444,7 @@
           <t>PPIFIS</t>
         </is>
       </c>
-      <c r="N23" s="49" t="n">
+      <c r="N23" s="48" t="n">
         <v>45992</v>
       </c>
       <c r="O23" s="6" t="inlineStr">
@@ -2907,7 +2907,7 @@
         </is>
       </c>
       <c r="N29" s="49" t="n">
-        <v>46057</v>
+        <v>46058</v>
       </c>
       <c r="O29" s="6" t="inlineStr">
         <is>
@@ -2920,19 +2920,19 @@
         </is>
       </c>
       <c r="Q29" s="6" t="n">
-        <v>2.19</v>
+        <v>2.16</v>
       </c>
       <c r="R29" s="6" t="n">
         <v>2.19</v>
       </c>
       <c r="S29" s="6" t="n">
+        <v>2.19</v>
+      </c>
+      <c r="T29" s="6" t="n">
         <v>2.18</v>
       </c>
-      <c r="T29" s="6" t="n">
+      <c r="U29" s="21" t="n">
         <v>2.19</v>
-      </c>
-      <c r="U29" s="21" t="n">
-        <v>2.18</v>
       </c>
     </row>
     <row r="30">
@@ -2986,7 +2986,7 @@
         </is>
       </c>
       <c r="N30" s="49" t="n">
-        <v>46057</v>
+        <v>46058</v>
       </c>
       <c r="O30" s="6" t="inlineStr">
         <is>
@@ -2999,19 +2999,19 @@
         </is>
       </c>
       <c r="Q30" s="6" t="n">
+        <v>2.32</v>
+      </c>
+      <c r="R30" s="6" t="n">
         <v>2.35</v>
       </c>
-      <c r="R30" s="6" t="n">
+      <c r="S30" s="6" t="n">
         <v>2.36</v>
       </c>
-      <c r="S30" s="6" t="n">
+      <c r="T30" s="6" t="n">
         <v>2.35</v>
       </c>
-      <c r="T30" s="6" t="n">
+      <c r="U30" s="21" t="n">
         <v>2.36</v>
-      </c>
-      <c r="U30" s="21" t="n">
-        <v>2.35</v>
       </c>
     </row>
     <row r="31">
@@ -4253,7 +4253,7 @@
         </is>
       </c>
       <c r="N47" s="49" t="n">
-        <v>46056</v>
+        <v>46057</v>
       </c>
       <c r="O47" s="6" t="inlineStr">
         <is>
@@ -4332,7 +4332,7 @@
         </is>
       </c>
       <c r="N48" s="49" t="n">
-        <v>46056</v>
+        <v>46057</v>
       </c>
       <c r="O48" s="6" t="inlineStr">
         <is>
@@ -4351,13 +4351,13 @@
         <v>3.57</v>
       </c>
       <c r="S48" s="6" t="n">
+        <v>3.57</v>
+      </c>
+      <c r="T48" s="6" t="n">
         <v>3.52</v>
       </c>
-      <c r="T48" s="6" t="n">
+      <c r="U48" s="21" t="n">
         <v>3.53</v>
-      </c>
-      <c r="U48" s="21" t="n">
-        <v>3.56</v>
       </c>
     </row>
     <row r="49">
@@ -4407,7 +4407,7 @@
         </is>
       </c>
       <c r="N49" s="49" t="n">
-        <v>46056</v>
+        <v>46057</v>
       </c>
       <c r="O49" s="6" t="inlineStr">
         <is>
@@ -4426,13 +4426,13 @@
         <v>3.83</v>
       </c>
       <c r="S49" s="6" t="n">
+        <v>3.83</v>
+      </c>
+      <c r="T49" s="6" t="n">
         <v>3.79</v>
       </c>
-      <c r="T49" s="6" t="n">
+      <c r="U49" s="21" t="n">
         <v>3.8</v>
-      </c>
-      <c r="U49" s="21" t="n">
-        <v>3.83</v>
       </c>
     </row>
     <row r="50">
@@ -4486,7 +4486,7 @@
         </is>
       </c>
       <c r="N50" s="49" t="n">
-        <v>46056</v>
+        <v>46057</v>
       </c>
       <c r="O50" s="6" t="inlineStr">
         <is>
@@ -4499,19 +4499,19 @@
         </is>
       </c>
       <c r="Q50" s="6" t="n">
+        <v>4.29</v>
+      </c>
+      <c r="R50" s="6" t="n">
         <v>4.28</v>
       </c>
-      <c r="R50" s="6" t="n">
+      <c r="S50" s="6" t="n">
         <v>4.29</v>
       </c>
-      <c r="S50" s="6" t="n">
+      <c r="T50" s="6" t="n">
         <v>4.26</v>
       </c>
-      <c r="T50" s="6" t="n">
+      <c r="U50" s="21" t="n">
         <v>4.24</v>
-      </c>
-      <c r="U50" s="21" t="n">
-        <v>4.26</v>
       </c>
     </row>
     <row r="51" ht="31.5" customHeight="1">
@@ -4560,8 +4560,8 @@
           <t>MORTGAGE30US</t>
         </is>
       </c>
-      <c r="N51" s="48" t="n">
-        <v>46048</v>
+      <c r="N51" s="49" t="n">
+        <v>46055</v>
       </c>
       <c r="O51" s="6" t="inlineStr">
         <is>
@@ -4574,19 +4574,19 @@
         </is>
       </c>
       <c r="Q51" s="6" t="n">
+        <v>6.11</v>
+      </c>
+      <c r="R51" s="6" t="n">
         <v>6.1</v>
       </c>
-      <c r="R51" s="6" t="n">
+      <c r="S51" s="6" t="n">
         <v>6.09</v>
       </c>
-      <c r="S51" s="6" t="n">
+      <c r="T51" s="6" t="n">
         <v>6.06</v>
       </c>
-      <c r="T51" s="6" t="n">
+      <c r="U51" s="21" t="n">
         <v>6.16</v>
-      </c>
-      <c r="U51" s="21" t="n">
-        <v>6.15</v>
       </c>
     </row>
     <row r="52" ht="16.15" customHeight="1" thickBot="1">
@@ -4612,7 +4612,7 @@
         </is>
       </c>
       <c r="N52" s="50" t="n">
-        <v>46056</v>
+        <v>46057</v>
       </c>
       <c r="O52" s="9" t="inlineStr">
         <is>
@@ -4625,19 +4625,19 @@
         </is>
       </c>
       <c r="Q52" s="9" t="n">
+        <v>5.93</v>
+      </c>
+      <c r="R52" s="9" t="n">
         <v>5.91</v>
       </c>
-      <c r="R52" s="9" t="n">
+      <c r="S52" s="9" t="n">
         <v>5.9</v>
       </c>
-      <c r="S52" s="9" t="n">
+      <c r="T52" s="9" t="n">
         <v>5.88</v>
       </c>
-      <c r="T52" s="9" t="n">
+      <c r="U52" s="22" t="n">
         <v>5.87</v>
-      </c>
-      <c r="U52" s="22" t="n">
-        <v>5.88</v>
       </c>
     </row>
     <row r="53" ht="21" customHeight="1">

</xml_diff>

<commit_message>
Update dashboards - 2026-02-07
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -2335,8 +2335,8 @@
           <t>TOTALSA</t>
         </is>
       </c>
-      <c r="C22" s="48" t="n">
-        <v>45992</v>
+      <c r="C22" s="49" t="n">
+        <v>46023</v>
       </c>
       <c r="D22" s="6" t="inlineStr">
         <is>
@@ -2349,19 +2349,19 @@
         </is>
       </c>
       <c r="F22" s="24" t="n">
-        <v>16.481</v>
+        <v>15.396</v>
       </c>
       <c r="G22" s="24" t="n">
-        <v>16.117</v>
+        <v>16.394</v>
       </c>
       <c r="H22" s="24" t="n">
-        <v>15.807</v>
+        <v>16.003</v>
       </c>
       <c r="I22" s="24" t="n">
-        <v>16.663</v>
+        <v>15.836</v>
       </c>
       <c r="J22" s="24" t="n">
-        <v>16.916</v>
+        <v>16.982</v>
       </c>
       <c r="K22" s="5" t="n"/>
       <c r="L22" s="28" t="inlineStr">
@@ -2410,8 +2410,8 @@
           <t>TOTALSA</t>
         </is>
       </c>
-      <c r="C23" s="48" t="n">
-        <v>45992</v>
+      <c r="C23" s="49" t="n">
+        <v>46023</v>
       </c>
       <c r="D23" s="6" t="inlineStr">
         <is>
@@ -2424,19 +2424,19 @@
         </is>
       </c>
       <c r="F23" s="25" t="n">
-        <v>-0.04761629586824606</v>
+        <v>-0.03473354231974912</v>
       </c>
       <c r="G23" s="25" t="n">
-        <v>-0.05221993531314308</v>
+        <v>-0.05242471533437374</v>
       </c>
       <c r="H23" s="25" t="n">
-        <v>-0.04524039623097369</v>
+        <v>-0.0535249585994796</v>
       </c>
       <c r="I23" s="25" t="n">
-        <v>0.02114229685010411</v>
+        <v>-0.03983508154974828</v>
       </c>
       <c r="J23" s="25" t="n">
-        <v>0.05976694649793263</v>
+        <v>0.03922648552720141</v>
       </c>
       <c r="K23" s="5" t="n"/>
       <c r="M23" s="15" t="inlineStr">
@@ -2484,8 +2484,8 @@
           <t>REVOLSL</t>
         </is>
       </c>
-      <c r="C24" s="48" t="n">
-        <v>45962</v>
+      <c r="C24" s="49" t="n">
+        <v>45992</v>
       </c>
       <c r="D24" s="6" t="inlineStr">
         <is>
@@ -2498,19 +2498,19 @@
         </is>
       </c>
       <c r="F24" s="38" t="n">
-        <v>-0.001551215487983981</v>
+        <v>0.0105318556006937</v>
       </c>
       <c r="G24" s="38" t="n">
-        <v>0.004120302067736503</v>
+        <v>-0.001281418924231392</v>
       </c>
       <c r="H24" s="38" t="n">
-        <v>0.003065216912115698</v>
+        <v>0.004454853076971466</v>
       </c>
       <c r="I24" s="38" t="n">
-        <v>-0.003484844670176512</v>
+        <v>0.00339828596255809</v>
       </c>
       <c r="J24" s="38" t="n">
-        <v>0.008311712980978658</v>
+        <v>-0.003651114145611811</v>
       </c>
       <c r="K24" s="5" t="n"/>
       <c r="L24" s="28" t="inlineStr">
@@ -2563,8 +2563,8 @@
           <t>NONREVSL</t>
         </is>
       </c>
-      <c r="C25" s="48" t="n">
-        <v>45962</v>
+      <c r="C25" s="49" t="n">
+        <v>45992</v>
       </c>
       <c r="D25" s="6" t="inlineStr">
         <is>
@@ -2577,19 +2577,19 @@
         </is>
       </c>
       <c r="F25" s="38" t="n">
-        <v>0.001665686369376251</v>
+        <v>0.002704782960157415</v>
       </c>
       <c r="G25" s="38" t="n">
-        <v>0.001019986599621658</v>
+        <v>0.001696137399219255</v>
       </c>
       <c r="H25" s="38" t="n">
-        <v>0.001988823510608029</v>
+        <v>0.0009232413445350307</v>
       </c>
       <c r="I25" s="38" t="n">
-        <v>0.001936089671301433</v>
+        <v>0.001873721239173287</v>
       </c>
       <c r="J25" s="38" t="n">
-        <v>0.0009927073679749654</v>
+        <v>0.001994229089696598</v>
       </c>
       <c r="K25" s="5" t="n"/>
       <c r="L25" s="28" t="n"/>
@@ -2907,7 +2907,7 @@
         </is>
       </c>
       <c r="N29" s="49" t="n">
-        <v>46058</v>
+        <v>46059</v>
       </c>
       <c r="O29" s="6" t="inlineStr">
         <is>
@@ -2920,19 +2920,19 @@
         </is>
       </c>
       <c r="Q29" s="6" t="n">
+        <v>2.18</v>
+      </c>
+      <c r="R29" s="6" t="n">
         <v>2.16</v>
-      </c>
-      <c r="R29" s="6" t="n">
-        <v>2.19</v>
       </c>
       <c r="S29" s="6" t="n">
         <v>2.19</v>
       </c>
       <c r="T29" s="6" t="n">
+        <v>2.19</v>
+      </c>
+      <c r="U29" s="21" t="n">
         <v>2.18</v>
-      </c>
-      <c r="U29" s="21" t="n">
-        <v>2.19</v>
       </c>
     </row>
     <row r="30">
@@ -2986,7 +2986,7 @@
         </is>
       </c>
       <c r="N30" s="49" t="n">
-        <v>46058</v>
+        <v>46059</v>
       </c>
       <c r="O30" s="6" t="inlineStr">
         <is>
@@ -2999,19 +2999,19 @@
         </is>
       </c>
       <c r="Q30" s="6" t="n">
+        <v>2.34</v>
+      </c>
+      <c r="R30" s="6" t="n">
         <v>2.32</v>
       </c>
-      <c r="R30" s="6" t="n">
+      <c r="S30" s="6" t="n">
         <v>2.35</v>
       </c>
-      <c r="S30" s="6" t="n">
+      <c r="T30" s="6" t="n">
         <v>2.36</v>
       </c>
-      <c r="T30" s="6" t="n">
+      <c r="U30" s="21" t="n">
         <v>2.35</v>
-      </c>
-      <c r="U30" s="21" t="n">
-        <v>2.36</v>
       </c>
     </row>
     <row r="31">
@@ -4253,7 +4253,7 @@
         </is>
       </c>
       <c r="N47" s="49" t="n">
-        <v>46057</v>
+        <v>46058</v>
       </c>
       <c r="O47" s="6" t="inlineStr">
         <is>
@@ -4332,7 +4332,7 @@
         </is>
       </c>
       <c r="N48" s="49" t="n">
-        <v>46057</v>
+        <v>46058</v>
       </c>
       <c r="O48" s="6" t="inlineStr">
         <is>
@@ -4345,7 +4345,7 @@
         </is>
       </c>
       <c r="Q48" s="6" t="n">
-        <v>3.57</v>
+        <v>3.47</v>
       </c>
       <c r="R48" s="6" t="n">
         <v>3.57</v>
@@ -4354,10 +4354,10 @@
         <v>3.57</v>
       </c>
       <c r="T48" s="6" t="n">
+        <v>3.57</v>
+      </c>
+      <c r="U48" s="21" t="n">
         <v>3.52</v>
-      </c>
-      <c r="U48" s="21" t="n">
-        <v>3.53</v>
       </c>
     </row>
     <row r="49">
@@ -4407,7 +4407,7 @@
         </is>
       </c>
       <c r="N49" s="49" t="n">
-        <v>46057</v>
+        <v>46058</v>
       </c>
       <c r="O49" s="6" t="inlineStr">
         <is>
@@ -4420,7 +4420,7 @@
         </is>
       </c>
       <c r="Q49" s="6" t="n">
-        <v>3.83</v>
+        <v>3.74</v>
       </c>
       <c r="R49" s="6" t="n">
         <v>3.83</v>
@@ -4429,10 +4429,10 @@
         <v>3.83</v>
       </c>
       <c r="T49" s="6" t="n">
+        <v>3.83</v>
+      </c>
+      <c r="U49" s="21" t="n">
         <v>3.79</v>
-      </c>
-      <c r="U49" s="21" t="n">
-        <v>3.8</v>
       </c>
     </row>
     <row r="50">
@@ -4486,7 +4486,7 @@
         </is>
       </c>
       <c r="N50" s="49" t="n">
-        <v>46057</v>
+        <v>46058</v>
       </c>
       <c r="O50" s="6" t="inlineStr">
         <is>
@@ -4499,19 +4499,19 @@
         </is>
       </c>
       <c r="Q50" s="6" t="n">
+        <v>4.21</v>
+      </c>
+      <c r="R50" s="6" t="n">
         <v>4.29</v>
       </c>
-      <c r="R50" s="6" t="n">
+      <c r="S50" s="6" t="n">
         <v>4.28</v>
       </c>
-      <c r="S50" s="6" t="n">
+      <c r="T50" s="6" t="n">
         <v>4.29</v>
       </c>
-      <c r="T50" s="6" t="n">
+      <c r="U50" s="21" t="n">
         <v>4.26</v>
-      </c>
-      <c r="U50" s="21" t="n">
-        <v>4.24</v>
       </c>
     </row>
     <row r="51" ht="31.5" customHeight="1">
@@ -4612,7 +4612,7 @@
         </is>
       </c>
       <c r="N52" s="50" t="n">
-        <v>46057</v>
+        <v>46058</v>
       </c>
       <c r="O52" s="9" t="inlineStr">
         <is>
@@ -4625,19 +4625,19 @@
         </is>
       </c>
       <c r="Q52" s="9" t="n">
+        <v>5.88</v>
+      </c>
+      <c r="R52" s="9" t="n">
         <v>5.93</v>
       </c>
-      <c r="R52" s="9" t="n">
+      <c r="S52" s="9" t="n">
         <v>5.91</v>
       </c>
-      <c r="S52" s="9" t="n">
+      <c r="T52" s="9" t="n">
         <v>5.9</v>
       </c>
-      <c r="T52" s="9" t="n">
+      <c r="U52" s="22" t="n">
         <v>5.88</v>
-      </c>
-      <c r="U52" s="22" t="n">
-        <v>5.87</v>
       </c>
     </row>
     <row r="53" ht="21" customHeight="1">

</xml_diff>

<commit_message>
Update dashboards - 2026-02-09
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -1277,7 +1277,7 @@
           <t>RECPROUSM156N</t>
         </is>
       </c>
-      <c r="C8" s="49" t="n">
+      <c r="C8" s="48" t="n">
         <v>45992</v>
       </c>
       <c r="D8" s="6" t="inlineStr">
@@ -3664,7 +3664,7 @@
           <t>TWEXBGSMTH</t>
         </is>
       </c>
-      <c r="N39" s="49" t="n">
+      <c r="N39" s="48" t="n">
         <v>46023</v>
       </c>
       <c r="O39" s="6" t="inlineStr">
@@ -3739,7 +3739,7 @@
           <t>TWEXBGSMTH</t>
         </is>
       </c>
-      <c r="N40" s="49" t="n">
+      <c r="N40" s="48" t="n">
         <v>46023</v>
       </c>
       <c r="O40" s="6" t="inlineStr">

</xml_diff>

<commit_message>
Update dashboards - 2026-02-10
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -1944,8 +1944,8 @@
           <t>RSAFS</t>
         </is>
       </c>
-      <c r="C17" s="48" t="n">
-        <v>45962</v>
+      <c r="C17" s="49" t="n">
+        <v>45992</v>
       </c>
       <c r="D17" s="6" t="inlineStr">
         <is>
@@ -1958,19 +1958,19 @@
         </is>
       </c>
       <c r="F17" s="25" t="n">
-        <v>0.006141545394387826</v>
+        <v>-0.000160525653495891</v>
       </c>
       <c r="G17" s="25" t="n">
-        <v>-0.001065294349023249</v>
+        <v>0.005518082869731433</v>
       </c>
       <c r="H17" s="25" t="n">
+        <v>-0.001558334425942887</v>
+      </c>
+      <c r="I17" s="25" t="n">
         <v>0.0006724067240673204</v>
       </c>
-      <c r="I17" s="25" t="n">
+      <c r="J17" s="25" t="n">
         <v>0.00545946488174831</v>
-      </c>
-      <c r="J17" s="25" t="n">
-        <v>0.006492096487988874</v>
       </c>
       <c r="K17" s="5" t="n"/>
       <c r="L17" s="29" t="inlineStr">
@@ -2031,8 +2031,8 @@
           <t>RSAFS</t>
         </is>
       </c>
-      <c r="C18" s="48" t="n">
-        <v>45962</v>
+      <c r="C18" s="49" t="n">
+        <v>45992</v>
       </c>
       <c r="D18" s="6" t="inlineStr">
         <is>
@@ -2045,19 +2045,19 @@
         </is>
       </c>
       <c r="F18" s="25" t="n">
-        <v>0.03331905781584583</v>
+        <v>0.02427715536403887</v>
       </c>
       <c r="G18" s="25" t="n">
-        <v>0.03264482062432054</v>
+        <v>0.03263595152369941</v>
       </c>
       <c r="H18" s="25" t="n">
+        <v>0.03213514238518121</v>
+      </c>
+      <c r="I18" s="25" t="n">
         <v>0.04144341481107452</v>
       </c>
-      <c r="I18" s="25" t="n">
+      <c r="J18" s="25" t="n">
         <v>0.04972605550048132</v>
-      </c>
-      <c r="J18" s="25" t="n">
-        <v>0.04134309243240536</v>
       </c>
       <c r="K18" s="5" t="n"/>
       <c r="L18" s="28" t="inlineStr">
@@ -2907,7 +2907,7 @@
         </is>
       </c>
       <c r="N29" s="49" t="n">
-        <v>46059</v>
+        <v>46062</v>
       </c>
       <c r="O29" s="6" t="inlineStr">
         <is>
@@ -2920,19 +2920,19 @@
         </is>
       </c>
       <c r="Q29" s="6" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="R29" s="6" t="n">
         <v>2.18</v>
       </c>
-      <c r="R29" s="6" t="n">
+      <c r="S29" s="6" t="n">
         <v>2.16</v>
-      </c>
-      <c r="S29" s="6" t="n">
-        <v>2.19</v>
       </c>
       <c r="T29" s="6" t="n">
         <v>2.19</v>
       </c>
       <c r="U29" s="21" t="n">
-        <v>2.18</v>
+        <v>2.19</v>
       </c>
     </row>
     <row r="30">
@@ -2986,7 +2986,7 @@
         </is>
       </c>
       <c r="N30" s="49" t="n">
-        <v>46059</v>
+        <v>46062</v>
       </c>
       <c r="O30" s="6" t="inlineStr">
         <is>
@@ -2999,19 +2999,19 @@
         </is>
       </c>
       <c r="Q30" s="6" t="n">
+        <v>2.35</v>
+      </c>
+      <c r="R30" s="6" t="n">
         <v>2.34</v>
       </c>
-      <c r="R30" s="6" t="n">
+      <c r="S30" s="6" t="n">
         <v>2.32</v>
       </c>
-      <c r="S30" s="6" t="n">
+      <c r="T30" s="6" t="n">
         <v>2.35</v>
       </c>
-      <c r="T30" s="6" t="n">
+      <c r="U30" s="21" t="n">
         <v>2.36</v>
-      </c>
-      <c r="U30" s="21" t="n">
-        <v>2.35</v>
       </c>
     </row>
     <row r="31">
@@ -3060,8 +3060,8 @@
           <t>ECIWAG</t>
         </is>
       </c>
-      <c r="N31" s="48" t="n">
-        <v>45839</v>
+      <c r="N31" s="49" t="n">
+        <v>45931</v>
       </c>
       <c r="O31" s="6" t="inlineStr">
         <is>
@@ -3074,19 +3074,19 @@
         </is>
       </c>
       <c r="Q31" s="38" t="n">
+        <v>0.007310493043885868</v>
+      </c>
+      <c r="R31" s="38" t="n">
         <v>0.007996957929548465</v>
       </c>
-      <c r="R31" s="38" t="n">
+      <c r="S31" s="38" t="n">
         <v>0.01027939464493599</v>
       </c>
-      <c r="S31" s="38" t="n">
+      <c r="T31" s="38" t="n">
         <v>0.007624633431085215</v>
       </c>
-      <c r="T31" s="38" t="n">
+      <c r="U31" s="23" t="n">
         <v>0.009473060982829962</v>
-      </c>
-      <c r="U31" s="23" t="n">
-        <v>0.007756563245823411</v>
       </c>
     </row>
     <row r="32">
@@ -3135,8 +3135,8 @@
           <t>ECIWAG</t>
         </is>
       </c>
-      <c r="N32" s="48" t="n">
-        <v>45839</v>
+      <c r="N32" s="49" t="n">
+        <v>45931</v>
       </c>
       <c r="O32" s="6" t="inlineStr">
         <is>
@@ -3149,19 +3149,19 @@
         </is>
       </c>
       <c r="Q32" s="38" t="n">
+        <v>0.03362463343108507</v>
+      </c>
+      <c r="R32" s="38" t="n">
         <v>0.03584369449378332</v>
       </c>
-      <c r="R32" s="38" t="n">
+      <c r="S32" s="38" t="n">
         <v>0.03559665871121723</v>
       </c>
-      <c r="S32" s="38" t="n">
+      <c r="T32" s="38" t="n">
         <v>0.03369434416365838</v>
       </c>
-      <c r="T32" s="38" t="n">
+      <c r="U32" s="23" t="n">
         <v>0.03710462287104619</v>
-      </c>
-      <c r="U32" s="23" t="n">
-        <v>0.03746928746928743</v>
       </c>
     </row>
     <row r="33" ht="31.5" customHeight="1">
@@ -3814,8 +3814,8 @@
           <t>IQ</t>
         </is>
       </c>
-      <c r="N41" s="48" t="n">
-        <v>45962</v>
+      <c r="N41" s="49" t="n">
+        <v>45992</v>
       </c>
       <c r="O41" s="6" t="inlineStr">
         <is>
@@ -3828,19 +3828,19 @@
         </is>
       </c>
       <c r="Q41" s="38" t="n">
-        <v/>
+        <v>0.003255208333333259</v>
       </c>
       <c r="R41" s="38" t="n">
         <v/>
       </c>
       <c r="S41" s="38" t="n">
+        <v/>
+      </c>
+      <c r="T41" s="38" t="n">
         <v>0</v>
       </c>
-      <c r="T41" s="38" t="n">
+      <c r="U41" s="23" t="n">
         <v>0.00130890052356003</v>
-      </c>
-      <c r="U41" s="23" t="n">
-        <v>0.003282994090610725</v>
       </c>
     </row>
     <row r="42">
@@ -3889,8 +3889,8 @@
           <t>IQ</t>
         </is>
       </c>
-      <c r="N42" s="48" t="n">
-        <v>45962</v>
+      <c r="N42" s="49" t="n">
+        <v>45992</v>
       </c>
       <c r="O42" s="6" t="inlineStr">
         <is>
@@ -3903,19 +3903,19 @@
         </is>
       </c>
       <c r="Q42" s="38" t="n">
-        <v>0.03293010752688157</v>
+        <v>0.03076923076923073</v>
       </c>
       <c r="R42" s="38" t="n">
+        <v>0.03225806451612891</v>
+      </c>
+      <c r="S42" s="38" t="n">
         <v/>
       </c>
-      <c r="S42" s="38" t="n">
+      <c r="T42" s="38" t="n">
         <v>0.03869653767820766</v>
       </c>
-      <c r="T42" s="38" t="n">
+      <c r="U42" s="23" t="n">
         <v>0.03238866396761141</v>
-      </c>
-      <c r="U42" s="23" t="n">
-        <v>0.0241286863270779</v>
       </c>
     </row>
     <row r="43">
@@ -3964,8 +3964,8 @@
           <t>IR</t>
         </is>
       </c>
-      <c r="N43" s="48" t="n">
-        <v>45962</v>
+      <c r="N43" s="49" t="n">
+        <v>45992</v>
       </c>
       <c r="O43" s="6" t="inlineStr">
         <is>
@@ -3978,19 +3978,19 @@
         </is>
       </c>
       <c r="Q43" s="38" t="n">
-        <v/>
+        <v>0.00141643059490093</v>
       </c>
       <c r="R43" s="38" t="n">
         <v/>
       </c>
       <c r="S43" s="38" t="n">
-        <v>-0.0007092198581559739</v>
+        <v/>
       </c>
       <c r="T43" s="38" t="n">
+        <v>-0.001418439716311948</v>
+      </c>
+      <c r="U43" s="23" t="n">
         <v>-0.001416430594900819</v>
-      </c>
-      <c r="U43" s="23" t="n">
-        <v>0.00284090909090895</v>
       </c>
     </row>
     <row r="44">
@@ -4039,8 +4039,8 @@
           <t>IR</t>
         </is>
       </c>
-      <c r="N44" s="48" t="n">
-        <v>45962</v>
+      <c r="N44" s="49" t="n">
+        <v>45992</v>
       </c>
       <c r="O44" s="6" t="inlineStr">
         <is>
@@ -4053,19 +4053,19 @@
         </is>
       </c>
       <c r="Q44" s="38" t="n">
-        <v>0.0007077140835102215</v>
+        <v>0</v>
       </c>
       <c r="R44" s="38" t="n">
+        <v>-0.0007077140835104227</v>
+      </c>
+      <c r="S44" s="38" t="n">
         <v/>
       </c>
-      <c r="S44" s="38" t="n">
-        <v>0</v>
-      </c>
       <c r="T44" s="38" t="n">
+        <v>-0.0007097232079488595</v>
+      </c>
+      <c r="U44" s="23" t="n">
         <v>-0.002828854314002869</v>
-      </c>
-      <c r="U44" s="23" t="n">
-        <v>-0.004231311706629215</v>
       </c>
     </row>
     <row r="45">
@@ -4253,7 +4253,7 @@
         </is>
       </c>
       <c r="N47" s="49" t="n">
-        <v>46058</v>
+        <v>46059</v>
       </c>
       <c r="O47" s="6" t="inlineStr">
         <is>
@@ -4332,7 +4332,7 @@
         </is>
       </c>
       <c r="N48" s="49" t="n">
-        <v>46058</v>
+        <v>46059</v>
       </c>
       <c r="O48" s="6" t="inlineStr">
         <is>
@@ -4345,10 +4345,10 @@
         </is>
       </c>
       <c r="Q48" s="6" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="R48" s="6" t="n">
         <v>3.47</v>
-      </c>
-      <c r="R48" s="6" t="n">
-        <v>3.57</v>
       </c>
       <c r="S48" s="6" t="n">
         <v>3.57</v>
@@ -4357,7 +4357,7 @@
         <v>3.57</v>
       </c>
       <c r="U48" s="21" t="n">
-        <v>3.52</v>
+        <v>3.57</v>
       </c>
     </row>
     <row r="49">
@@ -4407,7 +4407,7 @@
         </is>
       </c>
       <c r="N49" s="49" t="n">
-        <v>46058</v>
+        <v>46059</v>
       </c>
       <c r="O49" s="6" t="inlineStr">
         <is>
@@ -4420,10 +4420,10 @@
         </is>
       </c>
       <c r="Q49" s="6" t="n">
+        <v>3.76</v>
+      </c>
+      <c r="R49" s="6" t="n">
         <v>3.74</v>
-      </c>
-      <c r="R49" s="6" t="n">
-        <v>3.83</v>
       </c>
       <c r="S49" s="6" t="n">
         <v>3.83</v>
@@ -4432,7 +4432,7 @@
         <v>3.83</v>
       </c>
       <c r="U49" s="21" t="n">
-        <v>3.79</v>
+        <v>3.83</v>
       </c>
     </row>
     <row r="50">
@@ -4486,7 +4486,7 @@
         </is>
       </c>
       <c r="N50" s="49" t="n">
-        <v>46058</v>
+        <v>46059</v>
       </c>
       <c r="O50" s="6" t="inlineStr">
         <is>
@@ -4499,19 +4499,19 @@
         </is>
       </c>
       <c r="Q50" s="6" t="n">
+        <v>4.22</v>
+      </c>
+      <c r="R50" s="6" t="n">
         <v>4.21</v>
       </c>
-      <c r="R50" s="6" t="n">
+      <c r="S50" s="6" t="n">
         <v>4.29</v>
       </c>
-      <c r="S50" s="6" t="n">
+      <c r="T50" s="6" t="n">
         <v>4.28</v>
       </c>
-      <c r="T50" s="6" t="n">
+      <c r="U50" s="21" t="n">
         <v>4.29</v>
-      </c>
-      <c r="U50" s="21" t="n">
-        <v>4.26</v>
       </c>
     </row>
     <row r="51" ht="31.5" customHeight="1">
@@ -4612,7 +4612,7 @@
         </is>
       </c>
       <c r="N52" s="50" t="n">
-        <v>46058</v>
+        <v>46059</v>
       </c>
       <c r="O52" s="9" t="inlineStr">
         <is>
@@ -4625,19 +4625,19 @@
         </is>
       </c>
       <c r="Q52" s="9" t="n">
+        <v>5.87</v>
+      </c>
+      <c r="R52" s="9" t="n">
         <v>5.88</v>
       </c>
-      <c r="R52" s="9" t="n">
+      <c r="S52" s="9" t="n">
         <v>5.93</v>
       </c>
-      <c r="S52" s="9" t="n">
+      <c r="T52" s="9" t="n">
         <v>5.91</v>
       </c>
-      <c r="T52" s="9" t="n">
+      <c r="U52" s="22" t="n">
         <v>5.9</v>
-      </c>
-      <c r="U52" s="22" t="n">
-        <v>5.88</v>
       </c>
     </row>
     <row r="53" ht="21" customHeight="1">

</xml_diff>

<commit_message>
Update dashboards - 2026-02-11
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -933,8 +933,8 @@
           <t>PAYEMS</t>
         </is>
       </c>
-      <c r="N3" s="48" t="n">
-        <v>45992</v>
+      <c r="N3" s="49" t="n">
+        <v>46023</v>
       </c>
       <c r="O3" s="6" t="inlineStr">
         <is>
@@ -947,19 +947,19 @@
         </is>
       </c>
       <c r="Q3" s="24" t="n">
-        <v>50</v>
+        <v>130</v>
       </c>
       <c r="R3" s="24" t="n">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="S3" s="24" t="n">
-        <v>-173</v>
+        <v>41</v>
       </c>
       <c r="T3" s="24" t="n">
-        <v>108</v>
+        <v>-140</v>
       </c>
       <c r="U3" s="26" t="n">
-        <v>-26</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4">
@@ -1004,8 +1004,8 @@
           <t>PAYEMS</t>
         </is>
       </c>
-      <c r="N4" s="48" t="n">
-        <v>45992</v>
+      <c r="N4" s="49" t="n">
+        <v>46023</v>
       </c>
       <c r="O4" s="6" t="inlineStr">
         <is>
@@ -1018,19 +1018,19 @@
         </is>
       </c>
       <c r="Q4" s="38" t="n">
-        <v>0.003674296284179135</v>
+        <v>0.002268304395076705</v>
       </c>
       <c r="R4" s="38" t="n">
-        <v>0.005402883639412681</v>
+        <v>0.001143283054144875</v>
       </c>
       <c r="S4" s="38" t="n">
-        <v>0.006706323646421399</v>
+        <v>0.002340601850973247</v>
       </c>
       <c r="T4" s="38" t="n">
-        <v>0.008078881210758367</v>
+        <v>0.002931400170945582</v>
       </c>
       <c r="U4" s="23" t="n">
-        <v>0.008926199121930236</v>
+        <v>0.004027559653477886</v>
       </c>
     </row>
     <row r="5" ht="31.5" customHeight="1">
@@ -1083,7 +1083,7 @@
           <t>ADPMNUSNERSA</t>
         </is>
       </c>
-      <c r="N5" s="49" t="n">
+      <c r="N5" s="48" t="n">
         <v>46023</v>
       </c>
       <c r="O5" s="6" t="inlineStr">
@@ -1158,8 +1158,8 @@
           <t>UNRATE</t>
         </is>
       </c>
-      <c r="N6" s="48" t="n">
-        <v>45992</v>
+      <c r="N6" s="49" t="n">
+        <v>46023</v>
       </c>
       <c r="O6" s="6" t="inlineStr">
         <is>
@@ -1172,19 +1172,19 @@
         </is>
       </c>
       <c r="Q6" s="6" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="R6" s="6" t="n">
         <v>4.4</v>
       </c>
-      <c r="R6" s="6" t="n">
+      <c r="S6" s="6" t="n">
         <v>4.5</v>
       </c>
-      <c r="S6" s="6" t="n">
+      <c r="T6" s="6" t="n">
         <v/>
       </c>
-      <c r="T6" s="6" t="n">
+      <c r="U6" s="21" t="n">
         <v>4.4</v>
-      </c>
-      <c r="U6" s="21" t="n">
-        <v>4.3</v>
       </c>
     </row>
     <row r="7" ht="16.15" customHeight="1">
@@ -1237,8 +1237,8 @@
           <t>U6RATE</t>
         </is>
       </c>
-      <c r="N7" s="48" t="n">
-        <v>45992</v>
+      <c r="N7" s="49" t="n">
+        <v>46023</v>
       </c>
       <c r="O7" s="6" t="inlineStr">
         <is>
@@ -1251,16 +1251,16 @@
         </is>
       </c>
       <c r="Q7" s="6" t="n">
+        <v>8</v>
+      </c>
+      <c r="R7" s="6" t="n">
         <v>8.4</v>
       </c>
-      <c r="R7" s="6" t="n">
+      <c r="S7" s="6" t="n">
         <v>8.699999999999999</v>
       </c>
-      <c r="S7" s="6" t="n">
+      <c r="T7" s="6" t="n">
         <v/>
-      </c>
-      <c r="T7" s="6" t="n">
-        <v>8.1</v>
       </c>
       <c r="U7" s="21" t="n">
         <v>8.1</v>
@@ -1316,8 +1316,8 @@
           <t>CIVPART</t>
         </is>
       </c>
-      <c r="N8" s="48" t="n">
-        <v>45992</v>
+      <c r="N8" s="49" t="n">
+        <v>46023</v>
       </c>
       <c r="O8" s="6" t="inlineStr">
         <is>
@@ -1330,19 +1330,19 @@
         </is>
       </c>
       <c r="Q8" s="6" t="n">
+        <v>62.5</v>
+      </c>
+      <c r="R8" s="6" t="n">
         <v>62.4</v>
       </c>
-      <c r="R8" s="6" t="n">
+      <c r="S8" s="6" t="n">
         <v>62.5</v>
       </c>
-      <c r="S8" s="6" t="n">
+      <c r="T8" s="6" t="n">
         <v/>
       </c>
-      <c r="T8" s="6" t="n">
+      <c r="U8" s="21" t="n">
         <v>62.5</v>
-      </c>
-      <c r="U8" s="21" t="n">
-        <v>62.3</v>
       </c>
     </row>
     <row r="9">
@@ -1395,8 +1395,8 @@
           <t>EMRATIO</t>
         </is>
       </c>
-      <c r="N9" s="48" t="n">
-        <v>45992</v>
+      <c r="N9" s="49" t="n">
+        <v>46023</v>
       </c>
       <c r="O9" s="6" t="inlineStr">
         <is>
@@ -1409,19 +1409,19 @@
         </is>
       </c>
       <c r="Q9" s="6" t="n">
+        <v>59.8</v>
+      </c>
+      <c r="R9" s="6" t="n">
         <v>59.7</v>
       </c>
-      <c r="R9" s="6" t="n">
+      <c r="S9" s="6" t="n">
         <v>59.6</v>
       </c>
-      <c r="S9" s="6" t="n">
+      <c r="T9" s="6" t="n">
         <v/>
       </c>
-      <c r="T9" s="6" t="n">
+      <c r="U9" s="21" t="n">
         <v>59.7</v>
-      </c>
-      <c r="U9" s="21" t="n">
-        <v>59.6</v>
       </c>
     </row>
     <row r="10">
@@ -1857,8 +1857,8 @@
           <t>AWHAETP</t>
         </is>
       </c>
-      <c r="N15" s="48" t="n">
-        <v>45992</v>
+      <c r="N15" s="49" t="n">
+        <v>46023</v>
       </c>
       <c r="O15" s="6" t="inlineStr">
         <is>
@@ -1871,13 +1871,13 @@
         </is>
       </c>
       <c r="Q15" s="24" t="n">
+        <v>34.3</v>
+      </c>
+      <c r="R15" s="24" t="n">
         <v>34.2</v>
       </c>
-      <c r="R15" s="24" t="n">
+      <c r="S15" s="24" t="n">
         <v>34.3</v>
-      </c>
-      <c r="S15" s="24" t="n">
-        <v>34.2</v>
       </c>
       <c r="T15" s="24" t="n">
         <v>34.2</v>
@@ -2907,7 +2907,7 @@
         </is>
       </c>
       <c r="N29" s="49" t="n">
-        <v>46062</v>
+        <v>46063</v>
       </c>
       <c r="O29" s="6" t="inlineStr">
         <is>
@@ -2920,16 +2920,16 @@
         </is>
       </c>
       <c r="Q29" s="6" t="n">
+        <v>2.17</v>
+      </c>
+      <c r="R29" s="6" t="n">
         <v>2.2</v>
       </c>
-      <c r="R29" s="6" t="n">
+      <c r="S29" s="6" t="n">
         <v>2.18</v>
       </c>
-      <c r="S29" s="6" t="n">
+      <c r="T29" s="6" t="n">
         <v>2.16</v>
-      </c>
-      <c r="T29" s="6" t="n">
-        <v>2.19</v>
       </c>
       <c r="U29" s="21" t="n">
         <v>2.19</v>
@@ -2986,7 +2986,7 @@
         </is>
       </c>
       <c r="N30" s="49" t="n">
-        <v>46062</v>
+        <v>46063</v>
       </c>
       <c r="O30" s="6" t="inlineStr">
         <is>
@@ -2999,19 +2999,19 @@
         </is>
       </c>
       <c r="Q30" s="6" t="n">
+        <v>2.32</v>
+      </c>
+      <c r="R30" s="6" t="n">
         <v>2.35</v>
       </c>
-      <c r="R30" s="6" t="n">
+      <c r="S30" s="6" t="n">
         <v>2.34</v>
       </c>
-      <c r="S30" s="6" t="n">
+      <c r="T30" s="6" t="n">
         <v>2.32</v>
       </c>
-      <c r="T30" s="6" t="n">
+      <c r="U30" s="21" t="n">
         <v>2.35</v>
-      </c>
-      <c r="U30" s="21" t="n">
-        <v>2.36</v>
       </c>
     </row>
     <row r="31">
@@ -3210,8 +3210,8 @@
           <t>CES0500000003</t>
         </is>
       </c>
-      <c r="N33" s="48" t="n">
-        <v>45992</v>
+      <c r="N33" s="49" t="n">
+        <v>46023</v>
       </c>
       <c r="O33" s="6" t="inlineStr">
         <is>
@@ -3224,19 +3224,19 @@
         </is>
       </c>
       <c r="Q33" s="38" t="n">
-        <v>0.003252032520325354</v>
+        <v>0.004051863857374327</v>
       </c>
       <c r="R33" s="38" t="n">
-        <v>0.002444987775060969</v>
+        <v>0.000540540540540535</v>
       </c>
       <c r="S33" s="38" t="n">
-        <v>0.004365620736698661</v>
+        <v>0.00407055630936215</v>
       </c>
       <c r="T33" s="38" t="n">
-        <v>0.001913613996719521</v>
+        <v>0.004087193460490468</v>
       </c>
       <c r="U33" s="23" t="n">
-        <v>0.004117485588800429</v>
+        <v>0.002184598580011077</v>
       </c>
     </row>
     <row r="34" ht="31.5" customHeight="1">
@@ -3299,19 +3299,19 @@
         </is>
       </c>
       <c r="Q34" s="38" t="n">
-        <v>0.008267996311731092</v>
+        <v>0.01128441879087681</v>
       </c>
       <c r="R34" s="38" t="n">
-        <v>0.01042628043129703</v>
+        <v>0.0120947871629743</v>
       </c>
       <c r="S34" s="38" t="n">
-        <v>0.009230301788676142</v>
+        <v>0.01032118383222275</v>
       </c>
       <c r="T34" s="38" t="n">
-        <v>0.01055343698833223</v>
+        <v>0.01194571058798364</v>
       </c>
       <c r="U34" s="23" t="n">
-        <v>0.01240099690797541</v>
+        <v>0.01322369465705905</v>
       </c>
     </row>
     <row r="35" ht="31.5" customHeight="1">
@@ -3378,19 +3378,19 @@
         </is>
       </c>
       <c r="Q35" s="38" t="n">
-        <v>0.0003711201807323761</v>
+        <v>0.00199332572360067</v>
       </c>
       <c r="R35" s="38" t="n">
-        <v>0.002770616347913979</v>
+        <v>0.002492631234120024</v>
       </c>
       <c r="S35" s="38" t="n">
-        <v>-0.0006927352283296884</v>
+        <v>-0.0004224555765300897</v>
       </c>
       <c r="T35" s="38" t="n">
-        <v>0.001490702319483894</v>
+        <v>0.001486198108683112</v>
       </c>
       <c r="U35" s="23" t="n">
-        <v>0.001590026251228505</v>
+        <v>0.001310931935978976</v>
       </c>
     </row>
     <row r="36" ht="31.5" customHeight="1">
@@ -3449,19 +3449,19 @@
         </is>
       </c>
       <c r="Q36" s="38" t="n">
-        <v>0.008267996311731092</v>
+        <v>0.01128441879087681</v>
       </c>
       <c r="R36" s="38" t="n">
-        <v>0.01042628043129703</v>
+        <v>0.0120947871629743</v>
       </c>
       <c r="S36" s="38" t="n">
-        <v>0.009230301788676142</v>
+        <v>0.01032118383222275</v>
       </c>
       <c r="T36" s="38" t="n">
-        <v>0.01055343698833223</v>
+        <v>0.01194571058798364</v>
       </c>
       <c r="U36" s="23" t="n">
-        <v>0.01240099690797541</v>
+        <v>0.01322369465705905</v>
       </c>
     </row>
     <row r="37">
@@ -4253,7 +4253,7 @@
         </is>
       </c>
       <c r="N47" s="49" t="n">
-        <v>46059</v>
+        <v>46062</v>
       </c>
       <c r="O47" s="6" t="inlineStr">
         <is>
@@ -4332,7 +4332,7 @@
         </is>
       </c>
       <c r="N48" s="49" t="n">
-        <v>46059</v>
+        <v>46062</v>
       </c>
       <c r="O48" s="6" t="inlineStr">
         <is>
@@ -4345,13 +4345,13 @@
         </is>
       </c>
       <c r="Q48" s="6" t="n">
+        <v>3.48</v>
+      </c>
+      <c r="R48" s="6" t="n">
         <v>3.5</v>
       </c>
-      <c r="R48" s="6" t="n">
+      <c r="S48" s="6" t="n">
         <v>3.47</v>
-      </c>
-      <c r="S48" s="6" t="n">
-        <v>3.57</v>
       </c>
       <c r="T48" s="6" t="n">
         <v>3.57</v>
@@ -4407,7 +4407,7 @@
         </is>
       </c>
       <c r="N49" s="49" t="n">
-        <v>46059</v>
+        <v>46062</v>
       </c>
       <c r="O49" s="6" t="inlineStr">
         <is>
@@ -4420,13 +4420,13 @@
         </is>
       </c>
       <c r="Q49" s="6" t="n">
+        <v>3.75</v>
+      </c>
+      <c r="R49" s="6" t="n">
         <v>3.76</v>
       </c>
-      <c r="R49" s="6" t="n">
+      <c r="S49" s="6" t="n">
         <v>3.74</v>
-      </c>
-      <c r="S49" s="6" t="n">
-        <v>3.83</v>
       </c>
       <c r="T49" s="6" t="n">
         <v>3.83</v>
@@ -4486,7 +4486,7 @@
         </is>
       </c>
       <c r="N50" s="49" t="n">
-        <v>46059</v>
+        <v>46062</v>
       </c>
       <c r="O50" s="6" t="inlineStr">
         <is>
@@ -4502,16 +4502,16 @@
         <v>4.22</v>
       </c>
       <c r="R50" s="6" t="n">
+        <v>4.22</v>
+      </c>
+      <c r="S50" s="6" t="n">
         <v>4.21</v>
       </c>
-      <c r="S50" s="6" t="n">
+      <c r="T50" s="6" t="n">
         <v>4.29</v>
       </c>
-      <c r="T50" s="6" t="n">
+      <c r="U50" s="21" t="n">
         <v>4.28</v>
-      </c>
-      <c r="U50" s="21" t="n">
-        <v>4.29</v>
       </c>
     </row>
     <row r="51" ht="31.5" customHeight="1">
@@ -4612,7 +4612,7 @@
         </is>
       </c>
       <c r="N52" s="50" t="n">
-        <v>46059</v>
+        <v>46062</v>
       </c>
       <c r="O52" s="9" t="inlineStr">
         <is>
@@ -4625,19 +4625,19 @@
         </is>
       </c>
       <c r="Q52" s="9" t="n">
+        <v>5.86</v>
+      </c>
+      <c r="R52" s="9" t="n">
         <v>5.87</v>
       </c>
-      <c r="R52" s="9" t="n">
+      <c r="S52" s="9" t="n">
         <v>5.88</v>
       </c>
-      <c r="S52" s="9" t="n">
+      <c r="T52" s="9" t="n">
         <v>5.93</v>
       </c>
-      <c r="T52" s="9" t="n">
+      <c r="U52" s="22" t="n">
         <v>5.91</v>
-      </c>
-      <c r="U52" s="22" t="n">
-        <v>5.9</v>
       </c>
     </row>
     <row r="53" ht="21" customHeight="1">

</xml_diff>

<commit_message>
Update dashboards - 2026-02-12
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -1470,7 +1470,7 @@
           <t>JTSJOR</t>
         </is>
       </c>
-      <c r="N10" s="49" t="n">
+      <c r="N10" s="48" t="n">
         <v>45992</v>
       </c>
       <c r="O10" s="6" t="inlineStr">
@@ -1549,7 +1549,7 @@
           <t>JTSHIR</t>
         </is>
       </c>
-      <c r="N11" s="49" t="n">
+      <c r="N11" s="48" t="n">
         <v>45992</v>
       </c>
       <c r="O11" s="6" t="inlineStr">
@@ -1624,7 +1624,7 @@
           <t>JTSTSR</t>
         </is>
       </c>
-      <c r="N12" s="49" t="n">
+      <c r="N12" s="48" t="n">
         <v>45992</v>
       </c>
       <c r="O12" s="6" t="inlineStr">
@@ -1704,7 +1704,7 @@
         </is>
       </c>
       <c r="N13" s="49" t="n">
-        <v>46048</v>
+        <v>46055</v>
       </c>
       <c r="O13" s="6" t="inlineStr">
         <is>
@@ -1717,19 +1717,19 @@
         </is>
       </c>
       <c r="Q13" s="24" t="n">
-        <v>231000</v>
+        <v>227000</v>
       </c>
       <c r="R13" s="24" t="n">
+        <v>232000</v>
+      </c>
+      <c r="S13" s="24" t="n">
         <v>209000</v>
       </c>
-      <c r="S13" s="24" t="n">
+      <c r="T13" s="24" t="n">
         <v>210000</v>
       </c>
-      <c r="T13" s="24" t="n">
+      <c r="U13" s="26" t="n">
         <v>199000</v>
-      </c>
-      <c r="U13" s="26" t="n">
-        <v>207000</v>
       </c>
     </row>
     <row r="14">
@@ -1779,7 +1779,7 @@
         </is>
       </c>
       <c r="N14" s="49" t="n">
-        <v>46041</v>
+        <v>46048</v>
       </c>
       <c r="O14" s="6" t="inlineStr">
         <is>
@@ -1792,19 +1792,19 @@
         </is>
       </c>
       <c r="Q14" s="24" t="n">
-        <v>1844000</v>
+        <v>1862000</v>
       </c>
       <c r="R14" s="24" t="n">
+        <v>1841000</v>
+      </c>
+      <c r="S14" s="24" t="n">
         <v>1819000</v>
       </c>
-      <c r="S14" s="24" t="n">
+      <c r="T14" s="24" t="n">
         <v>1865000</v>
       </c>
-      <c r="T14" s="24" t="n">
+      <c r="U14" s="26" t="n">
         <v>1875000</v>
-      </c>
-      <c r="U14" s="26" t="n">
-        <v>1903000</v>
       </c>
     </row>
     <row r="15">
@@ -2907,7 +2907,7 @@
         </is>
       </c>
       <c r="N29" s="49" t="n">
-        <v>46063</v>
+        <v>46064</v>
       </c>
       <c r="O29" s="6" t="inlineStr">
         <is>
@@ -2920,19 +2920,19 @@
         </is>
       </c>
       <c r="Q29" s="6" t="n">
+        <v>2.15</v>
+      </c>
+      <c r="R29" s="6" t="n">
         <v>2.17</v>
       </c>
-      <c r="R29" s="6" t="n">
+      <c r="S29" s="6" t="n">
         <v>2.2</v>
       </c>
-      <c r="S29" s="6" t="n">
+      <c r="T29" s="6" t="n">
         <v>2.18</v>
       </c>
-      <c r="T29" s="6" t="n">
+      <c r="U29" s="21" t="n">
         <v>2.16</v>
-      </c>
-      <c r="U29" s="21" t="n">
-        <v>2.19</v>
       </c>
     </row>
     <row r="30">
@@ -2986,7 +2986,7 @@
         </is>
       </c>
       <c r="N30" s="49" t="n">
-        <v>46063</v>
+        <v>46064</v>
       </c>
       <c r="O30" s="6" t="inlineStr">
         <is>
@@ -3002,16 +3002,16 @@
         <v>2.32</v>
       </c>
       <c r="R30" s="6" t="n">
+        <v>2.32</v>
+      </c>
+      <c r="S30" s="6" t="n">
         <v>2.35</v>
       </c>
-      <c r="S30" s="6" t="n">
+      <c r="T30" s="6" t="n">
         <v>2.34</v>
       </c>
-      <c r="T30" s="6" t="n">
+      <c r="U30" s="21" t="n">
         <v>2.32</v>
-      </c>
-      <c r="U30" s="21" t="n">
-        <v>2.35</v>
       </c>
     </row>
     <row r="31">
@@ -4253,7 +4253,7 @@
         </is>
       </c>
       <c r="N47" s="49" t="n">
-        <v>46062</v>
+        <v>46063</v>
       </c>
       <c r="O47" s="6" t="inlineStr">
         <is>
@@ -4332,7 +4332,7 @@
         </is>
       </c>
       <c r="N48" s="49" t="n">
-        <v>46062</v>
+        <v>46063</v>
       </c>
       <c r="O48" s="6" t="inlineStr">
         <is>
@@ -4345,16 +4345,16 @@
         </is>
       </c>
       <c r="Q48" s="6" t="n">
+        <v>3.45</v>
+      </c>
+      <c r="R48" s="6" t="n">
         <v>3.48</v>
       </c>
-      <c r="R48" s="6" t="n">
+      <c r="S48" s="6" t="n">
         <v>3.5</v>
       </c>
-      <c r="S48" s="6" t="n">
+      <c r="T48" s="6" t="n">
         <v>3.47</v>
-      </c>
-      <c r="T48" s="6" t="n">
-        <v>3.57</v>
       </c>
       <c r="U48" s="21" t="n">
         <v>3.57</v>
@@ -4407,7 +4407,7 @@
         </is>
       </c>
       <c r="N49" s="49" t="n">
-        <v>46062</v>
+        <v>46063</v>
       </c>
       <c r="O49" s="6" t="inlineStr">
         <is>
@@ -4420,16 +4420,16 @@
         </is>
       </c>
       <c r="Q49" s="6" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="R49" s="6" t="n">
         <v>3.75</v>
       </c>
-      <c r="R49" s="6" t="n">
+      <c r="S49" s="6" t="n">
         <v>3.76</v>
       </c>
-      <c r="S49" s="6" t="n">
+      <c r="T49" s="6" t="n">
         <v>3.74</v>
-      </c>
-      <c r="T49" s="6" t="n">
-        <v>3.83</v>
       </c>
       <c r="U49" s="21" t="n">
         <v>3.83</v>
@@ -4486,7 +4486,7 @@
         </is>
       </c>
       <c r="N50" s="49" t="n">
-        <v>46062</v>
+        <v>46063</v>
       </c>
       <c r="O50" s="6" t="inlineStr">
         <is>
@@ -4499,19 +4499,19 @@
         </is>
       </c>
       <c r="Q50" s="6" t="n">
-        <v>4.22</v>
+        <v>4.16</v>
       </c>
       <c r="R50" s="6" t="n">
         <v>4.22</v>
       </c>
       <c r="S50" s="6" t="n">
+        <v>4.22</v>
+      </c>
+      <c r="T50" s="6" t="n">
         <v>4.21</v>
       </c>
-      <c r="T50" s="6" t="n">
+      <c r="U50" s="21" t="n">
         <v>4.29</v>
-      </c>
-      <c r="U50" s="21" t="n">
-        <v>4.28</v>
       </c>
     </row>
     <row r="51" ht="31.5" customHeight="1">
@@ -4560,7 +4560,7 @@
           <t>MORTGAGE30US</t>
         </is>
       </c>
-      <c r="N51" s="49" t="n">
+      <c r="N51" s="48" t="n">
         <v>46055</v>
       </c>
       <c r="O51" s="6" t="inlineStr">
@@ -4612,7 +4612,7 @@
         </is>
       </c>
       <c r="N52" s="50" t="n">
-        <v>46062</v>
+        <v>46063</v>
       </c>
       <c r="O52" s="9" t="inlineStr">
         <is>
@@ -4625,19 +4625,19 @@
         </is>
       </c>
       <c r="Q52" s="9" t="n">
+        <v>5.82</v>
+      </c>
+      <c r="R52" s="9" t="n">
         <v>5.86</v>
       </c>
-      <c r="R52" s="9" t="n">
+      <c r="S52" s="9" t="n">
         <v>5.87</v>
       </c>
-      <c r="S52" s="9" t="n">
+      <c r="T52" s="9" t="n">
         <v>5.88</v>
       </c>
-      <c r="T52" s="9" t="n">
+      <c r="U52" s="22" t="n">
         <v>5.93</v>
-      </c>
-      <c r="U52" s="22" t="n">
-        <v>5.91</v>
       </c>
     </row>
     <row r="53" ht="21" customHeight="1">

</xml_diff>

<commit_message>
Update dashboards - 2026-02-13
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -2070,8 +2070,8 @@
           <t>CPIAUCSL</t>
         </is>
       </c>
-      <c r="N18" s="48" t="n">
-        <v>45992</v>
+      <c r="N18" s="49" t="n">
+        <v>46023</v>
       </c>
       <c r="O18" s="6" t="inlineStr">
         <is>
@@ -2084,19 +2084,19 @@
         </is>
       </c>
       <c r="Q18" s="38" t="n">
-        <v>0.003073552984176775</v>
+        <v>0.00170842649932057</v>
       </c>
       <c r="R18" s="38" t="n">
-        <v/>
+        <v>0.00297788428704604</v>
       </c>
       <c r="S18" s="38" t="n">
         <v/>
       </c>
       <c r="T18" s="38" t="n">
-        <v>0.00310486015759337</v>
+        <v/>
       </c>
       <c r="U18" s="23" t="n">
-        <v>0.003824519141221616</v>
+        <v>0.002950901819104068</v>
       </c>
     </row>
     <row r="19" ht="31.5" customHeight="1">
@@ -2145,8 +2145,8 @@
           <t>CPIAUCSL</t>
         </is>
       </c>
-      <c r="N19" s="48" t="n">
-        <v>45992</v>
+      <c r="N19" s="49" t="n">
+        <v>46023</v>
       </c>
       <c r="O19" s="6" t="inlineStr">
         <is>
@@ -2159,19 +2159,19 @@
         </is>
       </c>
       <c r="Q19" s="38" t="n">
-        <v>0.02653312468710926</v>
+        <v>0.02391201432150015</v>
       </c>
       <c r="R19" s="38" t="n">
-        <v>0.0271196938527219</v>
+        <v>0.02653304114557758</v>
       </c>
       <c r="S19" s="38" t="n">
+        <v>0.02696443916493949</v>
+      </c>
+      <c r="T19" s="38" t="n">
         <v/>
       </c>
-      <c r="T19" s="38" t="n">
-        <v>0.03022699626172379</v>
-      </c>
       <c r="U19" s="23" t="n">
-        <v>0.02939219624933549</v>
+        <v>0.03022571584713336</v>
       </c>
     </row>
     <row r="20">
@@ -2220,8 +2220,8 @@
           <t>CPILFESL</t>
         </is>
       </c>
-      <c r="N20" s="48" t="n">
-        <v>45992</v>
+      <c r="N20" s="49" t="n">
+        <v>46023</v>
       </c>
       <c r="O20" s="6" t="inlineStr">
         <is>
@@ -2234,19 +2234,19 @@
         </is>
       </c>
       <c r="Q20" s="38" t="n">
-        <v>0.00239225778389951</v>
+        <v>0.002950448142634121</v>
       </c>
       <c r="R20" s="38" t="n">
-        <v/>
+        <v>0.002329002576704653</v>
       </c>
       <c r="S20" s="38" t="n">
         <v/>
       </c>
       <c r="T20" s="38" t="n">
-        <v>0.002271121582325675</v>
+        <v/>
       </c>
       <c r="U20" s="23" t="n">
-        <v>0.003459544325982167</v>
+        <v>0.002177737336973129</v>
       </c>
     </row>
     <row r="21">
@@ -2295,8 +2295,8 @@
           <t>CPILFESL</t>
         </is>
       </c>
-      <c r="N21" s="48" t="n">
-        <v>45992</v>
+      <c r="N21" s="49" t="n">
+        <v>46023</v>
       </c>
       <c r="O21" s="6" t="inlineStr">
         <is>
@@ -2309,19 +2309,19 @@
         </is>
       </c>
       <c r="Q21" s="38" t="n">
-        <v>0.02648965653766215</v>
+        <v>0.02512028782828883</v>
       </c>
       <c r="R21" s="38" t="n">
-        <v>0.02618878615332623</v>
+        <v>0.02646484707309002</v>
       </c>
       <c r="S21" s="38" t="n">
+        <v>0.02599044806094405</v>
+      </c>
+      <c r="T21" s="38" t="n">
         <v/>
       </c>
-      <c r="T21" s="38" t="n">
-        <v>0.03025542724453378</v>
-      </c>
       <c r="U21" s="23" t="n">
-        <v>0.03112190821006822</v>
+        <v>0.03019966825885779</v>
       </c>
     </row>
     <row r="22">
@@ -2335,7 +2335,7 @@
           <t>TOTALSA</t>
         </is>
       </c>
-      <c r="C22" s="49" t="n">
+      <c r="C22" s="48" t="n">
         <v>46023</v>
       </c>
       <c r="D22" s="6" t="inlineStr">
@@ -2410,7 +2410,7 @@
           <t>TOTALSA</t>
         </is>
       </c>
-      <c r="C23" s="49" t="n">
+      <c r="C23" s="48" t="n">
         <v>46023</v>
       </c>
       <c r="D23" s="6" t="inlineStr">
@@ -2484,7 +2484,7 @@
           <t>REVOLSL</t>
         </is>
       </c>
-      <c r="C24" s="49" t="n">
+      <c r="C24" s="48" t="n">
         <v>45992</v>
       </c>
       <c r="D24" s="6" t="inlineStr">
@@ -2563,7 +2563,7 @@
           <t>NONREVSL</t>
         </is>
       </c>
-      <c r="C25" s="49" t="n">
+      <c r="C25" s="48" t="n">
         <v>45992</v>
       </c>
       <c r="D25" s="6" t="inlineStr">
@@ -2907,7 +2907,7 @@
         </is>
       </c>
       <c r="N29" s="49" t="n">
-        <v>46064</v>
+        <v>46065</v>
       </c>
       <c r="O29" s="6" t="inlineStr">
         <is>
@@ -2920,19 +2920,19 @@
         </is>
       </c>
       <c r="Q29" s="6" t="n">
+        <v>2.13</v>
+      </c>
+      <c r="R29" s="6" t="n">
         <v>2.15</v>
       </c>
-      <c r="R29" s="6" t="n">
+      <c r="S29" s="6" t="n">
         <v>2.17</v>
       </c>
-      <c r="S29" s="6" t="n">
+      <c r="T29" s="6" t="n">
         <v>2.2</v>
       </c>
-      <c r="T29" s="6" t="n">
+      <c r="U29" s="21" t="n">
         <v>2.18</v>
-      </c>
-      <c r="U29" s="21" t="n">
-        <v>2.16</v>
       </c>
     </row>
     <row r="30">
@@ -2986,7 +2986,7 @@
         </is>
       </c>
       <c r="N30" s="49" t="n">
-        <v>46064</v>
+        <v>46065</v>
       </c>
       <c r="O30" s="6" t="inlineStr">
         <is>
@@ -2999,19 +2999,19 @@
         </is>
       </c>
       <c r="Q30" s="6" t="n">
-        <v>2.32</v>
+        <v>2.29</v>
       </c>
       <c r="R30" s="6" t="n">
         <v>2.32</v>
       </c>
       <c r="S30" s="6" t="n">
+        <v>2.32</v>
+      </c>
+      <c r="T30" s="6" t="n">
         <v>2.35</v>
       </c>
-      <c r="T30" s="6" t="n">
+      <c r="U30" s="21" t="n">
         <v>2.34</v>
-      </c>
-      <c r="U30" s="21" t="n">
-        <v>2.32</v>
       </c>
     </row>
     <row r="31">
@@ -3855,7 +3855,7 @@
         </is>
       </c>
       <c r="C42" s="48" t="n">
-        <v>45992</v>
+        <v>46023</v>
       </c>
       <c r="D42" s="6" t="inlineStr">
         <is>
@@ -3868,19 +3868,19 @@
         </is>
       </c>
       <c r="F42" s="39" t="n">
-        <v>4350000</v>
+        <v>3910000</v>
       </c>
       <c r="G42" s="39" t="n">
-        <v>4140000</v>
+        <v>4270000</v>
       </c>
       <c r="H42" s="39" t="n">
+        <v>4090000</v>
+      </c>
+      <c r="I42" s="39" t="n">
         <v>4110000</v>
       </c>
-      <c r="I42" s="39" t="n">
-        <v>4050000</v>
-      </c>
       <c r="J42" s="39" t="n">
-        <v>4000000</v>
+        <v>4080000</v>
       </c>
       <c r="K42" s="7" t="n"/>
       <c r="L42" s="28" t="n"/>
@@ -3926,7 +3926,7 @@
         </is>
       </c>
       <c r="C43" s="48" t="n">
-        <v>45992</v>
+        <v>46023</v>
       </c>
       <c r="D43" s="6" t="inlineStr">
         <is>
@@ -3939,7 +3939,7 @@
         </is>
       </c>
       <c r="F43" s="38" t="n">
-        <v>0.01398601398601399</v>
+        <v>-0.04400977995110025</v>
       </c>
       <c r="G43" s="38" t="n">
         <v/>
@@ -4253,7 +4253,7 @@
         </is>
       </c>
       <c r="N47" s="49" t="n">
-        <v>46063</v>
+        <v>46064</v>
       </c>
       <c r="O47" s="6" t="inlineStr">
         <is>
@@ -4332,7 +4332,7 @@
         </is>
       </c>
       <c r="N48" s="49" t="n">
-        <v>46063</v>
+        <v>46064</v>
       </c>
       <c r="O48" s="6" t="inlineStr">
         <is>
@@ -4345,19 +4345,19 @@
         </is>
       </c>
       <c r="Q48" s="6" t="n">
+        <v>3.52</v>
+      </c>
+      <c r="R48" s="6" t="n">
         <v>3.45</v>
       </c>
-      <c r="R48" s="6" t="n">
+      <c r="S48" s="6" t="n">
         <v>3.48</v>
       </c>
-      <c r="S48" s="6" t="n">
+      <c r="T48" s="6" t="n">
         <v>3.5</v>
       </c>
-      <c r="T48" s="6" t="n">
+      <c r="U48" s="21" t="n">
         <v>3.47</v>
-      </c>
-      <c r="U48" s="21" t="n">
-        <v>3.57</v>
       </c>
     </row>
     <row r="49">
@@ -4407,7 +4407,7 @@
         </is>
       </c>
       <c r="N49" s="49" t="n">
-        <v>46063</v>
+        <v>46064</v>
       </c>
       <c r="O49" s="6" t="inlineStr">
         <is>
@@ -4420,19 +4420,19 @@
         </is>
       </c>
       <c r="Q49" s="6" t="n">
+        <v>3.75</v>
+      </c>
+      <c r="R49" s="6" t="n">
         <v>3.7</v>
       </c>
-      <c r="R49" s="6" t="n">
+      <c r="S49" s="6" t="n">
         <v>3.75</v>
       </c>
-      <c r="S49" s="6" t="n">
+      <c r="T49" s="6" t="n">
         <v>3.76</v>
       </c>
-      <c r="T49" s="6" t="n">
+      <c r="U49" s="21" t="n">
         <v>3.74</v>
-      </c>
-      <c r="U49" s="21" t="n">
-        <v>3.83</v>
       </c>
     </row>
     <row r="50">
@@ -4486,7 +4486,7 @@
         </is>
       </c>
       <c r="N50" s="49" t="n">
-        <v>46063</v>
+        <v>46064</v>
       </c>
       <c r="O50" s="6" t="inlineStr">
         <is>
@@ -4499,19 +4499,19 @@
         </is>
       </c>
       <c r="Q50" s="6" t="n">
+        <v>4.18</v>
+      </c>
+      <c r="R50" s="6" t="n">
         <v>4.16</v>
-      </c>
-      <c r="R50" s="6" t="n">
-        <v>4.22</v>
       </c>
       <c r="S50" s="6" t="n">
         <v>4.22</v>
       </c>
       <c r="T50" s="6" t="n">
+        <v>4.22</v>
+      </c>
+      <c r="U50" s="21" t="n">
         <v>4.21</v>
-      </c>
-      <c r="U50" s="21" t="n">
-        <v>4.29</v>
       </c>
     </row>
     <row r="51" ht="31.5" customHeight="1">
@@ -4560,8 +4560,8 @@
           <t>MORTGAGE30US</t>
         </is>
       </c>
-      <c r="N51" s="48" t="n">
-        <v>46055</v>
+      <c r="N51" s="49" t="n">
+        <v>46062</v>
       </c>
       <c r="O51" s="6" t="inlineStr">
         <is>
@@ -4574,19 +4574,19 @@
         </is>
       </c>
       <c r="Q51" s="6" t="n">
+        <v>6.09</v>
+      </c>
+      <c r="R51" s="6" t="n">
         <v>6.11</v>
       </c>
-      <c r="R51" s="6" t="n">
+      <c r="S51" s="6" t="n">
         <v>6.1</v>
       </c>
-      <c r="S51" s="6" t="n">
+      <c r="T51" s="6" t="n">
         <v>6.09</v>
       </c>
-      <c r="T51" s="6" t="n">
+      <c r="U51" s="21" t="n">
         <v>6.06</v>
-      </c>
-      <c r="U51" s="21" t="n">
-        <v>6.16</v>
       </c>
     </row>
     <row r="52" ht="16.15" customHeight="1" thickBot="1">
@@ -4612,7 +4612,7 @@
         </is>
       </c>
       <c r="N52" s="50" t="n">
-        <v>46063</v>
+        <v>46064</v>
       </c>
       <c r="O52" s="9" t="inlineStr">
         <is>
@@ -4625,19 +4625,19 @@
         </is>
       </c>
       <c r="Q52" s="9" t="n">
+        <v>5.85</v>
+      </c>
+      <c r="R52" s="9" t="n">
         <v>5.82</v>
       </c>
-      <c r="R52" s="9" t="n">
+      <c r="S52" s="9" t="n">
         <v>5.86</v>
       </c>
-      <c r="S52" s="9" t="n">
+      <c r="T52" s="9" t="n">
         <v>5.87</v>
       </c>
-      <c r="T52" s="9" t="n">
+      <c r="U52" s="22" t="n">
         <v>5.88</v>
-      </c>
-      <c r="U52" s="22" t="n">
-        <v>5.93</v>
       </c>
     </row>
     <row r="53" ht="21" customHeight="1">

</xml_diff>

<commit_message>
Update dashboards - 2026-02-14
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -2907,7 +2907,7 @@
         </is>
       </c>
       <c r="N29" s="49" t="n">
-        <v>46065</v>
+        <v>46066</v>
       </c>
       <c r="O29" s="6" t="inlineStr">
         <is>
@@ -2920,19 +2920,19 @@
         </is>
       </c>
       <c r="Q29" s="6" t="n">
+        <v>2.12</v>
+      </c>
+      <c r="R29" s="6" t="n">
         <v>2.13</v>
       </c>
-      <c r="R29" s="6" t="n">
+      <c r="S29" s="6" t="n">
         <v>2.15</v>
       </c>
-      <c r="S29" s="6" t="n">
+      <c r="T29" s="6" t="n">
         <v>2.17</v>
       </c>
-      <c r="T29" s="6" t="n">
+      <c r="U29" s="21" t="n">
         <v>2.2</v>
-      </c>
-      <c r="U29" s="21" t="n">
-        <v>2.18</v>
       </c>
     </row>
     <row r="30">
@@ -2986,7 +2986,7 @@
         </is>
       </c>
       <c r="N30" s="49" t="n">
-        <v>46065</v>
+        <v>46066</v>
       </c>
       <c r="O30" s="6" t="inlineStr">
         <is>
@@ -2999,19 +2999,19 @@
         </is>
       </c>
       <c r="Q30" s="6" t="n">
+        <v>2.27</v>
+      </c>
+      <c r="R30" s="6" t="n">
         <v>2.29</v>
-      </c>
-      <c r="R30" s="6" t="n">
-        <v>2.32</v>
       </c>
       <c r="S30" s="6" t="n">
         <v>2.32</v>
       </c>
       <c r="T30" s="6" t="n">
+        <v>2.32</v>
+      </c>
+      <c r="U30" s="21" t="n">
         <v>2.35</v>
-      </c>
-      <c r="U30" s="21" t="n">
-        <v>2.34</v>
       </c>
     </row>
     <row r="31">
@@ -4253,7 +4253,7 @@
         </is>
       </c>
       <c r="N47" s="49" t="n">
-        <v>46064</v>
+        <v>46065</v>
       </c>
       <c r="O47" s="6" t="inlineStr">
         <is>
@@ -4332,7 +4332,7 @@
         </is>
       </c>
       <c r="N48" s="49" t="n">
-        <v>46064</v>
+        <v>46065</v>
       </c>
       <c r="O48" s="6" t="inlineStr">
         <is>
@@ -4345,19 +4345,19 @@
         </is>
       </c>
       <c r="Q48" s="6" t="n">
+        <v>3.47</v>
+      </c>
+      <c r="R48" s="6" t="n">
         <v>3.52</v>
       </c>
-      <c r="R48" s="6" t="n">
+      <c r="S48" s="6" t="n">
         <v>3.45</v>
       </c>
-      <c r="S48" s="6" t="n">
+      <c r="T48" s="6" t="n">
         <v>3.48</v>
       </c>
-      <c r="T48" s="6" t="n">
+      <c r="U48" s="21" t="n">
         <v>3.5</v>
-      </c>
-      <c r="U48" s="21" t="n">
-        <v>3.47</v>
       </c>
     </row>
     <row r="49">
@@ -4407,7 +4407,7 @@
         </is>
       </c>
       <c r="N49" s="49" t="n">
-        <v>46064</v>
+        <v>46065</v>
       </c>
       <c r="O49" s="6" t="inlineStr">
         <is>
@@ -4420,19 +4420,19 @@
         </is>
       </c>
       <c r="Q49" s="6" t="n">
+        <v>3.67</v>
+      </c>
+      <c r="R49" s="6" t="n">
         <v>3.75</v>
       </c>
-      <c r="R49" s="6" t="n">
+      <c r="S49" s="6" t="n">
         <v>3.7</v>
       </c>
-      <c r="S49" s="6" t="n">
+      <c r="T49" s="6" t="n">
         <v>3.75</v>
       </c>
-      <c r="T49" s="6" t="n">
+      <c r="U49" s="21" t="n">
         <v>3.76</v>
-      </c>
-      <c r="U49" s="21" t="n">
-        <v>3.74</v>
       </c>
     </row>
     <row r="50">
@@ -4486,7 +4486,7 @@
         </is>
       </c>
       <c r="N50" s="49" t="n">
-        <v>46064</v>
+        <v>46065</v>
       </c>
       <c r="O50" s="6" t="inlineStr">
         <is>
@@ -4499,19 +4499,19 @@
         </is>
       </c>
       <c r="Q50" s="6" t="n">
+        <v>4.09</v>
+      </c>
+      <c r="R50" s="6" t="n">
         <v>4.18</v>
       </c>
-      <c r="R50" s="6" t="n">
+      <c r="S50" s="6" t="n">
         <v>4.16</v>
-      </c>
-      <c r="S50" s="6" t="n">
-        <v>4.22</v>
       </c>
       <c r="T50" s="6" t="n">
         <v>4.22</v>
       </c>
       <c r="U50" s="21" t="n">
-        <v>4.21</v>
+        <v>4.22</v>
       </c>
     </row>
     <row r="51" ht="31.5" customHeight="1">
@@ -4612,7 +4612,7 @@
         </is>
       </c>
       <c r="N52" s="50" t="n">
-        <v>46064</v>
+        <v>46065</v>
       </c>
       <c r="O52" s="9" t="inlineStr">
         <is>
@@ -4625,19 +4625,19 @@
         </is>
       </c>
       <c r="Q52" s="9" t="n">
+        <v>5.77</v>
+      </c>
+      <c r="R52" s="9" t="n">
         <v>5.85</v>
       </c>
-      <c r="R52" s="9" t="n">
+      <c r="S52" s="9" t="n">
         <v>5.82</v>
       </c>
-      <c r="S52" s="9" t="n">
+      <c r="T52" s="9" t="n">
         <v>5.86</v>
       </c>
-      <c r="T52" s="9" t="n">
+      <c r="U52" s="22" t="n">
         <v>5.87</v>
-      </c>
-      <c r="U52" s="22" t="n">
-        <v>5.88</v>
       </c>
     </row>
     <row r="53" ht="21" customHeight="1">

</xml_diff>

<commit_message>
Update dashboards - 2026-02-17
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -1944,7 +1944,7 @@
           <t>RSAFS</t>
         </is>
       </c>
-      <c r="C17" s="49" t="n">
+      <c r="C17" s="48" t="n">
         <v>45992</v>
       </c>
       <c r="D17" s="6" t="inlineStr">
@@ -2031,7 +2031,7 @@
           <t>RSAFS</t>
         </is>
       </c>
-      <c r="C18" s="49" t="n">
+      <c r="C18" s="48" t="n">
         <v>45992</v>
       </c>
       <c r="D18" s="6" t="inlineStr">
@@ -3060,7 +3060,7 @@
           <t>ECIWAG</t>
         </is>
       </c>
-      <c r="N31" s="49" t="n">
+      <c r="N31" s="48" t="n">
         <v>45931</v>
       </c>
       <c r="O31" s="6" t="inlineStr">
@@ -3135,7 +3135,7 @@
           <t>ECIWAG</t>
         </is>
       </c>
-      <c r="N32" s="49" t="n">
+      <c r="N32" s="48" t="n">
         <v>45931</v>
       </c>
       <c r="O32" s="6" t="inlineStr">
@@ -3814,7 +3814,7 @@
           <t>IQ</t>
         </is>
       </c>
-      <c r="N41" s="49" t="n">
+      <c r="N41" s="48" t="n">
         <v>45992</v>
       </c>
       <c r="O41" s="6" t="inlineStr">
@@ -3889,7 +3889,7 @@
           <t>IQ</t>
         </is>
       </c>
-      <c r="N42" s="49" t="n">
+      <c r="N42" s="48" t="n">
         <v>45992</v>
       </c>
       <c r="O42" s="6" t="inlineStr">
@@ -3964,7 +3964,7 @@
           <t>IR</t>
         </is>
       </c>
-      <c r="N43" s="49" t="n">
+      <c r="N43" s="48" t="n">
         <v>45992</v>
       </c>
       <c r="O43" s="6" t="inlineStr">
@@ -4039,7 +4039,7 @@
           <t>IR</t>
         </is>
       </c>
-      <c r="N44" s="49" t="n">
+      <c r="N44" s="48" t="n">
         <v>45992</v>
       </c>
       <c r="O44" s="6" t="inlineStr">

</xml_diff>

<commit_message>
Update dashboards - 2026-02-18
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -933,7 +933,7 @@
           <t>PAYEMS</t>
         </is>
       </c>
-      <c r="N3" s="49" t="n">
+      <c r="N3" s="48" t="n">
         <v>46023</v>
       </c>
       <c r="O3" s="6" t="inlineStr">
@@ -1004,7 +1004,7 @@
           <t>PAYEMS</t>
         </is>
       </c>
-      <c r="N4" s="49" t="n">
+      <c r="N4" s="48" t="n">
         <v>46023</v>
       </c>
       <c r="O4" s="6" t="inlineStr">
@@ -1158,7 +1158,7 @@
           <t>UNRATE</t>
         </is>
       </c>
-      <c r="N6" s="49" t="n">
+      <c r="N6" s="48" t="n">
         <v>46023</v>
       </c>
       <c r="O6" s="6" t="inlineStr">
@@ -1237,7 +1237,7 @@
           <t>U6RATE</t>
         </is>
       </c>
-      <c r="N7" s="49" t="n">
+      <c r="N7" s="48" t="n">
         <v>46023</v>
       </c>
       <c r="O7" s="6" t="inlineStr">
@@ -1316,7 +1316,7 @@
           <t>CIVPART</t>
         </is>
       </c>
-      <c r="N8" s="49" t="n">
+      <c r="N8" s="48" t="n">
         <v>46023</v>
       </c>
       <c r="O8" s="6" t="inlineStr">
@@ -1395,7 +1395,7 @@
           <t>EMRATIO</t>
         </is>
       </c>
-      <c r="N9" s="49" t="n">
+      <c r="N9" s="48" t="n">
         <v>46023</v>
       </c>
       <c r="O9" s="6" t="inlineStr">
@@ -1857,7 +1857,7 @@
           <t>AWHAETP</t>
         </is>
       </c>
-      <c r="N15" s="49" t="n">
+      <c r="N15" s="48" t="n">
         <v>46023</v>
       </c>
       <c r="O15" s="6" t="inlineStr">
@@ -2792,8 +2792,8 @@
           <t>DGORDER</t>
         </is>
       </c>
-      <c r="C28" s="48" t="n">
-        <v>45962</v>
+      <c r="C28" s="49" t="n">
+        <v>45992</v>
       </c>
       <c r="D28" s="6" t="inlineStr">
         <is>
@@ -2806,19 +2806,19 @@
         </is>
       </c>
       <c r="F28" s="25" t="n">
-        <v>0.0526514289430049</v>
+        <v>-0.01425751734772551</v>
       </c>
       <c r="G28" s="25" t="n">
+        <v>0.05423155704392491</v>
+      </c>
+      <c r="H28" s="25" t="n">
         <v>-0.02093605859677161</v>
       </c>
-      <c r="H28" s="25" t="n">
+      <c r="I28" s="25" t="n">
         <v>0.006436255758670795</v>
       </c>
-      <c r="I28" s="25" t="n">
+      <c r="J28" s="25" t="n">
         <v>0.03004963172206243</v>
-      </c>
-      <c r="J28" s="25" t="n">
-        <v>-0.02799901206372835</v>
       </c>
       <c r="K28" s="5" t="n"/>
       <c r="L28" s="28" t="inlineStr">
@@ -2867,8 +2867,8 @@
           <t>DGORDER</t>
         </is>
       </c>
-      <c r="C29" s="48" t="n">
-        <v>45962</v>
+      <c r="C29" s="49" t="n">
+        <v>45992</v>
       </c>
       <c r="D29" s="6" t="inlineStr">
         <is>
@@ -2881,19 +2881,19 @@
         </is>
       </c>
       <c r="F29" s="25" t="n">
-        <v>0.1228549628910314</v>
+        <v>0.1000416438657897</v>
       </c>
       <c r="G29" s="25" t="n">
+        <v>0.1245404730526462</v>
+      </c>
+      <c r="H29" s="25" t="n">
         <v>0.04877483240471108</v>
       </c>
-      <c r="H29" s="25" t="n">
+      <c r="I29" s="25" t="n">
         <v>0.07412067603746038</v>
       </c>
-      <c r="I29" s="25" t="n">
+      <c r="J29" s="25" t="n">
         <v>0.07661265288383932</v>
-      </c>
-      <c r="J29" s="25" t="n">
-        <v>0.03341358778313566</v>
       </c>
       <c r="K29" s="5" t="n"/>
       <c r="L29" s="28" t="inlineStr">
@@ -2907,7 +2907,7 @@
         </is>
       </c>
       <c r="N29" s="49" t="n">
-        <v>46066</v>
+        <v>46070</v>
       </c>
       <c r="O29" s="6" t="inlineStr">
         <is>
@@ -2920,19 +2920,19 @@
         </is>
       </c>
       <c r="Q29" s="6" t="n">
+        <v>2.13</v>
+      </c>
+      <c r="R29" s="6" t="n">
         <v>2.12</v>
       </c>
-      <c r="R29" s="6" t="n">
+      <c r="S29" s="6" t="n">
         <v>2.13</v>
       </c>
-      <c r="S29" s="6" t="n">
+      <c r="T29" s="6" t="n">
         <v>2.15</v>
       </c>
-      <c r="T29" s="6" t="n">
+      <c r="U29" s="21" t="n">
         <v>2.17</v>
-      </c>
-      <c r="U29" s="21" t="n">
-        <v>2.2</v>
       </c>
     </row>
     <row r="30">
@@ -2946,8 +2946,8 @@
           <t>ADXDNO</t>
         </is>
       </c>
-      <c r="C30" s="48" t="n">
-        <v>45962</v>
+      <c r="C30" s="49" t="n">
+        <v>45992</v>
       </c>
       <c r="D30" s="6" t="inlineStr">
         <is>
@@ -2960,19 +2960,19 @@
         </is>
       </c>
       <c r="F30" s="25" t="n">
-        <v>0.06490461658514834</v>
+        <v>-0.02458405517602069</v>
       </c>
       <c r="G30" s="25" t="n">
+        <v>0.06576508785864577</v>
+      </c>
+      <c r="H30" s="25" t="n">
         <v>-0.0128376635658648</v>
       </c>
-      <c r="H30" s="25" t="n">
+      <c r="I30" s="25" t="n">
         <v>0.001174064535676367</v>
       </c>
-      <c r="I30" s="25" t="n">
+      <c r="J30" s="25" t="n">
         <v>0.01907672443132968</v>
-      </c>
-      <c r="J30" s="25" t="n">
-        <v>-0.02404555711932721</v>
       </c>
       <c r="K30" s="5" t="n"/>
       <c r="L30" s="28" t="inlineStr">
@@ -2986,7 +2986,7 @@
         </is>
       </c>
       <c r="N30" s="49" t="n">
-        <v>46066</v>
+        <v>46070</v>
       </c>
       <c r="O30" s="6" t="inlineStr">
         <is>
@@ -2999,19 +2999,19 @@
         </is>
       </c>
       <c r="Q30" s="6" t="n">
+        <v>2.26</v>
+      </c>
+      <c r="R30" s="6" t="n">
         <v>2.27</v>
       </c>
-      <c r="R30" s="6" t="n">
+      <c r="S30" s="6" t="n">
         <v>2.29</v>
-      </c>
-      <c r="S30" s="6" t="n">
-        <v>2.32</v>
       </c>
       <c r="T30" s="6" t="n">
         <v>2.32</v>
       </c>
       <c r="U30" s="21" t="n">
-        <v>2.35</v>
+        <v>2.32</v>
       </c>
     </row>
     <row r="31">
@@ -3021,8 +3021,8 @@
           <t>ADXDNO</t>
         </is>
       </c>
-      <c r="C31" s="48" t="n">
-        <v>45962</v>
+      <c r="C31" s="49" t="n">
+        <v>45992</v>
       </c>
       <c r="D31" s="6" t="inlineStr">
         <is>
@@ -3035,19 +3035,19 @@
         </is>
       </c>
       <c r="F31" s="25" t="n">
-        <v>0.1254482530098303</v>
+        <v>0.09489005566012468</v>
       </c>
       <c r="G31" s="25" t="n">
+        <v>0.1263576451529767</v>
+      </c>
+      <c r="H31" s="25" t="n">
         <v>0.05011084527755218</v>
       </c>
-      <c r="H31" s="25" t="n">
+      <c r="I31" s="25" t="n">
         <v>0.06502168244015354</v>
       </c>
-      <c r="I31" s="25" t="n">
+      <c r="J31" s="25" t="n">
         <v>0.06671073894520346</v>
-      </c>
-      <c r="J31" s="25" t="n">
-        <v>0.0329297153895499</v>
       </c>
       <c r="K31" s="5" t="n"/>
       <c r="L31" s="28" t="inlineStr">
@@ -3100,8 +3100,8 @@
           <t>INDPRO</t>
         </is>
       </c>
-      <c r="C32" s="48" t="n">
-        <v>45992</v>
+      <c r="C32" s="49" t="n">
+        <v>46023</v>
       </c>
       <c r="D32" s="6" t="inlineStr">
         <is>
@@ -3114,19 +3114,19 @@
         </is>
       </c>
       <c r="F32" s="25" t="n">
-        <v>0.003650708955516668</v>
+        <v>0.007001897085101128</v>
       </c>
       <c r="G32" s="25" t="n">
-        <v>0.004299802100746319</v>
+        <v>0.002486745086434317</v>
       </c>
       <c r="H32" s="25" t="n">
-        <v>-0.002570302590248041</v>
+        <v>0.001190041182338009</v>
       </c>
       <c r="I32" s="25" t="n">
-        <v>0.001882136145775037</v>
+        <v>-0.004413706579460941</v>
       </c>
       <c r="J32" s="25" t="n">
-        <v>-0.003015879247060815</v>
+        <v>0.0007990183488855163</v>
       </c>
       <c r="K32" s="5" t="n"/>
       <c r="L32" s="28" t="n"/>
@@ -3171,8 +3171,8 @@
           <t>INDPRO</t>
         </is>
       </c>
-      <c r="C33" s="48" t="n">
-        <v>45992</v>
+      <c r="C33" s="49" t="n">
+        <v>46023</v>
       </c>
       <c r="D33" s="6" t="inlineStr">
         <is>
@@ -3185,19 +3185,19 @@
         </is>
       </c>
       <c r="F33" s="25" t="n">
-        <v>0.01991182858504125</v>
+        <v>0.02275028056847218</v>
       </c>
       <c r="G33" s="25" t="n">
-        <v>0.02679255734320309</v>
+        <v>0.01298051477514099</v>
       </c>
       <c r="H33" s="25" t="n">
-        <v>0.02057716184358024</v>
+        <v>0.02099856484628742</v>
       </c>
       <c r="I33" s="25" t="n">
-        <v>0.01973280806024339</v>
+        <v>0.01797033261452011</v>
       </c>
       <c r="J33" s="25" t="n">
-        <v>0.01150841026018884</v>
+        <v>0.01901142589200902</v>
       </c>
       <c r="K33" s="5" t="n"/>
       <c r="L33" s="28" t="inlineStr">
@@ -3210,7 +3210,7 @@
           <t>CES0500000003</t>
         </is>
       </c>
-      <c r="N33" s="49" t="n">
+      <c r="N33" s="48" t="n">
         <v>46023</v>
       </c>
       <c r="O33" s="6" t="inlineStr">
@@ -3250,8 +3250,8 @@
           <t>TCU</t>
         </is>
       </c>
-      <c r="C34" s="48" t="n">
-        <v>45992</v>
+      <c r="C34" s="49" t="n">
+        <v>46023</v>
       </c>
       <c r="D34" s="6" t="inlineStr">
         <is>
@@ -3264,19 +3264,19 @@
         </is>
       </c>
       <c r="F34" s="24" t="n">
-        <v>76.2615</v>
+        <v>76.2119</v>
       </c>
       <c r="G34" s="24" t="n">
-        <v>76.07550000000001</v>
+        <v>75.7433</v>
       </c>
       <c r="H34" s="24" t="n">
-        <v>75.8411</v>
+        <v>75.64619999999999</v>
       </c>
       <c r="I34" s="24" t="n">
-        <v>76.1283</v>
+        <v>75.6474</v>
       </c>
       <c r="J34" s="24" t="n">
-        <v>76.077</v>
+        <v>76.0745</v>
       </c>
       <c r="K34" s="5" t="n"/>
       <c r="L34" s="28" t="n"/>
@@ -3400,8 +3400,8 @@
           <t>HOUST</t>
         </is>
       </c>
-      <c r="C36" s="48" t="n">
-        <v>45931</v>
+      <c r="C36" s="49" t="n">
+        <v>45992</v>
       </c>
       <c r="D36" s="6" t="inlineStr">
         <is>
@@ -3414,19 +3414,19 @@
         </is>
       </c>
       <c r="F36" s="24" t="n">
-        <v>1246</v>
+        <v>1404</v>
       </c>
       <c r="G36" s="24" t="n">
-        <v>1306</v>
+        <v>1322</v>
       </c>
       <c r="H36" s="24" t="n">
+        <v>1272</v>
+      </c>
+      <c r="I36" s="24" t="n">
+        <v>1328</v>
+      </c>
+      <c r="J36" s="24" t="n">
         <v>1291</v>
-      </c>
-      <c r="I36" s="24" t="n">
-        <v>1420</v>
-      </c>
-      <c r="J36" s="24" t="n">
-        <v>1382</v>
       </c>
       <c r="K36" s="5" t="n"/>
       <c r="L36" s="28" t="n"/>
@@ -3475,8 +3475,8 @@
           <t>HOUST</t>
         </is>
       </c>
-      <c r="C37" s="48" t="n">
-        <v>45931</v>
+      <c r="C37" s="49" t="n">
+        <v>45992</v>
       </c>
       <c r="D37" s="6" t="inlineStr">
         <is>
@@ -3489,19 +3489,19 @@
         </is>
       </c>
       <c r="F37" s="25" t="n">
-        <v>-0.07840236686390532</v>
+        <v>-0.0726552179656539</v>
       </c>
       <c r="G37" s="25" t="n">
-        <v>-0.03758290346352248</v>
+        <v>0.02084942084942085</v>
       </c>
       <c r="H37" s="25" t="n">
+        <v>-0.05917159763313609</v>
+      </c>
+      <c r="I37" s="25" t="n">
+        <v>-0.02137067059690494</v>
+      </c>
+      <c r="J37" s="25" t="n">
         <v>-0.07189072609633357</v>
-      </c>
-      <c r="I37" s="25" t="n">
-        <v>0.1225296442687747</v>
-      </c>
-      <c r="J37" s="25" t="n">
-        <v>0.04144687264506405</v>
       </c>
       <c r="K37" s="5" t="n"/>
       <c r="L37" s="28" t="inlineStr">
@@ -3554,8 +3554,8 @@
           <t>PERMIT</t>
         </is>
       </c>
-      <c r="C38" s="48" t="n">
-        <v>45931</v>
+      <c r="C38" s="49" t="n">
+        <v>45992</v>
       </c>
       <c r="D38" s="6" t="inlineStr">
         <is>
@@ -3568,19 +3568,19 @@
         </is>
       </c>
       <c r="F38" s="24" t="n">
+        <v>1448</v>
+      </c>
+      <c r="G38" s="24" t="n">
+        <v>1388</v>
+      </c>
+      <c r="H38" s="24" t="n">
         <v>1411</v>
       </c>
-      <c r="G38" s="24" t="n">
+      <c r="I38" s="24" t="n">
         <v>1415</v>
       </c>
-      <c r="H38" s="24" t="n">
+      <c r="J38" s="24" t="n">
         <v>1330</v>
-      </c>
-      <c r="I38" s="24" t="n">
-        <v>1362</v>
-      </c>
-      <c r="J38" s="24" t="n">
-        <v>1393</v>
       </c>
       <c r="K38" s="5" t="n"/>
       <c r="L38" s="28" t="n"/>
@@ -3625,8 +3625,8 @@
           <t>PERMIT</t>
         </is>
       </c>
-      <c r="C39" s="48" t="n">
-        <v>45931</v>
+      <c r="C39" s="49" t="n">
+        <v>45992</v>
       </c>
       <c r="D39" s="6" t="inlineStr">
         <is>
@@ -3639,19 +3639,19 @@
         </is>
       </c>
       <c r="F39" s="38" t="n">
+        <v>-0.02162162162162162</v>
+      </c>
+      <c r="G39" s="38" t="n">
+        <v>-0.07957559681697612</v>
+      </c>
+      <c r="H39" s="38" t="n">
         <v>-0.0119047619047619</v>
       </c>
-      <c r="G39" s="38" t="n">
+      <c r="I39" s="38" t="n">
         <v>-0.01324965132496513</v>
       </c>
-      <c r="H39" s="38" t="n">
+      <c r="J39" s="38" t="n">
         <v>-0.0989159891598916</v>
-      </c>
-      <c r="I39" s="38" t="n">
-        <v>-0.05153203342618384</v>
-      </c>
-      <c r="J39" s="38" t="n">
-        <v>-0.04654346338124572</v>
       </c>
       <c r="K39" s="5" t="n"/>
       <c r="L39" s="28" t="inlineStr">
@@ -4253,7 +4253,7 @@
         </is>
       </c>
       <c r="N47" s="49" t="n">
-        <v>46065</v>
+        <v>46069</v>
       </c>
       <c r="O47" s="6" t="inlineStr">
         <is>
@@ -4332,7 +4332,7 @@
         </is>
       </c>
       <c r="N48" s="49" t="n">
-        <v>46065</v>
+        <v>46066</v>
       </c>
       <c r="O48" s="6" t="inlineStr">
         <is>
@@ -4345,19 +4345,19 @@
         </is>
       </c>
       <c r="Q48" s="6" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="R48" s="6" t="n">
         <v>3.47</v>
       </c>
-      <c r="R48" s="6" t="n">
+      <c r="S48" s="6" t="n">
         <v>3.52</v>
       </c>
-      <c r="S48" s="6" t="n">
+      <c r="T48" s="6" t="n">
         <v>3.45</v>
       </c>
-      <c r="T48" s="6" t="n">
+      <c r="U48" s="21" t="n">
         <v>3.48</v>
-      </c>
-      <c r="U48" s="21" t="n">
-        <v>3.5</v>
       </c>
     </row>
     <row r="49">
@@ -4407,7 +4407,7 @@
         </is>
       </c>
       <c r="N49" s="49" t="n">
-        <v>46065</v>
+        <v>46066</v>
       </c>
       <c r="O49" s="6" t="inlineStr">
         <is>
@@ -4420,19 +4420,19 @@
         </is>
       </c>
       <c r="Q49" s="6" t="n">
+        <v>3.61</v>
+      </c>
+      <c r="R49" s="6" t="n">
         <v>3.67</v>
       </c>
-      <c r="R49" s="6" t="n">
+      <c r="S49" s="6" t="n">
         <v>3.75</v>
       </c>
-      <c r="S49" s="6" t="n">
+      <c r="T49" s="6" t="n">
         <v>3.7</v>
       </c>
-      <c r="T49" s="6" t="n">
+      <c r="U49" s="21" t="n">
         <v>3.75</v>
-      </c>
-      <c r="U49" s="21" t="n">
-        <v>3.76</v>
       </c>
     </row>
     <row r="50">
@@ -4486,7 +4486,7 @@
         </is>
       </c>
       <c r="N50" s="49" t="n">
-        <v>46065</v>
+        <v>46066</v>
       </c>
       <c r="O50" s="6" t="inlineStr">
         <is>
@@ -4499,16 +4499,16 @@
         </is>
       </c>
       <c r="Q50" s="6" t="n">
+        <v>4.04</v>
+      </c>
+      <c r="R50" s="6" t="n">
         <v>4.09</v>
       </c>
-      <c r="R50" s="6" t="n">
+      <c r="S50" s="6" t="n">
         <v>4.18</v>
       </c>
-      <c r="S50" s="6" t="n">
+      <c r="T50" s="6" t="n">
         <v>4.16</v>
-      </c>
-      <c r="T50" s="6" t="n">
-        <v>4.22</v>
       </c>
       <c r="U50" s="21" t="n">
         <v>4.22</v>
@@ -4612,7 +4612,7 @@
         </is>
       </c>
       <c r="N52" s="50" t="n">
-        <v>46065</v>
+        <v>46066</v>
       </c>
       <c r="O52" s="9" t="inlineStr">
         <is>
@@ -4625,19 +4625,19 @@
         </is>
       </c>
       <c r="Q52" s="9" t="n">
+        <v>5.76</v>
+      </c>
+      <c r="R52" s="9" t="n">
         <v>5.77</v>
       </c>
-      <c r="R52" s="9" t="n">
+      <c r="S52" s="9" t="n">
         <v>5.85</v>
       </c>
-      <c r="S52" s="9" t="n">
+      <c r="T52" s="9" t="n">
         <v>5.82</v>
       </c>
-      <c r="T52" s="9" t="n">
+      <c r="U52" s="22" t="n">
         <v>5.86</v>
-      </c>
-      <c r="U52" s="22" t="n">
-        <v>5.87</v>
       </c>
     </row>
     <row r="53" ht="21" customHeight="1">

</xml_diff>

<commit_message>
Update dashboards - 2026-02-19
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -1704,7 +1704,7 @@
         </is>
       </c>
       <c r="N13" s="49" t="n">
-        <v>46055</v>
+        <v>46062</v>
       </c>
       <c r="O13" s="6" t="inlineStr">
         <is>
@@ -1717,19 +1717,19 @@
         </is>
       </c>
       <c r="Q13" s="24" t="n">
-        <v>227000</v>
+        <v>206000</v>
       </c>
       <c r="R13" s="24" t="n">
+        <v>229000</v>
+      </c>
+      <c r="S13" s="24" t="n">
         <v>232000</v>
       </c>
-      <c r="S13" s="24" t="n">
+      <c r="T13" s="24" t="n">
         <v>209000</v>
       </c>
-      <c r="T13" s="24" t="n">
+      <c r="U13" s="26" t="n">
         <v>210000</v>
-      </c>
-      <c r="U13" s="26" t="n">
-        <v>199000</v>
       </c>
     </row>
     <row r="14">
@@ -1779,7 +1779,7 @@
         </is>
       </c>
       <c r="N14" s="49" t="n">
-        <v>46048</v>
+        <v>46055</v>
       </c>
       <c r="O14" s="6" t="inlineStr">
         <is>
@@ -1792,19 +1792,19 @@
         </is>
       </c>
       <c r="Q14" s="24" t="n">
-        <v>1862000</v>
+        <v>1869000</v>
       </c>
       <c r="R14" s="24" t="n">
+        <v>1852000</v>
+      </c>
+      <c r="S14" s="24" t="n">
         <v>1841000</v>
       </c>
-      <c r="S14" s="24" t="n">
+      <c r="T14" s="24" t="n">
         <v>1819000</v>
       </c>
-      <c r="T14" s="24" t="n">
+      <c r="U14" s="26" t="n">
         <v>1865000</v>
-      </c>
-      <c r="U14" s="26" t="n">
-        <v>1875000</v>
       </c>
     </row>
     <row r="15">
@@ -2907,7 +2907,7 @@
         </is>
       </c>
       <c r="N29" s="49" t="n">
-        <v>46070</v>
+        <v>46071</v>
       </c>
       <c r="O29" s="6" t="inlineStr">
         <is>
@@ -2920,19 +2920,19 @@
         </is>
       </c>
       <c r="Q29" s="6" t="n">
+        <v>2.15</v>
+      </c>
+      <c r="R29" s="6" t="n">
         <v>2.13</v>
       </c>
-      <c r="R29" s="6" t="n">
+      <c r="S29" s="6" t="n">
         <v>2.12</v>
       </c>
-      <c r="S29" s="6" t="n">
+      <c r="T29" s="6" t="n">
         <v>2.13</v>
       </c>
-      <c r="T29" s="6" t="n">
+      <c r="U29" s="21" t="n">
         <v>2.15</v>
-      </c>
-      <c r="U29" s="21" t="n">
-        <v>2.17</v>
       </c>
     </row>
     <row r="30">
@@ -2986,7 +2986,7 @@
         </is>
       </c>
       <c r="N30" s="49" t="n">
-        <v>46070</v>
+        <v>46071</v>
       </c>
       <c r="O30" s="6" t="inlineStr">
         <is>
@@ -2999,16 +2999,16 @@
         </is>
       </c>
       <c r="Q30" s="6" t="n">
+        <v>2.29</v>
+      </c>
+      <c r="R30" s="6" t="n">
         <v>2.26</v>
       </c>
-      <c r="R30" s="6" t="n">
+      <c r="S30" s="6" t="n">
         <v>2.27</v>
       </c>
-      <c r="S30" s="6" t="n">
+      <c r="T30" s="6" t="n">
         <v>2.29</v>
-      </c>
-      <c r="T30" s="6" t="n">
-        <v>2.32</v>
       </c>
       <c r="U30" s="21" t="n">
         <v>2.32</v>
@@ -4126,8 +4126,8 @@
           <t>BOPTEXP</t>
         </is>
       </c>
-      <c r="C46" s="48" t="n">
-        <v>45962</v>
+      <c r="C46" s="49" t="n">
+        <v>45992</v>
       </c>
       <c r="D46" s="6" t="inlineStr">
         <is>
@@ -4140,19 +4140,19 @@
         </is>
       </c>
       <c r="F46" s="24" t="n">
-        <v>292052</v>
+        <v>287287</v>
       </c>
       <c r="G46" s="24" t="n">
-        <v>302919</v>
+        <v>292290</v>
       </c>
       <c r="H46" s="24" t="n">
-        <v>294225</v>
+        <v>302594</v>
       </c>
       <c r="I46" s="24" t="n">
-        <v>284060</v>
+        <v>293901</v>
       </c>
       <c r="J46" s="24" t="n">
-        <v>283923</v>
+        <v>283736</v>
       </c>
       <c r="K46" s="5" t="n"/>
       <c r="L46" s="29" t="inlineStr">
@@ -4213,8 +4213,8 @@
           <t>BOPTEXP</t>
         </is>
       </c>
-      <c r="C47" s="48" t="n">
-        <v>45962</v>
+      <c r="C47" s="49" t="n">
+        <v>45992</v>
       </c>
       <c r="D47" s="6" t="inlineStr">
         <is>
@@ -4227,19 +4227,19 @@
         </is>
       </c>
       <c r="F47" s="38" t="n">
-        <v>-0.0358742766218032</v>
+        <v>-0.01711656231824554</v>
       </c>
       <c r="G47" s="38" t="n">
-        <v>0.02954881468264081</v>
+        <v>-0.03405222839844813</v>
       </c>
       <c r="H47" s="38" t="n">
-        <v>0.03578469337463908</v>
+        <v>0.02957798714533122</v>
       </c>
       <c r="I47" s="38" t="n">
-        <v>0.0004825251916893425</v>
+        <v>0.03582555615078808</v>
       </c>
       <c r="J47" s="38" t="n">
-        <v>0.01213465041583639</v>
+        <v>0.0004866042778863822</v>
       </c>
       <c r="K47" s="5" t="n"/>
       <c r="L47" s="28" t="inlineStr">
@@ -4253,7 +4253,7 @@
         </is>
       </c>
       <c r="N47" s="49" t="n">
-        <v>46069</v>
+        <v>46070</v>
       </c>
       <c r="O47" s="6" t="inlineStr">
         <is>
@@ -4292,8 +4292,8 @@
           <t>BOPTIMP</t>
         </is>
       </c>
-      <c r="C48" s="48" t="n">
-        <v>45962</v>
+      <c r="C48" s="49" t="n">
+        <v>45992</v>
       </c>
       <c r="D48" s="6" t="inlineStr">
         <is>
@@ -4306,19 +4306,19 @@
         </is>
       </c>
       <c r="F48" s="24" t="n">
-        <v>348877</v>
+        <v>357598</v>
       </c>
       <c r="G48" s="24" t="n">
-        <v>332124</v>
+        <v>345334</v>
       </c>
       <c r="H48" s="24" t="n">
-        <v>342363</v>
+        <v>331343</v>
       </c>
       <c r="I48" s="24" t="n">
-        <v>339690</v>
+        <v>341582</v>
       </c>
       <c r="J48" s="24" t="n">
-        <v>358321</v>
+        <v>338909</v>
       </c>
       <c r="K48" s="5" t="n"/>
       <c r="L48" s="28" t="inlineStr">
@@ -4332,7 +4332,7 @@
         </is>
       </c>
       <c r="N48" s="49" t="n">
-        <v>46066</v>
+        <v>46070</v>
       </c>
       <c r="O48" s="6" t="inlineStr">
         <is>
@@ -4345,19 +4345,19 @@
         </is>
       </c>
       <c r="Q48" s="6" t="n">
+        <v>3.43</v>
+      </c>
+      <c r="R48" s="6" t="n">
         <v>3.4</v>
       </c>
-      <c r="R48" s="6" t="n">
+      <c r="S48" s="6" t="n">
         <v>3.47</v>
       </c>
-      <c r="S48" s="6" t="n">
+      <c r="T48" s="6" t="n">
         <v>3.52</v>
       </c>
-      <c r="T48" s="6" t="n">
+      <c r="U48" s="21" t="n">
         <v>3.45</v>
-      </c>
-      <c r="U48" s="21" t="n">
-        <v>3.48</v>
       </c>
     </row>
     <row r="49">
@@ -4367,8 +4367,8 @@
           <t>BOPTIMP</t>
         </is>
       </c>
-      <c r="C49" s="48" t="n">
-        <v>45962</v>
+      <c r="C49" s="49" t="n">
+        <v>45992</v>
       </c>
       <c r="D49" s="6" t="inlineStr">
         <is>
@@ -4381,19 +4381,19 @@
         </is>
       </c>
       <c r="F49" s="38" t="n">
-        <v>0.05044200358902096</v>
+        <v>0.0355134449547394</v>
       </c>
       <c r="G49" s="38" t="n">
-        <v>-0.02990685325224984</v>
+        <v>0.04222512622871166</v>
       </c>
       <c r="H49" s="38" t="n">
-        <v>0.007868939327033475</v>
+        <v>-0.02997523288697879</v>
       </c>
       <c r="I49" s="38" t="n">
-        <v>-0.05199527797700942</v>
+        <v>0.007887072931081818</v>
       </c>
       <c r="J49" s="38" t="n">
-        <v>0.05791782795597333</v>
+        <v>-0.05210885495329198</v>
       </c>
       <c r="K49" s="5" t="n"/>
       <c r="L49" s="28" t="inlineStr">
@@ -4407,7 +4407,7 @@
         </is>
       </c>
       <c r="N49" s="49" t="n">
-        <v>46066</v>
+        <v>46070</v>
       </c>
       <c r="O49" s="6" t="inlineStr">
         <is>
@@ -4420,19 +4420,19 @@
         </is>
       </c>
       <c r="Q49" s="6" t="n">
+        <v>3.63</v>
+      </c>
+      <c r="R49" s="6" t="n">
         <v>3.61</v>
       </c>
-      <c r="R49" s="6" t="n">
+      <c r="S49" s="6" t="n">
         <v>3.67</v>
       </c>
-      <c r="S49" s="6" t="n">
+      <c r="T49" s="6" t="n">
         <v>3.75</v>
       </c>
-      <c r="T49" s="6" t="n">
+      <c r="U49" s="21" t="n">
         <v>3.7</v>
-      </c>
-      <c r="U49" s="21" t="n">
-        <v>3.75</v>
       </c>
     </row>
     <row r="50">
@@ -4446,8 +4446,8 @@
           <t>BOPSTB</t>
         </is>
       </c>
-      <c r="C50" s="48" t="n">
-        <v>45962</v>
+      <c r="C50" s="49" t="n">
+        <v>45992</v>
       </c>
       <c r="D50" s="6" t="inlineStr">
         <is>
@@ -4460,19 +4460,19 @@
         </is>
       </c>
       <c r="F50" s="24" t="n">
-        <v>30075</v>
+        <v>29018</v>
       </c>
       <c r="G50" s="24" t="n">
+        <v>30597</v>
+      </c>
+      <c r="H50" s="24" t="n">
         <v>29777</v>
       </c>
-      <c r="H50" s="24" t="n">
+      <c r="I50" s="24" t="n">
         <v>30169</v>
       </c>
-      <c r="I50" s="24" t="n">
+      <c r="J50" s="24" t="n">
         <v>30416</v>
-      </c>
-      <c r="J50" s="24" t="n">
-        <v>28606</v>
       </c>
       <c r="K50" s="5" t="n"/>
       <c r="L50" s="28" t="inlineStr">
@@ -4486,7 +4486,7 @@
         </is>
       </c>
       <c r="N50" s="49" t="n">
-        <v>46066</v>
+        <v>46070</v>
       </c>
       <c r="O50" s="6" t="inlineStr">
         <is>
@@ -4499,19 +4499,19 @@
         </is>
       </c>
       <c r="Q50" s="6" t="n">
+        <v>4.05</v>
+      </c>
+      <c r="R50" s="6" t="n">
         <v>4.04</v>
       </c>
-      <c r="R50" s="6" t="n">
+      <c r="S50" s="6" t="n">
         <v>4.09</v>
       </c>
-      <c r="S50" s="6" t="n">
+      <c r="T50" s="6" t="n">
         <v>4.18</v>
       </c>
-      <c r="T50" s="6" t="n">
+      <c r="U50" s="21" t="n">
         <v>4.16</v>
-      </c>
-      <c r="U50" s="21" t="n">
-        <v>4.22</v>
       </c>
     </row>
     <row r="51" ht="31.5" customHeight="1">
@@ -4521,8 +4521,8 @@
           <t>BOPSTB</t>
         </is>
       </c>
-      <c r="C51" s="48" t="n">
-        <v>45962</v>
+      <c r="C51" s="49" t="n">
+        <v>45992</v>
       </c>
       <c r="D51" s="6" t="inlineStr">
         <is>
@@ -4535,19 +4535,19 @@
         </is>
       </c>
       <c r="F51" s="38" t="n">
-        <v>0.01000772408234551</v>
+        <v>-0.05160636663725204</v>
       </c>
       <c r="G51" s="38" t="n">
+        <v>0.02753803270980959</v>
+      </c>
+      <c r="H51" s="38" t="n">
         <v>-0.01299347011833341</v>
       </c>
-      <c r="H51" s="38" t="n">
+      <c r="I51" s="38" t="n">
         <v>-0.008120725933719042</v>
       </c>
-      <c r="I51" s="38" t="n">
+      <c r="J51" s="38" t="n">
         <v>0.06327343913864225</v>
-      </c>
-      <c r="J51" s="38" t="n">
-        <v>0.02755127698552395</v>
       </c>
       <c r="K51" s="5" t="n"/>
       <c r="L51" s="28" t="inlineStr">
@@ -4560,7 +4560,7 @@
           <t>MORTGAGE30US</t>
         </is>
       </c>
-      <c r="N51" s="49" t="n">
+      <c r="N51" s="48" t="n">
         <v>46062</v>
       </c>
       <c r="O51" s="6" t="inlineStr">
@@ -4612,7 +4612,7 @@
         </is>
       </c>
       <c r="N52" s="50" t="n">
-        <v>46066</v>
+        <v>46070</v>
       </c>
       <c r="O52" s="9" t="inlineStr">
         <is>
@@ -4625,19 +4625,19 @@
         </is>
       </c>
       <c r="Q52" s="9" t="n">
+        <v>5.75</v>
+      </c>
+      <c r="R52" s="9" t="n">
         <v>5.76</v>
       </c>
-      <c r="R52" s="9" t="n">
+      <c r="S52" s="9" t="n">
         <v>5.77</v>
       </c>
-      <c r="S52" s="9" t="n">
+      <c r="T52" s="9" t="n">
         <v>5.85</v>
       </c>
-      <c r="T52" s="9" t="n">
+      <c r="U52" s="22" t="n">
         <v>5.82</v>
-      </c>
-      <c r="U52" s="22" t="n">
-        <v>5.86</v>
       </c>
     </row>
     <row r="53" ht="21" customHeight="1">

</xml_diff>

<commit_message>
Update dashboards - 2026-02-20
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -337,6 +337,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -346,18 +349,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="168" fontId="1" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="168" fontId="1" fillId="3" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -728,8 +728,8 @@
   </sheetPr>
   <dimension ref="A1:U80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="76" zoomScaleNormal="51" workbookViewId="0">
-      <selection activeCell="I41" sqref="I41"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="76" zoomScaleNormal="51" workbookViewId="0">
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9.1328125" defaultRowHeight="15.75"/>
@@ -895,7 +895,7 @@
         </is>
       </c>
       <c r="C3" s="48" t="n">
-        <v>45839</v>
+        <v>45931</v>
       </c>
       <c r="D3" s="6" t="inlineStr">
         <is>
@@ -908,19 +908,19 @@
         </is>
       </c>
       <c r="F3" s="24" t="n">
+        <v>24111.83</v>
+      </c>
+      <c r="G3" s="24" t="n">
         <v>24026.834</v>
       </c>
-      <c r="G3" s="24" t="n">
+      <c r="H3" s="24" t="n">
         <v>23770.976</v>
       </c>
-      <c r="H3" s="24" t="n">
+      <c r="I3" s="24" t="n">
         <v>23548.21</v>
       </c>
-      <c r="I3" s="24" t="n">
+      <c r="J3" s="24" t="n">
         <v>23586.542</v>
-      </c>
-      <c r="J3" s="24" t="n">
-        <v>23478.57</v>
       </c>
       <c r="K3" s="5" t="n"/>
       <c r="L3" s="28" t="inlineStr">
@@ -933,7 +933,7 @@
           <t>PAYEMS</t>
         </is>
       </c>
-      <c r="N3" s="48" t="n">
+      <c r="N3" s="49" t="n">
         <v>46023</v>
       </c>
       <c r="O3" s="6" t="inlineStr">
@@ -970,7 +970,7 @@
         </is>
       </c>
       <c r="C4" s="48" t="n">
-        <v>45839</v>
+        <v>45931</v>
       </c>
       <c r="D4" s="6" t="inlineStr">
         <is>
@@ -983,19 +983,19 @@
         </is>
       </c>
       <c r="F4" s="25" t="n">
+        <v>0.003537544730196407</v>
+      </c>
+      <c r="G4" s="25" t="n">
         <v>0.0107634621312982</v>
       </c>
-      <c r="G4" s="25" t="n">
+      <c r="H4" s="25" t="n">
         <v>0.009459997171759493</v>
       </c>
-      <c r="H4" s="25" t="n">
+      <c r="I4" s="25" t="n">
         <v>-0.001625164044818495</v>
       </c>
-      <c r="I4" s="25" t="n">
+      <c r="J4" s="25" t="n">
         <v>0.004598746857240599</v>
-      </c>
-      <c r="J4" s="25" t="n">
-        <v>0.008247780216767531</v>
       </c>
       <c r="K4" s="5" t="n"/>
       <c r="L4" s="28" t="n"/>
@@ -1004,7 +1004,7 @@
           <t>PAYEMS</t>
         </is>
       </c>
-      <c r="N4" s="48" t="n">
+      <c r="N4" s="49" t="n">
         <v>46023</v>
       </c>
       <c r="O4" s="6" t="inlineStr">
@@ -1044,7 +1044,7 @@
           <t>NGDPSAXDCUSQ</t>
         </is>
       </c>
-      <c r="C5" s="48" t="n">
+      <c r="C5" s="49" t="n">
         <v>45839</v>
       </c>
       <c r="D5" s="6" t="inlineStr">
@@ -1083,7 +1083,7 @@
           <t>ADPMNUSNERSA</t>
         </is>
       </c>
-      <c r="N5" s="48" t="n">
+      <c r="N5" s="49" t="n">
         <v>46023</v>
       </c>
       <c r="O5" s="6" t="inlineStr">
@@ -1119,7 +1119,7 @@
           <t>NGDPSAXDCUSQ</t>
         </is>
       </c>
-      <c r="C6" s="48" t="n">
+      <c r="C6" s="49" t="n">
         <v>45839</v>
       </c>
       <c r="D6" s="6" t="inlineStr">
@@ -1158,7 +1158,7 @@
           <t>UNRATE</t>
         </is>
       </c>
-      <c r="N6" s="48" t="n">
+      <c r="N6" s="49" t="n">
         <v>46023</v>
       </c>
       <c r="O6" s="6" t="inlineStr">
@@ -1198,7 +1198,7 @@
           <t>GDPNOW</t>
         </is>
       </c>
-      <c r="C7" s="48" t="n">
+      <c r="C7" s="49" t="n">
         <v>45931</v>
       </c>
       <c r="D7" s="6" t="inlineStr">
@@ -1211,19 +1211,19 @@
           <t>Q</t>
         </is>
       </c>
-      <c r="F7" s="44" t="n">
+      <c r="F7" s="41" t="n">
         <v>4.2373</v>
       </c>
-      <c r="G7" s="44" t="n">
+      <c r="G7" s="41" t="n">
         <v>3.4728</v>
       </c>
-      <c r="H7" s="44" t="n">
+      <c r="H7" s="41" t="n">
         <v>2.902</v>
       </c>
-      <c r="I7" s="44" t="n">
+      <c r="I7" s="41" t="n">
         <v>-2.7318</v>
       </c>
-      <c r="J7" s="44" t="n">
+      <c r="J7" s="41" t="n">
         <v>2.2711</v>
       </c>
       <c r="K7" s="5" t="n"/>
@@ -1237,7 +1237,7 @@
           <t>U6RATE</t>
         </is>
       </c>
-      <c r="N7" s="48" t="n">
+      <c r="N7" s="49" t="n">
         <v>46023</v>
       </c>
       <c r="O7" s="6" t="inlineStr">
@@ -1277,7 +1277,7 @@
           <t>RECPROUSM156N</t>
         </is>
       </c>
-      <c r="C8" s="48" t="n">
+      <c r="C8" s="49" t="n">
         <v>45992</v>
       </c>
       <c r="D8" s="6" t="inlineStr">
@@ -1316,7 +1316,7 @@
           <t>CIVPART</t>
         </is>
       </c>
-      <c r="N8" s="48" t="n">
+      <c r="N8" s="49" t="n">
         <v>46023</v>
       </c>
       <c r="O8" s="6" t="inlineStr">
@@ -1357,7 +1357,7 @@
         </is>
       </c>
       <c r="C9" s="48" t="n">
-        <v>45839</v>
+        <v>45931</v>
       </c>
       <c r="D9" s="6" t="inlineStr">
         <is>
@@ -1370,19 +1370,19 @@
         </is>
       </c>
       <c r="F9" s="24" t="n">
+        <v>16682.486</v>
+      </c>
+      <c r="G9" s="24" t="n">
         <v>16585.878</v>
       </c>
-      <c r="G9" s="24" t="n">
+      <c r="H9" s="24" t="n">
         <v>16445.685</v>
       </c>
-      <c r="H9" s="24" t="n">
+      <c r="I9" s="24" t="n">
         <v>16345.793</v>
       </c>
-      <c r="I9" s="24" t="n">
+      <c r="J9" s="24" t="n">
         <v>16320.89</v>
-      </c>
-      <c r="J9" s="24" t="n">
-        <v>16165.768</v>
       </c>
       <c r="K9" s="5" t="n"/>
       <c r="L9" s="28" t="inlineStr">
@@ -1395,7 +1395,7 @@
           <t>EMRATIO</t>
         </is>
       </c>
-      <c r="N9" s="48" t="n">
+      <c r="N9" s="49" t="n">
         <v>46023</v>
       </c>
       <c r="O9" s="6" t="inlineStr">
@@ -1432,7 +1432,7 @@
         </is>
       </c>
       <c r="C10" s="48" t="n">
-        <v>45839</v>
+        <v>45931</v>
       </c>
       <c r="D10" s="6" t="inlineStr">
         <is>
@@ -1445,19 +1445,19 @@
         </is>
       </c>
       <c r="F10" s="25" t="n">
+        <v>0.00582471425389719</v>
+      </c>
+      <c r="G10" s="25" t="n">
         <v>0.008524606910566446</v>
       </c>
-      <c r="G10" s="25" t="n">
+      <c r="H10" s="25" t="n">
         <v>0.006111174905983452</v>
       </c>
-      <c r="H10" s="25" t="n">
+      <c r="I10" s="25" t="n">
         <v>0.001525835907232986</v>
       </c>
-      <c r="I10" s="25" t="n">
+      <c r="J10" s="25" t="n">
         <v>0.009595708660423696</v>
-      </c>
-      <c r="J10" s="25" t="n">
-        <v>0.009752313559639125</v>
       </c>
       <c r="K10" s="5" t="n"/>
       <c r="L10" s="28" t="inlineStr">
@@ -1470,7 +1470,7 @@
           <t>JTSJOR</t>
         </is>
       </c>
-      <c r="N10" s="48" t="n">
+      <c r="N10" s="49" t="n">
         <v>45992</v>
       </c>
       <c r="O10" s="6" t="inlineStr">
@@ -1511,7 +1511,7 @@
         </is>
       </c>
       <c r="C11" s="48" t="n">
-        <v>45962</v>
+        <v>45992</v>
       </c>
       <c r="D11" s="6" t="inlineStr">
         <is>
@@ -1524,19 +1524,19 @@
         </is>
       </c>
       <c r="F11" s="25" t="n">
-        <v>0.006303109534036899</v>
+        <v>-0.008854919140606765</v>
       </c>
       <c r="G11" s="25" t="n">
-        <v>0.003232001498899351</v>
+        <v>0.005152948892116038</v>
       </c>
       <c r="H11" s="25" t="n">
+        <v>-9.368120286679105e-05</v>
+      </c>
+      <c r="I11" s="25" t="n">
         <v>-0.00461581499440511</v>
       </c>
-      <c r="I11" s="25" t="n">
+      <c r="J11" s="25" t="n">
         <v>0.001494209936496294</v>
-      </c>
-      <c r="J11" s="25" t="n">
-        <v>0.01310374189885977</v>
       </c>
       <c r="K11" s="5" t="n"/>
       <c r="L11" s="28" t="inlineStr">
@@ -1549,7 +1549,7 @@
           <t>JTSHIR</t>
         </is>
       </c>
-      <c r="N11" s="48" t="n">
+      <c r="N11" s="49" t="n">
         <v>45992</v>
       </c>
       <c r="O11" s="6" t="inlineStr">
@@ -1586,7 +1586,7 @@
         </is>
       </c>
       <c r="C12" s="48" t="n">
-        <v>45962</v>
+        <v>45992</v>
       </c>
       <c r="D12" s="6" t="inlineStr">
         <is>
@@ -1599,19 +1599,19 @@
         </is>
       </c>
       <c r="F12" s="25" t="n">
-        <v>0.01107097621616567</v>
+        <v>-0.02783872737246302</v>
       </c>
       <c r="G12" s="25" t="n">
-        <v>0.02185114503816803</v>
+        <v>0.006567528263826993</v>
       </c>
       <c r="H12" s="25" t="n">
+        <v>0.01846374045801518</v>
+      </c>
+      <c r="I12" s="25" t="n">
         <v>0.02290259211345895</v>
       </c>
-      <c r="I12" s="25" t="n">
+      <c r="J12" s="25" t="n">
         <v>0.03914728682170551</v>
-      </c>
-      <c r="J12" s="25" t="n">
-        <v>0.0341397460041527</v>
       </c>
       <c r="K12" s="5" t="n"/>
       <c r="L12" s="28" t="inlineStr">
@@ -1624,7 +1624,7 @@
           <t>JTSTSR</t>
         </is>
       </c>
-      <c r="N12" s="48" t="n">
+      <c r="N12" s="49" t="n">
         <v>45992</v>
       </c>
       <c r="O12" s="6" t="inlineStr">
@@ -1665,7 +1665,7 @@
         </is>
       </c>
       <c r="C13" s="48" t="n">
-        <v>45962</v>
+        <v>45992</v>
       </c>
       <c r="D13" s="6" t="inlineStr">
         <is>
@@ -1678,19 +1678,19 @@
         </is>
       </c>
       <c r="F13" s="25" t="n">
-        <v>0.005120414134593743</v>
+        <v>-0.002845310871341211</v>
       </c>
       <c r="G13" s="25" t="n">
-        <v>0.004379892056853851</v>
+        <v>0.001580090855224148</v>
       </c>
       <c r="H13" s="25" t="n">
+        <v>0.001469383141654124</v>
+      </c>
+      <c r="I13" s="25" t="n">
         <v>-0.00357585313661446</v>
       </c>
-      <c r="I13" s="25" t="n">
+      <c r="J13" s="25" t="n">
         <v>0.005207743688441013</v>
-      </c>
-      <c r="J13" s="25" t="n">
-        <v>0.002952197115930311</v>
       </c>
       <c r="K13" s="5" t="n"/>
       <c r="L13" s="28" t="inlineStr">
@@ -1703,7 +1703,7 @@
           <t>ICSA</t>
         </is>
       </c>
-      <c r="N13" s="49" t="n">
+      <c r="N13" s="48" t="n">
         <v>46062</v>
       </c>
       <c r="O13" s="6" t="inlineStr">
@@ -1740,7 +1740,7 @@
         </is>
       </c>
       <c r="C14" s="48" t="n">
-        <v>45962</v>
+        <v>45992</v>
       </c>
       <c r="D14" s="6" t="inlineStr">
         <is>
@@ -1753,19 +1753,19 @@
         </is>
       </c>
       <c r="F14" s="25" t="n">
-        <v>0.03287172222382833</v>
+        <v>0.01357310577859232</v>
       </c>
       <c r="G14" s="25" t="n">
-        <v>0.02743170978465099</v>
+        <v>0.02625112029836067</v>
       </c>
       <c r="H14" s="25" t="n">
+        <v>0.02445440092498914</v>
+      </c>
+      <c r="I14" s="25" t="n">
         <v>0.02153393181883783</v>
       </c>
-      <c r="I14" s="25" t="n">
+      <c r="J14" s="25" t="n">
         <v>0.03793325150505573</v>
-      </c>
-      <c r="J14" s="25" t="n">
-        <v>0.03053813621117101</v>
       </c>
       <c r="K14" s="5" t="n"/>
       <c r="L14" s="28" t="inlineStr">
@@ -1778,7 +1778,7 @@
           <t>CCSA</t>
         </is>
       </c>
-      <c r="N14" s="49" t="n">
+      <c r="N14" s="48" t="n">
         <v>46055</v>
       </c>
       <c r="O14" s="6" t="inlineStr">
@@ -1819,7 +1819,7 @@
         </is>
       </c>
       <c r="C15" s="48" t="n">
-        <v>45962</v>
+        <v>45992</v>
       </c>
       <c r="D15" s="6" t="inlineStr">
         <is>
@@ -1832,19 +1832,19 @@
         </is>
       </c>
       <c r="F15" s="25" t="n">
-        <v>0.001899602810321532</v>
+        <v>0.003201726937135607</v>
       </c>
       <c r="G15" s="25" t="n">
-        <v>0.002642778380250288</v>
+        <v>0.001180498170227917</v>
       </c>
       <c r="H15" s="25" t="n">
+        <v>0.003554081269991682</v>
+      </c>
+      <c r="I15" s="25" t="n">
         <v>0.003374053619106698</v>
       </c>
-      <c r="I15" s="25" t="n">
+      <c r="J15" s="25" t="n">
         <v>0.002493308400249195</v>
-      </c>
-      <c r="J15" s="25" t="n">
-        <v>0.004234479711318961</v>
       </c>
       <c r="K15" s="5" t="n"/>
       <c r="L15" s="28" t="inlineStr">
@@ -1857,7 +1857,7 @@
           <t>AWHAETP</t>
         </is>
       </c>
-      <c r="N15" s="48" t="n">
+      <c r="N15" s="49" t="n">
         <v>46023</v>
       </c>
       <c r="O15" s="6" t="inlineStr">
@@ -1894,7 +1894,7 @@
         </is>
       </c>
       <c r="C16" s="48" t="n">
-        <v>45962</v>
+        <v>45992</v>
       </c>
       <c r="D16" s="6" t="inlineStr">
         <is>
@@ -1907,19 +1907,19 @@
         </is>
       </c>
       <c r="F16" s="25" t="n">
-        <v>0.02567156402073092</v>
+        <v>0.02574422702401932</v>
       </c>
       <c r="G16" s="25" t="n">
-        <v>0.02575027269930347</v>
+        <v>0.02586696193462544</v>
       </c>
       <c r="H16" s="25" t="n">
+        <v>0.02668257801064683</v>
+      </c>
+      <c r="I16" s="25" t="n">
         <v>0.0245940671714955</v>
       </c>
-      <c r="I16" s="25" t="n">
+      <c r="J16" s="25" t="n">
         <v>0.02312614601653996</v>
-      </c>
-      <c r="J16" s="25" t="n">
-        <v>0.02374204688350444</v>
       </c>
       <c r="K16" s="5" t="n"/>
       <c r="L16" s="28" t="n"/>
@@ -1944,7 +1944,7 @@
           <t>RSAFS</t>
         </is>
       </c>
-      <c r="C17" s="48" t="n">
+      <c r="C17" s="49" t="n">
         <v>45992</v>
       </c>
       <c r="D17" s="6" t="inlineStr">
@@ -2031,7 +2031,7 @@
           <t>RSAFS</t>
         </is>
       </c>
-      <c r="C18" s="48" t="n">
+      <c r="C18" s="49" t="n">
         <v>45992</v>
       </c>
       <c r="D18" s="6" t="inlineStr">
@@ -2111,7 +2111,7 @@
         </is>
       </c>
       <c r="C19" s="48" t="n">
-        <v>45962</v>
+        <v>45992</v>
       </c>
       <c r="D19" s="6" t="inlineStr">
         <is>
@@ -2124,19 +2124,19 @@
         </is>
       </c>
       <c r="F19" s="25" t="n">
-        <v>0.0006937237425563847</v>
+        <v>-0.0002827474178507261</v>
       </c>
       <c r="G19" s="25" t="n">
-        <v>-0.001064425459726515</v>
+        <v>0.001248973066589665</v>
       </c>
       <c r="H19" s="25" t="n">
+        <v>-0.001280636881233477</v>
+      </c>
+      <c r="I19" s="25" t="n">
         <v>0.0005713461581133839</v>
       </c>
-      <c r="I19" s="25" t="n">
+      <c r="J19" s="25" t="n">
         <v>0.001005025125628167</v>
-      </c>
-      <c r="J19" s="25" t="n">
-        <v>0.00263888966212189</v>
       </c>
       <c r="K19" s="5" t="n"/>
       <c r="L19" s="28" t="n"/>
@@ -2182,7 +2182,7 @@
         </is>
       </c>
       <c r="C20" s="48" t="n">
-        <v>45962</v>
+        <v>45992</v>
       </c>
       <c r="D20" s="6" t="inlineStr">
         <is>
@@ -2195,19 +2195,19 @@
         </is>
       </c>
       <c r="F20" s="25" t="n">
-        <v>0.01007203916779632</v>
+        <v>0.009195260774909153</v>
       </c>
       <c r="G20" s="25" t="n">
-        <v>0.01168973358412177</v>
+        <v>0.01041374906169812</v>
       </c>
       <c r="H20" s="25" t="n">
+        <v>0.01147076162937589</v>
+      </c>
+      <c r="I20" s="25" t="n">
         <v>0.01508168307081075</v>
       </c>
-      <c r="I20" s="25" t="n">
+      <c r="J20" s="25" t="n">
         <v>0.01547352826862074</v>
-      </c>
-      <c r="J20" s="25" t="n">
-        <v>0.01500856666215786</v>
       </c>
       <c r="K20" s="5" t="n"/>
       <c r="L20" s="28" t="inlineStr">
@@ -2261,7 +2261,7 @@
         </is>
       </c>
       <c r="C21" s="48" t="n">
-        <v>45962</v>
+        <v>45992</v>
       </c>
       <c r="D21" s="6" t="inlineStr">
         <is>
@@ -2274,19 +2274,19 @@
         </is>
       </c>
       <c r="F21" s="6" t="n">
-        <v>3.5</v>
+        <v>3.6</v>
       </c>
       <c r="G21" s="6" t="n">
         <v>3.7</v>
       </c>
       <c r="H21" s="6" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="I21" s="6" t="n">
         <v>4</v>
       </c>
-      <c r="I21" s="6" t="n">
+      <c r="J21" s="6" t="n">
         <v>4.1</v>
-      </c>
-      <c r="J21" s="6" t="n">
-        <v>4.3</v>
       </c>
       <c r="K21" s="5" t="n"/>
       <c r="L21" s="28" t="n"/>
@@ -2335,7 +2335,7 @@
           <t>TOTALSA</t>
         </is>
       </c>
-      <c r="C22" s="48" t="n">
+      <c r="C22" s="49" t="n">
         <v>46023</v>
       </c>
       <c r="D22" s="6" t="inlineStr">
@@ -2374,7 +2374,7 @@
           <t>PPIFIS</t>
         </is>
       </c>
-      <c r="N22" s="48" t="n">
+      <c r="N22" s="49" t="n">
         <v>45992</v>
       </c>
       <c r="O22" s="6" t="inlineStr">
@@ -2410,7 +2410,7 @@
           <t>TOTALSA</t>
         </is>
       </c>
-      <c r="C23" s="48" t="n">
+      <c r="C23" s="49" t="n">
         <v>46023</v>
       </c>
       <c r="D23" s="6" t="inlineStr">
@@ -2444,7 +2444,7 @@
           <t>PPIFIS</t>
         </is>
       </c>
-      <c r="N23" s="48" t="n">
+      <c r="N23" s="49" t="n">
         <v>45992</v>
       </c>
       <c r="O23" s="6" t="inlineStr">
@@ -2484,7 +2484,7 @@
           <t>REVOLSL</t>
         </is>
       </c>
-      <c r="C24" s="48" t="n">
+      <c r="C24" s="49" t="n">
         <v>45992</v>
       </c>
       <c r="D24" s="6" t="inlineStr">
@@ -2524,7 +2524,7 @@
         </is>
       </c>
       <c r="N24" s="48" t="n">
-        <v>45962</v>
+        <v>45992</v>
       </c>
       <c r="O24" s="6" t="inlineStr">
         <is>
@@ -2537,19 +2537,19 @@
         </is>
       </c>
       <c r="Q24" s="38" t="n">
-        <v>0.002073098225740644</v>
+        <v>0.003558357849066329</v>
       </c>
       <c r="R24" s="38" t="n">
-        <v>0.001590597453477116</v>
+        <v>0.002111370905308885</v>
       </c>
       <c r="S24" s="38" t="n">
+        <v>0.001990205680705293</v>
+      </c>
+      <c r="T24" s="38" t="n">
         <v>0.002608155986582039</v>
       </c>
-      <c r="T24" s="38" t="n">
+      <c r="U24" s="23" t="n">
         <v>0.002622873345935917</v>
-      </c>
-      <c r="U24" s="23" t="n">
-        <v>0.001712126113473822</v>
       </c>
     </row>
     <row r="25">
@@ -2563,7 +2563,7 @@
           <t>NONREVSL</t>
         </is>
       </c>
-      <c r="C25" s="48" t="n">
+      <c r="C25" s="49" t="n">
         <v>45992</v>
       </c>
       <c r="D25" s="6" t="inlineStr">
@@ -2599,7 +2599,7 @@
         </is>
       </c>
       <c r="N25" s="48" t="n">
-        <v>45962</v>
+        <v>45992</v>
       </c>
       <c r="O25" s="6" t="inlineStr">
         <is>
@@ -2612,19 +2612,19 @@
         </is>
       </c>
       <c r="Q25" s="38" t="n">
-        <v>0.02772852363262907</v>
+        <v>0.02901287416285929</v>
       </c>
       <c r="R25" s="38" t="n">
-        <v>0.02678040708789181</v>
+        <v>0.02817782841371343</v>
       </c>
       <c r="S25" s="38" t="n">
+        <v>0.02719006538467721</v>
+      </c>
+      <c r="T25" s="38" t="n">
         <v>0.02787442414870654</v>
       </c>
-      <c r="T25" s="38" t="n">
+      <c r="U25" s="23" t="n">
         <v>0.02747620854151709</v>
-      </c>
-      <c r="U25" s="23" t="n">
-        <v>0.0260554729423934</v>
       </c>
     </row>
     <row r="26">
@@ -2639,7 +2639,7 @@
         </is>
       </c>
       <c r="C26" s="48" t="n">
-        <v>45839</v>
+        <v>45931</v>
       </c>
       <c r="D26" s="6" t="inlineStr">
         <is>
@@ -2652,19 +2652,19 @@
         </is>
       </c>
       <c r="F26" s="38" t="n">
+        <v>0.009152775755367104</v>
+      </c>
+      <c r="G26" s="38" t="n">
         <v>0.007794617579222285</v>
       </c>
-      <c r="G26" s="38" t="n">
+      <c r="H26" s="38" t="n">
         <v>0.01778138610314484</v>
       </c>
-      <c r="H26" s="38" t="n">
+      <c r="I26" s="38" t="n">
         <v>0.02303791460563676</v>
       </c>
-      <c r="I26" s="38" t="n">
+      <c r="J26" s="38" t="n">
         <v>-0.009359213919614473</v>
-      </c>
-      <c r="J26" s="38" t="n">
-        <v>0.008576359077288709</v>
       </c>
       <c r="K26" s="5" t="n"/>
       <c r="L26" s="28" t="inlineStr">
@@ -2678,7 +2678,7 @@
         </is>
       </c>
       <c r="N26" s="48" t="n">
-        <v>45962</v>
+        <v>45992</v>
       </c>
       <c r="O26" s="6" t="inlineStr">
         <is>
@@ -2691,19 +2691,19 @@
         </is>
       </c>
       <c r="Q26" s="38" t="n">
-        <v>0.001603546667924283</v>
+        <v>0.003553916761463993</v>
       </c>
       <c r="R26" s="38" t="n">
-        <v>0.002079493359799622</v>
+        <v>0.001673844026027105</v>
       </c>
       <c r="S26" s="38" t="n">
+        <v>0.002347306898561774</v>
+      </c>
+      <c r="T26" s="38" t="n">
         <v>0.001894029073346237</v>
       </c>
-      <c r="T26" s="38" t="n">
+      <c r="U26" s="23" t="n">
         <v>0.002246302301668779</v>
-      </c>
-      <c r="U26" s="23" t="n">
-        <v>0.002450028147572558</v>
       </c>
     </row>
     <row r="27">
@@ -2718,7 +2718,7 @@
         </is>
       </c>
       <c r="C27" s="48" t="n">
-        <v>45839</v>
+        <v>45931</v>
       </c>
       <c r="D27" s="6" t="inlineStr">
         <is>
@@ -2731,19 +2731,19 @@
         </is>
       </c>
       <c r="F27" s="38" t="n">
+        <v>-0.003824604651284313</v>
+      </c>
+      <c r="G27" s="38" t="n">
         <v>-0.01832684674964358</v>
       </c>
-      <c r="G27" s="38" t="n">
+      <c r="H27" s="38" t="n">
         <v>-0.01299350008050415</v>
       </c>
-      <c r="H27" s="38" t="n">
+      <c r="I27" s="38" t="n">
         <v>-0.002410568051752549</v>
       </c>
-      <c r="I27" s="38" t="n">
+      <c r="J27" s="38" t="n">
         <v>0.01049622222903812</v>
-      </c>
-      <c r="J27" s="38" t="n">
-        <v>-0.01224730930325912</v>
       </c>
       <c r="K27" s="5" t="n"/>
       <c r="L27" s="28" t="n"/>
@@ -2753,7 +2753,7 @@
         </is>
       </c>
       <c r="N27" s="48" t="n">
-        <v>45962</v>
+        <v>45992</v>
       </c>
       <c r="O27" s="6" t="inlineStr">
         <is>
@@ -2766,19 +2766,19 @@
         </is>
       </c>
       <c r="Q27" s="38" t="n">
-        <v>0.02791177941627268</v>
+        <v>0.02996875905826282</v>
       </c>
       <c r="R27" s="38" t="n">
-        <v>0.02734349764196662</v>
+        <v>0.02825865991190849</v>
       </c>
       <c r="S27" s="38" t="n">
+        <v>0.02761806318237614</v>
+      </c>
+      <c r="T27" s="38" t="n">
         <v>0.02825069249833962</v>
       </c>
-      <c r="T27" s="38" t="n">
+      <c r="U27" s="23" t="n">
         <v>0.02912416347215904</v>
-      </c>
-      <c r="U27" s="23" t="n">
-        <v>0.02863047245567936</v>
       </c>
     </row>
     <row r="28">
@@ -2792,7 +2792,7 @@
           <t>DGORDER</t>
         </is>
       </c>
-      <c r="C28" s="49" t="n">
+      <c r="C28" s="48" t="n">
         <v>45992</v>
       </c>
       <c r="D28" s="6" t="inlineStr">
@@ -2831,7 +2831,7 @@
           <t>MICH</t>
         </is>
       </c>
-      <c r="N28" s="48" t="n">
+      <c r="N28" s="49" t="n">
         <v>45992</v>
       </c>
       <c r="O28" s="6" t="inlineStr">
@@ -2867,7 +2867,7 @@
           <t>DGORDER</t>
         </is>
       </c>
-      <c r="C29" s="49" t="n">
+      <c r="C29" s="48" t="n">
         <v>45992</v>
       </c>
       <c r="D29" s="6" t="inlineStr">
@@ -2906,8 +2906,8 @@
           <t>T5YIFR</t>
         </is>
       </c>
-      <c r="N29" s="49" t="n">
-        <v>46071</v>
+      <c r="N29" s="48" t="n">
+        <v>46072</v>
       </c>
       <c r="O29" s="6" t="inlineStr">
         <is>
@@ -2923,16 +2923,16 @@
         <v>2.15</v>
       </c>
       <c r="R29" s="6" t="n">
+        <v>2.15</v>
+      </c>
+      <c r="S29" s="6" t="n">
         <v>2.13</v>
       </c>
-      <c r="S29" s="6" t="n">
+      <c r="T29" s="6" t="n">
         <v>2.12</v>
       </c>
-      <c r="T29" s="6" t="n">
+      <c r="U29" s="21" t="n">
         <v>2.13</v>
-      </c>
-      <c r="U29" s="21" t="n">
-        <v>2.15</v>
       </c>
     </row>
     <row r="30">
@@ -2946,7 +2946,7 @@
           <t>ADXDNO</t>
         </is>
       </c>
-      <c r="C30" s="49" t="n">
+      <c r="C30" s="48" t="n">
         <v>45992</v>
       </c>
       <c r="D30" s="6" t="inlineStr">
@@ -2985,8 +2985,8 @@
           <t>T10YIE</t>
         </is>
       </c>
-      <c r="N30" s="49" t="n">
-        <v>46071</v>
+      <c r="N30" s="48" t="n">
+        <v>46072</v>
       </c>
       <c r="O30" s="6" t="inlineStr">
         <is>
@@ -3002,16 +3002,16 @@
         <v>2.29</v>
       </c>
       <c r="R30" s="6" t="n">
+        <v>2.29</v>
+      </c>
+      <c r="S30" s="6" t="n">
         <v>2.26</v>
       </c>
-      <c r="S30" s="6" t="n">
+      <c r="T30" s="6" t="n">
         <v>2.27</v>
       </c>
-      <c r="T30" s="6" t="n">
+      <c r="U30" s="21" t="n">
         <v>2.29</v>
-      </c>
-      <c r="U30" s="21" t="n">
-        <v>2.32</v>
       </c>
     </row>
     <row r="31">
@@ -3021,7 +3021,7 @@
           <t>ADXDNO</t>
         </is>
       </c>
-      <c r="C31" s="49" t="n">
+      <c r="C31" s="48" t="n">
         <v>45992</v>
       </c>
       <c r="D31" s="6" t="inlineStr">
@@ -3060,7 +3060,7 @@
           <t>ECIWAG</t>
         </is>
       </c>
-      <c r="N31" s="48" t="n">
+      <c r="N31" s="49" t="n">
         <v>45931</v>
       </c>
       <c r="O31" s="6" t="inlineStr">
@@ -3100,7 +3100,7 @@
           <t>INDPRO</t>
         </is>
       </c>
-      <c r="C32" s="49" t="n">
+      <c r="C32" s="48" t="n">
         <v>46023</v>
       </c>
       <c r="D32" s="6" t="inlineStr">
@@ -3135,7 +3135,7 @@
           <t>ECIWAG</t>
         </is>
       </c>
-      <c r="N32" s="48" t="n">
+      <c r="N32" s="49" t="n">
         <v>45931</v>
       </c>
       <c r="O32" s="6" t="inlineStr">
@@ -3171,7 +3171,7 @@
           <t>INDPRO</t>
         </is>
       </c>
-      <c r="C33" s="49" t="n">
+      <c r="C33" s="48" t="n">
         <v>46023</v>
       </c>
       <c r="D33" s="6" t="inlineStr">
@@ -3210,7 +3210,7 @@
           <t>CES0500000003</t>
         </is>
       </c>
-      <c r="N33" s="48" t="n">
+      <c r="N33" s="49" t="n">
         <v>46023</v>
       </c>
       <c r="O33" s="6" t="inlineStr">
@@ -3250,7 +3250,7 @@
           <t>TCU</t>
         </is>
       </c>
-      <c r="C34" s="49" t="n">
+      <c r="C34" s="48" t="n">
         <v>46023</v>
       </c>
       <c r="D34" s="6" t="inlineStr">
@@ -3285,8 +3285,8 @@
           <t>RCES0500000003*</t>
         </is>
       </c>
-      <c r="N34" s="48" t="n">
-        <v>45962</v>
+      <c r="N34" s="49" t="n">
+        <v>45992</v>
       </c>
       <c r="O34" s="6" t="inlineStr">
         <is>
@@ -3299,19 +3299,19 @@
         </is>
       </c>
       <c r="Q34" s="38" t="n">
-        <v>0.01128441879087681</v>
+        <v>0.008019789135629696</v>
       </c>
       <c r="R34" s="38" t="n">
-        <v>0.0120947871629743</v>
+        <v>0.01084249628307491</v>
       </c>
       <c r="S34" s="38" t="n">
+        <v>0.01169114908209064</v>
+      </c>
+      <c r="T34" s="38" t="n">
         <v>0.01032118383222275</v>
       </c>
-      <c r="T34" s="38" t="n">
+      <c r="U34" s="23" t="n">
         <v>0.01194571058798364</v>
-      </c>
-      <c r="U34" s="23" t="n">
-        <v>0.01322369465705905</v>
       </c>
     </row>
     <row r="35" ht="31.5" customHeight="1">
@@ -3325,7 +3325,7 @@
           <t>PRS85006092</t>
         </is>
       </c>
-      <c r="C35" s="48" t="n">
+      <c r="C35" s="49" t="n">
         <v>45839</v>
       </c>
       <c r="D35" s="6" t="inlineStr">
@@ -3338,19 +3338,19 @@
           <t>Q</t>
         </is>
       </c>
-      <c r="F35" s="44" t="n">
+      <c r="F35" s="41" t="n">
         <v>4.9</v>
       </c>
-      <c r="G35" s="44" t="n">
+      <c r="G35" s="41" t="n">
         <v>4.1</v>
       </c>
-      <c r="H35" s="44" t="n">
+      <c r="H35" s="41" t="n">
         <v>-2.1</v>
       </c>
-      <c r="I35" s="44" t="n">
+      <c r="I35" s="41" t="n">
         <v>0.9</v>
       </c>
-      <c r="J35" s="44" t="n">
+      <c r="J35" s="41" t="n">
         <v>3.1</v>
       </c>
       <c r="K35" s="5" t="n"/>
@@ -3364,8 +3364,8 @@
           <t>RCES0500000003*</t>
         </is>
       </c>
-      <c r="N35" s="48" t="n">
-        <v>45962</v>
+      <c r="N35" s="49" t="n">
+        <v>45992</v>
       </c>
       <c r="O35" s="6" t="inlineStr">
         <is>
@@ -3378,29 +3378,33 @@
         </is>
       </c>
       <c r="Q35" s="38" t="n">
-        <v>0.00199332572360067</v>
+        <v>-0.00300711691046418</v>
       </c>
       <c r="R35" s="38" t="n">
-        <v>0.002492631234120024</v>
+        <v>0.001955057552418982</v>
       </c>
       <c r="S35" s="38" t="n">
+        <v>0.002092822632293601</v>
+      </c>
+      <c r="T35" s="38" t="n">
         <v>-0.0004224555765300897</v>
       </c>
-      <c r="T35" s="38" t="n">
+      <c r="U35" s="23" t="n">
         <v>0.001486198108683112</v>
       </c>
-      <c r="U35" s="23" t="n">
-        <v>0.001310931935978976</v>
-      </c>
     </row>
     <row r="36" ht="31.5" customHeight="1">
-      <c r="A36" s="33" t="n"/>
+      <c r="A36" s="33" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hou. Starts </t>
+        </is>
+      </c>
       <c r="B36" s="15" t="inlineStr">
         <is>
           <t>HOUST</t>
         </is>
       </c>
-      <c r="C36" s="49" t="n">
+      <c r="C36" s="48" t="n">
         <v>45992</v>
       </c>
       <c r="D36" s="6" t="inlineStr">
@@ -3435,8 +3439,8 @@
           <t>RCES0500000003*</t>
         </is>
       </c>
-      <c r="N36" s="48" t="n">
-        <v>45962</v>
+      <c r="N36" s="49" t="n">
+        <v>45992</v>
       </c>
       <c r="O36" s="6" t="inlineStr">
         <is>
@@ -3449,33 +3453,29 @@
         </is>
       </c>
       <c r="Q36" s="38" t="n">
-        <v>0.01128441879087681</v>
+        <v>0.008019789135629696</v>
       </c>
       <c r="R36" s="38" t="n">
-        <v>0.0120947871629743</v>
+        <v>0.01084249628307491</v>
       </c>
       <c r="S36" s="38" t="n">
+        <v>0.01169114908209064</v>
+      </c>
+      <c r="T36" s="38" t="n">
         <v>0.01032118383222275</v>
       </c>
-      <c r="T36" s="38" t="n">
+      <c r="U36" s="23" t="n">
         <v>0.01194571058798364</v>
       </c>
-      <c r="U36" s="23" t="n">
-        <v>0.01322369465705905</v>
-      </c>
     </row>
     <row r="37">
-      <c r="A37" s="33" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Hou. Starts </t>
-        </is>
-      </c>
+      <c r="A37" s="33" t="n"/>
       <c r="B37" s="15" t="inlineStr">
         <is>
           <t>HOUST</t>
         </is>
       </c>
-      <c r="C37" s="49" t="n">
+      <c r="C37" s="48" t="n">
         <v>45992</v>
       </c>
       <c r="D37" s="6" t="inlineStr">
@@ -3514,7 +3514,7 @@
           <t>CSUSHPINSA</t>
         </is>
       </c>
-      <c r="N37" s="48" t="n">
+      <c r="N37" s="49" t="n">
         <v>45962</v>
       </c>
       <c r="O37" s="6" t="inlineStr">
@@ -3554,7 +3554,7 @@
           <t>PERMIT</t>
         </is>
       </c>
-      <c r="C38" s="49" t="n">
+      <c r="C38" s="48" t="n">
         <v>45992</v>
       </c>
       <c r="D38" s="6" t="inlineStr">
@@ -3589,7 +3589,7 @@
           <t>CSUSHPINSA</t>
         </is>
       </c>
-      <c r="N38" s="48" t="n">
+      <c r="N38" s="49" t="n">
         <v>45962</v>
       </c>
       <c r="O38" s="6" t="inlineStr">
@@ -3625,7 +3625,7 @@
           <t>PERMIT</t>
         </is>
       </c>
-      <c r="C39" s="49" t="n">
+      <c r="C39" s="48" t="n">
         <v>45992</v>
       </c>
       <c r="D39" s="6" t="inlineStr">
@@ -3664,7 +3664,7 @@
           <t>TWEXBGSMTH</t>
         </is>
       </c>
-      <c r="N39" s="48" t="n">
+      <c r="N39" s="49" t="n">
         <v>46023</v>
       </c>
       <c r="O39" s="6" t="inlineStr">
@@ -3704,7 +3704,7 @@
           <t>HSN1F</t>
         </is>
       </c>
-      <c r="C40" s="48" t="n">
+      <c r="C40" s="49" t="n">
         <v>45931</v>
       </c>
       <c r="D40" s="6" t="inlineStr">
@@ -3739,7 +3739,7 @@
           <t>TWEXBGSMTH</t>
         </is>
       </c>
-      <c r="N40" s="48" t="n">
+      <c r="N40" s="49" t="n">
         <v>46023</v>
       </c>
       <c r="O40" s="6" t="inlineStr">
@@ -3775,7 +3775,7 @@
           <t>HSN1F</t>
         </is>
       </c>
-      <c r="C41" s="48" t="n">
+      <c r="C41" s="49" t="n">
         <v>45931</v>
       </c>
       <c r="D41" s="6" t="inlineStr">
@@ -3814,7 +3814,7 @@
           <t>IQ</t>
         </is>
       </c>
-      <c r="N41" s="48" t="n">
+      <c r="N41" s="49" t="n">
         <v>45992</v>
       </c>
       <c r="O41" s="6" t="inlineStr">
@@ -3854,7 +3854,7 @@
           <t>EXHOSLUSM495S</t>
         </is>
       </c>
-      <c r="C42" s="48" t="n">
+      <c r="C42" s="49" t="n">
         <v>46023</v>
       </c>
       <c r="D42" s="6" t="inlineStr">
@@ -3889,7 +3889,7 @@
           <t>IQ</t>
         </is>
       </c>
-      <c r="N42" s="48" t="n">
+      <c r="N42" s="49" t="n">
         <v>45992</v>
       </c>
       <c r="O42" s="6" t="inlineStr">
@@ -3925,7 +3925,7 @@
           <t>EXHOSLUSM495S</t>
         </is>
       </c>
-      <c r="C43" s="48" t="n">
+      <c r="C43" s="49" t="n">
         <v>46023</v>
       </c>
       <c r="D43" s="6" t="inlineStr">
@@ -3964,7 +3964,7 @@
           <t>IR</t>
         </is>
       </c>
-      <c r="N43" s="48" t="n">
+      <c r="N43" s="49" t="n">
         <v>45992</v>
       </c>
       <c r="O43" s="6" t="inlineStr">
@@ -4005,7 +4005,7 @@
         </is>
       </c>
       <c r="C44" s="48" t="n">
-        <v>45839</v>
+        <v>45931</v>
       </c>
       <c r="D44" s="6" t="inlineStr">
         <is>
@@ -4018,19 +4018,19 @@
         </is>
       </c>
       <c r="F44" s="24" t="n">
+        <v>5346.421</v>
+      </c>
+      <c r="G44" s="24" t="n">
         <v>5324.402</v>
       </c>
-      <c r="G44" s="24" t="n">
+      <c r="H44" s="24" t="n">
         <v>5236.97</v>
       </c>
-      <c r="H44" s="24" t="n">
+      <c r="I44" s="24" t="n">
         <v>5195.517</v>
       </c>
-      <c r="I44" s="24" t="n">
+      <c r="J44" s="24" t="n">
         <v>5150.725</v>
-      </c>
-      <c r="J44" s="24" t="n">
-        <v>5086.922</v>
       </c>
       <c r="K44" s="5" t="n"/>
       <c r="L44" s="28" t="n"/>
@@ -4039,7 +4039,7 @@
           <t>IR</t>
         </is>
       </c>
-      <c r="N44" s="48" t="n">
+      <c r="N44" s="49" t="n">
         <v>45992</v>
       </c>
       <c r="O44" s="6" t="inlineStr">
@@ -4076,7 +4076,7 @@
         </is>
       </c>
       <c r="C45" s="48" t="n">
-        <v>45839</v>
+        <v>45931</v>
       </c>
       <c r="D45" s="6" t="inlineStr">
         <is>
@@ -4089,19 +4089,19 @@
         </is>
       </c>
       <c r="F45" s="38" t="n">
+        <v>0.004135487891410161</v>
+      </c>
+      <c r="G45" s="38" t="n">
         <v>0.01669515005814426</v>
       </c>
-      <c r="G45" s="38" t="n">
+      <c r="H45" s="38" t="n">
         <v>0.007978609251013902</v>
       </c>
-      <c r="H45" s="38" t="n">
+      <c r="I45" s="38" t="n">
         <v>0.008696251498575336</v>
       </c>
-      <c r="I45" s="38" t="n">
+      <c r="J45" s="38" t="n">
         <v>0.01254255520332359</v>
-      </c>
-      <c r="J45" s="38" t="n">
-        <v>0.01837222105442282</v>
       </c>
       <c r="K45" s="5" t="n"/>
       <c r="L45" s="28" t="n"/>
@@ -4126,7 +4126,7 @@
           <t>BOPTEXP</t>
         </is>
       </c>
-      <c r="C46" s="49" t="n">
+      <c r="C46" s="48" t="n">
         <v>45992</v>
       </c>
       <c r="D46" s="6" t="inlineStr">
@@ -4213,7 +4213,7 @@
           <t>BOPTEXP</t>
         </is>
       </c>
-      <c r="C47" s="49" t="n">
+      <c r="C47" s="48" t="n">
         <v>45992</v>
       </c>
       <c r="D47" s="6" t="inlineStr">
@@ -4252,8 +4252,8 @@
           <t>DFF</t>
         </is>
       </c>
-      <c r="N47" s="49" t="n">
-        <v>46070</v>
+      <c r="N47" s="48" t="n">
+        <v>46071</v>
       </c>
       <c r="O47" s="6" t="inlineStr">
         <is>
@@ -4292,7 +4292,7 @@
           <t>BOPTIMP</t>
         </is>
       </c>
-      <c r="C48" s="49" t="n">
+      <c r="C48" s="48" t="n">
         <v>45992</v>
       </c>
       <c r="D48" s="6" t="inlineStr">
@@ -4331,8 +4331,8 @@
           <t>DGS2</t>
         </is>
       </c>
-      <c r="N48" s="49" t="n">
-        <v>46070</v>
+      <c r="N48" s="48" t="n">
+        <v>46071</v>
       </c>
       <c r="O48" s="6" t="inlineStr">
         <is>
@@ -4345,19 +4345,19 @@
         </is>
       </c>
       <c r="Q48" s="6" t="n">
+        <v>3.47</v>
+      </c>
+      <c r="R48" s="6" t="n">
         <v>3.43</v>
       </c>
-      <c r="R48" s="6" t="n">
+      <c r="S48" s="6" t="n">
         <v>3.4</v>
       </c>
-      <c r="S48" s="6" t="n">
+      <c r="T48" s="6" t="n">
         <v>3.47</v>
       </c>
-      <c r="T48" s="6" t="n">
+      <c r="U48" s="21" t="n">
         <v>3.52</v>
-      </c>
-      <c r="U48" s="21" t="n">
-        <v>3.45</v>
       </c>
     </row>
     <row r="49">
@@ -4367,7 +4367,7 @@
           <t>BOPTIMP</t>
         </is>
       </c>
-      <c r="C49" s="49" t="n">
+      <c r="C49" s="48" t="n">
         <v>45992</v>
       </c>
       <c r="D49" s="6" t="inlineStr">
@@ -4406,8 +4406,8 @@
           <t>DGS5</t>
         </is>
       </c>
-      <c r="N49" s="49" t="n">
-        <v>46070</v>
+      <c r="N49" s="48" t="n">
+        <v>46071</v>
       </c>
       <c r="O49" s="6" t="inlineStr">
         <is>
@@ -4420,19 +4420,19 @@
         </is>
       </c>
       <c r="Q49" s="6" t="n">
+        <v>3.66</v>
+      </c>
+      <c r="R49" s="6" t="n">
         <v>3.63</v>
       </c>
-      <c r="R49" s="6" t="n">
+      <c r="S49" s="6" t="n">
         <v>3.61</v>
       </c>
-      <c r="S49" s="6" t="n">
+      <c r="T49" s="6" t="n">
         <v>3.67</v>
       </c>
-      <c r="T49" s="6" t="n">
+      <c r="U49" s="21" t="n">
         <v>3.75</v>
-      </c>
-      <c r="U49" s="21" t="n">
-        <v>3.7</v>
       </c>
     </row>
     <row r="50">
@@ -4446,7 +4446,7 @@
           <t>BOPSTB</t>
         </is>
       </c>
-      <c r="C50" s="49" t="n">
+      <c r="C50" s="48" t="n">
         <v>45992</v>
       </c>
       <c r="D50" s="6" t="inlineStr">
@@ -4485,8 +4485,8 @@
           <t>DGS10</t>
         </is>
       </c>
-      <c r="N50" s="49" t="n">
-        <v>46070</v>
+      <c r="N50" s="48" t="n">
+        <v>46071</v>
       </c>
       <c r="O50" s="6" t="inlineStr">
         <is>
@@ -4499,19 +4499,19 @@
         </is>
       </c>
       <c r="Q50" s="6" t="n">
+        <v>4.09</v>
+      </c>
+      <c r="R50" s="6" t="n">
         <v>4.05</v>
       </c>
-      <c r="R50" s="6" t="n">
+      <c r="S50" s="6" t="n">
         <v>4.04</v>
       </c>
-      <c r="S50" s="6" t="n">
+      <c r="T50" s="6" t="n">
         <v>4.09</v>
       </c>
-      <c r="T50" s="6" t="n">
+      <c r="U50" s="21" t="n">
         <v>4.18</v>
-      </c>
-      <c r="U50" s="21" t="n">
-        <v>4.16</v>
       </c>
     </row>
     <row r="51" ht="31.5" customHeight="1">
@@ -4521,7 +4521,7 @@
           <t>BOPSTB</t>
         </is>
       </c>
-      <c r="C51" s="49" t="n">
+      <c r="C51" s="48" t="n">
         <v>45992</v>
       </c>
       <c r="D51" s="6" t="inlineStr">
@@ -4561,7 +4561,7 @@
         </is>
       </c>
       <c r="N51" s="48" t="n">
-        <v>46062</v>
+        <v>46069</v>
       </c>
       <c r="O51" s="6" t="inlineStr">
         <is>
@@ -4574,19 +4574,19 @@
         </is>
       </c>
       <c r="Q51" s="6" t="n">
+        <v>6.01</v>
+      </c>
+      <c r="R51" s="6" t="n">
         <v>6.09</v>
       </c>
-      <c r="R51" s="6" t="n">
+      <c r="S51" s="6" t="n">
         <v>6.11</v>
       </c>
-      <c r="S51" s="6" t="n">
+      <c r="T51" s="6" t="n">
         <v>6.1</v>
       </c>
-      <c r="T51" s="6" t="n">
+      <c r="U51" s="21" t="n">
         <v>6.09</v>
-      </c>
-      <c r="U51" s="21" t="n">
-        <v>6.06</v>
       </c>
     </row>
     <row r="52" ht="16.15" customHeight="1" thickBot="1">
@@ -4612,7 +4612,7 @@
         </is>
       </c>
       <c r="N52" s="50" t="n">
-        <v>46070</v>
+        <v>46071</v>
       </c>
       <c r="O52" s="9" t="inlineStr">
         <is>
@@ -4625,19 +4625,19 @@
         </is>
       </c>
       <c r="Q52" s="9" t="n">
+        <v>5.76</v>
+      </c>
+      <c r="R52" s="9" t="n">
         <v>5.75</v>
       </c>
-      <c r="R52" s="9" t="n">
+      <c r="S52" s="9" t="n">
         <v>5.76</v>
       </c>
-      <c r="S52" s="9" t="n">
+      <c r="T52" s="9" t="n">
         <v>5.77</v>
       </c>
-      <c r="T52" s="9" t="n">
+      <c r="U52" s="22" t="n">
         <v>5.85</v>
-      </c>
-      <c r="U52" s="22" t="n">
-        <v>5.82</v>
       </c>
     </row>
     <row r="53" ht="21" customHeight="1">

</xml_diff>

<commit_message>
Update dashboards - 2026-02-21
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -62,18 +62,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -319,9 +313,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -349,18 +340,21 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="168" fontId="1" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="168" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="3" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="168" fontId="1" fillId="2" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -728,8 +722,8 @@
   </sheetPr>
   <dimension ref="A1:U80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="76" zoomScaleNormal="51" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="400" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9.1328125" defaultRowHeight="15.75"/>
@@ -884,7 +878,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="33" t="inlineStr">
+      <c r="A3" s="44" t="inlineStr">
         <is>
           <t>RGDP</t>
         </is>
@@ -1017,16 +1011,16 @@
           <t>M</t>
         </is>
       </c>
-      <c r="Q4" s="38" t="n">
+      <c r="Q4" s="37" t="n">
         <v>0.002268304395076705</v>
       </c>
-      <c r="R4" s="38" t="n">
+      <c r="R4" s="37" t="n">
         <v>0.001143283054144875</v>
       </c>
-      <c r="S4" s="38" t="n">
+      <c r="S4" s="37" t="n">
         <v>0.002340601850973247</v>
       </c>
-      <c r="T4" s="38" t="n">
+      <c r="T4" s="37" t="n">
         <v>0.002931400170945582</v>
       </c>
       <c r="U4" s="23" t="n">
@@ -1034,7 +1028,7 @@
       </c>
     </row>
     <row r="5" ht="31.5" customHeight="1">
-      <c r="A5" s="33" t="inlineStr">
+      <c r="A5" s="44" t="inlineStr">
         <is>
           <t>NGDP</t>
         </is>
@@ -1113,7 +1107,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="33" t="n"/>
+      <c r="A6" s="44" t="n"/>
       <c r="B6" s="15" t="inlineStr">
         <is>
           <t>NGDPSAXDCUSQ</t>
@@ -1188,7 +1182,7 @@
       </c>
     </row>
     <row r="7" ht="16.15" customHeight="1">
-      <c r="A7" s="33" t="inlineStr">
+      <c r="A7" s="44" t="inlineStr">
         <is>
           <t>GDP Nowcast</t>
         </is>
@@ -1211,19 +1205,19 @@
           <t>Q</t>
         </is>
       </c>
-      <c r="F7" s="41" t="n">
+      <c r="F7" s="40" t="n">
         <v>4.2373</v>
       </c>
-      <c r="G7" s="41" t="n">
+      <c r="G7" s="40" t="n">
         <v>3.4728</v>
       </c>
-      <c r="H7" s="41" t="n">
+      <c r="H7" s="40" t="n">
         <v>2.902</v>
       </c>
-      <c r="I7" s="41" t="n">
+      <c r="I7" s="40" t="n">
         <v>-2.7318</v>
       </c>
-      <c r="J7" s="41" t="n">
+      <c r="J7" s="40" t="n">
         <v>2.2711</v>
       </c>
       <c r="K7" s="5" t="n"/>
@@ -1267,7 +1261,7 @@
       </c>
     </row>
     <row r="8" ht="31.5" customHeight="1">
-      <c r="A8" s="33" t="inlineStr">
+      <c r="A8" s="44" t="inlineStr">
         <is>
           <t>Smoothed Recession Prob</t>
         </is>
@@ -1346,7 +1340,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="33" t="inlineStr">
+      <c r="A9" s="44" t="inlineStr">
         <is>
           <t>RPCE</t>
         </is>
@@ -1425,7 +1419,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="33" t="n"/>
+      <c r="A10" s="44" t="n"/>
       <c r="B10" s="15" t="inlineStr">
         <is>
           <t>PCECC96</t>
@@ -1500,7 +1494,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="33" t="inlineStr">
+      <c r="A11" s="44" t="inlineStr">
         <is>
           <t>RPCE Dur</t>
         </is>
@@ -1579,7 +1573,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="33" t="n"/>
+      <c r="A12" s="44" t="n"/>
       <c r="B12" s="15" t="inlineStr">
         <is>
           <t>PCEDGC96</t>
@@ -1654,7 +1648,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="35" t="inlineStr">
+      <c r="A13" s="44" t="inlineStr">
         <is>
           <t>RPCE Ndur</t>
         </is>
@@ -1733,7 +1727,7 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="34" t="n"/>
+      <c r="A14" s="44" t="n"/>
       <c r="B14" s="15" t="inlineStr">
         <is>
           <t>PCENDC96</t>
@@ -1808,7 +1802,7 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="33" t="inlineStr">
+      <c r="A15" s="44" t="inlineStr">
         <is>
           <t>RPCE Serv.</t>
         </is>
@@ -1887,7 +1881,7 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="33" t="n"/>
+      <c r="A16" s="44" t="n"/>
       <c r="B16" s="15" t="inlineStr">
         <is>
           <t>PCESC96</t>
@@ -1934,7 +1928,7 @@
       <c r="U16" s="21" t="n"/>
     </row>
     <row r="17" ht="16.15" customHeight="1" thickBot="1">
-      <c r="A17" s="33" t="inlineStr">
+      <c r="A17" s="44" t="inlineStr">
         <is>
           <t>Retail Sales</t>
         </is>
@@ -2025,7 +2019,7 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="33" t="n"/>
+      <c r="A18" s="44" t="n"/>
       <c r="B18" s="15" t="inlineStr">
         <is>
           <t>RSAFS</t>
@@ -2083,16 +2077,16 @@
           <t>M</t>
         </is>
       </c>
-      <c r="Q18" s="38" t="n">
+      <c r="Q18" s="37" t="n">
         <v>0.00170842649932057</v>
       </c>
-      <c r="R18" s="38" t="n">
+      <c r="R18" s="37" t="n">
         <v>0.00297788428704604</v>
       </c>
-      <c r="S18" s="38" t="n">
+      <c r="S18" s="37" t="n">
         <v/>
       </c>
-      <c r="T18" s="38" t="n">
+      <c r="T18" s="37" t="n">
         <v/>
       </c>
       <c r="U18" s="23" t="n">
@@ -2100,7 +2094,7 @@
       </c>
     </row>
     <row r="19" ht="31.5" customHeight="1">
-      <c r="A19" s="33" t="inlineStr">
+      <c r="A19" s="44" t="inlineStr">
         <is>
           <t>Real Disposable Personal Income</t>
         </is>
@@ -2158,16 +2152,16 @@
           <t>M</t>
         </is>
       </c>
-      <c r="Q19" s="38" t="n">
+      <c r="Q19" s="37" t="n">
         <v>0.02391201432150015</v>
       </c>
-      <c r="R19" s="38" t="n">
+      <c r="R19" s="37" t="n">
         <v>0.02653304114557758</v>
       </c>
-      <c r="S19" s="38" t="n">
+      <c r="S19" s="37" t="n">
         <v>0.02696443916493949</v>
       </c>
-      <c r="T19" s="38" t="n">
+      <c r="T19" s="37" t="n">
         <v/>
       </c>
       <c r="U19" s="23" t="n">
@@ -2175,7 +2169,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="33" t="n"/>
+      <c r="A20" s="44" t="n"/>
       <c r="B20" s="15" t="inlineStr">
         <is>
           <t>DSPIC96</t>
@@ -2233,16 +2227,16 @@
           <t>M</t>
         </is>
       </c>
-      <c r="Q20" s="38" t="n">
+      <c r="Q20" s="37" t="n">
         <v>0.002950448142634121</v>
       </c>
-      <c r="R20" s="38" t="n">
+      <c r="R20" s="37" t="n">
         <v>0.002329002576704653</v>
       </c>
-      <c r="S20" s="38" t="n">
+      <c r="S20" s="37" t="n">
         <v/>
       </c>
-      <c r="T20" s="38" t="n">
+      <c r="T20" s="37" t="n">
         <v/>
       </c>
       <c r="U20" s="23" t="n">
@@ -2250,7 +2244,7 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="33" t="inlineStr">
+      <c r="A21" s="44" t="inlineStr">
         <is>
           <t>Personal Saving Rate</t>
         </is>
@@ -2308,16 +2302,16 @@
           <t>M</t>
         </is>
       </c>
-      <c r="Q21" s="38" t="n">
+      <c r="Q21" s="37" t="n">
         <v>0.02512028782828883</v>
       </c>
-      <c r="R21" s="38" t="n">
+      <c r="R21" s="37" t="n">
         <v>0.02646484707309002</v>
       </c>
-      <c r="S21" s="38" t="n">
+      <c r="S21" s="37" t="n">
         <v>0.02599044806094405</v>
       </c>
-      <c r="T21" s="38" t="n">
+      <c r="T21" s="37" t="n">
         <v/>
       </c>
       <c r="U21" s="23" t="n">
@@ -2325,7 +2319,7 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="33" t="inlineStr">
+      <c r="A22" s="44" t="inlineStr">
         <is>
           <t>Vehicle Sales</t>
         </is>
@@ -2349,19 +2343,19 @@
         </is>
       </c>
       <c r="F22" s="24" t="n">
-        <v>15.396</v>
+        <v>15.199</v>
       </c>
       <c r="G22" s="24" t="n">
-        <v>16.394</v>
+        <v>16.401</v>
       </c>
       <c r="H22" s="24" t="n">
-        <v>16.003</v>
+        <v>16.006</v>
       </c>
       <c r="I22" s="24" t="n">
-        <v>15.836</v>
+        <v>15.843</v>
       </c>
       <c r="J22" s="24" t="n">
-        <v>16.982</v>
+        <v>16.985</v>
       </c>
       <c r="K22" s="5" t="n"/>
       <c r="L22" s="28" t="inlineStr">
@@ -2387,16 +2381,16 @@
           <t>M</t>
         </is>
       </c>
-      <c r="Q22" s="38" t="n">
+      <c r="Q22" s="37" t="n">
         <v>0.004902708763177221</v>
       </c>
-      <c r="R22" s="38" t="n">
+      <c r="R22" s="37" t="n">
         <v>0.002380714879468115</v>
       </c>
-      <c r="S22" s="38" t="n">
+      <c r="S22" s="37" t="n">
         <v>0.0008919003467759978</v>
       </c>
-      <c r="T22" s="38" t="n">
+      <c r="T22" s="37" t="n">
         <v>0.006579167755378368</v>
       </c>
       <c r="U22" s="23" t="n">
@@ -2404,7 +2398,7 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="33" t="n"/>
+      <c r="A23" s="44" t="n"/>
       <c r="B23" s="15" t="inlineStr">
         <is>
           <t>TOTALSA</t>
@@ -2424,19 +2418,19 @@
         </is>
       </c>
       <c r="F23" s="25" t="n">
-        <v>-0.03473354231974912</v>
+        <v>-0.04708463949843257</v>
       </c>
       <c r="G23" s="25" t="n">
-        <v>-0.05242471533437374</v>
+        <v>-0.0520201144442517</v>
       </c>
       <c r="H23" s="25" t="n">
-        <v>-0.0535249585994796</v>
+        <v>-0.05334752779749237</v>
       </c>
       <c r="I23" s="25" t="n">
-        <v>-0.03983508154974828</v>
+        <v>-0.03941065906748309</v>
       </c>
       <c r="J23" s="25" t="n">
-        <v>0.03922648552720141</v>
+        <v>0.03941007282296054</v>
       </c>
       <c r="K23" s="5" t="n"/>
       <c r="M23" s="15" t="inlineStr">
@@ -2457,16 +2451,16 @@
           <t>M</t>
         </is>
       </c>
-      <c r="Q23" s="38" t="n">
+      <c r="Q23" s="37" t="n">
         <v>0.02953930644481603</v>
       </c>
-      <c r="R23" s="38" t="n">
+      <c r="R23" s="37" t="n">
         <v>0.02966029332404323</v>
       </c>
-      <c r="S23" s="38" t="n">
+      <c r="S23" s="37" t="n">
         <v>0.02826137498119562</v>
       </c>
-      <c r="T23" s="38" t="n">
+      <c r="T23" s="37" t="n">
         <v>0.03051607769973669</v>
       </c>
       <c r="U23" s="23" t="n">
@@ -2474,7 +2468,7 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="33" t="inlineStr">
+      <c r="A24" s="44" t="inlineStr">
         <is>
           <t>Cons Credit - Revolving</t>
         </is>
@@ -2497,19 +2491,19 @@
           <t>M</t>
         </is>
       </c>
-      <c r="F24" s="38" t="n">
+      <c r="F24" s="37" t="n">
         <v>0.0105318556006937</v>
       </c>
-      <c r="G24" s="38" t="n">
+      <c r="G24" s="37" t="n">
         <v>-0.001281418924231392</v>
       </c>
-      <c r="H24" s="38" t="n">
+      <c r="H24" s="37" t="n">
         <v>0.004454853076971466</v>
       </c>
-      <c r="I24" s="38" t="n">
+      <c r="I24" s="37" t="n">
         <v>0.00339828596255809</v>
       </c>
-      <c r="J24" s="38" t="n">
+      <c r="J24" s="37" t="n">
         <v>-0.003651114145611811</v>
       </c>
       <c r="K24" s="5" t="n"/>
@@ -2536,16 +2530,16 @@
           <t>M</t>
         </is>
       </c>
-      <c r="Q24" s="38" t="n">
+      <c r="Q24" s="37" t="n">
         <v>0.003558357849066329</v>
       </c>
-      <c r="R24" s="38" t="n">
+      <c r="R24" s="37" t="n">
         <v>0.002111370905308885</v>
       </c>
-      <c r="S24" s="38" t="n">
+      <c r="S24" s="37" t="n">
         <v>0.001990205680705293</v>
       </c>
-      <c r="T24" s="38" t="n">
+      <c r="T24" s="37" t="n">
         <v>0.002608155986582039</v>
       </c>
       <c r="U24" s="23" t="n">
@@ -2553,7 +2547,7 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="33" t="inlineStr">
+      <c r="A25" s="44" t="inlineStr">
         <is>
           <t>Cons Credit - NonRevolving</t>
         </is>
@@ -2576,19 +2570,19 @@
           <t>M</t>
         </is>
       </c>
-      <c r="F25" s="38" t="n">
+      <c r="F25" s="37" t="n">
         <v>0.002704782960157415</v>
       </c>
-      <c r="G25" s="38" t="n">
+      <c r="G25" s="37" t="n">
         <v>0.001696137399219255</v>
       </c>
-      <c r="H25" s="38" t="n">
+      <c r="H25" s="37" t="n">
         <v>0.0009232413445350307</v>
       </c>
-      <c r="I25" s="38" t="n">
+      <c r="I25" s="37" t="n">
         <v>0.001873721239173287</v>
       </c>
-      <c r="J25" s="38" t="n">
+      <c r="J25" s="37" t="n">
         <v>0.001994229089696598</v>
       </c>
       <c r="K25" s="5" t="n"/>
@@ -2611,16 +2605,16 @@
           <t>M</t>
         </is>
       </c>
-      <c r="Q25" s="38" t="n">
+      <c r="Q25" s="37" t="n">
         <v>0.02901287416285929</v>
       </c>
-      <c r="R25" s="38" t="n">
+      <c r="R25" s="37" t="n">
         <v>0.02817782841371343</v>
       </c>
-      <c r="S25" s="38" t="n">
+      <c r="S25" s="37" t="n">
         <v>0.02719006538467721</v>
       </c>
-      <c r="T25" s="38" t="n">
+      <c r="T25" s="37" t="n">
         <v>0.02787442414870654</v>
       </c>
       <c r="U25" s="23" t="n">
@@ -2628,7 +2622,7 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="33" t="inlineStr">
+      <c r="A26" s="44" t="inlineStr">
         <is>
           <t>Gross Priv Fixed Inv Non Res</t>
         </is>
@@ -2651,19 +2645,19 @@
           <t>Q</t>
         </is>
       </c>
-      <c r="F26" s="38" t="n">
+      <c r="F26" s="37" t="n">
         <v>0.009152775755367104</v>
       </c>
-      <c r="G26" s="38" t="n">
+      <c r="G26" s="37" t="n">
         <v>0.007794617579222285</v>
       </c>
-      <c r="H26" s="38" t="n">
+      <c r="H26" s="37" t="n">
         <v>0.01778138610314484</v>
       </c>
-      <c r="I26" s="38" t="n">
+      <c r="I26" s="37" t="n">
         <v>0.02303791460563676</v>
       </c>
-      <c r="J26" s="38" t="n">
+      <c r="J26" s="37" t="n">
         <v>-0.009359213919614473</v>
       </c>
       <c r="K26" s="5" t="n"/>
@@ -2690,16 +2684,16 @@
           <t>M</t>
         </is>
       </c>
-      <c r="Q26" s="38" t="n">
+      <c r="Q26" s="37" t="n">
         <v>0.003553916761463993</v>
       </c>
-      <c r="R26" s="38" t="n">
+      <c r="R26" s="37" t="n">
         <v>0.001673844026027105</v>
       </c>
-      <c r="S26" s="38" t="n">
+      <c r="S26" s="37" t="n">
         <v>0.002347306898561774</v>
       </c>
-      <c r="T26" s="38" t="n">
+      <c r="T26" s="37" t="n">
         <v>0.001894029073346237</v>
       </c>
       <c r="U26" s="23" t="n">
@@ -2707,7 +2701,7 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="33" t="inlineStr">
+      <c r="A27" s="44" t="inlineStr">
         <is>
           <t>Gross Priv Fixed Inv Res</t>
         </is>
@@ -2730,19 +2724,19 @@
           <t>Q</t>
         </is>
       </c>
-      <c r="F27" s="38" t="n">
+      <c r="F27" s="37" t="n">
         <v>-0.003824604651284313</v>
       </c>
-      <c r="G27" s="38" t="n">
+      <c r="G27" s="37" t="n">
         <v>-0.01832684674964358</v>
       </c>
-      <c r="H27" s="38" t="n">
+      <c r="H27" s="37" t="n">
         <v>-0.01299350008050415</v>
       </c>
-      <c r="I27" s="38" t="n">
+      <c r="I27" s="37" t="n">
         <v>-0.002410568051752549</v>
       </c>
-      <c r="J27" s="38" t="n">
+      <c r="J27" s="37" t="n">
         <v>0.01049622222903812</v>
       </c>
       <c r="K27" s="5" t="n"/>
@@ -2765,16 +2759,16 @@
           <t>M</t>
         </is>
       </c>
-      <c r="Q27" s="38" t="n">
+      <c r="Q27" s="37" t="n">
         <v>0.02996875905826282</v>
       </c>
-      <c r="R27" s="38" t="n">
+      <c r="R27" s="37" t="n">
         <v>0.02825865991190849</v>
       </c>
-      <c r="S27" s="38" t="n">
+      <c r="S27" s="37" t="n">
         <v>0.02761806318237614</v>
       </c>
-      <c r="T27" s="38" t="n">
+      <c r="T27" s="37" t="n">
         <v>0.02825069249833962</v>
       </c>
       <c r="U27" s="23" t="n">
@@ -2782,7 +2776,7 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="33" t="inlineStr">
+      <c r="A28" s="44" t="inlineStr">
         <is>
           <t>Dur. Order</t>
         </is>
@@ -2832,7 +2826,7 @@
         </is>
       </c>
       <c r="N28" s="49" t="n">
-        <v>45992</v>
+        <v>46023</v>
       </c>
       <c r="O28" s="6" t="inlineStr">
         <is>
@@ -2845,23 +2839,23 @@
         </is>
       </c>
       <c r="Q28" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="R28" s="6" t="n">
         <v>4.2</v>
       </c>
-      <c r="R28" s="6" t="n">
+      <c r="S28" s="6" t="n">
         <v>4.5</v>
       </c>
-      <c r="S28" s="6" t="n">
+      <c r="T28" s="6" t="n">
         <v>4.6</v>
       </c>
-      <c r="T28" s="6" t="n">
+      <c r="U28" s="21" t="n">
         <v>4.7</v>
       </c>
-      <c r="U28" s="21" t="n">
-        <v>4.8</v>
-      </c>
     </row>
     <row r="29">
-      <c r="A29" s="33" t="n"/>
+      <c r="A29" s="44" t="n"/>
       <c r="B29" s="15" t="inlineStr">
         <is>
           <t>DGORDER</t>
@@ -2907,7 +2901,7 @@
         </is>
       </c>
       <c r="N29" s="48" t="n">
-        <v>46072</v>
+        <v>46073</v>
       </c>
       <c r="O29" s="6" t="inlineStr">
         <is>
@@ -2920,23 +2914,23 @@
         </is>
       </c>
       <c r="Q29" s="6" t="n">
-        <v>2.15</v>
+        <v>2.13</v>
       </c>
       <c r="R29" s="6" t="n">
         <v>2.15</v>
       </c>
       <c r="S29" s="6" t="n">
+        <v>2.15</v>
+      </c>
+      <c r="T29" s="6" t="n">
         <v>2.13</v>
       </c>
-      <c r="T29" s="6" t="n">
+      <c r="U29" s="21" t="n">
         <v>2.12</v>
       </c>
-      <c r="U29" s="21" t="n">
-        <v>2.13</v>
-      </c>
     </row>
     <row r="30">
-      <c r="A30" s="33" t="inlineStr">
+      <c r="A30" s="44" t="inlineStr">
         <is>
           <t>Dur Orders Non Def x Aicraft</t>
         </is>
@@ -2986,7 +2980,7 @@
         </is>
       </c>
       <c r="N30" s="48" t="n">
-        <v>46072</v>
+        <v>46073</v>
       </c>
       <c r="O30" s="6" t="inlineStr">
         <is>
@@ -2999,23 +2993,23 @@
         </is>
       </c>
       <c r="Q30" s="6" t="n">
-        <v>2.29</v>
+        <v>2.28</v>
       </c>
       <c r="R30" s="6" t="n">
         <v>2.29</v>
       </c>
       <c r="S30" s="6" t="n">
+        <v>2.29</v>
+      </c>
+      <c r="T30" s="6" t="n">
         <v>2.26</v>
       </c>
-      <c r="T30" s="6" t="n">
+      <c r="U30" s="21" t="n">
         <v>2.27</v>
       </c>
-      <c r="U30" s="21" t="n">
-        <v>2.29</v>
-      </c>
     </row>
     <row r="31">
-      <c r="A31" s="33" t="n"/>
+      <c r="A31" s="44" t="n"/>
       <c r="B31" s="15" t="inlineStr">
         <is>
           <t>ADXDNO</t>
@@ -3073,16 +3067,16 @@
           <t>Q</t>
         </is>
       </c>
-      <c r="Q31" s="38" t="n">
+      <c r="Q31" s="37" t="n">
         <v>0.007310493043885868</v>
       </c>
-      <c r="R31" s="38" t="n">
+      <c r="R31" s="37" t="n">
         <v>0.007996957929548465</v>
       </c>
-      <c r="S31" s="38" t="n">
+      <c r="S31" s="37" t="n">
         <v>0.01027939464493599</v>
       </c>
-      <c r="T31" s="38" t="n">
+      <c r="T31" s="37" t="n">
         <v>0.007624633431085215</v>
       </c>
       <c r="U31" s="23" t="n">
@@ -3090,7 +3084,7 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="33" t="inlineStr">
+      <c r="A32" s="44" t="inlineStr">
         <is>
           <t>IP</t>
         </is>
@@ -3148,16 +3142,16 @@
           <t>Q</t>
         </is>
       </c>
-      <c r="Q32" s="38" t="n">
+      <c r="Q32" s="37" t="n">
         <v>0.03362463343108507</v>
       </c>
-      <c r="R32" s="38" t="n">
+      <c r="R32" s="37" t="n">
         <v>0.03584369449378332</v>
       </c>
-      <c r="S32" s="38" t="n">
+      <c r="S32" s="37" t="n">
         <v>0.03559665871121723</v>
       </c>
-      <c r="T32" s="38" t="n">
+      <c r="T32" s="37" t="n">
         <v>0.03369434416365838</v>
       </c>
       <c r="U32" s="23" t="n">
@@ -3165,7 +3159,7 @@
       </c>
     </row>
     <row r="33" ht="31.5" customHeight="1">
-      <c r="A33" s="33" t="n"/>
+      <c r="A33" s="44" t="n"/>
       <c r="B33" s="15" t="inlineStr">
         <is>
           <t>INDPRO</t>
@@ -3223,16 +3217,16 @@
           <t>M</t>
         </is>
       </c>
-      <c r="Q33" s="38" t="n">
+      <c r="Q33" s="37" t="n">
         <v>0.004051863857374327</v>
       </c>
-      <c r="R33" s="38" t="n">
+      <c r="R33" s="37" t="n">
         <v>0.000540540540540535</v>
       </c>
-      <c r="S33" s="38" t="n">
+      <c r="S33" s="37" t="n">
         <v>0.00407055630936215</v>
       </c>
-      <c r="T33" s="38" t="n">
+      <c r="T33" s="37" t="n">
         <v>0.004087193460490468</v>
       </c>
       <c r="U33" s="23" t="n">
@@ -3240,7 +3234,7 @@
       </c>
     </row>
     <row r="34" ht="31.5" customHeight="1">
-      <c r="A34" s="33" t="inlineStr">
+      <c r="A34" s="44" t="inlineStr">
         <is>
           <t>Cap Util</t>
         </is>
@@ -3298,16 +3292,16 @@
           <t>M</t>
         </is>
       </c>
-      <c r="Q34" s="38" t="n">
+      <c r="Q34" s="37" t="n">
         <v>0.008019789135629696</v>
       </c>
-      <c r="R34" s="38" t="n">
+      <c r="R34" s="37" t="n">
         <v>0.01084249628307491</v>
       </c>
-      <c r="S34" s="38" t="n">
+      <c r="S34" s="37" t="n">
         <v>0.01169114908209064</v>
       </c>
-      <c r="T34" s="38" t="n">
+      <c r="T34" s="37" t="n">
         <v>0.01032118383222275</v>
       </c>
       <c r="U34" s="23" t="n">
@@ -3315,7 +3309,7 @@
       </c>
     </row>
     <row r="35" ht="31.5" customHeight="1">
-      <c r="A35" s="33" t="inlineStr">
+      <c r="A35" s="44" t="inlineStr">
         <is>
           <t xml:space="preserve">Productivity </t>
         </is>
@@ -3338,19 +3332,19 @@
           <t>Q</t>
         </is>
       </c>
-      <c r="F35" s="41" t="n">
+      <c r="F35" s="40" t="n">
         <v>4.9</v>
       </c>
-      <c r="G35" s="41" t="n">
+      <c r="G35" s="40" t="n">
         <v>4.1</v>
       </c>
-      <c r="H35" s="41" t="n">
+      <c r="H35" s="40" t="n">
         <v>-2.1</v>
       </c>
-      <c r="I35" s="41" t="n">
+      <c r="I35" s="40" t="n">
         <v>0.9</v>
       </c>
-      <c r="J35" s="41" t="n">
+      <c r="J35" s="40" t="n">
         <v>3.1</v>
       </c>
       <c r="K35" s="5" t="n"/>
@@ -3377,16 +3371,16 @@
           <t>M</t>
         </is>
       </c>
-      <c r="Q35" s="38" t="n">
+      <c r="Q35" s="37" t="n">
         <v>-0.00300711691046418</v>
       </c>
-      <c r="R35" s="38" t="n">
+      <c r="R35" s="37" t="n">
         <v>0.001955057552418982</v>
       </c>
-      <c r="S35" s="38" t="n">
+      <c r="S35" s="37" t="n">
         <v>0.002092822632293601</v>
       </c>
-      <c r="T35" s="38" t="n">
+      <c r="T35" s="37" t="n">
         <v>-0.0004224555765300897</v>
       </c>
       <c r="U35" s="23" t="n">
@@ -3394,7 +3388,7 @@
       </c>
     </row>
     <row r="36" ht="31.5" customHeight="1">
-      <c r="A36" s="33" t="inlineStr">
+      <c r="A36" s="44" t="inlineStr">
         <is>
           <t xml:space="preserve">Hou. Starts </t>
         </is>
@@ -3452,16 +3446,16 @@
           <t>M</t>
         </is>
       </c>
-      <c r="Q36" s="38" t="n">
+      <c r="Q36" s="37" t="n">
         <v>0.008019789135629696</v>
       </c>
-      <c r="R36" s="38" t="n">
+      <c r="R36" s="37" t="n">
         <v>0.01084249628307491</v>
       </c>
-      <c r="S36" s="38" t="n">
+      <c r="S36" s="37" t="n">
         <v>0.01169114908209064</v>
       </c>
-      <c r="T36" s="38" t="n">
+      <c r="T36" s="37" t="n">
         <v>0.01032118383222275</v>
       </c>
       <c r="U36" s="23" t="n">
@@ -3469,7 +3463,7 @@
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="33" t="n"/>
+      <c r="A37" s="44" t="n"/>
       <c r="B37" s="15" t="inlineStr">
         <is>
           <t>HOUST</t>
@@ -3527,16 +3521,16 @@
           <t>M</t>
         </is>
       </c>
-      <c r="Q37" s="38" t="n">
+      <c r="Q37" s="37" t="n">
         <v>-0.001086738141768961</v>
       </c>
-      <c r="R37" s="38" t="n">
+      <c r="R37" s="37" t="n">
         <v>-0.001422604825913387</v>
       </c>
-      <c r="S37" s="38" t="n">
+      <c r="S37" s="37" t="n">
         <v>-0.002737383934011794</v>
       </c>
-      <c r="T37" s="38" t="n">
+      <c r="T37" s="37" t="n">
         <v>-0.003323493777513176</v>
       </c>
       <c r="U37" s="23" t="n">
@@ -3544,7 +3538,7 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="33" t="inlineStr">
+      <c r="A38" s="44" t="inlineStr">
         <is>
           <t>Housing Permits</t>
         </is>
@@ -3602,16 +3596,16 @@
           <t>M</t>
         </is>
       </c>
-      <c r="Q38" s="38" t="n">
+      <c r="Q38" s="37" t="n">
         <v>0.0136158225247961</v>
       </c>
-      <c r="R38" s="38" t="n">
+      <c r="R38" s="37" t="n">
         <v>0.01383543760782397</v>
       </c>
-      <c r="S38" s="38" t="n">
+      <c r="S38" s="37" t="n">
         <v>0.01314419813616001</v>
       </c>
-      <c r="T38" s="38" t="n">
+      <c r="T38" s="37" t="n">
         <v>0.0147750973624467</v>
       </c>
       <c r="U38" s="23" t="n">
@@ -3619,7 +3613,7 @@
       </c>
     </row>
     <row r="39" ht="31.5" customHeight="1">
-      <c r="A39" s="33" t="n"/>
+      <c r="A39" s="44" t="n"/>
       <c r="B39" s="15" t="inlineStr">
         <is>
           <t>PERMIT</t>
@@ -3638,19 +3632,19 @@
           <t>M</t>
         </is>
       </c>
-      <c r="F39" s="38" t="n">
+      <c r="F39" s="37" t="n">
         <v>-0.02162162162162162</v>
       </c>
-      <c r="G39" s="38" t="n">
+      <c r="G39" s="37" t="n">
         <v>-0.07957559681697612</v>
       </c>
-      <c r="H39" s="38" t="n">
+      <c r="H39" s="37" t="n">
         <v>-0.0119047619047619</v>
       </c>
-      <c r="I39" s="38" t="n">
+      <c r="I39" s="37" t="n">
         <v>-0.01324965132496513</v>
       </c>
-      <c r="J39" s="38" t="n">
+      <c r="J39" s="37" t="n">
         <v>-0.0989159891598916</v>
       </c>
       <c r="K39" s="5" t="n"/>
@@ -3694,7 +3688,7 @@
       </c>
     </row>
     <row r="40" ht="31.5" customHeight="1">
-      <c r="A40" s="33" t="inlineStr">
+      <c r="A40" s="44" t="inlineStr">
         <is>
           <t>New Home Sales</t>
         </is>
@@ -3704,8 +3698,8 @@
           <t>HSN1F</t>
         </is>
       </c>
-      <c r="C40" s="49" t="n">
-        <v>45931</v>
+      <c r="C40" s="48" t="n">
+        <v>45992</v>
       </c>
       <c r="D40" s="6" t="inlineStr">
         <is>
@@ -3718,19 +3712,19 @@
         </is>
       </c>
       <c r="F40" s="24" t="n">
-        <v>737</v>
+        <v>745</v>
       </c>
       <c r="G40" s="24" t="n">
-        <v>738</v>
+        <v>758</v>
       </c>
       <c r="H40" s="24" t="n">
-        <v>711</v>
+        <v>656</v>
       </c>
       <c r="I40" s="24" t="n">
-        <v>639</v>
+        <v>719</v>
       </c>
       <c r="J40" s="24" t="n">
-        <v>662</v>
+        <v>706</v>
       </c>
       <c r="K40" s="5" t="n"/>
       <c r="L40" s="28" t="n"/>
@@ -3752,16 +3746,16 @@
           <t>M</t>
         </is>
       </c>
-      <c r="Q40" s="38" t="n">
+      <c r="Q40" s="37" t="n">
         <v>-0.07456792269916472</v>
       </c>
-      <c r="R40" s="38" t="n">
+      <c r="R40" s="37" t="n">
         <v>-0.05790675033979801</v>
       </c>
-      <c r="S40" s="38" t="n">
+      <c r="S40" s="37" t="n">
         <v>-0.03874237696864814</v>
       </c>
-      <c r="T40" s="38" t="n">
+      <c r="T40" s="37" t="n">
         <v>-0.02292562904900106</v>
       </c>
       <c r="U40" s="23" t="n">
@@ -3769,14 +3763,14 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="33" t="n"/>
+      <c r="A41" s="44" t="n"/>
       <c r="B41" s="15" t="inlineStr">
         <is>
           <t>HSN1F</t>
         </is>
       </c>
-      <c r="C41" s="49" t="n">
-        <v>45931</v>
+      <c r="C41" s="48" t="n">
+        <v>45992</v>
       </c>
       <c r="D41" s="6" t="inlineStr">
         <is>
@@ -3788,20 +3782,20 @@
           <t>M</t>
         </is>
       </c>
-      <c r="F41" s="38" t="n">
-        <v>0.1867954911433172</v>
-      </c>
-      <c r="G41" s="38" t="n">
-        <v>0.02928870292887029</v>
-      </c>
-      <c r="H41" s="38" t="n">
-        <v>0.02597402597402598</v>
-      </c>
-      <c r="I41" s="38" t="n">
-        <v>-0.1</v>
-      </c>
-      <c r="J41" s="38" t="n">
-        <v>-0.01341281669150522</v>
+      <c r="F41" s="37" t="n">
+        <v>0.03760445682451254</v>
+      </c>
+      <c r="G41" s="37" t="n">
+        <v>0.122962962962963</v>
+      </c>
+      <c r="H41" s="37" t="n">
+        <v>0.05636070853462158</v>
+      </c>
+      <c r="I41" s="37" t="n">
+        <v>0.002789400278940028</v>
+      </c>
+      <c r="J41" s="37" t="n">
+        <v>0.01875901875901876</v>
       </c>
       <c r="K41" s="5" t="n"/>
       <c r="L41" s="28" t="inlineStr">
@@ -3827,16 +3821,16 @@
           <t>M</t>
         </is>
       </c>
-      <c r="Q41" s="38" t="n">
+      <c r="Q41" s="37" t="n">
         <v>0.003255208333333259</v>
       </c>
-      <c r="R41" s="38" t="n">
+      <c r="R41" s="37" t="n">
         <v/>
       </c>
-      <c r="S41" s="38" t="n">
+      <c r="S41" s="37" t="n">
         <v/>
       </c>
-      <c r="T41" s="38" t="n">
+      <c r="T41" s="37" t="n">
         <v>0</v>
       </c>
       <c r="U41" s="23" t="n">
@@ -3844,7 +3838,7 @@
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="33" t="inlineStr">
+      <c r="A42" s="44" t="inlineStr">
         <is>
           <t>Existing Home Sales</t>
         </is>
@@ -3867,19 +3861,19 @@
           <t>M</t>
         </is>
       </c>
-      <c r="F42" s="39" t="n">
+      <c r="F42" s="38" t="n">
         <v>3910000</v>
       </c>
-      <c r="G42" s="39" t="n">
+      <c r="G42" s="38" t="n">
         <v>4270000</v>
       </c>
-      <c r="H42" s="39" t="n">
+      <c r="H42" s="38" t="n">
         <v>4090000</v>
       </c>
-      <c r="I42" s="39" t="n">
+      <c r="I42" s="38" t="n">
         <v>4110000</v>
       </c>
-      <c r="J42" s="39" t="n">
+      <c r="J42" s="38" t="n">
         <v>4080000</v>
       </c>
       <c r="K42" s="7" t="n"/>
@@ -3902,16 +3896,16 @@
           <t>M</t>
         </is>
       </c>
-      <c r="Q42" s="38" t="n">
+      <c r="Q42" s="37" t="n">
         <v>0.03076923076923073</v>
       </c>
-      <c r="R42" s="38" t="n">
+      <c r="R42" s="37" t="n">
         <v>0.03225806451612891</v>
       </c>
-      <c r="S42" s="38" t="n">
+      <c r="S42" s="37" t="n">
         <v/>
       </c>
-      <c r="T42" s="38" t="n">
+      <c r="T42" s="37" t="n">
         <v>0.03869653767820766</v>
       </c>
       <c r="U42" s="23" t="n">
@@ -3919,7 +3913,7 @@
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="33" t="n"/>
+      <c r="A43" s="44" t="n"/>
       <c r="B43" s="15" t="inlineStr">
         <is>
           <t>EXHOSLUSM495S</t>
@@ -3938,19 +3932,19 @@
           <t>M</t>
         </is>
       </c>
-      <c r="F43" s="38" t="n">
+      <c r="F43" s="37" t="n">
         <v>-0.04400977995110025</v>
       </c>
-      <c r="G43" s="38" t="n">
+      <c r="G43" s="37" t="n">
         <v/>
       </c>
-      <c r="H43" s="38" t="n">
+      <c r="H43" s="37" t="n">
         <v/>
       </c>
-      <c r="I43" s="38" t="n">
+      <c r="I43" s="37" t="n">
         <v/>
       </c>
-      <c r="J43" s="38" t="n">
+      <c r="J43" s="37" t="n">
         <v/>
       </c>
       <c r="K43" s="5" t="n"/>
@@ -3977,16 +3971,16 @@
           <t>M</t>
         </is>
       </c>
-      <c r="Q43" s="38" t="n">
+      <c r="Q43" s="37" t="n">
         <v>0.00141643059490093</v>
       </c>
-      <c r="R43" s="38" t="n">
+      <c r="R43" s="37" t="n">
         <v/>
       </c>
-      <c r="S43" s="38" t="n">
+      <c r="S43" s="37" t="n">
         <v/>
       </c>
-      <c r="T43" s="38" t="n">
+      <c r="T43" s="37" t="n">
         <v>-0.001418439716311948</v>
       </c>
       <c r="U43" s="23" t="n">
@@ -3994,7 +3988,7 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="33" t="inlineStr">
+      <c r="A44" s="44" t="inlineStr">
         <is>
           <t>Gov. Cons</t>
         </is>
@@ -4052,16 +4046,16 @@
           <t>M</t>
         </is>
       </c>
-      <c r="Q44" s="38" t="n">
+      <c r="Q44" s="37" t="n">
         <v>0</v>
       </c>
-      <c r="R44" s="38" t="n">
+      <c r="R44" s="37" t="n">
         <v>-0.0007077140835104227</v>
       </c>
-      <c r="S44" s="38" t="n">
+      <c r="S44" s="37" t="n">
         <v/>
       </c>
-      <c r="T44" s="38" t="n">
+      <c r="T44" s="37" t="n">
         <v>-0.0007097232079488595</v>
       </c>
       <c r="U44" s="23" t="n">
@@ -4069,7 +4063,7 @@
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="33" t="n"/>
+      <c r="A45" s="44" t="n"/>
       <c r="B45" s="15" t="inlineStr">
         <is>
           <t>GCE</t>
@@ -4088,19 +4082,19 @@
           <t>Q</t>
         </is>
       </c>
-      <c r="F45" s="38" t="n">
+      <c r="F45" s="37" t="n">
         <v>0.004135487891410161</v>
       </c>
-      <c r="G45" s="38" t="n">
+      <c r="G45" s="37" t="n">
         <v>0.01669515005814426</v>
       </c>
-      <c r="H45" s="38" t="n">
+      <c r="H45" s="37" t="n">
         <v>0.007978609251013902</v>
       </c>
-      <c r="I45" s="38" t="n">
+      <c r="I45" s="37" t="n">
         <v>0.008696251498575336</v>
       </c>
-      <c r="J45" s="38" t="n">
+      <c r="J45" s="37" t="n">
         <v>0.01254255520332359</v>
       </c>
       <c r="K45" s="5" t="n"/>
@@ -4116,7 +4110,7 @@
       <c r="U45" s="21" t="n"/>
     </row>
     <row r="46" ht="16.15" customHeight="1" thickBot="1">
-      <c r="A46" s="33" t="inlineStr">
+      <c r="A46" s="44" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -4207,7 +4201,7 @@
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="33" t="n"/>
+      <c r="A47" s="44" t="n"/>
       <c r="B47" s="15" t="inlineStr">
         <is>
           <t>BOPTEXP</t>
@@ -4226,19 +4220,19 @@
           <t>M</t>
         </is>
       </c>
-      <c r="F47" s="38" t="n">
+      <c r="F47" s="37" t="n">
         <v>-0.01711656231824554</v>
       </c>
-      <c r="G47" s="38" t="n">
+      <c r="G47" s="37" t="n">
         <v>-0.03405222839844813</v>
       </c>
-      <c r="H47" s="38" t="n">
+      <c r="H47" s="37" t="n">
         <v>0.02957798714533122</v>
       </c>
-      <c r="I47" s="38" t="n">
+      <c r="I47" s="37" t="n">
         <v>0.03582555615078808</v>
       </c>
-      <c r="J47" s="38" t="n">
+      <c r="J47" s="37" t="n">
         <v>0.0004866042778863822</v>
       </c>
       <c r="K47" s="5" t="n"/>
@@ -4253,7 +4247,7 @@
         </is>
       </c>
       <c r="N47" s="48" t="n">
-        <v>46071</v>
+        <v>46072</v>
       </c>
       <c r="O47" s="6" t="inlineStr">
         <is>
@@ -4282,7 +4276,7 @@
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="33" t="inlineStr">
+      <c r="A48" s="44" t="inlineStr">
         <is>
           <t>M</t>
         </is>
@@ -4332,7 +4326,7 @@
         </is>
       </c>
       <c r="N48" s="48" t="n">
-        <v>46071</v>
+        <v>46072</v>
       </c>
       <c r="O48" s="6" t="inlineStr">
         <is>
@@ -4348,20 +4342,20 @@
         <v>3.47</v>
       </c>
       <c r="R48" s="6" t="n">
+        <v>3.47</v>
+      </c>
+      <c r="S48" s="6" t="n">
         <v>3.43</v>
       </c>
-      <c r="S48" s="6" t="n">
+      <c r="T48" s="6" t="n">
         <v>3.4</v>
       </c>
-      <c r="T48" s="6" t="n">
+      <c r="U48" s="21" t="n">
         <v>3.47</v>
       </c>
-      <c r="U48" s="21" t="n">
-        <v>3.52</v>
-      </c>
     </row>
     <row r="49">
-      <c r="A49" s="33" t="n"/>
+      <c r="A49" s="44" t="n"/>
       <c r="B49" s="15" t="inlineStr">
         <is>
           <t>BOPTIMP</t>
@@ -4380,19 +4374,19 @@
           <t>M</t>
         </is>
       </c>
-      <c r="F49" s="38" t="n">
+      <c r="F49" s="37" t="n">
         <v>0.0355134449547394</v>
       </c>
-      <c r="G49" s="38" t="n">
+      <c r="G49" s="37" t="n">
         <v>0.04222512622871166</v>
       </c>
-      <c r="H49" s="38" t="n">
+      <c r="H49" s="37" t="n">
         <v>-0.02997523288697879</v>
       </c>
-      <c r="I49" s="38" t="n">
+      <c r="I49" s="37" t="n">
         <v>0.007887072931081818</v>
       </c>
-      <c r="J49" s="38" t="n">
+      <c r="J49" s="37" t="n">
         <v>-0.05210885495329198</v>
       </c>
       <c r="K49" s="5" t="n"/>
@@ -4407,7 +4401,7 @@
         </is>
       </c>
       <c r="N49" s="48" t="n">
-        <v>46071</v>
+        <v>46072</v>
       </c>
       <c r="O49" s="6" t="inlineStr">
         <is>
@@ -4420,23 +4414,23 @@
         </is>
       </c>
       <c r="Q49" s="6" t="n">
+        <v>3.65</v>
+      </c>
+      <c r="R49" s="6" t="n">
         <v>3.66</v>
       </c>
-      <c r="R49" s="6" t="n">
+      <c r="S49" s="6" t="n">
         <v>3.63</v>
       </c>
-      <c r="S49" s="6" t="n">
+      <c r="T49" s="6" t="n">
         <v>3.61</v>
       </c>
-      <c r="T49" s="6" t="n">
+      <c r="U49" s="21" t="n">
         <v>3.67</v>
       </c>
-      <c r="U49" s="21" t="n">
-        <v>3.75</v>
-      </c>
     </row>
     <row r="50">
-      <c r="A50" s="33" t="inlineStr">
+      <c r="A50" s="44" t="inlineStr">
         <is>
           <t>Trade Balance</t>
         </is>
@@ -4486,7 +4480,7 @@
         </is>
       </c>
       <c r="N50" s="48" t="n">
-        <v>46071</v>
+        <v>46072</v>
       </c>
       <c r="O50" s="6" t="inlineStr">
         <is>
@@ -4499,23 +4493,23 @@
         </is>
       </c>
       <c r="Q50" s="6" t="n">
+        <v>4.08</v>
+      </c>
+      <c r="R50" s="6" t="n">
         <v>4.09</v>
       </c>
-      <c r="R50" s="6" t="n">
+      <c r="S50" s="6" t="n">
         <v>4.05</v>
       </c>
-      <c r="S50" s="6" t="n">
+      <c r="T50" s="6" t="n">
         <v>4.04</v>
       </c>
-      <c r="T50" s="6" t="n">
+      <c r="U50" s="21" t="n">
         <v>4.09</v>
       </c>
-      <c r="U50" s="21" t="n">
-        <v>4.18</v>
-      </c>
     </row>
     <row r="51" ht="31.5" customHeight="1">
-      <c r="A51" s="33" t="n"/>
+      <c r="A51" s="44" t="n"/>
       <c r="B51" s="15" t="inlineStr">
         <is>
           <t>BOPSTB</t>
@@ -4534,19 +4528,19 @@
           <t>M</t>
         </is>
       </c>
-      <c r="F51" s="38" t="n">
+      <c r="F51" s="37" t="n">
         <v>-0.05160636663725204</v>
       </c>
-      <c r="G51" s="38" t="n">
+      <c r="G51" s="37" t="n">
         <v>0.02753803270980959</v>
       </c>
-      <c r="H51" s="38" t="n">
+      <c r="H51" s="37" t="n">
         <v>-0.01299347011833341</v>
       </c>
-      <c r="I51" s="38" t="n">
+      <c r="I51" s="37" t="n">
         <v>-0.008120725933719042</v>
       </c>
-      <c r="J51" s="38" t="n">
+      <c r="J51" s="37" t="n">
         <v>0.06327343913864225</v>
       </c>
       <c r="K51" s="5" t="n"/>
@@ -4590,7 +4584,7 @@
       </c>
     </row>
     <row r="52" ht="16.15" customHeight="1" thickBot="1">
-      <c r="A52" s="36" t="n"/>
+      <c r="A52" s="35" t="n"/>
       <c r="B52" s="17" t="n"/>
       <c r="C52" s="20" t="n"/>
       <c r="D52" s="9" t="n"/>
@@ -4612,7 +4606,7 @@
         </is>
       </c>
       <c r="N52" s="50" t="n">
-        <v>46071</v>
+        <v>46072</v>
       </c>
       <c r="O52" s="9" t="inlineStr">
         <is>
@@ -4628,25 +4622,25 @@
         <v>5.76</v>
       </c>
       <c r="R52" s="9" t="n">
+        <v>5.76</v>
+      </c>
+      <c r="S52" s="9" t="n">
         <v>5.75</v>
       </c>
-      <c r="S52" s="9" t="n">
+      <c r="T52" s="9" t="n">
         <v>5.76</v>
       </c>
-      <c r="T52" s="9" t="n">
+      <c r="U52" s="22" t="n">
         <v>5.77</v>
       </c>
-      <c r="U52" s="22" t="n">
-        <v>5.85</v>
-      </c>
     </row>
     <row r="53" ht="21" customHeight="1">
-      <c r="A53" s="37" t="inlineStr">
+      <c r="A53" s="36" t="inlineStr">
         <is>
           <t>Footnote: All data is Seasonally Adjusted unless otherwise indicated by NSA</t>
         </is>
       </c>
-      <c r="B53" s="40" t="inlineStr">
+      <c r="B53" s="39" t="inlineStr">
         <is>
           <t>*FRED doesn't include real avg. hourly earning data. Calculated through chained PCE deflator (FRED ticker: PCEPI). Ticker "RCES0500000003" is only for reference in the raw data table</t>
         </is>
@@ -4672,7 +4666,7 @@
       <c r="U53" s="6" t="n"/>
     </row>
     <row r="54" ht="21" customHeight="1">
-      <c r="A54" s="37" t="inlineStr">
+      <c r="A54" s="36" t="inlineStr">
         <is>
           <t>Source: All data collected via FRED from the St. Louis Fed</t>
         </is>
@@ -4698,10 +4692,11 @@
       <c r="T54" s="6" t="n"/>
       <c r="U54" s="6" t="n"/>
     </row>
-    <row r="55" ht="21" customHeight="1">
-      <c r="A55" s="37" t="inlineStr">
-        <is>
-          <t>Mike Aguilar | mike.aguilar@duke.edu | www.market-observatory.com</t>
+    <row r="55" ht="31.5" customHeight="1">
+      <c r="A55" s="36" t="inlineStr">
+        <is>
+          <t>Mike Aguilar | mike.aguilar@duke.edu |
+Jacky Yang    | jacky.yang@duke.edu     | www.market-observatory.com</t>
         </is>
       </c>
       <c r="B55" s="15" t="n"/>

</xml_diff>

<commit_message>
Update dashboards - 2026-02-23
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -1038,8 +1038,8 @@
           <t>NGDPSAXDCUSQ</t>
         </is>
       </c>
-      <c r="C5" s="49" t="n">
-        <v>45839</v>
+      <c r="C5" s="48" t="n">
+        <v>45931</v>
       </c>
       <c r="D5" s="6" t="inlineStr">
         <is>
@@ -1052,19 +1052,19 @@
         </is>
       </c>
       <c r="F5" s="24" t="n">
+        <v>7872517.5</v>
+      </c>
+      <c r="G5" s="24" t="n">
         <v>7774506.8</v>
       </c>
-      <c r="G5" s="24" t="n">
+      <c r="H5" s="24" t="n">
         <v>7621432.3</v>
       </c>
-      <c r="H5" s="24" t="n">
+      <c r="I5" s="24" t="n">
         <v>7510528.3</v>
       </c>
-      <c r="I5" s="24" t="n">
+      <c r="J5" s="24" t="n">
         <v>7456295.5</v>
-      </c>
-      <c r="J5" s="24" t="n">
-        <v>7377916</v>
       </c>
       <c r="K5" s="5" t="n"/>
       <c r="L5" s="28" t="inlineStr">
@@ -1113,8 +1113,8 @@
           <t>NGDPSAXDCUSQ</t>
         </is>
       </c>
-      <c r="C6" s="49" t="n">
-        <v>45839</v>
+      <c r="C6" s="48" t="n">
+        <v>45931</v>
       </c>
       <c r="D6" s="6" t="inlineStr">
         <is>
@@ -1127,19 +1127,19 @@
         </is>
       </c>
       <c r="F6" s="25" t="n">
+        <v>0.01260667750653965</v>
+      </c>
+      <c r="G6" s="25" t="n">
         <v>0.02008474181421249</v>
       </c>
-      <c r="G6" s="25" t="n">
+      <c r="H6" s="25" t="n">
         <v>0.0147664712214719</v>
       </c>
-      <c r="H6" s="25" t="n">
+      <c r="I6" s="25" t="n">
         <v>0.007273424182290045</v>
       </c>
-      <c r="I6" s="25" t="n">
+      <c r="J6" s="25" t="n">
         <v>0.01062352837847436</v>
-      </c>
-      <c r="J6" s="25" t="n">
-        <v>0.01250967336516173</v>
       </c>
       <c r="K6" s="5" t="n"/>
       <c r="L6" s="28" t="inlineStr">

</xml_diff>

<commit_message>
Update dashboards - 2026-02-24
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -2901,7 +2901,7 @@
         </is>
       </c>
       <c r="N29" s="48" t="n">
-        <v>46073</v>
+        <v>46076</v>
       </c>
       <c r="O29" s="6" t="inlineStr">
         <is>
@@ -2914,19 +2914,19 @@
         </is>
       </c>
       <c r="Q29" s="6" t="n">
+        <v>2.12</v>
+      </c>
+      <c r="R29" s="6" t="n">
         <v>2.13</v>
-      </c>
-      <c r="R29" s="6" t="n">
-        <v>2.15</v>
       </c>
       <c r="S29" s="6" t="n">
         <v>2.15</v>
       </c>
       <c r="T29" s="6" t="n">
+        <v>2.15</v>
+      </c>
+      <c r="U29" s="21" t="n">
         <v>2.13</v>
-      </c>
-      <c r="U29" s="21" t="n">
-        <v>2.12</v>
       </c>
     </row>
     <row r="30">
@@ -2980,7 +2980,7 @@
         </is>
       </c>
       <c r="N30" s="48" t="n">
-        <v>46073</v>
+        <v>46076</v>
       </c>
       <c r="O30" s="6" t="inlineStr">
         <is>
@@ -2993,19 +2993,19 @@
         </is>
       </c>
       <c r="Q30" s="6" t="n">
+        <v>2.26</v>
+      </c>
+      <c r="R30" s="6" t="n">
         <v>2.28</v>
-      </c>
-      <c r="R30" s="6" t="n">
-        <v>2.29</v>
       </c>
       <c r="S30" s="6" t="n">
         <v>2.29</v>
       </c>
       <c r="T30" s="6" t="n">
+        <v>2.29</v>
+      </c>
+      <c r="U30" s="21" t="n">
         <v>2.26</v>
-      </c>
-      <c r="U30" s="21" t="n">
-        <v>2.27</v>
       </c>
     </row>
     <row r="31">
@@ -3508,8 +3508,8 @@
           <t>CSUSHPINSA</t>
         </is>
       </c>
-      <c r="N37" s="49" t="n">
-        <v>45962</v>
+      <c r="N37" s="48" t="n">
+        <v>45992</v>
       </c>
       <c r="O37" s="6" t="inlineStr">
         <is>
@@ -3522,19 +3522,19 @@
         </is>
       </c>
       <c r="Q37" s="37" t="n">
-        <v>-0.001086738141768961</v>
+        <v>-0.00273486156666769</v>
       </c>
       <c r="R37" s="37" t="n">
-        <v>-0.001422604825913387</v>
+        <v>-0.0006239385435752309</v>
       </c>
       <c r="S37" s="37" t="n">
-        <v>-0.002737383934011794</v>
+        <v>-0.001255429809922437</v>
       </c>
       <c r="T37" s="37" t="n">
-        <v>-0.003323493777513176</v>
+        <v>-0.002710199627120158</v>
       </c>
       <c r="U37" s="23" t="n">
-        <v>-0.001935956624922186</v>
+        <v>-0.003326625695690755</v>
       </c>
     </row>
     <row r="38">
@@ -3583,8 +3583,8 @@
           <t>CSUSHPINSA</t>
         </is>
       </c>
-      <c r="N38" s="49" t="n">
-        <v>45962</v>
+      <c r="N38" s="48" t="n">
+        <v>45992</v>
       </c>
       <c r="O38" s="6" t="inlineStr">
         <is>
@@ -3597,19 +3597,19 @@
         </is>
       </c>
       <c r="Q38" s="37" t="n">
-        <v>0.0136158225247961</v>
+        <v>0.01272340965111129</v>
       </c>
       <c r="R38" s="37" t="n">
-        <v>0.01383543760782397</v>
+        <v>0.01427415269420379</v>
       </c>
       <c r="S38" s="37" t="n">
-        <v>0.01314419813616001</v>
+        <v>0.01402408537902678</v>
       </c>
       <c r="T38" s="37" t="n">
-        <v>0.0147750973624467</v>
+        <v>0.01316616157883059</v>
       </c>
       <c r="U38" s="23" t="n">
-        <v>0.01642359863525655</v>
+        <v>0.01475691239986718</v>
       </c>
     </row>
     <row r="39" ht="31.5" customHeight="1">
@@ -4247,7 +4247,7 @@
         </is>
       </c>
       <c r="N47" s="48" t="n">
-        <v>46072</v>
+        <v>46073</v>
       </c>
       <c r="O47" s="6" t="inlineStr">
         <is>
@@ -4326,7 +4326,7 @@
         </is>
       </c>
       <c r="N48" s="48" t="n">
-        <v>46072</v>
+        <v>46073</v>
       </c>
       <c r="O48" s="6" t="inlineStr">
         <is>
@@ -4339,19 +4339,19 @@
         </is>
       </c>
       <c r="Q48" s="6" t="n">
-        <v>3.47</v>
+        <v>3.48</v>
       </c>
       <c r="R48" s="6" t="n">
         <v>3.47</v>
       </c>
       <c r="S48" s="6" t="n">
+        <v>3.47</v>
+      </c>
+      <c r="T48" s="6" t="n">
         <v>3.43</v>
       </c>
-      <c r="T48" s="6" t="n">
+      <c r="U48" s="21" t="n">
         <v>3.4</v>
-      </c>
-      <c r="U48" s="21" t="n">
-        <v>3.47</v>
       </c>
     </row>
     <row r="49">
@@ -4401,7 +4401,7 @@
         </is>
       </c>
       <c r="N49" s="48" t="n">
-        <v>46072</v>
+        <v>46073</v>
       </c>
       <c r="O49" s="6" t="inlineStr">
         <is>
@@ -4417,16 +4417,16 @@
         <v>3.65</v>
       </c>
       <c r="R49" s="6" t="n">
+        <v>3.65</v>
+      </c>
+      <c r="S49" s="6" t="n">
         <v>3.66</v>
       </c>
-      <c r="S49" s="6" t="n">
+      <c r="T49" s="6" t="n">
         <v>3.63</v>
       </c>
-      <c r="T49" s="6" t="n">
+      <c r="U49" s="21" t="n">
         <v>3.61</v>
-      </c>
-      <c r="U49" s="21" t="n">
-        <v>3.67</v>
       </c>
     </row>
     <row r="50">
@@ -4480,7 +4480,7 @@
         </is>
       </c>
       <c r="N50" s="48" t="n">
-        <v>46072</v>
+        <v>46073</v>
       </c>
       <c r="O50" s="6" t="inlineStr">
         <is>
@@ -4496,16 +4496,16 @@
         <v>4.08</v>
       </c>
       <c r="R50" s="6" t="n">
+        <v>4.08</v>
+      </c>
+      <c r="S50" s="6" t="n">
         <v>4.09</v>
       </c>
-      <c r="S50" s="6" t="n">
+      <c r="T50" s="6" t="n">
         <v>4.05</v>
       </c>
-      <c r="T50" s="6" t="n">
+      <c r="U50" s="21" t="n">
         <v>4.04</v>
-      </c>
-      <c r="U50" s="21" t="n">
-        <v>4.09</v>
       </c>
     </row>
     <row r="51" ht="31.5" customHeight="1">
@@ -4606,7 +4606,7 @@
         </is>
       </c>
       <c r="N52" s="50" t="n">
-        <v>46072</v>
+        <v>46073</v>
       </c>
       <c r="O52" s="9" t="inlineStr">
         <is>
@@ -4619,19 +4619,19 @@
         </is>
       </c>
       <c r="Q52" s="9" t="n">
-        <v>5.76</v>
+        <v>5.77</v>
       </c>
       <c r="R52" s="9" t="n">
         <v>5.76</v>
       </c>
       <c r="S52" s="9" t="n">
+        <v>5.76</v>
+      </c>
+      <c r="T52" s="9" t="n">
         <v>5.75</v>
       </c>
-      <c r="T52" s="9" t="n">
+      <c r="U52" s="22" t="n">
         <v>5.76</v>
-      </c>
-      <c r="U52" s="22" t="n">
-        <v>5.77</v>
       </c>
     </row>
     <row r="53" ht="21" customHeight="1">

</xml_diff>

<commit_message>
Update dashboards - 2026-02-25
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -2786,7 +2786,7 @@
           <t>DGORDER</t>
         </is>
       </c>
-      <c r="C28" s="48" t="n">
+      <c r="C28" s="49" t="n">
         <v>45992</v>
       </c>
       <c r="D28" s="6" t="inlineStr">
@@ -2861,7 +2861,7 @@
           <t>DGORDER</t>
         </is>
       </c>
-      <c r="C29" s="48" t="n">
+      <c r="C29" s="49" t="n">
         <v>45992</v>
       </c>
       <c r="D29" s="6" t="inlineStr">
@@ -2901,7 +2901,7 @@
         </is>
       </c>
       <c r="N29" s="48" t="n">
-        <v>46076</v>
+        <v>46077</v>
       </c>
       <c r="O29" s="6" t="inlineStr">
         <is>
@@ -2917,16 +2917,16 @@
         <v>2.12</v>
       </c>
       <c r="R29" s="6" t="n">
+        <v>2.12</v>
+      </c>
+      <c r="S29" s="6" t="n">
         <v>2.13</v>
-      </c>
-      <c r="S29" s="6" t="n">
-        <v>2.15</v>
       </c>
       <c r="T29" s="6" t="n">
         <v>2.15</v>
       </c>
       <c r="U29" s="21" t="n">
-        <v>2.13</v>
+        <v>2.15</v>
       </c>
     </row>
     <row r="30">
@@ -2940,7 +2940,7 @@
           <t>ADXDNO</t>
         </is>
       </c>
-      <c r="C30" s="48" t="n">
+      <c r="C30" s="49" t="n">
         <v>45992</v>
       </c>
       <c r="D30" s="6" t="inlineStr">
@@ -2980,7 +2980,7 @@
         </is>
       </c>
       <c r="N30" s="48" t="n">
-        <v>46076</v>
+        <v>46077</v>
       </c>
       <c r="O30" s="6" t="inlineStr">
         <is>
@@ -2996,16 +2996,16 @@
         <v>2.26</v>
       </c>
       <c r="R30" s="6" t="n">
+        <v>2.26</v>
+      </c>
+      <c r="S30" s="6" t="n">
         <v>2.28</v>
-      </c>
-      <c r="S30" s="6" t="n">
-        <v>2.29</v>
       </c>
       <c r="T30" s="6" t="n">
         <v>2.29</v>
       </c>
       <c r="U30" s="21" t="n">
-        <v>2.26</v>
+        <v>2.29</v>
       </c>
     </row>
     <row r="31">
@@ -3015,7 +3015,7 @@
           <t>ADXDNO</t>
         </is>
       </c>
-      <c r="C31" s="48" t="n">
+      <c r="C31" s="49" t="n">
         <v>45992</v>
       </c>
       <c r="D31" s="6" t="inlineStr">
@@ -3094,7 +3094,7 @@
           <t>INDPRO</t>
         </is>
       </c>
-      <c r="C32" s="48" t="n">
+      <c r="C32" s="49" t="n">
         <v>46023</v>
       </c>
       <c r="D32" s="6" t="inlineStr">
@@ -3165,7 +3165,7 @@
           <t>INDPRO</t>
         </is>
       </c>
-      <c r="C33" s="48" t="n">
+      <c r="C33" s="49" t="n">
         <v>46023</v>
       </c>
       <c r="D33" s="6" t="inlineStr">
@@ -3244,7 +3244,7 @@
           <t>TCU</t>
         </is>
       </c>
-      <c r="C34" s="48" t="n">
+      <c r="C34" s="49" t="n">
         <v>46023</v>
       </c>
       <c r="D34" s="6" t="inlineStr">
@@ -3398,7 +3398,7 @@
           <t>HOUST</t>
         </is>
       </c>
-      <c r="C36" s="48" t="n">
+      <c r="C36" s="49" t="n">
         <v>45992</v>
       </c>
       <c r="D36" s="6" t="inlineStr">
@@ -3469,7 +3469,7 @@
           <t>HOUST</t>
         </is>
       </c>
-      <c r="C37" s="48" t="n">
+      <c r="C37" s="49" t="n">
         <v>45992</v>
       </c>
       <c r="D37" s="6" t="inlineStr">
@@ -3548,7 +3548,7 @@
           <t>PERMIT</t>
         </is>
       </c>
-      <c r="C38" s="48" t="n">
+      <c r="C38" s="49" t="n">
         <v>45992</v>
       </c>
       <c r="D38" s="6" t="inlineStr">
@@ -3619,7 +3619,7 @@
           <t>PERMIT</t>
         </is>
       </c>
-      <c r="C39" s="48" t="n">
+      <c r="C39" s="49" t="n">
         <v>45992</v>
       </c>
       <c r="D39" s="6" t="inlineStr">
@@ -4247,7 +4247,7 @@
         </is>
       </c>
       <c r="N47" s="48" t="n">
-        <v>46073</v>
+        <v>46076</v>
       </c>
       <c r="O47" s="6" t="inlineStr">
         <is>
@@ -4326,7 +4326,7 @@
         </is>
       </c>
       <c r="N48" s="48" t="n">
-        <v>46073</v>
+        <v>46076</v>
       </c>
       <c r="O48" s="6" t="inlineStr">
         <is>
@@ -4339,19 +4339,19 @@
         </is>
       </c>
       <c r="Q48" s="6" t="n">
+        <v>3.43</v>
+      </c>
+      <c r="R48" s="6" t="n">
         <v>3.48</v>
-      </c>
-      <c r="R48" s="6" t="n">
-        <v>3.47</v>
       </c>
       <c r="S48" s="6" t="n">
         <v>3.47</v>
       </c>
       <c r="T48" s="6" t="n">
+        <v>3.47</v>
+      </c>
+      <c r="U48" s="21" t="n">
         <v>3.43</v>
-      </c>
-      <c r="U48" s="21" t="n">
-        <v>3.4</v>
       </c>
     </row>
     <row r="49">
@@ -4401,7 +4401,7 @@
         </is>
       </c>
       <c r="N49" s="48" t="n">
-        <v>46073</v>
+        <v>46076</v>
       </c>
       <c r="O49" s="6" t="inlineStr">
         <is>
@@ -4414,19 +4414,19 @@
         </is>
       </c>
       <c r="Q49" s="6" t="n">
-        <v>3.65</v>
+        <v>3.59</v>
       </c>
       <c r="R49" s="6" t="n">
         <v>3.65</v>
       </c>
       <c r="S49" s="6" t="n">
+        <v>3.65</v>
+      </c>
+      <c r="T49" s="6" t="n">
         <v>3.66</v>
       </c>
-      <c r="T49" s="6" t="n">
+      <c r="U49" s="21" t="n">
         <v>3.63</v>
-      </c>
-      <c r="U49" s="21" t="n">
-        <v>3.61</v>
       </c>
     </row>
     <row r="50">
@@ -4480,7 +4480,7 @@
         </is>
       </c>
       <c r="N50" s="48" t="n">
-        <v>46073</v>
+        <v>46076</v>
       </c>
       <c r="O50" s="6" t="inlineStr">
         <is>
@@ -4493,19 +4493,19 @@
         </is>
       </c>
       <c r="Q50" s="6" t="n">
-        <v>4.08</v>
+        <v>4.03</v>
       </c>
       <c r="R50" s="6" t="n">
         <v>4.08</v>
       </c>
       <c r="S50" s="6" t="n">
+        <v>4.08</v>
+      </c>
+      <c r="T50" s="6" t="n">
         <v>4.09</v>
       </c>
-      <c r="T50" s="6" t="n">
+      <c r="U50" s="21" t="n">
         <v>4.05</v>
-      </c>
-      <c r="U50" s="21" t="n">
-        <v>4.04</v>
       </c>
     </row>
     <row r="51" ht="31.5" customHeight="1">
@@ -4606,7 +4606,7 @@
         </is>
       </c>
       <c r="N52" s="50" t="n">
-        <v>46073</v>
+        <v>46076</v>
       </c>
       <c r="O52" s="9" t="inlineStr">
         <is>
@@ -4619,19 +4619,19 @@
         </is>
       </c>
       <c r="Q52" s="9" t="n">
+        <v>5.76</v>
+      </c>
+      <c r="R52" s="9" t="n">
         <v>5.77</v>
-      </c>
-      <c r="R52" s="9" t="n">
-        <v>5.76</v>
       </c>
       <c r="S52" s="9" t="n">
         <v>5.76</v>
       </c>
       <c r="T52" s="9" t="n">
+        <v>5.76</v>
+      </c>
+      <c r="U52" s="22" t="n">
         <v>5.75</v>
-      </c>
-      <c r="U52" s="22" t="n">
-        <v>5.76</v>
       </c>
     </row>
     <row r="53" ht="21" customHeight="1">

</xml_diff>

<commit_message>
Update dashboards - 2026-02-26
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -1698,7 +1698,7 @@
         </is>
       </c>
       <c r="N13" s="48" t="n">
-        <v>46062</v>
+        <v>46069</v>
       </c>
       <c r="O13" s="6" t="inlineStr">
         <is>
@@ -1711,19 +1711,19 @@
         </is>
       </c>
       <c r="Q13" s="24" t="n">
-        <v>206000</v>
+        <v>212000</v>
       </c>
       <c r="R13" s="24" t="n">
+        <v>208000</v>
+      </c>
+      <c r="S13" s="24" t="n">
         <v>229000</v>
       </c>
-      <c r="S13" s="24" t="n">
+      <c r="T13" s="24" t="n">
         <v>232000</v>
       </c>
-      <c r="T13" s="24" t="n">
+      <c r="U13" s="26" t="n">
         <v>209000</v>
-      </c>
-      <c r="U13" s="26" t="n">
-        <v>210000</v>
       </c>
     </row>
     <row r="14">
@@ -1773,7 +1773,7 @@
         </is>
       </c>
       <c r="N14" s="48" t="n">
-        <v>46055</v>
+        <v>46062</v>
       </c>
       <c r="O14" s="6" t="inlineStr">
         <is>
@@ -1786,19 +1786,19 @@
         </is>
       </c>
       <c r="Q14" s="24" t="n">
-        <v>1869000</v>
+        <v>1833000</v>
       </c>
       <c r="R14" s="24" t="n">
+        <v>1864000</v>
+      </c>
+      <c r="S14" s="24" t="n">
         <v>1852000</v>
       </c>
-      <c r="S14" s="24" t="n">
+      <c r="T14" s="24" t="n">
         <v>1841000</v>
       </c>
-      <c r="T14" s="24" t="n">
+      <c r="U14" s="26" t="n">
         <v>1819000</v>
-      </c>
-      <c r="U14" s="26" t="n">
-        <v>1865000</v>
       </c>
     </row>
     <row r="15">
@@ -2800,10 +2800,10 @@
         </is>
       </c>
       <c r="F28" s="25" t="n">
-        <v>-0.01425751734772551</v>
+        <v>-0.01358905968147273</v>
       </c>
       <c r="G28" s="25" t="n">
-        <v>0.05423155704392491</v>
+        <v>0.05441037812530491</v>
       </c>
       <c r="H28" s="25" t="n">
         <v>-0.02093605859677161</v>
@@ -2875,10 +2875,10 @@
         </is>
       </c>
       <c r="F29" s="25" t="n">
-        <v>0.1000416438657897</v>
+        <v>0.1009743287938078</v>
       </c>
       <c r="G29" s="25" t="n">
-        <v>0.1245404730526462</v>
+        <v>0.1247312200873968</v>
       </c>
       <c r="H29" s="25" t="n">
         <v>0.04877483240471108</v>
@@ -2901,7 +2901,7 @@
         </is>
       </c>
       <c r="N29" s="48" t="n">
-        <v>46077</v>
+        <v>46078</v>
       </c>
       <c r="O29" s="6" t="inlineStr">
         <is>
@@ -2914,16 +2914,16 @@
         </is>
       </c>
       <c r="Q29" s="6" t="n">
-        <v>2.12</v>
+        <v>2.14</v>
       </c>
       <c r="R29" s="6" t="n">
         <v>2.12</v>
       </c>
       <c r="S29" s="6" t="n">
+        <v>2.12</v>
+      </c>
+      <c r="T29" s="6" t="n">
         <v>2.13</v>
-      </c>
-      <c r="T29" s="6" t="n">
-        <v>2.15</v>
       </c>
       <c r="U29" s="21" t="n">
         <v>2.15</v>
@@ -2954,10 +2954,10 @@
         </is>
       </c>
       <c r="F30" s="25" t="n">
-        <v>-0.02458405517602069</v>
+        <v>-0.02377629691120575</v>
       </c>
       <c r="G30" s="25" t="n">
-        <v>0.06576508785864577</v>
+        <v>0.06592882125886601</v>
       </c>
       <c r="H30" s="25" t="n">
         <v>-0.0128376635658648</v>
@@ -2980,7 +2980,7 @@
         </is>
       </c>
       <c r="N30" s="48" t="n">
-        <v>46077</v>
+        <v>46078</v>
       </c>
       <c r="O30" s="6" t="inlineStr">
         <is>
@@ -2993,16 +2993,16 @@
         </is>
       </c>
       <c r="Q30" s="6" t="n">
-        <v>2.26</v>
+        <v>2.28</v>
       </c>
       <c r="R30" s="6" t="n">
         <v>2.26</v>
       </c>
       <c r="S30" s="6" t="n">
+        <v>2.26</v>
+      </c>
+      <c r="T30" s="6" t="n">
         <v>2.28</v>
-      </c>
-      <c r="T30" s="6" t="n">
-        <v>2.29</v>
       </c>
       <c r="U30" s="21" t="n">
         <v>2.29</v>
@@ -3029,10 +3029,10 @@
         </is>
       </c>
       <c r="F31" s="25" t="n">
-        <v>0.09489005566012468</v>
+        <v>0.09596509959750062</v>
       </c>
       <c r="G31" s="25" t="n">
-        <v>0.1263576451529767</v>
+        <v>0.1265306873826442</v>
       </c>
       <c r="H31" s="25" t="n">
         <v>0.05011084527755218</v>
@@ -4120,7 +4120,7 @@
           <t>BOPTEXP</t>
         </is>
       </c>
-      <c r="C46" s="48" t="n">
+      <c r="C46" s="49" t="n">
         <v>45992</v>
       </c>
       <c r="D46" s="6" t="inlineStr">
@@ -4207,7 +4207,7 @@
           <t>BOPTEXP</t>
         </is>
       </c>
-      <c r="C47" s="48" t="n">
+      <c r="C47" s="49" t="n">
         <v>45992</v>
       </c>
       <c r="D47" s="6" t="inlineStr">
@@ -4247,7 +4247,7 @@
         </is>
       </c>
       <c r="N47" s="48" t="n">
-        <v>46076</v>
+        <v>46077</v>
       </c>
       <c r="O47" s="6" t="inlineStr">
         <is>
@@ -4286,7 +4286,7 @@
           <t>BOPTIMP</t>
         </is>
       </c>
-      <c r="C48" s="48" t="n">
+      <c r="C48" s="49" t="n">
         <v>45992</v>
       </c>
       <c r="D48" s="6" t="inlineStr">
@@ -4326,7 +4326,7 @@
         </is>
       </c>
       <c r="N48" s="48" t="n">
-        <v>46076</v>
+        <v>46077</v>
       </c>
       <c r="O48" s="6" t="inlineStr">
         <is>
@@ -4342,16 +4342,16 @@
         <v>3.43</v>
       </c>
       <c r="R48" s="6" t="n">
+        <v>3.43</v>
+      </c>
+      <c r="S48" s="6" t="n">
         <v>3.48</v>
-      </c>
-      <c r="S48" s="6" t="n">
-        <v>3.47</v>
       </c>
       <c r="T48" s="6" t="n">
         <v>3.47</v>
       </c>
       <c r="U48" s="21" t="n">
-        <v>3.43</v>
+        <v>3.47</v>
       </c>
     </row>
     <row r="49">
@@ -4361,7 +4361,7 @@
           <t>BOPTIMP</t>
         </is>
       </c>
-      <c r="C49" s="48" t="n">
+      <c r="C49" s="49" t="n">
         <v>45992</v>
       </c>
       <c r="D49" s="6" t="inlineStr">
@@ -4401,7 +4401,7 @@
         </is>
       </c>
       <c r="N49" s="48" t="n">
-        <v>46076</v>
+        <v>46077</v>
       </c>
       <c r="O49" s="6" t="inlineStr">
         <is>
@@ -4414,19 +4414,19 @@
         </is>
       </c>
       <c r="Q49" s="6" t="n">
+        <v>3.61</v>
+      </c>
+      <c r="R49" s="6" t="n">
         <v>3.59</v>
-      </c>
-      <c r="R49" s="6" t="n">
-        <v>3.65</v>
       </c>
       <c r="S49" s="6" t="n">
         <v>3.65</v>
       </c>
       <c r="T49" s="6" t="n">
+        <v>3.65</v>
+      </c>
+      <c r="U49" s="21" t="n">
         <v>3.66</v>
-      </c>
-      <c r="U49" s="21" t="n">
-        <v>3.63</v>
       </c>
     </row>
     <row r="50">
@@ -4440,7 +4440,7 @@
           <t>BOPSTB</t>
         </is>
       </c>
-      <c r="C50" s="48" t="n">
+      <c r="C50" s="49" t="n">
         <v>45992</v>
       </c>
       <c r="D50" s="6" t="inlineStr">
@@ -4480,7 +4480,7 @@
         </is>
       </c>
       <c r="N50" s="48" t="n">
-        <v>46076</v>
+        <v>46077</v>
       </c>
       <c r="O50" s="6" t="inlineStr">
         <is>
@@ -4493,19 +4493,19 @@
         </is>
       </c>
       <c r="Q50" s="6" t="n">
+        <v>4.04</v>
+      </c>
+      <c r="R50" s="6" t="n">
         <v>4.03</v>
-      </c>
-      <c r="R50" s="6" t="n">
-        <v>4.08</v>
       </c>
       <c r="S50" s="6" t="n">
         <v>4.08</v>
       </c>
       <c r="T50" s="6" t="n">
+        <v>4.08</v>
+      </c>
+      <c r="U50" s="21" t="n">
         <v>4.09</v>
-      </c>
-      <c r="U50" s="21" t="n">
-        <v>4.05</v>
       </c>
     </row>
     <row r="51" ht="31.5" customHeight="1">
@@ -4515,7 +4515,7 @@
           <t>BOPSTB</t>
         </is>
       </c>
-      <c r="C51" s="48" t="n">
+      <c r="C51" s="49" t="n">
         <v>45992</v>
       </c>
       <c r="D51" s="6" t="inlineStr">
@@ -4554,7 +4554,7 @@
           <t>MORTGAGE30US</t>
         </is>
       </c>
-      <c r="N51" s="48" t="n">
+      <c r="N51" s="49" t="n">
         <v>46069</v>
       </c>
       <c r="O51" s="6" t="inlineStr">
@@ -4606,7 +4606,7 @@
         </is>
       </c>
       <c r="N52" s="50" t="n">
-        <v>46076</v>
+        <v>46077</v>
       </c>
       <c r="O52" s="9" t="inlineStr">
         <is>
@@ -4619,19 +4619,19 @@
         </is>
       </c>
       <c r="Q52" s="9" t="n">
+        <v>5.77</v>
+      </c>
+      <c r="R52" s="9" t="n">
         <v>5.76</v>
       </c>
-      <c r="R52" s="9" t="n">
+      <c r="S52" s="9" t="n">
         <v>5.77</v>
-      </c>
-      <c r="S52" s="9" t="n">
-        <v>5.76</v>
       </c>
       <c r="T52" s="9" t="n">
         <v>5.76</v>
       </c>
       <c r="U52" s="22" t="n">
-        <v>5.75</v>
+        <v>5.76</v>
       </c>
     </row>
     <row r="53" ht="21" customHeight="1">

</xml_diff>

<commit_message>
Update dashboards - 2026-02-27
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -354,10 +354,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="168" fontId="1" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="168" fontId="1" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="168" fontId="1" fillId="3" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -933,7 +933,7 @@
           <t>PAYEMS</t>
         </is>
       </c>
-      <c r="N3" s="49" t="n">
+      <c r="N3" s="48" t="n">
         <v>46023</v>
       </c>
       <c r="O3" s="6" t="inlineStr">
@@ -1004,7 +1004,7 @@
           <t>PAYEMS</t>
         </is>
       </c>
-      <c r="N4" s="49" t="n">
+      <c r="N4" s="48" t="n">
         <v>46023</v>
       </c>
       <c r="O4" s="6" t="inlineStr">
@@ -1044,7 +1044,7 @@
           <t>NGDPSAXDCUSQ</t>
         </is>
       </c>
-      <c r="C5" s="48" t="n">
+      <c r="C5" s="49" t="n">
         <v>45931</v>
       </c>
       <c r="D5" s="6" t="inlineStr">
@@ -1083,7 +1083,7 @@
           <t>ADPMNUSNERSA</t>
         </is>
       </c>
-      <c r="N5" s="49" t="n">
+      <c r="N5" s="48" t="n">
         <v>46023</v>
       </c>
       <c r="O5" s="6" t="inlineStr">
@@ -1119,7 +1119,7 @@
           <t>NGDPSAXDCUSQ</t>
         </is>
       </c>
-      <c r="C6" s="48" t="n">
+      <c r="C6" s="49" t="n">
         <v>45931</v>
       </c>
       <c r="D6" s="6" t="inlineStr">
@@ -1158,7 +1158,7 @@
           <t>UNRATE</t>
         </is>
       </c>
-      <c r="N6" s="49" t="n">
+      <c r="N6" s="48" t="n">
         <v>46023</v>
       </c>
       <c r="O6" s="6" t="inlineStr">
@@ -1198,7 +1198,7 @@
           <t>GDPNOW</t>
         </is>
       </c>
-      <c r="C7" s="49" t="n">
+      <c r="C7" s="48" t="n">
         <v>45931</v>
       </c>
       <c r="D7" s="6" t="inlineStr">
@@ -1237,7 +1237,7 @@
           <t>U6RATE</t>
         </is>
       </c>
-      <c r="N7" s="49" t="n">
+      <c r="N7" s="48" t="n">
         <v>46023</v>
       </c>
       <c r="O7" s="6" t="inlineStr">
@@ -1277,7 +1277,7 @@
           <t>RECPROUSM156N</t>
         </is>
       </c>
-      <c r="C8" s="49" t="n">
+      <c r="C8" s="48" t="n">
         <v>45992</v>
       </c>
       <c r="D8" s="6" t="inlineStr">
@@ -1316,7 +1316,7 @@
           <t>CIVPART</t>
         </is>
       </c>
-      <c r="N8" s="49" t="n">
+      <c r="N8" s="48" t="n">
         <v>46023</v>
       </c>
       <c r="O8" s="6" t="inlineStr">
@@ -1395,7 +1395,7 @@
           <t>EMRATIO</t>
         </is>
       </c>
-      <c r="N9" s="49" t="n">
+      <c r="N9" s="48" t="n">
         <v>46023</v>
       </c>
       <c r="O9" s="6" t="inlineStr">
@@ -1470,7 +1470,7 @@
           <t>JTSJOR</t>
         </is>
       </c>
-      <c r="N10" s="49" t="n">
+      <c r="N10" s="48" t="n">
         <v>45992</v>
       </c>
       <c r="O10" s="6" t="inlineStr">
@@ -1549,7 +1549,7 @@
           <t>JTSHIR</t>
         </is>
       </c>
-      <c r="N11" s="49" t="n">
+      <c r="N11" s="48" t="n">
         <v>45992</v>
       </c>
       <c r="O11" s="6" t="inlineStr">
@@ -1624,7 +1624,7 @@
           <t>JTSTSR</t>
         </is>
       </c>
-      <c r="N12" s="49" t="n">
+      <c r="N12" s="48" t="n">
         <v>45992</v>
       </c>
       <c r="O12" s="6" t="inlineStr">
@@ -1703,7 +1703,7 @@
           <t>ICSA</t>
         </is>
       </c>
-      <c r="N13" s="48" t="n">
+      <c r="N13" s="49" t="n">
         <v>46069</v>
       </c>
       <c r="O13" s="6" t="inlineStr">
@@ -1778,7 +1778,7 @@
           <t>CCSA</t>
         </is>
       </c>
-      <c r="N14" s="48" t="n">
+      <c r="N14" s="49" t="n">
         <v>46062</v>
       </c>
       <c r="O14" s="6" t="inlineStr">
@@ -1857,7 +1857,7 @@
           <t>AWHAETP</t>
         </is>
       </c>
-      <c r="N15" s="49" t="n">
+      <c r="N15" s="48" t="n">
         <v>46023</v>
       </c>
       <c r="O15" s="6" t="inlineStr">
@@ -1944,7 +1944,7 @@
           <t>RSAFS</t>
         </is>
       </c>
-      <c r="C17" s="49" t="n">
+      <c r="C17" s="48" t="n">
         <v>45992</v>
       </c>
       <c r="D17" s="6" t="inlineStr">
@@ -2031,7 +2031,7 @@
           <t>RSAFS</t>
         </is>
       </c>
-      <c r="C18" s="49" t="n">
+      <c r="C18" s="48" t="n">
         <v>45992</v>
       </c>
       <c r="D18" s="6" t="inlineStr">
@@ -2070,7 +2070,7 @@
           <t>CPIAUCSL</t>
         </is>
       </c>
-      <c r="N18" s="49" t="n">
+      <c r="N18" s="48" t="n">
         <v>46023</v>
       </c>
       <c r="O18" s="6" t="inlineStr">
@@ -2145,7 +2145,7 @@
           <t>CPIAUCSL</t>
         </is>
       </c>
-      <c r="N19" s="49" t="n">
+      <c r="N19" s="48" t="n">
         <v>46023</v>
       </c>
       <c r="O19" s="6" t="inlineStr">
@@ -2220,7 +2220,7 @@
           <t>CPILFESL</t>
         </is>
       </c>
-      <c r="N20" s="49" t="n">
+      <c r="N20" s="48" t="n">
         <v>46023</v>
       </c>
       <c r="O20" s="6" t="inlineStr">
@@ -2295,7 +2295,7 @@
           <t>CPILFESL</t>
         </is>
       </c>
-      <c r="N21" s="49" t="n">
+      <c r="N21" s="48" t="n">
         <v>46023</v>
       </c>
       <c r="O21" s="6" t="inlineStr">
@@ -2335,7 +2335,7 @@
           <t>TOTALSA</t>
         </is>
       </c>
-      <c r="C22" s="49" t="n">
+      <c r="C22" s="48" t="n">
         <v>46023</v>
       </c>
       <c r="D22" s="6" t="inlineStr">
@@ -2374,7 +2374,7 @@
           <t>PPIFIS</t>
         </is>
       </c>
-      <c r="N22" s="49" t="n">
+      <c r="N22" s="48" t="n">
         <v>45992</v>
       </c>
       <c r="O22" s="6" t="inlineStr">
@@ -2410,7 +2410,7 @@
           <t>TOTALSA</t>
         </is>
       </c>
-      <c r="C23" s="49" t="n">
+      <c r="C23" s="48" t="n">
         <v>46023</v>
       </c>
       <c r="D23" s="6" t="inlineStr">
@@ -2444,7 +2444,7 @@
           <t>PPIFIS</t>
         </is>
       </c>
-      <c r="N23" s="49" t="n">
+      <c r="N23" s="48" t="n">
         <v>45992</v>
       </c>
       <c r="O23" s="6" t="inlineStr">
@@ -2484,7 +2484,7 @@
           <t>REVOLSL</t>
         </is>
       </c>
-      <c r="C24" s="49" t="n">
+      <c r="C24" s="48" t="n">
         <v>45992</v>
       </c>
       <c r="D24" s="6" t="inlineStr">
@@ -2563,7 +2563,7 @@
           <t>NONREVSL</t>
         </is>
       </c>
-      <c r="C25" s="49" t="n">
+      <c r="C25" s="48" t="n">
         <v>45992</v>
       </c>
       <c r="D25" s="6" t="inlineStr">
@@ -2792,7 +2792,7 @@
           <t>DGORDER</t>
         </is>
       </c>
-      <c r="C28" s="49" t="n">
+      <c r="C28" s="48" t="n">
         <v>45992</v>
       </c>
       <c r="D28" s="6" t="inlineStr">
@@ -2831,7 +2831,7 @@
           <t>MICH</t>
         </is>
       </c>
-      <c r="N28" s="49" t="n">
+      <c r="N28" s="48" t="n">
         <v>46023</v>
       </c>
       <c r="O28" s="6" t="inlineStr">
@@ -2867,7 +2867,7 @@
           <t>DGORDER</t>
         </is>
       </c>
-      <c r="C29" s="49" t="n">
+      <c r="C29" s="48" t="n">
         <v>45992</v>
       </c>
       <c r="D29" s="6" t="inlineStr">
@@ -2906,7 +2906,7 @@
           <t>T5YIFR</t>
         </is>
       </c>
-      <c r="N29" s="48" t="n">
+      <c r="N29" s="49" t="n">
         <v>46079</v>
       </c>
       <c r="O29" s="6" t="inlineStr">
@@ -2946,7 +2946,7 @@
           <t>ADXDNO</t>
         </is>
       </c>
-      <c r="C30" s="49" t="n">
+      <c r="C30" s="48" t="n">
         <v>45992</v>
       </c>
       <c r="D30" s="6" t="inlineStr">
@@ -2985,7 +2985,7 @@
           <t>T10YIE</t>
         </is>
       </c>
-      <c r="N30" s="48" t="n">
+      <c r="N30" s="49" t="n">
         <v>46079</v>
       </c>
       <c r="O30" s="6" t="inlineStr">
@@ -3021,7 +3021,7 @@
           <t>ADXDNO</t>
         </is>
       </c>
-      <c r="C31" s="49" t="n">
+      <c r="C31" s="48" t="n">
         <v>45992</v>
       </c>
       <c r="D31" s="6" t="inlineStr">
@@ -3060,7 +3060,7 @@
           <t>ECIWAG</t>
         </is>
       </c>
-      <c r="N31" s="49" t="n">
+      <c r="N31" s="48" t="n">
         <v>45931</v>
       </c>
       <c r="O31" s="6" t="inlineStr">
@@ -3100,7 +3100,7 @@
           <t>INDPRO</t>
         </is>
       </c>
-      <c r="C32" s="49" t="n">
+      <c r="C32" s="48" t="n">
         <v>46023</v>
       </c>
       <c r="D32" s="6" t="inlineStr">
@@ -3135,7 +3135,7 @@
           <t>ECIWAG</t>
         </is>
       </c>
-      <c r="N32" s="49" t="n">
+      <c r="N32" s="48" t="n">
         <v>45931</v>
       </c>
       <c r="O32" s="6" t="inlineStr">
@@ -3171,7 +3171,7 @@
           <t>INDPRO</t>
         </is>
       </c>
-      <c r="C33" s="49" t="n">
+      <c r="C33" s="48" t="n">
         <v>46023</v>
       </c>
       <c r="D33" s="6" t="inlineStr">
@@ -3210,7 +3210,7 @@
           <t>CES0500000003</t>
         </is>
       </c>
-      <c r="N33" s="49" t="n">
+      <c r="N33" s="48" t="n">
         <v>46023</v>
       </c>
       <c r="O33" s="6" t="inlineStr">
@@ -3250,7 +3250,7 @@
           <t>TCU</t>
         </is>
       </c>
-      <c r="C34" s="49" t="n">
+      <c r="C34" s="48" t="n">
         <v>46023</v>
       </c>
       <c r="D34" s="6" t="inlineStr">
@@ -3285,7 +3285,7 @@
           <t>RCES0500000003*</t>
         </is>
       </c>
-      <c r="N34" s="49" t="n">
+      <c r="N34" s="48" t="n">
         <v>45992</v>
       </c>
       <c r="O34" s="6" t="inlineStr">
@@ -3325,7 +3325,7 @@
           <t>PRS85006092</t>
         </is>
       </c>
-      <c r="C35" s="49" t="n">
+      <c r="C35" s="48" t="n">
         <v>45839</v>
       </c>
       <c r="D35" s="6" t="inlineStr">
@@ -3364,7 +3364,7 @@
           <t>RCES0500000003*</t>
         </is>
       </c>
-      <c r="N35" s="49" t="n">
+      <c r="N35" s="48" t="n">
         <v>45992</v>
       </c>
       <c r="O35" s="6" t="inlineStr">
@@ -3404,7 +3404,7 @@
           <t>HOUST</t>
         </is>
       </c>
-      <c r="C36" s="49" t="n">
+      <c r="C36" s="48" t="n">
         <v>45992</v>
       </c>
       <c r="D36" s="6" t="inlineStr">
@@ -3439,7 +3439,7 @@
           <t>RCES0500000003*</t>
         </is>
       </c>
-      <c r="N36" s="49" t="n">
+      <c r="N36" s="48" t="n">
         <v>45992</v>
       </c>
       <c r="O36" s="6" t="inlineStr">
@@ -3475,7 +3475,7 @@
           <t>HOUST</t>
         </is>
       </c>
-      <c r="C37" s="49" t="n">
+      <c r="C37" s="48" t="n">
         <v>45992</v>
       </c>
       <c r="D37" s="6" t="inlineStr">
@@ -3514,7 +3514,7 @@
           <t>CSUSHPINSA</t>
         </is>
       </c>
-      <c r="N37" s="48" t="n">
+      <c r="N37" s="49" t="n">
         <v>45992</v>
       </c>
       <c r="O37" s="6" t="inlineStr">
@@ -3554,7 +3554,7 @@
           <t>PERMIT</t>
         </is>
       </c>
-      <c r="C38" s="49" t="n">
+      <c r="C38" s="48" t="n">
         <v>45992</v>
       </c>
       <c r="D38" s="6" t="inlineStr">
@@ -3589,7 +3589,7 @@
           <t>CSUSHPINSA</t>
         </is>
       </c>
-      <c r="N38" s="48" t="n">
+      <c r="N38" s="49" t="n">
         <v>45992</v>
       </c>
       <c r="O38" s="6" t="inlineStr">
@@ -3625,7 +3625,7 @@
           <t>PERMIT</t>
         </is>
       </c>
-      <c r="C39" s="49" t="n">
+      <c r="C39" s="48" t="n">
         <v>45992</v>
       </c>
       <c r="D39" s="6" t="inlineStr">
@@ -3664,7 +3664,7 @@
           <t>TWEXBGSMTH</t>
         </is>
       </c>
-      <c r="N39" s="49" t="n">
+      <c r="N39" s="48" t="n">
         <v>46023</v>
       </c>
       <c r="O39" s="6" t="inlineStr">
@@ -3739,7 +3739,7 @@
           <t>TWEXBGSMTH</t>
         </is>
       </c>
-      <c r="N40" s="49" t="n">
+      <c r="N40" s="48" t="n">
         <v>46023</v>
       </c>
       <c r="O40" s="6" t="inlineStr">
@@ -3814,7 +3814,7 @@
           <t>IQ</t>
         </is>
       </c>
-      <c r="N41" s="49" t="n">
+      <c r="N41" s="48" t="n">
         <v>45992</v>
       </c>
       <c r="O41" s="6" t="inlineStr">
@@ -3854,7 +3854,7 @@
           <t>EXHOSLUSM495S</t>
         </is>
       </c>
-      <c r="C42" s="49" t="n">
+      <c r="C42" s="48" t="n">
         <v>46023</v>
       </c>
       <c r="D42" s="6" t="inlineStr">
@@ -3889,7 +3889,7 @@
           <t>IQ</t>
         </is>
       </c>
-      <c r="N42" s="49" t="n">
+      <c r="N42" s="48" t="n">
         <v>45992</v>
       </c>
       <c r="O42" s="6" t="inlineStr">
@@ -3925,7 +3925,7 @@
           <t>EXHOSLUSM495S</t>
         </is>
       </c>
-      <c r="C43" s="49" t="n">
+      <c r="C43" s="48" t="n">
         <v>46023</v>
       </c>
       <c r="D43" s="6" t="inlineStr">
@@ -3964,7 +3964,7 @@
           <t>IR</t>
         </is>
       </c>
-      <c r="N43" s="49" t="n">
+      <c r="N43" s="48" t="n">
         <v>45992</v>
       </c>
       <c r="O43" s="6" t="inlineStr">
@@ -4039,7 +4039,7 @@
           <t>IR</t>
         </is>
       </c>
-      <c r="N44" s="49" t="n">
+      <c r="N44" s="48" t="n">
         <v>45992</v>
       </c>
       <c r="O44" s="6" t="inlineStr">
@@ -4126,7 +4126,7 @@
           <t>BOPTEXP</t>
         </is>
       </c>
-      <c r="C46" s="49" t="n">
+      <c r="C46" s="48" t="n">
         <v>45992</v>
       </c>
       <c r="D46" s="6" t="inlineStr">
@@ -4213,7 +4213,7 @@
           <t>BOPTEXP</t>
         </is>
       </c>
-      <c r="C47" s="49" t="n">
+      <c r="C47" s="48" t="n">
         <v>45992</v>
       </c>
       <c r="D47" s="6" t="inlineStr">
@@ -4252,7 +4252,7 @@
           <t>DFF</t>
         </is>
       </c>
-      <c r="N47" s="48" t="n">
+      <c r="N47" s="49" t="n">
         <v>46078</v>
       </c>
       <c r="O47" s="6" t="inlineStr">
@@ -4292,7 +4292,7 @@
           <t>BOPTIMP</t>
         </is>
       </c>
-      <c r="C48" s="49" t="n">
+      <c r="C48" s="48" t="n">
         <v>45992</v>
       </c>
       <c r="D48" s="6" t="inlineStr">
@@ -4331,7 +4331,7 @@
           <t>DGS2</t>
         </is>
       </c>
-      <c r="N48" s="48" t="n">
+      <c r="N48" s="49" t="n">
         <v>46078</v>
       </c>
       <c r="O48" s="6" t="inlineStr">
@@ -4367,7 +4367,7 @@
           <t>BOPTIMP</t>
         </is>
       </c>
-      <c r="C49" s="49" t="n">
+      <c r="C49" s="48" t="n">
         <v>45992</v>
       </c>
       <c r="D49" s="6" t="inlineStr">
@@ -4406,7 +4406,7 @@
           <t>DGS5</t>
         </is>
       </c>
-      <c r="N49" s="48" t="n">
+      <c r="N49" s="49" t="n">
         <v>46078</v>
       </c>
       <c r="O49" s="6" t="inlineStr">
@@ -4446,7 +4446,7 @@
           <t>BOPSTB</t>
         </is>
       </c>
-      <c r="C50" s="49" t="n">
+      <c r="C50" s="48" t="n">
         <v>45992</v>
       </c>
       <c r="D50" s="6" t="inlineStr">
@@ -4485,7 +4485,7 @@
           <t>DGS10</t>
         </is>
       </c>
-      <c r="N50" s="48" t="n">
+      <c r="N50" s="49" t="n">
         <v>46078</v>
       </c>
       <c r="O50" s="6" t="inlineStr">
@@ -4521,7 +4521,7 @@
           <t>BOPSTB</t>
         </is>
       </c>
-      <c r="C51" s="49" t="n">
+      <c r="C51" s="48" t="n">
         <v>45992</v>
       </c>
       <c r="D51" s="6" t="inlineStr">
@@ -4560,7 +4560,7 @@
           <t>MORTGAGE30US</t>
         </is>
       </c>
-      <c r="N51" s="48" t="n">
+      <c r="N51" s="49" t="n">
         <v>46076</v>
       </c>
       <c r="O51" s="6" t="inlineStr">

</xml_diff>

<commit_message>
Update dashboards - 2026-02-28
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -2368,8 +2368,8 @@
           <t>PPIFIS</t>
         </is>
       </c>
-      <c r="N22" s="48" t="n">
-        <v>45992</v>
+      <c r="N22" s="49" t="n">
+        <v>46023</v>
       </c>
       <c r="O22" s="6" t="inlineStr">
         <is>
@@ -2382,19 +2382,19 @@
         </is>
       </c>
       <c r="Q22" s="37" t="n">
-        <v>0.004902708763177221</v>
+        <v>0.00480699391202144</v>
       </c>
       <c r="R22" s="37" t="n">
-        <v>0.002380714879468115</v>
+        <v>0.004303799147197918</v>
       </c>
       <c r="S22" s="37" t="n">
-        <v>0.0008919003467759978</v>
+        <v>0.00248632190555953</v>
       </c>
       <c r="T22" s="37" t="n">
-        <v>0.006579167755378368</v>
+        <v>0.001184731605045064</v>
       </c>
       <c r="U22" s="23" t="n">
-        <v>-0.001852396747271667</v>
+        <v>0.006147582151921682</v>
       </c>
     </row>
     <row r="23">
@@ -2438,8 +2438,8 @@
           <t>PPIFIS</t>
         </is>
       </c>
-      <c r="N23" s="48" t="n">
-        <v>45992</v>
+      <c r="N23" s="49" t="n">
+        <v>46023</v>
       </c>
       <c r="O23" s="6" t="inlineStr">
         <is>
@@ -2452,19 +2452,19 @@
         </is>
       </c>
       <c r="Q23" s="37" t="n">
-        <v>0.02953930644481603</v>
+        <v>0.02837641493495531</v>
       </c>
       <c r="R23" s="37" t="n">
-        <v>0.02966029332404323</v>
+        <v>0.02988058645921175</v>
       </c>
       <c r="S23" s="37" t="n">
-        <v>0.02826137498119562</v>
+        <v>0.02970357876911097</v>
       </c>
       <c r="T23" s="37" t="n">
-        <v>0.03051607769973669</v>
+        <v>0.02822398731321852</v>
       </c>
       <c r="U23" s="23" t="n">
-        <v>0.02682305998899265</v>
+        <v>0.03046576545064236</v>
       </c>
     </row>
     <row r="24">
@@ -2901,7 +2901,7 @@
         </is>
       </c>
       <c r="N29" s="49" t="n">
-        <v>46079</v>
+        <v>46080</v>
       </c>
       <c r="O29" s="6" t="inlineStr">
         <is>
@@ -2914,19 +2914,19 @@
         </is>
       </c>
       <c r="Q29" s="6" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="R29" s="6" t="n">
         <v>2.13</v>
       </c>
-      <c r="R29" s="6" t="n">
+      <c r="S29" s="6" t="n">
         <v>2.14</v>
-      </c>
-      <c r="S29" s="6" t="n">
-        <v>2.12</v>
       </c>
       <c r="T29" s="6" t="n">
         <v>2.12</v>
       </c>
       <c r="U29" s="21" t="n">
-        <v>2.13</v>
+        <v>2.12</v>
       </c>
     </row>
     <row r="30">
@@ -2980,7 +2980,7 @@
         </is>
       </c>
       <c r="N30" s="49" t="n">
-        <v>46079</v>
+        <v>46080</v>
       </c>
       <c r="O30" s="6" t="inlineStr">
         <is>
@@ -2993,19 +2993,19 @@
         </is>
       </c>
       <c r="Q30" s="6" t="n">
-        <v>2.28</v>
+        <v>2.25</v>
       </c>
       <c r="R30" s="6" t="n">
         <v>2.28</v>
       </c>
       <c r="S30" s="6" t="n">
-        <v>2.26</v>
+        <v>2.28</v>
       </c>
       <c r="T30" s="6" t="n">
         <v>2.26</v>
       </c>
       <c r="U30" s="21" t="n">
-        <v>2.28</v>
+        <v>2.26</v>
       </c>
     </row>
     <row r="31">
@@ -4247,7 +4247,7 @@
         </is>
       </c>
       <c r="N47" s="49" t="n">
-        <v>46078</v>
+        <v>46079</v>
       </c>
       <c r="O47" s="6" t="inlineStr">
         <is>
@@ -4326,7 +4326,7 @@
         </is>
       </c>
       <c r="N48" s="49" t="n">
-        <v>46078</v>
+        <v>46079</v>
       </c>
       <c r="O48" s="6" t="inlineStr">
         <is>
@@ -4339,19 +4339,19 @@
         </is>
       </c>
       <c r="Q48" s="6" t="n">
+        <v>3.42</v>
+      </c>
+      <c r="R48" s="6" t="n">
         <v>3.45</v>
-      </c>
-      <c r="R48" s="6" t="n">
-        <v>3.43</v>
       </c>
       <c r="S48" s="6" t="n">
         <v>3.43</v>
       </c>
       <c r="T48" s="6" t="n">
+        <v>3.43</v>
+      </c>
+      <c r="U48" s="21" t="n">
         <v>3.48</v>
-      </c>
-      <c r="U48" s="21" t="n">
-        <v>3.47</v>
       </c>
     </row>
     <row r="49">
@@ -4401,7 +4401,7 @@
         </is>
       </c>
       <c r="N49" s="49" t="n">
-        <v>46078</v>
+        <v>46079</v>
       </c>
       <c r="O49" s="6" t="inlineStr">
         <is>
@@ -4414,16 +4414,16 @@
         </is>
       </c>
       <c r="Q49" s="6" t="n">
-        <v>3.61</v>
+        <v>3.57</v>
       </c>
       <c r="R49" s="6" t="n">
         <v>3.61</v>
       </c>
       <c r="S49" s="6" t="n">
+        <v>3.61</v>
+      </c>
+      <c r="T49" s="6" t="n">
         <v>3.59</v>
-      </c>
-      <c r="T49" s="6" t="n">
-        <v>3.65</v>
       </c>
       <c r="U49" s="21" t="n">
         <v>3.65</v>
@@ -4480,7 +4480,7 @@
         </is>
       </c>
       <c r="N50" s="49" t="n">
-        <v>46078</v>
+        <v>46079</v>
       </c>
       <c r="O50" s="6" t="inlineStr">
         <is>
@@ -4493,16 +4493,16 @@
         </is>
       </c>
       <c r="Q50" s="6" t="n">
+        <v>4.02</v>
+      </c>
+      <c r="R50" s="6" t="n">
         <v>4.05</v>
       </c>
-      <c r="R50" s="6" t="n">
+      <c r="S50" s="6" t="n">
         <v>4.04</v>
       </c>
-      <c r="S50" s="6" t="n">
+      <c r="T50" s="6" t="n">
         <v>4.03</v>
-      </c>
-      <c r="T50" s="6" t="n">
-        <v>4.08</v>
       </c>
       <c r="U50" s="21" t="n">
         <v>4.08</v>

</xml_diff>

<commit_message>
Update dashboards - 2026-03-01
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template-UPDATE.xlsx
@@ -2374,8 +2374,8 @@
           <t>PPIFIS</t>
         </is>
       </c>
-      <c r="N22" s="48" t="n">
-        <v>45992</v>
+      <c r="N22" s="49" t="n">
+        <v>46023</v>
       </c>
       <c r="O22" s="6" t="inlineStr">
         <is>
@@ -2388,19 +2388,19 @@
         </is>
       </c>
       <c r="Q22" s="38" t="n">
-        <v>0.004902708763177221</v>
+        <v>0.00480699391202144</v>
       </c>
       <c r="R22" s="38" t="n">
-        <v>0.002380714879468115</v>
+        <v>0.004303799147197918</v>
       </c>
       <c r="S22" s="38" t="n">
-        <v>0.0008919003467759978</v>
+        <v>0.00248632190555953</v>
       </c>
       <c r="T22" s="38" t="n">
-        <v>0.006579167755378368</v>
+        <v>0.001184731605045064</v>
       </c>
       <c r="U22" s="23" t="n">
-        <v>-0.001852396747271667</v>
+        <v>0.006147582151921682</v>
       </c>
     </row>
     <row r="23">
@@ -2444,8 +2444,8 @@
           <t>PPIFIS</t>
         </is>
       </c>
-      <c r="N23" s="48" t="n">
-        <v>45992</v>
+      <c r="N23" s="49" t="n">
+        <v>46023</v>
       </c>
       <c r="O23" s="6" t="inlineStr">
         <is>
@@ -2458,19 +2458,19 @@
         </is>
       </c>
       <c r="Q23" s="38" t="n">
-        <v>0.02953930644481603</v>
+        <v>0.02837641493495531</v>
       </c>
       <c r="R23" s="38" t="n">
-        <v>0.02966029332404323</v>
+        <v>0.02988058645921175</v>
       </c>
       <c r="S23" s="38" t="n">
-        <v>0.02826137498119562</v>
+        <v>0.02970357876911097</v>
       </c>
       <c r="T23" s="38" t="n">
-        <v>0.03051607769973669</v>
+        <v>0.02822398731321852</v>
       </c>
       <c r="U23" s="23" t="n">
-        <v>0.02682305998899265</v>
+        <v>0.03046576545064236</v>
       </c>
     </row>
     <row r="24">
@@ -2907,7 +2907,7 @@
         </is>
       </c>
       <c r="N29" s="49" t="n">
-        <v>46079</v>
+        <v>46080</v>
       </c>
       <c r="O29" s="6" t="inlineStr">
         <is>
@@ -2920,19 +2920,19 @@
         </is>
       </c>
       <c r="Q29" s="6" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="R29" s="6" t="n">
         <v>2.13</v>
       </c>
-      <c r="R29" s="6" t="n">
+      <c r="S29" s="6" t="n">
         <v>2.14</v>
-      </c>
-      <c r="S29" s="6" t="n">
-        <v>2.12</v>
       </c>
       <c r="T29" s="6" t="n">
         <v>2.12</v>
       </c>
       <c r="U29" s="21" t="n">
-        <v>2.13</v>
+        <v>2.12</v>
       </c>
     </row>
     <row r="30">
@@ -2986,7 +2986,7 @@
         </is>
       </c>
       <c r="N30" s="49" t="n">
-        <v>46079</v>
+        <v>46080</v>
       </c>
       <c r="O30" s="6" t="inlineStr">
         <is>
@@ -2999,19 +2999,19 @@
         </is>
       </c>
       <c r="Q30" s="6" t="n">
-        <v>2.28</v>
+        <v>2.25</v>
       </c>
       <c r="R30" s="6" t="n">
         <v>2.28</v>
       </c>
       <c r="S30" s="6" t="n">
-        <v>2.26</v>
+        <v>2.28</v>
       </c>
       <c r="T30" s="6" t="n">
         <v>2.26</v>
       </c>
       <c r="U30" s="21" t="n">
-        <v>2.28</v>
+        <v>2.26</v>
       </c>
     </row>
     <row r="31">
@@ -4253,7 +4253,7 @@
         </is>
       </c>
       <c r="N47" s="49" t="n">
-        <v>46078</v>
+        <v>46079</v>
       </c>
       <c r="O47" s="6" t="inlineStr">
         <is>
@@ -4332,7 +4332,7 @@
         </is>
       </c>
       <c r="N48" s="49" t="n">
-        <v>46078</v>
+        <v>46079</v>
       </c>
       <c r="O48" s="6" t="inlineStr">
         <is>
@@ -4345,19 +4345,19 @@
         </is>
       </c>
       <c r="Q48" s="6" t="n">
+        <v>3.42</v>
+      </c>
+      <c r="R48" s="6" t="n">
         <v>3.45</v>
-      </c>
-      <c r="R48" s="6" t="n">
-        <v>3.43</v>
       </c>
       <c r="S48" s="6" t="n">
         <v>3.43</v>
       </c>
       <c r="T48" s="6" t="n">
+        <v>3.43</v>
+      </c>
+      <c r="U48" s="21" t="n">
         <v>3.48</v>
-      </c>
-      <c r="U48" s="21" t="n">
-        <v>3.47</v>
       </c>
     </row>
     <row r="49">
@@ -4407,7 +4407,7 @@
         </is>
       </c>
       <c r="N49" s="49" t="n">
-        <v>46078</v>
+        <v>46079</v>
       </c>
       <c r="O49" s="6" t="inlineStr">
         <is>
@@ -4420,16 +4420,16 @@
         </is>
       </c>
       <c r="Q49" s="6" t="n">
-        <v>3.61</v>
+        <v>3.57</v>
       </c>
       <c r="R49" s="6" t="n">
         <v>3.61</v>
       </c>
       <c r="S49" s="6" t="n">
+        <v>3.61</v>
+      </c>
+      <c r="T49" s="6" t="n">
         <v>3.59</v>
-      </c>
-      <c r="T49" s="6" t="n">
-        <v>3.65</v>
       </c>
       <c r="U49" s="21" t="n">
         <v>3.65</v>
@@ -4486,7 +4486,7 @@
         </is>
       </c>
       <c r="N50" s="49" t="n">
-        <v>46078</v>
+        <v>46079</v>
       </c>
       <c r="O50" s="6" t="inlineStr">
         <is>
@@ -4499,16 +4499,16 @@
         </is>
       </c>
       <c r="Q50" s="6" t="n">
+        <v>4.02</v>
+      </c>
+      <c r="R50" s="6" t="n">
         <v>4.05</v>
       </c>
-      <c r="R50" s="6" t="n">
+      <c r="S50" s="6" t="n">
         <v>4.04</v>
       </c>
-      <c r="S50" s="6" t="n">
+      <c r="T50" s="6" t="n">
         <v>4.03</v>
-      </c>
-      <c r="T50" s="6" t="n">
-        <v>4.08</v>
       </c>
       <c r="U50" s="21" t="n">
         <v>4.08</v>

</xml_diff>